<commit_message>
rename vitals, test SearchParameter description, update CapabilityStatement
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\US-Core-R4\input\resources_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72BC494A-7D45-4FDB-886A-EBB0229E3A9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E563653-E32C-4BBB-B3E5-24F934AA064F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38355" windowHeight="15795" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4980" yWindow="1170" windowWidth="38355" windowHeight="15795" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -48,7 +48,7 @@
     <author>User</author>
   </authors>
   <commentList>
-    <comment ref="A25" authorId="0" shapeId="0" xr:uid="{5BD04D3A-61B4-4353-A042-87021061D1BC}">
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{1602FA8F-AF8A-4828-872F-93D3D42FD6D9}">
       <text>
         <r>
           <rPr>
@@ -145,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1938" uniqueCount="531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1983" uniqueCount="557">
   <si>
     <t>Element</t>
   </si>
@@ -1508,18 +1508,6 @@
     <t>GET [base]/CarePlan?patient=1137192&amp;category=http://hl7.org/fhir/us/core/CodeSystem/careplan-category\|assess-plan&amp;status=active&amp;date=ge2019~GET [base]/CarePlan?patient=1137192&amp;category=http://hl7.org/fhir/us/core/CodeSystem/careplan-category\|assess-plan&amp;status=active&amp;date=ge2018&amp;date=le2019</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/pediatric-weight-for-height</t>
-  </si>
-  <si>
-    <t>US Core Pediatric Weight  for Height Observation Profile</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/pediatric-bmi-for-age</t>
-  </si>
-  <si>
-    <t>US Core Pediatric BMI for Age Observation Profile</t>
-  </si>
-  <si>
     <t>A client **SHOULD** be capable of transacting a $docref operation and capable of receiving at least a reference to a generated CCD document, and  **MAY** be able to receive other document types, if available.   **SHOULD**  be capable of receiving documents as included resources in response to the operation.
 `GET [base]/DocumentReference/$docref?patient=[id]`</t>
   </si>
@@ -1530,12 +1518,6 @@
     <t>This conformance expectation applies **only**  to the *US Core DiagnosticReport Profile for Report and Note exchange* profile.  The conformance expectation for the *US Core DiagnosticReport Profile for Laboratory Results Reporting* is  **MAY**.</t>
   </si>
   <si>
-    <t>The MedicationStatement resources can represent a medication using either a code or refer to the Medication resource. When referencing Medication, the resource may be [contained](http://hl7.org/fhir/R4/references.html#contained) or an external resource. The server application **MAY** choose any one way or more than one method, but if an external reference to Medication is used, the server **SHALL** support the _include` parameter for searching this element. The client application must support all methods.
- For example, A server **SHALL** be capable of returning all medications for a patient using one of or both:
- `GET /MedicationStatement?patient=[id]`
- `GET /MedicationStatement?patient=[id]&amp;_include=MedicationStatement:medication`</t>
-  </si>
-  <si>
     <t>US Core Implantable Device Profile</t>
   </si>
   <si>
@@ -1692,9 +1674,6 @@
     <t>packagepath</t>
   </si>
   <si>
-    <t>//ERICS-AIR-2/ehaas/Documents/FHIR/US-Core-R4/output</t>
-  </si>
-  <si>
     <t>pre</t>
   </si>
   <si>
@@ -1722,38 +1701,171 @@
     <t>http://hl7.org/fhir/us/core/ImplementationGuide/hl7.fhir.us.core|3.1.1</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/head-occipital-frontal-circumference-percentile</t>
-  </si>
-  <si>
-    <t>US Core Pediatric Head Occipital-frontal Circumference Percentile Profile</t>
-  </si>
-  <si>
     <t>!http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationstatement</t>
   </si>
   <si>
-    <t>The MedicationRequest resource can represent a medication, using an external reference to a Medication resource. If an external Medication Resource is used in a MedicationRequest, then the READ **SHALL**  be supported.</t>
-  </si>
-  <si>
     <t>profile_conf</t>
   </si>
   <si>
     <t>//ERICS-AIR-2/ehaas/Documents/FHIR/US-Core-R4/input/</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-vital-signs</t>
+  </si>
+  <si>
+    <t>US Core Vital Signs Profile</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-blood-pressure</t>
+  </si>
+  <si>
+    <t>US Core Blood Pressure Profile</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-bmi</t>
+  </si>
+  <si>
+    <t>US Core BMI Profile</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-head-circumference</t>
+  </si>
+  <si>
+    <t>US Core Head Circumference Profile</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-body-height</t>
+  </si>
+  <si>
+    <t>US Core Body Height Profile</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-body-weight</t>
+  </si>
+  <si>
+    <t>US Core Body Weight Profile</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-body-temperature</t>
+  </si>
+  <si>
+    <t>US Core Body Temperature Profile</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-heart-rate</t>
+  </si>
+  <si>
+    <t>US Core Heart Rate Profile</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/pediatric-bmi-for-age-observation</t>
+  </si>
+  <si>
+    <t>Pediatric BMI for Age Observation Profile</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/pediatric-head-occipital-frontal-circumference-percentile</t>
+  </si>
+  <si>
+    <t>Pediatric Head Occipital-frontal Circumference Percentile Profile</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/pediatric-weight-for-height-observation</t>
+  </si>
+  <si>
+    <t>Pediatric Weight for Height Observation Profile</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-respiratory-rate</t>
+  </si>
+  <si>
+    <t>US Core Respiratory Rate Profile</t>
+  </si>
+  <si>
+    <t>http://build.fhir.org/ig/HL7/US-Core/package.tgz</t>
+  </si>
+  <si>
+    <t>* Additional considerations for systems aligning with [HL7 Consolidated (C-CDA)](http://www.hl7.org/implement/standards/product_brief.cfm?product_id=492) Care Plan requirements:
+    - US Core Goal **SHOULD** be present in CarePlan.goal
+    - US Core Condition **SHOULD** be present in CarePlan.addresses
+    - Assement and Plan **MAY** be included as narrative text</t>
   </si>
   <si>
     <t>* The Encounter resource can represent a reason using either a code with `Encounter.reasonCode`, or a reference with `Encounter.reasonReference` to  Condition or other resource.
    * Although both are marked as must support, the server systems are not required to support both a code and a reference, but they **SHALL** support *at least one* of these elements.
    * The client application **SHALL** support both elements.
    * if `Encounter.reasonReference` references an Observation, it **SHOULD** conform to a US Core Observation if applicable. (for example, a laboratory result should conform to the US Core Laboratory Result Observation Profile)
-* The base FHIR Location resource is being referenced by `Encounter.location`.  However, it **SHOULD** conform to US Core Location.</t>
-  </si>
-  <si>
-    <t>The MedicationRequest resources can represent a medication using either a code or refer to the Medication resource. When referencing Medication, the resource may be [contained](http://hl7.org/fhir/R4/references.html#contained) or an external resource. The server application **MAY** choose any one way or more than one method, but if an external reference to Medication is used, the server **SHALL** support the _include` parameter for searching this element. The client application must support all methods.
+* The intent of this profile is to support *where the encounter occurred*.  The location address can be represented by either by the Location referenced by `Encounter.location.location` or indirectly through the Organization referenced by `Encounter.serviceProvider`.
+  * Although both are marked as must support, the server systems are not required to support both `Encounter.location.location` and `Encounter.serviceProvider`, but they **SHALL** support *at least one* of these elements.
+  * The client application **SHALL** support both elements.
+  * if using `Encounter.locatison.location` it **SHOULD** conform to US Core Location.  However, as a result of implementation feedback, it **MAY**  reference the base FHIR Location resource.  See this guidance on [Referencing US Core Profiles]</t>
+  </si>
+  <si>
+    <t>* Based upon the ONC U.S. Core Data for Interoperability (USCDI) v1 requirements, CVX vaccine codes are required and the NDC vaccine codes **SHOULD** be supported as translations to them.</t>
+  </si>
+  <si>
+    <t>* The US Core Location  and PractitionerRole Profiles are not explicitly referenced in any US Core Profile. However they **SHOULD** be used as the default profile if referenced by another US Core profile.</t>
+  </si>
+  <si>
+    <t>* The  MedicationRequest resource can represent a medication, using an external reference to a Medication resource. If an external Medication Resource is used in a MedicationRequest, then the READ  **SHALL**  be supported.</t>
+  </si>
+  <si>
+    <t>* The MedicationRequest resources can represent a medication using either a code or refer to the Medication resource. When referencing Medication, the resource may be [contained](http://hl7.org/fhir/R4/references.html#contained) or an external resource. The server application **MAY** choose any one way or more than one method, but if an external reference to Medication is used, the server **SHALL** support the _include` parameter for searching this element. The client application must support all methods.
  For example, A server **SHALL** be capable of returning all medications for a patient using one of or both:
  `GET /MedicationRequest?patient=[id]`
  `GET /MedicationRequest?patient=[id]&amp;_include=MedicationRequest:medication`
 * The MedicationRequest resource can represent that information is from a secondary source using either a boolean flag or reference in `MedicationRequest.reportedBoolean`, or a reference using `MedicationRequest.reportedReference` to Practitioner or other resource.
    *   Although both are marked as must support, the server systems are not required to support both a boolean and a reference, but **SHALL** choose to support at least one of these elements.
    *  The client application **SHALL** support both elements.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The MedicationStatement resources can represent a medication using either a code or refer to the Medication resource. When referencing Medication, the resource may be [contained](http://hl7.org/fhir/R4/references.html#contained) or an external resource. The server application **MAY** choose any one way or more than one method, but if an external reference to Medication is used, the server **SHALL** support the _include` parameter for searching this element. The client application must support all methods.
+ For example, A server **SHALL** be capable of returning all medications for a patient using one of or both:
+ `GET /MedicationStatement?patient=[id]`
+ `GET /MedicationStatement?patient=[id]&amp;_include=MedicationStatement:medication`
+</t>
+  </si>
+  <si>
+    <t>* Systems **SHOULD** support `Observation.effectivePeriod` to accurately represent laboratory tests that are collected over a period of time (for example, a 24-Hour Urine Collection test).
+* An Observation without a value, **SHALL** include a reason why the data is absent unless there are component observations, or references to other Observations that are grouped within it.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* For ONC's USCDI requirements, each Patient must support the following additional elements. These elements are included in the formal definition of the profile. The patient examples include all of these elements.
+1. contact detail (e.g. a telephone number or an email address)
+1. a communication language
+1. a race
+1. an ethnicity
+1. a birth sex*
+1. previous name
+   - Previous name is represented by providing an end date in the `Patient.name.period` element for a previous name.
+1. suffix
+   - Suffix is represented using the `Patient.name.suffix` element.
+</t>
+  </si>
+  <si>
+    <t>*  A procedure including an implantable device **SHOULD** use `Procedure.focalDevice` with a reference to the [US Core Implantable Device Profile].</t>
+  </si>
+  <si>
+    <t>* If a system receives a provider in `Provenance.agent.who` as free text they must capture who sent them the information as the organization. On request they **SHALL** provide this organization as the source and **MAY** include the free text provider.
+* Systems that need to know the activity has occurred **SHOULD** populate the activity.</t>
+  </si>
+  <si>
+    <t>*  Implantable medical devices that have UDI information **SHALL** represent this information in either `carrierAIDC` or `carrierHRF`.
+     - UDI may not be present in all scenarios such as historical implantable devices, patient reported implant information, payer reported devices, or improperly documented implants.
+     - Servers are not required to support both `carrierAIDC` and `carrierHR`.
+* For Implantable medical devices that have UDI information, at least one of the Production Identifiers (UDI-PI) **SHALL** be present.
+* Servers **SHOULD** support query by Device.type to allow clients to request the patient's devices by a specific type. Note: The Device.type is too granular to differentiate implantable vs. non-implantable devices.  
+* In the [Quick Start] section below, searching for all devices is described. Records of implanted devices **MAY** be queried against UDI data including:
+    - UDI HRF string (`udi-carrier`)
+    - UDI Device Identifier (`udi-di`)
+    - Manufacturer (`manufacturer`)
+    - Model number (`model`)
+* Implementers **MAY** also adopt custom SearchParameters for searching by:
+    - lot numbers
+    - serial number
+    - expiration date
+    - manufacture date
+    - distinct identifier</t>
   </si>
 </sst>
 </file>
@@ -2229,7 +2341,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2248,34 +2360,34 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>528</v>
+        <v>519</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>513</v>
+        <v>544</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2283,12 +2395,12 @@
         <v>70</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>61</v>
@@ -2296,10 +2408,10 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
     </row>
   </sheetData>
@@ -3257,7 +3369,7 @@
         <v>155</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="J34" s="5" t="s">
         <v>151</v>
@@ -3350,7 +3462,7 @@
         <v>346</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -3795,7 +3907,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>73</v>
@@ -3804,16 +3916,16 @@
         <v>111</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -3828,7 +3940,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>73</v>
@@ -3837,16 +3949,16 @@
         <v>111</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="H53" s="5" t="s">
         <v>194</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -3861,7 +3973,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>73</v>
@@ -3870,16 +3982,16 @@
         <v>111</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="H54" s="5" t="s">
         <v>194</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -3894,7 +4006,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>73</v>
@@ -3903,16 +4015,16 @@
         <v>229</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="H55" s="5" t="s">
         <v>244</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -3920,7 +4032,7 @@
         <v>73</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="C56" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3951,7 +4063,7 @@
         <v>74</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="C57" s="1" t="str">
         <f t="shared" si="2"/>
@@ -4089,13 +4201,13 @@
         <v>111</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="H61" s="5" t="s">
         <v>297</v>
       </c>
       <c r="I61" s="5" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="J61" s="5" t="s">
         <v>342</v>
@@ -4121,13 +4233,13 @@
         <v>111</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="H62" s="5" t="s">
         <v>233</v>
       </c>
       <c r="I62" s="5" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="J62" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B62&amp;" resources for the specified patient and a category code = `laboratory`"</f>
@@ -4184,13 +4296,13 @@
         <v>229</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="H64" s="5" t="s">
         <v>238</v>
       </c>
       <c r="I64" s="5" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="J64" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B64&amp;" resources for the specified patient and date and a category code = `laboratory`"</f>
@@ -4472,13 +4584,13 @@
         <v>111</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="H73" s="5" t="s">
         <v>296</v>
       </c>
       <c r="I73" s="5" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="J73" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B73&amp;" resources for the specified "&amp;SUBSTITUTE(D73,","," and ")</f>
@@ -4505,13 +4617,13 @@
         <v>111</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="H74" s="5" t="s">
         <v>295</v>
       </c>
       <c r="I74" s="5" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="J74" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B74&amp;" resources for the specified patient and a category code = `vital-signs`"</f>
@@ -4538,7 +4650,7 @@
         <v>111</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="H75" s="5" t="s">
         <v>298</v>
@@ -4571,13 +4683,13 @@
         <v>229</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="H76" s="5" t="s">
         <v>301</v>
       </c>
       <c r="I76" s="5" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="J76" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B76&amp;" resources for the specified patient and date and a category code = `vital-signs`"</f>
@@ -4809,7 +4921,7 @@
         <v>266</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>123</v>
@@ -4866,15 +4978,15 @@
         <v>69</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="1" customFormat="1">
       <c r="A3" s="1" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -4898,7 +5010,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -4955,10 +5067,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -4976,115 +5088,115 @@
       <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>358</v>
+        <v>76</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="C2" t="s">
+        <v>391</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
-        <v>262</v>
+      <c r="D2" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>525</v>
+        <v>250</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>360</v>
+        <v>383</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
-        <v>192</v>
+      <c r="D3" s="1" t="s">
+        <v>248</v>
       </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>462</v>
+        <v>358</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>461</v>
+        <v>359</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>361</v>
+        <v>370</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>362</v>
+        <v>371</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>284</v>
+        <v>143</v>
       </c>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>78</v>
+        <v>457</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>389</v>
+        <v>456</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>22</v>
+        <v>266</v>
       </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>363</v>
+        <v>197</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>364</v>
+        <v>388</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>292</v>
+        <v>198</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>365</v>
+        <v>380</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="F8" s="1"/>
     </row>
@@ -5105,106 +5217,106 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>369</v>
+        <v>390</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>189</v>
+        <v>23</v>
       </c>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>370</v>
+        <v>384</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>371</v>
+        <v>385</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>143</v>
+        <v>188</v>
       </c>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>390</v>
+        <v>364</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>23</v>
+        <v>167</v>
       </c>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>373</v>
+        <v>386</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>374</v>
+        <v>387</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>453</v>
+        <v>377</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>454</v>
+        <v>378</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>191</v>
+        <v>379</v>
       </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>377</v>
+        <v>517</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>378</v>
+        <v>360</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>379</v>
+        <v>192</v>
       </c>
       <c r="F16" s="1"/>
     </row>
@@ -5225,85 +5337,85 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>198</v>
+        <v>520</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>380</v>
+        <v>521</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
-        <v>381</v>
+        <v>522</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>382</v>
+        <v>523</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>286</v>
+        <v>191</v>
       </c>
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
-        <v>250</v>
+        <v>524</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>383</v>
+        <v>525</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>248</v>
+        <v>191</v>
       </c>
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
-        <v>384</v>
+        <v>526</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>385</v>
+        <v>527</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
-        <v>386</v>
+        <v>528</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>387</v>
+        <v>529</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>267</v>
+        <v>191</v>
       </c>
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
-        <v>455</v>
+        <v>530</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>456</v>
+        <v>531</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>12</v>
@@ -5314,11 +5426,11 @@
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" s="1" customFormat="1">
-      <c r="A24" s="11" t="s">
-        <v>468</v>
+      <c r="A24" s="1" t="s">
+        <v>532</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>469</v>
+        <v>533</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>12</v>
@@ -5329,58 +5441,184 @@
     </row>
     <row r="25" spans="1:6" s="1" customFormat="1">
       <c r="A25" s="1" t="s">
-        <v>197</v>
+        <v>534</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>388</v>
+        <v>535</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="1" customFormat="1">
       <c r="A26" s="1" t="s">
-        <v>76</v>
+        <v>536</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>391</v>
+        <v>537</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>21</v>
+        <v>191</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="1" customFormat="1">
       <c r="A27" s="1" t="s">
-        <v>470</v>
+        <v>538</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>471</v>
+        <v>539</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>472</v>
+        <v>191</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="1" customFormat="1">
       <c r="A28" s="1" t="s">
-        <v>523</v>
+        <v>540</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>524</v>
+        <v>541</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>191</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>467</v>
       </c>
     </row>
   </sheetData>
@@ -5398,14 +5636,14 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="17.25" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="36.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="25.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="54.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="49.7109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="8.140625" style="2" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" style="2" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" style="1" customWidth="1"/>
@@ -5432,7 +5670,7 @@
         <v>41</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>527</v>
+        <v>518</v>
       </c>
       <c r="F1" t="s">
         <v>15</v>
@@ -5513,7 +5751,7 @@
       <c r="T2"/>
       <c r="X2" s="17"/>
       <c r="Y2" s="17" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="Z2" t="s">
         <v>20</v>
@@ -5526,9 +5764,12 @@
       <c r="B3" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="C3" s="2" t="s">
+        <v>545</v>
+      </c>
       <c r="X3" s="17"/>
       <c r="Y3" s="17" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="17.25" customHeight="1">
@@ -5540,7 +5781,7 @@
       </c>
       <c r="X4" s="17"/>
       <c r="Y4" s="17" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="17.25" customHeight="1">
@@ -5552,7 +5793,7 @@
       </c>
       <c r="X5" s="17"/>
       <c r="Y5" s="17" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="Z5" t="s">
         <v>24</v>
@@ -5565,9 +5806,12 @@
       <c r="B6" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="C6" s="2" t="s">
+        <v>556</v>
+      </c>
       <c r="X6" s="17"/>
       <c r="Y6" s="17" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="17.25" customHeight="1">
@@ -5579,7 +5823,7 @@
       </c>
       <c r="X7" s="17"/>
       <c r="Y7" s="17" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="17.25" customHeight="1">
@@ -5594,7 +5838,7 @@
       </c>
       <c r="X8" s="17"/>
       <c r="Y8" s="17" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="17.25" customHeight="1">
@@ -5605,11 +5849,11 @@
         <v>73</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>529</v>
+        <v>546</v>
       </c>
       <c r="X9" s="17"/>
       <c r="Y9" s="17" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="17.25" customHeight="1">
@@ -5621,7 +5865,7 @@
       </c>
       <c r="X10" s="17"/>
       <c r="Y10" s="17" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="17.25" customHeight="1">
@@ -5631,9 +5875,12 @@
       <c r="B11" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="C11" s="2" t="s">
+        <v>547</v>
+      </c>
       <c r="X11" s="17"/>
       <c r="Y11" s="17" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="17.25" customHeight="1">
@@ -5643,6 +5890,9 @@
       <c r="B12" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="C12" s="2" t="s">
+        <v>548</v>
+      </c>
       <c r="X12" s="17"/>
       <c r="Y12" s="17"/>
     </row>
@@ -5654,7 +5904,7 @@
         <v>73</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>526</v>
+        <v>549</v>
       </c>
       <c r="X13" s="17"/>
       <c r="Y13" s="17"/>
@@ -5667,32 +5917,32 @@
         <v>73</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>530</v>
+        <v>550</v>
       </c>
       <c r="W14" s="7" t="s">
         <v>219</v>
       </c>
       <c r="X14" s="17"/>
       <c r="Y14" s="17" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="17.25" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>460</v>
+        <v>551</v>
       </c>
       <c r="W15" s="7" t="s">
         <v>423</v>
       </c>
       <c r="X15" s="17"/>
       <c r="Y15" s="17" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="17.25" customHeight="1">
@@ -5702,9 +5952,12 @@
       <c r="B16" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="C16" s="2" t="s">
+        <v>552</v>
+      </c>
       <c r="X16" s="17"/>
       <c r="Y16" s="17" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
     </row>
     <row r="17" spans="1:25" ht="17.25" customHeight="1">
@@ -5724,9 +5977,12 @@
       <c r="B18" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="C18" s="2" t="s">
+        <v>553</v>
+      </c>
       <c r="X18" s="17"/>
       <c r="Y18" s="17" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
     </row>
     <row r="19" spans="1:25" ht="17.25" customHeight="1">
@@ -5746,6 +6002,9 @@
       <c r="B20" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="C20" s="2" t="s">
+        <v>548</v>
+      </c>
       <c r="W20" s="1" t="s">
         <v>290</v>
       </c>
@@ -5759,25 +6018,30 @@
       <c r="B21" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="C21" s="2" t="s">
+        <v>554</v>
+      </c>
       <c r="X21" s="17"/>
       <c r="Y21" s="17" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="22" spans="1:25" s="1" customFormat="1" ht="15">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" s="1" customFormat="1" ht="120">
       <c r="A22" s="1" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C22" s="2"/>
+      <c r="C22" s="2" t="s">
+        <v>555</v>
+      </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:25" s="1" customFormat="1" ht="15">
       <c r="A23" s="1" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>73</v>
@@ -5857,24 +6121,24 @@
         <v>73</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="1" customFormat="1" ht="113.25" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>73</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -5924,7 +6188,7 @@
         <v>397</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>398</v>
@@ -5957,7 +6221,7 @@
         <v>407</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>408</v>
@@ -5975,10 +6239,10 @@
         <v>412</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -6001,7 +6265,7 @@
         <v>32</v>
       </c>
       <c r="G2" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
@@ -6622,12 +6886,12 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>32</v>
@@ -6636,7 +6900,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>32</v>
@@ -6645,7 +6909,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>32</v>
@@ -6654,7 +6918,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>32</v>
@@ -9573,7 +9837,7 @@
         <v>189</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>73</v>
@@ -9677,7 +9941,7 @@
         <v>189</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>73</v>
@@ -9779,7 +10043,7 @@
         <v>56</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>63</v>
@@ -9832,7 +10096,7 @@
         <v>57</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>94</v>
@@ -9890,7 +10154,7 @@
         <v>58</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>242</v>

</xml_diff>

<commit_message>
fix cap statement errors
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\US-Core-R4\input\resources_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E563653-E32C-4BBB-B3E5-24F934AA064F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2FCB426-90EB-4E0C-BF83-F5DD03AB89FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4980" yWindow="1170" windowWidth="38355" windowHeight="15795" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4635" yWindow="825" windowWidth="38355" windowHeight="15795" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -1758,19 +1758,10 @@
     <t>US Core Heart Rate Profile</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/pediatric-bmi-for-age-observation</t>
-  </si>
-  <si>
     <t>Pediatric BMI for Age Observation Profile</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/pediatric-head-occipital-frontal-circumference-percentile</t>
-  </si>
-  <si>
     <t>Pediatric Head Occipital-frontal Circumference Percentile Profile</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/pediatric-weight-for-height-observation</t>
   </si>
   <si>
     <t>Pediatric Weight for Height Observation Profile</t>
@@ -1866,6 +1857,15 @@
     - expiration date
     - manufacture date
     - distinct identifier</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/bmi-for-age-observation</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/head-occipital-frontal-circumference-percentile</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/weight-for-height-observation</t>
   </si>
 </sst>
 </file>
@@ -2371,7 +2371,7 @@
         <v>507</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -5069,8 +5069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A5" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -5455,10 +5455,10 @@
     </row>
     <row r="26" spans="1:6" s="1" customFormat="1">
       <c r="A26" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>536</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>537</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>12</v>
@@ -5469,10 +5469,10 @@
     </row>
     <row r="27" spans="1:6" s="1" customFormat="1">
       <c r="A27" s="1" t="s">
-        <v>538</v>
+        <v>555</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>12</v>
@@ -5483,10 +5483,10 @@
     </row>
     <row r="28" spans="1:6" s="1" customFormat="1">
       <c r="A28" s="1" t="s">
-        <v>540</v>
+        <v>556</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>12</v>
@@ -5511,10 +5511,10 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>12</v>
@@ -5632,7 +5632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Z59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -5765,7 +5765,7 @@
         <v>73</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="X3" s="17"/>
       <c r="Y3" s="17" t="s">
@@ -5807,7 +5807,7 @@
         <v>73</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="X6" s="17"/>
       <c r="Y6" s="17" t="s">
@@ -5849,7 +5849,7 @@
         <v>73</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="X9" s="17"/>
       <c r="Y9" s="17" t="s">
@@ -5876,7 +5876,7 @@
         <v>73</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="X11" s="17"/>
       <c r="Y11" s="17" t="s">
@@ -5891,7 +5891,7 @@
         <v>73</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="X12" s="17"/>
       <c r="Y12" s="17"/>
@@ -5904,7 +5904,7 @@
         <v>73</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="X13" s="17"/>
       <c r="Y13" s="17"/>
@@ -5917,7 +5917,7 @@
         <v>73</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="W14" s="7" t="s">
         <v>219</v>
@@ -5935,7 +5935,7 @@
         <v>73</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="W15" s="7" t="s">
         <v>423</v>
@@ -5953,7 +5953,7 @@
         <v>73</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="X16" s="17"/>
       <c r="Y16" s="17" t="s">
@@ -5978,7 +5978,7 @@
         <v>73</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="X18" s="17"/>
       <c r="Y18" s="17" t="s">
@@ -6003,7 +6003,7 @@
         <v>73</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="W20" s="1" t="s">
         <v>290</v>
@@ -6019,7 +6019,7 @@
         <v>73</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="X21" s="17"/>
       <c r="Y21" s="17" t="s">
@@ -6034,7 +6034,7 @@
         <v>73</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>

</xml_diff>

<commit_message>
fix qa errors in cap statements
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\US-Core-R4\input\resources_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E9428CA-B050-438B-BD95-CC897D1A898E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E1ED33-5A50-4FE6-A861-4119255B20FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4980" yWindow="1170" windowWidth="38355" windowHeight="15795" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4980" yWindow="1170" windowWidth="38355" windowHeight="15795" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -1755,15 +1755,6 @@
     <t>US Core Heart Rate Profile</t>
   </si>
   <si>
-    <t>Pediatric BMI for Age Observation Profile</t>
-  </si>
-  <si>
-    <t>Pediatric Head Occipital-frontal Circumference Percentile Profile</t>
-  </si>
-  <si>
-    <t>Pediatric Weight for Height Observation Profile</t>
-  </si>
-  <si>
     <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-respiratory-rate</t>
   </si>
   <si>
@@ -1856,16 +1847,25 @@
     - distinct identifier</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/bmi-for-age-observation</t>
-  </si>
-  <si>
     <t>http://hl7.org/fhir/us/core/StructureDefinition/head-occipital-frontal-circumference-percentile</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/weight-for-height-observation</t>
-  </si>
-  <si>
     <t>This Section describes the expected capabilities of the US Core Client which is responsible for creating and initiating the queries for information about an individual patient. The complete list of FHIR profiles, RESTful operations, and search parameters supported by US Core Servers are defined in the [Conformance Requirements for Server](CapabilityStatement-us-core-server.html). US Core Clients have the option of choosing from this list to access necessary data based on their local use cases and other contextual requirements.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/pediatric-bmi-for-age</t>
+  </si>
+  <si>
+    <t>US Core Pediatric BMI for Age Observation Profile</t>
+  </si>
+  <si>
+    <t>US Core Pediatric Head Occipital-frontal Circumference Percentile Profile</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/pediatric-weight-for-height</t>
+  </si>
+  <si>
+    <t>US Core Pediatric Weight for Height Observation Profile</t>
   </si>
 </sst>
 </file>
@@ -2371,7 +2371,7 @@
         <v>506</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -4955,7 +4955,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -5002,7 +5002,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -5069,8 +5069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A5" sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -5455,10 +5455,10 @@
     </row>
     <row r="26" spans="1:6" s="1" customFormat="1">
       <c r="A26" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>553</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>535</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>12</v>
@@ -5469,10 +5469,10 @@
     </row>
     <row r="27" spans="1:6" s="1" customFormat="1">
       <c r="A27" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>554</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>536</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>12</v>
@@ -5486,7 +5486,7 @@
         <v>555</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>537</v>
+        <v>556</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>12</v>
@@ -5511,10 +5511,10 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>12</v>
@@ -5765,7 +5765,7 @@
         <v>73</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="X3" s="17"/>
       <c r="Y3" s="17" t="s">
@@ -5807,7 +5807,7 @@
         <v>73</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="X6" s="17"/>
       <c r="Y6" s="17" t="s">
@@ -5849,7 +5849,7 @@
         <v>73</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="X9" s="17"/>
       <c r="Y9" s="17" t="s">
@@ -5876,7 +5876,7 @@
         <v>73</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="X11" s="17"/>
       <c r="Y11" s="17" t="s">
@@ -5891,7 +5891,7 @@
         <v>73</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="X12" s="17"/>
       <c r="Y12" s="17"/>
@@ -5904,7 +5904,7 @@
         <v>73</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="X13" s="17"/>
       <c r="Y13" s="17"/>
@@ -5917,7 +5917,7 @@
         <v>73</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="W14" s="7" t="s">
         <v>219</v>
@@ -5935,7 +5935,7 @@
         <v>73</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="W15" s="7" t="s">
         <v>423</v>
@@ -5953,7 +5953,7 @@
         <v>73</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="X16" s="17"/>
       <c r="Y16" s="17" t="s">
@@ -5978,7 +5978,7 @@
         <v>73</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="X18" s="17"/>
       <c r="Y18" s="17" t="s">
@@ -6003,7 +6003,7 @@
         <v>73</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="W20" s="1" t="s">
         <v>290</v>
@@ -6019,7 +6019,7 @@
         <v>73</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="X21" s="17"/>
       <c r="Y21" s="17" t="s">
@@ -6034,7 +6034,7 @@
         <v>73</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>

</xml_diff>

<commit_message>
updates to quickstarts FHIR-27905, FHIR-27906
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\US-Core-R4\input\resources_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B4ABAAB-7046-45D3-A805-D34F0A693EEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16DDBA53-D4B4-423A-B6D6-90B39D432A62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5325" yWindow="1515" windowWidth="38355" windowHeight="15795" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6705" yWindow="2700" windowWidth="38355" windowHeight="15795" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -145,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2047" uniqueCount="561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2047" uniqueCount="560">
   <si>
     <t>Element</t>
   </si>
@@ -657,9 +657,6 @@
     <t>GET [base]/Immunization?patient=1137192&amp;status=completed</t>
   </si>
   <si>
-    <t>GET [base]/Immunization?patient=1137192&amp;date=ge2019-01-14</t>
-  </si>
-  <si>
     <t>patient,date</t>
   </si>
   <si>
@@ -765,9 +762,6 @@
     <t>GET [base]/DiagnosticReport?patient=f201&amp;category=http://terminology.hl7.org/CodeSystem/v2-0074\|LAB</t>
   </si>
   <si>
-    <t>GET [base]/DiagnosticReport?patient=f201&amp;category=http://terminology.hl7.org/CodeSystem/v2-0074\|LAB&amp;date=ge2010-01-14</t>
-  </si>
-  <si>
     <t>GET [base]/DiagnosticReport?patient=1032702&amp;code=http://loinc.org\|24323-8</t>
   </si>
   <si>
@@ -786,9 +780,6 @@
     <t>GET [base]/DiagnosticReport?patient=f201&amp;category=http://loinc.org\|LP29684-5</t>
   </si>
   <si>
-    <t>GET [base]/DiagnosticReport?patient=f201&amp;category=http://loinc.org\|LP29684-5&amp;date=ge2010-01-14</t>
-  </si>
-  <si>
     <t>GET [base]/Procedure?patient=1137192&amp;status=completed</t>
   </si>
   <si>
@@ -843,15 +834,9 @@
     <t>support searching for reports by code and date</t>
   </si>
   <si>
-    <t>GET [base]/DiagnosticReport?patient=f201&amp;code=http://loinc.org\|24323-8&amp;date=ge2019-01-14</t>
-  </si>
-  <si>
     <t>support searching for all laboratory results</t>
   </si>
   <si>
-    <t>GET [base]Observation?patient=555580&amp;code=http://loinc.org\|2339-0&amp;date=ge2019</t>
-  </si>
-  <si>
     <t>support searching for all laboratory reports by code  (for example, search for all metabolic panel reports for a patient, or search for all cbcs, metabolic panels, and urinalysis panels for a patient)</t>
   </si>
   <si>
@@ -870,9 +855,6 @@
     <t xml:space="preserve">support searching for procedures for a patient by code and date </t>
   </si>
   <si>
-    <t>GET [base]/Procedure?patient=1137192&amp;date=ge2019-01-14&amp;code=http://snomed.info/sct\|35637008</t>
-  </si>
-  <si>
     <t>effective</t>
   </si>
   <si>
@@ -1047,9 +1029,6 @@
     <t>GET [base]/Observation?patient=1186747&amp;code=http://loinc.org\|8867-4,http://loinc.org\|9279-1,http://loinc.org\|85354-9</t>
   </si>
   <si>
-    <t>GET [base]/Observation?patient=1186747&amp;code=http://loinc.org\|8867-4,http://loinc.org\|9279-1,http://loinc.org\|85354-9&amp;date=ge2019</t>
-  </si>
-  <si>
     <t>support searching for all vital sign observations by date (for example, find all the vital sign observations for 2019)</t>
   </si>
   <si>
@@ -1089,9 +1068,6 @@
     <t>support searching for all clinical notes for a given patient</t>
   </si>
   <si>
-    <t>GET [base]/DocumentReference?patient=1235541&amp;category=http://hl7.org/fhir/us/core/CodeSystem/us-core-documentreference-category\|clinical-note&amp;date=ge2019</t>
-  </si>
-  <si>
     <t>support searching for all clinical notes for a given patient by date (for example, since 2019)</t>
   </si>
   <si>
@@ -1128,9 +1104,6 @@
     <t>GET [base]/Encounter?patient=example1&amp;class= http://terminology.hl7.org/CodeSystem/v3-ActCode code\|AMB</t>
   </si>
   <si>
-    <t>GET [base]/Encounter?patient=example1&amp;date=ge2019</t>
-  </si>
-  <si>
     <t>GET [base]/Encounter?patient=1137192&amp;type=http://www.ama-assn.org/go/cpt code\|99201</t>
   </si>
   <si>
@@ -1167,9 +1140,6 @@
     <t>should_include</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-vitalsigns</t>
-  </si>
-  <si>
     <t>!Observation</t>
   </si>
   <si>
@@ -1390,9 +1360,6 @@
   </si>
   <si>
     <t>support searching for a specific device type for a patient (for example, implantable devices)</t>
-  </si>
-  <si>
-    <t>GET [base]/DocumentReference?patient=2169591&amp;type=http://loinc.org \|34133-9&amp;period=ge2019</t>
   </si>
   <si>
     <t>GET [base]/DocumentReference?patient=1316024&amp;type=http://loinc.org\|18842-5</t>
@@ -1499,12 +1466,6 @@
     <t>GET [base]/MedicationStatement?patient=1137192&amp;date=ge2019~GET [base]/MedicationRequest?patient=1137192&amp;date=ge2019&amp;_include=MedicationStatement:medication</t>
   </si>
   <si>
-    <t>GET [base]/CarePlan?patient=1137192&amp;category=http://hl7.org/fhir/us/core/CodeSystem/careplan-category\|assess-plan&amp;date=ge2019~GET [base]/CarePlan?patient=1137192&amp;category=http://hl7.org/fhir/us/core/CodeSystem/careplan-category\|assess-plan&amp;date=ge2018&amp;date=le2018</t>
-  </si>
-  <si>
-    <t>GET [base]/CarePlan?patient=1137192&amp;category=http://hl7.org/fhir/us/core/CodeSystem/careplan-category\|assess-plan&amp;status=active&amp;date=ge2019~GET [base]/CarePlan?patient=1137192&amp;category=http://hl7.org/fhir/us/core/CodeSystem/careplan-category\|assess-plan&amp;status=active&amp;date=ge2018&amp;date=le2019</t>
-  </si>
-  <si>
     <t>A client **SHOULD** be capable of transacting a $docref operation and capable of receiving at least a reference to a generated CCD document, and  **MAY** be able to receive other document types, if available.   **SHOULD**  be capable of receiving documents as included resources in response to the operation.
 `GET [base]/DocumentReference/$docref?patient=[id]`</t>
   </si>
@@ -1581,9 +1542,6 @@
     <t>GET [base]/Observation?patient=1134281&amp;category=http://terminology.hl7.org/CodeSystem/observation-category\|laboratory</t>
   </si>
   <si>
-    <t>GET [base]Observation?patient=555580&amp;category=http://terminology.hl7.org/CodeSystem/observation-category\|laboratory&amp;date=ge2018-03-14</t>
-  </si>
-  <si>
     <t>category=http://terminology.hl7.org/CodeSystem/observation-category|vital-signs</t>
   </si>
   <si>
@@ -1593,9 +1551,6 @@
     <t>GET [base]/Observation?patient=1134281&amp;category=http://terminology.hl7.org/CodeSystem/observation-category\|vital-signs</t>
   </si>
   <si>
-    <t>GET [base]/Observation?patient=1134281&amp;category=http://terminology.hl7.org/CodeSystem/observation-category\|vital-signs&amp;date=ge2019</t>
-  </si>
-  <si>
     <t>intent</t>
   </si>
   <si>
@@ -1651,9 +1606,6 @@
   </si>
   <si>
     <t>Fetches a bundle of all MedicationRequest resources for the specified patient and intent  code = `order,plan` and encounter</t>
-  </si>
-  <si>
-    <t>GET [base]/MedicationRequest?patient=1137192&amp;intent=order,plan&amp;authoredon=ge2019~GET [base]/MedicationRequest?patient=1137192&amp;intent=order,plan&amp;authoredon=ge2019&amp;_include=MedicationRequest:medication</t>
   </si>
   <si>
     <t>Fetches a bundle of all MedicationRequest resources for the specified patient and intent  code = `order,plan` and authoredon date</t>
@@ -1882,6 +1834,51 @@
   <si>
     <t>A client **SHALL** provide a value precise to the *day*.
 A server **SHALL** support a value a value precise to the *day*.</t>
+  </si>
+  <si>
+    <t>GET [base]/Encounter?patient=example1&amp;date=ge2019-01-01T00:00:00Z</t>
+  </si>
+  <si>
+    <t>GET [base]/Immunization?patient=1137192&amp;date=ge2019-01-14T00:00:00Z</t>
+  </si>
+  <si>
+    <t>GET [base]/DiagnosticReport?patient=f201&amp;category=http://terminology.hl7.org/CodeSystem/v2-0074\|LAB&amp;date=ge2010-01-14T00:00:00Z</t>
+  </si>
+  <si>
+    <t>GET [base]/DiagnosticReport?patient=f201&amp;code=http://loinc.org\|24323-8&amp;date=ge2019-01-14T00:00:00Z</t>
+  </si>
+  <si>
+    <t>GET [base]/DiagnosticReport?patient=f201&amp;category=http://loinc.org\|LP29684-5&amp;date=ge2010-01-14T00:00:00Z</t>
+  </si>
+  <si>
+    <t>GET [base]/MedicationRequest?patient=1137192&amp;intent=order,plan&amp;authoredon=ge2019-01-01T00:00:00Z~GET [base]/MedicationRequest?patient=1137192&amp;intent=order,plan&amp;authoredon=ge2019-01-01T00:00:00Z&amp;_include=MedicationRequest:medication</t>
+  </si>
+  <si>
+    <t>GET [base]/Procedure?patient=1137192&amp;date=ge2019-01-14T00:00:00Z&amp;code=http://snomed.info/sct\|35637008</t>
+  </si>
+  <si>
+    <t>GET [base]Observation?patient=555580&amp;category=http://terminology.hl7.org/CodeSystem/observation-category\|laboratory&amp;date=ge2018-03-14T00:00:00Z</t>
+  </si>
+  <si>
+    <t>GET [base]Observation?patient=555580&amp;code=http://loinc.org\|2339-0&amp;date=ge2019-01-01T00:00:00Z</t>
+  </si>
+  <si>
+    <t>GET [base]/CarePlan?patient=1137192&amp;category=http://hl7.org/fhir/us/core/CodeSystem/careplan-category\|assess-plan&amp;date=ge2019-01-01T00:00:00Z~GET [base]/CarePlan?patient=1137192&amp;category=http://hl7.org/fhir/us/core/CodeSystem/careplan-category\|assess-plan&amp;date=ge2018-01-01T00:00:00Z&amp;date=le2019-01-01T00:00:00Z</t>
+  </si>
+  <si>
+    <t>GET [base]/CarePlan?patient=1137192&amp;category=http://hl7.org/fhir/us/core/CodeSystem/careplan-category\|assess-plan&amp;status=active&amp;date=ge2019-01-01T00:00:00Z~GET [base]/CarePlan?patient=1137192&amp;category=http://hl7.org/fhir/us/core/CodeSystem/careplan-category\|assess-plan&amp;status=active&amp;date=ge2018-01-01T00:00:00Z&amp;date=le2019-01-01T00:00:00Z</t>
+  </si>
+  <si>
+    <t>GET [base]/Observation?patient=1134281&amp;category=http://terminology.hl7.org/CodeSystem/observation-category\|vital-signs&amp;date=ge2020-01-01T00:00:00Z</t>
+  </si>
+  <si>
+    <t>GET [base]/Observation?patient=1186747&amp;code=http://loinc.org\|8867-4,http://loinc.org\|9279-1,http://loinc.org\|85354-9&amp;date=ge2020-01-01T00:00:00Z</t>
+  </si>
+  <si>
+    <t>GET [base]/DocumentReference?patient=1235541&amp;category=http://hl7.org/fhir/us/core/CodeSystem/us-core-documentreference-category\|clinical-note&amp;date=ge2020-01-01T00:00:00Z</t>
+  </si>
+  <si>
+    <t>GET [base]/DocumentReference?patient=2169591&amp;type=http://loinc.org \|34133-9&amp;period=ge2020-01-01T00:00:00Z</t>
   </si>
 </sst>
 </file>
@@ -2376,34 +2373,34 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>505</v>
+        <v>489</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>517</v>
+        <v>501</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>506</v>
+        <v>490</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>536</v>
+        <v>520</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>507</v>
+        <v>491</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>508</v>
+        <v>492</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>509</v>
+        <v>493</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>510</v>
+        <v>494</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2411,12 +2408,12 @@
         <v>70</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>511</v>
+        <v>495</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>512</v>
+        <v>496</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>61</v>
@@ -2424,10 +2421,10 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>513</v>
+        <v>497</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>514</v>
+        <v>498</v>
       </c>
     </row>
   </sheetData>
@@ -2439,8 +2436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:J84"/>
   <sheetViews>
-    <sheetView topLeftCell="I39" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J57" sqref="J57"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2453,7 +2450,7 @@
     <col min="6" max="6" width="21.42578125" style="1" customWidth="1"/>
     <col min="7" max="7" width="18.85546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="88.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="82.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="255.5703125" style="1" customWidth="1"/>
     <col min="10" max="10" width="83.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="8.85546875" style="1"/>
   </cols>
@@ -2478,7 +2475,7 @@
         <v>103</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>3</v>
@@ -2611,10 +2608,10 @@
         <v>111</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="J6" s="5" t="str">
         <f t="shared" si="1"/>
@@ -2796,10 +2793,10 @@
         <v>118</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>327</v>
+        <v>545</v>
       </c>
       <c r="J13" s="5" t="str">
         <f t="shared" si="1"/>
@@ -2877,10 +2874,10 @@
         <v>111</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="J16" s="5" t="str">
         <f t="shared" si="1"/>
@@ -2934,10 +2931,10 @@
         <v>111</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="J18" s="5" t="str">
         <f t="shared" si="1"/>
@@ -3225,10 +3222,10 @@
         <v>139</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J29" s="5" t="str">
         <f t="shared" si="1"/>
@@ -3256,10 +3253,10 @@
         <v>139</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J30" s="5" t="str">
         <f t="shared" si="1"/>
@@ -3287,10 +3284,10 @@
         <v>132</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J31" s="5" t="str">
         <f t="shared" si="1"/>
@@ -3318,10 +3315,10 @@
         <v>132</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J32" s="5" t="str">
         <f t="shared" si="1"/>
@@ -3349,16 +3346,16 @@
         <v>111</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>445</v>
+        <v>434</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>161</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -3385,7 +3382,7 @@
         <v>155</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>492</v>
+        <v>477</v>
       </c>
       <c r="J34" s="5" t="s">
         <v>151</v>
@@ -3415,7 +3412,7 @@
         <v>156</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="J35" s="5" t="s">
         <v>157</v>
@@ -3475,10 +3472,10 @@
         <v>168</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>484</v>
+        <v>469</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -3493,7 +3490,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-immunization</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>73</v>
@@ -3502,10 +3499,10 @@
         <v>118</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>170</v>
+        <v>546</v>
       </c>
       <c r="J38" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B38&amp;" resources for the specified "&amp;SUBSTITUTE(D38,","," and ")</f>
@@ -3533,7 +3530,7 @@
         <v>154</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="I39" s="5" t="s">
         <v>169</v>
@@ -3548,10 +3545,10 @@
         <v>49</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>121</v>
@@ -3563,10 +3560,10 @@
         <v>111</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J40" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B40&amp;" resources for the specified "&amp;SUBSTITUTE(D40,","," and ")</f>
@@ -3578,10 +3575,10 @@
         <v>50</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>150</v>
@@ -3593,13 +3590,13 @@
         <v>111</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I41" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J41" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B41&amp;" resources for the specified patient and  a category code = `LAB`"</f>
@@ -3611,10 +3608,10 @@
         <v>51</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>152</v>
@@ -3626,10 +3623,10 @@
         <v>111</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="I42" s="9" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="J42" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B42&amp;" resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes."</f>
@@ -3641,28 +3638,28 @@
         <v>52</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D43" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="H43" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="E43" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="H43" s="5" t="s">
-        <v>204</v>
-      </c>
       <c r="I43" s="9" t="s">
-        <v>206</v>
+        <v>547</v>
       </c>
       <c r="J43" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B43&amp;" resources for the specified patient and date and a category code = `LAB`"</f>
@@ -3674,25 +3671,25 @@
         <v>53</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>73</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>232</v>
+        <v>548</v>
       </c>
       <c r="J44" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B44&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
@@ -3704,10 +3701,10 @@
         <v>56</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>121</v>
@@ -3719,10 +3716,10 @@
         <v>111</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J45" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B45&amp;" resources for the specified "&amp;SUBSTITUTE(D45,","," and ")</f>
@@ -3734,10 +3731,10 @@
         <v>57</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>150</v>
@@ -3749,10 +3746,10 @@
         <v>111</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="J46" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B46&amp;" resources for the specified patient and  a category code specified in US Core DiagnosticReport Category Codes"</f>
@@ -3764,10 +3761,10 @@
         <v>58</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>152</v>
@@ -3779,10 +3776,10 @@
         <v>111</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="I47" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="J47" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B47&amp;" resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes."</f>
@@ -3794,25 +3791,25 @@
         <v>59</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>73</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="I48" s="5" t="s">
-        <v>213</v>
+        <v>549</v>
       </c>
       <c r="J48" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B48&amp;" resources for the specified patient and date and a category code specified in US Core DiagnosticReport Category Codes"</f>
@@ -3824,25 +3821,25 @@
         <v>60</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>73</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>232</v>
+        <v>548</v>
       </c>
       <c r="J49" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B49&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
@@ -3854,14 +3851,14 @@
         <v>63</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C50" s="1" t="str">
         <f t="shared" ref="C50:C60" si="2">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B50)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>73</v>
@@ -3870,10 +3867,10 @@
         <v>111</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I50" s="5" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="J50" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B50&amp;" resources for the specified "&amp;SUBSTITUTE(D50,","," and ")</f>
@@ -3885,14 +3882,14 @@
         <v>64</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C51" s="1" t="str">
         <f t="shared" si="2"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>446</v>
+        <v>435</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>73</v>
@@ -3901,10 +3898,10 @@
         <v>154</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>447</v>
+        <v>436</v>
       </c>
       <c r="J51" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B51&amp;" resources for the specified "&amp;SUBSTITUTE(D51,","," and ")</f>
@@ -3916,14 +3913,14 @@
         <v>67</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C52" s="1" t="str">
         <f t="shared" si="2"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>468</v>
+        <v>455</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>73</v>
@@ -3932,16 +3929,16 @@
         <v>111</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>494</v>
+        <v>479</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>469</v>
+        <v>456</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>496</v>
+        <v>481</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -3949,14 +3946,14 @@
         <v>68</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C53" s="1" t="str">
         <f t="shared" si="2"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>470</v>
+        <v>457</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>73</v>
@@ -3965,16 +3962,16 @@
         <v>111</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>494</v>
+        <v>479</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>497</v>
+        <v>482</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>498</v>
+        <v>483</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -3982,14 +3979,14 @@
         <v>69</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C54" s="1" t="str">
         <f t="shared" si="2"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>471</v>
+        <v>458</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>73</v>
@@ -3998,16 +3995,16 @@
         <v>111</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>494</v>
+        <v>479</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>499</v>
+        <v>484</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>500</v>
+        <v>485</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -4015,32 +4012,32 @@
         <v>70</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C55" s="1" t="str">
         <f t="shared" si="2"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>472</v>
+        <v>459</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>73</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>494</v>
+        <v>479</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>501</v>
+        <v>550</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>502</v>
+        <v>486</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -4048,7 +4045,7 @@
         <v>73</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>473</v>
+        <v>460</v>
       </c>
       <c r="C56" s="1" t="str">
         <f t="shared" si="2"/>
@@ -4064,10 +4061,10 @@
         <v>111</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>448</v>
+        <v>437</v>
       </c>
       <c r="J56" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B56&amp;" resources for the specified "&amp;SUBSTITUTE(D56,","," and ")</f>
@@ -4079,14 +4076,14 @@
         <v>74</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>473</v>
+        <v>460</v>
       </c>
       <c r="C57" s="1" t="str">
         <f t="shared" si="2"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationstatement</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>73</v>
@@ -4095,13 +4092,13 @@
         <v>154</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="I57" s="5" t="s">
-        <v>449</v>
+        <v>438</v>
       </c>
       <c r="J57" s="5" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -4109,7 +4106,7 @@
         <v>75</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C58" s="1" t="str">
         <f t="shared" si="2"/>
@@ -4125,10 +4122,10 @@
         <v>111</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="I58" s="5" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="J58" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B58&amp;" resources for the specified "&amp;SUBSTITUTE(D58,","," and ")</f>
@@ -4140,14 +4137,14 @@
         <v>76</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C59" s="1" t="str">
         <f t="shared" si="2"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>73</v>
@@ -4156,10 +4153,10 @@
         <v>111</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="I59" s="5" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="J59" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B59&amp;" resources for the specified "&amp;SUBSTITUTE(D59,","," and ")</f>
@@ -4171,26 +4168,26 @@
         <v>77</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C60" s="1" t="str">
         <f t="shared" si="2"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>73</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="I60" s="5" t="s">
-        <v>241</v>
+        <v>551</v>
       </c>
       <c r="J60" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B60&amp;" resources for the specified patient and date and procedure code(s).  SHOULD support search by multiple codes."</f>
@@ -4202,13 +4199,13 @@
         <v>80</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>439</v>
+        <v>428</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>73</v>
@@ -4217,16 +4214,16 @@
         <v>111</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>474</v>
+        <v>461</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="I61" s="5" t="s">
-        <v>475</v>
+        <v>462</v>
       </c>
       <c r="J61" s="5" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -4234,10 +4231,10 @@
         <v>81</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>439</v>
+        <v>428</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>150</v>
@@ -4249,13 +4246,13 @@
         <v>111</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>474</v>
+        <v>461</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="I62" s="5" t="s">
-        <v>476</v>
+        <v>463</v>
       </c>
       <c r="J62" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B62&amp;" resources for the specified patient and a category code = `laboratory`"</f>
@@ -4267,10 +4264,10 @@
         <v>82</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>439</v>
+        <v>428</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>152</v>
@@ -4282,10 +4279,10 @@
         <v>111</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="I63" s="5" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="J63" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B63&amp;" resources for the specified patient and observation code(s).  SHOULD support search by multiple report codes. The Observation `code` parameter searches `Observation.code only."</f>
@@ -4297,28 +4294,28 @@
         <v>83</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>439</v>
+        <v>428</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>73</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>474</v>
+        <v>461</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="I64" s="5" t="s">
-        <v>477</v>
+        <v>552</v>
       </c>
       <c r="J64" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B64&amp;" resources for the specified patient and date and a category code = `laboratory`"</f>
@@ -4330,25 +4327,25 @@
         <v>84</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>439</v>
+        <v>428</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>73</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="I65" s="5" t="s">
-        <v>234</v>
+        <v>553</v>
       </c>
       <c r="J65" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B65&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
@@ -4360,10 +4357,10 @@
         <v>85</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>439</v>
+        <v>428</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>121</v>
@@ -4375,10 +4372,10 @@
         <v>111</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="I66" s="5" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="J66" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B66&amp;" resources for the specified "&amp;SUBSTITUTE(D66,","," and ")</f>
@@ -4390,10 +4387,10 @@
         <v>88</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>150</v>
@@ -4405,13 +4402,13 @@
         <v>111</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="I67" s="5" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="J67" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B67&amp;" resources for the specified "&amp;SUBSTITUTE(D67,","," and ")&amp;"=`assess-plan`"</f>
@@ -4423,31 +4420,31 @@
         <v>89</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>73</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="H68" s="5" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="I68" s="5" t="s">
-        <v>450</v>
+        <v>554</v>
       </c>
       <c r="J68" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -4455,13 +4452,13 @@
         <v>90</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>73</v>
@@ -4470,16 +4467,16 @@
         <v>111</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="H69" s="5" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="I69" s="5" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="J69" s="5" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -4487,31 +4484,31 @@
         <v>91</v>
       </c>
       <c r="B70" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C70" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="H70" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="C70" s="11" t="s">
-        <v>250</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="G70" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="H70" s="5" t="s">
-        <v>254</v>
-      </c>
       <c r="I70" s="5" t="s">
-        <v>451</v>
+        <v>555</v>
       </c>
       <c r="J70" s="5" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -4519,7 +4516,7 @@
         <v>94</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="C71" s="1" t="str">
         <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B71)</f>
@@ -4535,16 +4532,16 @@
         <v>111</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="I71" s="5" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="J71" s="5" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="15.75">
@@ -4552,10 +4549,10 @@
         <v>97</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C72" s="10" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>152</v>
@@ -4567,13 +4564,13 @@
         <v>111</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="I72" s="5" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="J72" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B72&amp;" resources for the specified patient and observation code."</f>
@@ -4585,13 +4582,13 @@
         <v>100</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>340</v>
+        <v>502</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>73</v>
@@ -4600,13 +4597,13 @@
         <v>111</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>478</v>
+        <v>464</v>
       </c>
       <c r="H73" s="5" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="I73" s="5" t="s">
-        <v>479</v>
+        <v>465</v>
       </c>
       <c r="J73" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B73&amp;" resources for the specified "&amp;SUBSTITUTE(D73,","," and ")</f>
@@ -4618,10 +4615,10 @@
         <v>101</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>340</v>
+        <v>502</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>150</v>
@@ -4633,13 +4630,13 @@
         <v>111</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>478</v>
+        <v>464</v>
       </c>
       <c r="H74" s="5" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="I74" s="5" t="s">
-        <v>480</v>
+        <v>466</v>
       </c>
       <c r="J74" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B74&amp;" resources for the specified patient and a category code = `vital-signs`"</f>
@@ -4651,10 +4648,10 @@
         <v>102</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>340</v>
+        <v>502</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>152</v>
@@ -4666,13 +4663,13 @@
         <v>111</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>478</v>
+        <v>464</v>
       </c>
       <c r="H75" s="5" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="I75" s="5" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="J75" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B75&amp;" resources for the specified patient and observation code(s).  SHOULD support search by multiple codes. The Observation `code` parameter searches `Observation.code only."</f>
@@ -4684,28 +4681,28 @@
         <v>103</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>340</v>
+        <v>502</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>73</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>478</v>
+        <v>464</v>
       </c>
       <c r="H76" s="5" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="I76" s="5" t="s">
-        <v>481</v>
+        <v>556</v>
       </c>
       <c r="J76" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B76&amp;" resources for the specified patient and date and a category code = `vital-signs`"</f>
@@ -4717,25 +4714,25 @@
         <v>104</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>340</v>
+        <v>502</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>73</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="H77" s="5" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="I77" s="5" t="s">
-        <v>300</v>
+        <v>557</v>
       </c>
       <c r="J77" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B77&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple codes."</f>
@@ -4747,7 +4744,7 @@
         <v>107</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C78" s="1" t="str">
         <f t="shared" ref="C78:C83" si="3">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B78)</f>
@@ -4763,10 +4760,10 @@
         <v>111</v>
       </c>
       <c r="H78" s="5" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="I78" s="5" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="J78" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B78&amp;" resources for the specified "&amp;SUBSTITUTE(D78,","," and ") &amp;". See the implementation notes above for how to access the actual document."</f>
@@ -4778,14 +4775,14 @@
         <v>108</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="C79" s="1" t="str">
         <f t="shared" si="3"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!documentreference</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>73</v>
@@ -4794,7 +4791,7 @@
         <v>154</v>
       </c>
       <c r="H79" s="5" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="I79" s="5"/>
       <c r="J79" s="5" t="str">
@@ -4807,7 +4804,7 @@
         <v>109</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C80" s="1" t="str">
         <f t="shared" si="3"/>
@@ -4823,16 +4820,16 @@
         <v>111</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="H80" s="5" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="I80" s="5" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="J80" s="5" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
     </row>
     <row r="81" spans="1:10" ht="20.25" customHeight="1">
@@ -4840,32 +4837,32 @@
         <v>110</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C81" s="1" t="str">
         <f t="shared" si="3"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>73</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="H81" s="5" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="I81" s="9" t="s">
-        <v>314</v>
+        <v>558</v>
       </c>
       <c r="J81" s="5" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
     </row>
     <row r="82" spans="1:10">
@@ -4873,7 +4870,7 @@
         <v>111</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C82" s="1" t="str">
         <f t="shared" si="3"/>
@@ -4889,13 +4886,13 @@
         <v>111</v>
       </c>
       <c r="H82" s="5" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="I82" s="5" t="s">
-        <v>416</v>
+        <v>405</v>
       </c>
       <c r="J82" s="5" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
     </row>
     <row r="83" spans="1:10" ht="20.25" customHeight="1">
@@ -4903,26 +4900,26 @@
         <v>112</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C83" s="1" t="str">
         <f t="shared" si="3"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>73</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="H83" s="5" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="I83" s="5" t="s">
-        <v>415</v>
+        <v>559</v>
       </c>
       <c r="J83" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B83&amp;" resources for the specified "&amp;SUBSTITUTE(D83,","," and ") &amp;". See the implementation notes above for how to access the actual document."</f>
@@ -4934,10 +4931,10 @@
         <v>115</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>456</v>
+        <v>443</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>123</v>
@@ -4949,13 +4946,13 @@
         <v>111</v>
       </c>
       <c r="H84" s="5" t="s">
-        <v>414</v>
+        <v>404</v>
       </c>
       <c r="I84" s="5" t="s">
-        <v>417</v>
+        <v>406</v>
       </c>
       <c r="J84" s="5" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
     </row>
   </sheetData>
@@ -4994,15 +4991,15 @@
         <v>69</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>504</v>
+        <v>488</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="1" customFormat="1">
       <c r="A3" s="1" t="s">
-        <v>493</v>
+        <v>478</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>503</v>
+        <v>487</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -5010,7 +5007,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>436</v>
+        <v>425</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="105" customHeight="1">
@@ -5018,7 +5015,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>550</v>
+        <v>534</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -5026,7 +5023,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>556</v>
+        <v>540</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -5034,7 +5031,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>434</v>
+        <v>423</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="141" customHeight="1">
@@ -5042,7 +5039,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>435</v>
+        <v>424</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="103.5" customHeight="1">
@@ -5050,7 +5047,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>438</v>
+        <v>427</v>
       </c>
     </row>
   </sheetData>
@@ -5116,7 +5113,7 @@
         <v>76</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>12</v>
@@ -5128,40 +5125,40 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>12</v>
@@ -5173,70 +5170,70 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>456</v>
+        <v>443</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>455</v>
+        <v>442</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>12</v>
@@ -5248,25 +5245,25 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>384</v>
+        <v>374</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>12</v>
@@ -5278,293 +5275,293 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>515</v>
+        <v>499</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>439</v>
+        <v>428</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>440</v>
+        <v>429</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>518</v>
+        <v>502</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>519</v>
+        <v>503</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
-        <v>520</v>
+        <v>504</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>521</v>
+        <v>505</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
-        <v>522</v>
+        <v>506</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>523</v>
+        <v>507</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
-        <v>524</v>
+        <v>508</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>525</v>
+        <v>509</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
-        <v>526</v>
+        <v>510</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>527</v>
+        <v>511</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
-        <v>528</v>
+        <v>512</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>529</v>
+        <v>513</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" s="1" customFormat="1">
       <c r="A24" s="1" t="s">
-        <v>530</v>
+        <v>514</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>531</v>
+        <v>515</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="1" customFormat="1">
       <c r="A25" s="1" t="s">
-        <v>532</v>
+        <v>516</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>533</v>
+        <v>517</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="1" customFormat="1">
       <c r="A26" s="1" t="s">
-        <v>551</v>
+        <v>535</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>552</v>
+        <v>536</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="1" customFormat="1">
       <c r="A27" s="1" t="s">
-        <v>549</v>
+        <v>533</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>553</v>
+        <v>537</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="1" customFormat="1">
       <c r="A28" s="1" t="s">
-        <v>554</v>
+        <v>538</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>555</v>
+        <v>539</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1" t="s">
-        <v>462</v>
+        <v>449</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>463</v>
+        <v>450</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
-        <v>534</v>
+        <v>518</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>535</v>
+        <v>519</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="1" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="1" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -5572,7 +5569,7 @@
         <v>78</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>12</v>
@@ -5583,58 +5580,58 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="1" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="1" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="1" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="1" t="s">
-        <v>464</v>
+        <v>451</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>465</v>
+        <v>452</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>466</v>
+        <v>453</v>
       </c>
     </row>
   </sheetData>
@@ -5686,67 +5683,67 @@
         <v>41</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>516</v>
+        <v>500</v>
       </c>
       <c r="F1" t="s">
         <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>426</v>
+        <v>415</v>
       </c>
       <c r="H1" t="s">
         <v>16</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>427</v>
+        <v>416</v>
       </c>
       <c r="J1" t="s">
         <v>17</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>431</v>
-      </c>
       <c r="R1" s="1" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>432</v>
+        <v>421</v>
       </c>
       <c r="T1" t="s">
         <v>18</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>433</v>
+        <v>422</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="W1" s="4" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="X1" s="4" t="s">
-        <v>421</v>
+        <v>410</v>
       </c>
       <c r="Y1" s="4" t="s">
-        <v>422</v>
+        <v>411</v>
       </c>
       <c r="Z1" t="s">
         <v>19</v>
@@ -5767,7 +5764,7 @@
       <c r="T2"/>
       <c r="X2" s="17"/>
       <c r="Y2" s="17" t="s">
-        <v>490</v>
+        <v>475</v>
       </c>
       <c r="Z2" t="s">
         <v>20</v>
@@ -5775,29 +5772,29 @@
     </row>
     <row r="3" spans="1:26" ht="17.25" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>537</v>
+        <v>521</v>
       </c>
       <c r="X3" s="17"/>
       <c r="Y3" s="17" t="s">
-        <v>490</v>
+        <v>475</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="17.25" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>73</v>
       </c>
       <c r="X4" s="17"/>
       <c r="Y4" s="17" t="s">
-        <v>490</v>
+        <v>475</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="17.25" customHeight="1">
@@ -5809,7 +5806,7 @@
       </c>
       <c r="X5" s="17"/>
       <c r="Y5" s="17" t="s">
-        <v>490</v>
+        <v>475</v>
       </c>
       <c r="Z5" t="s">
         <v>24</v>
@@ -5817,44 +5814,44 @@
     </row>
     <row r="6" spans="1:26" ht="17.25" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>548</v>
+        <v>532</v>
       </c>
       <c r="X6" s="17"/>
       <c r="Y6" s="17" t="s">
-        <v>490</v>
+        <v>475</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="17.25" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>73</v>
       </c>
       <c r="X7" s="17"/>
       <c r="Y7" s="17" t="s">
-        <v>490</v>
+        <v>475</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="17.25" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>437</v>
+        <v>426</v>
       </c>
       <c r="X8" s="17"/>
       <c r="Y8" s="17" t="s">
-        <v>490</v>
+        <v>475</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="17.25" customHeight="1">
@@ -5865,23 +5862,23 @@
         <v>73</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>538</v>
+        <v>522</v>
       </c>
       <c r="X9" s="17"/>
       <c r="Y9" s="17" t="s">
-        <v>490</v>
+        <v>475</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="17.25" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>73</v>
       </c>
       <c r="X10" s="17"/>
       <c r="Y10" s="17" t="s">
-        <v>490</v>
+        <v>475</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="17.25" customHeight="1">
@@ -5892,93 +5889,93 @@
         <v>73</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>539</v>
+        <v>523</v>
       </c>
       <c r="X11" s="17"/>
       <c r="Y11" s="17" t="s">
-        <v>490</v>
+        <v>475</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="17.25" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>540</v>
+        <v>524</v>
       </c>
       <c r="X12" s="17"/>
       <c r="Y12" s="17"/>
     </row>
     <row r="13" spans="1:26" ht="17.25" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>541</v>
+        <v>525</v>
       </c>
       <c r="X13" s="17"/>
       <c r="Y13" s="17"/>
     </row>
     <row r="14" spans="1:26" ht="17.25" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>542</v>
+        <v>526</v>
       </c>
       <c r="W14" s="7" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="X14" s="17"/>
       <c r="Y14" s="17" t="s">
-        <v>490</v>
+        <v>475</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="17.25" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>473</v>
+        <v>460</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>543</v>
+        <v>527</v>
       </c>
       <c r="W15" s="7" t="s">
-        <v>423</v>
+        <v>412</v>
       </c>
       <c r="X15" s="17"/>
       <c r="Y15" s="17" t="s">
-        <v>490</v>
+        <v>475</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="17.25" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>544</v>
+        <v>528</v>
       </c>
       <c r="X16" s="17"/>
       <c r="Y16" s="17" t="s">
-        <v>490</v>
+        <v>475</v>
       </c>
     </row>
     <row r="17" spans="1:25" ht="17.25" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>73</v>
@@ -5994,16 +5991,16 @@
         <v>73</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>545</v>
+        <v>529</v>
       </c>
       <c r="X18" s="17"/>
       <c r="Y18" s="17" t="s">
-        <v>490</v>
+        <v>475</v>
       </c>
     </row>
     <row r="19" spans="1:25" ht="17.25" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>73</v>
@@ -6013,51 +6010,51 @@
     </row>
     <row r="20" spans="1:25" ht="17.25" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>540</v>
+        <v>524</v>
       </c>
       <c r="W20" s="1" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="X20" s="17"/>
       <c r="Y20" s="17"/>
     </row>
     <row r="21" spans="1:25" ht="17.25" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>546</v>
+        <v>530</v>
       </c>
       <c r="X21" s="17"/>
       <c r="Y21" s="17" t="s">
-        <v>490</v>
+        <v>475</v>
       </c>
     </row>
     <row r="22" spans="1:25" s="1" customFormat="1" ht="120">
       <c r="A22" s="1" t="s">
-        <v>466</v>
+        <v>453</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>547</v>
+        <v>531</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:25" s="1" customFormat="1" ht="15">
       <c r="A23" s="1" t="s">
-        <v>485</v>
+        <v>470</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>73</v>
@@ -6125,36 +6122,36 @@
     </row>
     <row r="2" spans="1:5" ht="90.75" thickBot="1">
       <c r="A2" s="15" t="s">
-        <v>392</v>
+        <v>382</v>
       </c>
       <c r="B2" t="s">
-        <v>413</v>
+        <v>403</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D2" t="s">
         <v>73</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>452</v>
+        <v>439</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="1" customFormat="1" ht="113.25" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>487</v>
+        <v>472</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>488</v>
+        <v>473</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>485</v>
+        <v>470</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>73</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>486</v>
+        <v>471</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -6189,76 +6186,76 @@
         <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>397</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>453</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="W1" t="s">
         <v>402</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>403</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>491</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="W1" t="s">
-        <v>412</v>
-      </c>
       <c r="X1" s="1" t="s">
-        <v>467</v>
+        <v>454</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>489</v>
+        <v>474</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -6281,7 +6278,7 @@
         <v>32</v>
       </c>
       <c r="G2" t="s">
-        <v>454</v>
+        <v>441</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
@@ -6902,12 +6899,12 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>457</v>
+        <v>444</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>458</v>
+        <v>445</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>32</v>
@@ -6916,7 +6913,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>459</v>
+        <v>446</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>32</v>
@@ -6925,7 +6922,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>460</v>
+        <v>447</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>32</v>
@@ -6934,7 +6931,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>461</v>
+        <v>448</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>32</v>
@@ -6950,7 +6947,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AC94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="7" ySplit="1" topLeftCell="H90" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -7036,28 +7033,28 @@
         <v>48</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>441</v>
+        <v>430</v>
       </c>
       <c r="Q1" s="4" t="s">
         <v>49</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>442</v>
+        <v>431</v>
       </c>
       <c r="S1" s="4" t="s">
         <v>50</v>
       </c>
       <c r="T1" s="4" t="s">
-        <v>443</v>
+        <v>432</v>
       </c>
       <c r="U1" s="4" t="s">
         <v>51</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="W1" s="4" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="X1" s="4" t="s">
         <v>52</v>
@@ -7075,7 +7072,7 @@
         <v>55</v>
       </c>
       <c r="AC1" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="45.75" customHeight="1" thickTop="1">
@@ -7083,7 +7080,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>145</v>
@@ -7133,7 +7130,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>28</v>
@@ -7180,7 +7177,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>83</v>
@@ -7234,7 +7231,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>94</v>
@@ -7246,7 +7243,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>557</v>
+        <v>541</v>
       </c>
       <c r="G5" s="1" t="str">
         <f t="shared" si="1"/>
@@ -7296,7 +7293,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>63</v>
@@ -7381,7 +7378,7 @@
         <v>57</v>
       </c>
       <c r="Z7" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="AA7" s="5" t="s">
         <v>91</v>
@@ -7432,7 +7429,7 @@
         <v>57</v>
       </c>
       <c r="Z8" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="AA8" s="1" t="s">
         <v>93</v>
@@ -7460,7 +7457,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>558</v>
+        <v>542</v>
       </c>
       <c r="G9" s="1" t="str">
         <f t="shared" si="1"/>
@@ -7509,7 +7506,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>557</v>
+        <v>541</v>
       </c>
       <c r="G10" s="1" t="str">
         <f t="shared" si="1"/>
@@ -7567,7 +7564,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>558</v>
+        <v>542</v>
       </c>
       <c r="G11" s="1" t="str">
         <f t="shared" si="1"/>
@@ -7620,7 +7617,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>558</v>
+        <v>542</v>
       </c>
       <c r="G12" s="1" t="str">
         <f t="shared" si="1"/>
@@ -7671,7 +7668,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>557</v>
+        <v>541</v>
       </c>
       <c r="G13" s="1" t="str">
         <f t="shared" si="1"/>
@@ -7755,13 +7752,13 @@
         <v>57</v>
       </c>
       <c r="Z14" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AA14" s="5" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="AB14" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AC14" s="1" t="str">
         <f t="shared" si="5"/>
@@ -7785,7 +7782,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>558</v>
+        <v>542</v>
       </c>
       <c r="G15" s="1" t="str">
         <f t="shared" si="1"/>
@@ -7838,7 +7835,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>559</v>
+        <v>543</v>
       </c>
       <c r="G16" s="1" t="str">
         <f t="shared" si="1"/>
@@ -7895,7 +7892,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>558</v>
+        <v>542</v>
       </c>
       <c r="G17" s="1" t="str">
         <f t="shared" si="1"/>
@@ -7921,7 +7918,7 @@
         <v>57</v>
       </c>
       <c r="Z17" s="5" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="AA17" s="1" t="s">
         <v>166</v>
@@ -7952,7 +7949,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>557</v>
+        <v>541</v>
       </c>
       <c r="G18" s="1" t="str">
         <f t="shared" si="1"/>
@@ -8013,7 +8010,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>558</v>
+        <v>542</v>
       </c>
       <c r="G19" s="1" t="str">
         <f t="shared" si="1"/>
@@ -8066,7 +8063,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>558</v>
+        <v>542</v>
       </c>
       <c r="G20" s="1" t="str">
         <f t="shared" si="1"/>
@@ -8142,7 +8139,7 @@
         <v>79</v>
       </c>
       <c r="AA21" s="5" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="AC21" s="1" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B21)&amp;"-"&amp;SUBSTITUTE(C21,"_","")&amp;".html")</f>
@@ -8166,7 +8163,7 @@
         <v>0</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>560</v>
+        <v>544</v>
       </c>
       <c r="G22" s="1" t="str">
         <f t="shared" si="1"/>
@@ -8259,7 +8256,7 @@
         <v>0</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>558</v>
+        <v>542</v>
       </c>
       <c r="G24" s="1" t="str">
         <f t="shared" si="1"/>
@@ -8354,7 +8351,7 @@
         <v>1</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>558</v>
+        <v>542</v>
       </c>
       <c r="G26" s="1" t="str">
         <f t="shared" si="1"/>
@@ -8380,7 +8377,7 @@
         <v>57</v>
       </c>
       <c r="Z26" s="5" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="AA26" s="1" t="s">
         <v>165</v>
@@ -8437,10 +8434,10 @@
         <v>81</v>
       </c>
       <c r="Z27" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA27" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="AA27" s="1" t="s">
-        <v>181</v>
       </c>
       <c r="AB27" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B27&amp;" resources matching the name"</f>
@@ -8799,7 +8796,7 @@
         <v>0</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>559</v>
+        <v>543</v>
       </c>
       <c r="G35" s="1" t="str">
         <f t="shared" si="1"/>
@@ -8853,7 +8850,7 @@
         <v>0</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>558</v>
+        <v>542</v>
       </c>
       <c r="G36" s="1" t="str">
         <f t="shared" si="1"/>
@@ -8903,7 +8900,7 @@
         <v>1</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>557</v>
+        <v>541</v>
       </c>
       <c r="G37" s="1" t="str">
         <f t="shared" si="1"/>
@@ -8965,7 +8962,7 @@
         <v>0</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>558</v>
+        <v>542</v>
       </c>
       <c r="G38" s="1" t="str">
         <f t="shared" si="1"/>
@@ -9018,7 +9015,7 @@
         <v>0</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>559</v>
+        <v>543</v>
       </c>
       <c r="G39" s="1" t="str">
         <f t="shared" si="1"/>
@@ -9063,7 +9060,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>56</v>
@@ -9098,13 +9095,13 @@
         <v>57</v>
       </c>
       <c r="Z40" s="5" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="AA40" s="5" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="AB40" s="2" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="AC40" s="1" t="str">
         <f t="shared" si="4"/>
@@ -9116,7 +9113,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>63</v>
@@ -9128,7 +9125,7 @@
         <v>0</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>558</v>
+        <v>542</v>
       </c>
       <c r="G41" s="1" t="str">
         <f t="shared" si="1"/>
@@ -9172,7 +9169,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>94</v>
@@ -9184,7 +9181,7 @@
         <v>1</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>557</v>
+        <v>541</v>
       </c>
       <c r="G42" s="1" t="str">
         <f t="shared" si="1"/>
@@ -9234,7 +9231,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>145</v>
@@ -9246,7 +9243,7 @@
         <v>0</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>558</v>
+        <v>542</v>
       </c>
       <c r="G43" s="1" t="str">
         <f t="shared" si="1"/>
@@ -9287,7 +9284,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>13</v>
@@ -9299,7 +9296,7 @@
         <v>0</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>558</v>
+        <v>542</v>
       </c>
       <c r="G44" s="1" t="str">
         <f t="shared" si="1"/>
@@ -9337,7 +9334,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>83</v>
@@ -9349,7 +9346,7 @@
         <v>0</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>559</v>
+        <v>543</v>
       </c>
       <c r="G45" s="1" t="str">
         <f t="shared" si="1"/>
@@ -9394,10 +9391,10 @@
         <v>44</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>73</v>
@@ -9406,7 +9403,7 @@
         <v>0</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>559</v>
+        <v>543</v>
       </c>
       <c r="G46" s="1" t="str">
         <f t="shared" si="1"/>
@@ -9422,7 +9419,7 @@
         <v>83</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="L46" s="1" t="s">
         <v>57</v>
@@ -9450,7 +9447,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>63</v>
@@ -9462,7 +9459,7 @@
         <v>0</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>558</v>
+        <v>542</v>
       </c>
       <c r="G47" s="1" t="str">
         <f t="shared" si="1"/>
@@ -9506,7 +9503,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>94</v>
@@ -9518,7 +9515,7 @@
         <v>1</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>557</v>
+        <v>541</v>
       </c>
       <c r="G48" s="1" t="str">
         <f t="shared" si="1"/>
@@ -9568,7 +9565,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>145</v>
@@ -9580,7 +9577,7 @@
         <v>0</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>558</v>
+        <v>542</v>
       </c>
       <c r="G49" s="1" t="str">
         <f t="shared" si="1"/>
@@ -9621,7 +9618,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>28</v>
@@ -9633,7 +9630,7 @@
         <v>0</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>558</v>
+        <v>542</v>
       </c>
       <c r="G50" s="1" t="str">
         <f t="shared" si="1"/>
@@ -9674,7 +9671,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>83</v>
@@ -9686,7 +9683,7 @@
         <v>0</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>559</v>
+        <v>543</v>
       </c>
       <c r="G51" s="1" t="str">
         <f t="shared" si="1"/>
@@ -9731,10 +9728,10 @@
         <v>50</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>73</v>
@@ -9743,7 +9740,7 @@
         <v>0</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>558</v>
+        <v>542</v>
       </c>
       <c r="G52" s="1" t="str">
         <f t="shared" si="1"/>
@@ -9784,7 +9781,7 @@
         <v>51</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>94</v>
@@ -9796,7 +9793,7 @@
         <v>1</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>557</v>
+        <v>541</v>
       </c>
       <c r="G53" s="1" t="str">
         <f t="shared" si="1"/>
@@ -9846,10 +9843,10 @@
         <v>52</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>444</v>
+        <v>433</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>73</v>
@@ -9858,7 +9855,7 @@
         <v>0</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>560</v>
+        <v>544</v>
       </c>
       <c r="G54" s="1" t="str">
         <f t="shared" si="1"/>
@@ -9903,7 +9900,7 @@
         <v>53</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>63</v>
@@ -9915,7 +9912,7 @@
         <v>0</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>558</v>
+        <v>542</v>
       </c>
       <c r="G55" s="1" t="str">
         <f t="shared" si="1"/>
@@ -9959,10 +9956,10 @@
         <v>53</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>482</v>
+        <v>467</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>73</v>
@@ -9971,7 +9968,7 @@
         <v>0</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>558</v>
+        <v>542</v>
       </c>
       <c r="G56" s="1" t="str">
         <f t="shared" si="1"/>
@@ -10015,7 +10012,7 @@
         <v>54</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>94</v>
@@ -10027,7 +10024,7 @@
         <v>0</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>557</v>
+        <v>541</v>
       </c>
       <c r="G57" s="1" t="str">
         <f t="shared" si="1"/>
@@ -10069,10 +10066,10 @@
         <v>54</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>483</v>
+        <v>468</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>73</v>
@@ -10081,7 +10078,7 @@
         <v>0</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>557</v>
+        <v>541</v>
       </c>
       <c r="G58" s="1" t="str">
         <f t="shared" si="1"/>
@@ -10123,10 +10120,10 @@
         <v>55</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>73</v>
@@ -10135,7 +10132,7 @@
         <v>0</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>559</v>
+        <v>543</v>
       </c>
       <c r="G59" s="1" t="str">
         <f t="shared" si="1"/>
@@ -10180,7 +10177,7 @@
         <v>56</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>473</v>
+        <v>460</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>63</v>
@@ -10192,7 +10189,7 @@
         <v>0</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>558</v>
+        <v>542</v>
       </c>
       <c r="G60" s="1" t="str">
         <f t="shared" si="1"/>
@@ -10236,7 +10233,7 @@
         <v>57</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>473</v>
+        <v>460</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>94</v>
@@ -10248,7 +10245,7 @@
         <v>1</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>557</v>
+        <v>541</v>
       </c>
       <c r="G61" s="1" t="str">
         <f t="shared" si="1"/>
@@ -10278,10 +10275,10 @@
         <v>96</v>
       </c>
       <c r="Z61" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="AA61" s="12" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="AB61" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B61&amp; " resources for the specified patient. Mandatory for client to support the _include parameter. Optional for server to support the _include parameter."</f>
@@ -10297,10 +10294,10 @@
         <v>58</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>473</v>
+        <v>460</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>73</v>
@@ -10309,7 +10306,7 @@
         <v>0</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>559</v>
+        <v>543</v>
       </c>
       <c r="G62" s="1" t="str">
         <f t="shared" si="1"/>
@@ -10354,7 +10351,7 @@
         <v>59</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>63</v>
@@ -10366,7 +10363,7 @@
         <v>0</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>558</v>
+        <v>542</v>
       </c>
       <c r="G63" s="1" t="str">
         <f t="shared" si="1"/>
@@ -10410,7 +10407,7 @@
         <v>60</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>94</v>
@@ -10422,7 +10419,7 @@
         <v>1</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>557</v>
+        <v>541</v>
       </c>
       <c r="G64" s="1" t="str">
         <f t="shared" si="1"/>
@@ -10455,7 +10452,7 @@
         <v>support searching for all procedures for a patient</v>
       </c>
       <c r="AA64" s="5" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="AB64" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B64&amp; " resources for the specified patient"</f>
@@ -10471,7 +10468,7 @@
         <v>61</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>83</v>
@@ -10483,7 +10480,7 @@
         <v>0</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>559</v>
+        <v>543</v>
       </c>
       <c r="G65" s="1" t="str">
         <f t="shared" si="1"/>
@@ -10528,7 +10525,7 @@
         <v>62</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>28</v>
@@ -10540,7 +10537,7 @@
         <v>0</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>558</v>
+        <v>542</v>
       </c>
       <c r="G66" s="1" t="str">
         <f t="shared" si="1"/>
@@ -10581,7 +10578,7 @@
         <v>63</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>63</v>
@@ -10593,7 +10590,7 @@
         <v>0</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>558</v>
+        <v>542</v>
       </c>
       <c r="G67" s="1" t="str">
         <f t="shared" ref="G67:G94" si="12">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B67)</f>
@@ -10637,7 +10634,7 @@
         <v>64</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>145</v>
@@ -10649,7 +10646,7 @@
         <v>0</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>558</v>
+        <v>542</v>
       </c>
       <c r="G68" s="1" t="str">
         <f t="shared" si="12"/>
@@ -10690,7 +10687,7 @@
         <v>65</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>28</v>
@@ -10702,7 +10699,7 @@
         <v>0</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>558</v>
+        <v>542</v>
       </c>
       <c r="G69" s="1" t="str">
         <f t="shared" si="12"/>
@@ -10743,7 +10740,7 @@
         <v>66</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>83</v>
@@ -10755,7 +10752,7 @@
         <v>0</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>559</v>
+        <v>543</v>
       </c>
       <c r="G70" s="1" t="str">
         <f t="shared" si="12"/>
@@ -10800,7 +10797,7 @@
         <v>67</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>94</v>
@@ -10812,7 +10809,7 @@
         <v>0</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>557</v>
+        <v>541</v>
       </c>
       <c r="G71" s="1" t="str">
         <f t="shared" si="12"/>
@@ -10862,7 +10859,7 @@
         <v>68</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>145</v>
@@ -10874,7 +10871,7 @@
         <v>0</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>558</v>
+        <v>542</v>
       </c>
       <c r="G72" s="1" t="str">
         <f t="shared" si="12"/>
@@ -10915,7 +10912,7 @@
         <v>69</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>28</v>
@@ -10927,7 +10924,7 @@
         <v>0</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>558</v>
+        <v>542</v>
       </c>
       <c r="G73" s="1" t="str">
         <f t="shared" si="12"/>
@@ -10965,7 +10962,7 @@
         <v>70</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>83</v>
@@ -10977,7 +10974,7 @@
         <v>0</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>559</v>
+        <v>543</v>
       </c>
       <c r="G74" s="1" t="str">
         <f t="shared" si="12"/>
@@ -11022,7 +11019,7 @@
         <v>71</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>94</v>
@@ -11034,7 +11031,7 @@
         <v>0</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>557</v>
+        <v>541</v>
       </c>
       <c r="G75" s="1" t="str">
         <f t="shared" si="12"/>
@@ -11084,7 +11081,7 @@
         <v>72</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>63</v>
@@ -11096,7 +11093,7 @@
         <v>0</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>558</v>
+        <v>542</v>
       </c>
       <c r="G76" s="1" t="str">
         <f t="shared" si="12"/>
@@ -11140,7 +11137,7 @@
         <v>73</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>94</v>
@@ -11152,7 +11149,7 @@
         <v>0</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>557</v>
+        <v>541</v>
       </c>
       <c r="G77" s="1" t="str">
         <f t="shared" si="12"/>
@@ -11202,7 +11199,7 @@
         <v>74</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>63</v>
@@ -11214,7 +11211,7 @@
         <v>0</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>558</v>
+        <v>542</v>
       </c>
       <c r="G78" s="1" t="str">
         <f t="shared" si="12"/>
@@ -11258,7 +11255,7 @@
         <v>75</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>94</v>
@@ -11270,7 +11267,7 @@
         <v>1</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>557</v>
+        <v>541</v>
       </c>
       <c r="G79" s="1" t="str">
         <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-implantable-"&amp;LOWER(B79)</f>
@@ -11320,7 +11317,7 @@
         <v>76</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>13</v>
@@ -11332,7 +11329,7 @@
         <v>0</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>558</v>
+        <v>542</v>
       </c>
       <c r="G80" s="1" t="str">
         <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-implantable-"&amp;LOWER(B80)</f>
@@ -11369,7 +11366,7 @@
         <v>77</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>25</v>
@@ -11404,7 +11401,7 @@
         <v>57</v>
       </c>
       <c r="Z81" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="AA81" s="5" t="str">
         <f>"GET [base]/"&amp;B81&amp;"?name=Health"</f>
@@ -11424,7 +11421,7 @@
         <v>78</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>90</v>
@@ -11459,7 +11456,7 @@
         <v>57</v>
       </c>
       <c r="Z82" s="1" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="AA82" s="5" t="str">
         <f>"GET [base]/"&amp;B82&amp;"?address=Arbor"</f>
@@ -11479,10 +11476,10 @@
         <v>79</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>73</v>
@@ -11514,7 +11511,7 @@
         <v>57</v>
       </c>
       <c r="Z83" s="1" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="AA83" s="5" t="str">
         <f>"GET [base]/"&amp;B83&amp;"?address-city=Ann Arbor"</f>
@@ -11534,10 +11531,10 @@
         <v>80</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>73</v>
@@ -11569,10 +11566,10 @@
         <v>57</v>
       </c>
       <c r="Z84" s="1" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="AA84" s="5" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="AB84" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B84&amp; " resources for the state"</f>
@@ -11588,10 +11585,10 @@
         <v>81</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>73</v>
@@ -11623,7 +11620,7 @@
         <v>57</v>
       </c>
       <c r="Z85" s="1" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="AA85" s="5" t="str">
         <f>"GET [base]/"&amp;B85&amp;"?address-postalcode=48104"</f>
@@ -11643,7 +11640,7 @@
         <v>82</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>25</v>
@@ -11678,7 +11675,7 @@
         <v>57</v>
       </c>
       <c r="Z86" s="1" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="AA86" s="5" t="str">
         <f>"GET [base]/"&amp;B86&amp;"?name=Health"</f>
@@ -11698,7 +11695,7 @@
         <v>83</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>90</v>
@@ -11733,7 +11730,7 @@
         <v>57</v>
       </c>
       <c r="Z87" s="1" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="AA87" s="5" t="str">
         <f>"GET [base]/"&amp;B87&amp;"?address=Arbor"</f>
@@ -11753,10 +11750,10 @@
         <v>84</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>73</v>
@@ -11788,7 +11785,7 @@
         <v>57</v>
       </c>
       <c r="Z88" s="1" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="AA88" s="5" t="str">
         <f>"GET [base]/"&amp;B88&amp;"?address-city=Ann Arbor"</f>
@@ -11808,10 +11805,10 @@
         <v>85</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>73</v>
@@ -11843,7 +11840,7 @@
         <v>57</v>
       </c>
       <c r="Z89" s="1" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="AA89" s="5" t="str">
         <f>"GET [base]/"&amp;B89&amp;"?address-state=MI"</f>
@@ -11863,10 +11860,10 @@
         <v>86</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>73</v>
@@ -11898,7 +11895,7 @@
         <v>57</v>
       </c>
       <c r="Z90" s="1" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="AA90" s="5" t="str">
         <f>"GET [base]/"&amp;B90&amp;"?address-postalcode=48104"</f>
@@ -11918,7 +11915,7 @@
         <v>87</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>25</v>
@@ -11956,7 +11953,7 @@
         <v>81</v>
       </c>
       <c r="Z91" s="5" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="AA91" s="5" t="str">
         <f>"GET [base]/"&amp;B91&amp;"?name=Smith"</f>
@@ -11976,7 +11973,7 @@
         <v>88</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>80</v>
@@ -11988,7 +11985,7 @@
         <v>1</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>558</v>
+        <v>542</v>
       </c>
       <c r="G92" s="1" t="str">
         <f t="shared" si="12"/>
@@ -12014,7 +12011,7 @@
         <v>57</v>
       </c>
       <c r="Z92" s="5" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
       <c r="AA92" s="5" t="str">
         <f>"GET [base]/"&amp;B92&amp;"?dentifier=http://hl7.org/fhir/sid/us-npi\|97860456"</f>
@@ -12034,10 +12031,10 @@
         <v>89</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>73</v>
@@ -12046,7 +12043,7 @@
         <v>1</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>558</v>
+        <v>542</v>
       </c>
       <c r="G93" s="1" t="str">
         <f t="shared" si="12"/>
@@ -12072,10 +12069,10 @@
         <v>57</v>
       </c>
       <c r="W93" s="1" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="Z93" s="5" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
       <c r="AA93" s="5" t="str">
         <f>"GET [base]/"&amp;B93&amp;"?specialty=http://nucc.org/provider-taxonomy\|208D0000X"</f>
@@ -12095,10 +12092,10 @@
         <v>90</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>73</v>
@@ -12107,7 +12104,7 @@
         <v>1</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>557</v>
+        <v>541</v>
       </c>
       <c r="G94" s="1" t="str">
         <f t="shared" si="12"/>
@@ -12133,13 +12130,13 @@
         <v>57</v>
       </c>
       <c r="T94" s="1" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="W94" s="1" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="Z94" s="5" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="AA94" s="5" t="str">
         <f>_xlfn.CONCAT("GET [base]/",B94,"?practitioner.identifier=http://hl7.org/fhir/sid/us-npi\|97860456&amp;_include=PractitionerRole:practitioner","&amp;_include=PractitionerRole?endpoint~GET [base]/PractitionerRole?practitioner.name=Henry&amp;_include=PractitionerRole:practitioner&amp;_include=PractitionerRole?endpoint")</f>

</xml_diff>

<commit_message>
update cs to fix qa error
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core-R4/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C854AA25-6E78-E140-B0A9-9DCCB9B14E28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79983E1D-9B29-1C45-A306-7FC2FF3BB91B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2060" yWindow="-21140" windowWidth="30580" windowHeight="19040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1907,7 +1907,7 @@
     <t>http://fhir-registry.smarthealthit.org</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/uv/bulkdata/STU1.0.1/ImplementationGuide-hl7.fhir.uv.bulkdata.html</t>
+    <t>http://hl7.org/fhir/uv/bulkdata/STU1.0.1/ImplementationGuide-hl7.fhir.uv.bulkdata</t>
   </si>
 </sst>
 </file>
@@ -10363,7 +10363,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
initial Sexual Orientation Design
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core-R4/input/resources_spreadsheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\US-Core\input\resources_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7AB31D6-9A42-4343-8363-73A9F81E898E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBEFBBC0-4696-44B6-AC67-5E148F521460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2090" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2094" uniqueCount="580">
   <si>
     <t>Element</t>
   </si>
@@ -1918,12 +1918,18 @@
   <si>
     <t>CapabilityStatement-us-core-client.html</t>
   </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-sexual-orientation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	US Core Sexual Orientation Observation Profile</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2418,13 +2424,13 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2432,7 +2438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>483</v>
       </c>
@@ -2440,7 +2446,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>484</v>
       </c>
@@ -2448,7 +2454,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
         <v>485</v>
       </c>
@@ -2456,7 +2462,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
         <v>487</v>
       </c>
@@ -2464,7 +2470,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
         <v>66</v>
       </c>
@@ -2472,7 +2478,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
         <v>490</v>
       </c>
@@ -2480,7 +2486,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
         <v>491</v>
       </c>
@@ -2488,7 +2494,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
         <v>551</v>
       </c>
@@ -2512,39 +2518,39 @@
       <selection pane="bottomRight" activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="45.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="45.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="1"/>
-    <col min="2" max="2" width="21.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="33.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="21.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="33.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1" customWidth="1"/>
-    <col min="6" max="6" width="68.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="73.83203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.83203125" style="1"/>
-    <col min="9" max="9" width="14.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="8.83203125" style="1"/>
-    <col min="11" max="11" width="36.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="22.5" style="1" customWidth="1"/>
-    <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="10.33203125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="16.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="68.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="73.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" style="1"/>
+    <col min="9" max="9" width="14.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" style="1"/>
+    <col min="11" max="11" width="36.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="22.42578125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="10.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="16.28515625" style="1" customWidth="1"/>
     <col min="17" max="17" width="18" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="49.6640625" style="1" customWidth="1"/>
-    <col min="22" max="23" width="38.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="49.7109375" style="1" customWidth="1"/>
+    <col min="22" max="23" width="38.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="16" style="1" customWidth="1"/>
-    <col min="25" max="25" width="50.83203125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="68.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="90.6640625" style="1" customWidth="1"/>
-    <col min="28" max="28" width="83.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="38.1640625" style="1" customWidth="1"/>
-    <col min="30" max="16384" width="8.83203125" style="1"/>
+    <col min="25" max="25" width="50.85546875" style="1" customWidth="1"/>
+    <col min="26" max="26" width="68.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="90.7109375" style="1" customWidth="1"/>
+    <col min="28" max="28" width="83.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="38.140625" style="1" customWidth="1"/>
+    <col min="30" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" ht="45.75" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>142</v>
       </c>
@@ -2633,7 +2639,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="45.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29" ht="45.75" customHeight="1" thickTop="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2683,7 +2689,7 @@
         <v>SearchParameter-us-core-!example category search-category.html</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29" ht="45.75" customHeight="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2730,7 +2736,7 @@
         <v>SearchParameter-us-core-!example code search-code.html</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" ht="45.75" customHeight="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2784,7 +2790,7 @@
         <v>SearchParameter-us-core-!example date search-date.html</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:29" ht="45.75" customHeight="1">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2846,7 +2852,7 @@
         <v>SearchParameter-us-core-!example patient search-patient.html</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:29" ht="45.75" customHeight="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2896,7 +2902,7 @@
         <v>SearchParameter-us-core-!example status search-status.html</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:29" ht="45.75" customHeight="1">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2947,7 +2953,7 @@
         <v>SearchParameter-us-core-!patient-address.html</v>
       </c>
     </row>
-    <row r="8" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:29" ht="45.75" customHeight="1">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2998,7 +3004,7 @@
         <v>SearchParameter-us-core-!patient-telecom.html</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:29" ht="45.75" customHeight="1">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -3047,7 +3053,7 @@
         <v>SearchParameter-us-core-allergyintolerance-clinical-status.html</v>
       </c>
     </row>
-    <row r="10" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:29" ht="45.75" customHeight="1">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -3105,7 +3111,7 @@
         <v>SearchParameter-us-core-allergyintolerance-patient.html</v>
       </c>
     </row>
-    <row r="11" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29" ht="45.75" customHeight="1">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -3158,7 +3164,7 @@
         <v>SearchParameter-us-core-condition-category.html</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:29" ht="45.75" customHeight="1">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -3209,7 +3215,7 @@
         <v>SearchParameter-us-core-condition-clinical-status.html</v>
       </c>
     </row>
-    <row r="13" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:29" ht="45.75" customHeight="1">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -3270,7 +3276,7 @@
         <v>SearchParameter-us-core-condition-patient.html</v>
       </c>
     </row>
-    <row r="14" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:29" ht="45.75" customHeight="1">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -3323,7 +3329,7 @@
         <v>SearchParameter-us-core-encounter-id.html</v>
       </c>
     </row>
-    <row r="15" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:29" ht="45.75" customHeight="1">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -3376,7 +3382,7 @@
         <v>SearchParameter-us-core-encounter-class.html</v>
       </c>
     </row>
-    <row r="16" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:29" ht="45.75" customHeight="1">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -3433,7 +3439,7 @@
         <v>SearchParameter-us-core-encounter-date.html</v>
       </c>
     </row>
-    <row r="17" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:29" ht="45.75" customHeight="1">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -3490,7 +3496,7 @@
         <v>SearchParameter-us-core-encounter-identifier.html</v>
       </c>
     </row>
-    <row r="18" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:29" ht="45.75" customHeight="1">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -3551,7 +3557,7 @@
         <v>SearchParameter-us-core-encounter-patient.html</v>
       </c>
     </row>
-    <row r="19" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:29" ht="45.75" customHeight="1">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -3604,7 +3610,7 @@
         <v>SearchParameter-us-core-encounter-status.html</v>
       </c>
     </row>
-    <row r="20" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:29" ht="45.75" customHeight="1">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -3654,7 +3660,7 @@
         <v>SearchParameter-us-core-encounter-type.html</v>
       </c>
     </row>
-    <row r="21" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:29" ht="45.75" customHeight="1">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -3704,7 +3710,7 @@
         <v>SearchParameter-us-core-patient-id.html</v>
       </c>
     </row>
-    <row r="22" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:29" ht="45.75" customHeight="1">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -3754,7 +3760,7 @@
         <v>SearchParameter-us-core-patient-birthdate.html</v>
       </c>
     </row>
-    <row r="23" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:29" ht="45.75" customHeight="1">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -3797,7 +3803,7 @@
         <v>SearchParameter-us-core-patient-family.html</v>
       </c>
     </row>
-    <row r="24" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:29" ht="45.75" customHeight="1">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -3848,7 +3854,7 @@
         <v>SearchParameter-us-core-patient-gender.html</v>
       </c>
     </row>
-    <row r="25" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:29" ht="45.75" customHeight="1">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -3892,7 +3898,7 @@
         <v>SearchParameter-us-core-patient-given.html</v>
       </c>
     </row>
-    <row r="26" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:29" ht="45.75" customHeight="1">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -3949,7 +3955,7 @@
         <v>SearchParameter-us-core-patient-identifier.html</v>
       </c>
     </row>
-    <row r="27" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:29" ht="45.75" customHeight="1">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -4006,7 +4012,7 @@
         <v>SearchParameter-us-core-patient-name.html</v>
       </c>
     </row>
-    <row r="28" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:29" ht="45.75" customHeight="1">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -4049,7 +4055,7 @@
         <v>SearchParameter-us-core-!questionnaire-_id.html</v>
       </c>
     </row>
-    <row r="29" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:29" ht="45.75" customHeight="1">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -4093,7 +4099,7 @@
         <v>SearchParameter-us-core-!questionnaire-context-type-value.html</v>
       </c>
     </row>
-    <row r="30" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:29" ht="45.75" customHeight="1">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -4143,7 +4149,7 @@
         <v>SearchParameter-us-core-!questionnaire-publisher.html</v>
       </c>
     </row>
-    <row r="31" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:29" ht="45.75" customHeight="1">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -4190,7 +4196,7 @@
         <v>SearchParameter-us-core-!questionnaire-status.html</v>
       </c>
     </row>
-    <row r="32" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:29" ht="45.75" customHeight="1">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -4249,7 +4255,7 @@
         <v>SearchParameter-us-core-!questionnaire-title.html</v>
       </c>
     </row>
-    <row r="33" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:29" ht="45.75" customHeight="1">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -4293,7 +4299,7 @@
         <v>SearchParameter-us-core-!questionnaire-url.html</v>
       </c>
     </row>
-    <row r="34" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:29" ht="45.75" customHeight="1">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -4337,7 +4343,7 @@
         <v>SearchParameter-us-core-!questionnaire-version.html</v>
       </c>
     </row>
-    <row r="35" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:29" ht="45.75" customHeight="1">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -4391,7 +4397,7 @@
         <v>SearchParameter-us-core-condition-onset-date.html</v>
       </c>
     </row>
-    <row r="36" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:29" ht="45.75" customHeight="1">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -4441,7 +4447,7 @@
         <v>SearchParameter-us-core-condition-code.html</v>
       </c>
     </row>
-    <row r="37" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:29" ht="45.75" customHeight="1">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -4503,7 +4509,7 @@
         <v>SearchParameter-us-core-immunization-patient.html</v>
       </c>
     </row>
-    <row r="38" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:29" ht="45.75" customHeight="1">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -4556,7 +4562,7 @@
         <v>SearchParameter-us-core-immunization-status.html</v>
       </c>
     </row>
-    <row r="39" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:29" ht="45.75" customHeight="1">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -4613,7 +4619,7 @@
         <v>SearchParameter-us-core-immunization-date.html</v>
       </c>
     </row>
-    <row r="40" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:29" ht="45.75" customHeight="1">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -4666,7 +4672,7 @@
         <v>SearchParameter-us-core-documentreference-_id.html</v>
       </c>
     </row>
-    <row r="41" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:29" ht="45.75" customHeight="1">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -4722,7 +4728,7 @@
         <v>SearchParameter-us-core-documentreference-status.html</v>
       </c>
     </row>
-    <row r="42" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:29" ht="45.75" customHeight="1">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -4784,7 +4790,7 @@
         <v>SearchParameter-us-core-documentreference-patient.html</v>
       </c>
     </row>
-    <row r="43" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:29" ht="45.75" customHeight="1">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -4837,7 +4843,7 @@
         <v>SearchParameter-us-core-documentreference-category.html</v>
       </c>
     </row>
-    <row r="44" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:29" ht="45.75" customHeight="1">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -4887,7 +4893,7 @@
         <v>SearchParameter-us-core-documentreference-type.html</v>
       </c>
     </row>
-    <row r="45" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:29" ht="45.75" customHeight="1">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -4944,7 +4950,7 @@
         <v>SearchParameter-us-core-documentreference-date.html</v>
       </c>
     </row>
-    <row r="46" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:29" ht="45.75" customHeight="1">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -5000,7 +5006,7 @@
         <v>SearchParameter-us-core-documentreference-period.html</v>
       </c>
     </row>
-    <row r="47" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:29" ht="45.75" customHeight="1">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -5056,7 +5062,7 @@
         <v>SearchParameter-us-core-diagnosticreport-status.html</v>
       </c>
     </row>
-    <row r="48" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:29" ht="45.75" customHeight="1">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -5118,7 +5124,7 @@
         <v>SearchParameter-us-core-diagnosticreport-patient.html</v>
       </c>
     </row>
-    <row r="49" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:29" ht="45.75" customHeight="1">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -5171,7 +5177,7 @@
         <v>SearchParameter-us-core-diagnosticreport-category.html</v>
       </c>
     </row>
-    <row r="50" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:29" ht="45.75" customHeight="1">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -5224,7 +5230,7 @@
         <v>SearchParameter-us-core-diagnosticreport-code.html</v>
       </c>
     </row>
-    <row r="51" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:29" ht="45.75" customHeight="1">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -5281,7 +5287,7 @@
         <v>SearchParameter-us-core-diagnosticreport-date.html</v>
       </c>
     </row>
-    <row r="52" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:29" ht="45.75" customHeight="1">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -5334,7 +5340,7 @@
         <v>SearchParameter-us-core-goal-lifecycle-status.html</v>
       </c>
     </row>
-    <row r="53" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:29" ht="45.75" customHeight="1">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -5396,7 +5402,7 @@
         <v>SearchParameter-us-core-goal-patient.html</v>
       </c>
     </row>
-    <row r="54" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:29" ht="45.75" customHeight="1">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -5453,7 +5459,7 @@
         <v>SearchParameter-us-core-goal-target-date.html</v>
       </c>
     </row>
-    <row r="55" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:29" ht="45.75" customHeight="1">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -5509,7 +5515,7 @@
         <v>SearchParameter-us-core-medicationrequest-status.html</v>
       </c>
     </row>
-    <row r="56" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:29" ht="45.75" customHeight="1">
       <c r="A56" s="1">
         <v>53</v>
       </c>
@@ -5565,7 +5571,7 @@
         <v>SearchParameter-us-core-medicationrequest-intent.html</v>
       </c>
     </row>
-    <row r="57" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:29" ht="45.75" customHeight="1">
       <c r="A57" s="1">
         <v>54</v>
       </c>
@@ -5619,7 +5625,7 @@
         <v>SearchParameter-us-core-medicationrequest-patient.html</v>
       </c>
     </row>
-    <row r="58" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:29" ht="45.75" customHeight="1">
       <c r="A58" s="1">
         <v>54</v>
       </c>
@@ -5673,7 +5679,7 @@
         <v>SearchParameter-us-core-medicationrequest-encounter.html</v>
       </c>
     </row>
-    <row r="59" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:29" ht="45.75" customHeight="1">
       <c r="A59" s="1">
         <v>55</v>
       </c>
@@ -5730,7 +5736,7 @@
         <v>SearchParameter-us-core-medicationrequest-authoredon.html</v>
       </c>
     </row>
-    <row r="60" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:29" ht="45.75" customHeight="1">
       <c r="A60" s="1">
         <v>56</v>
       </c>
@@ -5786,7 +5792,7 @@
         <v>SearchParameter-us-core-!medicationstatement-status.html</v>
       </c>
     </row>
-    <row r="61" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:29" ht="45.75" customHeight="1">
       <c r="A61" s="1">
         <v>57</v>
       </c>
@@ -5847,7 +5853,7 @@
         <v>SearchParameter-us-core-!medicationstatement-patient.html</v>
       </c>
     </row>
-    <row r="62" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:29" ht="45.75" customHeight="1">
       <c r="A62" s="1">
         <v>58</v>
       </c>
@@ -5904,7 +5910,7 @@
         <v>SearchParameter-us-core-!medicationstatement-effective.html</v>
       </c>
     </row>
-    <row r="63" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:29" ht="45.75" customHeight="1">
       <c r="A63" s="1">
         <v>59</v>
       </c>
@@ -5960,7 +5966,7 @@
         <v>SearchParameter-us-core-procedure-status.html</v>
       </c>
     </row>
-    <row r="64" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:29" ht="45.75" customHeight="1">
       <c r="A64" s="1">
         <v>60</v>
       </c>
@@ -6021,7 +6027,7 @@
         <v>SearchParameter-us-core-procedure-patient.html</v>
       </c>
     </row>
-    <row r="65" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:29" ht="45.75" customHeight="1">
       <c r="A65" s="1">
         <v>61</v>
       </c>
@@ -6078,7 +6084,7 @@
         <v>SearchParameter-us-core-procedure-date.html</v>
       </c>
     </row>
-    <row r="66" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:29" ht="45.75" customHeight="1">
       <c r="A66" s="1">
         <v>62</v>
       </c>
@@ -6131,7 +6137,7 @@
         <v>SearchParameter-us-core-procedure-code.html</v>
       </c>
     </row>
-    <row r="67" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:29" ht="45.75" customHeight="1">
       <c r="A67" s="1">
         <v>63</v>
       </c>
@@ -6187,7 +6193,7 @@
         <v>SearchParameter-us-core-observation-status.html</v>
       </c>
     </row>
-    <row r="68" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:29" ht="45.75" customHeight="1">
       <c r="A68" s="1">
         <v>64</v>
       </c>
@@ -6240,7 +6246,7 @@
         <v>SearchParameter-us-core-observation-category.html</v>
       </c>
     </row>
-    <row r="69" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:29" ht="45.75" customHeight="1">
       <c r="A69" s="1">
         <v>65</v>
       </c>
@@ -6293,7 +6299,7 @@
         <v>SearchParameter-us-core-observation-code.html</v>
       </c>
     </row>
-    <row r="70" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:29" ht="45.75" customHeight="1">
       <c r="A70" s="1">
         <v>66</v>
       </c>
@@ -6350,7 +6356,7 @@
         <v>SearchParameter-us-core-observation-date.html</v>
       </c>
     </row>
-    <row r="71" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:29" ht="45.75" customHeight="1">
       <c r="A71" s="1">
         <v>67</v>
       </c>
@@ -6412,7 +6418,7 @@
         <v>SearchParameter-us-core-observation-patient.html</v>
       </c>
     </row>
-    <row r="72" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:29" ht="45.75" customHeight="1">
       <c r="A72" s="1">
         <v>68</v>
       </c>
@@ -6465,7 +6471,7 @@
         <v>SearchParameter-us-core-careplan-category.html</v>
       </c>
     </row>
-    <row r="73" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:29" ht="45.75" customHeight="1">
       <c r="A73" s="1">
         <v>69</v>
       </c>
@@ -6515,7 +6521,7 @@
         <v>SearchParameter-us-core-!careplan-code.html</v>
       </c>
     </row>
-    <row r="74" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:29" ht="45.75" customHeight="1">
       <c r="A74" s="1">
         <v>70</v>
       </c>
@@ -6572,7 +6578,7 @@
         <v>SearchParameter-us-core-careplan-date.html</v>
       </c>
     </row>
-    <row r="75" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:29" ht="45.75" customHeight="1">
       <c r="A75" s="1">
         <v>71</v>
       </c>
@@ -6634,7 +6640,7 @@
         <v>SearchParameter-us-core-careplan-patient.html</v>
       </c>
     </row>
-    <row r="76" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:29" ht="45.75" customHeight="1">
       <c r="A76" s="1">
         <v>72</v>
       </c>
@@ -6690,7 +6696,7 @@
         <v>SearchParameter-us-core-careplan-status.html</v>
       </c>
     </row>
-    <row r="77" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:29" ht="45.75" customHeight="1">
       <c r="A77" s="1">
         <v>73</v>
       </c>
@@ -6752,7 +6758,7 @@
         <v>SearchParameter-us-core-careteam-patient.html</v>
       </c>
     </row>
-    <row r="78" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:29" ht="45.75" customHeight="1">
       <c r="A78" s="1">
         <v>74</v>
       </c>
@@ -6808,7 +6814,7 @@
         <v>SearchParameter-us-core-careteam-status.html</v>
       </c>
     </row>
-    <row r="79" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:29" ht="45.75" customHeight="1">
       <c r="A79" s="1">
         <v>75</v>
       </c>
@@ -6870,7 +6876,7 @@
         <v>SearchParameter-us-core-device-patient.html</v>
       </c>
     </row>
-    <row r="80" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:29" ht="45.75" customHeight="1">
       <c r="A80" s="1">
         <v>76</v>
       </c>
@@ -6919,7 +6925,7 @@
         <v>SearchParameter-us-core-device-type.html</v>
       </c>
     </row>
-    <row r="81" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:29" ht="45.75" customHeight="1">
       <c r="A81" s="1">
         <v>77</v>
       </c>
@@ -6974,7 +6980,7 @@
         <v>SearchParameter-us-core-location-name.html</v>
       </c>
     </row>
-    <row r="82" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:29" ht="45.75" customHeight="1">
       <c r="A82" s="1">
         <v>78</v>
       </c>
@@ -7029,7 +7035,7 @@
         <v>SearchParameter-us-core-location-address.html</v>
       </c>
     </row>
-    <row r="83" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:29" ht="45.75" customHeight="1">
       <c r="A83" s="1">
         <v>79</v>
       </c>
@@ -7084,7 +7090,7 @@
         <v>SearchParameter-us-core-location-address-city.html</v>
       </c>
     </row>
-    <row r="84" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:29" ht="45.75" customHeight="1">
       <c r="A84" s="1">
         <v>80</v>
       </c>
@@ -7138,7 +7144,7 @@
         <v>SearchParameter-us-core-location-address-state.html</v>
       </c>
     </row>
-    <row r="85" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:29" ht="45.75" customHeight="1">
       <c r="A85" s="1">
         <v>81</v>
       </c>
@@ -7193,7 +7199,7 @@
         <v>SearchParameter-us-core-location-address-postalcode.html</v>
       </c>
     </row>
-    <row r="86" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:29" ht="45.75" customHeight="1">
       <c r="A86" s="1">
         <v>82</v>
       </c>
@@ -7248,7 +7254,7 @@
         <v>SearchParameter-us-core-organization-name.html</v>
       </c>
     </row>
-    <row r="87" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:29" ht="45.75" customHeight="1">
       <c r="A87" s="1">
         <v>83</v>
       </c>
@@ -7303,7 +7309,7 @@
         <v>SearchParameter-us-core-organization-address.html</v>
       </c>
     </row>
-    <row r="88" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:29" ht="45.75" customHeight="1">
       <c r="A88" s="1">
         <v>84</v>
       </c>
@@ -7358,7 +7364,7 @@
         <v>SearchParameter-us-core-!organization-address-city.html</v>
       </c>
     </row>
-    <row r="89" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:29" ht="45.75" customHeight="1">
       <c r="A89" s="1">
         <v>85</v>
       </c>
@@ -7413,7 +7419,7 @@
         <v>SearchParameter-us-core-!organization-adress-state.html</v>
       </c>
     </row>
-    <row r="90" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:29" ht="45.75" customHeight="1">
       <c r="A90" s="1">
         <v>86</v>
       </c>
@@ -7468,7 +7474,7 @@
         <v>SearchParameter-us-core-!organization-address-postalcode.html</v>
       </c>
     </row>
-    <row r="91" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:29" ht="45.75" customHeight="1">
       <c r="A91" s="1">
         <v>87</v>
       </c>
@@ -7526,7 +7532,7 @@
         <v>SearchParameter-us-core-practitioner-name.html</v>
       </c>
     </row>
-    <row r="92" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:29" ht="45.75" customHeight="1">
       <c r="A92" s="1">
         <v>88</v>
       </c>
@@ -7584,7 +7590,7 @@
         <v>SearchParameter-us-core-practitioner-identifier.html</v>
       </c>
     </row>
-    <row r="93" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:29" ht="45.75" customHeight="1">
       <c r="A93" s="1">
         <v>89</v>
       </c>
@@ -7645,7 +7651,7 @@
         <v>SearchParameter-us-core-practitionerrole-specialty.html</v>
       </c>
     </row>
-    <row r="94" spans="1:29" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:29" ht="45.75" customHeight="1">
       <c r="A94" s="1">
         <v>90</v>
       </c>
@@ -7728,22 +7734,22 @@
       <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="1"/>
-    <col min="2" max="2" width="21.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="96.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.83203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="88.83203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="255.5" style="1" customWidth="1"/>
-    <col min="10" max="10" width="83.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="21.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="96.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="88.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="255.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="83.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>144</v>
       </c>
@@ -7775,7 +7781,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="15.75" thickTop="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -7800,7 +7806,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -7825,7 +7831,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and patient</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -7850,7 +7856,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and patient and type</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -7875,7 +7881,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and type</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -7906,7 +7912,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified class and patient</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -7931,7 +7937,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and status</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -7956,7 +7962,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and status and type</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -7982,7 +7988,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and type</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -8009,7 +8015,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and status</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -8035,7 +8041,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and status and type</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -8060,7 +8066,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and type</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -8091,7 +8097,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified date and patient</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -8116,7 +8122,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified date and patient and type</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -8141,7 +8147,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified date and type</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -8172,7 +8178,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified patient and type</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -8198,7 +8204,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified patient and status and type</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -8229,7 +8235,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified patient and status</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -8256,7 +8262,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified status and type</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10">
       <c r="A20" s="1">
         <v>21</v>
       </c>
@@ -8282,7 +8288,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and publisher</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10">
       <c r="A21" s="1">
         <v>22</v>
       </c>
@@ -8307,7 +8313,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and publisher and status</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10">
       <c r="A22" s="1">
         <v>23</v>
       </c>
@@ -8333,7 +8339,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and status</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10">
       <c r="A23" s="1">
         <v>24</v>
       </c>
@@ -8360,7 +8366,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and status</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10">
       <c r="A24" s="1">
         <v>25</v>
       </c>
@@ -8387,7 +8393,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and status and version</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10">
       <c r="A25" s="1">
         <v>26</v>
       </c>
@@ -8414,7 +8420,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and version</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10">
       <c r="A26" s="1">
         <v>27</v>
       </c>
@@ -8439,7 +8445,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified status and title and version</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10">
       <c r="A27" s="1">
         <v>28</v>
       </c>
@@ -8464,7 +8470,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified status and version</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10">
       <c r="A28" s="1">
         <v>29</v>
       </c>
@@ -8489,7 +8495,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified title and version</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10">
       <c r="A29" s="1">
         <v>30</v>
       </c>
@@ -8520,7 +8526,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified birthdate and family</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10">
       <c r="A30" s="1">
         <v>31</v>
       </c>
@@ -8551,7 +8557,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified birthdate and name</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10">
       <c r="A31" s="1">
         <v>32</v>
       </c>
@@ -8582,7 +8588,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified family and gender</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10">
       <c r="A32" s="1">
         <v>33</v>
       </c>
@@ -8613,7 +8619,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified gender and name</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10">
       <c r="A33" s="1">
         <v>36</v>
       </c>
@@ -8646,7 +8652,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10">
       <c r="A34" s="1">
         <v>37</v>
       </c>
@@ -8676,7 +8682,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10">
       <c r="A35" s="1">
         <v>38</v>
       </c>
@@ -8706,7 +8712,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10">
       <c r="A36" s="1">
         <v>39</v>
       </c>
@@ -8736,7 +8742,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10">
       <c r="A37" s="1">
         <v>42</v>
       </c>
@@ -8766,7 +8772,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10">
       <c r="A38" s="1">
         <v>45</v>
       </c>
@@ -8797,7 +8803,7 @@
         <v>Fetches a bundle of all Immunization resources for the specified patient and date</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10">
       <c r="A39" s="1">
         <v>46</v>
       </c>
@@ -8828,7 +8834,7 @@
         <v>Fetches a bundle of all Immunization resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10">
       <c r="A40" s="1">
         <v>49</v>
       </c>
@@ -8858,7 +8864,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" ht="15.75">
       <c r="A41" s="1">
         <v>50</v>
       </c>
@@ -8891,7 +8897,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  a category code = `LAB`</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" ht="15.75">
       <c r="A42" s="1">
         <v>51</v>
       </c>
@@ -8921,7 +8927,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" ht="15.75">
       <c r="A43" s="1">
         <v>52</v>
       </c>
@@ -8954,7 +8960,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and a category code = `LAB`</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10">
       <c r="A44" s="1">
         <v>53</v>
       </c>
@@ -8984,7 +8990,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10">
       <c r="A45" s="1">
         <v>56</v>
       </c>
@@ -9014,7 +9020,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10">
       <c r="A46" s="1">
         <v>57</v>
       </c>
@@ -9044,7 +9050,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  a category code specified in US Core DiagnosticReport Category Codes</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10">
       <c r="A47" s="1">
         <v>58</v>
       </c>
@@ -9074,7 +9080,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10">
       <c r="A48" s="1">
         <v>59</v>
       </c>
@@ -9104,7 +9110,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and a category code specified in US Core DiagnosticReport Category Codes</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10">
       <c r="A49" s="1">
         <v>60</v>
       </c>
@@ -9134,7 +9140,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10">
       <c r="A50" s="1">
         <v>63</v>
       </c>
@@ -9165,7 +9171,7 @@
         <v>Fetches a bundle of all Goal resources for the specified patient and lifecycle-status</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10">
       <c r="A51" s="1">
         <v>64</v>
       </c>
@@ -9196,7 +9202,7 @@
         <v>Fetches a bundle of all Goal resources for the specified patient and target-date</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10">
       <c r="A52" s="1">
         <v>67</v>
       </c>
@@ -9229,7 +9235,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10">
       <c r="A53" s="1">
         <v>68</v>
       </c>
@@ -9262,7 +9268,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10">
       <c r="A54" s="1">
         <v>69</v>
       </c>
@@ -9295,7 +9301,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10">
       <c r="A55" s="1">
         <v>70</v>
       </c>
@@ -9328,7 +9334,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10">
       <c r="A56" s="1">
         <v>73</v>
       </c>
@@ -9359,7 +9365,7 @@
         <v>Fetches a bundle of all !MedicationStatement resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10">
       <c r="A57" s="1">
         <v>74</v>
       </c>
@@ -9389,7 +9395,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10">
       <c r="A58" s="1">
         <v>75</v>
       </c>
@@ -9420,7 +9426,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10">
       <c r="A59" s="1">
         <v>76</v>
       </c>
@@ -9451,7 +9457,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and date</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10">
       <c r="A60" s="1">
         <v>77</v>
       </c>
@@ -9482,7 +9488,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and date and procedure code(s).  SHOULD support search by multiple codes.</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10">
       <c r="A61" s="1">
         <v>80</v>
       </c>
@@ -9514,7 +9520,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10">
       <c r="A62" s="1">
         <v>81</v>
       </c>
@@ -9547,7 +9553,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and a category code = `laboratory`</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10">
       <c r="A63" s="1">
         <v>82</v>
       </c>
@@ -9577,7 +9583,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and observation code(s).  SHOULD support search by multiple report codes. The Observation `code` parameter searches `Observation.code only.</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10">
       <c r="A64" s="1">
         <v>83</v>
       </c>
@@ -9610,7 +9616,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and date and a category code = `laboratory`</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10">
       <c r="A65" s="1">
         <v>84</v>
       </c>
@@ -9640,7 +9646,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10">
       <c r="A66" s="1">
         <v>85</v>
       </c>
@@ -9670,7 +9676,7 @@
         <v>Fetches a bundle of all !Observation resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10">
       <c r="A67" s="1">
         <v>88</v>
       </c>
@@ -9703,7 +9709,7 @@
         <v>Fetches a bundle of all CarePlan resources for the specified patient and category=`assess-plan`</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10">
       <c r="A68" s="1">
         <v>89</v>
       </c>
@@ -9735,7 +9741,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10">
       <c r="A69" s="1">
         <v>90</v>
       </c>
@@ -9767,7 +9773,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10">
       <c r="A70" s="1">
         <v>91</v>
       </c>
@@ -9799,7 +9805,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:10">
       <c r="A71" s="1">
         <v>94</v>
       </c>
@@ -9832,7 +9838,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10" ht="15.75">
       <c r="A72" s="1">
         <v>97</v>
       </c>
@@ -9865,7 +9871,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and observation code.</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10">
       <c r="A73" s="1">
         <v>100</v>
       </c>
@@ -9898,7 +9904,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and category and status</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10">
       <c r="A74" s="1">
         <v>101</v>
       </c>
@@ -9931,7 +9937,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and a category code = `vital-signs`</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10">
       <c r="A75" s="1">
         <v>102</v>
       </c>
@@ -9964,7 +9970,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and observation code(s).  SHOULD support search by multiple codes. The Observation `code` parameter searches `Observation.code only.</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:10">
       <c r="A76" s="1">
         <v>103</v>
       </c>
@@ -9997,7 +10003,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and date and a category code = `vital-signs`</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10">
       <c r="A77" s="1">
         <v>104</v>
       </c>
@@ -10027,7 +10033,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and date and report code(s).  SHOULD support search by multiple codes.</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:10">
       <c r="A78" s="1">
         <v>107</v>
       </c>
@@ -10058,7 +10064,7 @@
         <v>Fetches a bundle of all DocumentReference resources for the specified patient and status. See the implementation notes above for how to access the actual document.</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:10" ht="20.25" customHeight="1">
       <c r="A79" s="1">
         <v>108</v>
       </c>
@@ -10087,7 +10093,7 @@
         <v>Fetches a bundle of all !DocumentReference resources for the specified patient and period. See the implementation notes above for how to access the actual document.</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10">
       <c r="A80" s="1">
         <v>109</v>
       </c>
@@ -10120,7 +10126,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10" ht="20.25" customHeight="1">
       <c r="A81" s="1">
         <v>110</v>
       </c>
@@ -10153,7 +10159,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10">
       <c r="A82" s="1">
         <v>111</v>
       </c>
@@ -10183,7 +10189,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:10" ht="20.25" customHeight="1">
       <c r="A83" s="1">
         <v>112</v>
       </c>
@@ -10214,7 +10220,7 @@
         <v>Fetches a bundle of all DocumentReference resources for the specified patient and type and period. See the implementation notes above for how to access the actual document.</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:10">
       <c r="A84" s="1">
         <v>115</v>
       </c>
@@ -10260,13 +10266,13 @@
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="95.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="95.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10274,7 +10280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>65</v>
       </c>
@@ -10282,7 +10288,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" s="1" customFormat="1">
       <c r="A3" s="1" t="s">
         <v>472</v>
       </c>
@@ -10290,7 +10296,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -10298,7 +10304,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="105" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="105" customHeight="1">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -10306,7 +10312,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -10314,7 +10320,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="141" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="141" customHeight="1">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -10322,7 +10328,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="103.5" customHeight="1">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -10330,7 +10336,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="9" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" s="1" customFormat="1">
       <c r="A9" s="1" t="s">
         <v>553</v>
       </c>
@@ -10338,7 +10344,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" s="1" customFormat="1">
       <c r="A10" s="1" t="s">
         <v>555</v>
       </c>
@@ -10346,7 +10352,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" s="1" customFormat="1">
       <c r="A11" s="1" t="s">
         <v>557</v>
       </c>
@@ -10354,7 +10360,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="12" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" s="1" customFormat="1">
       <c r="A12" s="1" t="s">
         <v>559</v>
       </c>
@@ -10375,13 +10381,13 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -10395,7 +10401,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>561</v>
       </c>
@@ -10409,7 +10415,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="15.75">
       <c r="A3" s="1" t="s">
         <v>562</v>
       </c>
@@ -10432,22 +10438,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B31AD37-8183-744F-9AC6-9E533D1B51F5}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="1"/>
-    <col min="2" max="2" width="13.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="69.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="13.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="69.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>563</v>
       </c>
@@ -10467,7 +10473,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="15.75">
       <c r="B2" s="20" t="b">
         <v>1</v>
       </c>
@@ -10491,22 +10497,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="94" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="60.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.1640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -10523,7 +10529,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
         <v>72</v>
       </c>
@@ -10538,7 +10544,7 @@
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
         <v>240</v>
       </c>
@@ -10553,7 +10559,7 @@
       </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
         <v>344</v>
       </c>
@@ -10568,7 +10574,7 @@
       </c>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
         <v>356</v>
       </c>
@@ -10583,7 +10589,7 @@
       </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
         <v>437</v>
       </c>
@@ -10598,7 +10604,7 @@
       </c>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
         <v>192</v>
       </c>
@@ -10613,7 +10619,7 @@
       </c>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
         <v>193</v>
       </c>
@@ -10628,7 +10634,7 @@
       </c>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
         <v>352</v>
       </c>
@@ -10643,7 +10649,7 @@
       </c>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
         <v>358</v>
       </c>
@@ -10658,7 +10664,7 @@
       </c>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
         <v>370</v>
       </c>
@@ -10673,7 +10679,7 @@
       </c>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
         <v>349</v>
       </c>
@@ -10688,7 +10694,7 @@
       </c>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
         <v>372</v>
       </c>
@@ -10703,7 +10709,7 @@
       </c>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
         <v>363</v>
       </c>
@@ -10718,7 +10724,7 @@
       </c>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7">
       <c r="A15" s="1" t="s">
         <v>354</v>
       </c>
@@ -10733,7 +10739,7 @@
       </c>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
         <v>493</v>
       </c>
@@ -10748,7 +10754,7 @@
       </c>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7">
       <c r="A17" s="1" t="s">
         <v>422</v>
       </c>
@@ -10763,7 +10769,7 @@
       </c>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="A18" s="1" t="s">
         <v>495</v>
       </c>
@@ -10778,7 +10784,7 @@
       </c>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="A19" s="1" t="s">
         <v>497</v>
       </c>
@@ -10793,7 +10799,7 @@
       </c>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7">
       <c r="A20" s="1" t="s">
         <v>499</v>
       </c>
@@ -10808,7 +10814,7 @@
       </c>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7">
       <c r="A21" s="1" t="s">
         <v>501</v>
       </c>
@@ -10823,7 +10829,7 @@
       </c>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="A22" s="1" t="s">
         <v>503</v>
       </c>
@@ -10838,7 +10844,7 @@
       </c>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7">
       <c r="A23" s="1" t="s">
         <v>505</v>
       </c>
@@ -10853,7 +10859,7 @@
       </c>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" s="1" customFormat="1">
       <c r="A24" s="1" t="s">
         <v>507</v>
       </c>
@@ -10867,7 +10873,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" s="1" customFormat="1">
       <c r="A25" s="1" t="s">
         <v>509</v>
       </c>
@@ -10881,7 +10887,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" s="1" customFormat="1">
       <c r="A26" s="1" t="s">
         <v>527</v>
       </c>
@@ -10895,7 +10901,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" s="1" customFormat="1">
       <c r="A27" s="1" t="s">
         <v>525</v>
       </c>
@@ -10909,7 +10915,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" s="1" customFormat="1">
       <c r="A28" s="1" t="s">
         <v>530</v>
       </c>
@@ -10923,7 +10929,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7">
       <c r="A29" s="1" t="s">
         <v>443</v>
       </c>
@@ -10937,7 +10943,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7">
       <c r="A30" s="1" t="s">
         <v>511</v>
       </c>
@@ -10951,12 +10957,12 @@
         <v>186</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" s="1" customFormat="1">
       <c r="A31" s="1" t="s">
-        <v>282</v>
+        <v>578</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>351</v>
+        <v>579</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>11</v>
@@ -10965,87 +10971,101 @@
         <v>186</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7">
       <c r="A32" s="1" t="s">
-        <v>359</v>
+        <v>282</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" s="1" t="s">
-        <v>74</v>
+        <v>359</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>375</v>
+        <v>360</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" s="1" t="s">
-        <v>347</v>
+        <v>74</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>348</v>
+        <v>375</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" s="1" t="s">
-        <v>367</v>
+        <v>347</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>368</v>
+        <v>348</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" s="1" t="s">
-        <v>361</v>
+        <v>367</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>362</v>
+        <v>368</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" s="1" t="s">
-        <v>445</v>
+        <v>361</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>446</v>
+        <v>362</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E37" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>447</v>
       </c>
     </row>
@@ -11067,23 +11087,23 @@
       <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="17.25" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="36.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="49.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="8.1640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="36.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="49.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="9" style="1" customWidth="1"/>
-    <col min="8" max="14" width="17.5" style="1" customWidth="1"/>
-    <col min="15" max="15" width="20.5" style="1" customWidth="1"/>
-    <col min="16" max="19" width="17.5" style="1" customWidth="1"/>
-    <col min="20" max="21" width="20.5" style="1" customWidth="1"/>
-    <col min="22" max="25" width="38.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="14" width="17.42578125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="20.42578125" style="1" customWidth="1"/>
+    <col min="16" max="19" width="17.42578125" style="1" customWidth="1"/>
+    <col min="20" max="21" width="20.42578125" style="1" customWidth="1"/>
+    <col min="22" max="25" width="38.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="17.25" customHeight="1" thickBot="1">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -11160,7 +11180,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="17.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="17.25" customHeight="1" thickTop="1">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -11180,7 +11200,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="17.25" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>238</v>
       </c>
@@ -11197,7 +11217,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="17.25" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>252</v>
       </c>
@@ -11211,7 +11231,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="17.25" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>139</v>
       </c>
@@ -11225,7 +11245,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="17.25" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>256</v>
       </c>
@@ -11242,7 +11262,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="17.25" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>182</v>
       </c>
@@ -11256,7 +11276,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="17.25" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>181</v>
       </c>
@@ -11273,7 +11293,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="17.25" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -11290,7 +11310,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="17.25" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>183</v>
       </c>
@@ -11304,7 +11324,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="17.25" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>163</v>
       </c>
@@ -11321,7 +11341,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="17.25" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>257</v>
       </c>
@@ -11334,7 +11354,7 @@
       <c r="X12" s="17"/>
       <c r="Y12" s="17"/>
     </row>
-    <row r="13" spans="1:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" ht="17.25" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>365</v>
       </c>
@@ -11347,7 +11367,7 @@
       <c r="X13" s="17"/>
       <c r="Y13" s="17"/>
     </row>
-    <row r="14" spans="1:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" ht="17.25" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>184</v>
       </c>
@@ -11370,7 +11390,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="17.25" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>454</v>
       </c>
@@ -11393,7 +11413,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="17.25" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>186</v>
       </c>
@@ -11410,7 +11430,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" ht="17.25" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>267</v>
       </c>
@@ -11420,7 +11440,7 @@
       <c r="X17" s="17"/>
       <c r="Y17" s="17"/>
     </row>
-    <row r="18" spans="1:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" ht="17.25" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -11437,7 +11457,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" ht="17.25" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>274</v>
       </c>
@@ -11447,7 +11467,7 @@
       <c r="X19" s="17"/>
       <c r="Y19" s="17"/>
     </row>
-    <row r="20" spans="1:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" ht="17.25" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>276</v>
       </c>
@@ -11466,7 +11486,7 @@
       <c r="X20" s="17"/>
       <c r="Y20" s="17"/>
     </row>
-    <row r="21" spans="1:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" ht="17.25" customHeight="1">
       <c r="A21" s="1" t="s">
         <v>185</v>
       </c>
@@ -11483,7 +11503,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:25" s="1" customFormat="1" ht="112" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:25" s="1" customFormat="1" ht="120">
       <c r="A22" s="1" t="s">
         <v>447</v>
       </c>
@@ -11496,7 +11516,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:25" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:25" s="1" customFormat="1" ht="15">
       <c r="A23" s="1" t="s">
         <v>464</v>
       </c>
@@ -11507,18 +11527,18 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:25" ht="17.25" customHeight="1">
       <c r="A24"/>
     </row>
-    <row r="25" spans="1:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:25" ht="17.25" customHeight="1">
       <c r="A25"/>
     </row>
-    <row r="56" spans="22:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="22:25" ht="17.25" customHeight="1">
       <c r="V56" s="7"/>
       <c r="X56" s="7"/>
       <c r="Y56" s="7"/>
     </row>
-    <row r="59" spans="22:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="22:25" ht="17.25" customHeight="1">
       <c r="Y59" s="7"/>
     </row>
   </sheetData>
@@ -11538,15 +11558,15 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" customWidth="1"/>
     <col min="5" max="5" width="89" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -11563,7 +11583,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="81" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="90.75" thickBot="1">
       <c r="A2" s="15" t="s">
         <v>378</v>
       </c>
@@ -11580,7 +11600,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" s="1" customFormat="1" ht="113.25" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>466</v>
       </c>
@@ -11597,7 +11617,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="E4" s="2"/>
     </row>
   </sheetData>
@@ -11613,18 +11633,18 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.83203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="1" customWidth="1"/>
-    <col min="7" max="7" width="35.33203125" customWidth="1"/>
-    <col min="8" max="8" width="28.1640625" customWidth="1"/>
-    <col min="18" max="18" width="8.83203125" style="1"/>
-    <col min="24" max="24" width="16.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.28515625" customWidth="1"/>
+    <col min="8" max="8" width="28.140625" customWidth="1"/>
+    <col min="18" max="18" width="8.85546875" style="1"/>
+    <col min="24" max="24" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -11701,7 +11721,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -11772,7 +11792,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -11842,7 +11862,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -11910,7 +11930,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -11978,7 +11998,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -12047,7 +12067,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -12115,7 +12135,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -12183,7 +12203,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -12251,7 +12271,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -12332,9 +12352,9 @@
       <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -12345,7 +12365,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>439</v>
       </c>
@@ -12354,7 +12374,7 @@
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>440</v>
       </c>
@@ -12363,7 +12383,7 @@
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>441</v>
       </c>
@@ -12372,7 +12392,7 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>442</v>
       </c>

</xml_diff>

<commit_message>
Update SearchParameter Narrative to align with changes in ig-publisher
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4445F5C2-90A2-7342-B7B8-B06EB7B07A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6E8DBE-64DF-724C-9286-650C87347DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2924,10 +2924,10 @@
   <dimension ref="A1:AB117"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="H60" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="Z60" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B113" sqref="B113"/>
+      <selection pane="bottomRight" activeCell="AA113" sqref="AA113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2944,7 +2944,7 @@
     <col min="11" max="11" width="8.83203125" style="1"/>
     <col min="12" max="12" width="31.1640625" style="1" customWidth="1"/>
     <col min="13" max="24" width="13.33203125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="27.83203125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="75.33203125" style="1" customWidth="1"/>
     <col min="26" max="26" width="90.6640625" style="1" customWidth="1"/>
     <col min="27" max="27" width="83.5" style="2" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="38.1640625" style="1" customWidth="1"/>
@@ -9015,8 +9015,8 @@
         <v>51</v>
       </c>
       <c r="Y113" s="1" t="str">
-        <f>"support searching for all "&amp;LOWER(B113)&amp;"s for a patient ...combo description field ...DOES THIS DO ANYTHING?"</f>
-        <v>support searching for all questionnaireresponses for a patient ...combo description field ...DOES THIS DO ANYTHING?</v>
+        <f>"support searching for all "&amp;LOWER(B113)&amp;"s for a patient"</f>
+        <v>support searching for all questionnaireresponses for a patient</v>
       </c>
       <c r="Z113" s="5" t="str">
         <f>"GET [base]/"&amp;B113&amp;"?patient=1032702"</f>
@@ -9254,8 +9254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:K102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B107" sqref="B107"/>
+    <sheetView tabSelected="1" topLeftCell="I85" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I110" sqref="I110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fxi links, update version and title
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6E8DBE-64DF-724C-9286-650C87347DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97AA98B6-9E3F-6842-BD31-0632E8CB070D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -1838,27 +1838,417 @@
     <t>SHOULD,SHOULD</t>
   </si>
   <si>
+    <t>http://hl7.org/fhir/uv/bulkdata/ImplementationGuide/hl7.fhir.uv.bulkdata</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/smart-app-launch/index.html</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/uv/bulkdata/index.html</t>
+  </si>
+  <si>
+    <t>CapabilityStatement-us-core-client.html</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-sexual-orientation</t>
+  </si>
+  <si>
+    <t>5.0.0</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/smart-app-launch/ImplementationGuide/hl7.fhir.uv.smart-app-launch</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-clinical-test</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-relatedperson</t>
+  </si>
+  <si>
+    <t>US Core RelatedPerson Profile</t>
+  </si>
+  <si>
+    <t>RelatedPerson</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</t>
+  </si>
+  <si>
+    <t>US Core ServiceRequest Profile</t>
+  </si>
+  <si>
+    <t>ServiceRequest</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-imaging</t>
+  </si>
+  <si>
+    <t>resolves</t>
+  </si>
+  <si>
+    <t>In order to access care team member's names, identifiers, locations, and contact information, the CareTeam profile supports several types of care team participants. They are represented as references to other profiles and include the following four profiles which are marked as must support:
+  1. US Core Practitioner Profile
+  1. US Core PractitionerRole Profile
+  1. US Core Patient Profile
+  1. US Core RelatedPerson Profile
+  * Although *both* US Core Practitioner Profile and US Core PractitionerRole are must support, the server system is not required to support both types of references (and `_include` search parameters), but **SHALL** support *at least* one of them.
+  * The client application **SHALL** support all four profile references.
+  * Bacause the US Core PractitionerRole Profile supplies the provider's location and contact information and a reference to the Practitioner, server systems **SHOULD** reference it instead of the US Core Practitioner Profile. An example of how to access the practitioner name and identifier is shown in the quick start section below.
+  * Servers that supports only US Core Practitioner Profile **SHALL** provide implementation specific guidance how to access a provider's location and contact information using only the Practitioner resource.</t>
+  </si>
+  <si>
+    <t>SHOULD,SHOULD,SHOULD,SHOULD</t>
+  </si>
+  <si>
+    <t>CareTeam:participant:PractitionerRole,CareTeam:participant:Practitioner,CareTeam:participant:Patient,CareTeam:participant:RelatedPerson</t>
+  </si>
+  <si>
+    <t>* To search for an encounter diagnosis, query for Conditions that reference the Encounter of interest and have a category of `encounter-diagnosis`.
+    * When `Condition.category` is "encounter-diagnosis" the encounter, **SHOULD** be referenced in `Condition.encounter`.
+* See SDOH Guidance for more information when exchanging Social Determinants of Health (SDOH) Conditions/Health Concerns.
+* There is no single element in Condition that represents the date of diagnosis. It may be the assertedDate Extension, `Condition.onsetDate`, or `Condition.recordedDate`.
+    * Although all three are marked as must support, the server is not required to support all.
+	* A server **SHALL** support `Condition.recordedDate`.
+    * A server **SHALL** support at least one of [assertedDate Extension] and `Condition.onsetDate`. A server may support both, which means they support all 3 locations.
+    * The client application **SHALL** support all three elements.</t>
+  </si>
+  <si>
+    <t>Diagnostic imaging results in visual images requiring interpretation and clinical test results/reports may also reference images as part of the report. DiagnosticReport resource can link to both DICOM imaging studies and binary images directly by referencing ImagingStudy in `DocumentReference.imagingStudy`, or Media  in`DocumentReference.media`.
+   *   Although both are marked as must support, the server system is not required to support both, but **SHALL** support at least one of these elements.
+   * The client application **SHALL** support both elements and target resources.</t>
+  </si>
+  <si>
+    <t>* Systems **SHOULD** support `Observation.effectivePeriod` to accurately represent tests that are collected over a period of time (for example, a 24-Hour Urine Collection test).
+* An Observation without a value, **SHALL** include a reason why the data is absent unless there are component observations, or references to other Observations that are grouped within it
+    * Systems that never provide an observation without a value are not required to support `Observation.dataAbsentReason`
+*  An `Observation.component` without a value, **SHALL** include a reason why the data is absent.
+    * Systems that never provide an component observation without a component value are not required to support `Observation.component.dataAbsentReason`.</t>
+  </si>
+  <si>
+    <t>conf_RelatedPerson</t>
+  </si>
+  <si>
+    <t>conf_ServiceRequest</t>
+  </si>
+  <si>
+    <t>is_new</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>discharge-disposition</t>
+  </si>
+  <si>
+    <t>A server **SHALL** support a value precise to the *day*.</t>
+  </si>
+  <si>
+    <t>support searching for a patient by a server defined search that matches any of the string fields in the HumanName, including family, give, prefix, suffix, suffix, and/or text</t>
+  </si>
+  <si>
+    <t>asserted-date</t>
+  </si>
+  <si>
+    <t>recorded-date</t>
+  </si>
+  <si>
+    <t>abatement-date</t>
+  </si>
+  <si>
+    <t>support searching for all encounter diagnosis for a patient for an encounter</t>
+  </si>
+  <si>
+    <t>DOES THIS DO ANYTHING?</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>support searching a careteam by participant role</t>
+  </si>
+  <si>
+    <t>authored</t>
+  </si>
+  <si>
+    <t>support fetching a ServiceRequest</t>
+  </si>
+  <si>
+    <t>GET [base]/ServiceRequest/1032702~GET [base]/ServiceRequest?_id=1032702</t>
+  </si>
+  <si>
+    <t>support fetching a RelatedPerson</t>
+  </si>
+  <si>
+    <t>GET [base]/RelatedPerson/shaw-niece~GET [base]/RelatedPerson?_id=shaw-niece</t>
+  </si>
+  <si>
+    <t>patient,location</t>
+  </si>
+  <si>
+    <t>GET [base]/Encounter?patient=1137192&amp;location=Location/hospital</t>
+  </si>
+  <si>
+    <t>patient,discharge-disposition</t>
+  </si>
+  <si>
+    <t>GET [base]/Encounter?patient=example1&amp;discharge-disposition=01</t>
+  </si>
+  <si>
+    <t>patient,category,encounter</t>
+  </si>
+  <si>
+    <t>GET [base]/Condition?patient=1032702&amp;category=http://terminology.hl7.org/CodeSystem/condition-category\|encounter-diagnosis?encounter=1036</t>
+  </si>
+  <si>
+    <t>Fetches a bundle of all Condition resources for the specified patient and category and encounter. When category = "encounter-diagnosis" will return the encounter diagnosis for the encounter.</t>
+  </si>
+  <si>
+    <t>GET [base]Condition?patient=555580&amp;onset-date=ge2018-01-14</t>
+  </si>
+  <si>
+    <t>patient,asserted-date</t>
+  </si>
+  <si>
+    <t>GET [base]Condition?patient=555580&amp;asserted-date=ge2018-01-14</t>
+  </si>
+  <si>
+    <t>patient,recorded-date</t>
+  </si>
+  <si>
+    <t>GET [base]Condition?patient=555580&amp;recorded-date=ge2018-01-14</t>
+  </si>
+  <si>
+    <t>patient,abatement-date</t>
+  </si>
+  <si>
+    <t>GET [base]Condition?patient=555580&amp;abatement-date=ge2018-01-14</t>
+  </si>
+  <si>
+    <t>support searching for all current care team members for a patient. DOES THIS DO ANYTHING?</t>
+  </si>
+  <si>
+    <t>GET [base]/CareTeam?patient=1137192&amp;status=active~GET [base]/CareTeam?patient=1137192&amp;status=active&amp;_include=CareTeam:participant:RelatedPerson&amp;_include=CareTeam:participant:Patient&amp;_include=CareTeam:participant:Practitioner&amp;_include=CareTeam:participant:PractitionerRole</t>
+  </si>
+  <si>
+    <t>Fetches a bundle of all CareTeam resources for the specified patient and status =`active` and may include CareTeam Patient, RelatedPerson and Practitioner and PractitionerRole participants.  
+To get Practitioner name and identifier using PractitionerRole:  
+1) Search for the careteam PractitionerRole: GET [base]/CareTeam?patient=[id]&amp;status=active&amp;_include=CareTeam:participant:PractitionerRole  
+2) using the FHIR _id from the PractitionerRole.practitioner element resource,  fetch the Practitioner resources using  GET [base]/Practitioner?_id=[id]</t>
+  </si>
+  <si>
+    <t>patient,role</t>
+  </si>
+  <si>
+    <t>support searching for all current care team member roles for a patient. DOES THIS DO ANYTHING?</t>
+  </si>
+  <si>
+    <t>GET [base]/CareTeam?patient=1137192&amp;role=http://snomed.info/sct\|17561000</t>
+  </si>
+  <si>
+    <t>Fetches a bundle of all CareTeam resources for the specified patient and participant role</t>
+  </si>
+  <si>
+    <t>GET [base]/ServiceRequest?patient=1137192&amp;status=completed</t>
+  </si>
+  <si>
+    <t>GET [base]/ServiceRequest?patient=f201&amp;category=http://loinc.org\|LG41762-2</t>
+  </si>
+  <si>
+    <t>GET [base]/ServiceRequest?patient=1032702&amp;code=http://snomed.info/sct\|35637008</t>
+  </si>
+  <si>
+    <t>patient,category,authored</t>
+  </si>
+  <si>
+    <t>GET [base]/ServiceRequest?patient=f201&amp;category=http://loinc.org\|LG41762-2&amp;date=ge2010-01-14T00:00:00Z</t>
+  </si>
+  <si>
+    <t>patient,code,authored</t>
+  </si>
+  <si>
+    <t>support searching for reports by code and date DOES THIS DO ANYTHING!!!!</t>
+  </si>
+  <si>
+    <t>GET [base]/ServiceRequest?patient=f201&amp;code=http://snomed.info/sct\|35637008&amp;date=ge2019-01-14T00:00:00Z</t>
+  </si>
+  <si>
+    <t>patient,description</t>
+  </si>
+  <si>
+    <t>support searching for all goals for a patient by date DOES THIS DO ANYTHING!!!</t>
+  </si>
+  <si>
+    <t>GET [base]/Goal?patient=1137192&amp;description=http://snomed.info/sct\|1078229009</t>
+  </si>
+  <si>
+    <t>* The Encounter resource can represent a reason using either a code with `Encounter.reasonCode`, or a reference with `Encounter.reasonReference` to  Condition or other resource.
+   * Although both are marked as must support, the server systems are not required to support both a code and a reference, but they **SHALL** support *at least one* of these elements.
+   * The client application **SHALL** support both elements.
+   * if `Encounter.reasonReference` references an Observation, it **SHOULD** conform to a US Core Observation if applicable. (for example, a laboratory result should conform to the US Core Laboratory Result Observation Profile)
+* The intent of this profile is to support *where the encounter occurred*.  The location address can be represented by either by the Location referenced by `Encounter.location.location` or indirectly through the Organization referenced by `Encounter.serviceProvider`.
+  * Although both are marked as must support, the server systems are not required to support both `Encounter.location.location` and `Encounter.serviceProvider`, but they **SHALL** support *at least one* of these elements.
+  * The client application **SHALL** support both elements.
+  * if using `Encounter.location.location` it **SHOULD** conform to US Core Location.  However, as a result of implementation feedback, it **MAY**  reference the base FHIR Location resource.  See this guidance on Referencing US Core Profiles</t>
+  </si>
+  <si>
+    <t>Documents/FHIR/US-Core/input/</t>
+  </si>
+  <si>
+    <t>HL7 International - Cross-Group Projects</t>
+  </si>
+  <si>
+    <t>http://www.hl7.org/Special/committees/cgp</t>
+  </si>
+  <si>
+    <t>!http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</t>
+  </si>
+  <si>
+    <t>!http://hl7.org/fhir/us/core/StructureDefinition/us-core-direct</t>
+  </si>
+  <si>
+    <t>US Core Direct email Extension</t>
+  </si>
+  <si>
+    <t>Extension</t>
+  </si>
+  <si>
+    <t>!http://hl7.org/fhir/us/core/StructureDefinition/us-core-race</t>
+  </si>
+  <si>
+    <t>US Core Race Extension</t>
+  </si>
+  <si>
+    <t>!http://hl7.org/fhir/us/core/StructureDefinition/us-core-birthsex</t>
+  </si>
+  <si>
+    <t>US Core Birth Sex Extension</t>
+  </si>
+  <si>
+    <t>!http://hl7.org/fhir/us/core/StructureDefinition/us-core-genderIdentity</t>
+  </si>
+  <si>
+    <t>US Core Gender Identity Extension</t>
+  </si>
+  <si>
+    <t>!http://hl7.org/fhir/us/core/StructureDefinition/us-core-ethnicity</t>
+  </si>
+  <si>
+    <t>US Core Ethnicity Extension</t>
+  </si>
+  <si>
+    <t>!http://hl7.org/fhir/us/core/StructureDefinition/us-core-extension-questionnaire-uri</t>
+  </si>
+  <si>
+    <t>US Core Extension Questionnaire URI</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-sdoh-assessment</t>
+  </si>
+  <si>
+    <t>US Core Observation SDOH Assessment Profile</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-social-history</t>
+  </si>
+  <si>
+    <t>US Core Observation Social History Profile</t>
+  </si>
+  <si>
+    <t>US Core Observation Sexual Orientation Profile</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-survey</t>
+  </si>
+  <si>
+    <t>US Core Observation Survey Profile</t>
+  </si>
+  <si>
+    <t>US Core Observation Imaging Result Profile</t>
+  </si>
+  <si>
+    <t>US Core Observation Clinical Test Result Profile</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</t>
+  </si>
+  <si>
+    <t>US Core QuestionnaireResponse Profile</t>
+  </si>
+  <si>
+    <t>QuestionnaireResponse</t>
+  </si>
+  <si>
+    <t>US Core provides two ways to represent SDOH assessment screening results using: 
+1. Observation: [US Core Observation SDOH Assessment Profile] 
+1. QuestionnaireResponse: [US Core QuestionnaireResponse Profile]
+US Core Servers **SHALL** support [US Core Observation SDOH Assessment Profile] for SDOH Assessments and **MAY** support the [US Core QuestionnaireResponse Profile] for SDOH Assessments.</t>
+  </si>
+  <si>
+    <t>conf_QuestionnaireResponse</t>
+  </si>
+  <si>
+    <t>GET [base]/QuestionnaireResponse/AHC-HRSN-screening-example~GET [base]/QuestionnaireResponse/?_id=AHC-HRSN-screening-example</t>
+  </si>
+  <si>
+    <t>Allows retrieving QuestionnaireResponses that are complete (or incomplete)</t>
+  </si>
+  <si>
+    <t>_tag</t>
+  </si>
+  <si>
+    <t>QuestionnaireResponse.meta._tag</t>
+  </si>
+  <si>
+    <t>Allows filtering for QuestionnaireResponse that have tag of “sdoh”</t>
+  </si>
+  <si>
+    <t>Allows filtering for QuestionnaireResponses by when they were created/last edited</t>
+  </si>
+  <si>
+    <t>questionnaire</t>
+  </si>
+  <si>
+    <t>Allows retrieving QuestionnaireResponses that have been completed against a specified form</t>
+  </si>
+  <si>
+    <t>combo description field ...DOES THIS DO ANYTHING?</t>
+  </si>
+  <si>
+    <t>GET [base]/QuestionnaireResponse?patient=1137192&amp;status=completed</t>
+  </si>
+  <si>
+    <t>patient,_tag</t>
+  </si>
+  <si>
+    <t>_tag=sdoh</t>
+  </si>
+  <si>
+    <t>GET [base]/QuestionnaireResponse?patient=1137192&amp;_tag=sdoh</t>
+  </si>
+  <si>
+    <t>patient,authored</t>
+  </si>
+  <si>
+    <t>GET [base]/QuestionnaireResponse?patient=113192&amp;date=ge2021</t>
+  </si>
+  <si>
+    <t>patient,_tag,authored</t>
+  </si>
+  <si>
+    <t>GET [base]/QuestionnaireResponse?patient=113192&amp;date=ge2021&amp;_tag=sdoh</t>
+  </si>
+  <si>
+    <t>patient,questionnaire</t>
+  </si>
+  <si>
+    <t>GET [base]/QuestionnaireResponse?patient=113192&amp;questionnaire=http://hl7.org/fhir/us/sdoh-clinicalcare/Questionnaire/SDOHCC-QuestionnaireHungerVitalSign</t>
+  </si>
+  <si>
     <t>* Implantable medical devices that have UDI information **SHALL** represent the UDI code in `Device.udiCarrier.carrierHRF`.
    - All of the five UDI-PI elements that are present in the UDI code **SHALL** be represented in the corresponding US Core Implantable Device Profile element.
    UDI may not be present in all scenarios such as historical implantable devices, patient reported implant information, payer reported devices, or improperly documented implants. If UDI is not present and the manufacturer and/or model number information is available, they **SHOULD** be included to support historical reports of implantable medical devices as follows:
-    &lt;table&gt;
-    &lt;thead&gt;
-    &lt;tr class="header"&gt;
-    &lt;th&gt;data element&lt;/th&gt;
-    &lt;th&gt;US Core Implantable Device Profile element&lt;/th&gt;
-    &lt;/tr&gt;
-    &lt;/thead&gt;
-    &lt;tbody&gt;
-    &lt;tr class="odd"&gt;
-    &lt;td&gt;manufacturer&lt;/td&gt;
-    &lt;td&gt;Device.manufacturer&lt;/td&gt;
-    &lt;/tr&gt;
-    &lt;tr class="even"&gt;
-    &lt;td&gt;model&lt;/td&gt;
-    &lt;td&gt;Device.model&lt;/td&gt;
-    &lt;/tr&gt;
-    &lt;/tbody&gt;
-    &lt;/table&gt;
+   manufacturer -&gt; `Device.manufacturer`  
+   model -&gt; `Device.model`  
 * Servers **SHOULD** support query by Device.type to allow clients to request the patient's devices by a specific type. Note: The Device.type is too granular to differentiate implantable vs. non-implantable devices.  
 * In the Quick Start section below, searching for all devices is described. Records of implanted devices **MAY** be queried against UDI data including:
     - UDI HRF string (`udi-carrier`)
@@ -1871,412 +2261,6 @@
     - expiration date
     - manufacture date
     - distinct identifier</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/uv/bulkdata/ImplementationGuide/hl7.fhir.uv.bulkdata</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/smart-app-launch/index.html</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/uv/bulkdata/index.html</t>
-  </si>
-  <si>
-    <t>CapabilityStatement-us-core-client.html</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-sexual-orientation</t>
-  </si>
-  <si>
-    <t>5.0.0</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/smart-app-launch/ImplementationGuide/hl7.fhir.uv.smart-app-launch</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-clinical-test</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-relatedperson</t>
-  </si>
-  <si>
-    <t>US Core RelatedPerson Profile</t>
-  </si>
-  <si>
-    <t>RelatedPerson</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</t>
-  </si>
-  <si>
-    <t>US Core ServiceRequest Profile</t>
-  </si>
-  <si>
-    <t>ServiceRequest</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-imaging</t>
-  </si>
-  <si>
-    <t>resolves</t>
-  </si>
-  <si>
-    <t>In order to access care team member's names, identifiers, locations, and contact information, the CareTeam profile supports several types of care team participants. They are represented as references to other profiles and include the following four profiles which are marked as must support:
-  1. US Core Practitioner Profile
-  1. US Core PractitionerRole Profile
-  1. US Core Patient Profile
-  1. US Core RelatedPerson Profile
-  * Although *both* US Core Practitioner Profile and US Core PractitionerRole are must support, the server system is not required to support both types of references (and `_include` search parameters), but **SHALL** support *at least* one of them.
-  * The client application **SHALL** support all four profile references.
-  * Bacause the US Core PractitionerRole Profile supplies the provider's location and contact information and a reference to the Practitioner, server systems **SHOULD** reference it instead of the US Core Practitioner Profile. An example of how to access the practitioner name and identifier is shown in the quick start section below.
-  * Servers that supports only US Core Practitioner Profile **SHALL** provide implementation specific guidance how to access a provider's location and contact information using only the Practitioner resource.</t>
-  </si>
-  <si>
-    <t>SHOULD,SHOULD,SHOULD,SHOULD</t>
-  </si>
-  <si>
-    <t>CareTeam:participant:PractitionerRole,CareTeam:participant:Practitioner,CareTeam:participant:Patient,CareTeam:participant:RelatedPerson</t>
-  </si>
-  <si>
-    <t>* To search for an encounter diagnosis, query for Conditions that reference the Encounter of interest and have a category of `encounter-diagnosis`.
-    * When `Condition.category` is "encounter-diagnosis" the encounter, **SHOULD** be referenced in `Condition.encounter`.
-* See SDOH Guidance for more information when exchanging Social Determinants of Health (SDOH) Conditions/Health Concerns.
-* There is no single element in Condition that represents the date of diagnosis. It may be the assertedDate Extension, `Condition.onsetDate`, or `Condition.recordedDate`.
-    * Although all three are marked as must support, the server is not required to support all.
-	* A server **SHALL** support `Condition.recordedDate`.
-    * A server **SHALL** support at least one of [assertedDate Extension] and `Condition.onsetDate`. A server may support both, which means they support all 3 locations.
-    * The client application **SHALL** support all three elements.</t>
-  </si>
-  <si>
-    <t>Diagnostic imaging results in visual images requiring interpretation and clinical test results/reports may also reference images as part of the report. DiagnosticReport resource can link to both DICOM imaging studies and binary images directly by referencing ImagingStudy in `DocumentReference.imagingStudy`, or Media  in`DocumentReference.media`.
-   *   Although both are marked as must support, the server system is not required to support both, but **SHALL** support at least one of these elements.
-   * The client application **SHALL** support both elements and target resources.</t>
-  </si>
-  <si>
-    <t>* Systems **SHOULD** support `Observation.effectivePeriod` to accurately represent tests that are collected over a period of time (for example, a 24-Hour Urine Collection test).
-* An Observation without a value, **SHALL** include a reason why the data is absent unless there are component observations, or references to other Observations that are grouped within it
-    * Systems that never provide an observation without a value are not required to support `Observation.dataAbsentReason`
-*  An `Observation.component` without a value, **SHALL** include a reason why the data is absent.
-    * Systems that never provide an component observation without a component value are not required to support `Observation.component.dataAbsentReason`.</t>
-  </si>
-  <si>
-    <t>conf_RelatedPerson</t>
-  </si>
-  <si>
-    <t>conf_ServiceRequest</t>
-  </si>
-  <si>
-    <t>is_new</t>
-  </si>
-  <si>
-    <t>location</t>
-  </si>
-  <si>
-    <t>discharge-disposition</t>
-  </si>
-  <si>
-    <t>A server **SHALL** support a value precise to the *day*.</t>
-  </si>
-  <si>
-    <t>support searching for a patient by a server defined search that matches any of the string fields in the HumanName, including family, give, prefix, suffix, suffix, and/or text</t>
-  </si>
-  <si>
-    <t>asserted-date</t>
-  </si>
-  <si>
-    <t>recorded-date</t>
-  </si>
-  <si>
-    <t>abatement-date</t>
-  </si>
-  <si>
-    <t>support searching for all encounter diagnosis for a patient for an encounter</t>
-  </si>
-  <si>
-    <t>DOES THIS DO ANYTHING?</t>
-  </si>
-  <si>
-    <t>role</t>
-  </si>
-  <si>
-    <t>support searching a careteam by participant role</t>
-  </si>
-  <si>
-    <t>authored</t>
-  </si>
-  <si>
-    <t>support fetching a ServiceRequest</t>
-  </si>
-  <si>
-    <t>GET [base]/ServiceRequest/1032702~GET [base]/ServiceRequest?_id=1032702</t>
-  </si>
-  <si>
-    <t>support fetching a RelatedPerson</t>
-  </si>
-  <si>
-    <t>GET [base]/RelatedPerson/shaw-niece~GET [base]/RelatedPerson?_id=shaw-niece</t>
-  </si>
-  <si>
-    <t>patient,location</t>
-  </si>
-  <si>
-    <t>GET [base]/Encounter?patient=1137192&amp;location=Location/hospital</t>
-  </si>
-  <si>
-    <t>patient,discharge-disposition</t>
-  </si>
-  <si>
-    <t>GET [base]/Encounter?patient=example1&amp;discharge-disposition=01</t>
-  </si>
-  <si>
-    <t>patient,category,encounter</t>
-  </si>
-  <si>
-    <t>GET [base]/Condition?patient=1032702&amp;category=http://terminology.hl7.org/CodeSystem/condition-category\|encounter-diagnosis?encounter=1036</t>
-  </si>
-  <si>
-    <t>Fetches a bundle of all Condition resources for the specified patient and category and encounter. When category = "encounter-diagnosis" will return the encounter diagnosis for the encounter.</t>
-  </si>
-  <si>
-    <t>GET [base]Condition?patient=555580&amp;onset-date=ge2018-01-14</t>
-  </si>
-  <si>
-    <t>patient,asserted-date</t>
-  </si>
-  <si>
-    <t>GET [base]Condition?patient=555580&amp;asserted-date=ge2018-01-14</t>
-  </si>
-  <si>
-    <t>patient,recorded-date</t>
-  </si>
-  <si>
-    <t>GET [base]Condition?patient=555580&amp;recorded-date=ge2018-01-14</t>
-  </si>
-  <si>
-    <t>patient,abatement-date</t>
-  </si>
-  <si>
-    <t>GET [base]Condition?patient=555580&amp;abatement-date=ge2018-01-14</t>
-  </si>
-  <si>
-    <t>support searching for all current care team members for a patient. DOES THIS DO ANYTHING?</t>
-  </si>
-  <si>
-    <t>GET [base]/CareTeam?patient=1137192&amp;status=active~GET [base]/CareTeam?patient=1137192&amp;status=active&amp;_include=CareTeam:participant:RelatedPerson&amp;_include=CareTeam:participant:Patient&amp;_include=CareTeam:participant:Practitioner&amp;_include=CareTeam:participant:PractitionerRole</t>
-  </si>
-  <si>
-    <t>Fetches a bundle of all CareTeam resources for the specified patient and status =`active` and may include CareTeam Patient, RelatedPerson and Practitioner and PractitionerRole participants.  
-To get Practitioner name and identifier using PractitionerRole:  
-1) Search for the careteam PractitionerRole: GET [base]/CareTeam?patient=[id]&amp;status=active&amp;_include=CareTeam:participant:PractitionerRole  
-2) using the FHIR _id from the PractitionerRole.practitioner element resource,  fetch the Practitioner resources using  GET [base]/Practitioner?_id=[id]</t>
-  </si>
-  <si>
-    <t>patient,role</t>
-  </si>
-  <si>
-    <t>support searching for all current care team member roles for a patient. DOES THIS DO ANYTHING?</t>
-  </si>
-  <si>
-    <t>GET [base]/CareTeam?patient=1137192&amp;role=http://snomed.info/sct\|17561000</t>
-  </si>
-  <si>
-    <t>Fetches a bundle of all CareTeam resources for the specified patient and participant role</t>
-  </si>
-  <si>
-    <t>GET [base]/ServiceRequest?patient=1137192&amp;status=completed</t>
-  </si>
-  <si>
-    <t>GET [base]/ServiceRequest?patient=f201&amp;category=http://loinc.org\|LG41762-2</t>
-  </si>
-  <si>
-    <t>GET [base]/ServiceRequest?patient=1032702&amp;code=http://snomed.info/sct\|35637008</t>
-  </si>
-  <si>
-    <t>patient,category,authored</t>
-  </si>
-  <si>
-    <t>GET [base]/ServiceRequest?patient=f201&amp;category=http://loinc.org\|LG41762-2&amp;date=ge2010-01-14T00:00:00Z</t>
-  </si>
-  <si>
-    <t>patient,code,authored</t>
-  </si>
-  <si>
-    <t>support searching for reports by code and date DOES THIS DO ANYTHING!!!!</t>
-  </si>
-  <si>
-    <t>GET [base]/ServiceRequest?patient=f201&amp;code=http://snomed.info/sct\|35637008&amp;date=ge2019-01-14T00:00:00Z</t>
-  </si>
-  <si>
-    <t>patient,description</t>
-  </si>
-  <si>
-    <t>support searching for all goals for a patient by date DOES THIS DO ANYTHING!!!</t>
-  </si>
-  <si>
-    <t>GET [base]/Goal?patient=1137192&amp;description=http://snomed.info/sct\|1078229009</t>
-  </si>
-  <si>
-    <t>* The Encounter resource can represent a reason using either a code with `Encounter.reasonCode`, or a reference with `Encounter.reasonReference` to  Condition or other resource.
-   * Although both are marked as must support, the server systems are not required to support both a code and a reference, but they **SHALL** support *at least one* of these elements.
-   * The client application **SHALL** support both elements.
-   * if `Encounter.reasonReference` references an Observation, it **SHOULD** conform to a US Core Observation if applicable. (for example, a laboratory result should conform to the US Core Laboratory Result Observation Profile)
-* The intent of this profile is to support *where the encounter occurred*.  The location address can be represented by either by the Location referenced by `Encounter.location.location` or indirectly through the Organization referenced by `Encounter.serviceProvider`.
-  * Although both are marked as must support, the server systems are not required to support both `Encounter.location.location` and `Encounter.serviceProvider`, but they **SHALL** support *at least one* of these elements.
-  * The client application **SHALL** support both elements.
-  * if using `Encounter.location.location` it **SHOULD** conform to US Core Location.  However, as a result of implementation feedback, it **MAY**  reference the base FHIR Location resource.  See this guidance on Referencing US Core Profiles</t>
-  </si>
-  <si>
-    <t>Documents/FHIR/US-Core/input/</t>
-  </si>
-  <si>
-    <t>HL7 International - Cross-Group Projects</t>
-  </si>
-  <si>
-    <t>http://www.hl7.org/Special/committees/cgp</t>
-  </si>
-  <si>
-    <t>!http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</t>
-  </si>
-  <si>
-    <t>!http://hl7.org/fhir/us/core/StructureDefinition/us-core-direct</t>
-  </si>
-  <si>
-    <t>US Core Direct email Extension</t>
-  </si>
-  <si>
-    <t>Extension</t>
-  </si>
-  <si>
-    <t>!http://hl7.org/fhir/us/core/StructureDefinition/us-core-race</t>
-  </si>
-  <si>
-    <t>US Core Race Extension</t>
-  </si>
-  <si>
-    <t>!http://hl7.org/fhir/us/core/StructureDefinition/us-core-birthsex</t>
-  </si>
-  <si>
-    <t>US Core Birth Sex Extension</t>
-  </si>
-  <si>
-    <t>!http://hl7.org/fhir/us/core/StructureDefinition/us-core-genderIdentity</t>
-  </si>
-  <si>
-    <t>US Core Gender Identity Extension</t>
-  </si>
-  <si>
-    <t>!http://hl7.org/fhir/us/core/StructureDefinition/us-core-ethnicity</t>
-  </si>
-  <si>
-    <t>US Core Ethnicity Extension</t>
-  </si>
-  <si>
-    <t>!http://hl7.org/fhir/us/core/StructureDefinition/us-core-extension-questionnaire-uri</t>
-  </si>
-  <si>
-    <t>US Core Extension Questionnaire URI</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-sdoh-assessment</t>
-  </si>
-  <si>
-    <t>US Core Observation SDOH Assessment Profile</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-social-history</t>
-  </si>
-  <si>
-    <t>US Core Observation Social History Profile</t>
-  </si>
-  <si>
-    <t>US Core Observation Sexual Orientation Profile</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-survey</t>
-  </si>
-  <si>
-    <t>US Core Observation Survey Profile</t>
-  </si>
-  <si>
-    <t>US Core Observation Imaging Result Profile</t>
-  </si>
-  <si>
-    <t>US Core Observation Clinical Test Result Profile</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</t>
-  </si>
-  <si>
-    <t>US Core QuestionnaireResponse Profile</t>
-  </si>
-  <si>
-    <t>QuestionnaireResponse</t>
-  </si>
-  <si>
-    <t>US Core provides two ways to represent SDOH assessment screening results using: 
-1. Observation: [US Core Observation SDOH Assessment Profile] 
-1. QuestionnaireResponse: [US Core QuestionnaireResponse Profile]
-US Core Servers **SHALL** support [US Core Observation SDOH Assessment Profile] for SDOH Assessments and **MAY** support the [US Core QuestionnaireResponse Profile] for SDOH Assessments.</t>
-  </si>
-  <si>
-    <t>conf_QuestionnaireResponse</t>
-  </si>
-  <si>
-    <t>GET [base]/QuestionnaireResponse/AHC-HRSN-screening-example~GET [base]/QuestionnaireResponse/?_id=AHC-HRSN-screening-example</t>
-  </si>
-  <si>
-    <t>Allows retrieving QuestionnaireResponses that are complete (or incomplete)</t>
-  </si>
-  <si>
-    <t>_tag</t>
-  </si>
-  <si>
-    <t>QuestionnaireResponse.meta._tag</t>
-  </si>
-  <si>
-    <t>Allows filtering for QuestionnaireResponse that have tag of “sdoh”</t>
-  </si>
-  <si>
-    <t>Allows filtering for QuestionnaireResponses by when they were created/last edited</t>
-  </si>
-  <si>
-    <t>questionnaire</t>
-  </si>
-  <si>
-    <t>Allows retrieving QuestionnaireResponses that have been completed against a specified form</t>
-  </si>
-  <si>
-    <t>combo description field ...DOES THIS DO ANYTHING?</t>
-  </si>
-  <si>
-    <t>GET [base]/QuestionnaireResponse?patient=1137192&amp;status=completed</t>
-  </si>
-  <si>
-    <t>patient,_tag</t>
-  </si>
-  <si>
-    <t>_tag=sdoh</t>
-  </si>
-  <si>
-    <t>GET [base]/QuestionnaireResponse?patient=1137192&amp;_tag=sdoh</t>
-  </si>
-  <si>
-    <t>patient,authored</t>
-  </si>
-  <si>
-    <t>GET [base]/QuestionnaireResponse?patient=113192&amp;date=ge2021</t>
-  </si>
-  <si>
-    <t>patient,_tag,authored</t>
-  </si>
-  <si>
-    <t>GET [base]/QuestionnaireResponse?patient=113192&amp;date=ge2021&amp;_tag=sdoh</t>
-  </si>
-  <si>
-    <t>patient,questionnaire</t>
-  </si>
-  <si>
-    <t>GET [base]/QuestionnaireResponse?patient=113192&amp;questionnaire=http://hl7.org/fhir/us/sdoh-clinicalcare/Questionnaire/SDOHCC-QuestionnaireHungerVitalSign</t>
   </si>
 </sst>
 </file>
@@ -2852,7 +2836,7 @@
         <v>468</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -2884,7 +2868,7 @@
         <v>63</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -2900,7 +2884,7 @@
         <v>475</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -2977,7 +2961,7 @@
         <v>39</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>30</v>
@@ -3933,7 +3917,7 @@
         <v>20</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>28</v>
@@ -4094,7 +4078,7 @@
         <v>20</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>28</v>
@@ -4253,7 +4237,7 @@
         <v>0</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="G25" s="1" t="str">
         <f t="shared" si="1"/>
@@ -4471,7 +4455,7 @@
         <v>51</v>
       </c>
       <c r="Y29" s="5" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="Z29" s="1" t="s">
         <v>168</v>
@@ -4869,7 +4853,7 @@
         <v>133</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>28</v>
@@ -4926,7 +4910,7 @@
         <v>133</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>28</v>
@@ -4983,7 +4967,7 @@
         <v>133</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>28</v>
@@ -5128,7 +5112,7 @@
         <v>51</v>
       </c>
       <c r="Y42" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="Z42" s="5" t="str">
         <f>"GET [base]/"&amp;B42&amp;"?patient=1137192"</f>
@@ -7333,7 +7317,7 @@
         <v>51</v>
       </c>
       <c r="X83" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="Y83" s="1" t="str">
         <f>"support searching for all "&amp;LOWER(B83)&amp;"s for a patient"</f>
@@ -7403,7 +7387,7 @@
         <v>GET [base]/Practitioner/practitioner-1~GET [base]/Practitioner?_id=practitioner-1</v>
       </c>
       <c r="AA84" s="10" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="AB84" s="1" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B84)&amp;"-"&amp;SUBSTITUTE(C84,"_","")&amp;".html")</f>
@@ -7471,7 +7455,7 @@
         <v>243</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>65</v>
@@ -7512,7 +7496,7 @@
         <v>51</v>
       </c>
       <c r="Y86" s="5" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="Z86" s="5" t="str">
         <f>"GET [base]/"&amp;B86&amp;"?"&amp;C86&amp;"=http://snomed.info/sct\|17561000"</f>
@@ -8424,7 +8408,7 @@
         <v>49</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>57</v>
@@ -8480,7 +8464,7 @@
         <v>50</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>85</v>
@@ -8542,7 +8526,7 @@
         <v>51</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>135</v>
@@ -8595,7 +8579,7 @@
         <v>52</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>24</v>
@@ -8651,10 +8635,10 @@
         <v>53</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>28</v>
@@ -8708,7 +8692,7 @@
         <v>20</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>50</v>
@@ -8746,10 +8730,10 @@
         <v>51</v>
       </c>
       <c r="Y108" s="5" t="s">
+        <v>588</v>
+      </c>
+      <c r="Z108" s="5" t="s">
         <v>589</v>
-      </c>
-      <c r="Z108" s="5" t="s">
-        <v>590</v>
       </c>
       <c r="AB108" s="1" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B108)&amp;"-"&amp;SUBSTITUTE(C108,"_","")&amp;".html")</f>
@@ -8810,7 +8794,7 @@
         <v>20</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>50</v>
@@ -8848,10 +8832,10 @@
         <v>51</v>
       </c>
       <c r="Y110" s="5" t="s">
+        <v>590</v>
+      </c>
+      <c r="Z110" s="5" t="s">
         <v>591</v>
-      </c>
-      <c r="Z110" s="5" t="s">
-        <v>592</v>
       </c>
       <c r="AA110" s="10"/>
       <c r="AB110" s="1" t="str">
@@ -8864,7 +8848,7 @@
         <v>79</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>85</v>
@@ -8926,7 +8910,7 @@
         <v>80</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>50</v>
@@ -8965,7 +8949,7 @@
         <v>support fetching a QuestionnaireResponse</v>
       </c>
       <c r="Z112" s="5" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="AB112" s="1" t="str">
         <f t="shared" ref="AB112:AB117" si="25">"SearchParameter-us-core-"&amp;LOWER((B112)&amp;"-"&amp;SUBSTITUTE(C112,"_","")&amp;".html")</f>
@@ -8977,7 +8961,7 @@
         <v>81</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>85</v>
@@ -9036,7 +9020,7 @@
         <v>82</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>57</v>
@@ -9077,7 +9061,7 @@
         <v>51</v>
       </c>
       <c r="Y114" s="22" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="AB114" s="1" t="str">
         <f t="shared" si="25"/>
@@ -9089,10 +9073,10 @@
         <v>83</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>28</v>
@@ -9117,16 +9101,16 @@
         <v>52</v>
       </c>
       <c r="L115" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="M115" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O115" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y115" s="22" t="s">
         <v>660</v>
-      </c>
-      <c r="M115" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="O115" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y115" s="22" t="s">
-        <v>661</v>
       </c>
       <c r="AB115" s="1" t="str">
         <f t="shared" si="25"/>
@@ -9138,10 +9122,10 @@
         <v>84</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>28</v>
@@ -9182,7 +9166,7 @@
         <v>88</v>
       </c>
       <c r="Y116" s="22" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="AB116" s="1" t="str">
         <f t="shared" si="25"/>
@@ -9194,10 +9178,10 @@
         <v>85</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>28</v>
@@ -9232,7 +9216,7 @@
         <v>51</v>
       </c>
       <c r="Y117" s="22" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="AB117" s="1" t="str">
         <f t="shared" si="25"/>
@@ -9254,7 +9238,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:K102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I85" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="I85" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="I110" sqref="I110"/>
     </sheetView>
   </sheetViews>
@@ -9288,7 +9272,7 @@
         <v>91</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>92</v>
@@ -9718,7 +9702,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="E17" s="1" t="b">
         <v>1</v>
@@ -9733,7 +9717,7 @@
         <v>300</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="K17" s="5" t="str">
         <f t="shared" si="1"/>
@@ -9809,7 +9793,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="E20" s="1" t="b">
         <v>1</v>
@@ -9824,7 +9808,7 @@
         <v>305</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="K20" s="5" t="str">
         <f t="shared" si="1"/>
@@ -10290,7 +10274,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="E37" s="1" t="b">
         <v>1</v>
@@ -10305,10 +10289,10 @@
         <v>145</v>
       </c>
       <c r="J37" s="5" t="s">
+        <v>597</v>
+      </c>
+      <c r="K37" s="5" t="s">
         <v>598</v>
-      </c>
-      <c r="K37" s="5" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
@@ -10365,7 +10349,7 @@
         <v>148</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="K39" s="5" t="s">
         <v>151</v>
@@ -10383,7 +10367,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="E40" s="1" t="b">
         <v>1</v>
@@ -10398,7 +10382,7 @@
         <v>148</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="K40" s="5" t="s">
         <v>151</v>
@@ -10416,7 +10400,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E41" s="1" t="b">
         <v>1</v>
@@ -10431,7 +10415,7 @@
         <v>148</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="K41" s="5" t="s">
         <v>151</v>
@@ -10449,7 +10433,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="E42" s="1" t="b">
         <v>1</v>
@@ -10464,7 +10448,7 @@
         <v>148</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="K42" s="5" t="s">
         <v>151</v>
@@ -11561,13 +11545,13 @@
         <v>306</v>
       </c>
       <c r="I77" s="5" t="s">
+        <v>606</v>
+      </c>
+      <c r="J77" s="5" t="s">
         <v>607</v>
       </c>
-      <c r="J77" s="5" t="s">
+      <c r="K77" s="10" t="s">
         <v>608</v>
-      </c>
-      <c r="K77" s="10" t="s">
-        <v>609</v>
       </c>
     </row>
     <row r="78" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -11993,7 +11977,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="E91" s="1" t="b">
         <v>1</v>
@@ -12005,13 +11989,13 @@
         <v>101</v>
       </c>
       <c r="I91" s="5" t="s">
+        <v>610</v>
+      </c>
+      <c r="J91" s="5" t="s">
         <v>611</v>
       </c>
-      <c r="J91" s="5" t="s">
+      <c r="K91" s="5" t="s">
         <v>612</v>
-      </c>
-      <c r="K91" s="5" t="s">
-        <v>613</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.2">
@@ -12019,10 +12003,10 @@
         <v>56</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>111</v>
@@ -12040,7 +12024,7 @@
         <v>298</v>
       </c>
       <c r="J92" s="5" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="K92" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B92&amp;" resources for the specified "&amp;SUBSTITUTE(D92,","," and ")</f>
@@ -12052,10 +12036,10 @@
         <v>57</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>140</v>
@@ -12073,7 +12057,7 @@
         <v>193</v>
       </c>
       <c r="J93" s="5" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K93" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B93&amp;" resources for the specified patient and  a category code"</f>
@@ -12085,10 +12069,10 @@
         <v>58</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>142</v>
@@ -12106,7 +12090,7 @@
         <v>194</v>
       </c>
       <c r="J94" s="5" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="K94" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B94&amp;" resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes."</f>
@@ -12118,13 +12102,13 @@
         <v>59</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="E95" s="1" t="b">
         <v>1</v>
@@ -12139,7 +12123,7 @@
         <v>196</v>
       </c>
       <c r="J95" s="5" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="K95" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient and date and a category code"</f>
@@ -12151,13 +12135,13 @@
         <v>60</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="E96" s="1" t="b">
         <v>1</v>
@@ -12169,10 +12153,10 @@
         <v>213</v>
       </c>
       <c r="I96" s="5" t="s">
+        <v>619</v>
+      </c>
+      <c r="J96" s="5" t="s">
         <v>620</v>
-      </c>
-      <c r="J96" s="5" t="s">
-        <v>621</v>
       </c>
       <c r="K96" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B96&amp;" resources for the specified patient and date and service code(s).  SHOULD support search by multiple report codes."</f>
@@ -12191,7 +12175,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="E97" s="1" t="b">
         <v>1</v>
@@ -12203,10 +12187,10 @@
         <v>101</v>
       </c>
       <c r="I97" s="5" t="s">
+        <v>622</v>
+      </c>
+      <c r="J97" s="5" t="s">
         <v>623</v>
-      </c>
-      <c r="J97" s="5" t="s">
-        <v>624</v>
       </c>
       <c r="K97" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B97&amp;" resources for the specified "&amp;SUBSTITUTE(D97,","," and ")</f>
@@ -12218,10 +12202,10 @@
         <v>65</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="C98" s="21" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>111</v>
@@ -12233,10 +12217,10 @@
         <v>101</v>
       </c>
       <c r="I98" s="1" t="s">
+        <v>664</v>
+      </c>
+      <c r="J98" s="5" t="s">
         <v>665</v>
-      </c>
-      <c r="J98" s="5" t="s">
-        <v>666</v>
       </c>
       <c r="K98" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B98&amp;" resources for the specified "&amp;SUBSTITUTE(D98,","," and ")</f>
@@ -12248,13 +12232,13 @@
         <v>66</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="C99" s="21" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="F99" s="1" t="s">
         <v>65</v>
@@ -12263,13 +12247,13 @@
         <v>101</v>
       </c>
       <c r="H99" s="1" t="s">
+        <v>667</v>
+      </c>
+      <c r="I99" s="1" t="s">
+        <v>664</v>
+      </c>
+      <c r="J99" s="5" t="s">
         <v>668</v>
-      </c>
-      <c r="I99" s="1" t="s">
-        <v>665</v>
-      </c>
-      <c r="J99" s="5" t="s">
-        <v>669</v>
       </c>
       <c r="K99" s="1" t="str">
         <f>"Fetches a bundle of all "&amp;B99&amp;" resources for the specified "&amp;SUBSTITUTE(D99,","," and  ") &amp; "= 'sdoh'"</f>
@@ -12281,13 +12265,13 @@
         <v>67</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="C100" s="21" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>65</v>
@@ -12296,10 +12280,10 @@
         <v>144</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="J100" s="5" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="K100" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B100&amp;" resources for the specified patient and date"</f>
@@ -12311,13 +12295,13 @@
         <v>68</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="C101" s="21" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="D101" s="18" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>65</v>
@@ -12326,13 +12310,13 @@
         <v>213</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="J101" s="5" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="K101" s="1" t="str">
         <f>"Fetches a bundle of all "&amp;B101&amp;" resources tagged as 'sdoh' for the specified patient and date"</f>
@@ -12344,13 +12328,13 @@
         <v>69</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="C102" s="21" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="D102" s="18" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="F102" s="1" t="s">
         <v>65</v>
@@ -12359,10 +12343,10 @@
         <v>86</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="J102" s="5" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="K102" s="1" t="str">
         <f>"Fetches a bundle of all "&amp;B102&amp;" resources for the specified patient that have been completed against a specified form."</f>
@@ -12406,7 +12390,7 @@
         <v>62</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -12527,10 +12511,10 @@
         <v>540</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>65</v>
@@ -12541,10 +12525,10 @@
         <v>541</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>65</v>
@@ -12605,7 +12589,7 @@
         <v>545</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>11</v>
@@ -12806,7 +12790,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="21" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>362</v>
@@ -12822,96 +12806,96 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="21" t="s">
+        <v>629</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>630</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="D13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>631</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>632</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="21" t="s">
+        <v>632</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>633</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>634</v>
-      </c>
       <c r="D14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="21" t="s">
+        <v>634</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>635</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>636</v>
-      </c>
       <c r="D15" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="21" t="s">
+        <v>636</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>637</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>638</v>
-      </c>
       <c r="D16" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="21" t="s">
+        <v>638</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>639</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>640</v>
-      </c>
       <c r="D17" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="21" t="s">
+        <v>640</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>641</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>642</v>
-      </c>
       <c r="D18" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -13012,10 +12996,10 @@
     </row>
     <row r="25" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="21" t="s">
+        <v>642</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>643</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>644</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>11</v>
@@ -13040,10 +13024,10 @@
     </row>
     <row r="27" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="21" t="s">
+        <v>644</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>645</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>646</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>11</v>
@@ -13130,10 +13114,10 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="21" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>11</v>
@@ -13194,10 +13178,10 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="21" t="s">
+        <v>647</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>648</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>649</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>11</v>
@@ -13226,10 +13210,10 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="21" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>11</v>
@@ -13242,10 +13226,10 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="21" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>11</v>
@@ -13418,48 +13402,48 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="21" t="s">
+        <v>651</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>652</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="D51" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" s="1" t="s">
         <v>653</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>654</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="21" t="s">
+        <v>559</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>560</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="D52" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>561</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>562</v>
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="21" t="s">
+        <v>562</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>563</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="D53" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E53" s="1" t="s">
         <v>564</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>565</v>
       </c>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
@@ -13475,11 +13459,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Y62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E27" sqref="E27"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="23" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13587,7 +13571,7 @@
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="T2" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="U2" s="1" t="s">
         <v>65</v>
@@ -13610,7 +13594,7 @@
         <v>496</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="U3" s="1" t="s">
         <v>65</v>
@@ -13630,19 +13614,19 @@
         <v>65</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="V4" s="1" t="s">
         <v>568</v>
       </c>
-      <c r="T4" s="1" t="s">
-        <v>567</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="V4" s="1" t="s">
+      <c r="W4" s="1" t="s">
         <v>569</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>570</v>
       </c>
       <c r="X4" s="15" t="s">
         <v>455</v>
@@ -13659,10 +13643,10 @@
         <v>65</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="U5" s="1" t="s">
         <v>65</v>
@@ -13682,10 +13666,10 @@
         <v>65</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>551</v>
+        <v>675</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="U6" s="1" t="s">
         <v>65</v>
@@ -13705,10 +13689,10 @@
         <v>65</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="U7" s="1" t="s">
         <v>65</v>
@@ -13731,7 +13715,7 @@
         <v>406</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="U8" s="1" t="s">
         <v>65</v>
@@ -13751,10 +13735,10 @@
         <v>65</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="U9" s="1" t="s">
         <v>65</v>
@@ -13774,7 +13758,7 @@
         <v>65</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="U10" s="1" t="s">
         <v>65</v>
@@ -13797,7 +13781,7 @@
         <v>497</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="U11" s="1" t="s">
         <v>65</v>
@@ -13820,7 +13804,7 @@
         <v>498</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="U12" s="1" t="s">
         <v>65</v>
@@ -13839,7 +13823,7 @@
         <v>499</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="U13" s="1" t="s">
         <v>65</v>
@@ -13858,7 +13842,7 @@
         <v>500</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="U14" s="1" t="s">
         <v>65</v>
@@ -13887,7 +13871,7 @@
         <v>501</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="U15" s="1" t="s">
         <v>65</v>
@@ -13913,10 +13897,10 @@
         <v>65</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="T16" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="U16" s="1" t="s">
         <v>65</v>
@@ -13936,7 +13920,7 @@
         <v>65</v>
       </c>
       <c r="T17" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="U17" s="1" t="s">
         <v>65</v>
@@ -13955,7 +13939,7 @@
         <v>502</v>
       </c>
       <c r="T18" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="U18" s="1" t="s">
         <v>65</v>
@@ -13975,7 +13959,7 @@
         <v>65</v>
       </c>
       <c r="T19" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="U19" s="1" t="s">
         <v>65</v>
@@ -13994,7 +13978,7 @@
         <v>498</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="U20" s="1" t="s">
         <v>65</v>
@@ -14019,7 +14003,7 @@
         <v>503</v>
       </c>
       <c r="T21" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="U21" s="1" t="s">
         <v>65</v>
@@ -14042,7 +14026,7 @@
         <v>504</v>
       </c>
       <c r="T22" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="U22" s="1" t="s">
         <v>65</v>
@@ -14050,16 +14034,16 @@
     </row>
     <row r="23" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>654</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>655</v>
-      </c>
       <c r="T23" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="U23" s="1" t="s">
         <v>65</v>
@@ -14073,13 +14057,13 @@
     </row>
     <row r="24" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>65</v>
       </c>
       <c r="T24" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="U24" s="1" t="s">
         <v>65</v>
@@ -14093,13 +14077,13 @@
     </row>
     <row r="25" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>65</v>
       </c>
       <c r="T25" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="U25" s="1" t="s">
         <v>65</v>
@@ -14305,13 +14289,13 @@
         <v>434</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="Z1" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>574</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>575</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>454</v>

</xml_diff>

<commit_message>
qa update to client CapabilityStatement - missing profiles
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97AA98B6-9E3F-6842-BD31-0632E8CB070D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E4831E-60E4-9E4D-8E3C-1C08F5A7D707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2552" uniqueCount="676">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2548" uniqueCount="678">
   <si>
     <t>Element</t>
   </si>
@@ -1181,12 +1181,6 @@
   </si>
   <si>
     <t>US Core MedicationRequest Profile</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</t>
-  </si>
-  <si>
-    <t>US Core Condition Profile</t>
   </si>
   <si>
     <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-organization</t>
@@ -2262,12 +2256,24 @@
     - manufacture date
     - distinct identifier</t>
   </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core//StructureDefinition/us-core-condition-encounter-diagnosis</t>
+  </si>
+  <si>
+    <t>US Core Condition Encounter Diagnosis Profile</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core//StructureDefinition/us-core-condition-problems-health-concerns</t>
+  </si>
+  <si>
+    <t>US Core Condition Problems and Health Concerns Profile</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2364,14 +2370,6 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="16"/>
       <color rgb="FF333333"/>
       <name val="Helvetica Neue"/>
@@ -2419,10 +2417,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2455,13 +2452,12 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2813,7 +2809,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40F68824-E615-4729-AAE0-A6F75FBDE06B}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="400" zoomScaleNormal="400" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -2833,34 +2829,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -2868,12 +2864,12 @@
         <v>63</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>55</v>
@@ -2881,24 +2877,21 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>627</v>
+        <v>473</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>625</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="B9" s="1" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1" xr:uid="{F0F03EA1-31BA-804B-9035-810D43F90501}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2961,7 +2954,7 @@
         <v>39</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>30</v>
@@ -2985,19 +2978,19 @@
         <v>44</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="R1" s="4" t="s">
         <v>45</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="T1" s="4" t="s">
         <v>46</v>
       </c>
       <c r="U1" s="4" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="V1" s="4" t="s">
         <v>47</v>
@@ -3183,7 +3176,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="G5" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3391,7 +3384,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G9" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3440,7 +3433,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="G10" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3498,7 +3491,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G11" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3548,7 +3541,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G12" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3596,7 +3589,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="G13" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3707,7 +3700,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G15" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3757,7 +3750,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="G16" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3811,7 +3804,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G17" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3868,7 +3861,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="G18" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3917,7 +3910,7 @@
         <v>20</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>28</v>
@@ -3926,7 +3919,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="G19" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3987,7 +3980,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G20" s="1" t="str">
         <f t="shared" si="1"/>
@@ -4037,7 +4030,7 @@
         <v>0</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G21" s="1" t="str">
         <f t="shared" si="1"/>
@@ -4078,7 +4071,7 @@
         <v>20</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>28</v>
@@ -4087,7 +4080,7 @@
         <v>0</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G22" s="1" t="str">
         <f t="shared" si="1"/>
@@ -4190,7 +4183,7 @@
         <v>0</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="G24" s="1" t="str">
         <f t="shared" si="1"/>
@@ -4237,7 +4230,7 @@
         <v>0</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="G25" s="1" t="str">
         <f t="shared" si="1"/>
@@ -4283,7 +4276,7 @@
         <v>0</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G26" s="1" t="str">
         <f t="shared" si="1"/>
@@ -4375,7 +4368,7 @@
         <v>1</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G28" s="1" t="str">
         <f t="shared" si="1"/>
@@ -4455,7 +4448,7 @@
         <v>51</v>
       </c>
       <c r="Y29" s="5" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="Z29" s="1" t="s">
         <v>168</v>
@@ -4808,7 +4801,7 @@
         <v>0</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="G37" s="1" t="str">
         <f t="shared" si="1"/>
@@ -4853,7 +4846,7 @@
         <v>133</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>28</v>
@@ -4862,7 +4855,7 @@
         <v>0</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="G38" s="1" t="str">
         <f t="shared" si="1"/>
@@ -4910,7 +4903,7 @@
         <v>133</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>28</v>
@@ -4919,7 +4912,7 @@
         <v>0</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="G39" s="1" t="str">
         <f t="shared" si="1"/>
@@ -4967,7 +4960,7 @@
         <v>133</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>28</v>
@@ -4976,7 +4969,7 @@
         <v>0</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="G40" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5033,7 +5026,7 @@
         <v>0</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G41" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5074,7 +5067,7 @@
         <v>133</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>28</v>
@@ -5083,7 +5076,7 @@
         <v>0</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="G42" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5112,7 +5105,7 @@
         <v>51</v>
       </c>
       <c r="Y42" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="Z42" s="5" t="str">
         <f>"GET [base]/"&amp;B42&amp;"?patient=1137192"</f>
@@ -5144,7 +5137,7 @@
         <v>1</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="G43" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5203,7 +5196,7 @@
         <v>0</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G44" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5253,7 +5246,7 @@
         <v>0</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="G45" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5360,7 +5353,7 @@
         <v>0</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G47" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5413,7 +5406,7 @@
         <v>1</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="G48" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5472,7 +5465,7 @@
         <v>0</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G49" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5522,7 +5515,7 @@
         <v>0</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G50" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5572,7 +5565,7 @@
         <v>0</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="G51" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5626,7 +5619,7 @@
         <v>0</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="G52" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5679,7 +5672,7 @@
         <v>0</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G53" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5732,7 +5725,7 @@
         <v>1</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="G54" s="1" t="str">
         <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B54)</f>
@@ -5791,7 +5784,7 @@
         <v>0</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G55" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5841,7 +5834,7 @@
         <v>0</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G56" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5894,7 +5887,7 @@
         <v>0</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="G57" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5948,7 +5941,7 @@
         <v>0</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G58" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5998,7 +5991,7 @@
         <v>1</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="G59" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6048,7 +6041,7 @@
         <v>175</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>28</v>
@@ -6057,7 +6050,7 @@
         <v>0</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="G60" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6111,7 +6104,7 @@
         <v>0</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G61" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6155,7 +6148,7 @@
         <v>176</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>28</v>
@@ -6164,7 +6157,7 @@
         <v>0</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G62" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6217,7 +6210,7 @@
         <v>0</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="G63" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6259,7 +6252,7 @@
         <v>176</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>28</v>
@@ -6268,7 +6261,7 @@
         <v>0</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="G64" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6319,7 +6312,7 @@
         <v>0</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="G65" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6361,7 +6354,7 @@
         <v>62</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>57</v>
@@ -6373,7 +6366,7 @@
         <v>0</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G66" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6414,7 +6407,7 @@
         <v>63</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>85</v>
@@ -6426,7 +6419,7 @@
         <v>1</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="G67" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6472,7 +6465,7 @@
         <v>64</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>223</v>
@@ -6484,7 +6477,7 @@
         <v>0</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="G68" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6538,7 +6531,7 @@
         <v>0</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G69" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6591,7 +6584,7 @@
         <v>1</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="G70" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6649,7 +6642,7 @@
         <v>0</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="G71" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6703,7 +6696,7 @@
         <v>0</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G72" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6756,7 +6749,7 @@
         <v>0</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G73" s="1" t="str">
         <f t="shared" ref="G73:G103" si="14">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B73)</f>
@@ -6809,7 +6802,7 @@
         <v>0</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G74" s="1" t="str">
         <f t="shared" si="14"/>
@@ -6859,7 +6852,7 @@
         <v>0</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G75" s="1" t="str">
         <f t="shared" si="14"/>
@@ -6912,7 +6905,7 @@
         <v>0</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="G76" s="1" t="str">
         <f t="shared" si="14"/>
@@ -6966,7 +6959,7 @@
         <v>0</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="G77" s="1" t="str">
         <f t="shared" si="14"/>
@@ -7025,7 +7018,7 @@
         <v>0</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G78" s="1" t="str">
         <f t="shared" si="14"/>
@@ -7075,7 +7068,7 @@
         <v>0</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G79" s="1" t="str">
         <f t="shared" si="14"/>
@@ -7125,7 +7118,7 @@
         <v>0</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="G80" s="1" t="str">
         <f t="shared" si="14"/>
@@ -7179,7 +7172,7 @@
         <v>0</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="G81" s="1" t="str">
         <f t="shared" si="14"/>
@@ -7238,7 +7231,7 @@
         <v>0</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G82" s="1" t="str">
         <f t="shared" si="14"/>
@@ -7291,7 +7284,7 @@
         <v>0</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="G83" s="1" t="str">
         <f t="shared" si="14"/>
@@ -7317,7 +7310,7 @@
         <v>51</v>
       </c>
       <c r="X83" s="1" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="Y83" s="1" t="str">
         <f>"support searching for all "&amp;LOWER(B83)&amp;"s for a patient"</f>
@@ -7387,7 +7380,7 @@
         <v>GET [base]/Practitioner/practitioner-1~GET [base]/Practitioner?_id=practitioner-1</v>
       </c>
       <c r="AA84" s="10" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="AB84" s="1" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B84)&amp;"-"&amp;SUBSTITUTE(C84,"_","")&amp;".html")</f>
@@ -7411,7 +7404,7 @@
         <v>0</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G85" s="1" t="str">
         <f t="shared" si="14"/>
@@ -7455,7 +7448,7 @@
         <v>243</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>65</v>
@@ -7464,7 +7457,7 @@
         <v>0</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G86" s="1" t="str">
         <f t="shared" si="14"/>
@@ -7496,7 +7489,7 @@
         <v>51</v>
       </c>
       <c r="Y86" s="5" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="Z86" s="5" t="str">
         <f>"GET [base]/"&amp;B86&amp;"?"&amp;C86&amp;"=http://snomed.info/sct\|17561000"</f>
@@ -7525,7 +7518,7 @@
         <v>1</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="G87" s="1" t="str">
         <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-implantable-"&amp;LOWER(B87)</f>
@@ -7584,7 +7577,7 @@
         <v>0</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G88" s="1" t="str">
         <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-implantable-"&amp;LOWER(B88)</f>
@@ -8237,7 +8230,7 @@
         <v>1</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G100" s="1" t="str">
         <f t="shared" si="14"/>
@@ -8295,7 +8288,7 @@
         <v>1</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G101" s="1" t="str">
         <f t="shared" si="14"/>
@@ -8356,7 +8349,7 @@
         <v>1</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="G102" s="1" t="str">
         <f t="shared" si="14"/>
@@ -8408,7 +8401,7 @@
         <v>49</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>57</v>
@@ -8420,7 +8413,7 @@
         <v>0</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G103" s="1" t="str">
         <f t="shared" si="14"/>
@@ -8464,7 +8457,7 @@
         <v>50</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>85</v>
@@ -8476,7 +8469,7 @@
         <v>1</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="G104" s="1" t="str">
         <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B104)</f>
@@ -8526,7 +8519,7 @@
         <v>51</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>135</v>
@@ -8538,7 +8531,7 @@
         <v>0</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G105" s="1" t="str">
         <f t="shared" ref="G105:G117" si="22">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B105)</f>
@@ -8579,7 +8572,7 @@
         <v>52</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>24</v>
@@ -8591,7 +8584,7 @@
         <v>0</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G106" s="1" t="str">
         <f t="shared" si="22"/>
@@ -8635,10 +8628,10 @@
         <v>53</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>28</v>
@@ -8647,7 +8640,7 @@
         <v>0</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="G107" s="1" t="str">
         <f t="shared" si="22"/>
@@ -8692,7 +8685,7 @@
         <v>20</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>50</v>
@@ -8730,10 +8723,10 @@
         <v>51</v>
       </c>
       <c r="Y108" s="5" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="Z108" s="5" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="AB108" s="1" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B108)&amp;"-"&amp;SUBSTITUTE(C108,"_","")&amp;".html")</f>
@@ -8794,7 +8787,7 @@
         <v>20</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>50</v>
@@ -8832,10 +8825,10 @@
         <v>51</v>
       </c>
       <c r="Y110" s="5" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="Z110" s="5" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="AA110" s="10"/>
       <c r="AB110" s="1" t="str">
@@ -8848,7 +8841,7 @@
         <v>79</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>85</v>
@@ -8860,7 +8853,7 @@
         <v>1</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="G111" s="1" t="str">
         <f t="shared" si="22"/>
@@ -8910,7 +8903,7 @@
         <v>80</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>50</v>
@@ -8949,7 +8942,7 @@
         <v>support fetching a QuestionnaireResponse</v>
       </c>
       <c r="Z112" s="5" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="AB112" s="1" t="str">
         <f t="shared" ref="AB112:AB117" si="25">"SearchParameter-us-core-"&amp;LOWER((B112)&amp;"-"&amp;SUBSTITUTE(C112,"_","")&amp;".html")</f>
@@ -8961,7 +8954,7 @@
         <v>81</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>85</v>
@@ -8973,7 +8966,7 @@
         <v>1</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="G113" s="1" t="str">
         <f t="shared" si="22"/>
@@ -9020,7 +9013,7 @@
         <v>82</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>57</v>
@@ -9032,7 +9025,7 @@
         <v>0</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G114" s="1" t="str">
         <f t="shared" si="22"/>
@@ -9060,8 +9053,8 @@
       <c r="O114" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="Y114" s="22" t="s">
-        <v>657</v>
+      <c r="Y114" s="21" t="s">
+        <v>655</v>
       </c>
       <c r="AB114" s="1" t="str">
         <f t="shared" si="25"/>
@@ -9073,10 +9066,10 @@
         <v>83</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>28</v>
@@ -9085,7 +9078,7 @@
         <v>0</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G115" s="1" t="str">
         <f t="shared" si="22"/>
@@ -9101,7 +9094,7 @@
         <v>52</v>
       </c>
       <c r="L115" s="1" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="M115" s="1" t="s">
         <v>51</v>
@@ -9109,8 +9102,8 @@
       <c r="O115" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="Y115" s="22" t="s">
-        <v>660</v>
+      <c r="Y115" s="21" t="s">
+        <v>658</v>
       </c>
       <c r="AB115" s="1" t="str">
         <f t="shared" si="25"/>
@@ -9122,10 +9115,10 @@
         <v>84</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>28</v>
@@ -9134,7 +9127,7 @@
         <v>0</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="G116" s="1" t="str">
         <f t="shared" si="22"/>
@@ -9165,8 +9158,8 @@
       <c r="S116" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="Y116" s="22" t="s">
-        <v>661</v>
+      <c r="Y116" s="21" t="s">
+        <v>659</v>
       </c>
       <c r="AB116" s="1" t="str">
         <f t="shared" si="25"/>
@@ -9178,10 +9171,10 @@
         <v>85</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>28</v>
@@ -9190,7 +9183,7 @@
         <v>0</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="G117" s="1" t="str">
         <f t="shared" si="22"/>
@@ -9215,8 +9208,8 @@
       <c r="O117" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="Y117" s="22" t="s">
-        <v>663</v>
+      <c r="Y117" s="21" t="s">
+        <v>661</v>
       </c>
       <c r="AB117" s="1" t="str">
         <f t="shared" si="25"/>
@@ -9238,7 +9231,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:K102"/>
   <sheetViews>
-    <sheetView topLeftCell="I85" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I85" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="I110" sqref="I110"/>
     </sheetView>
   </sheetViews>
@@ -9272,7 +9265,7 @@
         <v>91</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>92</v>
@@ -9602,7 +9595,7 @@
         <v>299</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="K13" s="5" t="str">
         <f t="shared" si="1"/>
@@ -9702,7 +9695,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="E17" s="1" t="b">
         <v>1</v>
@@ -9717,7 +9710,7 @@
         <v>300</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="K17" s="5" t="str">
         <f t="shared" si="1"/>
@@ -9793,7 +9786,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="E20" s="1" t="b">
         <v>1</v>
@@ -9808,7 +9801,7 @@
         <v>305</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="K20" s="5" t="str">
         <f t="shared" si="1"/>
@@ -10220,7 +10213,7 @@
         <v>101</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="I35" s="5" t="s">
         <v>150</v>
@@ -10256,7 +10249,7 @@
         <v>145</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="K36" s="5" t="s">
         <v>141</v>
@@ -10274,7 +10267,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="E37" s="1" t="b">
         <v>1</v>
@@ -10289,10 +10282,10 @@
         <v>145</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
@@ -10349,7 +10342,7 @@
         <v>148</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="K39" s="5" t="s">
         <v>151</v>
@@ -10367,7 +10360,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="E40" s="1" t="b">
         <v>1</v>
@@ -10382,7 +10375,7 @@
         <v>148</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="K40" s="5" t="s">
         <v>151</v>
@@ -10400,7 +10393,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="E41" s="1" t="b">
         <v>1</v>
@@ -10415,7 +10408,7 @@
         <v>148</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K41" s="5" t="s">
         <v>151</v>
@@ -10433,7 +10426,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="E42" s="1" t="b">
         <v>1</v>
@@ -10448,7 +10441,7 @@
         <v>148</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="K42" s="5" t="s">
         <v>151</v>
@@ -10481,7 +10474,7 @@
         <v>320</v>
       </c>
       <c r="K43" s="5" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
@@ -10508,7 +10501,7 @@
         <v>162</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="K44" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B44&amp;" resources for the specified "&amp;SUBSTITUTE(D44,","," and ")</f>
@@ -10665,7 +10658,7 @@
         <v>190</v>
       </c>
       <c r="J49" s="8" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="K49" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B49&amp;" resources for the specified patient and date and a category code = `LAB`"</f>
@@ -10695,7 +10688,7 @@
         <v>221</v>
       </c>
       <c r="J50" s="5" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="K50" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B50&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
@@ -10815,7 +10808,7 @@
         <v>196</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="K54" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B54&amp;" resources for the specified patient and date and a category code specified in US Core DiagnosticReport Category Codes"</f>
@@ -10845,7 +10838,7 @@
         <v>215</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="K55" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B55&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
@@ -10895,7 +10888,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>65</v>
@@ -10907,7 +10900,7 @@
         <v>202</v>
       </c>
       <c r="J57" s="5" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="K57" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B57&amp;" resources for the specified "&amp;SUBSTITUTE(D57,","," and ")</f>
@@ -10926,7 +10919,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>11</v>
@@ -10935,16 +10928,16 @@
         <v>101</v>
       </c>
       <c r="H58" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="I58" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="J58" s="5" t="s">
+        <v>458</v>
+      </c>
+      <c r="K58" s="5" t="s">
         <v>459</v>
-      </c>
-      <c r="I58" s="5" t="s">
-        <v>436</v>
-      </c>
-      <c r="J58" s="5" t="s">
-        <v>460</v>
-      </c>
-      <c r="K58" s="5" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
@@ -10959,7 +10952,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>11</v>
@@ -10968,16 +10961,16 @@
         <v>101</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="I59" s="5" t="s">
         <v>180</v>
       </c>
       <c r="J59" s="5" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="K59" s="5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
@@ -10992,7 +10985,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>65</v>
@@ -11001,16 +10994,16 @@
         <v>101</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="I60" s="5" t="s">
         <v>180</v>
       </c>
       <c r="J60" s="5" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="K60" s="5" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
@@ -11025,7 +11018,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>65</v>
@@ -11034,16 +11027,16 @@
         <v>213</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="I61" s="5" t="s">
         <v>225</v>
       </c>
       <c r="J61" s="5" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="K61" s="5" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
@@ -11051,7 +11044,7 @@
         <v>73</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C62" s="1" t="str">
         <f t="shared" si="2"/>
@@ -11070,7 +11063,7 @@
         <v>182</v>
       </c>
       <c r="J62" s="5" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="K62" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B62&amp;" resources for the specified "&amp;SUBSTITUTE(D62,","," and ")</f>
@@ -11083,7 +11076,7 @@
         <v>0</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C63" s="1" t="str">
         <f t="shared" si="2"/>
@@ -11102,7 +11095,7 @@
         <v>226</v>
       </c>
       <c r="J63" s="5" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="K63" s="5" t="s">
         <v>228</v>
@@ -11194,7 +11187,7 @@
         <v>222</v>
       </c>
       <c r="J66" s="5" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="K66" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B66&amp;" resources for the specified patient and date and procedure code(s).  SHOULD support search by multiple codes."</f>
@@ -11209,7 +11202,7 @@
         <v>178</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>232</v>
@@ -11221,13 +11214,13 @@
         <v>101</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="I67" s="5" t="s">
         <v>275</v>
       </c>
       <c r="J67" s="5" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="K67" s="5" t="s">
         <v>316</v>
@@ -11241,7 +11234,7 @@
         <v>178</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>140</v>
@@ -11253,13 +11246,13 @@
         <v>101</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="I68" s="5" t="s">
         <v>216</v>
       </c>
       <c r="J68" s="5" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="K68" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B68&amp;" resources for the specified patient and a category code = `laboratory`"</f>
@@ -11274,7 +11267,7 @@
         <v>178</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>142</v>
@@ -11304,7 +11297,7 @@
         <v>178</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>189</v>
@@ -11316,13 +11309,13 @@
         <v>213</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="I70" s="5" t="s">
         <v>220</v>
       </c>
       <c r="J70" s="5" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="K70" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B70&amp;" resources for the specified patient and date and a category code = `laboratory`"</f>
@@ -11337,7 +11330,7 @@
         <v>178</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>214</v>
@@ -11352,7 +11345,7 @@
         <v>218</v>
       </c>
       <c r="J71" s="5" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="K71" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B71&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
@@ -11367,7 +11360,7 @@
         <v>315</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>111</v>
@@ -11448,7 +11441,7 @@
         <v>236</v>
       </c>
       <c r="J74" s="5" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="K74" s="5" t="s">
         <v>240</v>
@@ -11512,7 +11505,7 @@
         <v>235</v>
       </c>
       <c r="J76" s="5" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="K76" s="5" t="s">
         <v>242</v>
@@ -11545,13 +11538,13 @@
         <v>306</v>
       </c>
       <c r="I77" s="5" t="s">
+        <v>604</v>
+      </c>
+      <c r="J77" s="5" t="s">
+        <v>605</v>
+      </c>
+      <c r="K77" s="10" t="s">
         <v>606</v>
-      </c>
-      <c r="J77" s="5" t="s">
-        <v>607</v>
-      </c>
-      <c r="K77" s="10" t="s">
-        <v>608</v>
       </c>
     </row>
     <row r="78" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -11595,7 +11588,7 @@
         <v>178</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>232</v>
@@ -11607,13 +11600,13 @@
         <v>101</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="I79" s="5" t="s">
         <v>274</v>
       </c>
       <c r="J79" s="5" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="K79" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B79&amp;" resources for the specified "&amp;SUBSTITUTE(D79,","," and ")</f>
@@ -11628,7 +11621,7 @@
         <v>178</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>140</v>
@@ -11640,13 +11633,13 @@
         <v>101</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="I80" s="5" t="s">
         <v>273</v>
       </c>
       <c r="J80" s="5" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="K80" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B80&amp;" resources for the specified patient and a category code = `vital-signs`"</f>
@@ -11661,7 +11654,7 @@
         <v>178</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>142</v>
@@ -11673,7 +11666,7 @@
         <v>101</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="I81" s="5" t="s">
         <v>276</v>
@@ -11694,7 +11687,7 @@
         <v>178</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>189</v>
@@ -11706,13 +11699,13 @@
         <v>213</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="I82" s="5" t="s">
         <v>278</v>
       </c>
       <c r="J82" s="5" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="K82" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B82&amp;" resources for the specified patient and date and a category code = `vital-signs`"</f>
@@ -11727,7 +11720,7 @@
         <v>178</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>214</v>
@@ -11742,7 +11735,7 @@
         <v>279</v>
       </c>
       <c r="J83" s="5" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="K83" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B83&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple codes."</f>
@@ -11869,7 +11862,7 @@
         <v>291</v>
       </c>
       <c r="J87" s="8" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="K87" s="5" t="s">
         <v>293</v>
@@ -11899,7 +11892,7 @@
         <v>295</v>
       </c>
       <c r="J88" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="K88" s="5" t="s">
         <v>292</v>
@@ -11929,7 +11922,7 @@
         <v>296</v>
       </c>
       <c r="J89" s="5" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="K89" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B89&amp;" resources for the specified "&amp;SUBSTITUTE(D89,","," and ") &amp;". See the implementation notes above for how to access the actual document."</f>
@@ -11944,7 +11937,7 @@
         <v>244</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>113</v>
@@ -11956,13 +11949,13 @@
         <v>101</v>
       </c>
       <c r="I90" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="J90" s="5" t="s">
         <v>386</v>
       </c>
-      <c r="J90" s="5" t="s">
-        <v>388</v>
-      </c>
       <c r="K90" s="5" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.2">
@@ -11977,7 +11970,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="E91" s="1" t="b">
         <v>1</v>
@@ -11989,13 +11982,13 @@
         <v>101</v>
       </c>
       <c r="I91" s="5" t="s">
+        <v>608</v>
+      </c>
+      <c r="J91" s="5" t="s">
+        <v>609</v>
+      </c>
+      <c r="K91" s="5" t="s">
         <v>610</v>
-      </c>
-      <c r="J91" s="5" t="s">
-        <v>611</v>
-      </c>
-      <c r="K91" s="5" t="s">
-        <v>612</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.2">
@@ -12003,10 +11996,10 @@
         <v>56</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>111</v>
@@ -12024,7 +12017,7 @@
         <v>298</v>
       </c>
       <c r="J92" s="5" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="K92" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B92&amp;" resources for the specified "&amp;SUBSTITUTE(D92,","," and ")</f>
@@ -12036,10 +12029,10 @@
         <v>57</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>140</v>
@@ -12057,7 +12050,7 @@
         <v>193</v>
       </c>
       <c r="J93" s="5" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="K93" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B93&amp;" resources for the specified patient and  a category code"</f>
@@ -12069,10 +12062,10 @@
         <v>58</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>142</v>
@@ -12090,7 +12083,7 @@
         <v>194</v>
       </c>
       <c r="J94" s="5" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="K94" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B94&amp;" resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes."</f>
@@ -12102,13 +12095,13 @@
         <v>59</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="E95" s="1" t="b">
         <v>1</v>
@@ -12123,7 +12116,7 @@
         <v>196</v>
       </c>
       <c r="J95" s="5" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="K95" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient and date and a category code"</f>
@@ -12135,13 +12128,13 @@
         <v>60</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E96" s="1" t="b">
         <v>1</v>
@@ -12153,10 +12146,10 @@
         <v>213</v>
       </c>
       <c r="I96" s="5" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="J96" s="5" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="K96" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B96&amp;" resources for the specified patient and date and service code(s).  SHOULD support search by multiple report codes."</f>
@@ -12175,7 +12168,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="E97" s="1" t="b">
         <v>1</v>
@@ -12187,10 +12180,10 @@
         <v>101</v>
       </c>
       <c r="I97" s="5" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="J97" s="5" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="K97" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B97&amp;" resources for the specified "&amp;SUBSTITUTE(D97,","," and ")</f>
@@ -12202,10 +12195,10 @@
         <v>65</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>653</v>
-      </c>
-      <c r="C98" s="21" t="s">
         <v>651</v>
+      </c>
+      <c r="C98" s="20" t="s">
+        <v>649</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>111</v>
@@ -12217,10 +12210,10 @@
         <v>101</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="J98" s="5" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="K98" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B98&amp;" resources for the specified "&amp;SUBSTITUTE(D98,","," and ")</f>
@@ -12232,13 +12225,13 @@
         <v>66</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>653</v>
-      </c>
-      <c r="C99" s="21" t="s">
         <v>651</v>
       </c>
+      <c r="C99" s="20" t="s">
+        <v>649</v>
+      </c>
       <c r="D99" s="1" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="F99" s="1" t="s">
         <v>65</v>
@@ -12247,13 +12240,13 @@
         <v>101</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="J99" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="K99" s="1" t="str">
         <f>"Fetches a bundle of all "&amp;B99&amp;" resources for the specified "&amp;SUBSTITUTE(D99,","," and  ") &amp; "= 'sdoh'"</f>
@@ -12265,13 +12258,13 @@
         <v>67</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>653</v>
-      </c>
-      <c r="C100" s="21" t="s">
         <v>651</v>
       </c>
+      <c r="C100" s="20" t="s">
+        <v>649</v>
+      </c>
       <c r="D100" s="1" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>65</v>
@@ -12280,10 +12273,10 @@
         <v>144</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="J100" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="K100" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B100&amp;" resources for the specified patient and date"</f>
@@ -12295,13 +12288,13 @@
         <v>68</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>653</v>
-      </c>
-      <c r="C101" s="21" t="s">
         <v>651</v>
       </c>
+      <c r="C101" s="20" t="s">
+        <v>649</v>
+      </c>
       <c r="D101" s="18" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>65</v>
@@ -12310,13 +12303,13 @@
         <v>213</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="J101" s="5" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="K101" s="1" t="str">
         <f>"Fetches a bundle of all "&amp;B101&amp;" resources tagged as 'sdoh' for the specified patient and date"</f>
@@ -12328,13 +12321,13 @@
         <v>69</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>653</v>
-      </c>
-      <c r="C102" s="21" t="s">
         <v>651</v>
       </c>
+      <c r="C102" s="20" t="s">
+        <v>649</v>
+      </c>
       <c r="D102" s="18" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="F102" s="1" t="s">
         <v>65</v>
@@ -12343,10 +12336,10 @@
         <v>86</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="J102" s="5" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="K102" s="1" t="str">
         <f>"Fetches a bundle of all "&amp;B102&amp;" resources for the specified patient that have been completed against a specified form."</f>
@@ -12367,7 +12360,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -12390,15 +12383,15 @@
         <v>62</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -12406,7 +12399,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -12414,7 +12407,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -12422,7 +12415,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="141" customHeight="1" x14ac:dyDescent="0.2">
@@ -12430,7 +12423,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -12438,36 +12431,36 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="9" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="11" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="12" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>65</v>
@@ -12497,7 +12490,7 @@
         <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>55</v>
@@ -12508,13 +12501,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>65</v>
@@ -12522,13 +12515,13 @@
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="C3" s="17" t="s">
         <v>551</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>553</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>65</v>
@@ -12560,16 +12553,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>55</v>
@@ -12583,13 +12576,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>11</v>
@@ -12604,8 +12597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:G53"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12639,7 +12632,7 @@
         <v>68</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -12654,7 +12647,7 @@
         <v>231</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -12681,10 +12674,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>343</v>
+        <v>674</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>344</v>
+        <v>675</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -12696,56 +12689,56 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>423</v>
+        <v>676</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>422</v>
+        <v>677</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>244</v>
+        <v>133</v>
       </c>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>183</v>
+        <v>421</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>360</v>
+        <v>420</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="21" t="s">
-        <v>423</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>244</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="21" t="s">
-        <v>184</v>
+      <c r="A9" s="20" t="s">
+        <v>183</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>352</v>
+        <v>358</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>11</v>
@@ -12757,71 +12750,71 @@
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="21" t="s">
-        <v>183</v>
+      <c r="A10" s="20" t="s">
+        <v>339</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>360</v>
+        <v>340</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="21" t="s">
-        <v>339</v>
+      <c r="A11" s="20" t="s">
+        <v>626</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>340</v>
+        <v>360</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>173</v>
+        <v>20</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="20" t="s">
+        <v>627</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>628</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>362</v>
-      </c>
       <c r="D12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>20</v>
+        <v>629</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="20" t="s">
+        <v>630</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>629</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>630</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>631</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="20" t="s">
         <v>632</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -12831,13 +12824,13 @@
         <v>11</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="20" t="s">
         <v>634</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -12847,13 +12840,13 @@
         <v>11</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="20" t="s">
         <v>636</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -12863,13 +12856,13 @@
         <v>11</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="20" t="s">
         <v>638</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -12879,113 +12872,113 @@
         <v>11</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="21" t="s">
-        <v>640</v>
+      <c r="A18" s="20" t="s">
+        <v>354</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>641</v>
+        <v>355</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>631</v>
+        <v>175</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="21" t="s">
-        <v>356</v>
+      <c r="A19" s="20" t="s">
+        <v>336</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>357</v>
+        <v>337</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="21" t="s">
-        <v>336</v>
+      <c r="A20" s="20" t="s">
+        <v>356</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>337</v>
+        <v>357</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>156</v>
+        <v>245</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="21" t="s">
-        <v>358</v>
+      <c r="A21" s="20" t="s">
+        <v>347</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>359</v>
+        <v>348</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>245</v>
+        <v>349</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="21" t="s">
-        <v>349</v>
+      <c r="A22" s="20" t="s">
+        <v>341</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>351</v>
+        <v>176</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="21" t="s">
-        <v>341</v>
+      <c r="A23" s="20" t="s">
+        <v>406</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>342</v>
+        <v>407</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="21" t="s">
-        <v>408</v>
+      <c r="A24" s="20" t="s">
+        <v>640</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>409</v>
+        <v>641</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>11</v>
@@ -12995,11 +12988,11 @@
       </c>
     </row>
     <row r="25" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="21" t="s">
-        <v>642</v>
+      <c r="A25" s="20" t="s">
+        <v>491</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>643</v>
+        <v>492</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>11</v>
@@ -13009,11 +13002,11 @@
       </c>
     </row>
     <row r="26" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="21" t="s">
-        <v>493</v>
+      <c r="A26" s="20" t="s">
+        <v>642</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>494</v>
+        <v>643</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>11</v>
@@ -13023,11 +13016,11 @@
       </c>
     </row>
     <row r="27" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="21" t="s">
-        <v>644</v>
+      <c r="A27" s="20" t="s">
+        <v>489</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>645</v>
+        <v>490</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>11</v>
@@ -13037,11 +13030,11 @@
       </c>
     </row>
     <row r="28" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="21" t="s">
-        <v>491</v>
+      <c r="A28" s="20" t="s">
+        <v>487</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>11</v>
@@ -13051,11 +13044,11 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="21" t="s">
-        <v>489</v>
+      <c r="A29" s="20" t="s">
+        <v>508</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>490</v>
+        <v>509</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>11</v>
@@ -13067,11 +13060,11 @@
       <c r="G29" s="1"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="21" t="s">
-        <v>510</v>
+      <c r="A30" s="20" t="s">
+        <v>427</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>511</v>
+        <v>428</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>11</v>
@@ -13083,11 +13076,11 @@
       <c r="G30" s="1"/>
     </row>
     <row r="31" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="21" t="s">
-        <v>429</v>
+      <c r="A31" s="20" t="s">
+        <v>270</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>430</v>
+        <v>338</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>11</v>
@@ -13097,11 +13090,11 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="21" t="s">
-        <v>270</v>
+      <c r="A32" s="20" t="s">
+        <v>553</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>338</v>
+        <v>644</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>11</v>
@@ -13113,11 +13106,11 @@
       <c r="G32" s="1"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="21" t="s">
-        <v>555</v>
+      <c r="A33" s="20" t="s">
+        <v>481</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>646</v>
+        <v>482</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>11</v>
@@ -13129,7 +13122,7 @@
       <c r="G33" s="1"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="21" t="s">
+      <c r="A34" s="20" t="s">
         <v>483</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -13145,11 +13138,11 @@
       <c r="G34" s="1"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="21" t="s">
-        <v>485</v>
+      <c r="A35" s="20" t="s">
+        <v>479</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>11</v>
@@ -13161,11 +13154,11 @@
       <c r="G35" s="1"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="21" t="s">
-        <v>481</v>
+      <c r="A36" s="20" t="s">
+        <v>645</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>482</v>
+        <v>646</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>11</v>
@@ -13177,11 +13170,11 @@
       <c r="G36" s="1"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="21" t="s">
-        <v>647</v>
+      <c r="A37" s="20" t="s">
+        <v>477</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>648</v>
+        <v>478</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>11</v>
@@ -13193,11 +13186,11 @@
       <c r="G37" s="1"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="21" t="s">
-        <v>479</v>
+      <c r="A38" s="20" t="s">
+        <v>563</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>480</v>
+        <v>647</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>11</v>
@@ -13209,11 +13202,11 @@
       <c r="G38" s="1"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="21" t="s">
-        <v>565</v>
+      <c r="A39" s="20" t="s">
+        <v>556</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>11</v>
@@ -13225,11 +13218,11 @@
       <c r="G39" s="1"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="21" t="s">
-        <v>558</v>
+      <c r="A40" s="20" t="s">
+        <v>505</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>650</v>
+        <v>506</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>11</v>
@@ -13241,11 +13234,11 @@
       <c r="G40" s="1"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="21" t="s">
+      <c r="A41" s="20" t="s">
+        <v>503</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>507</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>508</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>11</v>
@@ -13257,11 +13250,11 @@
       <c r="G41" s="1"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="21" t="s">
-        <v>505</v>
+      <c r="A42" s="20" t="s">
+        <v>485</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>509</v>
+        <v>486</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>11</v>
@@ -13273,11 +13266,11 @@
       <c r="G42" s="1"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="21" t="s">
-        <v>487</v>
+      <c r="A43" s="20" t="s">
+        <v>475</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>488</v>
+        <v>476</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>11</v>
@@ -13289,162 +13282,151 @@
       <c r="G43" s="1"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="21" t="s">
-        <v>477</v>
+      <c r="A44" s="20" t="s">
+        <v>343</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>478</v>
+        <v>344</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>178</v>
+        <v>255</v>
       </c>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="21" t="s">
-        <v>345</v>
+      <c r="A45" s="20" t="s">
+        <v>70</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>346</v>
+        <v>359</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>255</v>
+        <v>19</v>
       </c>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="21" t="s">
-        <v>70</v>
+      <c r="A46" s="20" t="s">
+        <v>334</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>361</v>
+        <v>335</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>19</v>
+        <v>262</v>
       </c>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="21" t="s">
-        <v>334</v>
+      <c r="A47" s="20" t="s">
+        <v>351</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>335</v>
+        <v>352</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="21" t="s">
-        <v>353</v>
+      <c r="A48" s="20" t="s">
+        <v>345</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>264</v>
+        <v>177</v>
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="21" t="s">
-        <v>347</v>
+      <c r="A49" s="20" t="s">
+        <v>429</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>348</v>
+        <v>430</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>177</v>
+        <v>431</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="21" t="s">
-        <v>431</v>
+      <c r="A50" s="20" t="s">
+        <v>649</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>432</v>
+        <v>650</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>433</v>
+        <v>651</v>
       </c>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" s="21" t="s">
-        <v>651</v>
+      <c r="A51" s="20" t="s">
+        <v>557</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>652</v>
+        <v>558</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>653</v>
+        <v>559</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="21" t="s">
-        <v>559</v>
+      <c r="A52" s="20" t="s">
+        <v>560</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" s="21" t="s">
-        <v>562</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>563</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>564</v>
-      </c>
+      <c r="A53" s="20"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
     </row>
@@ -13459,11 +13441,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Y62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomRight" activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="23" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13497,67 +13479,67 @@
         <v>37</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>397</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>399</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>401</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="V1" s="4" t="s">
+        <v>544</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="X1" s="4" t="s">
         <v>546</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>547</v>
-      </c>
-      <c r="X1" s="4" t="s">
-        <v>548</v>
-      </c>
-      <c r="Y1" s="4" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="23" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -13571,13 +13553,13 @@
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="T2" s="1" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="U2" s="1" t="s">
         <v>65</v>
       </c>
       <c r="X2" s="15" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="Y2" s="15" t="s">
         <v>65</v>
@@ -13591,16 +13573,16 @@
         <v>65</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="U3" s="1" t="s">
         <v>65</v>
       </c>
       <c r="X3" s="15" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="Y3" s="15" t="s">
         <v>65</v>
@@ -13614,22 +13596,22 @@
         <v>65</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="W4" s="1" t="s">
         <v>567</v>
       </c>
-      <c r="T4" s="1" t="s">
-        <v>566</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>569</v>
-      </c>
       <c r="X4" s="15" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="Y4" s="15" t="s">
         <v>65</v>
@@ -13643,16 +13625,16 @@
         <v>65</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="U5" s="1" t="s">
         <v>65</v>
       </c>
       <c r="X5" s="15" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="Y5" s="15" t="s">
         <v>65</v>
@@ -13666,16 +13648,16 @@
         <v>65</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="U6" s="1" t="s">
         <v>65</v>
       </c>
       <c r="X6" s="15" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="Y6" s="15" t="s">
         <v>65</v>
@@ -13689,16 +13671,16 @@
         <v>65</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="U7" s="1" t="s">
         <v>65</v>
       </c>
       <c r="X7" s="15" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="Y7" s="15" t="s">
         <v>65</v>
@@ -13712,16 +13694,16 @@
         <v>65</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="U8" s="1" t="s">
         <v>65</v>
       </c>
       <c r="X8" s="15" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="Y8" s="15" t="s">
         <v>65</v>
@@ -13735,16 +13717,16 @@
         <v>65</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="U9" s="1" t="s">
         <v>65</v>
       </c>
       <c r="X9" s="15" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="Y9" s="15" t="s">
         <v>65</v>
@@ -13758,13 +13740,13 @@
         <v>65</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="U10" s="1" t="s">
         <v>65</v>
       </c>
       <c r="X10" s="15" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="Y10" s="15" t="s">
         <v>65</v>
@@ -13778,16 +13760,16 @@
         <v>65</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="U11" s="1" t="s">
         <v>65</v>
       </c>
       <c r="X11" s="15" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="Y11" s="15" t="s">
         <v>65</v>
@@ -13801,10 +13783,10 @@
         <v>65</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="U12" s="1" t="s">
         <v>65</v>
@@ -13814,16 +13796,16 @@
     </row>
     <row r="13" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>65</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="U13" s="1" t="s">
         <v>65</v>
@@ -13839,10 +13821,10 @@
         <v>65</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="U14" s="1" t="s">
         <v>65</v>
@@ -13854,7 +13836,7 @@
         <v>203</v>
       </c>
       <c r="X14" s="15" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="Y14" s="15" t="s">
         <v>65</v>
@@ -13862,16 +13844,16 @@
     </row>
     <row r="15" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>65</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="U15" s="1" t="s">
         <v>65</v>
@@ -13880,10 +13862,10 @@
         <v>65</v>
       </c>
       <c r="W15" s="7" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="X15" s="15" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="Y15" s="15" t="s">
         <v>65</v>
@@ -13897,16 +13879,16 @@
         <v>65</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="T16" s="1" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="U16" s="1" t="s">
         <v>65</v>
       </c>
       <c r="X16" s="15" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="Y16" s="15" t="s">
         <v>65</v>
@@ -13920,7 +13902,7 @@
         <v>65</v>
       </c>
       <c r="T17" s="1" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="U17" s="1" t="s">
         <v>65</v>
@@ -13936,16 +13918,16 @@
         <v>65</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="T18" s="1" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="U18" s="1" t="s">
         <v>65</v>
       </c>
       <c r="X18" s="15" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="Y18" s="15" t="s">
         <v>65</v>
@@ -13959,7 +13941,7 @@
         <v>65</v>
       </c>
       <c r="T19" s="1" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="U19" s="1" t="s">
         <v>65</v>
@@ -13975,16 +13957,16 @@
         <v>65</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="U20" s="1" t="s">
         <v>65</v>
       </c>
       <c r="V20" s="1" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="W20" s="1" t="s">
         <v>268</v>
@@ -14000,16 +13982,16 @@
         <v>65</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="T21" s="1" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="U21" s="1" t="s">
         <v>65</v>
       </c>
       <c r="X21" s="15" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="Y21" s="15" t="s">
         <v>65</v>
@@ -14017,16 +13999,16 @@
     </row>
     <row r="22" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>65</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="T22" s="1" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="U22" s="1" t="s">
         <v>65</v>
@@ -14034,22 +14016,22 @@
     </row>
     <row r="23" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>65</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="T23" s="1" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="U23" s="1" t="s">
         <v>65</v>
       </c>
       <c r="X23" s="15" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="Y23" s="15" t="s">
         <v>65</v>
@@ -14057,19 +14039,19 @@
     </row>
     <row r="24" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>65</v>
       </c>
       <c r="T24" s="1" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="U24" s="1" t="s">
         <v>65</v>
       </c>
       <c r="X24" s="15" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="Y24" s="15" t="s">
         <v>65</v>
@@ -14077,19 +14059,19 @@
     </row>
     <row r="25" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="T25" s="1" t="s">
         <v>564</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="T25" s="1" t="s">
-        <v>566</v>
-      </c>
       <c r="U25" s="1" t="s">
         <v>65</v>
       </c>
       <c r="X25" s="15" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="Y25" s="15" t="s">
         <v>65</v>
@@ -14097,7 +14079,7 @@
     </row>
     <row r="26" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>65</v>
@@ -14155,10 +14137,10 @@
     </row>
     <row r="2" spans="1:5" ht="81" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>173</v>
@@ -14167,24 +14149,24 @@
         <v>65</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="1" customFormat="1" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>65</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -14220,85 +14202,85 @@
         <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>456</v>
-      </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" t="s">
         <v>382</v>
       </c>
-      <c r="V1" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="W1" t="s">
-        <v>384</v>
-      </c>
       <c r="X1" s="1" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.2">
@@ -14321,7 +14303,7 @@
         <v>28</v>
       </c>
       <c r="G2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="H2" t="s">
         <v>11</v>
@@ -15023,12 +15005,12 @@
         <v>23</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>28</v>
@@ -15037,7 +15019,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>28</v>
@@ -15046,7 +15028,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>28</v>
@@ -15055,7 +15037,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
Correct Errata in Version 5.0.1 of US Cor update version, package-list, apply FHIR-37585 FHIR-37586 (partially)
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE58424-A49E-D444-B376-6E7F5F1083EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78FBD953-0309-1043-954F-247D85F70394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -2161,13 +2161,7 @@
     <t>GET [base]/QuestionnaireResponse?patient=113192&amp;questionnaire=http://hl7.org/fhir/us/sdoh-clinicalcare/Questionnaire/SDOHCC-QuestionnaireHungerVitalSign</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/core//StructureDefinition/us-core-condition-encounter-diagnosis</t>
-  </si>
-  <si>
     <t>US Core Condition Encounter Diagnosis Profile</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core//StructureDefinition/us-core-condition-problems-health-concerns</t>
   </si>
   <si>
     <t>US Core Condition Problems and Health Concerns Profile</t>
@@ -2306,6 +2300,12 @@
   * US Core DocumentReference Profile
 * If a system receives a provider in `Provenance.agent.who` as free text they must capture who sent them the information as the organization. On request they **SHALL** provide this organization as the source and **MAY** include the free text provider.
 * Systems that need to know the activity has occurred **SHOULD** populate the activity.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition-encounter-diagnosis</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition-problems-health-concerns</t>
   </si>
 </sst>
 </file>
@@ -12369,7 +12369,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -12377,7 +12377,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
     </row>
     <row r="9" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -12543,8 +12543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12620,10 +12620,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>676</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>661</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>662</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -12635,10 +12635,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>663</v>
+        <v>677</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -13387,11 +13387,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Y62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1:C1048576"/>
+      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="23" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13542,7 +13542,7 @@
         <v>65</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="T4" s="1" t="s">
         <v>557</v>
@@ -13571,7 +13571,7 @@
         <v>65</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="T5" s="1" t="s">
         <v>557</v>
@@ -13594,7 +13594,7 @@
         <v>65</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="T6" s="1" t="s">
         <v>557</v>
@@ -13638,7 +13638,7 @@
         <v>65</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="T8" s="1" t="s">
         <v>557</v>
@@ -13661,7 +13661,7 @@
         <v>65</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="T9" s="1" t="s">
         <v>557</v>
@@ -13704,7 +13704,7 @@
         <v>65</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="T11" s="1" t="s">
         <v>557</v>
@@ -13823,7 +13823,7 @@
         <v>65</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="T16" s="1" t="s">
         <v>557</v>
@@ -13846,7 +13846,7 @@
         <v>65</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="T17" s="1" t="s">
         <v>557</v>
@@ -13865,7 +13865,7 @@
         <v>65</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="T18" s="1" t="s">
         <v>557</v>
@@ -13929,7 +13929,7 @@
         <v>65</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="T21" s="1" t="s">
         <v>557</v>
@@ -13952,7 +13952,7 @@
         <v>65</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="T22" s="1" t="s">
         <v>557</v>

</xml_diff>

<commit_message>
Added supportedProfiles to US Core CapabilityStatements FHIR-37766
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9458C636-72DD-394D-A39B-6F2E9A938F45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C494EE-163D-9F43-ABB9-E84FC788AEB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -2014,9 +2014,6 @@
     <t>http://www.hl7.org/Special/committees/cgp</t>
   </si>
   <si>
-    <t>!http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</t>
-  </si>
-  <si>
     <t>!http://hl7.org/fhir/us/core/StructureDefinition/us-core-direct</t>
   </si>
   <si>
@@ -2307,12 +2304,15 @@
 * If a system receives a provider in `Provenance.agent.who` as free text they must capture who sent them the information as the organization. On request they **SHALL** provide this organization as the source and **MAY** include the free text provider.
 * Systems that need to know the activity has occurred **SHOULD** populate the activity.</t>
   </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2414,13 +2414,33 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -2456,11 +2476,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2492,9 +2514,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -8885,7 +8911,7 @@
         <v>80</v>
       </c>
       <c r="B112" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C112" t="s">
         <v>50</v>
@@ -8924,7 +8950,7 @@
         <v>support fetching a QuestionnaireResponse</v>
       </c>
       <c r="Z112" s="4" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="AB112" t="str">
         <f t="shared" ref="AB112:AB117" si="25">"SearchParameter-us-core-"&amp;LOWER((B112)&amp;"-"&amp;SUBSTITUTE(C112,"_","")&amp;".html")</f>
@@ -8936,7 +8962,7 @@
         <v>81</v>
       </c>
       <c r="B113" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C113" t="s">
         <v>85</v>
@@ -8995,7 +9021,7 @@
         <v>82</v>
       </c>
       <c r="B114" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C114" t="s">
         <v>57</v>
@@ -9036,7 +9062,7 @@
         <v>51</v>
       </c>
       <c r="Y114" s="20" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="AB114" t="str">
         <f t="shared" si="25"/>
@@ -9048,10 +9074,10 @@
         <v>83</v>
       </c>
       <c r="B115" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C115" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="D115" t="s">
         <v>28</v>
@@ -9076,16 +9102,16 @@
         <v>52</v>
       </c>
       <c r="L115" t="s">
+        <v>643</v>
+      </c>
+      <c r="M115" t="s">
+        <v>51</v>
+      </c>
+      <c r="O115" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y115" s="20" t="s">
         <v>644</v>
-      </c>
-      <c r="M115" t="s">
-        <v>51</v>
-      </c>
-      <c r="O115" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y115" s="20" t="s">
-        <v>645</v>
       </c>
       <c r="AB115" t="str">
         <f t="shared" si="25"/>
@@ -9097,7 +9123,7 @@
         <v>84</v>
       </c>
       <c r="B116" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C116" t="s">
         <v>573</v>
@@ -9141,7 +9167,7 @@
         <v>88</v>
       </c>
       <c r="Y116" s="20" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="AB116" t="str">
         <f t="shared" si="25"/>
@@ -9153,10 +9179,10 @@
         <v>85</v>
       </c>
       <c r="B117" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C117" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="D117" t="s">
         <v>28</v>
@@ -9191,7 +9217,7 @@
         <v>51</v>
       </c>
       <c r="Y117" s="20" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="AB117" t="str">
         <f t="shared" si="25"/>
@@ -12133,10 +12159,10 @@
         <v>65</v>
       </c>
       <c r="B98" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C98" s="19" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="D98" t="s">
         <v>111</v>
@@ -12148,10 +12174,10 @@
         <v>101</v>
       </c>
       <c r="I98" t="s">
+        <v>648</v>
+      </c>
+      <c r="J98" s="4" t="s">
         <v>649</v>
-      </c>
-      <c r="J98" s="4" t="s">
-        <v>650</v>
       </c>
       <c r="K98" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B98&amp;" resources for the specified "&amp;SUBSTITUTE(D98,","," and ")</f>
@@ -12163,13 +12189,13 @@
         <v>66</v>
       </c>
       <c r="B99" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C99" s="19" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="D99" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="F99" t="s">
         <v>65</v>
@@ -12178,13 +12204,13 @@
         <v>101</v>
       </c>
       <c r="H99" t="s">
+        <v>651</v>
+      </c>
+      <c r="I99" t="s">
+        <v>648</v>
+      </c>
+      <c r="J99" s="4" t="s">
         <v>652</v>
-      </c>
-      <c r="I99" t="s">
-        <v>649</v>
-      </c>
-      <c r="J99" s="4" t="s">
-        <v>653</v>
       </c>
       <c r="K99" t="str">
         <f>"Fetches a bundle of all "&amp;B99&amp;" resources for the specified "&amp;SUBSTITUTE(D99,","," and  ") &amp; "= 'sdoh'"</f>
@@ -12196,13 +12222,13 @@
         <v>67</v>
       </c>
       <c r="B100" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C100" s="19" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="D100" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="F100" t="s">
         <v>65</v>
@@ -12211,10 +12237,10 @@
         <v>144</v>
       </c>
       <c r="I100" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="J100" s="4" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="K100" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B100&amp;" resources for the specified patient and date"</f>
@@ -12226,13 +12252,13 @@
         <v>68</v>
       </c>
       <c r="B101" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C101" s="19" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="D101" s="17" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="F101" t="s">
         <v>65</v>
@@ -12241,13 +12267,13 @@
         <v>213</v>
       </c>
       <c r="H101" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="I101" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="J101" s="4" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="K101" t="str">
         <f>"Fetches a bundle of all "&amp;B101&amp;" resources tagged as 'sdoh' for the specified patient and date"</f>
@@ -12259,13 +12285,13 @@
         <v>69</v>
       </c>
       <c r="B102" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C102" s="19" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="D102" s="17" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="F102" t="s">
         <v>65</v>
@@ -12274,10 +12300,10 @@
         <v>86</v>
       </c>
       <c r="I102" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="J102" s="4" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="K102" t="str">
         <f>"Fetches a bundle of all "&amp;B102&amp;" resources for the specified patient that have been completed against a specified form."</f>
@@ -12361,7 +12387,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -12369,7 +12395,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -12534,7 +12560,7 @@
   <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12607,10 +12633,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B5" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
@@ -12621,10 +12647,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B6" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -12690,8 +12716,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="19" t="s">
-        <v>613</v>
+      <c r="A11" s="22" t="s">
+        <v>677</v>
       </c>
       <c r="B11" t="s">
         <v>360</v>
@@ -12703,88 +12729,88 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="19" t="s">
+    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="21" t="s">
+        <v>613</v>
+      </c>
+      <c r="B12" t="s">
         <v>614</v>
       </c>
-      <c r="B12" t="s">
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
         <v>615</v>
       </c>
-      <c r="D12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" t="s">
+    </row>
+    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="21" t="s">
         <v>616</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="19" t="s">
+      <c r="B13" t="s">
         <v>617</v>
       </c>
-      <c r="B13" t="s">
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="21" t="s">
         <v>618</v>
       </c>
-      <c r="D13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="19" t="s">
+      <c r="B14" t="s">
         <v>619</v>
       </c>
-      <c r="B14" t="s">
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="21" t="s">
         <v>620</v>
       </c>
-      <c r="D14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="19" t="s">
+      <c r="B15" t="s">
         <v>621</v>
       </c>
-      <c r="B15" t="s">
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="21" t="s">
         <v>622</v>
       </c>
-      <c r="D15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="19" t="s">
+      <c r="B16" t="s">
         <v>623</v>
       </c>
-      <c r="B16" t="s">
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="21" t="s">
         <v>624</v>
       </c>
-      <c r="D16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="19" t="s">
+      <c r="B17" t="s">
         <v>625</v>
       </c>
-      <c r="B17" t="s">
-        <v>626</v>
-      </c>
       <c r="D17" t="s">
         <v>11</v>
       </c>
       <c r="E17" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -12873,10 +12899,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="19" t="s">
+        <v>626</v>
+      </c>
+      <c r="B24" t="s">
         <v>627</v>
-      </c>
-      <c r="B24" t="s">
-        <v>628</v>
       </c>
       <c r="D24" t="s">
         <v>11</v>
@@ -12901,10 +12927,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="19" t="s">
+        <v>628</v>
+      </c>
+      <c r="B26" t="s">
         <v>629</v>
-      </c>
-      <c r="B26" t="s">
-        <v>630</v>
       </c>
       <c r="D26" t="s">
         <v>11</v>
@@ -12988,7 +13014,7 @@
         <v>545</v>
       </c>
       <c r="B32" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="D32" t="s">
         <v>11</v>
@@ -13041,10 +13067,10 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="19" t="s">
+        <v>631</v>
+      </c>
+      <c r="B36" t="s">
         <v>632</v>
-      </c>
-      <c r="B36" t="s">
-        <v>633</v>
       </c>
       <c r="D36" t="s">
         <v>11</v>
@@ -13072,7 +13098,7 @@
         <v>555</v>
       </c>
       <c r="B38" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="D38" t="s">
         <v>11</v>
@@ -13086,7 +13112,7 @@
         <v>548</v>
       </c>
       <c r="B39" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="D39" t="s">
         <v>11</v>
@@ -13114,7 +13140,7 @@
         <v>496</v>
       </c>
       <c r="B41" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="D41" t="s">
         <v>11</v>
@@ -13237,16 +13263,16 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="19" t="s">
+        <v>635</v>
+      </c>
+      <c r="B50" t="s">
         <v>636</v>
       </c>
-      <c r="B50" t="s">
+      <c r="D50" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" t="s">
         <v>637</v>
-      </c>
-      <c r="D50" t="s">
-        <v>11</v>
-      </c>
-      <c r="E50" t="s">
-        <v>638</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -13281,9 +13307,12 @@
       <c r="A53" s="19"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A11" r:id="rId1" xr:uid="{B6FCA6B1-777C-8E4D-A3C8-5CA8CC95525A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -13445,7 +13474,7 @@
         <v>65</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="T4" t="s">
         <v>556</v>
@@ -13474,7 +13503,7 @@
         <v>65</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="T5" t="s">
         <v>556</v>
@@ -13497,7 +13526,7 @@
         <v>65</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="T6" t="s">
         <v>556</v>
@@ -13541,7 +13570,7 @@
         <v>65</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="T8" t="s">
         <v>556</v>
@@ -13564,7 +13593,7 @@
         <v>65</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="T9" t="s">
         <v>556</v>
@@ -13607,7 +13636,7 @@
         <v>65</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="T11" t="s">
         <v>556</v>
@@ -13726,7 +13755,7 @@
         <v>65</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="T16" t="s">
         <v>556</v>
@@ -13749,7 +13778,7 @@
         <v>65</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="T17" t="s">
         <v>556</v>
@@ -13768,7 +13797,7 @@
         <v>65</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="T18" t="s">
         <v>556</v>
@@ -13832,7 +13861,7 @@
         <v>65</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="T21" t="s">
         <v>556</v>
@@ -13855,7 +13884,7 @@
         <v>65</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="T22" t="s">
         <v>556</v>
@@ -13866,13 +13895,13 @@
     </row>
     <row r="23" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>637</v>
+      </c>
+      <c r="B23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>638</v>
-      </c>
-      <c r="B23" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>639</v>
       </c>
       <c r="T23" t="s">
         <v>556</v>
@@ -14120,7 +14149,7 @@
         <v>429</v>
       </c>
       <c r="Y1" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="Z1" t="s">
         <v>559</v>

</xml_diff>

<commit_message>
change 'resources' to 'profiles' FHIR-37343
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C494EE-163D-9F43-ABB9-E84FC788AEB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635B4D3C-AAD7-9A4C-8327-019C5B3B5F76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -2260,52 +2260,30 @@
     <t>US Core Pediatric Head Occipital Frontal Circumference Percentile Profile</t>
   </si>
   <si>
-    <t>* The US Core Provenance resource **SHALL** be supported for these US Core
-resources:
-  * US Core CarePlan Profile
-  * US Core DiagnosticReport Profile for Laboratory Results Reporting
-  * US Core Encounter Profile
-  * US Core Observation Sexual Orientation Profile
-  * US Core Head Circumference Profile
-  * US Core ServiceRequest Profile
-  * US Core Vital Signs Profile
-  * US Core DiagnosticReport Profile for Report and Note Exchange
-  * US Core Implantable Device Profile
-  * US Core Observation Imaging Result Profile
-  * US Core CareTeam Profile
-  * US Core Pulse Oximetry Profile
-  * US Core BMI Profile
-  * US Core Blood Pressure Profile
-  * US Core Body Weight Profile
-  * US Core RelatedPerson Profile
-  * US Core Pediatric BMI for Age Observation Profile
-  * US Core MedicationRequest Profile
-  * US Core Condition Encounter Diagnosis Profile
-  * US Core Pediatric Head Occipital Frontal Circumference Percentile Profile
-  * US Core Procedure Profile
-  * US Core Laboratory Result Observation Profile
-  * US Core Body Height Profile
-  * US Core Observation SDOH Assessment Profile
-  * US Core Observation Survey Profile
-  * US Core Body Temperature Profile
-  * US Core Condition Problems and Health Concerns Profile
-  * US Core Pediatric Weight for Height Observation Profile
-  * US Core Goal Profile
-  * US Core AllergyIntolerance Profile
-  * US Core Immunization Profile
-  * US Core Observation Social History Profile
-  * US Core Heart Rate Profile
-  * US Core Smoking Status Observation Profile
-  * US Core Patient Profile
-  * US Core QuestionnaireResponse Profile
-  * US Core Respiratory Rate Profile
-  * US Core Observation Clinical Test Result Profile
-  * US Core DocumentReference Profile
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</t>
+  </si>
+  <si>
+    <t>* The US Core Provenance resource **SHALL** be supported for these US Core resources:
+    * AllergyIntolerance
+    * CarePlan
+    * CareTeam
+    * Condition
+    * Coverage
+    * Device
+    * DiagnosticReport
+    * DocumentReference
+    * Encounter
+    * Goal
+    * Immunization
+    * MedicationDispense
+    * MedicationRequest
+    * Observation
+    * Patient
+    * Procedure
+    * RelatedPerson
+    * ServiceRequest
 * If a system receives a provider in `Provenance.agent.who` as free text they must capture who sent them the information as the organization. On request they **SHALL** provide this organization as the source and **MAY** include the free text provider.
 * Systems that need to know the activity has occurred **SHOULD** populate the activity.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</t>
   </si>
 </sst>
 </file>
@@ -12559,7 +12537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -12717,7 +12695,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="22" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B11" t="s">
         <v>360</v>
@@ -13320,11 +13298,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Y62"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomRight" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="23" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13884,7 +13862,7 @@
         <v>65</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="T22" t="s">
         <v>556</v>

</xml_diff>

<commit_message>
Update US Core Practitioner to clarify work related contact information FHIR-36765
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1765EE5B-0B0E-5942-8B22-35EA2477251F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6FE1348-146A-3C44-96D3-FB6464D7B2A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2593" uniqueCount="689">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2594" uniqueCount="690">
   <si>
     <t>Element</t>
   </si>
@@ -2317,6 +2317,9 @@
     *  The `content.url` may refer to a FHIR Binary Resource (i.e. [base]/Binary/[id]), FHIR Document Bundle (i.e [base]/Bundle/[id] or another endpoint.
         * If the endpoint is outside the FHIR base URL, it **SHOULD NOT** require additional authorization to access.
 * Every DocumentReference must have a responsible Organization. The organization responsible for the DocumentReference **SHALL** be present either in `DocumentReference.custodian` or accessible in the Provenance resource targeting the DocumentReference using `Provenance.agent.who` or `Provenance.agent.onBehalfOf`.</t>
+  </si>
+  <si>
+    <t>Servers that support only US Core Practitioner Profile **SHALL** provide implementation specific guidance how to access a provider’s location and contact information using only the Practitioner resource.</t>
   </si>
 </sst>
 </file>
@@ -13674,10 +13677,10 @@
   <dimension ref="A1:Y62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="23" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -14171,6 +14174,9 @@
       </c>
       <c r="B19" t="s">
         <v>65</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>689</v>
       </c>
       <c r="T19" t="s">
         <v>537</v>

</xml_diff>

<commit_message>
Improve docref documentation FHIR-38746, Specify $docref's operates on DocumentReference endpoint FHIR-38658, Update $docref type input to multiple Codings FHIR-37894, Remove comment in $docref FHIR-38686
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6FE1348-146A-3C44-96D3-FB6464D7B2A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5890291E-8B7F-E04D-BC86-4FC4F978DC73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2594" uniqueCount="690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2594" uniqueCount="691">
   <si>
     <t>Element</t>
   </si>
@@ -1741,9 +1741,6 @@
     <t>http://hl7.org/fhir/uv/bulkdata/ImplementationGuide/hl7.fhir.uv.bulkdata</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/smart-app-launch/index.html</t>
-  </si>
-  <si>
     <t>http://hl7.org/fhir/uv/bulkdata/index.html</t>
   </si>
   <si>
@@ -2012,9 +2009,6 @@
   </si>
   <si>
     <t>US Core Observation Clinical Test Result Profile</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</t>
   </si>
   <si>
     <t>US Core QuestionnaireResponse Profile</t>
@@ -2320,6 +2314,15 @@
   </si>
   <si>
     <t>Servers that support only US Core Practitioner Profile **SHALL** provide implementation specific guidance how to access a provider’s location and contact information using only the Practitioner resource.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/smart-app-launch/history.html</t>
+  </si>
+  <si>
+    <t>!http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</t>
+  </si>
+  <si>
+    <t>!QuestionnaireResponse</t>
   </si>
 </sst>
 </file>
@@ -2496,7 +2499,7 @@
     <xf numFmtId="0" fontId="15" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2528,8 +2531,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="15" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -2537,7 +2541,68 @@
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2909,7 +2974,7 @@
         <v>448</v>
       </c>
       <c r="B2" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -2941,7 +3006,7 @@
         <v>63</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -2957,7 +3022,7 @@
         <v>455</v>
       </c>
       <c r="B8" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -2977,11 +3042,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD0B6320-EBCC-D945-ADE1-C0DCBBAED044}">
   <dimension ref="A1:AB126"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C90" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C93" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F133" sqref="F133"/>
+      <selection pane="bottomRight" activeCell="B116" sqref="B116:B121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3027,7 +3092,7 @@
         <v>39</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>30</v>
@@ -3983,7 +4048,7 @@
         <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="D19" t="s">
         <v>28</v>
@@ -4141,7 +4206,7 @@
         <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D22" t="s">
         <v>28</v>
@@ -4291,7 +4356,7 @@
         <v>19</v>
       </c>
       <c r="C25" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="D25" t="s">
         <v>28</v>
@@ -4350,7 +4415,7 @@
         <v>0</v>
       </c>
       <c r="F26" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="G26" t="str">
         <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B26)</f>
@@ -4568,7 +4633,7 @@
         <v>51</v>
       </c>
       <c r="Y30" s="4" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="Z30" t="s">
         <v>168</v>
@@ -4590,7 +4655,7 @@
         <v>80</v>
       </c>
       <c r="C31" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="D31" t="s">
         <v>28</v>
@@ -4615,19 +4680,19 @@
         <v>52</v>
       </c>
       <c r="L31" t="s">
+        <v>656</v>
+      </c>
+      <c r="M31" t="s">
+        <v>51</v>
+      </c>
+      <c r="O31" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y31" s="4" t="s">
+        <v>657</v>
+      </c>
+      <c r="Z31" t="s">
         <v>658</v>
-      </c>
-      <c r="M31" t="s">
-        <v>51</v>
-      </c>
-      <c r="O31" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y31" s="4" t="s">
-        <v>659</v>
-      </c>
-      <c r="Z31" t="s">
-        <v>660</v>
       </c>
       <c r="AA31" s="8" t="str">
         <f>"Fetches a bundle of all "&amp;B31&amp;" resources matching the name"</f>
@@ -5022,7 +5087,7 @@
         <v>133</v>
       </c>
       <c r="C40" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D40" t="s">
         <v>28</v>
@@ -5076,7 +5141,7 @@
         <v>133</v>
       </c>
       <c r="C41" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D41" t="s">
         <v>28</v>
@@ -5130,7 +5195,7 @@
         <v>133</v>
       </c>
       <c r="C42" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D42" t="s">
         <v>28</v>
@@ -5269,7 +5334,7 @@
         <v>51</v>
       </c>
       <c r="Y44" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="Z44" s="4" t="str">
         <f>"GET [base]/"&amp;B44&amp;"?patient=1137192"</f>
@@ -7476,7 +7541,7 @@
         <v>51</v>
       </c>
       <c r="X85" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="Y85" t="str">
         <f>"support searching for all "&amp;LOWER(B85)&amp;"s for a patient"</f>
@@ -7609,7 +7674,7 @@
         <v>241</v>
       </c>
       <c r="C88" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D88" t="s">
         <v>65</v>
@@ -7647,7 +7712,7 @@
         <v>51</v>
       </c>
       <c r="Y88" s="4" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="Z88" s="4" t="str">
         <f>"GET [base]/"&amp;B88&amp;"?"&amp;C88&amp;"=http://snomed.info/sct\|17561000"</f>
@@ -8611,7 +8676,7 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C106" t="s">
         <v>57</v>
@@ -8664,7 +8729,7 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C107" t="s">
         <v>85</v>
@@ -8723,7 +8788,7 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C108" t="s">
         <v>135</v>
@@ -8773,7 +8838,7 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C109" t="s">
         <v>24</v>
@@ -8826,10 +8891,10 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C110" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D110" t="s">
         <v>28</v>
@@ -8880,7 +8945,7 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C111" t="s">
         <v>50</v>
@@ -8915,10 +8980,10 @@
         <v>51</v>
       </c>
       <c r="Y111" s="4" t="s">
+        <v>552</v>
+      </c>
+      <c r="Z111" s="4" t="s">
         <v>553</v>
-      </c>
-      <c r="Z111" s="4" t="s">
-        <v>554</v>
       </c>
       <c r="AB111" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B111)&amp;"-"&amp;SUBSTITUTE(C111,"_","")&amp;".html")</f>
@@ -8976,7 +9041,7 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C113" t="s">
         <v>50</v>
@@ -9011,10 +9076,10 @@
         <v>51</v>
       </c>
       <c r="Y113" s="4" t="s">
+        <v>554</v>
+      </c>
+      <c r="Z113" s="4" t="s">
         <v>555</v>
-      </c>
-      <c r="Z113" s="4" t="s">
-        <v>556</v>
       </c>
       <c r="AA113" s="8"/>
       <c r="AB113" t="str">
@@ -9027,7 +9092,7 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C114" t="s">
         <v>85</v>
@@ -9086,7 +9151,7 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C115" t="s">
         <v>21</v>
@@ -9124,7 +9189,7 @@
         <v>51</v>
       </c>
       <c r="Y115" s="4" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="Z115" s="4" t="str">
         <f>"GET [base]/"&amp;B115&amp;"?"&amp;C115&amp;"=Mary Shaw"</f>
@@ -9144,7 +9209,7 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>615</v>
+        <v>690</v>
       </c>
       <c r="C116" t="s">
         <v>50</v>
@@ -9157,7 +9222,7 @@
       </c>
       <c r="G116" t="str">
         <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B116)</f>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="H116" t="s">
         <v>51</v>
@@ -9170,7 +9235,7 @@
       </c>
       <c r="L116" t="str">
         <f>B116&amp;"."&amp;C116</f>
-        <v>QuestionnaireResponse._id</v>
+        <v>!QuestionnaireResponse._id</v>
       </c>
       <c r="M116" t="s">
         <v>51</v>
@@ -9180,14 +9245,14 @@
       </c>
       <c r="Y116" s="4" t="str">
         <f>"support fetching a "&amp;B116</f>
-        <v>support fetching a QuestionnaireResponse</v>
+        <v>support fetching a !QuestionnaireResponse</v>
       </c>
       <c r="Z116" s="4" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="AB116" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B116)&amp;"-"&amp;SUBSTITUTE(C116,"_","")&amp;".html")</f>
-        <v>SearchParameter-us-core-questionnaireresponse-id.html</v>
+        <v>SearchParameter-us-core-!questionnaireresponse-id.html</v>
       </c>
     </row>
     <row r="117" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -9195,7 +9260,7 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>615</v>
+        <v>690</v>
       </c>
       <c r="C117" t="s">
         <v>85</v>
@@ -9211,7 +9276,7 @@
       </c>
       <c r="G117" t="str">
         <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B117)</f>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="H117" t="s">
         <v>51</v>
@@ -9224,7 +9289,7 @@
       </c>
       <c r="L117" t="str">
         <f>B117&amp;"."&amp;C117</f>
-        <v>QuestionnaireResponse.patient</v>
+        <v>!QuestionnaireResponse.patient</v>
       </c>
       <c r="M117" t="s">
         <v>51</v>
@@ -9234,19 +9299,19 @@
       </c>
       <c r="Y117" t="str">
         <f>"support searching for all "&amp;LOWER(B117)&amp;"s for a patient"</f>
-        <v>support searching for all questionnaireresponses for a patient</v>
+        <v>support searching for all !questionnaireresponses for a patient</v>
       </c>
       <c r="Z117" s="4" t="str">
         <f>"GET [base]/"&amp;B117&amp;"?patient=1032702"</f>
-        <v>GET [base]/QuestionnaireResponse?patient=1032702</v>
+        <v>GET [base]/!QuestionnaireResponse?patient=1032702</v>
       </c>
       <c r="AA117" s="8" t="str">
         <f>"Fetches a bundle of all "&amp;B117&amp; " resources for the specified patient"</f>
-        <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient</v>
+        <v>Fetches a bundle of all !QuestionnaireResponse resources for the specified patient</v>
       </c>
       <c r="AB117" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B117)&amp;"-"&amp;SUBSTITUTE(C117,"_","")&amp;".html")</f>
-        <v>SearchParameter-us-core-questionnaireresponse-patient.html</v>
+        <v>SearchParameter-us-core-!questionnaireresponse-patient.html</v>
       </c>
     </row>
     <row r="118" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -9254,7 +9319,7 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>615</v>
+        <v>690</v>
       </c>
       <c r="C118" t="s">
         <v>57</v>
@@ -9270,7 +9335,7 @@
       </c>
       <c r="G118" t="str">
         <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B118)</f>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="H118" t="s">
         <v>51</v>
@@ -9283,7 +9348,7 @@
       </c>
       <c r="L118" t="str">
         <f>B118&amp;"."&amp;C118</f>
-        <v>QuestionnaireResponse.status</v>
+        <v>!QuestionnaireResponse.status</v>
       </c>
       <c r="M118" t="s">
         <v>51</v>
@@ -9295,11 +9360,11 @@
         <v>51</v>
       </c>
       <c r="Y118" s="19" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="AB118" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B118)&amp;"-"&amp;SUBSTITUTE(C118,"_","")&amp;".html")</f>
-        <v>SearchParameter-us-core-questionnaireresponse-status.html</v>
+        <v>SearchParameter-us-core-!questionnaireresponse-status.html</v>
       </c>
     </row>
     <row r="119" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -9307,10 +9372,10 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>615</v>
+        <v>690</v>
       </c>
       <c r="C119" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="D119" t="s">
         <v>28</v>
@@ -9323,7 +9388,7 @@
       </c>
       <c r="G119" t="str">
         <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B119)</f>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="H119" t="s">
         <v>51</v>
@@ -9335,7 +9400,7 @@
         <v>52</v>
       </c>
       <c r="L119" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="M119" t="s">
         <v>51</v>
@@ -9344,11 +9409,11 @@
         <v>51</v>
       </c>
       <c r="Y119" s="19" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="AB119" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B119)&amp;"-"&amp;SUBSTITUTE(C119,"_","")&amp;".html")</f>
-        <v>SearchParameter-us-core-questionnaireresponse-tag.html</v>
+        <v>SearchParameter-us-core-!questionnaireresponse-tag.html</v>
       </c>
     </row>
     <row r="120" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -9356,10 +9421,10 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>615</v>
+        <v>690</v>
       </c>
       <c r="C120" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D120" t="s">
         <v>28</v>
@@ -9372,7 +9437,7 @@
       </c>
       <c r="G120" t="str">
         <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B120)</f>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="H120" t="s">
         <v>51</v>
@@ -9385,7 +9450,7 @@
       </c>
       <c r="L120" t="str">
         <f>B120&amp;"."&amp;C120</f>
-        <v>QuestionnaireResponse.authored</v>
+        <v>!QuestionnaireResponse.authored</v>
       </c>
       <c r="M120" t="s">
         <v>51</v>
@@ -9400,11 +9465,11 @@
         <v>88</v>
       </c>
       <c r="Y120" s="19" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="AB120" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B120)&amp;"-"&amp;SUBSTITUTE(C120,"_","")&amp;".html")</f>
-        <v>SearchParameter-us-core-questionnaireresponse-authored.html</v>
+        <v>SearchParameter-us-core-!questionnaireresponse-authored.html</v>
       </c>
     </row>
     <row r="121" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -9412,10 +9477,10 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>615</v>
+        <v>690</v>
       </c>
       <c r="C121" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="D121" t="s">
         <v>28</v>
@@ -9428,7 +9493,7 @@
       </c>
       <c r="G121" t="str">
         <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B121)</f>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="H121" t="s">
         <v>51</v>
@@ -9441,7 +9506,7 @@
       </c>
       <c r="L121" t="str">
         <f>B121&amp;"."&amp;C121</f>
-        <v>QuestionnaireResponse.questionnaire</v>
+        <v>!QuestionnaireResponse.questionnaire</v>
       </c>
       <c r="M121" t="s">
         <v>51</v>
@@ -9450,11 +9515,11 @@
         <v>51</v>
       </c>
       <c r="Y121" s="19" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="AB121" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B121)&amp;"-"&amp;SUBSTITUTE(C121,"_","")&amp;".html")</f>
-        <v>SearchParameter-us-core-questionnaireresponse-questionnaire.html</v>
+        <v>SearchParameter-us-core-!questionnaireresponse-questionnaire.html</v>
       </c>
     </row>
     <row r="122" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -9462,7 +9527,7 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="C122" t="s">
         <v>85</v>
@@ -9503,7 +9568,7 @@
         <v>51</v>
       </c>
       <c r="Y122" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="Z122" s="4" t="str">
         <f>"GET [base]/"&amp;B122&amp;"?patient=1137192"</f>
@@ -9523,7 +9588,7 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="C123" t="s">
         <v>57</v>
@@ -9579,7 +9644,7 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="C124" t="s">
         <v>12</v>
@@ -9635,7 +9700,7 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="C125" t="s">
         <v>85</v>
@@ -9676,10 +9741,10 @@
         <v>51</v>
       </c>
       <c r="X125" s="6" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="Z125" s="8" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="AA125" s="8" t="str">
         <f>"Fetches a bundle of all "&amp;B125&amp; " resources for the specified patient."</f>
@@ -9695,10 +9760,10 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="C126" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="D126" t="s">
         <v>28</v>
@@ -9749,6 +9814,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AB126" xr:uid="{1CF5B17E-E72E-48B2-A597-9C21C12723F0}"/>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="!">
+      <formula>NOT(ISERROR(SEARCH("!",B1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -9794,7 +9864,7 @@
         <v>91</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>92</v>
@@ -10224,7 +10294,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D17" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="F17" t="s">
         <v>65</v>
@@ -10236,7 +10306,7 @@
         <v>290</v>
       </c>
       <c r="J17" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="K17" s="4" t="str">
         <f t="shared" si="1"/>
@@ -10312,7 +10382,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D20" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="F20" t="s">
         <v>65</v>
@@ -10324,7 +10394,7 @@
         <v>295</v>
       </c>
       <c r="J20" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="K20" s="4" t="str">
         <f t="shared" si="1"/>
@@ -10634,7 +10704,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D32" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F32" t="s">
         <v>65</v>
@@ -10643,10 +10713,10 @@
         <v>129</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="K32" s="4" t="str">
         <f t="shared" si="1"/>
@@ -10776,7 +10846,7 @@
         <v>313</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
@@ -10824,7 +10894,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D38" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="F38" t="s">
         <v>65</v>
@@ -10836,10 +10906,10 @@
         <v>145</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
@@ -10896,7 +10966,7 @@
         <v>148</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="K40" s="4" t="s">
         <v>151</v>
@@ -10914,7 +10984,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D41" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="F41" t="s">
         <v>65</v>
@@ -10926,7 +10996,7 @@
         <v>148</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="K41" s="4" t="s">
         <v>151</v>
@@ -10944,7 +11014,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D42" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F42" t="s">
         <v>65</v>
@@ -10956,7 +11026,7 @@
         <v>148</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="K42" s="4" t="s">
         <v>151</v>
@@ -10974,7 +11044,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D43" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="F43" t="s">
         <v>65</v>
@@ -10986,7 +11056,7 @@
         <v>148</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="K43" s="4" t="s">
         <v>151</v>
@@ -11092,7 +11162,7 @@
         <v>174</v>
       </c>
       <c r="C47" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="D47" t="s">
         <v>111</v>
@@ -11122,7 +11192,7 @@
         <v>174</v>
       </c>
       <c r="C48" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="D48" t="s">
         <v>140</v>
@@ -11155,7 +11225,7 @@
         <v>174</v>
       </c>
       <c r="C49" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="D49" t="s">
         <v>142</v>
@@ -11185,7 +11255,7 @@
         <v>174</v>
       </c>
       <c r="C50" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="D50" t="s">
         <v>189</v>
@@ -11218,7 +11288,7 @@
         <v>174</v>
       </c>
       <c r="C51" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="D51" t="s">
         <v>213</v>
@@ -11596,7 +11666,7 @@
         <v>178</v>
       </c>
       <c r="C63" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="D63" t="s">
         <v>230</v>
@@ -11628,7 +11698,7 @@
         <v>178</v>
       </c>
       <c r="C64" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="D64" t="s">
         <v>140</v>
@@ -11661,7 +11731,7 @@
         <v>178</v>
       </c>
       <c r="C65" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="D65" t="s">
         <v>142</v>
@@ -11691,7 +11761,7 @@
         <v>178</v>
       </c>
       <c r="C66" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="D66" t="s">
         <v>189</v>
@@ -11724,7 +11794,7 @@
         <v>178</v>
       </c>
       <c r="C67" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="D67" t="s">
         <v>213</v>
@@ -11754,7 +11824,7 @@
         <v>305</v>
       </c>
       <c r="C68" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="D68" t="s">
         <v>111</v>
@@ -11929,13 +11999,13 @@
         <v>296</v>
       </c>
       <c r="I73" s="4" t="s">
+        <v>569</v>
+      </c>
+      <c r="J73" s="4" t="s">
         <v>570</v>
       </c>
-      <c r="J73" s="4" t="s">
+      <c r="K73" s="8" t="s">
         <v>571</v>
-      </c>
-      <c r="K73" s="8" t="s">
-        <v>572</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
@@ -12133,7 +12203,7 @@
         <v>242</v>
       </c>
       <c r="C80" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="D80" t="s">
         <v>113</v>
@@ -12162,7 +12232,7 @@
         <v>242</v>
       </c>
       <c r="C81" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="D81" t="s">
         <v>111</v>
@@ -12177,13 +12247,13 @@
         <v>101</v>
       </c>
       <c r="I81" s="4" t="s">
+        <v>671</v>
+      </c>
+      <c r="J81" s="4" t="s">
+        <v>672</v>
+      </c>
+      <c r="K81" s="4" t="s">
         <v>673</v>
-      </c>
-      <c r="J81" s="4" t="s">
-        <v>674</v>
-      </c>
-      <c r="K81" s="4" t="s">
-        <v>675</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
@@ -12198,7 +12268,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
       </c>
       <c r="D82" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="F82" t="s">
         <v>65</v>
@@ -12207,13 +12277,13 @@
         <v>101</v>
       </c>
       <c r="I82" s="4" t="s">
+        <v>573</v>
+      </c>
+      <c r="J82" s="4" t="s">
         <v>574</v>
       </c>
-      <c r="J82" s="4" t="s">
+      <c r="K82" s="4" t="s">
         <v>575</v>
-      </c>
-      <c r="K82" s="4" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
@@ -12221,7 +12291,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C83" t="str">
         <f t="shared" ref="C83:C96" si="4">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B83)</f>
@@ -12240,7 +12310,7 @@
         <v>288</v>
       </c>
       <c r="J83" s="4" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="K83" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B83&amp;" resources for the specified "&amp;SUBSTITUTE(D83,","," and ")</f>
@@ -12252,7 +12322,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C84" t="str">
         <f t="shared" si="4"/>
@@ -12271,7 +12341,7 @@
         <v>193</v>
       </c>
       <c r="J84" s="4" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="K84" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B84&amp;" resources for the specified patient and  a category code"</f>
@@ -12283,7 +12353,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C85" t="str">
         <f t="shared" si="4"/>
@@ -12302,7 +12372,7 @@
         <v>194</v>
       </c>
       <c r="J85" s="4" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="K85" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B85&amp;" resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes."</f>
@@ -12314,14 +12384,14 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C86" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D86" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="F86" t="s">
         <v>11</v>
@@ -12333,7 +12403,7 @@
         <v>196</v>
       </c>
       <c r="J86" s="4" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="K86" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B86&amp;" resources for the specified patient and date and a category code"</f>
@@ -12345,14 +12415,14 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C87" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D87" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="F87" t="s">
         <v>65</v>
@@ -12361,10 +12431,10 @@
         <v>212</v>
       </c>
       <c r="I87" s="4" t="s">
+        <v>582</v>
+      </c>
+      <c r="J87" s="4" t="s">
         <v>583</v>
-      </c>
-      <c r="J87" s="4" t="s">
-        <v>584</v>
       </c>
       <c r="K87" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B87&amp;" resources for the specified patient and date and service code(s).  SHOULD support search by multiple report codes."</f>
@@ -12383,7 +12453,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D88" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="F88" t="s">
         <v>65</v>
@@ -12392,10 +12462,10 @@
         <v>101</v>
       </c>
       <c r="I88" s="4" t="s">
+        <v>585</v>
+      </c>
+      <c r="J88" s="4" t="s">
         <v>586</v>
-      </c>
-      <c r="J88" s="4" t="s">
-        <v>587</v>
       </c>
       <c r="K88" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B88&amp;" resources for the specified "&amp;SUBSTITUTE(D88,","," and ")</f>
@@ -12407,7 +12477,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="C89" t="str">
         <f t="shared" si="4"/>
@@ -12423,10 +12493,10 @@
         <v>101</v>
       </c>
       <c r="I89" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="J89" s="4" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="K89" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B89&amp;" resources for the specified "&amp;SUBSTITUTE(D89,","," and ")</f>
@@ -12438,14 +12508,14 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="C90" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D90" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="F90" t="s">
         <v>65</v>
@@ -12454,13 +12524,13 @@
         <v>101</v>
       </c>
       <c r="H90" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="I90" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="J90" s="4" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="K90" t="str">
         <f>"Fetches a bundle of all "&amp;B90&amp;" resources for the specified "&amp;SUBSTITUTE(D90,","," and  ") &amp; "= 'sdoh'"</f>
@@ -12472,14 +12542,14 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="C91" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D91" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="F91" t="s">
         <v>65</v>
@@ -12488,10 +12558,10 @@
         <v>144</v>
       </c>
       <c r="I91" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="J91" s="4" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="K91" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B91&amp;" resources for the specified patient and date"</f>
@@ -12503,14 +12573,14 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="C92" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D92" s="16" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="F92" t="s">
         <v>65</v>
@@ -12519,13 +12589,13 @@
         <v>212</v>
       </c>
       <c r="H92" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="I92" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="J92" s="4" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="K92" t="str">
         <f>"Fetches a bundle of all "&amp;B92&amp;" resources tagged as 'sdoh' for the specified patient and date"</f>
@@ -12537,14 +12607,14 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="C93" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D93" s="16" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="F93" t="s">
         <v>65</v>
@@ -12553,10 +12623,10 @@
         <v>86</v>
       </c>
       <c r="I93" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="J93" s="4" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="K93" t="str">
         <f>"Fetches a bundle of all "&amp;B93&amp;" resources for the specified patient that have been completed against a specified form."</f>
@@ -12568,7 +12638,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="16" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="C94" t="str">
         <f t="shared" si="4"/>
@@ -12588,10 +12658,10 @@
       </c>
       <c r="H94" s="16"/>
       <c r="I94" s="4" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="J94" s="4" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="K94" t="str">
         <f>"Fetches a bundle of all "&amp;B94&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed))."</f>
@@ -12603,7 +12673,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="16" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="C95" t="str">
         <f t="shared" si="4"/>
@@ -12623,10 +12693,10 @@
       </c>
       <c r="H95" s="16"/>
       <c r="I95" s="4" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="J95" s="4" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="K95" t="str">
         <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed) and type of dispense (e.g., partially dispensed)."</f>
@@ -12638,14 +12708,14 @@
         <v>95</v>
       </c>
       <c r="B96" s="16" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="C96" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationdispense</v>
       </c>
       <c r="D96" s="16" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="E96" s="16" t="s">
         <v>51</v>
@@ -12658,10 +12728,10 @@
       </c>
       <c r="H96" s="16"/>
       <c r="I96" s="4" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="J96" s="4" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="K96" t="str">
         <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient for a given dispense and date or range"</f>
@@ -12703,7 +12773,7 @@
         <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -12743,7 +12813,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -12751,7 +12821,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -12796,7 +12866,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12824,30 +12894,33 @@
         <v>512</v>
       </c>
       <c r="B2" t="s">
-        <v>528</v>
-      </c>
-      <c r="C2" t="s">
+        <v>527</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>688</v>
+      </c>
+      <c r="D2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="21" t="s">
+        <v>681</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>522</v>
+      </c>
+      <c r="C3" s="21" t="s">
         <v>523</v>
       </c>
-      <c r="D2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
-        <v>683</v>
-      </c>
-      <c r="B3" s="22" t="s">
-        <v>522</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>524</v>
-      </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>65</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{DEF66039-9B20-2C43-9CB5-B3AF8A8243E1}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -12900,7 +12973,7 @@
         <v>516</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -12915,8 +12988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView topLeftCell="A81" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A99" sqref="A99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12989,10 +13062,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="B5" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
@@ -13003,10 +13076,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="B6" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -13072,8 +13145,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="21" t="s">
-        <v>653</v>
+      <c r="A11" s="23" t="s">
+        <v>651</v>
       </c>
       <c r="B11" t="s">
         <v>348</v>
@@ -13087,86 +13160,86 @@
     </row>
     <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
+        <v>590</v>
+      </c>
+      <c r="B12" t="s">
         <v>591</v>
       </c>
-      <c r="B12" t="s">
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
         <v>592</v>
-      </c>
-      <c r="D12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" t="s">
-        <v>593</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
+        <v>593</v>
+      </c>
+      <c r="B13" t="s">
         <v>594</v>
       </c>
-      <c r="B13" t="s">
-        <v>595</v>
-      </c>
       <c r="D13" t="s">
         <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
+        <v>595</v>
+      </c>
+      <c r="B14" t="s">
         <v>596</v>
       </c>
-      <c r="B14" t="s">
-        <v>597</v>
-      </c>
       <c r="D14" t="s">
         <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
+        <v>597</v>
+      </c>
+      <c r="B15" t="s">
         <v>598</v>
       </c>
-      <c r="B15" t="s">
-        <v>599</v>
-      </c>
       <c r="D15" t="s">
         <v>11</v>
       </c>
       <c r="E15" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
+        <v>599</v>
+      </c>
+      <c r="B16" t="s">
         <v>600</v>
       </c>
-      <c r="B16" t="s">
-        <v>601</v>
-      </c>
       <c r="D16" t="s">
         <v>11</v>
       </c>
       <c r="E16" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
+        <v>601</v>
+      </c>
+      <c r="B17" t="s">
         <v>602</v>
       </c>
-      <c r="B17" t="s">
-        <v>603</v>
-      </c>
       <c r="D17" t="s">
         <v>11</v>
       </c>
       <c r="E17" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -13255,10 +13328,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="18" t="s">
+        <v>603</v>
+      </c>
+      <c r="B24" t="s">
         <v>604</v>
-      </c>
-      <c r="B24" t="s">
-        <v>605</v>
       </c>
       <c r="D24" t="s">
         <v>11</v>
@@ -13283,10 +13356,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="18" t="s">
+        <v>605</v>
+      </c>
+      <c r="B26" t="s">
         <v>606</v>
-      </c>
-      <c r="B26" t="s">
-        <v>607</v>
       </c>
       <c r="D26" t="s">
         <v>11</v>
@@ -13367,10 +13440,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="18" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B32" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D32" t="s">
         <v>11</v>
@@ -13423,10 +13496,10 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="18" t="s">
+        <v>608</v>
+      </c>
+      <c r="B36" t="s">
         <v>609</v>
-      </c>
-      <c r="B36" t="s">
-        <v>610</v>
       </c>
       <c r="D36" t="s">
         <v>11</v>
@@ -13451,10 +13524,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="18" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B38" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="D38" t="s">
         <v>11</v>
@@ -13465,10 +13538,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="18" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B39" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="D39" t="s">
         <v>11</v>
@@ -13496,7 +13569,7 @@
         <v>481</v>
       </c>
       <c r="B41" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="D41" t="s">
         <v>11</v>
@@ -13619,56 +13692,61 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="18" t="s">
+        <v>689</v>
+      </c>
+      <c r="B50" t="s">
+        <v>612</v>
+      </c>
+      <c r="D50" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" t="s">
         <v>613</v>
-      </c>
-      <c r="B50" t="s">
-        <v>614</v>
-      </c>
-      <c r="D50" t="s">
-        <v>11</v>
-      </c>
-      <c r="E50" t="s">
-        <v>615</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="18" t="s">
+        <v>529</v>
+      </c>
+      <c r="B51" t="s">
         <v>530</v>
       </c>
-      <c r="B51" t="s">
+      <c r="D51" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" t="s">
         <v>531</v>
-      </c>
-      <c r="D51" t="s">
-        <v>11</v>
-      </c>
-      <c r="E51" t="s">
-        <v>532</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="18" t="s">
+        <v>532</v>
+      </c>
+      <c r="B52" t="s">
         <v>533</v>
       </c>
-      <c r="B52" t="s">
+      <c r="D52" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" t="s">
         <v>534</v>
-      </c>
-      <c r="D52" t="s">
-        <v>11</v>
-      </c>
-      <c r="E52" t="s">
-        <v>535</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="18"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A11" r:id="rId1" xr:uid="{B6FCA6B1-777C-8E4D-A3C8-5CA8CC95525A}"/>
-  </hyperlinks>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>"!"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="!">
+      <formula>NOT(ISERROR(SEARCH("!",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -13676,11 +13754,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Y62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomRight" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="23" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13787,7 +13865,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="T2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="U2" t="s">
         <v>65</v>
@@ -13810,7 +13888,7 @@
         <v>476</v>
       </c>
       <c r="T3" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="U3" t="s">
         <v>65</v>
@@ -13830,19 +13908,19 @@
         <v>65</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="T4" t="s">
+        <v>536</v>
+      </c>
+      <c r="U4" t="s">
+        <v>65</v>
+      </c>
+      <c r="V4" t="s">
         <v>537</v>
       </c>
-      <c r="U4" t="s">
-        <v>65</v>
-      </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>538</v>
-      </c>
-      <c r="W4" t="s">
-        <v>539</v>
       </c>
       <c r="X4" s="13" t="s">
         <v>435</v>
@@ -13859,10 +13937,10 @@
         <v>65</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="T5" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="U5" t="s">
         <v>65</v>
@@ -13882,10 +13960,10 @@
         <v>65</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="T6" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="U6" t="s">
         <v>65</v>
@@ -13906,7 +13984,7 @@
       </c>
       <c r="C7" s="2"/>
       <c r="T7" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="U7" t="s">
         <v>65</v>
@@ -13926,10 +14004,10 @@
         <v>65</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="T8" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="U8" t="s">
         <v>65</v>
@@ -13949,10 +14027,10 @@
         <v>65</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="T9" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="U9" t="s">
         <v>65</v>
@@ -13972,7 +14050,7 @@
         <v>65</v>
       </c>
       <c r="T10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="U10" t="s">
         <v>65</v>
@@ -13992,10 +14070,10 @@
         <v>65</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="T11" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="U11" t="s">
         <v>65</v>
@@ -14018,7 +14096,7 @@
         <v>477</v>
       </c>
       <c r="T12" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="U12" t="s">
         <v>65</v>
@@ -14037,7 +14115,7 @@
         <v>478</v>
       </c>
       <c r="T13" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="U13" t="s">
         <v>65</v>
@@ -14056,7 +14134,7 @@
         <v>479</v>
       </c>
       <c r="T14" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="U14" t="s">
         <v>65</v>
@@ -14085,7 +14163,7 @@
         <v>480</v>
       </c>
       <c r="T15" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="U15" t="s">
         <v>65</v>
@@ -14111,10 +14189,10 @@
         <v>65</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="T16" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="U16" t="s">
         <v>65</v>
@@ -14134,10 +14212,10 @@
         <v>65</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="T17" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="U17" t="s">
         <v>65</v>
@@ -14153,10 +14231,10 @@
         <v>65</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="T18" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="U18" t="s">
         <v>65</v>
@@ -14176,10 +14254,10 @@
         <v>65</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="T19" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="U19" t="s">
         <v>65</v>
@@ -14198,7 +14276,7 @@
         <v>477</v>
       </c>
       <c r="T20" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="U20" t="s">
         <v>65</v>
@@ -14220,10 +14298,10 @@
         <v>65</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="T21" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="U21" t="s">
         <v>65</v>
@@ -14243,10 +14321,10 @@
         <v>65</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="T22" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="U22" t="s">
         <v>65</v>
@@ -14254,16 +14332,16 @@
     </row>
     <row r="23" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>615</v>
+        <v>690</v>
       </c>
       <c r="B23" t="s">
         <v>65</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="T23" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="U23" t="s">
         <v>65</v>
@@ -14277,13 +14355,13 @@
     </row>
     <row r="24" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B24" t="s">
         <v>65</v>
       </c>
       <c r="T24" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="U24" t="s">
         <v>65</v>
@@ -14297,13 +14375,13 @@
     </row>
     <row r="25" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B25" t="s">
         <v>65</v>
       </c>
       <c r="T25" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="U25" t="s">
         <v>65</v>
@@ -14335,6 +14413,11 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A21">
     <sortCondition ref="A2:A21"/>
   </sortState>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="!">
+      <formula>NOT(ISERROR(SEARCH("!",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
 </worksheet>
@@ -14508,13 +14591,13 @@
         <v>417</v>
       </c>
       <c r="Y1" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="Z1" t="s">
+        <v>539</v>
+      </c>
+      <c r="AA1" t="s">
         <v>540</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>541</v>
       </c>
       <c r="AB1" t="s">
         <v>434</v>

</xml_diff>

<commit_message>
Add Conformance expectation of SHOULD to resolve for server Capability FHIR-3790
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5890291E-8B7F-E04D-BC86-4FC4F978DC73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53396AB-3A5F-B54F-8186-5E2ED90D431E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2594" uniqueCount="691">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2546" uniqueCount="690">
   <si>
     <t>Element</t>
   </si>
@@ -1778,9 +1778,6 @@
   </si>
   <si>
     <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-imaging</t>
-  </si>
-  <si>
-    <t>resolves</t>
   </si>
   <si>
     <t>SHOULD,SHOULD,SHOULD,SHOULD</t>
@@ -2974,7 +2971,7 @@
         <v>448</v>
       </c>
       <c r="B2" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -3006,7 +3003,7 @@
         <v>63</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -3022,7 +3019,7 @@
         <v>455</v>
       </c>
       <c r="B8" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -3042,7 +3039,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD0B6320-EBCC-D945-ADE1-C0DCBBAED044}">
   <dimension ref="A1:AB126"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C93" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -3092,7 +3089,7 @@
         <v>39</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>30</v>
@@ -4048,7 +4045,7 @@
         <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D19" t="s">
         <v>28</v>
@@ -4206,7 +4203,7 @@
         <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="D22" t="s">
         <v>28</v>
@@ -4356,7 +4353,7 @@
         <v>19</v>
       </c>
       <c r="C25" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="D25" t="s">
         <v>28</v>
@@ -4415,7 +4412,7 @@
         <v>0</v>
       </c>
       <c r="F26" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="G26" t="str">
         <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B26)</f>
@@ -4633,7 +4630,7 @@
         <v>51</v>
       </c>
       <c r="Y30" s="4" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="Z30" t="s">
         <v>168</v>
@@ -4655,7 +4652,7 @@
         <v>80</v>
       </c>
       <c r="C31" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="D31" t="s">
         <v>28</v>
@@ -4680,19 +4677,19 @@
         <v>52</v>
       </c>
       <c r="L31" t="s">
+        <v>655</v>
+      </c>
+      <c r="M31" t="s">
+        <v>51</v>
+      </c>
+      <c r="O31" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y31" s="4" t="s">
         <v>656</v>
       </c>
-      <c r="M31" t="s">
-        <v>51</v>
-      </c>
-      <c r="O31" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y31" s="4" t="s">
+      <c r="Z31" t="s">
         <v>657</v>
-      </c>
-      <c r="Z31" t="s">
-        <v>658</v>
       </c>
       <c r="AA31" s="8" t="str">
         <f>"Fetches a bundle of all "&amp;B31&amp;" resources matching the name"</f>
@@ -5087,7 +5084,7 @@
         <v>133</v>
       </c>
       <c r="C40" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D40" t="s">
         <v>28</v>
@@ -5141,7 +5138,7 @@
         <v>133</v>
       </c>
       <c r="C41" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D41" t="s">
         <v>28</v>
@@ -5195,7 +5192,7 @@
         <v>133</v>
       </c>
       <c r="C42" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D42" t="s">
         <v>28</v>
@@ -5334,7 +5331,7 @@
         <v>51</v>
       </c>
       <c r="Y44" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="Z44" s="4" t="str">
         <f>"GET [base]/"&amp;B44&amp;"?patient=1137192"</f>
@@ -7541,7 +7538,7 @@
         <v>51</v>
       </c>
       <c r="X85" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="Y85" t="str">
         <f>"support searching for all "&amp;LOWER(B85)&amp;"s for a patient"</f>
@@ -7674,7 +7671,7 @@
         <v>241</v>
       </c>
       <c r="C88" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D88" t="s">
         <v>65</v>
@@ -7712,7 +7709,7 @@
         <v>51</v>
       </c>
       <c r="Y88" s="4" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="Z88" s="4" t="str">
         <f>"GET [base]/"&amp;B88&amp;"?"&amp;C88&amp;"=http://snomed.info/sct\|17561000"</f>
@@ -8894,7 +8891,7 @@
         <v>534</v>
       </c>
       <c r="C110" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="D110" t="s">
         <v>28</v>
@@ -8980,10 +8977,10 @@
         <v>51</v>
       </c>
       <c r="Y111" s="4" t="s">
+        <v>551</v>
+      </c>
+      <c r="Z111" s="4" t="s">
         <v>552</v>
-      </c>
-      <c r="Z111" s="4" t="s">
-        <v>553</v>
       </c>
       <c r="AB111" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B111)&amp;"-"&amp;SUBSTITUTE(C111,"_","")&amp;".html")</f>
@@ -9076,10 +9073,10 @@
         <v>51</v>
       </c>
       <c r="Y113" s="4" t="s">
+        <v>553</v>
+      </c>
+      <c r="Z113" s="4" t="s">
         <v>554</v>
-      </c>
-      <c r="Z113" s="4" t="s">
-        <v>555</v>
       </c>
       <c r="AA113" s="8"/>
       <c r="AB113" t="str">
@@ -9189,7 +9186,7 @@
         <v>51</v>
       </c>
       <c r="Y115" s="4" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="Z115" s="4" t="str">
         <f>"GET [base]/"&amp;B115&amp;"?"&amp;C115&amp;"=Mary Shaw"</f>
@@ -9209,7 +9206,7 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C116" t="s">
         <v>50</v>
@@ -9248,7 +9245,7 @@
         <v>support fetching a !QuestionnaireResponse</v>
       </c>
       <c r="Z116" s="4" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="AB116" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B116)&amp;"-"&amp;SUBSTITUTE(C116,"_","")&amp;".html")</f>
@@ -9260,7 +9257,7 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C117" t="s">
         <v>85</v>
@@ -9319,7 +9316,7 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C118" t="s">
         <v>57</v>
@@ -9360,7 +9357,7 @@
         <v>51</v>
       </c>
       <c r="Y118" s="19" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="AB118" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B118)&amp;"-"&amp;SUBSTITUTE(C118,"_","")&amp;".html")</f>
@@ -9372,10 +9369,10 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C119" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="D119" t="s">
         <v>28</v>
@@ -9400,16 +9397,16 @@
         <v>52</v>
       </c>
       <c r="L119" t="s">
+        <v>618</v>
+      </c>
+      <c r="M119" t="s">
+        <v>51</v>
+      </c>
+      <c r="O119" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y119" s="19" t="s">
         <v>619</v>
-      </c>
-      <c r="M119" t="s">
-        <v>51</v>
-      </c>
-      <c r="O119" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y119" s="19" t="s">
-        <v>620</v>
       </c>
       <c r="AB119" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B119)&amp;"-"&amp;SUBSTITUTE(C119,"_","")&amp;".html")</f>
@@ -9421,10 +9418,10 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C120" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="D120" t="s">
         <v>28</v>
@@ -9465,7 +9462,7 @@
         <v>88</v>
       </c>
       <c r="Y120" s="19" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="AB120" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B120)&amp;"-"&amp;SUBSTITUTE(C120,"_","")&amp;".html")</f>
@@ -9477,10 +9474,10 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C121" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="D121" t="s">
         <v>28</v>
@@ -9515,7 +9512,7 @@
         <v>51</v>
       </c>
       <c r="Y121" s="19" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="AB121" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B121)&amp;"-"&amp;SUBSTITUTE(C121,"_","")&amp;".html")</f>
@@ -9527,7 +9524,7 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="C122" t="s">
         <v>85</v>
@@ -9568,7 +9565,7 @@
         <v>51</v>
       </c>
       <c r="Y122" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="Z122" s="4" t="str">
         <f>"GET [base]/"&amp;B122&amp;"?patient=1137192"</f>
@@ -9588,7 +9585,7 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C123" t="s">
         <v>57</v>
@@ -9644,7 +9641,7 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C124" t="s">
         <v>12</v>
@@ -9700,7 +9697,7 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C125" t="s">
         <v>85</v>
@@ -9741,10 +9738,10 @@
         <v>51</v>
       </c>
       <c r="X125" s="6" t="s">
+        <v>661</v>
+      </c>
+      <c r="Z125" s="8" t="s">
         <v>662</v>
-      </c>
-      <c r="Z125" s="8" t="s">
-        <v>663</v>
       </c>
       <c r="AA125" s="8" t="str">
         <f>"Fetches a bundle of all "&amp;B125&amp; " resources for the specified patient."</f>
@@ -9760,10 +9757,10 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
+        <v>663</v>
+      </c>
+      <c r="C126" t="s">
         <v>664</v>
-      </c>
-      <c r="C126" t="s">
-        <v>665</v>
       </c>
       <c r="D126" t="s">
         <v>28</v>
@@ -9864,7 +9861,7 @@
         <v>91</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>92</v>
@@ -10294,7 +10291,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D17" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F17" t="s">
         <v>65</v>
@@ -10306,7 +10303,7 @@
         <v>290</v>
       </c>
       <c r="J17" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="K17" s="4" t="str">
         <f t="shared" si="1"/>
@@ -10382,7 +10379,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D20" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F20" t="s">
         <v>65</v>
@@ -10394,7 +10391,7 @@
         <v>295</v>
       </c>
       <c r="J20" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="K20" s="4" t="str">
         <f t="shared" si="1"/>
@@ -10704,7 +10701,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D32" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="F32" t="s">
         <v>65</v>
@@ -10713,10 +10710,10 @@
         <v>129</v>
       </c>
       <c r="I32" s="4" t="s">
+        <v>666</v>
+      </c>
+      <c r="J32" s="4" t="s">
         <v>667</v>
-      </c>
-      <c r="J32" s="4" t="s">
-        <v>668</v>
       </c>
       <c r="K32" s="4" t="str">
         <f t="shared" si="1"/>
@@ -10846,7 +10843,7 @@
         <v>313</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
@@ -10894,7 +10891,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D38" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="F38" t="s">
         <v>65</v>
@@ -10906,10 +10903,10 @@
         <v>145</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
@@ -10966,7 +10963,7 @@
         <v>148</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="K40" s="4" t="s">
         <v>151</v>
@@ -10984,7 +10981,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D41" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="F41" t="s">
         <v>65</v>
@@ -10996,7 +10993,7 @@
         <v>148</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="K41" s="4" t="s">
         <v>151</v>
@@ -11014,7 +11011,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D42" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="F42" t="s">
         <v>65</v>
@@ -11026,7 +11023,7 @@
         <v>148</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="K42" s="4" t="s">
         <v>151</v>
@@ -11044,7 +11041,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D43" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="F43" t="s">
         <v>65</v>
@@ -11056,7 +11053,7 @@
         <v>148</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="K43" s="4" t="s">
         <v>151</v>
@@ -11162,7 +11159,7 @@
         <v>174</v>
       </c>
       <c r="C47" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="D47" t="s">
         <v>111</v>
@@ -11192,7 +11189,7 @@
         <v>174</v>
       </c>
       <c r="C48" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="D48" t="s">
         <v>140</v>
@@ -11225,7 +11222,7 @@
         <v>174</v>
       </c>
       <c r="C49" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="D49" t="s">
         <v>142</v>
@@ -11255,7 +11252,7 @@
         <v>174</v>
       </c>
       <c r="C50" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="D50" t="s">
         <v>189</v>
@@ -11288,7 +11285,7 @@
         <v>174</v>
       </c>
       <c r="C51" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="D51" t="s">
         <v>213</v>
@@ -11666,7 +11663,7 @@
         <v>178</v>
       </c>
       <c r="C63" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D63" t="s">
         <v>230</v>
@@ -11698,7 +11695,7 @@
         <v>178</v>
       </c>
       <c r="C64" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D64" t="s">
         <v>140</v>
@@ -11731,7 +11728,7 @@
         <v>178</v>
       </c>
       <c r="C65" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D65" t="s">
         <v>142</v>
@@ -11761,7 +11758,7 @@
         <v>178</v>
       </c>
       <c r="C66" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D66" t="s">
         <v>189</v>
@@ -11794,7 +11791,7 @@
         <v>178</v>
       </c>
       <c r="C67" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D67" t="s">
         <v>213</v>
@@ -11824,7 +11821,7 @@
         <v>305</v>
       </c>
       <c r="C68" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D68" t="s">
         <v>111</v>
@@ -11999,13 +11996,13 @@
         <v>296</v>
       </c>
       <c r="I73" s="4" t="s">
+        <v>568</v>
+      </c>
+      <c r="J73" s="4" t="s">
         <v>569</v>
       </c>
-      <c r="J73" s="4" t="s">
+      <c r="K73" s="8" t="s">
         <v>570</v>
-      </c>
-      <c r="K73" s="8" t="s">
-        <v>571</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
@@ -12203,7 +12200,7 @@
         <v>242</v>
       </c>
       <c r="C80" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="D80" t="s">
         <v>113</v>
@@ -12232,7 +12229,7 @@
         <v>242</v>
       </c>
       <c r="C81" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="D81" t="s">
         <v>111</v>
@@ -12247,13 +12244,13 @@
         <v>101</v>
       </c>
       <c r="I81" s="4" t="s">
+        <v>670</v>
+      </c>
+      <c r="J81" s="4" t="s">
         <v>671</v>
       </c>
-      <c r="J81" s="4" t="s">
+      <c r="K81" s="4" t="s">
         <v>672</v>
-      </c>
-      <c r="K81" s="4" t="s">
-        <v>673</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
@@ -12268,7 +12265,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
       </c>
       <c r="D82" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="F82" t="s">
         <v>65</v>
@@ -12277,13 +12274,13 @@
         <v>101</v>
       </c>
       <c r="I82" s="4" t="s">
+        <v>572</v>
+      </c>
+      <c r="J82" s="4" t="s">
         <v>573</v>
       </c>
-      <c r="J82" s="4" t="s">
+      <c r="K82" s="4" t="s">
         <v>574</v>
-      </c>
-      <c r="K82" s="4" t="s">
-        <v>575</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
@@ -12310,7 +12307,7 @@
         <v>288</v>
       </c>
       <c r="J83" s="4" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="K83" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B83&amp;" resources for the specified "&amp;SUBSTITUTE(D83,","," and ")</f>
@@ -12341,7 +12338,7 @@
         <v>193</v>
       </c>
       <c r="J84" s="4" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="K84" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B84&amp;" resources for the specified patient and  a category code"</f>
@@ -12372,7 +12369,7 @@
         <v>194</v>
       </c>
       <c r="J85" s="4" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="K85" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B85&amp;" resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes."</f>
@@ -12391,7 +12388,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D86" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="F86" t="s">
         <v>11</v>
@@ -12403,7 +12400,7 @@
         <v>196</v>
       </c>
       <c r="J86" s="4" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="K86" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B86&amp;" resources for the specified patient and date and a category code"</f>
@@ -12422,7 +12419,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D87" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="F87" t="s">
         <v>65</v>
@@ -12431,10 +12428,10 @@
         <v>212</v>
       </c>
       <c r="I87" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="J87" s="4" t="s">
         <v>582</v>
-      </c>
-      <c r="J87" s="4" t="s">
-        <v>583</v>
       </c>
       <c r="K87" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B87&amp;" resources for the specified patient and date and service code(s).  SHOULD support search by multiple report codes."</f>
@@ -12453,7 +12450,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D88" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="F88" t="s">
         <v>65</v>
@@ -12462,10 +12459,10 @@
         <v>101</v>
       </c>
       <c r="I88" s="4" t="s">
+        <v>584</v>
+      </c>
+      <c r="J88" s="4" t="s">
         <v>585</v>
-      </c>
-      <c r="J88" s="4" t="s">
-        <v>586</v>
       </c>
       <c r="K88" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B88&amp;" resources for the specified "&amp;SUBSTITUTE(D88,","," and ")</f>
@@ -12477,7 +12474,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C89" t="str">
         <f t="shared" si="4"/>
@@ -12493,10 +12490,10 @@
         <v>101</v>
       </c>
       <c r="I89" t="s">
+        <v>623</v>
+      </c>
+      <c r="J89" s="4" t="s">
         <v>624</v>
-      </c>
-      <c r="J89" s="4" t="s">
-        <v>625</v>
       </c>
       <c r="K89" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B89&amp;" resources for the specified "&amp;SUBSTITUTE(D89,","," and ")</f>
@@ -12508,14 +12505,14 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C90" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D90" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="F90" t="s">
         <v>65</v>
@@ -12524,13 +12521,13 @@
         <v>101</v>
       </c>
       <c r="H90" t="s">
+        <v>626</v>
+      </c>
+      <c r="I90" t="s">
+        <v>623</v>
+      </c>
+      <c r="J90" s="4" t="s">
         <v>627</v>
-      </c>
-      <c r="I90" t="s">
-        <v>624</v>
-      </c>
-      <c r="J90" s="4" t="s">
-        <v>628</v>
       </c>
       <c r="K90" t="str">
         <f>"Fetches a bundle of all "&amp;B90&amp;" resources for the specified "&amp;SUBSTITUTE(D90,","," and  ") &amp; "= 'sdoh'"</f>
@@ -12542,14 +12539,14 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C91" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D91" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="F91" t="s">
         <v>65</v>
@@ -12558,10 +12555,10 @@
         <v>144</v>
       </c>
       <c r="I91" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="J91" s="4" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="K91" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B91&amp;" resources for the specified patient and date"</f>
@@ -12573,14 +12570,14 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C92" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D92" s="16" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="F92" t="s">
         <v>65</v>
@@ -12589,13 +12586,13 @@
         <v>212</v>
       </c>
       <c r="H92" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="I92" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="J92" s="4" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="K92" t="str">
         <f>"Fetches a bundle of all "&amp;B92&amp;" resources tagged as 'sdoh' for the specified patient and date"</f>
@@ -12607,14 +12604,14 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C93" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D93" s="16" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="F93" t="s">
         <v>65</v>
@@ -12623,10 +12620,10 @@
         <v>86</v>
       </c>
       <c r="I93" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="J93" s="4" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="K93" t="str">
         <f>"Fetches a bundle of all "&amp;B93&amp;" resources for the specified patient that have been completed against a specified form."</f>
@@ -12638,7 +12635,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="16" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C94" t="str">
         <f t="shared" si="4"/>
@@ -12658,10 +12655,10 @@
       </c>
       <c r="H94" s="16"/>
       <c r="I94" s="4" t="s">
+        <v>673</v>
+      </c>
+      <c r="J94" s="4" t="s">
         <v>674</v>
-      </c>
-      <c r="J94" s="4" t="s">
-        <v>675</v>
       </c>
       <c r="K94" t="str">
         <f>"Fetches a bundle of all "&amp;B94&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed))."</f>
@@ -12673,7 +12670,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="16" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C95" t="str">
         <f t="shared" si="4"/>
@@ -12693,10 +12690,10 @@
       </c>
       <c r="H95" s="16"/>
       <c r="I95" s="4" t="s">
+        <v>675</v>
+      </c>
+      <c r="J95" s="4" t="s">
         <v>676</v>
-      </c>
-      <c r="J95" s="4" t="s">
-        <v>677</v>
       </c>
       <c r="K95" t="str">
         <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed) and type of dispense (e.g., partially dispensed)."</f>
@@ -12708,14 +12705,14 @@
         <v>95</v>
       </c>
       <c r="B96" s="16" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="C96" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationdispense</v>
       </c>
       <c r="D96" s="16" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="E96" s="16" t="s">
         <v>51</v>
@@ -12728,10 +12725,10 @@
       </c>
       <c r="H96" s="16"/>
       <c r="I96" s="4" t="s">
+        <v>678</v>
+      </c>
+      <c r="J96" s="4" t="s">
         <v>679</v>
-      </c>
-      <c r="J96" s="4" t="s">
-        <v>680</v>
       </c>
       <c r="K96" t="str">
         <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient for a given dispense and date or range"</f>
@@ -12813,7 +12810,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -12821,7 +12818,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -12897,7 +12894,7 @@
         <v>527</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="D2" t="s">
         <v>65</v>
@@ -12905,7 +12902,7 @@
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>522</v>
@@ -13062,10 +13059,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B5" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
@@ -13076,10 +13073,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B6" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -13146,7 +13143,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B11" t="s">
         <v>348</v>
@@ -13160,86 +13157,86 @@
     </row>
     <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
+        <v>589</v>
+      </c>
+      <c r="B12" t="s">
         <v>590</v>
       </c>
-      <c r="B12" t="s">
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
         <v>591</v>
-      </c>
-      <c r="D12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
+        <v>592</v>
+      </c>
+      <c r="B13" t="s">
         <v>593</v>
       </c>
-      <c r="B13" t="s">
-        <v>594</v>
-      </c>
       <c r="D13" t="s">
         <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
+        <v>594</v>
+      </c>
+      <c r="B14" t="s">
         <v>595</v>
       </c>
-      <c r="B14" t="s">
-        <v>596</v>
-      </c>
       <c r="D14" t="s">
         <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
+        <v>596</v>
+      </c>
+      <c r="B15" t="s">
         <v>597</v>
       </c>
-      <c r="B15" t="s">
-        <v>598</v>
-      </c>
       <c r="D15" t="s">
         <v>11</v>
       </c>
       <c r="E15" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
+        <v>598</v>
+      </c>
+      <c r="B16" t="s">
         <v>599</v>
       </c>
-      <c r="B16" t="s">
-        <v>600</v>
-      </c>
       <c r="D16" t="s">
         <v>11</v>
       </c>
       <c r="E16" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
+        <v>600</v>
+      </c>
+      <c r="B17" t="s">
         <v>601</v>
       </c>
-      <c r="B17" t="s">
-        <v>602</v>
-      </c>
       <c r="D17" t="s">
         <v>11</v>
       </c>
       <c r="E17" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -13328,10 +13325,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="18" t="s">
+        <v>602</v>
+      </c>
+      <c r="B24" t="s">
         <v>603</v>
-      </c>
-      <c r="B24" t="s">
-        <v>604</v>
       </c>
       <c r="D24" t="s">
         <v>11</v>
@@ -13356,10 +13353,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="18" t="s">
+        <v>604</v>
+      </c>
+      <c r="B26" t="s">
         <v>605</v>
-      </c>
-      <c r="B26" t="s">
-        <v>606</v>
       </c>
       <c r="D26" t="s">
         <v>11</v>
@@ -13443,7 +13440,7 @@
         <v>525</v>
       </c>
       <c r="B32" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D32" t="s">
         <v>11</v>
@@ -13496,10 +13493,10 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="18" t="s">
+        <v>607</v>
+      </c>
+      <c r="B36" t="s">
         <v>608</v>
-      </c>
-      <c r="B36" t="s">
-        <v>609</v>
       </c>
       <c r="D36" t="s">
         <v>11</v>
@@ -13527,7 +13524,7 @@
         <v>535</v>
       </c>
       <c r="B38" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D38" t="s">
         <v>11</v>
@@ -13541,7 +13538,7 @@
         <v>528</v>
       </c>
       <c r="B39" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="D39" t="s">
         <v>11</v>
@@ -13569,7 +13566,7 @@
         <v>481</v>
       </c>
       <c r="B41" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="D41" t="s">
         <v>11</v>
@@ -13692,16 +13689,16 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="18" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B50" t="s">
+        <v>611</v>
+      </c>
+      <c r="D50" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" t="s">
         <v>612</v>
-      </c>
-      <c r="D50" t="s">
-        <v>11</v>
-      </c>
-      <c r="E50" t="s">
-        <v>613</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -13754,11 +13751,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Y62"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C27" sqref="C27"/>
+      <selection pane="bottomRight" activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="23" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13777,7 +13774,7 @@
     <col min="22" max="25" width="38.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -13854,7 +13851,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="25.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="23" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -13864,12 +13861,6 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="T2" t="s">
-        <v>536</v>
-      </c>
-      <c r="U2" t="s">
-        <v>65</v>
-      </c>
       <c r="X2" s="13" t="s">
         <v>435</v>
       </c>
@@ -13877,7 +13868,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="163" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>227</v>
       </c>
@@ -13887,12 +13878,6 @@
       <c r="C3" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="T3" t="s">
-        <v>536</v>
-      </c>
-      <c r="U3" t="s">
-        <v>65</v>
-      </c>
       <c r="X3" s="13" t="s">
         <v>435</v>
       </c>
@@ -13900,7 +13885,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="279" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>241</v>
       </c>
@@ -13908,19 +13893,13 @@
         <v>65</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>639</v>
-      </c>
-      <c r="T4" t="s">
+        <v>638</v>
+      </c>
+      <c r="V4" t="s">
         <v>536</v>
       </c>
-      <c r="U4" t="s">
-        <v>65</v>
-      </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>537</v>
-      </c>
-      <c r="W4" t="s">
-        <v>538</v>
       </c>
       <c r="X4" s="13" t="s">
         <v>435</v>
@@ -13929,7 +13908,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>133</v>
       </c>
@@ -13937,13 +13916,7 @@
         <v>65</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>640</v>
-      </c>
-      <c r="T5" t="s">
-        <v>536</v>
-      </c>
-      <c r="U5" t="s">
-        <v>65</v>
+        <v>639</v>
       </c>
       <c r="X5" s="13" t="s">
         <v>435</v>
@@ -13952,7 +13925,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>242</v>
       </c>
@@ -13960,13 +13933,7 @@
         <v>65</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>641</v>
-      </c>
-      <c r="T6" t="s">
-        <v>536</v>
-      </c>
-      <c r="U6" t="s">
-        <v>65</v>
+        <v>640</v>
       </c>
       <c r="X6" s="13" t="s">
         <v>435</v>
@@ -13975,7 +13942,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>174</v>
       </c>
@@ -13983,12 +13950,6 @@
         <v>65</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="T7" t="s">
-        <v>536</v>
-      </c>
-      <c r="U7" t="s">
-        <v>65</v>
-      </c>
       <c r="X7" s="13" t="s">
         <v>435</v>
       </c>
@@ -13996,7 +13957,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>173</v>
       </c>
@@ -14004,13 +13965,7 @@
         <v>65</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>686</v>
-      </c>
-      <c r="T8" t="s">
-        <v>536</v>
-      </c>
-      <c r="U8" t="s">
-        <v>65</v>
+        <v>685</v>
       </c>
       <c r="X8" s="13" t="s">
         <v>435</v>
@@ -14019,7 +13974,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -14027,13 +13982,7 @@
         <v>65</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>642</v>
-      </c>
-      <c r="T9" t="s">
-        <v>536</v>
-      </c>
-      <c r="U9" t="s">
-        <v>65</v>
+        <v>641</v>
       </c>
       <c r="X9" s="13" t="s">
         <v>435</v>
@@ -14042,19 +13991,13 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>175</v>
       </c>
       <c r="B10" t="s">
         <v>65</v>
       </c>
-      <c r="T10" t="s">
-        <v>536</v>
-      </c>
-      <c r="U10" t="s">
-        <v>65</v>
-      </c>
       <c r="X10" s="13" t="s">
         <v>435</v>
       </c>
@@ -14062,7 +14005,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>156</v>
       </c>
@@ -14070,13 +14013,7 @@
         <v>65</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>643</v>
-      </c>
-      <c r="T11" t="s">
-        <v>536</v>
-      </c>
-      <c r="U11" t="s">
-        <v>65</v>
+        <v>642</v>
       </c>
       <c r="X11" s="13" t="s">
         <v>435</v>
@@ -14085,7 +14022,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>243</v>
       </c>
@@ -14095,16 +14032,10 @@
       <c r="C12" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="T12" t="s">
-        <v>536</v>
-      </c>
-      <c r="U12" t="s">
-        <v>65</v>
-      </c>
       <c r="X12" s="13"/>
       <c r="Y12" s="13"/>
     </row>
-    <row r="13" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>337</v>
       </c>
@@ -14114,16 +14045,10 @@
       <c r="C13" s="1" t="s">
         <v>478</v>
       </c>
-      <c r="T13" t="s">
-        <v>536</v>
-      </c>
-      <c r="U13" t="s">
-        <v>65</v>
-      </c>
       <c r="X13" s="13"/>
       <c r="Y13" s="13"/>
     </row>
-    <row r="14" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>176</v>
       </c>
@@ -14133,12 +14058,6 @@
       <c r="C14" s="1" t="s">
         <v>479</v>
       </c>
-      <c r="T14" t="s">
-        <v>536</v>
-      </c>
-      <c r="U14" t="s">
-        <v>65</v>
-      </c>
       <c r="V14" t="s">
         <v>65</v>
       </c>
@@ -14152,7 +14071,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>423</v>
       </c>
@@ -14162,12 +14081,6 @@
       <c r="C15" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="T15" t="s">
-        <v>536</v>
-      </c>
-      <c r="U15" t="s">
-        <v>65</v>
-      </c>
       <c r="V15" t="s">
         <v>65</v>
       </c>
@@ -14181,7 +14094,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>178</v>
       </c>
@@ -14189,13 +14102,7 @@
         <v>65</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>644</v>
-      </c>
-      <c r="T16" t="s">
-        <v>536</v>
-      </c>
-      <c r="U16" t="s">
-        <v>65</v>
+        <v>643</v>
       </c>
       <c r="X16" s="13" t="s">
         <v>435</v>
@@ -14204,7 +14111,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>253</v>
       </c>
@@ -14212,18 +14119,12 @@
         <v>65</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>645</v>
-      </c>
-      <c r="T17" t="s">
-        <v>536</v>
-      </c>
-      <c r="U17" t="s">
-        <v>65</v>
+        <v>644</v>
       </c>
       <c r="X17" s="13"/>
       <c r="Y17" s="13"/>
     </row>
-    <row r="18" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -14231,13 +14132,7 @@
         <v>65</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>646</v>
-      </c>
-      <c r="T18" t="s">
-        <v>536</v>
-      </c>
-      <c r="U18" t="s">
-        <v>65</v>
+        <v>645</v>
       </c>
       <c r="X18" s="13" t="s">
         <v>435</v>
@@ -14246,7 +14141,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>260</v>
       </c>
@@ -14254,18 +14149,12 @@
         <v>65</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>687</v>
-      </c>
-      <c r="T19" t="s">
-        <v>536</v>
-      </c>
-      <c r="U19" t="s">
-        <v>65</v>
+        <v>686</v>
       </c>
       <c r="X19" s="13"/>
       <c r="Y19" s="13"/>
     </row>
-    <row r="20" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>262</v>
       </c>
@@ -14275,12 +14164,6 @@
       <c r="C20" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="T20" t="s">
-        <v>536</v>
-      </c>
-      <c r="U20" t="s">
-        <v>65</v>
-      </c>
       <c r="V20" t="s">
         <v>521</v>
       </c>
@@ -14290,7 +14173,7 @@
       <c r="X20" s="13"/>
       <c r="Y20" s="13"/>
     </row>
-    <row r="21" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>177</v>
       </c>
@@ -14298,13 +14181,7 @@
         <v>65</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>647</v>
-      </c>
-      <c r="T21" t="s">
-        <v>536</v>
-      </c>
-      <c r="U21" t="s">
-        <v>65</v>
+        <v>646</v>
       </c>
       <c r="X21" s="13" t="s">
         <v>435</v>
@@ -14313,7 +14190,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>416</v>
       </c>
@@ -14321,30 +14198,18 @@
         <v>65</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>652</v>
-      </c>
-      <c r="T22" t="s">
-        <v>536</v>
-      </c>
-      <c r="U22" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B23" t="s">
         <v>65</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>614</v>
-      </c>
-      <c r="T23" t="s">
-        <v>536</v>
-      </c>
-      <c r="U23" t="s">
-        <v>65</v>
+        <v>613</v>
       </c>
       <c r="X23" s="13" t="s">
         <v>435</v>
@@ -14353,19 +14218,13 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>531</v>
       </c>
       <c r="B24" t="s">
         <v>65</v>
       </c>
-      <c r="T24" t="s">
-        <v>536</v>
-      </c>
-      <c r="U24" t="s">
-        <v>65</v>
-      </c>
       <c r="X24" s="13" t="s">
         <v>435</v>
       </c>
@@ -14373,19 +14232,13 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>534</v>
       </c>
       <c r="B25" t="s">
         <v>65</v>
       </c>
-      <c r="T25" t="s">
-        <v>536</v>
-      </c>
-      <c r="U25" t="s">
-        <v>65</v>
-      </c>
       <c r="X25" s="13" t="s">
         <v>435</v>
       </c>
@@ -14393,7 +14246,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>430</v>
       </c>
@@ -14401,12 +14254,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="59" spans="22:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="22:25" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="V59" s="6"/>
       <c r="X59" s="6"/>
       <c r="Y59" s="6"/>
     </row>
-    <row r="62" spans="22:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="22:25" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y62" s="6"/>
     </row>
   </sheetData>
@@ -14591,13 +14444,13 @@
         <v>417</v>
       </c>
       <c r="Y1" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="Z1" t="s">
+        <v>538</v>
+      </c>
+      <c r="AA1" t="s">
         <v>539</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>540</v>
       </c>
       <c r="AB1" t="s">
         <v>434</v>

</xml_diff>

<commit_message>
Add USCDI V3 Requirements FHIR-38702 - reason for referral changes to SR and Proc and examples
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161F50B2-0AAB-5845-952B-2DD1FED5293F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAABF732-CEAF-DE46-8AD1-6EBD8667A141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
     <sheet name="meta" sheetId="1" r:id="rId2"/>
     <sheet name="igs" sheetId="10" r:id="rId3"/>
     <sheet name="capstatements" sheetId="13" r:id="rId4"/>
-    <sheet name="profiles" sheetId="2" r:id="rId5"/>
+    <sheet name="profiles" sheetId="23" r:id="rId5"/>
     <sheet name="resources" sheetId="4" r:id="rId6"/>
     <sheet name="ops" sheetId="5" r:id="rId7"/>
     <sheet name="interactions" sheetId="6" r:id="rId8"/>
     <sheet name="rest_interactions" sheetId="11" r:id="rId9"/>
     <sheet name="sps" sheetId="20" r:id="rId10"/>
-    <sheet name="sp_combos" sheetId="21" r:id="rId11"/>
+    <sheet name="sp_combos" sheetId="22" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">sp_combos!$A$1:$K$96</definedName>
@@ -44,40 +44,6 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>User</author>
-  </authors>
-  <commentList>
-    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{6820CBB5-E079-4C49-8DAA-4A5FA09B0DD0}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={F80C4D5F-754A-BE44-8144-8F9387CD5898}</author>
@@ -113,15 +79,15 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={4B683F90-C00C-A74C-9F16-520D513D279B}</author>
-    <author>tc={AD36599E-6850-6647-94F5-BC3E349388EE}</author>
-    <author>tc={1FB031C4-5603-CB46-9901-9885749EFFB1}</author>
+    <author>tc={D123EF51-46F1-1341-AF16-81EA94978931}</author>
+    <author>tc={A157258E-CBF6-C345-9459-64FF9319F2BC}</author>
+    <author>tc={D311E409-D311-0C43-BC63-D68872BACEF4}</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{4B683F90-C00C-A74C-9F16-520D513D279B}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{D123EF51-46F1-1341-AF16-81EA94978931}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -131,7 +97,7 @@
     make this a comma separate list of profiles</t>
       </text>
     </comment>
-    <comment ref="I1" authorId="1" shapeId="0" xr:uid="{AD36599E-6850-6647-94F5-BC3E349388EE}">
+    <comment ref="I1" authorId="1" shapeId="0" xr:uid="{A157258E-CBF6-C345-9459-64FF9319F2BC}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -139,7 +105,7 @@
     does this do anything if not delete row</t>
       </text>
     </comment>
-    <comment ref="I40" authorId="2" shapeId="0" xr:uid="{1FB031C4-5603-CB46-9901-9885749EFFB1}">
+    <comment ref="I40" authorId="2" shapeId="0" xr:uid="{D311E409-D311-0C43-BC63-D68872BACEF4}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -152,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2547" uniqueCount="690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2571" uniqueCount="703">
   <si>
     <t>Element</t>
   </si>
@@ -1753,9 +1719,6 @@
     <t>http://hl7.org/fhir/smart-app-launch/ImplementationGuide/hl7.fhir.uv.smart-app-launch</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-clinical-test</t>
-  </si>
-  <si>
     <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-relatedperson</t>
   </si>
   <si>
@@ -1772,9 +1735,6 @@
   </si>
   <si>
     <t>ServiceRequest</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-imaging</t>
   </si>
   <si>
     <t>SHOULD,SHOULD,SHOULD,SHOULD</t>
@@ -1978,13 +1938,7 @@
     <t>US Core Extension Questionnaire URI</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-sdoh-assessment</t>
-  </si>
-  <si>
     <t>US Core Observation SDOH Assessment Profile</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-social-history</t>
   </si>
   <si>
     <t>US Core Observation Social History Profile</t>
@@ -2321,12 +2275,63 @@
   <si>
     <t>Allows retrieving !QuestionnaireResponses that have been completed against a specified form</t>
   </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-coverage</t>
+  </si>
+  <si>
+    <t>US Core Coverage Profile</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</t>
+  </si>
+  <si>
+    <t>US Core MedicationDispense Profile</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-pregnancystatus</t>
+  </si>
+  <si>
+    <t>US Core Observation Pregnancy Status Profile</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-pregnancyintent</t>
+  </si>
+  <si>
+    <t>US Core Observation Pregnancy Intent Profile</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-occupation</t>
+  </si>
+  <si>
+    <t>US Core Observation Occupation Profile</t>
+  </si>
+  <si>
+    <t>!http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-sdoh-assessment</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-simple-observation</t>
+  </si>
+  <si>
+    <t>!http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-imaging</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-clinical-result</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-specimen</t>
+  </si>
+  <si>
+    <t>US Core Specimen Profile</t>
+  </si>
+  <si>
+    <t>Specimen</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2404,19 +2409,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="16"/>
       <color rgb="FF333333"/>
       <name val="Helvetica Neue"/>
@@ -2436,12 +2428,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2493,10 +2479,10 @@
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2526,10 +2512,11 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="13" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -2537,7 +2524,17 @@
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2908,16 +2905,16 @@
 
 <file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="C1" dT="2021-11-10T17:47:31.83" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{4B683F90-C00C-A74C-9F16-520D513D279B}">
+  <threadedComment ref="C1" dT="2021-11-10T17:47:31.83" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{D123EF51-46F1-1341-AF16-81EA94978931}">
     <text>add column for include file</text>
   </threadedComment>
-  <threadedComment ref="C1" dT="2021-11-10T17:48:52.85" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{2E8672F5-A2AB-DE4A-8FAD-F9E65AAA452C}" parentId="{4B683F90-C00C-A74C-9F16-520D513D279B}">
+  <threadedComment ref="C1" dT="2021-11-10T17:48:52.85" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{CE8B7051-AD03-244E-85A2-5F2F1087AA1F}" parentId="{D123EF51-46F1-1341-AF16-81EA94978931}">
     <text>make this a comma separate list of profiles</text>
   </threadedComment>
-  <threadedComment ref="I1" dT="2021-11-08T19:54:50.37" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{AD36599E-6850-6647-94F5-BC3E349388EE}">
+  <threadedComment ref="I1" dT="2021-11-08T19:54:50.37" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{A157258E-CBF6-C345-9459-64FF9319F2BC}">
     <text>does this do anything if not delete row</text>
   </threadedComment>
-  <threadedComment ref="I40" dT="2021-11-06T02:44:23.26" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{1FB031C4-5603-CB46-9901-9885749EFFB1}">
+  <threadedComment ref="I40" dT="2021-11-06T02:44:23.26" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{D311E409-D311-0C43-BC63-D68872BACEF4}">
     <text>is column being used???</text>
   </threadedComment>
 </ThreadedComments>
@@ -2950,7 +2947,7 @@
         <v>447</v>
       </c>
       <c r="B2" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -2982,7 +2979,7 @@
         <v>62</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -2998,7 +2995,7 @@
         <v>454</v>
       </c>
       <c r="B8" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -3069,7 +3066,7 @@
         <v>39</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>30</v>
@@ -4025,7 +4022,7 @@
         <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="D19" t="s">
         <v>28</v>
@@ -4183,7 +4180,7 @@
         <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="D22" t="s">
         <v>28</v>
@@ -4333,7 +4330,7 @@
         <v>19</v>
       </c>
       <c r="C25" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="D25" t="s">
         <v>28</v>
@@ -4392,7 +4389,7 @@
         <v>0</v>
       </c>
       <c r="F26" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="0"/>
@@ -4610,7 +4607,7 @@
         <v>51</v>
       </c>
       <c r="Y30" s="4" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="Z30" t="s">
         <v>167</v>
@@ -4632,7 +4629,7 @@
         <v>79</v>
       </c>
       <c r="C31" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="D31" t="s">
         <v>28</v>
@@ -4657,7 +4654,7 @@
         <v>52</v>
       </c>
       <c r="L31" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="M31" t="s">
         <v>51</v>
@@ -4666,10 +4663,10 @@
         <v>51</v>
       </c>
       <c r="Y31" s="4" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="Z31" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="AA31" s="8" t="str">
         <f>"Fetches a bundle of all "&amp;B31&amp;" resources matching the name"</f>
@@ -4685,7 +4682,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="C32" t="s">
         <v>50</v>
@@ -4710,7 +4707,7 @@
         <v>52</v>
       </c>
       <c r="L32" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="M32" t="s">
         <v>51</v>
@@ -4728,7 +4725,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="C33" t="s">
         <v>65</v>
@@ -4772,7 +4769,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="C34" t="s">
         <v>62</v>
@@ -4819,7 +4816,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="C35" t="s">
         <v>56</v>
@@ -4863,7 +4860,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="C36" t="s">
         <v>57</v>
@@ -4919,7 +4916,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="C37" t="s">
         <v>54</v>
@@ -4963,7 +4960,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="C38" t="s">
         <v>61</v>
@@ -5064,7 +5061,7 @@
         <v>132</v>
       </c>
       <c r="C40" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="D40" t="s">
         <v>28</v>
@@ -5118,7 +5115,7 @@
         <v>132</v>
       </c>
       <c r="C41" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="D41" t="s">
         <v>28</v>
@@ -5172,7 +5169,7 @@
         <v>132</v>
       </c>
       <c r="C42" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="D42" t="s">
         <v>28</v>
@@ -5311,7 +5308,7 @@
         <v>51</v>
       </c>
       <c r="Y44" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="Z44" s="4" t="str">
         <f>"GET [base]/"&amp;B44&amp;"?patient=1137192"</f>
@@ -7518,7 +7515,7 @@
         <v>51</v>
       </c>
       <c r="X85" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="Y85" t="str">
         <f>"support searching for all "&amp;LOWER(B85)&amp;"s for a patient"</f>
@@ -7651,7 +7648,7 @@
         <v>240</v>
       </c>
       <c r="C88" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="D88" t="s">
         <v>64</v>
@@ -7689,7 +7686,7 @@
         <v>51</v>
       </c>
       <c r="Y88" s="4" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="Z88" s="4" t="str">
         <f>"GET [base]/"&amp;B88&amp;"?"&amp;C88&amp;"=http://snomed.info/sct\|17561000"</f>
@@ -8656,7 +8653,7 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C106" t="s">
         <v>56</v>
@@ -8709,7 +8706,7 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C107" t="s">
         <v>84</v>
@@ -8768,7 +8765,7 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C108" t="s">
         <v>134</v>
@@ -8818,7 +8815,7 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C109" t="s">
         <v>24</v>
@@ -8871,10 +8868,10 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C110" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="D110" t="s">
         <v>28</v>
@@ -8925,7 +8922,7 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C111" t="s">
         <v>50</v>
@@ -8960,10 +8957,10 @@
         <v>51</v>
       </c>
       <c r="Y111" s="4" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="Z111" s="4" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="AB111" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B111)&amp;"-"&amp;SUBSTITUTE(C111,"_","")&amp;".html")</f>
@@ -9021,7 +9018,7 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C113" t="s">
         <v>50</v>
@@ -9056,10 +9053,10 @@
         <v>51</v>
       </c>
       <c r="Y113" s="4" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="Z113" s="4" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="AA113" s="8"/>
       <c r="AB113" t="str">
@@ -9072,7 +9069,7 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C114" t="s">
         <v>84</v>
@@ -9131,7 +9128,7 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C115" t="s">
         <v>21</v>
@@ -9169,7 +9166,7 @@
         <v>51</v>
       </c>
       <c r="Y115" s="4" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="Z115" s="4" t="str">
         <f>"GET [base]/"&amp;B115&amp;"?"&amp;C115&amp;"=Mary Shaw"</f>
@@ -9189,7 +9186,7 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="C116" t="s">
         <v>50</v>
@@ -9228,7 +9225,7 @@
         <v>support fetching a !QuestionnaireResponse</v>
       </c>
       <c r="Z116" s="4" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="AB116" t="str">
         <f t="shared" si="9"/>
@@ -9240,7 +9237,7 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="C117" t="s">
         <v>84</v>
@@ -9299,7 +9296,7 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="C118" t="s">
         <v>56</v>
@@ -9340,7 +9337,7 @@
         <v>51</v>
       </c>
       <c r="Y118" s="19" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="AB118" t="str">
         <f t="shared" si="9"/>
@@ -9352,10 +9349,10 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="C119" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="D119" t="s">
         <v>28</v>
@@ -9380,7 +9377,7 @@
         <v>52</v>
       </c>
       <c r="L119" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="M119" t="s">
         <v>51</v>
@@ -9389,7 +9386,7 @@
         <v>51</v>
       </c>
       <c r="Y119" s="19" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="AB119" t="str">
         <f t="shared" si="9"/>
@@ -9401,10 +9398,10 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="C120" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="D120" t="s">
         <v>28</v>
@@ -9445,7 +9442,7 @@
         <v>87</v>
       </c>
       <c r="Y120" s="19" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="AB120" t="str">
         <f t="shared" si="9"/>
@@ -9457,10 +9454,10 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="C121" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="D121" t="s">
         <v>28</v>
@@ -9495,7 +9492,7 @@
         <v>51</v>
       </c>
       <c r="Y121" s="19" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="AB121" t="str">
         <f t="shared" si="9"/>
@@ -9507,7 +9504,7 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="C122" t="s">
         <v>84</v>
@@ -9548,7 +9545,7 @@
         <v>51</v>
       </c>
       <c r="Y122" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="Z122" s="4" t="str">
         <f>"GET [base]/"&amp;B122&amp;"?patient=1137192"</f>
@@ -9568,7 +9565,7 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="C123" t="s">
         <v>56</v>
@@ -9624,7 +9621,7 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="C124" t="s">
         <v>12</v>
@@ -9680,7 +9677,7 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="C125" t="s">
         <v>84</v>
@@ -9721,10 +9718,10 @@
         <v>51</v>
       </c>
       <c r="X125" s="6" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="Z125" s="8" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="AA125" s="8" t="str">
         <f>"Fetches a bundle of all "&amp;B125&amp; " resources for the specified patient."</f>
@@ -9740,10 +9737,10 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="C126" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="D126" t="s">
         <v>28</v>
@@ -9801,7 +9798,7 @@
     </filterColumn>
   </autoFilter>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9812,12 +9809,11 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CF727CF-CEC3-F547-97AE-8C150084E4C3}">
-  <sheetPr filterMode="1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E7AC33C-2643-EE4B-9487-6CC99572F031}">
   <dimension ref="A1:K96"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C132" sqref="C132"/>
+    <sheetView topLeftCell="A56" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9848,7 +9844,7 @@
         <v>90</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>91</v>
@@ -9869,7 +9865,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -9894,7 +9890,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -9919,7 +9915,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and patient</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -9944,7 +9940,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and patient and type</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -9969,7 +9965,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and type</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -10000,7 +9996,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified class and patient</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -10025,7 +10021,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and status</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -10050,7 +10046,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and status and type</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -10076,7 +10072,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and type</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -10103,7 +10099,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and status</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -10129,7 +10125,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and status and type</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -10154,7 +10150,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and type</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -10185,7 +10181,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified date and patient</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -10210,7 +10206,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified date and patient and type</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -10235,7 +10231,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified date and type</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -10266,7 +10262,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified patient and type</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -10278,7 +10274,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D17" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="F17" t="s">
         <v>64</v>
@@ -10290,14 +10286,14 @@
         <v>289</v>
       </c>
       <c r="J17" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="K17" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Fetches a bundle of all Encounter resources matching the specified patient and location</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -10323,7 +10319,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified patient and status and type</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -10354,7 +10350,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified patient and status</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -10366,7 +10362,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D20" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="F20" t="s">
         <v>64</v>
@@ -10378,14 +10374,14 @@
         <v>294</v>
       </c>
       <c r="J20" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="K20" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Fetches a bundle of all Encounter resources matching the specified patient and discharge-disposition</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -10412,7 +10408,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified status and type</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -10438,7 +10434,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and publisher</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -10463,7 +10459,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and publisher and status</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -10489,7 +10485,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and status</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -10516,7 +10512,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and status</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -10543,7 +10539,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and status and version</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -10570,7 +10566,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and version</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -10595,7 +10591,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified status and title and version</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -10620,7 +10616,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified status and version</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -10645,7 +10641,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified title and version</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -10676,7 +10672,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified birthdate and family</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -10688,7 +10684,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D32" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="F32" t="s">
         <v>64</v>
@@ -10697,17 +10693,17 @@
         <v>128</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="K32" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Fetches a bundle of all Patient resources matching the specified death-date and family</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -10738,7 +10734,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified birthdate and name</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -10769,7 +10765,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified family and gender</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -10800,7 +10796,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified gender and name</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -10830,10 +10826,10 @@
         <v>312</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -10866,7 +10862,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -10878,7 +10874,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D38" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="F38" t="s">
         <v>64</v>
@@ -10890,13 +10886,13 @@
         <v>144</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -10926,7 +10922,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -10950,13 +10946,13 @@
         <v>147</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="K40" s="4" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -10968,7 +10964,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D41" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="F41" t="s">
         <v>64</v>
@@ -10980,13 +10976,13 @@
         <v>147</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="K41" s="4" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -10998,7 +10994,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D42" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="F42" t="s">
         <v>64</v>
@@ -11010,13 +11006,13 @@
         <v>147</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="K42" s="4" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -11028,7 +11024,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D43" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="F43" t="s">
         <v>64</v>
@@ -11040,13 +11036,13 @@
         <v>147</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="K43" s="4" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -11076,7 +11072,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -11107,7 +11103,7 @@
         <v>Fetches a bundle of all Immunization resources for the specified patient and date</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -11138,7 +11134,7 @@
         <v>Fetches a bundle of all Immunization resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -11146,7 +11142,7 @@
         <v>173</v>
       </c>
       <c r="C47" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="D47" t="s">
         <v>110</v>
@@ -11168,7 +11164,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="17" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -11176,7 +11172,7 @@
         <v>173</v>
       </c>
       <c r="C48" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="D48" t="s">
         <v>139</v>
@@ -11201,7 +11197,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  a category code = `LAB`</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="17" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -11209,7 +11205,7 @@
         <v>173</v>
       </c>
       <c r="C49" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="D49" t="s">
         <v>141</v>
@@ -11231,7 +11227,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="17" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -11239,7 +11235,7 @@
         <v>173</v>
       </c>
       <c r="C50" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="D50" t="s">
         <v>188</v>
@@ -11264,7 +11260,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and a category code = `LAB`</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -11272,7 +11268,7 @@
         <v>173</v>
       </c>
       <c r="C51" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="D51" t="s">
         <v>212</v>
@@ -11294,7 +11290,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -11325,7 +11321,7 @@
         <v>Fetches a bundle of all Goal resources for the specified patient and lifecycle-status</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -11356,7 +11352,7 @@
         <v>Fetches a bundle of all Goal resources for the specified patient and target-date</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -11389,7 +11385,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -11422,7 +11418,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -11455,7 +11451,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -11488,7 +11484,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -11519,7 +11515,7 @@
         <v>Fetches a bundle of all !MedicationStatement resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -11549,7 +11545,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -11580,7 +11576,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -11611,7 +11607,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and date</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -11642,7 +11638,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and date and procedure code(s).  SHOULD support search by multiple codes.</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -11650,7 +11646,7 @@
         <v>177</v>
       </c>
       <c r="C63" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="D63" t="s">
         <v>229</v>
@@ -11674,7 +11670,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -11682,7 +11678,7 @@
         <v>177</v>
       </c>
       <c r="C64" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="D64" t="s">
         <v>139</v>
@@ -11707,7 +11703,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and a category code = `laboratory`</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -11715,7 +11711,7 @@
         <v>177</v>
       </c>
       <c r="C65" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="D65" t="s">
         <v>141</v>
@@ -11737,7 +11733,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and observation code(s).  SHOULD support search by multiple report codes. The Observation `code` parameter searches `Observation.code only.</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -11745,7 +11741,7 @@
         <v>177</v>
       </c>
       <c r="C66" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="D66" t="s">
         <v>188</v>
@@ -11770,7 +11766,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and date and a category code = `laboratory`</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -11778,7 +11774,7 @@
         <v>177</v>
       </c>
       <c r="C67" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="D67" t="s">
         <v>212</v>
@@ -11800,7 +11796,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -11808,7 +11804,7 @@
         <v>304</v>
       </c>
       <c r="C68" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="D68" t="s">
         <v>110</v>
@@ -11830,7 +11826,7 @@
         <v>Fetches a bundle of all !Observation resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -11863,7 +11859,7 @@
         <v>Fetches a bundle of all CarePlan resources for the specified patient and category=`assess-plan`</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -11895,7 +11891,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -11927,7 +11923,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -11959,7 +11955,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="137" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" ht="136" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -11983,16 +11979,16 @@
         <v>295</v>
       </c>
       <c r="I73" s="4" t="s">
+        <v>565</v>
+      </c>
+      <c r="J73" s="4" t="s">
+        <v>566</v>
+      </c>
+      <c r="K73" s="8" t="s">
         <v>567</v>
       </c>
-      <c r="J73" s="4" t="s">
-        <v>568</v>
-      </c>
-      <c r="K73" s="8" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -12023,7 +12019,7 @@
         <v>Fetches a bundle of all DocumentReference resources for the specified patient and status. See the implementation notes above for how to access the actual document.</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -12052,7 +12048,7 @@
         <v>Fetches a bundle of all !DocumentReference resources for the specified patient and period. See the implementation notes above for how to access the actual document.</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -12085,7 +12081,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -12118,7 +12114,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
@@ -12148,7 +12144,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="79" spans="1:11" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>
@@ -12179,7 +12175,7 @@
         <v>Fetches a bundle of all DocumentReference resources for the specified patient and type and period. See the implementation notes above for how to access the actual document.</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>79</v>
       </c>
@@ -12187,7 +12183,7 @@
         <v>241</v>
       </c>
       <c r="C80" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="D80" t="s">
         <v>112</v>
@@ -12216,7 +12212,7 @@
         <v>241</v>
       </c>
       <c r="C81" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="D81" t="s">
         <v>110</v>
@@ -12231,16 +12227,16 @@
         <v>100</v>
       </c>
       <c r="I81" s="4" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="J81" s="4" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="K81" s="4" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>81</v>
       </c>
@@ -12252,7 +12248,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
       </c>
       <c r="D82" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="F82" t="s">
         <v>64</v>
@@ -12261,21 +12257,21 @@
         <v>100</v>
       </c>
       <c r="I82" s="4" t="s">
+        <v>569</v>
+      </c>
+      <c r="J82" s="4" t="s">
+        <v>570</v>
+      </c>
+      <c r="K82" s="4" t="s">
         <v>571</v>
       </c>
-      <c r="J82" s="4" t="s">
-        <v>572</v>
-      </c>
-      <c r="K82" s="4" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C83" t="str">
         <f t="shared" ref="C83:C96" si="4">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B83)</f>
@@ -12294,19 +12290,19 @@
         <v>287</v>
       </c>
       <c r="J83" s="4" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="K83" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B83&amp;" resources for the specified "&amp;SUBSTITUTE(D83,","," and ")</f>
         <v>Fetches a bundle of all ServiceRequest resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C84" t="str">
         <f t="shared" si="4"/>
@@ -12325,19 +12321,19 @@
         <v>192</v>
       </c>
       <c r="J84" s="4" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="K84" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B84&amp;" resources for the specified patient and  a category code"</f>
         <v>Fetches a bundle of all ServiceRequest resources for the specified patient and  a category code</v>
       </c>
     </row>
-    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C85" t="str">
         <f t="shared" si="4"/>
@@ -12356,26 +12352,26 @@
         <v>193</v>
       </c>
       <c r="J85" s="4" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="K85" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B85&amp;" resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes."</f>
         <v>Fetches a bundle of all ServiceRequest resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C86" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D86" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="F86" t="s">
         <v>11</v>
@@ -12387,26 +12383,26 @@
         <v>195</v>
       </c>
       <c r="J86" s="4" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="K86" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B86&amp;" resources for the specified patient and date and a category code"</f>
         <v>Fetches a bundle of all ServiceRequest resources for the specified patient and date and a category code</v>
       </c>
     </row>
-    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C87" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D87" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="F87" t="s">
         <v>64</v>
@@ -12415,17 +12411,17 @@
         <v>211</v>
       </c>
       <c r="I87" s="4" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="J87" s="4" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="K87" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B87&amp;" resources for the specified patient and date and service code(s).  SHOULD support search by multiple report codes."</f>
         <v>Fetches a bundle of all ServiceRequest resources for the specified patient and date and service code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>87</v>
       </c>
@@ -12437,7 +12433,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D88" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="F88" t="s">
         <v>64</v>
@@ -12446,26 +12442,26 @@
         <v>100</v>
       </c>
       <c r="I88" s="4" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="J88" s="4" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="K88" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B88&amp;" resources for the specified "&amp;SUBSTITUTE(D88,","," and ")</f>
         <v>Fetches a bundle of all Goal resources for the specified patient and description</v>
       </c>
     </row>
-    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>611</v>
+        <v>677</v>
       </c>
       <c r="C89" t="str">
         <f t="shared" si="4"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="D89" t="s">
         <v>110</v>
@@ -12477,29 +12473,29 @@
         <v>100</v>
       </c>
       <c r="I89" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="J89" s="4" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="K89" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B89&amp;" resources for the specified "&amp;SUBSTITUTE(D89,","," and ")</f>
-        <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient and status</v>
-      </c>
-    </row>
-    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+        <v>Fetches a bundle of all !QuestionnaireResponse resources for the specified patient and status</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>611</v>
+        <v>677</v>
       </c>
       <c r="C90" t="str">
         <f t="shared" si="4"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="D90" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="F90" t="s">
         <v>64</v>
@@ -12508,32 +12504,32 @@
         <v>100</v>
       </c>
       <c r="H90" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="I90" t="s">
+        <v>612</v>
+      </c>
+      <c r="J90" s="4" t="s">
         <v>616</v>
-      </c>
-      <c r="J90" s="4" t="s">
-        <v>620</v>
       </c>
       <c r="K90" t="str">
         <f>"Fetches a bundle of all "&amp;B90&amp;" resources for the specified "&amp;SUBSTITUTE(D90,","," and  ") &amp; "= 'sdoh'"</f>
-        <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient and  _tag= 'sdoh'</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+        <v>Fetches a bundle of all !QuestionnaireResponse resources for the specified patient and  _tag= 'sdoh'</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>611</v>
+        <v>677</v>
       </c>
       <c r="C91" t="str">
         <f t="shared" si="4"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="D91" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="F91" t="s">
         <v>64</v>
@@ -12542,29 +12538,29 @@
         <v>143</v>
       </c>
       <c r="I91" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="J91" s="4" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="K91" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B91&amp;" resources for the specified patient and date"</f>
-        <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient and date</v>
-      </c>
-    </row>
-    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+        <v>Fetches a bundle of all !QuestionnaireResponse resources for the specified patient and date</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>611</v>
+        <v>677</v>
       </c>
       <c r="C92" t="str">
         <f t="shared" si="4"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="D92" s="16" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="F92" t="s">
         <v>64</v>
@@ -12573,32 +12569,32 @@
         <v>211</v>
       </c>
       <c r="H92" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="I92" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="J92" s="4" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="K92" t="str">
         <f>"Fetches a bundle of all "&amp;B92&amp;" resources tagged as 'sdoh' for the specified patient and date"</f>
-        <v>Fetches a bundle of all QuestionnaireResponse resources tagged as 'sdoh' for the specified patient and date</v>
-      </c>
-    </row>
-    <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+        <v>Fetches a bundle of all !QuestionnaireResponse resources tagged as 'sdoh' for the specified patient and date</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>611</v>
+        <v>677</v>
       </c>
       <c r="C93" t="str">
         <f t="shared" si="4"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="D93" s="16" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="F93" t="s">
         <v>64</v>
@@ -12607,22 +12603,22 @@
         <v>85</v>
       </c>
       <c r="I93" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="J93" s="4" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="K93" t="str">
         <f>"Fetches a bundle of all "&amp;B93&amp;" resources for the specified patient that have been completed against a specified form."</f>
-        <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient that have been completed against a specified form.</v>
-      </c>
-    </row>
-    <row r="94" spans="1:11" ht="151" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>Fetches a bundle of all !QuestionnaireResponse resources for the specified patient that have been completed against a specified form.</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" ht="151" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>93</v>
       </c>
       <c r="B94" s="16" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="C94" t="str">
         <f t="shared" si="4"/>
@@ -12642,22 +12638,22 @@
       </c>
       <c r="H94" s="16"/>
       <c r="I94" s="4" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="J94" s="4" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="K94" t="str">
         <f>"Fetches a bundle of all "&amp;B94&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed))."</f>
         <v>Fetches a bundle of all MedicationDispense resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed)).</v>
       </c>
     </row>
-    <row r="95" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>94</v>
       </c>
       <c r="B95" s="16" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="C95" t="str">
         <f t="shared" si="4"/>
@@ -12677,29 +12673,29 @@
       </c>
       <c r="H95" s="16"/>
       <c r="I95" s="4" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="J95" s="4" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="K95" t="str">
         <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed) and type of dispense (e.g., partially dispensed)."</f>
         <v>Fetches a bundle of all MedicationDispense resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed) and type of dispense (e.g., partially dispensed).</v>
       </c>
     </row>
-    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>95</v>
       </c>
       <c r="B96" s="16" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="C96" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationdispense</v>
       </c>
       <c r="D96" s="16" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="E96" s="16" t="s">
         <v>51</v>
@@ -12712,10 +12708,10 @@
       </c>
       <c r="H96" s="16"/>
       <c r="I96" s="4" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="J96" s="4" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
       <c r="K96" t="str">
         <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient for a given dispense and date or range"</f>
@@ -12723,13 +12719,12 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K96" xr:uid="{331E0B16-168F-459B-8951-3DF614BF0371}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Device"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:K96" xr:uid="{331E0B16-168F-459B-8951-3DF614BF0371}"/>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="!">
+      <formula>NOT(ISERROR(SEARCH("!",B1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -12803,7 +12798,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -12811,7 +12806,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -12887,7 +12882,7 @@
         <v>526</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="D2" t="s">
         <v>64</v>
@@ -12895,7 +12890,7 @@
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>521</v>
@@ -12975,18 +12970,18 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E53"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5583FAA5-D04D-8A4F-B7E2-586644D7B670}">
+  <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView topLeftCell="A81" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A99" sqref="A99"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="94" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="60.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" customWidth="1"/>
     <col min="4" max="4" width="20.1640625" customWidth="1"/>
     <col min="5" max="5" width="16.1640625" customWidth="1"/>
   </cols>
@@ -13009,7 +13004,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="18" t="s">
         <v>67</v>
       </c>
       <c r="B2" t="s">
@@ -13023,7 +13018,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="18" t="s">
         <v>228</v>
       </c>
       <c r="B3" t="s">
@@ -13037,7 +13032,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="18" t="s">
         <v>319</v>
       </c>
       <c r="B4" t="s">
@@ -13051,11 +13046,11 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>640</v>
+      <c r="A5" s="18" t="s">
+        <v>636</v>
       </c>
       <c r="B5" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
@@ -13065,11 +13060,11 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>641</v>
+      <c r="A6" s="18" t="s">
+        <v>637</v>
       </c>
       <c r="B6" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -13080,38 +13075,38 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>405</v>
+        <v>686</v>
       </c>
       <c r="B7" t="s">
-        <v>404</v>
+        <v>687</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>241</v>
+        <v>647</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
-        <v>183</v>
+        <v>405</v>
       </c>
       <c r="B8" t="s">
-        <v>337</v>
+        <v>404</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>173</v>
+        <v>241</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B9" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -13122,220 +13117,220 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="B10" t="s">
+        <v>345</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="18" t="s">
         <v>326</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>327</v>
       </c>
-      <c r="D10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>643</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>639</v>
+      </c>
+      <c r="B12" t="s">
         <v>347</v>
       </c>
-      <c r="D11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="20" t="s">
-        <v>588</v>
-      </c>
-      <c r="B12" t="s">
-        <v>589</v>
-      </c>
-      <c r="D12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
       <c r="B13" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
       <c r="D13" t="s">
         <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="B14" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="D14" t="s">
         <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="B15" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="D15" t="s">
         <v>11</v>
       </c>
       <c r="E15" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="B16" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="D16" t="s">
         <v>11</v>
       </c>
       <c r="E16" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="B17" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="D17" t="s">
         <v>11</v>
       </c>
       <c r="E17" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="18" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="20" t="s">
+        <v>597</v>
+      </c>
+      <c r="B18" t="s">
+        <v>598</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>341</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>342</v>
       </c>
-      <c r="D18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="18" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>323</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>324</v>
       </c>
-      <c r="D19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="D20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" t="s">
         <v>155</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="18" t="s">
-        <v>343</v>
-      </c>
-      <c r="B20" t="s">
-        <v>344</v>
-      </c>
-      <c r="D20" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="18" t="s">
-        <v>334</v>
+        <v>343</v>
       </c>
       <c r="B21" t="s">
-        <v>335</v>
+        <v>344</v>
       </c>
       <c r="D21" t="s">
         <v>11</v>
       </c>
       <c r="E21" t="s">
-        <v>336</v>
+        <v>242</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="18" t="s">
-        <v>328</v>
+        <v>334</v>
       </c>
       <c r="B22" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="D22" t="s">
         <v>11</v>
       </c>
       <c r="E22" t="s">
-        <v>175</v>
+        <v>336</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="18" t="s">
-        <v>390</v>
+        <v>328</v>
       </c>
       <c r="B23" t="s">
-        <v>391</v>
+        <v>329</v>
       </c>
       <c r="D23" t="s">
         <v>11</v>
       </c>
       <c r="E23" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="18" t="s">
-        <v>601</v>
+      <c r="A24" t="s">
+        <v>688</v>
       </c>
       <c r="B24" t="s">
-        <v>602</v>
+        <v>689</v>
       </c>
       <c r="D24" t="s">
         <v>11</v>
       </c>
       <c r="E24" t="s">
-        <v>177</v>
+        <v>649</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="18" t="s">
-        <v>472</v>
+        <v>390</v>
       </c>
       <c r="B25" t="s">
-        <v>473</v>
+        <v>391</v>
       </c>
       <c r="D25" t="s">
         <v>11</v>
@@ -13345,11 +13340,11 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="18" t="s">
-        <v>603</v>
+      <c r="A26" t="s">
+        <v>690</v>
       </c>
       <c r="B26" t="s">
-        <v>604</v>
+        <v>691</v>
       </c>
       <c r="D26" t="s">
         <v>11</v>
@@ -13359,11 +13354,11 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="18" t="s">
-        <v>470</v>
+      <c r="A27" t="s">
+        <v>692</v>
       </c>
       <c r="B27" t="s">
-        <v>471</v>
+        <v>693</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
@@ -13373,11 +13368,11 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="18" t="s">
-        <v>468</v>
+      <c r="A28" t="s">
+        <v>694</v>
       </c>
       <c r="B28" t="s">
-        <v>469</v>
+        <v>695</v>
       </c>
       <c r="D28" t="s">
         <v>11</v>
@@ -13388,10 +13383,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="18" t="s">
-        <v>484</v>
+        <v>696</v>
       </c>
       <c r="B29" t="s">
-        <v>485</v>
+        <v>599</v>
       </c>
       <c r="D29" t="s">
         <v>11</v>
@@ -13402,10 +13397,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="18" t="s">
-        <v>411</v>
+        <v>472</v>
       </c>
       <c r="B30" t="s">
-        <v>412</v>
+        <v>473</v>
       </c>
       <c r="D30" t="s">
         <v>11</v>
@@ -13415,11 +13410,11 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="18" t="s">
-        <v>267</v>
+      <c r="A31" s="23" t="s">
+        <v>697</v>
       </c>
       <c r="B31" t="s">
-        <v>325</v>
+        <v>600</v>
       </c>
       <c r="D31" t="s">
         <v>11</v>
@@ -13430,10 +13425,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="18" t="s">
-        <v>524</v>
+        <v>470</v>
       </c>
       <c r="B32" t="s">
-        <v>605</v>
+        <v>471</v>
       </c>
       <c r="D32" t="s">
         <v>11</v>
@@ -13444,10 +13439,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="18" t="s">
-        <v>462</v>
+        <v>468</v>
       </c>
       <c r="B33" t="s">
-        <v>463</v>
+        <v>469</v>
       </c>
       <c r="D33" t="s">
         <v>11</v>
@@ -13458,10 +13453,10 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="18" t="s">
-        <v>464</v>
+        <v>484</v>
       </c>
       <c r="B34" t="s">
-        <v>465</v>
+        <v>485</v>
       </c>
       <c r="D34" t="s">
         <v>11</v>
@@ -13472,10 +13467,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="18" t="s">
-        <v>460</v>
+        <v>411</v>
       </c>
       <c r="B35" t="s">
-        <v>461</v>
+        <v>412</v>
       </c>
       <c r="D35" t="s">
         <v>11</v>
@@ -13486,10 +13481,10 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="18" t="s">
-        <v>606</v>
+        <v>267</v>
       </c>
       <c r="B36" t="s">
-        <v>607</v>
+        <v>325</v>
       </c>
       <c r="D36" t="s">
         <v>11</v>
@@ -13500,10 +13495,10 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="18" t="s">
-        <v>458</v>
+        <v>524</v>
       </c>
       <c r="B37" t="s">
-        <v>459</v>
+        <v>601</v>
       </c>
       <c r="D37" t="s">
         <v>11</v>
@@ -13514,10 +13509,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="18" t="s">
-        <v>534</v>
+        <v>462</v>
       </c>
       <c r="B38" t="s">
-        <v>608</v>
+        <v>463</v>
       </c>
       <c r="D38" t="s">
         <v>11</v>
@@ -13528,10 +13523,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="18" t="s">
-        <v>527</v>
+        <v>464</v>
       </c>
       <c r="B39" t="s">
-        <v>609</v>
+        <v>465</v>
       </c>
       <c r="D39" t="s">
         <v>11</v>
@@ -13542,10 +13537,10 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="18" t="s">
-        <v>482</v>
+        <v>460</v>
       </c>
       <c r="B40" t="s">
-        <v>483</v>
+        <v>461</v>
       </c>
       <c r="D40" t="s">
         <v>11</v>
@@ -13556,10 +13551,10 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="18" t="s">
-        <v>480</v>
+        <v>602</v>
       </c>
       <c r="B41" t="s">
-        <v>642</v>
+        <v>603</v>
       </c>
       <c r="D41" t="s">
         <v>11</v>
@@ -13570,10 +13565,10 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="18" t="s">
-        <v>466</v>
+        <v>458</v>
       </c>
       <c r="B42" t="s">
-        <v>467</v>
+        <v>459</v>
       </c>
       <c r="D42" t="s">
         <v>11</v>
@@ -13584,10 +13579,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="18" t="s">
-        <v>456</v>
+        <v>698</v>
       </c>
       <c r="B43" t="s">
-        <v>457</v>
+        <v>604</v>
       </c>
       <c r="D43" t="s">
         <v>11</v>
@@ -13597,146 +13592,228 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="18" t="s">
-        <v>330</v>
+      <c r="A44" s="23" t="s">
+        <v>699</v>
       </c>
       <c r="B44" t="s">
-        <v>331</v>
+        <v>605</v>
       </c>
       <c r="D44" t="s">
         <v>11</v>
       </c>
       <c r="E44" t="s">
-        <v>252</v>
+        <v>177</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="18" t="s">
-        <v>69</v>
+        <v>482</v>
       </c>
       <c r="B45" t="s">
-        <v>346</v>
+        <v>483</v>
       </c>
       <c r="D45" t="s">
         <v>11</v>
       </c>
       <c r="E45" t="s">
-        <v>19</v>
+        <v>177</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="18" t="s">
-        <v>321</v>
+        <v>480</v>
       </c>
       <c r="B46" t="s">
-        <v>322</v>
+        <v>638</v>
       </c>
       <c r="D46" t="s">
         <v>11</v>
       </c>
       <c r="E46" t="s">
-        <v>259</v>
+        <v>177</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="18" t="s">
-        <v>338</v>
+        <v>466</v>
       </c>
       <c r="B47" t="s">
-        <v>339</v>
+        <v>467</v>
       </c>
       <c r="D47" t="s">
         <v>11</v>
       </c>
       <c r="E47" t="s">
-        <v>261</v>
+        <v>177</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="18" t="s">
-        <v>332</v>
+        <v>456</v>
       </c>
       <c r="B48" t="s">
-        <v>333</v>
+        <v>457</v>
       </c>
       <c r="D48" t="s">
         <v>11</v>
       </c>
       <c r="E48" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="18" t="s">
-        <v>413</v>
+        <v>330</v>
       </c>
       <c r="B49" t="s">
-        <v>414</v>
+        <v>331</v>
       </c>
       <c r="D49" t="s">
         <v>11</v>
       </c>
       <c r="E49" t="s">
-        <v>415</v>
+        <v>252</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="18" t="s">
-        <v>680</v>
+        <v>69</v>
       </c>
       <c r="B50" t="s">
-        <v>610</v>
+        <v>346</v>
       </c>
       <c r="D50" t="s">
         <v>11</v>
       </c>
       <c r="E50" t="s">
-        <v>611</v>
+        <v>19</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="18" t="s">
-        <v>528</v>
+        <v>321</v>
       </c>
       <c r="B51" t="s">
-        <v>529</v>
+        <v>322</v>
       </c>
       <c r="D51" t="s">
         <v>11</v>
       </c>
       <c r="E51" t="s">
-        <v>530</v>
+        <v>259</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="18" t="s">
+        <v>338</v>
+      </c>
+      <c r="B52" t="s">
+        <v>339</v>
+      </c>
+      <c r="D52" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="18" t="s">
+        <v>332</v>
+      </c>
+      <c r="B53" t="s">
+        <v>333</v>
+      </c>
+      <c r="D53" t="s">
+        <v>11</v>
+      </c>
+      <c r="E53" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" s="18" t="s">
+        <v>413</v>
+      </c>
+      <c r="B54" t="s">
+        <v>414</v>
+      </c>
+      <c r="D54" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" s="18" t="s">
+        <v>676</v>
+      </c>
+      <c r="B55" t="s">
+        <v>606</v>
+      </c>
+      <c r="D55" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" s="18" t="s">
+        <v>527</v>
+      </c>
+      <c r="B56" t="s">
+        <v>528</v>
+      </c>
+      <c r="D56" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" s="18" t="s">
+        <v>530</v>
+      </c>
+      <c r="B57" t="s">
         <v>531</v>
       </c>
-      <c r="B52" t="s">
+      <c r="D57" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57" t="s">
         <v>532</v>
       </c>
-      <c r="D52" t="s">
-        <v>11</v>
-      </c>
-      <c r="E52" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" s="18"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" s="18" t="s">
+        <v>700</v>
+      </c>
+      <c r="B58" t="s">
+        <v>701</v>
+      </c>
+      <c r="D58" t="s">
+        <v>11</v>
+      </c>
+      <c r="E58" t="s">
+        <v>702</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A9">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="!">
+      <formula>NOT(ISERROR(SEARCH("!",A9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
-      <formula>"!"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -13886,13 +13963,13 @@
         <v>64</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="V4" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="W4" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="X4" s="13" t="s">
         <v>434</v>
@@ -13909,7 +13986,7 @@
         <v>64</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="X5" s="13" t="s">
         <v>434</v>
@@ -13926,7 +14003,7 @@
         <v>64</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="X6" s="13" t="s">
         <v>434</v>
@@ -13958,7 +14035,7 @@
         <v>64</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="X8" s="13" t="s">
         <v>434</v>
@@ -13975,7 +14052,7 @@
         <v>64</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="X9" s="13" t="s">
         <v>434</v>
@@ -14006,7 +14083,7 @@
         <v>64</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="X11" s="13" t="s">
         <v>434</v>
@@ -14095,7 +14172,7 @@
         <v>64</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="X16" s="13" t="s">
         <v>434</v>
@@ -14112,7 +14189,7 @@
         <v>64</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="X17" s="13"/>
       <c r="Y17" s="13"/>
@@ -14125,7 +14202,7 @@
         <v>64</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="X18" s="13" t="s">
         <v>434</v>
@@ -14142,7 +14219,7 @@
         <v>64</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="X19" s="13"/>
       <c r="Y19" s="13"/>
@@ -14174,7 +14251,7 @@
         <v>64</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="X21" s="13" t="s">
         <v>434</v>
@@ -14191,18 +14268,18 @@
         <v>64</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
     </row>
     <row r="23" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="B23" t="s">
         <v>64</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="X23" s="13" t="s">
         <v>434</v>
@@ -14213,7 +14290,7 @@
     </row>
     <row r="24" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B24" t="s">
         <v>64</v>
@@ -14227,7 +14304,7 @@
     </row>
     <row r="25" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B25" t="s">
         <v>64</v>
@@ -14260,7 +14337,7 @@
     <sortCondition ref="A2:A21"/>
   </sortState>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14437,13 +14514,13 @@
         <v>416</v>
       </c>
       <c r="Y1" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="Z1" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="AA1" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="AB1" t="s">
         <v>433</v>

</xml_diff>

<commit_message>
update changes between version table
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{888F22FF-1514-D54D-A2D3-EA98214427D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45C26DE-D8D2-6046-BB09-9D5C880F2069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52900" yWindow="600" windowWidth="51200" windowHeight="28300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9640" yWindow="1880" windowWidth="51200" windowHeight="28300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -37,6 +37,9 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
Keep QuestionnaireResponse and Update Screening and Assessments page [FHIR-39495]
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45C26DE-D8D2-6046-BB09-9D5C880F2069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3962CE87-7D7D-B849-A51F-A5EBC4FC1FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9640" yWindow="1880" windowWidth="51200" windowHeight="28300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51640" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -121,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2571" uniqueCount="703">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2588" uniqueCount="706">
   <si>
     <t>Element</t>
   </si>
@@ -1935,9 +1935,6 @@
     <t>US Core Ethnicity Extension</t>
   </si>
   <si>
-    <t>!http://hl7.org/fhir/us/core/StructureDefinition/us-core-extension-questionnaire-uri</t>
-  </si>
-  <si>
     <t>US Core Extension Questionnaire URI</t>
   </si>
   <si>
@@ -1954,12 +1951,6 @@
   </si>
   <si>
     <t>QuestionnaireResponse</t>
-  </si>
-  <si>
-    <t>US Core provides two ways to represent SDOH assessment screening results using: 
-1. Observation: [US Core Observation SDOH Assessment Profile] 
-1. QuestionnaireResponse: [US Core QuestionnaireResponse Profile]
-US Core Servers **SHALL** support [US Core Observation SDOH Assessment Profile] for SDOH Assessments and **MAY** support the [US Core QuestionnaireResponse Profile] for SDOH Assessments.</t>
   </si>
   <si>
     <t>conf_QuestionnaireResponse</t>
@@ -2237,12 +2228,6 @@
     <t>http://hl7.org/fhir/smart-app-launch/history.html</t>
   </si>
   <si>
-    <t>!http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</t>
-  </si>
-  <si>
-    <t>!QuestionnaireResponse</t>
-  </si>
-  <si>
     <t>!!Questionnaire</t>
   </si>
   <si>
@@ -2328,6 +2313,30 @@
   </si>
   <si>
     <t>US Core Observation Clinical Result Profile</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/uv/sdc/StructureDefinition/sdc-questionnaire</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-extension-questionnaire-uri</t>
+  </si>
+  <si>
+    <t>Questionnaire</t>
+  </si>
+  <si>
+    <t>conf_Questionnaire</t>
+  </si>
+  <si>
+    <t>SDC Base Questionnaire Profile</t>
+  </si>
+  <si>
+    <t>US Core defines two ways to represent the questions and responses to screening and assessment instruments:
+- Observation: [US Core Observation Screening Assessment Profile]
+- Questionnaire/QuestionnaireResponse: [SDC Base Questionnaire]/[US Core QuestionnaireResponse Profile]
+US Core Servers **SHALL** [US Core Observation Screening Assessment Profile] and **SHOULD** support the  [SDC Base Questionnaire Profile]/[US Core QuestionnaireResponse Profile]</t>
   </si>
 </sst>
 </file>
@@ -2485,7 +2494,7 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2519,6 +2528,8 @@
     <xf numFmtId="49" fontId="13" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -2526,7 +2537,27 @@
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3015,14 +3046,13 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B00118F-F6B9-6642-9BD4-D95AE82A4925}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AB126"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C89" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C96" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G130" sqref="G130"/>
+      <selection pane="bottomRight" activeCell="F104" sqref="F104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3128,7 +3158,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="19" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" ht="19" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3175,7 +3205,7 @@
         <v>SearchParameter-us-core-!example category search-category.html</v>
       </c>
     </row>
-    <row r="3" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3222,7 +3252,7 @@
         <v>SearchParameter-us-core-!example code search-code.html</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3273,7 +3303,7 @@
         <v>SearchParameter-us-core-!example date search-date.html</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3332,7 +3362,7 @@
         <v>SearchParameter-us-core-!example patient search-patient.html</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3379,7 +3409,7 @@
         <v>SearchParameter-us-core-!example status search-status.html</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3430,7 +3460,7 @@
         <v>SearchParameter-us-core-!patient-address.html</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3481,7 +3511,7 @@
         <v>SearchParameter-us-core-!patient-telecom.html</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3530,7 +3560,7 @@
         <v>SearchParameter-us-core-allergyintolerance-clinical-status.html</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3588,7 +3618,7 @@
         <v>SearchParameter-us-core-allergyintolerance-patient.html</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3638,7 +3668,7 @@
         <v>SearchParameter-us-core-condition-category.html</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3686,7 +3716,7 @@
         <v>SearchParameter-us-core-condition-clinical-status.html</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3744,7 +3774,7 @@
         <v>SearchParameter-us-core-condition-patient.html</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3797,7 +3827,7 @@
         <v>SearchParameter-us-core-encounter-id.html</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3847,7 +3877,7 @@
         <v>SearchParameter-us-core-encounter-class.html</v>
       </c>
     </row>
-    <row r="16" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3901,7 +3931,7 @@
         <v>SearchParameter-us-core-encounter-date.html</v>
       </c>
     </row>
-    <row r="17" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3958,7 +3988,7 @@
         <v>SearchParameter-us-core-encounter-identifier.html</v>
       </c>
     </row>
-    <row r="18" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4016,7 +4046,7 @@
         <v>SearchParameter-us-core-encounter-patient.html</v>
       </c>
     </row>
-    <row r="19" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4074,7 +4104,7 @@
         <v>SearchParameter-us-core-encounter-location.html</v>
       </c>
     </row>
-    <row r="20" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4124,7 +4154,7 @@
         <v>SearchParameter-us-core-encounter-status.html</v>
       </c>
     </row>
-    <row r="21" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4174,7 +4204,7 @@
         <v>SearchParameter-us-core-encounter-type.html</v>
       </c>
     </row>
-    <row r="22" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4224,7 +4254,7 @@
         <v>SearchParameter-us-core-encounter-discharge-disposition.html</v>
       </c>
     </row>
-    <row r="23" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -4277,7 +4307,7 @@
         <v>SearchParameter-us-core-patient-id.html</v>
       </c>
     </row>
-    <row r="24" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4324,7 +4354,7 @@
         <v>SearchParameter-us-core-patient-birthdate.html</v>
       </c>
     </row>
-    <row r="25" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -4332,7 +4362,7 @@
         <v>19</v>
       </c>
       <c r="C25" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="D25" t="s">
         <v>28</v>
@@ -4374,7 +4404,7 @@
         <v>SearchParameter-us-core-patient-death-date.html</v>
       </c>
     </row>
-    <row r="26" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -4420,7 +4450,7 @@
         <v>SearchParameter-us-core-patient-family.html</v>
       </c>
     </row>
-    <row r="27" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -4468,7 +4498,7 @@
         <v>SearchParameter-us-core-patient-gender.html</v>
       </c>
     </row>
-    <row r="28" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4512,7 +4542,7 @@
         <v>SearchParameter-us-core-patient-given.html</v>
       </c>
     </row>
-    <row r="29" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -4569,7 +4599,7 @@
         <v>SearchParameter-us-core-patient-identifier.html</v>
       </c>
     </row>
-    <row r="30" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -4609,7 +4639,7 @@
         <v>51</v>
       </c>
       <c r="Y30" s="4" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="Z30" t="s">
         <v>167</v>
@@ -4623,7 +4653,7 @@
         <v>SearchParameter-us-core-patient-name.html</v>
       </c>
     </row>
-    <row r="31" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4631,7 +4661,7 @@
         <v>79</v>
       </c>
       <c r="C31" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="D31" t="s">
         <v>28</v>
@@ -4656,19 +4686,19 @@
         <v>52</v>
       </c>
       <c r="L31" t="s">
+        <v>638</v>
+      </c>
+      <c r="M31" t="s">
+        <v>51</v>
+      </c>
+      <c r="O31" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y31" s="4" t="s">
+        <v>639</v>
+      </c>
+      <c r="Z31" t="s">
         <v>640</v>
-      </c>
-      <c r="M31" t="s">
-        <v>51</v>
-      </c>
-      <c r="O31" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y31" s="4" t="s">
-        <v>641</v>
-      </c>
-      <c r="Z31" t="s">
-        <v>642</v>
       </c>
       <c r="AA31" s="8" t="str">
         <f>"Fetches a bundle of all "&amp;B31&amp;" resources matching the name"</f>
@@ -4679,12 +4709,12 @@
         <v>SearchParameter-us-core-!patient-tribal-affiliation.html</v>
       </c>
     </row>
-    <row r="32" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="C32" t="s">
         <v>50</v>
@@ -4709,7 +4739,7 @@
         <v>52</v>
       </c>
       <c r="L32" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="M32" t="s">
         <v>51</v>
@@ -4722,12 +4752,12 @@
         <v>SearchParameter-us-core-!!questionnaire-_id.html</v>
       </c>
     </row>
-    <row r="33" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="C33" t="s">
         <v>65</v>
@@ -4766,12 +4796,12 @@
         <v>SearchParameter-us-core-!!questionnaire-context-type-value.html</v>
       </c>
     </row>
-    <row r="34" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="C34" t="s">
         <v>62</v>
@@ -4813,12 +4843,12 @@
         <v>SearchParameter-us-core-!!questionnaire-publisher.html</v>
       </c>
     </row>
-    <row r="35" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="C35" t="s">
         <v>56</v>
@@ -4857,12 +4887,12 @@
         <v>SearchParameter-us-core-!!questionnaire-status.html</v>
       </c>
     </row>
-    <row r="36" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="C36" t="s">
         <v>57</v>
@@ -4913,12 +4943,12 @@
         <v>SearchParameter-us-core-!!questionnaire-title.html</v>
       </c>
     </row>
-    <row r="37" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="C37" t="s">
         <v>54</v>
@@ -4957,12 +4987,12 @@
         <v>SearchParameter-us-core-!!questionnaire-url.html</v>
       </c>
     </row>
-    <row r="38" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="C38" t="s">
         <v>61</v>
@@ -5001,7 +5031,7 @@
         <v>SearchParameter-us-core-!!questionnaire-version.html</v>
       </c>
     </row>
-    <row r="39" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -5055,7 +5085,7 @@
         <v>SearchParameter-us-core-condition-onset-date.html</v>
       </c>
     </row>
-    <row r="40" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -5109,7 +5139,7 @@
         <v>SearchParameter-us-core-condition-asserted-date.html</v>
       </c>
     </row>
-    <row r="41" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -5163,7 +5193,7 @@
         <v>SearchParameter-us-core-condition-recorded-date.html</v>
       </c>
     </row>
-    <row r="42" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -5217,7 +5247,7 @@
         <v>SearchParameter-us-core-condition-abatement-date.html</v>
       </c>
     </row>
-    <row r="43" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -5267,7 +5297,7 @@
         <v>SearchParameter-us-core-condition-code.html</v>
       </c>
     </row>
-    <row r="44" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -5325,7 +5355,7 @@
         <v>SearchParameter-us-core-condition-encounter.html</v>
       </c>
     </row>
-    <row r="45" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -5384,7 +5414,7 @@
         <v>SearchParameter-us-core-immunization-patient.html</v>
       </c>
     </row>
-    <row r="46" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -5434,7 +5464,7 @@
         <v>SearchParameter-us-core-immunization-status.html</v>
       </c>
     </row>
-    <row r="47" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -5488,7 +5518,7 @@
         <v>SearchParameter-us-core-immunization-date.html</v>
       </c>
     </row>
-    <row r="48" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -5541,7 +5571,7 @@
         <v>SearchParameter-us-core-documentreference-_id.html</v>
       </c>
     </row>
-    <row r="49" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -5594,7 +5624,7 @@
         <v>SearchParameter-us-core-documentreference-status.html</v>
       </c>
     </row>
-    <row r="50" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -5653,7 +5683,7 @@
         <v>SearchParameter-us-core-documentreference-patient.html</v>
       </c>
     </row>
-    <row r="51" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -5703,7 +5733,7 @@
         <v>SearchParameter-us-core-documentreference-category.html</v>
       </c>
     </row>
-    <row r="52" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -5753,7 +5783,7 @@
         <v>SearchParameter-us-core-documentreference-type.html</v>
       </c>
     </row>
-    <row r="53" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -5807,7 +5837,7 @@
         <v>SearchParameter-us-core-documentreference-date.html</v>
       </c>
     </row>
-    <row r="54" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -5860,7 +5890,7 @@
         <v>SearchParameter-us-core-documentreference-period.html</v>
       </c>
     </row>
-    <row r="55" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -5913,7 +5943,7 @@
         <v>SearchParameter-us-core-diagnosticreport-status.html</v>
       </c>
     </row>
-    <row r="56" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -5972,7 +6002,7 @@
         <v>SearchParameter-us-core-diagnosticreport-patient.html</v>
       </c>
     </row>
-    <row r="57" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -6022,7 +6052,7 @@
         <v>SearchParameter-us-core-diagnosticreport-category.html</v>
       </c>
     </row>
-    <row r="58" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -6075,7 +6105,7 @@
         <v>SearchParameter-us-core-diagnosticreport-code.html</v>
       </c>
     </row>
-    <row r="59" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -6129,7 +6159,7 @@
         <v>SearchParameter-us-core-diagnosticreport-date.html</v>
       </c>
     </row>
-    <row r="60" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -6179,7 +6209,7 @@
         <v>SearchParameter-us-core-goal-lifecycle-status.html</v>
       </c>
     </row>
-    <row r="61" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -6238,7 +6268,7 @@
         <v>SearchParameter-us-core-goal-patient.html</v>
       </c>
     </row>
-    <row r="62" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -6292,7 +6322,7 @@
         <v>SearchParameter-us-core-goal-target-date.html</v>
       </c>
     </row>
-    <row r="63" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -6345,7 +6375,7 @@
         <v>SearchParameter-us-core-medicationrequest-status.html</v>
       </c>
     </row>
-    <row r="64" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -6398,7 +6428,7 @@
         <v>SearchParameter-us-core-medicationrequest-intent.html</v>
       </c>
     </row>
-    <row r="65" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -6451,7 +6481,7 @@
         <v>SearchParameter-us-core-medicationrequest-patient.html</v>
       </c>
     </row>
-    <row r="66" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -6502,7 +6532,7 @@
         <v>SearchParameter-us-core-medicationrequest-encounter.html</v>
       </c>
     </row>
-    <row r="67" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -6556,7 +6586,7 @@
         <v>SearchParameter-us-core-medicationrequest-authoredon.html</v>
       </c>
     </row>
-    <row r="68" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -6609,7 +6639,7 @@
         <v>SearchParameter-us-core-!medicationstatement-status.html</v>
       </c>
     </row>
-    <row r="69" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -6667,7 +6697,7 @@
         <v>SearchParameter-us-core-!medicationstatement-patient.html</v>
       </c>
     </row>
-    <row r="70" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -6721,7 +6751,7 @@
         <v>SearchParameter-us-core-!medicationstatement-effective.html</v>
       </c>
     </row>
-    <row r="71" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -6774,7 +6804,7 @@
         <v>SearchParameter-us-core-procedure-status.html</v>
       </c>
     </row>
-    <row r="72" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -6832,7 +6862,7 @@
         <v>SearchParameter-us-core-procedure-patient.html</v>
       </c>
     </row>
-    <row r="73" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -6886,7 +6916,7 @@
         <v>SearchParameter-us-core-procedure-date.html</v>
       </c>
     </row>
-    <row r="74" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -6939,7 +6969,7 @@
         <v>SearchParameter-us-core-procedure-code.html</v>
       </c>
     </row>
-    <row r="75" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -6992,7 +7022,7 @@
         <v>SearchParameter-us-core-observation-status.html</v>
       </c>
     </row>
-    <row r="76" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -7042,7 +7072,7 @@
         <v>SearchParameter-us-core-observation-category.html</v>
       </c>
     </row>
-    <row r="77" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -7095,7 +7125,7 @@
         <v>SearchParameter-us-core-observation-code.html</v>
       </c>
     </row>
-    <row r="78" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
@@ -7149,7 +7179,7 @@
         <v>SearchParameter-us-core-observation-date.html</v>
       </c>
     </row>
-    <row r="79" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>
@@ -7208,7 +7238,7 @@
         <v>SearchParameter-us-core-observation-patient.html</v>
       </c>
     </row>
-    <row r="80" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>79</v>
       </c>
@@ -7258,7 +7288,7 @@
         <v>SearchParameter-us-core-careplan-category.html</v>
       </c>
     </row>
-    <row r="81" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>80</v>
       </c>
@@ -7308,7 +7338,7 @@
         <v>SearchParameter-us-core-!careplan-code.html</v>
       </c>
     </row>
-    <row r="82" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>81</v>
       </c>
@@ -7362,7 +7392,7 @@
         <v>SearchParameter-us-core-careplan-date.html</v>
       </c>
     </row>
-    <row r="83" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>82</v>
       </c>
@@ -7421,7 +7451,7 @@
         <v>SearchParameter-us-core-careplan-patient.html</v>
       </c>
     </row>
-    <row r="84" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>83</v>
       </c>
@@ -7474,7 +7504,7 @@
         <v>SearchParameter-us-core-careplan-status.html</v>
       </c>
     </row>
-    <row r="85" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>84</v>
       </c>
@@ -7536,7 +7566,7 @@
         <v>SearchParameter-us-core-careteam-patient.html</v>
       </c>
     </row>
-    <row r="86" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>85</v>
       </c>
@@ -7589,7 +7619,7 @@
         <v>SearchParameter-us-core-practitioner-id.html</v>
       </c>
     </row>
-    <row r="87" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>86</v>
       </c>
@@ -7642,7 +7672,7 @@
         <v>SearchParameter-us-core-careteam-status.html</v>
       </c>
     </row>
-    <row r="88" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>87</v>
       </c>
@@ -7700,7 +7730,7 @@
         <v>SearchParameter-us-core-careteam-role.html</v>
       </c>
     </row>
-    <row r="89" spans="1:28" ht="19" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>88</v>
       </c>
@@ -7863,7 +7893,7 @@
         <v>SearchParameter-us-core-device-status.html</v>
       </c>
     </row>
-    <row r="92" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>91</v>
       </c>
@@ -7918,7 +7948,7 @@
         <v>SearchParameter-us-core-location-name.html</v>
       </c>
     </row>
-    <row r="93" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>92</v>
       </c>
@@ -7973,7 +8003,7 @@
         <v>SearchParameter-us-core-location-address.html</v>
       </c>
     </row>
-    <row r="94" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>93</v>
       </c>
@@ -8028,7 +8058,7 @@
         <v>SearchParameter-us-core-location-address-city.html</v>
       </c>
     </row>
-    <row r="95" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>94</v>
       </c>
@@ -8082,7 +8112,7 @@
         <v>SearchParameter-us-core-location-address-state.html</v>
       </c>
     </row>
-    <row r="96" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>95</v>
       </c>
@@ -8137,7 +8167,7 @@
         <v>SearchParameter-us-core-location-address-postalcode.html</v>
       </c>
     </row>
-    <row r="97" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>96</v>
       </c>
@@ -8192,7 +8222,7 @@
         <v>SearchParameter-us-core-organization-name.html</v>
       </c>
     </row>
-    <row r="98" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>97</v>
       </c>
@@ -8247,7 +8277,7 @@
         <v>SearchParameter-us-core-organization-address.html</v>
       </c>
     </row>
-    <row r="99" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>98</v>
       </c>
@@ -8302,7 +8332,7 @@
         <v>SearchParameter-us-core-!organization-address-city.html</v>
       </c>
     </row>
-    <row r="100" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>99</v>
       </c>
@@ -8357,7 +8387,7 @@
         <v>SearchParameter-us-core-!organization-adress-state.html</v>
       </c>
     </row>
-    <row r="101" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>100</v>
       </c>
@@ -8412,7 +8442,7 @@
         <v>SearchParameter-us-core-!organization-address-postalcode.html</v>
       </c>
     </row>
-    <row r="102" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>101</v>
       </c>
@@ -8467,7 +8497,7 @@
         <v>SearchParameter-us-core-practitioner-name.html</v>
       </c>
     </row>
-    <row r="103" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>102</v>
       </c>
@@ -8525,7 +8555,7 @@
         <v>SearchParameter-us-core-practitioner-identifier.html</v>
       </c>
     </row>
-    <row r="104" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>103</v>
       </c>
@@ -8586,7 +8616,7 @@
         <v>SearchParameter-us-core-practitionerrole-specialty.html</v>
       </c>
     </row>
-    <row r="105" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>104</v>
       </c>
@@ -8650,7 +8680,7 @@
         <v>SearchParameter-us-core-practitionerrole-practitioner.html</v>
       </c>
     </row>
-    <row r="106" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>105</v>
       </c>
@@ -8703,7 +8733,7 @@
         <v>SearchParameter-us-core-servicerequest-status.html</v>
       </c>
     </row>
-    <row r="107" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>106</v>
       </c>
@@ -8762,7 +8792,7 @@
         <v>SearchParameter-us-core-servicerequest-patient.html</v>
       </c>
     </row>
-    <row r="108" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>107</v>
       </c>
@@ -8812,7 +8842,7 @@
         <v>SearchParameter-us-core-servicerequest-category.html</v>
       </c>
     </row>
-    <row r="109" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>108</v>
       </c>
@@ -8865,7 +8895,7 @@
         <v>SearchParameter-us-core-servicerequest-code.html</v>
       </c>
     </row>
-    <row r="110" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>109</v>
       </c>
@@ -8919,7 +8949,7 @@
         <v>SearchParameter-us-core-servicerequest-authored.html</v>
       </c>
     </row>
-    <row r="111" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>110</v>
       </c>
@@ -8969,7 +8999,7 @@
         <v>SearchParameter-us-core-servicerequest-id.html</v>
       </c>
     </row>
-    <row r="112" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>111</v>
       </c>
@@ -9015,7 +9045,7 @@
         <v>SearchParameter-us-core-goal-description.html</v>
       </c>
     </row>
-    <row r="113" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>112</v>
       </c>
@@ -9066,7 +9096,7 @@
         <v>SearchParameter-us-core-relatedperson-id.html</v>
       </c>
     </row>
-    <row r="114" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>113</v>
       </c>
@@ -9125,7 +9155,7 @@
         <v>SearchParameter-us-core-relatedperson-patient.html</v>
       </c>
     </row>
-    <row r="115" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>114</v>
       </c>
@@ -9168,7 +9198,7 @@
         <v>51</v>
       </c>
       <c r="Y115" s="4" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="Z115" s="4" t="str">
         <f>"GET [base]/"&amp;B115&amp;"?"&amp;C115&amp;"=Mary Shaw"</f>
@@ -9183,12 +9213,12 @@
         <v>SearchParameter-us-core-relatedperson-name.html</v>
       </c>
     </row>
-    <row r="116" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>673</v>
+        <v>602</v>
       </c>
       <c r="C116" t="s">
         <v>50</v>
@@ -9201,7 +9231,7 @@
       </c>
       <c r="G116" t="str">
         <f t="shared" si="7"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="H116" t="s">
         <v>51</v>
@@ -9214,7 +9244,7 @@
       </c>
       <c r="L116" t="str">
         <f t="shared" si="6"/>
-        <v>!QuestionnaireResponse._id</v>
+        <v>QuestionnaireResponse._id</v>
       </c>
       <c r="M116" t="s">
         <v>51</v>
@@ -9224,22 +9254,22 @@
       </c>
       <c r="Y116" s="4" t="str">
         <f>"support fetching a "&amp;B116</f>
-        <v>support fetching a !QuestionnaireResponse</v>
+        <v>support fetching a QuestionnaireResponse</v>
       </c>
       <c r="Z116" s="4" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="AB116" t="str">
         <f t="shared" si="9"/>
-        <v>SearchParameter-us-core-!questionnaireresponse-id.html</v>
-      </c>
-    </row>
-    <row r="117" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>SearchParameter-us-core-questionnaireresponse-id.html</v>
+      </c>
+    </row>
+    <row r="117" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>673</v>
+        <v>602</v>
       </c>
       <c r="C117" t="s">
         <v>84</v>
@@ -9255,7 +9285,7 @@
       </c>
       <c r="G117" t="str">
         <f t="shared" si="7"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="H117" t="s">
         <v>51</v>
@@ -9268,7 +9298,7 @@
       </c>
       <c r="L117" t="str">
         <f t="shared" si="6"/>
-        <v>!QuestionnaireResponse.patient</v>
+        <v>QuestionnaireResponse.patient</v>
       </c>
       <c r="M117" t="s">
         <v>51</v>
@@ -9278,27 +9308,27 @@
       </c>
       <c r="Y117" t="str">
         <f>"support searching for all "&amp;LOWER(B117)&amp;"s for a patient"</f>
-        <v>support searching for all !questionnaireresponses for a patient</v>
+        <v>support searching for all questionnaireresponses for a patient</v>
       </c>
       <c r="Z117" s="4" t="str">
         <f>"GET [base]/"&amp;B117&amp;"?patient=1032702"</f>
-        <v>GET [base]/!QuestionnaireResponse?patient=1032702</v>
+        <v>GET [base]/QuestionnaireResponse?patient=1032702</v>
       </c>
       <c r="AA117" s="8" t="str">
         <f>"Fetches a bundle of all "&amp;B117&amp; " resources for the specified patient"</f>
-        <v>Fetches a bundle of all !QuestionnaireResponse resources for the specified patient</v>
+        <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient</v>
       </c>
       <c r="AB117" t="str">
         <f t="shared" si="9"/>
-        <v>SearchParameter-us-core-!questionnaireresponse-patient.html</v>
-      </c>
-    </row>
-    <row r="118" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>SearchParameter-us-core-questionnaireresponse-patient.html</v>
+      </c>
+    </row>
+    <row r="118" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>673</v>
+        <v>602</v>
       </c>
       <c r="C118" t="s">
         <v>56</v>
@@ -9314,7 +9344,7 @@
       </c>
       <c r="G118" t="str">
         <f t="shared" si="7"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="H118" t="s">
         <v>51</v>
@@ -9327,7 +9357,7 @@
       </c>
       <c r="L118" t="str">
         <f t="shared" si="6"/>
-        <v>!QuestionnaireResponse.status</v>
+        <v>QuestionnaireResponse.status</v>
       </c>
       <c r="M118" t="s">
         <v>51</v>
@@ -9339,22 +9369,22 @@
         <v>51</v>
       </c>
       <c r="Y118" s="19" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="AB118" t="str">
         <f t="shared" si="9"/>
-        <v>SearchParameter-us-core-!questionnaireresponse-status.html</v>
-      </c>
-    </row>
-    <row r="119" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>SearchParameter-us-core-questionnaireresponse-status.html</v>
+      </c>
+    </row>
+    <row r="119" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>673</v>
+        <v>602</v>
       </c>
       <c r="C119" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="D119" t="s">
         <v>28</v>
@@ -9367,7 +9397,7 @@
       </c>
       <c r="G119" t="str">
         <f t="shared" si="7"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="H119" t="s">
         <v>51</v>
@@ -9379,7 +9409,7 @@
         <v>52</v>
       </c>
       <c r="L119" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="M119" t="s">
         <v>51</v>
@@ -9388,19 +9418,19 @@
         <v>51</v>
       </c>
       <c r="Y119" s="19" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="AB119" t="str">
         <f t="shared" si="9"/>
-        <v>SearchParameter-us-core-!questionnaireresponse-tag.html</v>
-      </c>
-    </row>
-    <row r="120" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>SearchParameter-us-core-questionnaireresponse-tag.html</v>
+      </c>
+    </row>
+    <row r="120" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>673</v>
+        <v>602</v>
       </c>
       <c r="C120" t="s">
         <v>547</v>
@@ -9416,7 +9446,7 @@
       </c>
       <c r="G120" t="str">
         <f t="shared" si="7"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="H120" t="s">
         <v>51</v>
@@ -9429,7 +9459,7 @@
       </c>
       <c r="L120" t="str">
         <f t="shared" ref="L120:L126" si="10">B120&amp;"."&amp;C120</f>
-        <v>!QuestionnaireResponse.authored</v>
+        <v>QuestionnaireResponse.authored</v>
       </c>
       <c r="M120" t="s">
         <v>51</v>
@@ -9444,22 +9474,22 @@
         <v>87</v>
       </c>
       <c r="Y120" s="19" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="AB120" t="str">
         <f t="shared" si="9"/>
-        <v>SearchParameter-us-core-!questionnaireresponse-authored.html</v>
-      </c>
-    </row>
-    <row r="121" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>SearchParameter-us-core-questionnaireresponse-authored.html</v>
+      </c>
+    </row>
+    <row r="121" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>673</v>
+        <v>602</v>
       </c>
       <c r="C121" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="D121" t="s">
         <v>28</v>
@@ -9472,7 +9502,7 @@
       </c>
       <c r="G121" t="str">
         <f t="shared" si="7"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="H121" t="s">
         <v>51</v>
@@ -9485,7 +9515,7 @@
       </c>
       <c r="L121" t="str">
         <f t="shared" si="10"/>
-        <v>!QuestionnaireResponse.questionnaire</v>
+        <v>QuestionnaireResponse.questionnaire</v>
       </c>
       <c r="M121" t="s">
         <v>51</v>
@@ -9494,19 +9524,19 @@
         <v>51</v>
       </c>
       <c r="Y121" s="19" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="AB121" t="str">
         <f t="shared" si="9"/>
-        <v>SearchParameter-us-core-!questionnaireresponse-questionnaire.html</v>
-      </c>
-    </row>
-    <row r="122" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>SearchParameter-us-core-questionnaireresponse-questionnaire.html</v>
+      </c>
+    </row>
+    <row r="122" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="C122" t="s">
         <v>84</v>
@@ -9547,7 +9577,7 @@
         <v>51</v>
       </c>
       <c r="Y122" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="Z122" s="4" t="str">
         <f>"GET [base]/"&amp;B122&amp;"?patient=1137192"</f>
@@ -9562,12 +9592,12 @@
         <v>SearchParameter-us-core-coverage-patient.html</v>
       </c>
     </row>
-    <row r="123" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="C123" t="s">
         <v>56</v>
@@ -9618,12 +9648,12 @@
         <v>SearchParameter-us-core-medicationdispense-status.html</v>
       </c>
     </row>
-    <row r="124" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="C124" t="s">
         <v>12</v>
@@ -9674,12 +9704,12 @@
         <v>SearchParameter-us-core-medicationdispense-type.html</v>
       </c>
     </row>
-    <row r="125" spans="1:28" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:28" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="C125" t="s">
         <v>84</v>
@@ -9720,10 +9750,10 @@
         <v>51</v>
       </c>
       <c r="X125" s="6" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="Z125" s="8" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="AA125" s="8" t="str">
         <f>"Fetches a bundle of all "&amp;B125&amp; " resources for the specified patient."</f>
@@ -9734,15 +9764,15 @@
         <v>SearchParameter-us-core-medicationdispense-patient.html</v>
       </c>
     </row>
-    <row r="126" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>125</v>
       </c>
       <c r="B126" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="C126" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="D126" t="s">
         <v>28</v>
@@ -9792,15 +9822,9 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AB126" xr:uid="{1CF5B17E-E72E-48B2-A597-9C21C12723F0}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Device"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:AB126" xr:uid="{1CF5B17E-E72E-48B2-A597-9C21C12723F0}"/>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9814,8 +9838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E7AC33C-2643-EE4B-9487-6CC99572F031}">
   <dimension ref="A1:K96"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+    <sheetView topLeftCell="A64" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C94" sqref="C94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10686,7 +10710,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D32" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="F32" t="s">
         <v>64</v>
@@ -10695,10 +10719,10 @@
         <v>128</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="K32" s="4" t="str">
         <f t="shared" si="1"/>
@@ -10828,7 +10852,7 @@
         <v>312</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
@@ -10888,7 +10912,7 @@
         <v>144</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K38" s="4" t="s">
         <v>557</v>
@@ -11144,7 +11168,7 @@
         <v>173</v>
       </c>
       <c r="C47" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="D47" t="s">
         <v>110</v>
@@ -11174,7 +11198,7 @@
         <v>173</v>
       </c>
       <c r="C48" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="D48" t="s">
         <v>139</v>
@@ -11207,7 +11231,7 @@
         <v>173</v>
       </c>
       <c r="C49" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="D49" t="s">
         <v>141</v>
@@ -11237,7 +11261,7 @@
         <v>173</v>
       </c>
       <c r="C50" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="D50" t="s">
         <v>188</v>
@@ -11270,7 +11294,7 @@
         <v>173</v>
       </c>
       <c r="C51" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="D51" t="s">
         <v>212</v>
@@ -11648,7 +11672,7 @@
         <v>177</v>
       </c>
       <c r="C63" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="D63" t="s">
         <v>229</v>
@@ -11680,7 +11704,7 @@
         <v>177</v>
       </c>
       <c r="C64" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="D64" t="s">
         <v>139</v>
@@ -11713,7 +11737,7 @@
         <v>177</v>
       </c>
       <c r="C65" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="D65" t="s">
         <v>141</v>
@@ -11743,7 +11767,7 @@
         <v>177</v>
       </c>
       <c r="C66" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="D66" t="s">
         <v>188</v>
@@ -11776,7 +11800,7 @@
         <v>177</v>
       </c>
       <c r="C67" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="D67" t="s">
         <v>212</v>
@@ -11806,7 +11830,7 @@
         <v>304</v>
       </c>
       <c r="C68" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="D68" t="s">
         <v>110</v>
@@ -12185,7 +12209,7 @@
         <v>241</v>
       </c>
       <c r="C80" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="D80" t="s">
         <v>112</v>
@@ -12214,7 +12238,7 @@
         <v>241</v>
       </c>
       <c r="C81" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="D81" t="s">
         <v>110</v>
@@ -12229,13 +12253,13 @@
         <v>100</v>
       </c>
       <c r="I81" s="4" t="s">
+        <v>653</v>
+      </c>
+      <c r="J81" s="4" t="s">
+        <v>654</v>
+      </c>
+      <c r="K81" s="4" t="s">
         <v>655</v>
-      </c>
-      <c r="J81" s="4" t="s">
-        <v>656</v>
-      </c>
-      <c r="K81" s="4" t="s">
-        <v>657</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
@@ -12459,11 +12483,11 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>673</v>
+        <v>602</v>
       </c>
       <c r="C89" t="str">
         <f t="shared" si="4"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D89" t="s">
         <v>110</v>
@@ -12475,14 +12499,14 @@
         <v>100</v>
       </c>
       <c r="I89" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="J89" s="4" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="K89" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B89&amp;" resources for the specified "&amp;SUBSTITUTE(D89,","," and ")</f>
-        <v>Fetches a bundle of all !QuestionnaireResponse resources for the specified patient and status</v>
+        <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient and status</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.2">
@@ -12490,14 +12514,14 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>673</v>
+        <v>602</v>
       </c>
       <c r="C90" t="str">
         <f t="shared" si="4"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D90" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="F90" t="s">
         <v>64</v>
@@ -12506,17 +12530,17 @@
         <v>100</v>
       </c>
       <c r="H90" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="I90" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="J90" s="4" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="K90" t="str">
         <f>"Fetches a bundle of all "&amp;B90&amp;" resources for the specified "&amp;SUBSTITUTE(D90,","," and  ") &amp; "= 'sdoh'"</f>
-        <v>Fetches a bundle of all !QuestionnaireResponse resources for the specified patient and  _tag= 'sdoh'</v>
+        <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient and  _tag= 'sdoh'</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.2">
@@ -12524,14 +12548,14 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>673</v>
+        <v>602</v>
       </c>
       <c r="C91" t="str">
         <f t="shared" si="4"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D91" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="F91" t="s">
         <v>64</v>
@@ -12540,14 +12564,14 @@
         <v>143</v>
       </c>
       <c r="I91" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="J91" s="4" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="K91" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B91&amp;" resources for the specified patient and date"</f>
-        <v>Fetches a bundle of all !QuestionnaireResponse resources for the specified patient and date</v>
+        <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient and date</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.2">
@@ -12555,14 +12579,14 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>673</v>
+        <v>602</v>
       </c>
       <c r="C92" t="str">
         <f t="shared" si="4"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D92" s="16" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="F92" t="s">
         <v>64</v>
@@ -12571,17 +12595,17 @@
         <v>211</v>
       </c>
       <c r="H92" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="I92" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="J92" s="4" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="K92" t="str">
         <f>"Fetches a bundle of all "&amp;B92&amp;" resources tagged as 'sdoh' for the specified patient and date"</f>
-        <v>Fetches a bundle of all !QuestionnaireResponse resources tagged as 'sdoh' for the specified patient and date</v>
+        <v>Fetches a bundle of all QuestionnaireResponse resources tagged as 'sdoh' for the specified patient and date</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.2">
@@ -12589,14 +12613,14 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>673</v>
+        <v>602</v>
       </c>
       <c r="C93" t="str">
         <f t="shared" si="4"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D93" s="16" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="F93" t="s">
         <v>64</v>
@@ -12605,14 +12629,14 @@
         <v>85</v>
       </c>
       <c r="I93" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="J93" s="4" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="K93" t="str">
         <f>"Fetches a bundle of all "&amp;B93&amp;" resources for the specified patient that have been completed against a specified form."</f>
-        <v>Fetches a bundle of all !QuestionnaireResponse resources for the specified patient that have been completed against a specified form.</v>
+        <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient that have been completed against a specified form.</v>
       </c>
     </row>
     <row r="94" spans="1:11" ht="151" customHeight="1" x14ac:dyDescent="0.2">
@@ -12620,10 +12644,10 @@
         <v>93</v>
       </c>
       <c r="B94" s="16" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="C94" t="str">
-        <f t="shared" si="4"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B94)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</v>
       </c>
       <c r="D94" s="16" t="s">
@@ -12640,10 +12664,10 @@
       </c>
       <c r="H94" s="16"/>
       <c r="I94" s="4" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="J94" s="4" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="K94" t="str">
         <f>"Fetches a bundle of all "&amp;B94&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed))."</f>
@@ -12655,7 +12679,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="16" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="C95" t="str">
         <f t="shared" si="4"/>
@@ -12675,10 +12699,10 @@
       </c>
       <c r="H95" s="16"/>
       <c r="I95" s="4" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="J95" s="4" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="K95" t="str">
         <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed) and type of dispense (e.g., partially dispensed)."</f>
@@ -12690,14 +12714,14 @@
         <v>95</v>
       </c>
       <c r="B96" s="16" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="C96" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationdispense</v>
       </c>
       <c r="D96" s="16" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="E96" s="16" t="s">
         <v>51</v>
@@ -12710,10 +12734,10 @@
       </c>
       <c r="H96" s="16"/>
       <c r="I96" s="4" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="J96" s="4" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="K96" t="str">
         <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient for a given dispense and date or range"</f>
@@ -12723,7 +12747,7 @@
   </sheetData>
   <autoFilter ref="A1:K96" xr:uid="{331E0B16-168F-459B-8951-3DF614BF0371}"/>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12800,7 +12824,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -12808,7 +12832,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -12884,7 +12908,7 @@
         <v>526</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="D2" t="s">
         <v>64</v>
@@ -12892,7 +12916,7 @@
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>521</v>
@@ -12973,10 +12997,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AF3E0BA-3FCD-D647-BD07-B7C9B2EC4519}">
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView topLeftCell="A11" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13049,10 +13073,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B5" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
@@ -13063,10 +13087,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B6" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -13077,16 +13101,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="B7" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -13147,7 +13171,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="B12" t="s">
         <v>347</v>
@@ -13229,12 +13253,12 @@
         <v>588</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="20" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="24" t="s">
+        <v>701</v>
+      </c>
+      <c r="B18" t="s">
         <v>597</v>
-      </c>
-      <c r="B18" t="s">
-        <v>598</v>
       </c>
       <c r="D18" t="s">
         <v>11</v>
@@ -13315,16 +13339,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="B24" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="D24" t="s">
         <v>11</v>
       </c>
       <c r="E24" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -13343,10 +13367,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="B26" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="D26" t="s">
         <v>11</v>
@@ -13357,10 +13381,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="B27" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
@@ -13371,10 +13395,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="B28" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="D28" t="s">
         <v>11</v>
@@ -13385,10 +13409,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="18" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
       <c r="B29" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="D29" t="s">
         <v>11</v>
@@ -13413,10 +13437,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
       <c r="B31" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="D31" t="s">
         <v>11</v>
@@ -13500,7 +13524,7 @@
         <v>524</v>
       </c>
       <c r="B37" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D37" t="s">
         <v>11</v>
@@ -13553,10 +13577,10 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="B41" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="D41" t="s">
         <v>11</v>
@@ -13581,10 +13605,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="18" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="B43" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="D43" t="s">
         <v>11</v>
@@ -13595,10 +13619,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
       <c r="B44" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
       <c r="D44" t="s">
         <v>11</v>
@@ -13626,7 +13650,7 @@
         <v>480</v>
       </c>
       <c r="B46" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="D46" t="s">
         <v>11</v>
@@ -13748,86 +13772,108 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" s="18" t="s">
-        <v>672</v>
+      <c r="A55" s="23" t="s">
+        <v>699</v>
       </c>
       <c r="B55" t="s">
+        <v>704</v>
+      </c>
+      <c r="D55" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" s="23" t="s">
+        <v>700</v>
+      </c>
+      <c r="B56" t="s">
+        <v>601</v>
+      </c>
+      <c r="D56" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" t="s">
         <v>602</v>
-      </c>
-      <c r="D55" t="s">
-        <v>11</v>
-      </c>
-      <c r="E55" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" s="18" t="s">
-        <v>527</v>
-      </c>
-      <c r="B56" t="s">
-        <v>528</v>
-      </c>
-      <c r="D56" t="s">
-        <v>11</v>
-      </c>
-      <c r="E56" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="18" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="B57" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="D57" t="s">
         <v>11</v>
       </c>
       <c r="E57" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="18" t="s">
-        <v>696</v>
+        <v>530</v>
       </c>
       <c r="B58" t="s">
-        <v>697</v>
+        <v>531</v>
       </c>
       <c r="D58" t="s">
         <v>11</v>
       </c>
       <c r="E58" t="s">
-        <v>698</v>
+        <v>532</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" s="18" t="s">
+        <v>692</v>
+      </c>
+      <c r="B59" t="s">
+        <v>693</v>
+      </c>
+      <c r="D59" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59" t="s">
+        <v>694</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A9">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",A9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A55">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="!">
+      <formula>NOT(ISERROR(SEARCH("!",A55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="A18" r:id="rId1" xr:uid="{EB703517-1E0F-514C-9C3F-F3364468974B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:Y62"/>
+  <dimension ref="A1:Y63"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q2" sqref="Q2"/>
+      <selection pane="bottomRight" activeCell="C23" sqref="C23:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="23" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13965,7 +14011,7 @@
         <v>64</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="V4" t="s">
         <v>533</v>
@@ -13988,7 +14034,7 @@
         <v>64</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="X5" s="13" t="s">
         <v>434</v>
@@ -14005,7 +14051,7 @@
         <v>64</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="X6" s="13" t="s">
         <v>434</v>
@@ -14037,7 +14083,7 @@
         <v>64</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="X8" s="13" t="s">
         <v>434</v>
@@ -14054,7 +14100,7 @@
         <v>64</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="X9" s="13" t="s">
         <v>434</v>
@@ -14085,7 +14131,7 @@
         <v>64</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="X11" s="13" t="s">
         <v>434</v>
@@ -14174,7 +14220,7 @@
         <v>64</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="X16" s="13" t="s">
         <v>434</v>
@@ -14191,7 +14237,7 @@
         <v>64</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="X17" s="13"/>
       <c r="Y17" s="13"/>
@@ -14204,7 +14250,7 @@
         <v>64</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="X18" s="13" t="s">
         <v>434</v>
@@ -14221,7 +14267,7 @@
         <v>64</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="X19" s="13"/>
       <c r="Y19" s="13"/>
@@ -14253,7 +14299,7 @@
         <v>64</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="X21" s="13" t="s">
         <v>434</v>
@@ -14270,32 +14316,31 @@
         <v>64</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
     </row>
     <row r="23" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>673</v>
+        <v>702</v>
       </c>
       <c r="B23" t="s">
         <v>64</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>604</v>
-      </c>
-      <c r="X23" s="13" t="s">
-        <v>434</v>
-      </c>
-      <c r="Y23" s="13" t="s">
-        <v>64</v>
-      </c>
+        <v>705</v>
+      </c>
+      <c r="X23" s="13"/>
+      <c r="Y23" s="13"/>
     </row>
     <row r="24" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>529</v>
+        <v>602</v>
       </c>
       <c r="B24" t="s">
         <v>64</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>705</v>
       </c>
       <c r="X24" s="13" t="s">
         <v>434</v>
@@ -14306,7 +14351,7 @@
     </row>
     <row r="25" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="B25" t="s">
         <v>64</v>
@@ -14318,28 +14363,42 @@
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>532</v>
+      </c>
+      <c r="B26" t="s">
+        <v>64</v>
+      </c>
+      <c r="X26" s="13" t="s">
+        <v>434</v>
+      </c>
+      <c r="Y26" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>429</v>
       </c>
-      <c r="B26" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="59" spans="22:25" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="V59" s="6"/>
-      <c r="X59" s="6"/>
-      <c r="Y59" s="6"/>
-    </row>
-    <row r="62" spans="22:25" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Y62" s="6"/>
+      <c r="B27" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="60" spans="22:25" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V60" s="6"/>
+      <c r="X60" s="6"/>
+      <c r="Y60" s="6"/>
+    </row>
+    <row r="63" spans="22:25" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Y63" s="6"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A21">
     <sortCondition ref="A2:A21"/>
   </sortState>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14425,10 +14484,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:AB10"/>
+  <dimension ref="A1:AC10"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="Y1" sqref="Y1:Y1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14439,10 +14498,10 @@
     <col min="7" max="7" width="35.33203125" customWidth="1"/>
     <col min="8" max="8" width="28.1640625" customWidth="1"/>
     <col min="24" max="24" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="36.5" customWidth="1"/>
+    <col min="25" max="28" width="36.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -14516,19 +14575,22 @@
         <v>416</v>
       </c>
       <c r="Y1" t="s">
-        <v>605</v>
+        <v>703</v>
       </c>
       <c r="Z1" t="s">
+        <v>603</v>
+      </c>
+      <c r="AA1" t="s">
         <v>535</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>536</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -14607,8 +14669,11 @@
       <c r="AA2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -14678,7 +14743,7 @@
         <v>28</v>
       </c>
       <c r="Y3" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="Z3" t="s">
         <v>11</v>
@@ -14686,8 +14751,11 @@
       <c r="AA3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -14755,7 +14823,7 @@
         <v>11</v>
       </c>
       <c r="Y4" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="Z4" t="s">
         <v>11</v>
@@ -14763,8 +14831,11 @@
       <c r="AA4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -14840,8 +14911,11 @@
       <c r="AA5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -14917,8 +14991,11 @@
       <c r="AA6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -14994,8 +15071,11 @@
       <c r="AA7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -15071,8 +15151,11 @@
       <c r="AA8" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -15140,7 +15223,7 @@
         <v>64</v>
       </c>
       <c r="Y9" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="Z9" t="s">
         <v>64</v>
@@ -15148,8 +15231,11 @@
       <c r="AA9" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -15223,6 +15309,9 @@
         <v>28</v>
       </c>
       <c r="AA10" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB10" t="s">
         <v>28</v>
       </c>
     </row>
@@ -15236,7 +15325,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+      <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
**Pre-Applied:** Remove US Core QuestionnaireResponse Tag Element [FHIR-40742]
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3962CE87-7D7D-B849-A51F-A5EBC4FC1FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE67CF2-39DB-AE41-A9A7-4F224196D287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51640" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -2094,6 +2094,228 @@
     <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</t>
   </si>
   <si>
+    <t>death-date</t>
+  </si>
+  <si>
+    <t>support searching for a patient by a server defined search that matches any of the string fields in the HumanName, including family, given, prefix, suffix, and/or text</t>
+  </si>
+  <si>
+    <t>tribal-affiliation</t>
+  </si>
+  <si>
+    <t>Patient.extension.where(url = 'http://hl7.org/fhir/us/core/StructureDefinition/us-core-tribal-affiliation').extension.value.code</t>
+  </si>
+  <si>
+    <t>support searching for a patient by tribal affiliation code</t>
+  </si>
+  <si>
+    <t>GET [base]/Patient?tribal-affiliiation=Shaw</t>
+  </si>
+  <si>
+    <t>Coverage</t>
+  </si>
+  <si>
+    <t>support searching for all coverages for a patient</t>
+  </si>
+  <si>
+    <t>MedicationDispense</t>
+  </si>
+  <si>
+    <t>MedicationDispense:medication</t>
+  </si>
+  <si>
+    <t>GET [base]/MedicationDispense?patient=14676~GET [base]/MedicationStatement?patient=14676&amp;_include=MedicationDispense:medication</t>
+  </si>
+  <si>
+    <t>!MedicationDispense</t>
+  </si>
+  <si>
+    <t>whenHandedOver</t>
+  </si>
+  <si>
+    <t>death-date,family</t>
+  </si>
+  <si>
+    <t>support searching for a patient by date of death and family name</t>
+  </si>
+  <si>
+    <t>GET [base]/Patient?family=Shaw&amp;death-date=2022-07-22</t>
+  </si>
+  <si>
+    <t>Implementation Notes: Fetches a bundle of all Condition resources for the specified patient and all "active" statuses (active,relapse,remission). This will *exclude* diagnoses and health concerns without a clinicalStatus specified.</t>
+  </si>
+  <si>
+    <t>GET [base]/Condition?patient=1032702&amp;category=http://terminology.hl7.org/CodeSystem/condition-category\|encounter-diagnosis&amp;encounter=1036</t>
+  </si>
+  <si>
+    <t>support searching for all devices with a given status for a patient (for example all active devices)</t>
+  </si>
+  <si>
+    <t>GET [base]/Device?patient=1316024&amp;status=active</t>
+  </si>
+  <si>
+    <t>Fetches a bundle of all Device resources for the specified patient and status</t>
+  </si>
+  <si>
+    <t>support searching for prescriptions for a patient based on their dispensed status</t>
+  </si>
+  <si>
+    <t>GET [base]/MedicationDispense?patient=1137192&amp;status=completed~GET [base]/MedicationDispense?patient=1137192&amp;status=completed&amp;_include=MedicationDispense:medication</t>
+  </si>
+  <si>
+    <t>support searching for prescriptions for a patient based on their dispensed status and dispense type.</t>
+  </si>
+  <si>
+    <t>GET [base]/MedicationDispense?patient=1137192&amp;status=&amp;type=~GET [base]/MedicationDispense?patient=1137192&amp;status=&amp;type=FFP&amp;_include=MedicationDispense:medication</t>
+  </si>
+  <si>
+    <t>patient,whenhandedover</t>
+  </si>
+  <si>
+    <t>support searching for prescriptions for a patient based on when it was dispensed to the patient.</t>
+  </si>
+  <si>
+    <t>foo</t>
+  </si>
+  <si>
+    <t>!Bulk Data Access IG</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-diagnosticreport</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-device</t>
+  </si>
+  <si>
+    <t>* The `DocumentReference.type` binding **SHALL** support at a minimum the [5 Common Clinical Notes](ValueSet-us-core-clinical-note-type.html) and may extend to the full US Core DocumentReference Type Value Set
+* The DocumentReference resources can represent the referenced content using either an address where the document can be retrieved using `DocumentReference.attachment.url` or the content as inline base64 encoded data using `DocumentReference.attachment.data`.
+    *  Although both are marked as must support, the server system is not required to support an address, and inline base64 encoded data, but **SHALL** support at least one of these elements.
+    *  The client application **SHALL** support both elements.
+    *  The `content.url` may refer to a FHIR Binary Resource (i.e. [base]/Binary/[id]), FHIR Document Bundle (i.e [base]/Bundle/[id] or another endpoint.
+        * If the endpoint is outside the FHIR base URL, it **SHOULD NOT** require additional authorization to access.
+* Every DocumentReference must have a responsible Organization. The organization responsible for the DocumentReference **SHALL** be present either in `DocumentReference.custodian` or accessible in the Provenance resource targeting the DocumentReference using `Provenance.agent.who` or `Provenance.agent.onBehalfOf`.</t>
+  </si>
+  <si>
+    <t>Servers that support only US Core Practitioner Profile **SHALL** provide implementation specific guidance how to access a provider’s location and contact information using only the Practitioner resource.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/smart-app-launch/history.html</t>
+  </si>
+  <si>
+    <t>!!Questionnaire</t>
+  </si>
+  <si>
+    <t>!Questionnaire.id</t>
+  </si>
+  <si>
+    <t>GET [base]/!QuestionnaireResponse/AHC-HRSN-screening-example~GET [base]/!QuestionnaireResponse/?_id=AHC-HRSN-screening-example</t>
+  </si>
+  <si>
+    <t>Allows retrieving !QuestionnaireResponses that are complete (or incomplete)</t>
+  </si>
+  <si>
+    <t>!QuestionnaireResponse.meta._tag</t>
+  </si>
+  <si>
+    <t>Allows filtering for !QuestionnaireResponse that have tag of “sdoh”</t>
+  </si>
+  <si>
+    <t>Allows filtering for !QuestionnaireResponses by when they were created/last edited</t>
+  </si>
+  <si>
+    <t>Allows retrieving !QuestionnaireResponses that have been completed against a specified form</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-coverage</t>
+  </si>
+  <si>
+    <t>US Core Coverage Profile</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</t>
+  </si>
+  <si>
+    <t>US Core MedicationDispense Profile</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-pregnancystatus</t>
+  </si>
+  <si>
+    <t>US Core Observation Pregnancy Status Profile</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-pregnancyintent</t>
+  </si>
+  <si>
+    <t>US Core Observation Pregnancy Intent Profile</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-occupation</t>
+  </si>
+  <si>
+    <t>US Core Observation Occupation Profile</t>
+  </si>
+  <si>
+    <t>!http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-sdoh-assessment</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-simple-observation</t>
+  </si>
+  <si>
+    <t>!http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-imaging</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-clinical-result</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-specimen</t>
+  </si>
+  <si>
+    <t>US Core Specimen Profile</t>
+  </si>
+  <si>
+    <t>Specimen</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-screening-assessment</t>
+  </si>
+  <si>
+    <t>US Core Simple Observation Profile</t>
+  </si>
+  <si>
+    <t>US Core Observation Screening Assessment Profile</t>
+  </si>
+  <si>
+    <t>US Core Observation Clinical Result Profile</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/uv/sdc/StructureDefinition/sdc-questionnaire</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-extension-questionnaire-uri</t>
+  </si>
+  <si>
+    <t>Questionnaire</t>
+  </si>
+  <si>
+    <t>conf_Questionnaire</t>
+  </si>
+  <si>
+    <t>SDC Base Questionnaire Profile</t>
+  </si>
+  <si>
+    <t>US Core defines two ways to represent the questions and responses to screening and assessment instruments:
+- Observation: [US Core Observation Screening Assessment Profile]
+- Questionnaire/QuestionnaireResponse: [SDC Base Questionnaire]/[US Core QuestionnaireResponse Profile]
+US Core Servers **SHALL** [US Core Observation Screening Assessment Profile] and **SHOULD** support the  [SDC Base Questionnaire Profile]/[US Core QuestionnaireResponse Profile]</t>
+  </si>
+  <si>
     <t>* The US Core Provenance resource **SHALL** be supported for these US Core resources:
     * AllergyIntolerance
     * CarePlan
@@ -2111,232 +2333,11 @@
     * Observation
     * Patient
     * Procedure
+    * QuestionnaireResponse
     * RelatedPerson
     * ServiceRequest
 * If a system receives a provider in `Provenance.agent.who` as free text they must capture who sent them the information as the organization. On request they **SHALL** provide this organization as the source and **MAY** include the free text provider.
 * Systems that need to know the activity has occurred **SHOULD** populate the activity.</t>
-  </si>
-  <si>
-    <t>death-date</t>
-  </si>
-  <si>
-    <t>support searching for a patient by a server defined search that matches any of the string fields in the HumanName, including family, given, prefix, suffix, and/or text</t>
-  </si>
-  <si>
-    <t>tribal-affiliation</t>
-  </si>
-  <si>
-    <t>Patient.extension.where(url = 'http://hl7.org/fhir/us/core/StructureDefinition/us-core-tribal-affiliation').extension.value.code</t>
-  </si>
-  <si>
-    <t>support searching for a patient by tribal affiliation code</t>
-  </si>
-  <si>
-    <t>GET [base]/Patient?tribal-affiliiation=Shaw</t>
-  </si>
-  <si>
-    <t>Coverage</t>
-  </si>
-  <si>
-    <t>support searching for all coverages for a patient</t>
-  </si>
-  <si>
-    <t>MedicationDispense</t>
-  </si>
-  <si>
-    <t>MedicationDispense:medication</t>
-  </si>
-  <si>
-    <t>GET [base]/MedicationDispense?patient=14676~GET [base]/MedicationStatement?patient=14676&amp;_include=MedicationDispense:medication</t>
-  </si>
-  <si>
-    <t>!MedicationDispense</t>
-  </si>
-  <si>
-    <t>whenHandedOver</t>
-  </si>
-  <si>
-    <t>death-date,family</t>
-  </si>
-  <si>
-    <t>support searching for a patient by date of death and family name</t>
-  </si>
-  <si>
-    <t>GET [base]/Patient?family=Shaw&amp;death-date=2022-07-22</t>
-  </si>
-  <si>
-    <t>Implementation Notes: Fetches a bundle of all Condition resources for the specified patient and all "active" statuses (active,relapse,remission). This will *exclude* diagnoses and health concerns without a clinicalStatus specified.</t>
-  </si>
-  <si>
-    <t>GET [base]/Condition?patient=1032702&amp;category=http://terminology.hl7.org/CodeSystem/condition-category\|encounter-diagnosis&amp;encounter=1036</t>
-  </si>
-  <si>
-    <t>support searching for all devices with a given status for a patient (for example all active devices)</t>
-  </si>
-  <si>
-    <t>GET [base]/Device?patient=1316024&amp;status=active</t>
-  </si>
-  <si>
-    <t>Fetches a bundle of all Device resources for the specified patient and status</t>
-  </si>
-  <si>
-    <t>support searching for prescriptions for a patient based on their dispensed status</t>
-  </si>
-  <si>
-    <t>GET [base]/MedicationDispense?patient=1137192&amp;status=completed~GET [base]/MedicationDispense?patient=1137192&amp;status=completed&amp;_include=MedicationDispense:medication</t>
-  </si>
-  <si>
-    <t>support searching for prescriptions for a patient based on their dispensed status and dispense type.</t>
-  </si>
-  <si>
-    <t>GET [base]/MedicationDispense?patient=1137192&amp;status=&amp;type=~GET [base]/MedicationDispense?patient=1137192&amp;status=&amp;type=FFP&amp;_include=MedicationDispense:medication</t>
-  </si>
-  <si>
-    <t>patient,whenhandedover</t>
-  </si>
-  <si>
-    <t>support searching for prescriptions for a patient based on when it was dispensed to the patient.</t>
-  </si>
-  <si>
-    <t>foo</t>
-  </si>
-  <si>
-    <t>!Bulk Data Access IG</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-diagnosticreport</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-device</t>
-  </si>
-  <si>
-    <t>* The `DocumentReference.type` binding **SHALL** support at a minimum the [5 Common Clinical Notes](ValueSet-us-core-clinical-note-type.html) and may extend to the full US Core DocumentReference Type Value Set
-* The DocumentReference resources can represent the referenced content using either an address where the document can be retrieved using `DocumentReference.attachment.url` or the content as inline base64 encoded data using `DocumentReference.attachment.data`.
-    *  Although both are marked as must support, the server system is not required to support an address, and inline base64 encoded data, but **SHALL** support at least one of these elements.
-    *  The client application **SHALL** support both elements.
-    *  The `content.url` may refer to a FHIR Binary Resource (i.e. [base]/Binary/[id]), FHIR Document Bundle (i.e [base]/Bundle/[id] or another endpoint.
-        * If the endpoint is outside the FHIR base URL, it **SHOULD NOT** require additional authorization to access.
-* Every DocumentReference must have a responsible Organization. The organization responsible for the DocumentReference **SHALL** be present either in `DocumentReference.custodian` or accessible in the Provenance resource targeting the DocumentReference using `Provenance.agent.who` or `Provenance.agent.onBehalfOf`.</t>
-  </si>
-  <si>
-    <t>Servers that support only US Core Practitioner Profile **SHALL** provide implementation specific guidance how to access a provider’s location and contact information using only the Practitioner resource.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/smart-app-launch/history.html</t>
-  </si>
-  <si>
-    <t>!!Questionnaire</t>
-  </si>
-  <si>
-    <t>!Questionnaire.id</t>
-  </si>
-  <si>
-    <t>GET [base]/!QuestionnaireResponse/AHC-HRSN-screening-example~GET [base]/!QuestionnaireResponse/?_id=AHC-HRSN-screening-example</t>
-  </si>
-  <si>
-    <t>Allows retrieving !QuestionnaireResponses that are complete (or incomplete)</t>
-  </si>
-  <si>
-    <t>!QuestionnaireResponse.meta._tag</t>
-  </si>
-  <si>
-    <t>Allows filtering for !QuestionnaireResponse that have tag of “sdoh”</t>
-  </si>
-  <si>
-    <t>Allows filtering for !QuestionnaireResponses by when they were created/last edited</t>
-  </si>
-  <si>
-    <t>Allows retrieving !QuestionnaireResponses that have been completed against a specified form</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-coverage</t>
-  </si>
-  <si>
-    <t>US Core Coverage Profile</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</t>
-  </si>
-  <si>
-    <t>US Core MedicationDispense Profile</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-pregnancystatus</t>
-  </si>
-  <si>
-    <t>US Core Observation Pregnancy Status Profile</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-pregnancyintent</t>
-  </si>
-  <si>
-    <t>US Core Observation Pregnancy Intent Profile</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-occupation</t>
-  </si>
-  <si>
-    <t>US Core Observation Occupation Profile</t>
-  </si>
-  <si>
-    <t>!http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-sdoh-assessment</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-simple-observation</t>
-  </si>
-  <si>
-    <t>!http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-imaging</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-clinical-result</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-specimen</t>
-  </si>
-  <si>
-    <t>US Core Specimen Profile</t>
-  </si>
-  <si>
-    <t>Specimen</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-screening-assessment</t>
-  </si>
-  <si>
-    <t>US Core Simple Observation Profile</t>
-  </si>
-  <si>
-    <t>US Core Observation Screening Assessment Profile</t>
-  </si>
-  <si>
-    <t>US Core Observation Clinical Result Profile</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/uv/sdc/StructureDefinition/sdc-questionnaire</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-extension-questionnaire-uri</t>
-  </si>
-  <si>
-    <t>Questionnaire</t>
-  </si>
-  <si>
-    <t>conf_Questionnaire</t>
-  </si>
-  <si>
-    <t>SDC Base Questionnaire Profile</t>
-  </si>
-  <si>
-    <t>US Core defines two ways to represent the questions and responses to screening and assessment instruments:
-- Observation: [US Core Observation Screening Assessment Profile]
-- Questionnaire/QuestionnaireResponse: [SDC Base Questionnaire]/[US Core QuestionnaireResponse Profile]
-US Core Servers **SHALL** [US Core Observation Screening Assessment Profile] and **SHOULD** support the  [SDC Base Questionnaire Profile]/[US Core QuestionnaireResponse Profile]</t>
   </si>
 </sst>
 </file>
@@ -2537,17 +2538,7 @@
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4362,7 +4353,7 @@
         <v>19</v>
       </c>
       <c r="C25" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="D25" t="s">
         <v>28</v>
@@ -4639,7 +4630,7 @@
         <v>51</v>
       </c>
       <c r="Y30" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="Z30" t="s">
         <v>167</v>
@@ -4661,7 +4652,7 @@
         <v>79</v>
       </c>
       <c r="C31" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="D31" t="s">
         <v>28</v>
@@ -4686,19 +4677,19 @@
         <v>52</v>
       </c>
       <c r="L31" t="s">
+        <v>637</v>
+      </c>
+      <c r="M31" t="s">
+        <v>51</v>
+      </c>
+      <c r="O31" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y31" s="4" t="s">
         <v>638</v>
       </c>
-      <c r="M31" t="s">
-        <v>51</v>
-      </c>
-      <c r="O31" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y31" s="4" t="s">
+      <c r="Z31" t="s">
         <v>639</v>
-      </c>
-      <c r="Z31" t="s">
-        <v>640</v>
       </c>
       <c r="AA31" s="8" t="str">
         <f>"Fetches a bundle of all "&amp;B31&amp;" resources matching the name"</f>
@@ -4714,7 +4705,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="C32" t="s">
         <v>50</v>
@@ -4739,7 +4730,7 @@
         <v>52</v>
       </c>
       <c r="L32" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="M32" t="s">
         <v>51</v>
@@ -4757,7 +4748,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="C33" t="s">
         <v>65</v>
@@ -4801,7 +4792,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="C34" t="s">
         <v>62</v>
@@ -4848,7 +4839,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="C35" t="s">
         <v>56</v>
@@ -4892,7 +4883,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="C36" t="s">
         <v>57</v>
@@ -4948,7 +4939,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="C37" t="s">
         <v>54</v>
@@ -4992,7 +4983,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="C38" t="s">
         <v>61</v>
@@ -9198,7 +9189,7 @@
         <v>51</v>
       </c>
       <c r="Y115" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="Z115" s="4" t="str">
         <f>"GET [base]/"&amp;B115&amp;"?"&amp;C115&amp;"=Mary Shaw"</f>
@@ -9257,7 +9248,7 @@
         <v>support fetching a QuestionnaireResponse</v>
       </c>
       <c r="Z116" s="4" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="AB116" t="str">
         <f t="shared" si="9"/>
@@ -9369,7 +9360,7 @@
         <v>51</v>
       </c>
       <c r="Y118" s="19" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="AB118" t="str">
         <f t="shared" si="9"/>
@@ -9409,16 +9400,16 @@
         <v>52</v>
       </c>
       <c r="L119" t="s">
+        <v>673</v>
+      </c>
+      <c r="M119" t="s">
+        <v>51</v>
+      </c>
+      <c r="O119" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y119" s="19" t="s">
         <v>674</v>
-      </c>
-      <c r="M119" t="s">
-        <v>51</v>
-      </c>
-      <c r="O119" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y119" s="19" t="s">
-        <v>675</v>
       </c>
       <c r="AB119" t="str">
         <f t="shared" si="9"/>
@@ -9474,7 +9465,7 @@
         <v>87</v>
       </c>
       <c r="Y120" s="19" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="AB120" t="str">
         <f t="shared" si="9"/>
@@ -9524,7 +9515,7 @@
         <v>51</v>
       </c>
       <c r="Y121" s="19" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="AB121" t="str">
         <f t="shared" si="9"/>
@@ -9536,7 +9527,7 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="C122" t="s">
         <v>84</v>
@@ -9577,7 +9568,7 @@
         <v>51</v>
       </c>
       <c r="Y122" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="Z122" s="4" t="str">
         <f>"GET [base]/"&amp;B122&amp;"?patient=1137192"</f>
@@ -9597,7 +9588,7 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C123" t="s">
         <v>56</v>
@@ -9653,7 +9644,7 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C124" t="s">
         <v>12</v>
@@ -9709,7 +9700,7 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C125" t="s">
         <v>84</v>
@@ -9750,10 +9741,10 @@
         <v>51</v>
       </c>
       <c r="X125" s="6" t="s">
+        <v>643</v>
+      </c>
+      <c r="Z125" s="8" t="s">
         <v>644</v>
-      </c>
-      <c r="Z125" s="8" t="s">
-        <v>645</v>
       </c>
       <c r="AA125" s="8" t="str">
         <f>"Fetches a bundle of all "&amp;B125&amp; " resources for the specified patient."</f>
@@ -9769,10 +9760,10 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
+        <v>645</v>
+      </c>
+      <c r="C126" t="s">
         <v>646</v>
-      </c>
-      <c r="C126" t="s">
-        <v>647</v>
       </c>
       <c r="D126" t="s">
         <v>28</v>
@@ -10710,7 +10701,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D32" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="F32" t="s">
         <v>64</v>
@@ -10719,10 +10710,10 @@
         <v>128</v>
       </c>
       <c r="I32" s="4" t="s">
+        <v>648</v>
+      </c>
+      <c r="J32" s="4" t="s">
         <v>649</v>
-      </c>
-      <c r="J32" s="4" t="s">
-        <v>650</v>
       </c>
       <c r="K32" s="4" t="str">
         <f t="shared" si="1"/>
@@ -10852,7 +10843,7 @@
         <v>312</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
@@ -10912,7 +10903,7 @@
         <v>144</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="K38" s="4" t="s">
         <v>557</v>
@@ -11168,7 +11159,7 @@
         <v>173</v>
       </c>
       <c r="C47" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D47" t="s">
         <v>110</v>
@@ -11198,7 +11189,7 @@
         <v>173</v>
       </c>
       <c r="C48" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D48" t="s">
         <v>139</v>
@@ -11231,7 +11222,7 @@
         <v>173</v>
       </c>
       <c r="C49" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D49" t="s">
         <v>141</v>
@@ -11261,7 +11252,7 @@
         <v>173</v>
       </c>
       <c r="C50" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D50" t="s">
         <v>188</v>
@@ -11294,7 +11285,7 @@
         <v>173</v>
       </c>
       <c r="C51" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D51" t="s">
         <v>212</v>
@@ -11672,7 +11663,7 @@
         <v>177</v>
       </c>
       <c r="C63" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D63" t="s">
         <v>229</v>
@@ -11704,7 +11695,7 @@
         <v>177</v>
       </c>
       <c r="C64" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D64" t="s">
         <v>139</v>
@@ -11737,7 +11728,7 @@
         <v>177</v>
       </c>
       <c r="C65" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D65" t="s">
         <v>141</v>
@@ -11767,7 +11758,7 @@
         <v>177</v>
       </c>
       <c r="C66" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D66" t="s">
         <v>188</v>
@@ -11800,7 +11791,7 @@
         <v>177</v>
       </c>
       <c r="C67" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D67" t="s">
         <v>212</v>
@@ -11830,7 +11821,7 @@
         <v>304</v>
       </c>
       <c r="C68" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D68" t="s">
         <v>110</v>
@@ -12209,7 +12200,7 @@
         <v>241</v>
       </c>
       <c r="C80" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="D80" t="s">
         <v>112</v>
@@ -12238,7 +12229,7 @@
         <v>241</v>
       </c>
       <c r="C81" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="D81" t="s">
         <v>110</v>
@@ -12253,13 +12244,13 @@
         <v>100</v>
       </c>
       <c r="I81" s="4" t="s">
+        <v>652</v>
+      </c>
+      <c r="J81" s="4" t="s">
         <v>653</v>
       </c>
-      <c r="J81" s="4" t="s">
+      <c r="K81" s="4" t="s">
         <v>654</v>
-      </c>
-      <c r="K81" s="4" t="s">
-        <v>655</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
@@ -12644,7 +12635,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="16" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C94" t="str">
         <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B94)</f>
@@ -12664,10 +12655,10 @@
       </c>
       <c r="H94" s="16"/>
       <c r="I94" s="4" t="s">
+        <v>655</v>
+      </c>
+      <c r="J94" s="4" t="s">
         <v>656</v>
-      </c>
-      <c r="J94" s="4" t="s">
-        <v>657</v>
       </c>
       <c r="K94" t="str">
         <f>"Fetches a bundle of all "&amp;B94&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed))."</f>
@@ -12679,7 +12670,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="16" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C95" t="str">
         <f t="shared" si="4"/>
@@ -12699,10 +12690,10 @@
       </c>
       <c r="H95" s="16"/>
       <c r="I95" s="4" t="s">
+        <v>657</v>
+      </c>
+      <c r="J95" s="4" t="s">
         <v>658</v>
-      </c>
-      <c r="J95" s="4" t="s">
-        <v>659</v>
       </c>
       <c r="K95" t="str">
         <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed) and type of dispense (e.g., partially dispensed)."</f>
@@ -12714,14 +12705,14 @@
         <v>95</v>
       </c>
       <c r="B96" s="16" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="C96" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationdispense</v>
       </c>
       <c r="D96" s="16" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="E96" s="16" t="s">
         <v>51</v>
@@ -12734,10 +12725,10 @@
       </c>
       <c r="H96" s="16"/>
       <c r="I96" s="4" t="s">
+        <v>660</v>
+      </c>
+      <c r="J96" s="4" t="s">
         <v>661</v>
-      </c>
-      <c r="J96" s="4" t="s">
-        <v>662</v>
       </c>
       <c r="K96" t="str">
         <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient for a given dispense and date or range"</f>
@@ -12908,7 +12899,7 @@
         <v>526</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="D2" t="s">
         <v>64</v>
@@ -12916,7 +12907,7 @@
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>521</v>
@@ -13101,16 +13092,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>677</v>
+      </c>
+      <c r="B7" t="s">
         <v>678</v>
       </c>
-      <c r="B7" t="s">
-        <v>679</v>
-      </c>
       <c r="D7" t="s">
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -13255,7 +13246,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="24" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B18" t="s">
         <v>597</v>
@@ -13339,16 +13330,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>679</v>
+      </c>
+      <c r="B24" t="s">
         <v>680</v>
       </c>
-      <c r="B24" t="s">
-        <v>681</v>
-      </c>
       <c r="D24" t="s">
         <v>11</v>
       </c>
       <c r="E24" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -13367,10 +13358,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>681</v>
+      </c>
+      <c r="B26" t="s">
         <v>682</v>
-      </c>
-      <c r="B26" t="s">
-        <v>683</v>
       </c>
       <c r="D26" t="s">
         <v>11</v>
@@ -13381,10 +13372,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>683</v>
+      </c>
+      <c r="B27" t="s">
         <v>684</v>
-      </c>
-      <c r="B27" t="s">
-        <v>685</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
@@ -13395,10 +13386,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>685</v>
+      </c>
+      <c r="B28" t="s">
         <v>686</v>
-      </c>
-      <c r="B28" t="s">
-        <v>687</v>
       </c>
       <c r="D28" t="s">
         <v>11</v>
@@ -13409,7 +13400,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="18" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B29" t="s">
         <v>598</v>
@@ -13437,10 +13428,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B31" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="D31" t="s">
         <v>11</v>
@@ -13577,10 +13568,10 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B41" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="D41" t="s">
         <v>11</v>
@@ -13605,7 +13596,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="18" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B43" t="s">
         <v>600</v>
@@ -13619,10 +13610,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B44" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="D44" t="s">
         <v>11</v>
@@ -13773,21 +13764,21 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="23" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B55" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="D55" t="s">
         <v>11</v>
       </c>
       <c r="E55" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="23" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B56" t="s">
         <v>601</v>
@@ -13829,16 +13820,16 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="18" t="s">
+        <v>691</v>
+      </c>
+      <c r="B59" t="s">
         <v>692</v>
       </c>
-      <c r="B59" t="s">
+      <c r="D59" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59" t="s">
         <v>693</v>
-      </c>
-      <c r="D59" t="s">
-        <v>11</v>
-      </c>
-      <c r="E59" t="s">
-        <v>694</v>
       </c>
     </row>
   </sheetData>
@@ -13873,7 +13864,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C23" sqref="C23:C24"/>
+      <selection pane="bottomRight" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="23" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -14083,7 +14074,7 @@
         <v>64</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="X8" s="13" t="s">
         <v>434</v>
@@ -14267,7 +14258,7 @@
         <v>64</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="X19" s="13"/>
       <c r="Y19" s="13"/>
@@ -14316,18 +14307,18 @@
         <v>64</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>634</v>
+        <v>705</v>
       </c>
     </row>
     <row r="23" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B23" t="s">
         <v>64</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="X23" s="13"/>
       <c r="Y23" s="13"/>
@@ -14340,7 +14331,7 @@
         <v>64</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="X24" s="13" t="s">
         <v>434</v>
@@ -14575,7 +14566,7 @@
         <v>416</v>
       </c>
       <c r="Y1" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="Z1" t="s">
         <v>603</v>

</xml_diff>

<commit_message>
Add Goal.startDate as 0..1 MS with choice of supporting this or Goal.target.dueDate [FHIR-40103]
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE67CF2-39DB-AE41-A9A7-4F224196D287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C2E88C3-A6C6-864C-B2F5-6DB0CFB7C8A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="52080" yWindow="11940" windowWidth="51200" windowHeight="28300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -121,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2588" uniqueCount="706">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2589" uniqueCount="707">
   <si>
     <t>Element</t>
   </si>
@@ -2338,6 +2338,9 @@
     * ServiceRequest
 * If a system receives a provider in `Provenance.agent.who` as free text they must capture who sent them the information as the organization. On request they **SHALL** provide this organization as the source and **MAY** include the free text provider.
 * Systems that need to know the activity has occurred **SHOULD** populate the activity.</t>
+  </si>
+  <si>
+    <t>* Although both `Goal.startDate` and `Goal.target.dueDate` are marked as must support, the server system is not required to support both, but **SHALL** support at least one of these elements. The client application **SHALL** support both elements.</t>
   </si>
 </sst>
 </file>
@@ -2495,7 +2498,7 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2529,7 +2532,6 @@
     <xf numFmtId="49" fontId="13" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="14" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
@@ -13245,7 +13247,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="24" t="s">
+      <c r="A18" s="23" t="s">
         <v>700</v>
       </c>
       <c r="B18" t="s">
@@ -13763,7 +13765,7 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" s="23" t="s">
+      <c r="A55" t="s">
         <v>698</v>
       </c>
       <c r="B55" t="s">
@@ -13777,7 +13779,7 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" s="23" t="s">
+      <c r="A56" t="s">
         <v>699</v>
       </c>
       <c r="B56" t="s">
@@ -13864,7 +13866,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C24" sqref="C24"/>
+      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="23" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -14106,6 +14108,9 @@
       </c>
       <c r="B10" t="s">
         <v>64</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>706</v>
       </c>
       <c r="X10" s="13" t="s">
         <v>434</v>

</xml_diff>

<commit_message>
Correction and clarify use of $expand [FHIR-39719](https://jira.hl7.org/browse/FHIR-39719)
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C2E88C3-A6C6-864C-B2F5-6DB0CFB7C8A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F196065A-1344-0C49-8BD7-468C5072FC9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52080" yWindow="11940" windowWidth="51200" windowHeight="28300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -1414,9 +1414,6 @@
     <t>ValueSet</t>
   </si>
   <si>
-    <t>A  client can determine the note and report types support by a server by invoking the standard FHIR Value Set Expansion ($expand) operation defined in the FHIR R4 specification. Because servers may support different read and write formats, it also is used to determine the formats (for example, text, pdf) the server supports read and write transactions.</t>
-  </si>
-  <si>
     <t>expand</t>
   </si>
   <si>
@@ -2341,6 +2338,9 @@
   </si>
   <si>
     <t>* Although both `Goal.startDate` and `Goal.target.dueDate` are marked as must support, the server system is not required to support both, but **SHALL** support at least one of these elements. The client application **SHALL** support both elements.</t>
+  </si>
+  <si>
+    <t>If a server supports DocumentReference for creating, using, and sharing clinical notes, it **SHOULD** also support the `context` and `contextdirection` parameters of the $expand operation to enable clients to determine the supported note and report types, as well as the supported read/write formats for notes on the server.</t>
   </si>
 </sst>
 </file>
@@ -2498,7 +2498,7 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2533,6 +2533,9 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="49" fontId="14" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -2970,34 +2973,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B3" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>448</v>
+      </c>
+      <c r="B4" t="s">
         <v>449</v>
-      </c>
-      <c r="B4" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>450</v>
+      </c>
+      <c r="B5" t="s">
         <v>451</v>
-      </c>
-      <c r="B5" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -3005,12 +3008,12 @@
         <v>62</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B7" t="s">
         <v>54</v>
@@ -3018,15 +3021,15 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B8" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
@@ -3091,7 +3094,7 @@
         <v>39</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>30</v>
@@ -3313,7 +3316,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
@@ -3521,7 +3524,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
@@ -3570,7 +3573,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
@@ -3628,7 +3631,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
@@ -3678,7 +3681,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="0"/>
@@ -3726,7 +3729,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="0"/>
@@ -3837,7 +3840,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
@@ -3887,7 +3890,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="0"/>
@@ -3941,7 +3944,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
@@ -3998,7 +4001,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="0"/>
@@ -4047,7 +4050,7 @@
         <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D19" t="s">
         <v>28</v>
@@ -4056,7 +4059,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="0"/>
@@ -4114,7 +4117,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="0"/>
@@ -4164,7 +4167,7 @@
         <v>0</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="0"/>
@@ -4205,7 +4208,7 @@
         <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D22" t="s">
         <v>28</v>
@@ -4214,7 +4217,7 @@
         <v>0</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="0"/>
@@ -4317,7 +4320,7 @@
         <v>0</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="0"/>
@@ -4355,7 +4358,7 @@
         <v>19</v>
       </c>
       <c r="C25" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="D25" t="s">
         <v>28</v>
@@ -4364,7 +4367,7 @@
         <v>0</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" si="0"/>
@@ -4414,7 +4417,7 @@
         <v>0</v>
       </c>
       <c r="F26" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="0"/>
@@ -4460,7 +4463,7 @@
         <v>0</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" si="0"/>
@@ -4552,7 +4555,7 @@
         <v>1</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="0"/>
@@ -4632,7 +4635,7 @@
         <v>51</v>
       </c>
       <c r="Y30" s="4" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="Z30" t="s">
         <v>167</v>
@@ -4654,7 +4657,7 @@
         <v>79</v>
       </c>
       <c r="C31" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="D31" t="s">
         <v>28</v>
@@ -4679,19 +4682,19 @@
         <v>52</v>
       </c>
       <c r="L31" t="s">
+        <v>636</v>
+      </c>
+      <c r="M31" t="s">
+        <v>51</v>
+      </c>
+      <c r="O31" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y31" s="4" t="s">
         <v>637</v>
       </c>
-      <c r="M31" t="s">
-        <v>51</v>
-      </c>
-      <c r="O31" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y31" s="4" t="s">
+      <c r="Z31" t="s">
         <v>638</v>
-      </c>
-      <c r="Z31" t="s">
-        <v>639</v>
       </c>
       <c r="AA31" s="8" t="str">
         <f>"Fetches a bundle of all "&amp;B31&amp;" resources matching the name"</f>
@@ -4707,7 +4710,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="C32" t="s">
         <v>50</v>
@@ -4732,7 +4735,7 @@
         <v>52</v>
       </c>
       <c r="L32" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="M32" t="s">
         <v>51</v>
@@ -4750,7 +4753,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="C33" t="s">
         <v>65</v>
@@ -4794,7 +4797,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="C34" t="s">
         <v>62</v>
@@ -4841,7 +4844,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="C35" t="s">
         <v>56</v>
@@ -4885,7 +4888,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="C36" t="s">
         <v>57</v>
@@ -4941,7 +4944,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="C37" t="s">
         <v>54</v>
@@ -4985,7 +4988,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="C38" t="s">
         <v>61</v>
@@ -5041,7 +5044,7 @@
         <v>0</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="G39" t="str">
         <f t="shared" si="0"/>
@@ -5086,7 +5089,7 @@
         <v>132</v>
       </c>
       <c r="C40" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D40" t="s">
         <v>28</v>
@@ -5095,7 +5098,7 @@
         <v>0</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="G40" t="str">
         <f t="shared" si="0"/>
@@ -5140,7 +5143,7 @@
         <v>132</v>
       </c>
       <c r="C41" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D41" t="s">
         <v>28</v>
@@ -5149,7 +5152,7 @@
         <v>0</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="G41" t="str">
         <f t="shared" si="0"/>
@@ -5194,7 +5197,7 @@
         <v>132</v>
       </c>
       <c r="C42" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="D42" t="s">
         <v>28</v>
@@ -5203,7 +5206,7 @@
         <v>0</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="G42" t="str">
         <f t="shared" si="0"/>
@@ -5257,7 +5260,7 @@
         <v>0</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G43" t="str">
         <f t="shared" si="0"/>
@@ -5307,7 +5310,7 @@
         <v>0</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G44" t="str">
         <f t="shared" si="0"/>
@@ -5333,7 +5336,7 @@
         <v>51</v>
       </c>
       <c r="Y44" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="Z44" s="4" t="str">
         <f>"GET [base]/"&amp;B44&amp;"?patient=1137192"</f>
@@ -5365,7 +5368,7 @@
         <v>1</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G45" t="str">
         <f t="shared" si="0"/>
@@ -5424,7 +5427,7 @@
         <v>0</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G46" t="str">
         <f t="shared" si="0"/>
@@ -5474,7 +5477,7 @@
         <v>0</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="G47" t="str">
         <f t="shared" si="0"/>
@@ -5581,7 +5584,7 @@
         <v>0</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G49" t="str">
         <f t="shared" si="0"/>
@@ -5634,7 +5637,7 @@
         <v>1</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G50" t="str">
         <f t="shared" si="0"/>
@@ -5693,7 +5696,7 @@
         <v>0</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G51" t="str">
         <f t="shared" si="0"/>
@@ -5743,7 +5746,7 @@
         <v>0</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G52" t="str">
         <f t="shared" si="0"/>
@@ -5793,7 +5796,7 @@
         <v>0</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="G53" t="str">
         <f t="shared" si="0"/>
@@ -5847,7 +5850,7 @@
         <v>0</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="G54" t="str">
         <f t="shared" si="0"/>
@@ -5900,7 +5903,7 @@
         <v>0</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G55" t="str">
         <f t="shared" si="0"/>
@@ -5953,7 +5956,7 @@
         <v>1</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G56" t="str">
         <f t="shared" si="0"/>
@@ -6012,7 +6015,7 @@
         <v>0</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G57" t="str">
         <f t="shared" si="0"/>
@@ -6062,7 +6065,7 @@
         <v>0</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G58" t="str">
         <f t="shared" si="0"/>
@@ -6115,7 +6118,7 @@
         <v>0</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="G59" t="str">
         <f t="shared" si="0"/>
@@ -6169,7 +6172,7 @@
         <v>0</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G60" t="str">
         <f t="shared" si="0"/>
@@ -6219,7 +6222,7 @@
         <v>1</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G61" t="str">
         <f t="shared" si="0"/>
@@ -6278,7 +6281,7 @@
         <v>0</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="G62" t="str">
         <f t="shared" si="0"/>
@@ -6332,7 +6335,7 @@
         <v>0</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G63" t="str">
         <f t="shared" si="0"/>
@@ -6385,7 +6388,7 @@
         <v>0</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G64" t="str">
         <f t="shared" si="0"/>
@@ -6438,7 +6441,7 @@
         <v>0</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G65" t="str">
         <f t="shared" si="0"/>
@@ -6491,7 +6494,7 @@
         <v>0</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G66" t="str">
         <f t="shared" ref="G66:G126" si="7">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B66)</f>
@@ -6542,7 +6545,7 @@
         <v>0</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="G67" t="str">
         <f t="shared" si="7"/>
@@ -6596,7 +6599,7 @@
         <v>0</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G68" t="str">
         <f t="shared" si="7"/>
@@ -6649,7 +6652,7 @@
         <v>1</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G69" t="str">
         <f t="shared" si="7"/>
@@ -6707,7 +6710,7 @@
         <v>0</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="G70" t="str">
         <f t="shared" si="7"/>
@@ -6761,7 +6764,7 @@
         <v>0</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G71" t="str">
         <f t="shared" si="7"/>
@@ -6814,7 +6817,7 @@
         <v>1</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G72" t="str">
         <f t="shared" si="7"/>
@@ -6872,7 +6875,7 @@
         <v>0</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="G73" t="str">
         <f t="shared" si="7"/>
@@ -6926,7 +6929,7 @@
         <v>0</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G74" t="str">
         <f t="shared" si="7"/>
@@ -6979,7 +6982,7 @@
         <v>0</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G75" t="str">
         <f t="shared" si="7"/>
@@ -7032,7 +7035,7 @@
         <v>0</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G76" t="str">
         <f t="shared" si="7"/>
@@ -7082,7 +7085,7 @@
         <v>0</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G77" t="str">
         <f t="shared" si="7"/>
@@ -7135,7 +7138,7 @@
         <v>0</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="G78" t="str">
         <f t="shared" si="7"/>
@@ -7189,7 +7192,7 @@
         <v>0</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G79" t="str">
         <f t="shared" si="7"/>
@@ -7248,7 +7251,7 @@
         <v>0</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G80" t="str">
         <f t="shared" si="7"/>
@@ -7298,7 +7301,7 @@
         <v>0</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G81" t="str">
         <f t="shared" si="7"/>
@@ -7348,7 +7351,7 @@
         <v>0</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="G82" t="str">
         <f t="shared" si="7"/>
@@ -7402,7 +7405,7 @@
         <v>0</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G83" t="str">
         <f t="shared" si="7"/>
@@ -7461,7 +7464,7 @@
         <v>0</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G84" t="str">
         <f t="shared" si="7"/>
@@ -7514,7 +7517,7 @@
         <v>0</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G85" t="str">
         <f t="shared" si="7"/>
@@ -7540,7 +7543,7 @@
         <v>51</v>
       </c>
       <c r="X85" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="Y85" t="str">
         <f>"support searching for all "&amp;LOWER(B85)&amp;"s for a patient"</f>
@@ -7629,7 +7632,7 @@
         <v>0</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G87" t="str">
         <f t="shared" si="7"/>
@@ -7673,7 +7676,7 @@
         <v>240</v>
       </c>
       <c r="C88" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D88" t="s">
         <v>64</v>
@@ -7682,7 +7685,7 @@
         <v>0</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G88" t="str">
         <f t="shared" si="7"/>
@@ -7711,7 +7714,7 @@
         <v>51</v>
       </c>
       <c r="Y88" s="4" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="Z88" s="4" t="str">
         <f>"GET [base]/"&amp;B88&amp;"?"&amp;C88&amp;"=http://snomed.info/sct\|17561000"</f>
@@ -7740,7 +7743,7 @@
         <v>1</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G89" t="str">
         <f t="shared" si="7"/>
@@ -7799,7 +7802,7 @@
         <v>0</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G90" t="str">
         <f t="shared" si="7"/>
@@ -7848,7 +7851,7 @@
         <v>0</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G91" t="str">
         <f t="shared" si="7"/>
@@ -8507,7 +8510,7 @@
         <v>1</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G103" t="str">
         <f t="shared" si="7"/>
@@ -8565,7 +8568,7 @@
         <v>1</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G104" t="str">
         <f t="shared" si="7"/>
@@ -8626,7 +8629,7 @@
         <v>1</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G105" t="str">
         <f t="shared" si="7"/>
@@ -8678,7 +8681,7 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C106" t="s">
         <v>56</v>
@@ -8690,7 +8693,7 @@
         <v>0</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G106" t="str">
         <f t="shared" si="7"/>
@@ -8731,7 +8734,7 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C107" t="s">
         <v>84</v>
@@ -8743,7 +8746,7 @@
         <v>1</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G107" t="str">
         <f t="shared" si="7"/>
@@ -8790,7 +8793,7 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C108" t="s">
         <v>134</v>
@@ -8802,7 +8805,7 @@
         <v>0</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G108" t="str">
         <f t="shared" si="7"/>
@@ -8840,7 +8843,7 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C109" t="s">
         <v>24</v>
@@ -8852,7 +8855,7 @@
         <v>0</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G109" t="str">
         <f t="shared" si="7"/>
@@ -8893,10 +8896,10 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C110" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D110" t="s">
         <v>28</v>
@@ -8905,7 +8908,7 @@
         <v>0</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="G110" t="str">
         <f t="shared" si="7"/>
@@ -8947,7 +8950,7 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C111" t="s">
         <v>50</v>
@@ -8982,10 +8985,10 @@
         <v>51</v>
       </c>
       <c r="Y111" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="Z111" s="4" t="s">
         <v>548</v>
-      </c>
-      <c r="Z111" s="4" t="s">
-        <v>549</v>
       </c>
       <c r="AB111" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B111)&amp;"-"&amp;SUBSTITUTE(C111,"_","")&amp;".html")</f>
@@ -9043,7 +9046,7 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C113" t="s">
         <v>50</v>
@@ -9078,10 +9081,10 @@
         <v>51</v>
       </c>
       <c r="Y113" s="4" t="s">
+        <v>549</v>
+      </c>
+      <c r="Z113" s="4" t="s">
         <v>550</v>
-      </c>
-      <c r="Z113" s="4" t="s">
-        <v>551</v>
       </c>
       <c r="AA113" s="8"/>
       <c r="AB113" t="str">
@@ -9094,7 +9097,7 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C114" t="s">
         <v>84</v>
@@ -9106,7 +9109,7 @@
         <v>1</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G114" t="str">
         <f t="shared" si="7"/>
@@ -9153,7 +9156,7 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C115" t="s">
         <v>21</v>
@@ -9191,7 +9194,7 @@
         <v>51</v>
       </c>
       <c r="Y115" s="4" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="Z115" s="4" t="str">
         <f>"GET [base]/"&amp;B115&amp;"?"&amp;C115&amp;"=Mary Shaw"</f>
@@ -9211,7 +9214,7 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C116" t="s">
         <v>50</v>
@@ -9250,7 +9253,7 @@
         <v>support fetching a QuestionnaireResponse</v>
       </c>
       <c r="Z116" s="4" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="AB116" t="str">
         <f t="shared" si="9"/>
@@ -9262,7 +9265,7 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C117" t="s">
         <v>84</v>
@@ -9274,7 +9277,7 @@
         <v>1</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G117" t="str">
         <f t="shared" si="7"/>
@@ -9321,7 +9324,7 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C118" t="s">
         <v>56</v>
@@ -9333,7 +9336,7 @@
         <v>0</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G118" t="str">
         <f t="shared" si="7"/>
@@ -9362,7 +9365,7 @@
         <v>51</v>
       </c>
       <c r="Y118" s="19" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="AB118" t="str">
         <f t="shared" si="9"/>
@@ -9374,10 +9377,10 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C119" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="D119" t="s">
         <v>28</v>
@@ -9386,7 +9389,7 @@
         <v>0</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G119" t="str">
         <f t="shared" si="7"/>
@@ -9402,16 +9405,16 @@
         <v>52</v>
       </c>
       <c r="L119" t="s">
+        <v>672</v>
+      </c>
+      <c r="M119" t="s">
+        <v>51</v>
+      </c>
+      <c r="O119" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y119" s="19" t="s">
         <v>673</v>
-      </c>
-      <c r="M119" t="s">
-        <v>51</v>
-      </c>
-      <c r="O119" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y119" s="19" t="s">
-        <v>674</v>
       </c>
       <c r="AB119" t="str">
         <f t="shared" si="9"/>
@@ -9423,10 +9426,10 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C120" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D120" t="s">
         <v>28</v>
@@ -9435,7 +9438,7 @@
         <v>0</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="G120" t="str">
         <f t="shared" si="7"/>
@@ -9467,7 +9470,7 @@
         <v>87</v>
       </c>
       <c r="Y120" s="19" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="AB120" t="str">
         <f t="shared" si="9"/>
@@ -9479,10 +9482,10 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C121" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="D121" t="s">
         <v>28</v>
@@ -9491,7 +9494,7 @@
         <v>0</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G121" t="str">
         <f t="shared" si="7"/>
@@ -9517,7 +9520,7 @@
         <v>51</v>
       </c>
       <c r="Y121" s="19" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="AB121" t="str">
         <f t="shared" si="9"/>
@@ -9529,7 +9532,7 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C122" t="s">
         <v>84</v>
@@ -9541,7 +9544,7 @@
         <v>1</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G122" t="str">
         <f t="shared" si="7"/>
@@ -9570,7 +9573,7 @@
         <v>51</v>
       </c>
       <c r="Y122" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="Z122" s="4" t="str">
         <f>"GET [base]/"&amp;B122&amp;"?patient=1137192"</f>
@@ -9590,7 +9593,7 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C123" t="s">
         <v>56</v>
@@ -9602,7 +9605,7 @@
         <v>0</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G123" t="str">
         <f t="shared" si="7"/>
@@ -9646,7 +9649,7 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C124" t="s">
         <v>12</v>
@@ -9658,7 +9661,7 @@
         <v>0</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G124" t="str">
         <f t="shared" si="7"/>
@@ -9702,7 +9705,7 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C125" t="s">
         <v>84</v>
@@ -9714,7 +9717,7 @@
         <v>1</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G125" t="str">
         <f t="shared" si="7"/>
@@ -9743,10 +9746,10 @@
         <v>51</v>
       </c>
       <c r="X125" s="6" t="s">
+        <v>642</v>
+      </c>
+      <c r="Z125" s="8" t="s">
         <v>643</v>
-      </c>
-      <c r="Z125" s="8" t="s">
-        <v>644</v>
       </c>
       <c r="AA125" s="8" t="str">
         <f>"Fetches a bundle of all "&amp;B125&amp; " resources for the specified patient."</f>
@@ -9762,10 +9765,10 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
+        <v>644</v>
+      </c>
+      <c r="C126" t="s">
         <v>645</v>
-      </c>
-      <c r="C126" t="s">
-        <v>646</v>
       </c>
       <c r="D126" t="s">
         <v>28</v>
@@ -9774,7 +9777,7 @@
         <v>0</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="G126" t="str">
         <f t="shared" si="7"/>
@@ -9863,7 +9866,7 @@
         <v>90</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>91</v>
@@ -10193,7 +10196,7 @@
         <v>288</v>
       </c>
       <c r="J13" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="K13" s="4" t="str">
         <f t="shared" si="1"/>
@@ -10293,7 +10296,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D17" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="F17" t="s">
         <v>64</v>
@@ -10305,7 +10308,7 @@
         <v>289</v>
       </c>
       <c r="J17" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="K17" s="4" t="str">
         <f t="shared" si="1"/>
@@ -10381,7 +10384,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D20" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="F20" t="s">
         <v>64</v>
@@ -10393,7 +10396,7 @@
         <v>294</v>
       </c>
       <c r="J20" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="K20" s="4" t="str">
         <f t="shared" si="1"/>
@@ -10703,7 +10706,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D32" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="F32" t="s">
         <v>64</v>
@@ -10712,10 +10715,10 @@
         <v>128</v>
       </c>
       <c r="I32" s="4" t="s">
+        <v>647</v>
+      </c>
+      <c r="J32" s="4" t="s">
         <v>648</v>
-      </c>
-      <c r="J32" s="4" t="s">
-        <v>649</v>
       </c>
       <c r="K32" s="4" t="str">
         <f t="shared" si="1"/>
@@ -10845,7 +10848,7 @@
         <v>312</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
@@ -10875,7 +10878,7 @@
         <v>144</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="K37" s="4" t="s">
         <v>140</v>
@@ -10893,7 +10896,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D38" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F38" t="s">
         <v>64</v>
@@ -10905,10 +10908,10 @@
         <v>144</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
@@ -10965,7 +10968,7 @@
         <v>147</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="K40" s="4" t="s">
         <v>150</v>
@@ -10983,7 +10986,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D41" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="F41" t="s">
         <v>64</v>
@@ -10995,7 +10998,7 @@
         <v>147</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="K41" s="4" t="s">
         <v>150</v>
@@ -11013,7 +11016,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D42" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="F42" t="s">
         <v>64</v>
@@ -11025,7 +11028,7 @@
         <v>147</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="K42" s="4" t="s">
         <v>150</v>
@@ -11043,7 +11046,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D43" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="F43" t="s">
         <v>64</v>
@@ -11055,7 +11058,7 @@
         <v>147</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="K43" s="4" t="s">
         <v>150</v>
@@ -11115,7 +11118,7 @@
         <v>161</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="K45" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B45&amp;" resources for the specified "&amp;SUBSTITUTE(D45,","," and ")</f>
@@ -11161,7 +11164,7 @@
         <v>173</v>
       </c>
       <c r="C47" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="D47" t="s">
         <v>110</v>
@@ -11191,7 +11194,7 @@
         <v>173</v>
       </c>
       <c r="C48" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="D48" t="s">
         <v>139</v>
@@ -11224,7 +11227,7 @@
         <v>173</v>
       </c>
       <c r="C49" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="D49" t="s">
         <v>141</v>
@@ -11254,7 +11257,7 @@
         <v>173</v>
       </c>
       <c r="C50" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="D50" t="s">
         <v>188</v>
@@ -11272,7 +11275,7 @@
         <v>189</v>
       </c>
       <c r="J50" s="7" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="K50" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B50&amp;" resources for the specified patient and date and a category code = `LAB`"</f>
@@ -11287,7 +11290,7 @@
         <v>173</v>
       </c>
       <c r="C51" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="D51" t="s">
         <v>212</v>
@@ -11302,7 +11305,7 @@
         <v>218</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="K51" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B51&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
@@ -11392,16 +11395,16 @@
         <v>100</v>
       </c>
       <c r="H54" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="I54" s="4" t="s">
         <v>418</v>
       </c>
       <c r="J54" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="K54" s="4" t="s">
         <v>439</v>
-      </c>
-      <c r="K54" s="4" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
@@ -11425,16 +11428,16 @@
         <v>100</v>
       </c>
       <c r="H55" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="I55" s="4" t="s">
         <v>179</v>
       </c>
       <c r="J55" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="K55" s="4" t="s">
         <v>441</v>
-      </c>
-      <c r="K55" s="4" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
@@ -11458,16 +11461,16 @@
         <v>100</v>
       </c>
       <c r="H56" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="I56" s="4" t="s">
         <v>179</v>
       </c>
       <c r="J56" s="4" t="s">
+        <v>442</v>
+      </c>
+      <c r="K56" s="4" t="s">
         <v>443</v>
-      </c>
-      <c r="K56" s="4" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
@@ -11491,16 +11494,16 @@
         <v>211</v>
       </c>
       <c r="H57" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="I57" s="4" t="s">
         <v>222</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="K57" s="4" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
@@ -11650,7 +11653,7 @@
         <v>219</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="K62" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B62&amp;" resources for the specified patient and date and procedure code(s).  SHOULD support search by multiple codes."</f>
@@ -11665,7 +11668,7 @@
         <v>177</v>
       </c>
       <c r="C63" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D63" t="s">
         <v>229</v>
@@ -11697,7 +11700,7 @@
         <v>177</v>
       </c>
       <c r="C64" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D64" t="s">
         <v>139</v>
@@ -11730,7 +11733,7 @@
         <v>177</v>
       </c>
       <c r="C65" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D65" t="s">
         <v>141</v>
@@ -11760,7 +11763,7 @@
         <v>177</v>
       </c>
       <c r="C66" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D66" t="s">
         <v>188</v>
@@ -11778,7 +11781,7 @@
         <v>217</v>
       </c>
       <c r="J66" s="4" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="K66" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B66&amp;" resources for the specified patient and date and a category code = `laboratory`"</f>
@@ -11793,7 +11796,7 @@
         <v>177</v>
       </c>
       <c r="C67" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D67" t="s">
         <v>212</v>
@@ -11808,7 +11811,7 @@
         <v>215</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="K67" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B67&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
@@ -11823,7 +11826,7 @@
         <v>304</v>
       </c>
       <c r="C68" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D68" t="s">
         <v>110</v>
@@ -11904,7 +11907,7 @@
         <v>233</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="K70" s="4" t="s">
         <v>237</v>
@@ -11968,7 +11971,7 @@
         <v>232</v>
       </c>
       <c r="J72" s="4" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K72" s="4" t="s">
         <v>239</v>
@@ -11998,13 +12001,13 @@
         <v>295</v>
       </c>
       <c r="I73" s="4" t="s">
+        <v>564</v>
+      </c>
+      <c r="J73" s="4" t="s">
         <v>565</v>
       </c>
-      <c r="J73" s="4" t="s">
+      <c r="K73" s="8" t="s">
         <v>566</v>
-      </c>
-      <c r="K73" s="8" t="s">
-        <v>567</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
@@ -12127,7 +12130,7 @@
         <v>280</v>
       </c>
       <c r="J77" s="7" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="K77" s="4" t="s">
         <v>282</v>
@@ -12187,7 +12190,7 @@
         <v>285</v>
       </c>
       <c r="J79" s="4" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="K79" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B79&amp;" resources for the specified "&amp;SUBSTITUTE(D79,","," and ") &amp;". See the implementation notes above for how to access the actual document."</f>
@@ -12202,7 +12205,7 @@
         <v>241</v>
       </c>
       <c r="C80" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D80" t="s">
         <v>112</v>
@@ -12231,7 +12234,7 @@
         <v>241</v>
       </c>
       <c r="C81" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D81" t="s">
         <v>110</v>
@@ -12246,13 +12249,13 @@
         <v>100</v>
       </c>
       <c r="I81" s="4" t="s">
+        <v>651</v>
+      </c>
+      <c r="J81" s="4" t="s">
         <v>652</v>
       </c>
-      <c r="J81" s="4" t="s">
+      <c r="K81" s="4" t="s">
         <v>653</v>
-      </c>
-      <c r="K81" s="4" t="s">
-        <v>654</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
@@ -12267,7 +12270,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
       </c>
       <c r="D82" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="F82" t="s">
         <v>64</v>
@@ -12276,13 +12279,13 @@
         <v>100</v>
       </c>
       <c r="I82" s="4" t="s">
+        <v>568</v>
+      </c>
+      <c r="J82" s="4" t="s">
         <v>569</v>
       </c>
-      <c r="J82" s="4" t="s">
+      <c r="K82" s="4" t="s">
         <v>570</v>
-      </c>
-      <c r="K82" s="4" t="s">
-        <v>571</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
@@ -12290,7 +12293,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C83" t="str">
         <f t="shared" ref="C83:C96" si="4">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B83)</f>
@@ -12309,7 +12312,7 @@
         <v>287</v>
       </c>
       <c r="J83" s="4" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="K83" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B83&amp;" resources for the specified "&amp;SUBSTITUTE(D83,","," and ")</f>
@@ -12321,7 +12324,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C84" t="str">
         <f t="shared" si="4"/>
@@ -12340,7 +12343,7 @@
         <v>192</v>
       </c>
       <c r="J84" s="4" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="K84" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B84&amp;" resources for the specified patient and  a category code"</f>
@@ -12352,7 +12355,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C85" t="str">
         <f t="shared" si="4"/>
@@ -12371,7 +12374,7 @@
         <v>193</v>
       </c>
       <c r="J85" s="4" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="K85" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B85&amp;" resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes."</f>
@@ -12383,14 +12386,14 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C86" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D86" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="F86" t="s">
         <v>11</v>
@@ -12402,7 +12405,7 @@
         <v>195</v>
       </c>
       <c r="J86" s="4" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="K86" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B86&amp;" resources for the specified patient and date and a category code"</f>
@@ -12414,14 +12417,14 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C87" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D87" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="F87" t="s">
         <v>64</v>
@@ -12430,10 +12433,10 @@
         <v>211</v>
       </c>
       <c r="I87" s="4" t="s">
+        <v>577</v>
+      </c>
+      <c r="J87" s="4" t="s">
         <v>578</v>
-      </c>
-      <c r="J87" s="4" t="s">
-        <v>579</v>
       </c>
       <c r="K87" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B87&amp;" resources for the specified patient and date and service code(s).  SHOULD support search by multiple report codes."</f>
@@ -12452,7 +12455,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D88" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="F88" t="s">
         <v>64</v>
@@ -12461,10 +12464,10 @@
         <v>100</v>
       </c>
       <c r="I88" s="4" t="s">
+        <v>580</v>
+      </c>
+      <c r="J88" s="4" t="s">
         <v>581</v>
-      </c>
-      <c r="J88" s="4" t="s">
-        <v>582</v>
       </c>
       <c r="K88" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B88&amp;" resources for the specified "&amp;SUBSTITUTE(D88,","," and ")</f>
@@ -12476,7 +12479,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C89" t="str">
         <f t="shared" si="4"/>
@@ -12492,10 +12495,10 @@
         <v>100</v>
       </c>
       <c r="I89" t="s">
+        <v>605</v>
+      </c>
+      <c r="J89" s="4" t="s">
         <v>606</v>
-      </c>
-      <c r="J89" s="4" t="s">
-        <v>607</v>
       </c>
       <c r="K89" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B89&amp;" resources for the specified "&amp;SUBSTITUTE(D89,","," and ")</f>
@@ -12507,14 +12510,14 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C90" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D90" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="F90" t="s">
         <v>64</v>
@@ -12523,13 +12526,13 @@
         <v>100</v>
       </c>
       <c r="H90" t="s">
+        <v>608</v>
+      </c>
+      <c r="I90" t="s">
+        <v>605</v>
+      </c>
+      <c r="J90" s="4" t="s">
         <v>609</v>
-      </c>
-      <c r="I90" t="s">
-        <v>606</v>
-      </c>
-      <c r="J90" s="4" t="s">
-        <v>610</v>
       </c>
       <c r="K90" t="str">
         <f>"Fetches a bundle of all "&amp;B90&amp;" resources for the specified "&amp;SUBSTITUTE(D90,","," and  ") &amp; "= 'sdoh'"</f>
@@ -12541,14 +12544,14 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C91" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D91" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="F91" t="s">
         <v>64</v>
@@ -12557,10 +12560,10 @@
         <v>143</v>
       </c>
       <c r="I91" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="J91" s="4" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="K91" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B91&amp;" resources for the specified patient and date"</f>
@@ -12572,14 +12575,14 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C92" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D92" s="16" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="F92" t="s">
         <v>64</v>
@@ -12588,13 +12591,13 @@
         <v>211</v>
       </c>
       <c r="H92" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="I92" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="J92" s="4" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="K92" t="str">
         <f>"Fetches a bundle of all "&amp;B92&amp;" resources tagged as 'sdoh' for the specified patient and date"</f>
@@ -12606,14 +12609,14 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C93" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D93" s="16" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F93" t="s">
         <v>64</v>
@@ -12622,10 +12625,10 @@
         <v>85</v>
       </c>
       <c r="I93" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="J93" s="4" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="K93" t="str">
         <f>"Fetches a bundle of all "&amp;B93&amp;" resources for the specified patient that have been completed against a specified form."</f>
@@ -12637,7 +12640,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="16" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C94" t="str">
         <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B94)</f>
@@ -12657,10 +12660,10 @@
       </c>
       <c r="H94" s="16"/>
       <c r="I94" s="4" t="s">
+        <v>654</v>
+      </c>
+      <c r="J94" s="4" t="s">
         <v>655</v>
-      </c>
-      <c r="J94" s="4" t="s">
-        <v>656</v>
       </c>
       <c r="K94" t="str">
         <f>"Fetches a bundle of all "&amp;B94&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed))."</f>
@@ -12672,7 +12675,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="16" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C95" t="str">
         <f t="shared" si="4"/>
@@ -12692,10 +12695,10 @@
       </c>
       <c r="H95" s="16"/>
       <c r="I95" s="4" t="s">
+        <v>656</v>
+      </c>
+      <c r="J95" s="4" t="s">
         <v>657</v>
-      </c>
-      <c r="J95" s="4" t="s">
-        <v>658</v>
       </c>
       <c r="K95" t="str">
         <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed) and type of dispense (e.g., partially dispensed)."</f>
@@ -12707,14 +12710,14 @@
         <v>95</v>
       </c>
       <c r="B96" s="16" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="C96" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationdispense</v>
       </c>
       <c r="D96" s="16" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="E96" s="16" t="s">
         <v>51</v>
@@ -12727,10 +12730,10 @@
       </c>
       <c r="H96" s="16"/>
       <c r="I96" s="4" t="s">
+        <v>659</v>
+      </c>
+      <c r="J96" s="4" t="s">
         <v>660</v>
-      </c>
-      <c r="J96" s="4" t="s">
-        <v>661</v>
       </c>
       <c r="K96" t="str">
         <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient for a given dispense and date or range"</f>
@@ -12777,15 +12780,15 @@
         <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B3" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -12801,7 +12804,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -12817,7 +12820,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -12825,36 +12828,36 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>502</v>
+      </c>
+      <c r="B9" t="s">
         <v>503</v>
-      </c>
-      <c r="B9" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>504</v>
+      </c>
+      <c r="B10" t="s">
         <v>505</v>
-      </c>
-      <c r="B10" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>506</v>
+      </c>
+      <c r="B11" s="14" t="s">
         <v>507</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>508</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B12" t="s">
         <v>64</v>
@@ -12884,7 +12887,7 @@
         <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C1" t="s">
         <v>54</v>
@@ -12895,13 +12898,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="D2" t="s">
         <v>64</v>
@@ -12909,13 +12912,13 @@
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B3" s="21" t="s">
+        <v>520</v>
+      </c>
+      <c r="C3" s="21" t="s">
         <v>521</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>522</v>
       </c>
       <c r="D3" s="21" t="s">
         <v>64</v>
@@ -12948,16 +12951,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>511</v>
+      </c>
+      <c r="B1" t="s">
         <v>512</v>
-      </c>
-      <c r="B1" t="s">
-        <v>513</v>
       </c>
       <c r="C1" t="s">
         <v>21</v>
       </c>
       <c r="D1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E1" t="s">
         <v>54</v>
@@ -12971,13 +12974,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>513</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>514</v>
       </c>
-      <c r="D2" s="15" t="s">
-        <v>515</v>
-      </c>
       <c r="E2" s="15" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -13066,10 +13069,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B5" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
@@ -13080,10 +13083,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B6" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -13094,16 +13097,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>676</v>
+      </c>
+      <c r="B7" t="s">
         <v>677</v>
       </c>
-      <c r="B7" t="s">
-        <v>678</v>
-      </c>
       <c r="D7" t="s">
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -13164,7 +13167,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B12" t="s">
         <v>347</v>
@@ -13178,86 +13181,86 @@
     </row>
     <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
+        <v>585</v>
+      </c>
+      <c r="B13" t="s">
         <v>586</v>
       </c>
-      <c r="B13" t="s">
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
         <v>587</v>
-      </c>
-      <c r="D13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
+        <v>588</v>
+      </c>
+      <c r="B14" t="s">
         <v>589</v>
       </c>
-      <c r="B14" t="s">
-        <v>590</v>
-      </c>
       <c r="D14" t="s">
         <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
+        <v>590</v>
+      </c>
+      <c r="B15" t="s">
         <v>591</v>
       </c>
-      <c r="B15" t="s">
-        <v>592</v>
-      </c>
       <c r="D15" t="s">
         <v>11</v>
       </c>
       <c r="E15" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
+        <v>592</v>
+      </c>
+      <c r="B16" t="s">
         <v>593</v>
       </c>
-      <c r="B16" t="s">
-        <v>594</v>
-      </c>
       <c r="D16" t="s">
         <v>11</v>
       </c>
       <c r="E16" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
+        <v>594</v>
+      </c>
+      <c r="B17" t="s">
         <v>595</v>
       </c>
-      <c r="B17" t="s">
-        <v>596</v>
-      </c>
       <c r="D17" t="s">
         <v>11</v>
       </c>
       <c r="E17" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B18" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D18" t="s">
         <v>11</v>
       </c>
       <c r="E18" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -13332,16 +13335,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>678</v>
+      </c>
+      <c r="B24" t="s">
         <v>679</v>
       </c>
-      <c r="B24" t="s">
-        <v>680</v>
-      </c>
       <c r="D24" t="s">
         <v>11</v>
       </c>
       <c r="E24" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -13360,10 +13363,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>680</v>
+      </c>
+      <c r="B26" t="s">
         <v>681</v>
-      </c>
-      <c r="B26" t="s">
-        <v>682</v>
       </c>
       <c r="D26" t="s">
         <v>11</v>
@@ -13374,10 +13377,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>682</v>
+      </c>
+      <c r="B27" t="s">
         <v>683</v>
-      </c>
-      <c r="B27" t="s">
-        <v>684</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
@@ -13388,10 +13391,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>684</v>
+      </c>
+      <c r="B28" t="s">
         <v>685</v>
-      </c>
-      <c r="B28" t="s">
-        <v>686</v>
       </c>
       <c r="D28" t="s">
         <v>11</v>
@@ -13402,10 +13405,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="18" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B29" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="D29" t="s">
         <v>11</v>
@@ -13416,10 +13419,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="18" t="s">
+        <v>471</v>
+      </c>
+      <c r="B30" t="s">
         <v>472</v>
-      </c>
-      <c r="B30" t="s">
-        <v>473</v>
       </c>
       <c r="D30" t="s">
         <v>11</v>
@@ -13430,10 +13433,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B31" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="D31" t="s">
         <v>11</v>
@@ -13444,10 +13447,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="18" t="s">
+        <v>469</v>
+      </c>
+      <c r="B32" t="s">
         <v>470</v>
-      </c>
-      <c r="B32" t="s">
-        <v>471</v>
       </c>
       <c r="D32" t="s">
         <v>11</v>
@@ -13458,10 +13461,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="18" t="s">
+        <v>467</v>
+      </c>
+      <c r="B33" t="s">
         <v>468</v>
-      </c>
-      <c r="B33" t="s">
-        <v>469</v>
       </c>
       <c r="D33" t="s">
         <v>11</v>
@@ -13472,10 +13475,10 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="18" t="s">
+        <v>483</v>
+      </c>
+      <c r="B34" t="s">
         <v>484</v>
-      </c>
-      <c r="B34" t="s">
-        <v>485</v>
       </c>
       <c r="D34" t="s">
         <v>11</v>
@@ -13514,10 +13517,10 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="18" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B37" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="D37" t="s">
         <v>11</v>
@@ -13528,10 +13531,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="18" t="s">
+        <v>461</v>
+      </c>
+      <c r="B38" t="s">
         <v>462</v>
-      </c>
-      <c r="B38" t="s">
-        <v>463</v>
       </c>
       <c r="D38" t="s">
         <v>11</v>
@@ -13542,10 +13545,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="18" t="s">
+        <v>463</v>
+      </c>
+      <c r="B39" t="s">
         <v>464</v>
-      </c>
-      <c r="B39" t="s">
-        <v>465</v>
       </c>
       <c r="D39" t="s">
         <v>11</v>
@@ -13556,10 +13559,10 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="18" t="s">
+        <v>459</v>
+      </c>
+      <c r="B40" t="s">
         <v>460</v>
-      </c>
-      <c r="B40" t="s">
-        <v>461</v>
       </c>
       <c r="D40" t="s">
         <v>11</v>
@@ -13570,10 +13573,10 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="B41" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="D41" t="s">
         <v>11</v>
@@ -13584,10 +13587,10 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="18" t="s">
+        <v>457</v>
+      </c>
+      <c r="B42" t="s">
         <v>458</v>
-      </c>
-      <c r="B42" t="s">
-        <v>459</v>
       </c>
       <c r="D42" t="s">
         <v>11</v>
@@ -13598,10 +13601,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="18" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B43" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D43" t="s">
         <v>11</v>
@@ -13612,10 +13615,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B44" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="D44" t="s">
         <v>11</v>
@@ -13626,10 +13629,10 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="18" t="s">
+        <v>481</v>
+      </c>
+      <c r="B45" t="s">
         <v>482</v>
-      </c>
-      <c r="B45" t="s">
-        <v>483</v>
       </c>
       <c r="D45" t="s">
         <v>11</v>
@@ -13640,10 +13643,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="18" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B46" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="D46" t="s">
         <v>11</v>
@@ -13654,10 +13657,10 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="18" t="s">
+        <v>465</v>
+      </c>
+      <c r="B47" t="s">
         <v>466</v>
-      </c>
-      <c r="B47" t="s">
-        <v>467</v>
       </c>
       <c r="D47" t="s">
         <v>11</v>
@@ -13668,10 +13671,10 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="18" t="s">
+        <v>455</v>
+      </c>
+      <c r="B48" t="s">
         <v>456</v>
-      </c>
-      <c r="B48" t="s">
-        <v>457</v>
       </c>
       <c r="D48" t="s">
         <v>11</v>
@@ -13766,72 +13769,72 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B55" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="D55" t="s">
         <v>11</v>
       </c>
       <c r="E55" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B56" t="s">
+        <v>600</v>
+      </c>
+      <c r="D56" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" t="s">
         <v>601</v>
-      </c>
-      <c r="D56" t="s">
-        <v>11</v>
-      </c>
-      <c r="E56" t="s">
-        <v>602</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="18" t="s">
+        <v>526</v>
+      </c>
+      <c r="B57" t="s">
         <v>527</v>
       </c>
-      <c r="B57" t="s">
+      <c r="D57" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57" t="s">
         <v>528</v>
-      </c>
-      <c r="D57" t="s">
-        <v>11</v>
-      </c>
-      <c r="E57" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="18" t="s">
+        <v>529</v>
+      </c>
+      <c r="B58" t="s">
         <v>530</v>
       </c>
-      <c r="B58" t="s">
+      <c r="D58" t="s">
+        <v>11</v>
+      </c>
+      <c r="E58" t="s">
         <v>531</v>
-      </c>
-      <c r="D58" t="s">
-        <v>11</v>
-      </c>
-      <c r="E58" t="s">
-        <v>532</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="18" t="s">
+        <v>690</v>
+      </c>
+      <c r="B59" t="s">
         <v>691</v>
       </c>
-      <c r="B59" t="s">
+      <c r="D59" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59" t="s">
         <v>692</v>
-      </c>
-      <c r="D59" t="s">
-        <v>11</v>
-      </c>
-      <c r="E59" t="s">
-        <v>693</v>
       </c>
     </row>
   </sheetData>
@@ -13862,7 +13865,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Y63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -13899,7 +13902,7 @@
         <v>37</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="F1" t="s">
         <v>14</v>
@@ -13950,16 +13953,16 @@
         <v>387</v>
       </c>
       <c r="V1" s="3" t="s">
+        <v>515</v>
+      </c>
+      <c r="W1" s="3" t="s">
         <v>516</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>517</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>518</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="23" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -13973,7 +13976,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="X2" s="13" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="Y2" s="13" t="s">
         <v>64</v>
@@ -13987,10 +13990,10 @@
         <v>64</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="X3" s="13" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="Y3" s="13" t="s">
         <v>64</v>
@@ -14004,16 +14007,16 @@
         <v>64</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="V4" t="s">
+        <v>532</v>
+      </c>
+      <c r="W4" t="s">
         <v>533</v>
       </c>
-      <c r="W4" t="s">
-        <v>534</v>
-      </c>
       <c r="X4" s="13" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="Y4" s="13" t="s">
         <v>64</v>
@@ -14027,10 +14030,10 @@
         <v>64</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="X5" s="13" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="Y5" s="13" t="s">
         <v>64</v>
@@ -14044,10 +14047,10 @@
         <v>64</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="X6" s="13" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="Y6" s="13" t="s">
         <v>64</v>
@@ -14062,7 +14065,7 @@
       </c>
       <c r="C7" s="2"/>
       <c r="X7" s="13" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="Y7" s="13" t="s">
         <v>64</v>
@@ -14076,10 +14079,10 @@
         <v>64</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="X8" s="13" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="Y8" s="13" t="s">
         <v>64</v>
@@ -14093,10 +14096,10 @@
         <v>64</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="X9" s="13" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="Y9" s="13" t="s">
         <v>64</v>
@@ -14110,10 +14113,10 @@
         <v>64</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="X10" s="13" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="Y10" s="13" t="s">
         <v>64</v>
@@ -14127,10 +14130,10 @@
         <v>64</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="X11" s="13" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="Y11" s="13" t="s">
         <v>64</v>
@@ -14144,7 +14147,7 @@
         <v>64</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="X12" s="13"/>
       <c r="Y12" s="13"/>
@@ -14157,7 +14160,7 @@
         <v>64</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="X13" s="13"/>
       <c r="Y13" s="13"/>
@@ -14170,7 +14173,7 @@
         <v>64</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="V14" t="s">
         <v>64</v>
@@ -14179,7 +14182,7 @@
         <v>201</v>
       </c>
       <c r="X14" s="13" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="Y14" s="13" t="s">
         <v>64</v>
@@ -14193,7 +14196,7 @@
         <v>64</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="V15" t="s">
         <v>64</v>
@@ -14202,7 +14205,7 @@
         <v>377</v>
       </c>
       <c r="X15" s="13" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="Y15" s="13" t="s">
         <v>64</v>
@@ -14216,10 +14219,10 @@
         <v>64</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="X16" s="13" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="Y16" s="13" t="s">
         <v>64</v>
@@ -14233,7 +14236,7 @@
         <v>64</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="X17" s="13"/>
       <c r="Y17" s="13"/>
@@ -14246,10 +14249,10 @@
         <v>64</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="X18" s="13" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="Y18" s="13" t="s">
         <v>64</v>
@@ -14263,7 +14266,7 @@
         <v>64</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="X19" s="13"/>
       <c r="Y19" s="13"/>
@@ -14276,10 +14279,10 @@
         <v>64</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="V20" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="W20" t="s">
         <v>265</v>
@@ -14295,10 +14298,10 @@
         <v>64</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="X21" s="13" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="Y21" s="13" t="s">
         <v>64</v>
@@ -14312,34 +14315,34 @@
         <v>64</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="23" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B23" t="s">
         <v>64</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="X23" s="13"/>
       <c r="Y23" s="13"/>
     </row>
     <row r="24" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B24" t="s">
         <v>64</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="X24" s="13" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="Y24" s="13" t="s">
         <v>64</v>
@@ -14347,13 +14350,13 @@
     </row>
     <row r="25" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B25" t="s">
         <v>64</v>
       </c>
       <c r="X25" s="13" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="Y25" s="13" t="s">
         <v>64</v>
@@ -14361,13 +14364,13 @@
     </row>
     <row r="26" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B26" t="s">
         <v>64</v>
       </c>
       <c r="X26" s="13" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="Y26" s="13" t="s">
         <v>64</v>
@@ -14407,8 +14410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14455,10 +14458,10 @@
     </row>
     <row r="3" spans="1:5" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>430</v>
+      </c>
+      <c r="B3" t="s">
         <v>431</v>
-      </c>
-      <c r="B3" t="s">
-        <v>432</v>
       </c>
       <c r="C3" t="s">
         <v>429</v>
@@ -14466,8 +14469,8 @@
       <c r="D3" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>430</v>
+      <c r="E3" s="24" t="s">
+        <v>706</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -14550,7 +14553,7 @@
         <v>364</v>
       </c>
       <c r="R1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="S1" t="s">
         <v>365</v>
@@ -14571,19 +14574,19 @@
         <v>416</v>
       </c>
       <c r="Y1" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="Z1" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="AA1" t="s">
+        <v>534</v>
+      </c>
+      <c r="AB1" t="s">
         <v>535</v>
       </c>
-      <c r="AB1" t="s">
-        <v>536</v>
-      </c>
       <c r="AC1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add _include guidance for Specimen [FHIR-40180], Make Specimen.subject must support [FHIR-40136]
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F196065A-1344-0C49-8BD7-468C5072FC9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947654B0-C7EC-B34F-B74D-491A90A4800A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -121,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2589" uniqueCount="707">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2608" uniqueCount="709">
   <si>
     <t>Element</t>
   </si>
@@ -2341,6 +2341,12 @@
   </si>
   <si>
     <t>If a server supports DocumentReference for creating, using, and sharing clinical notes, it **SHOULD** also support the `context` and `contextdirection` parameters of the $expand operation to enable clients to determine the supported note and report types, as well as the supported read/write formats for notes on the server.</t>
+  </si>
+  <si>
+    <t>support fetching a Specimen</t>
+  </si>
+  <si>
+    <t>!QuestionnaireResponse</t>
   </si>
 </sst>
 </file>
@@ -2543,7 +2549,17 @@
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3042,13 +3058,13 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B00118F-F6B9-6642-9BD4-D95AE82A4925}">
-  <dimension ref="A1:AB126"/>
+  <dimension ref="A1:AB128"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C96" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F104" sqref="F104"/>
+      <selection pane="bottomRight" activeCell="A128" sqref="A128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6497,7 +6513,7 @@
         <v>485</v>
       </c>
       <c r="G66" t="str">
-        <f t="shared" ref="G66:G126" si="7">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B66)</f>
+        <f t="shared" ref="G66:G128" si="7">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B66)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="H66" t="s">
@@ -9454,7 +9470,7 @@
         <v>73</v>
       </c>
       <c r="L120" t="str">
-        <f t="shared" ref="L120:L126" si="10">B120&amp;"."&amp;C120</f>
+        <f t="shared" ref="L120:L128" si="10">B120&amp;"."&amp;C120</f>
         <v>QuestionnaireResponse.authored</v>
       </c>
       <c r="M120" t="s">
@@ -9817,11 +9833,129 @@
         <v>SearchParameter-us-core-!medicationdispense-whenhandedover.html</v>
       </c>
     </row>
+    <row r="127" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>126</v>
+      </c>
+      <c r="B127" t="s">
+        <v>692</v>
+      </c>
+      <c r="C127" t="s">
+        <v>50</v>
+      </c>
+      <c r="D127" t="s">
+        <v>11</v>
+      </c>
+      <c r="E127" t="b">
+        <v>1</v>
+      </c>
+      <c r="G127" t="str">
+        <f t="shared" si="7"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-specimen</v>
+      </c>
+      <c r="H127" t="s">
+        <v>51</v>
+      </c>
+      <c r="I127" t="s">
+        <v>51</v>
+      </c>
+      <c r="J127" t="s">
+        <v>51</v>
+      </c>
+      <c r="K127" t="s">
+        <v>52</v>
+      </c>
+      <c r="L127" t="str">
+        <f t="shared" si="10"/>
+        <v>Specimen._id</v>
+      </c>
+      <c r="M127" t="s">
+        <v>51</v>
+      </c>
+      <c r="O127" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y127" s="4" t="s">
+        <v>707</v>
+      </c>
+      <c r="Z127" s="4" t="str">
+        <f>"GET [base]/"&amp;B127&amp;"?"&amp;C127&amp;"=123"</f>
+        <v>GET [base]/Specimen?_id=123</v>
+      </c>
+      <c r="AB127" t="str">
+        <f>"SearchParameter-us-core-"&amp;LOWER((B127)&amp;"-"&amp;C127&amp;".html")</f>
+        <v>SearchParameter-us-core-specimen-_id.html</v>
+      </c>
+    </row>
+    <row r="128" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>127</v>
+      </c>
+      <c r="B128" t="s">
+        <v>692</v>
+      </c>
+      <c r="C128" t="s">
+        <v>84</v>
+      </c>
+      <c r="D128" t="s">
+        <v>64</v>
+      </c>
+      <c r="E128" t="b">
+        <v>1</v>
+      </c>
+      <c r="G128" t="str">
+        <f t="shared" si="7"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-specimen</v>
+      </c>
+      <c r="H128" t="s">
+        <v>51</v>
+      </c>
+      <c r="I128" t="s">
+        <v>51</v>
+      </c>
+      <c r="J128" t="s">
+        <v>51</v>
+      </c>
+      <c r="K128" t="s">
+        <v>85</v>
+      </c>
+      <c r="L128" t="str">
+        <f t="shared" si="10"/>
+        <v>Specimen.patient</v>
+      </c>
+      <c r="M128" t="s">
+        <v>51</v>
+      </c>
+      <c r="O128" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y128" t="str">
+        <f>"support searching for all "&amp;LOWER(B128)&amp;"s for a patient"</f>
+        <v>support searching for all specimens for a patient</v>
+      </c>
+      <c r="Z128" s="4" t="str">
+        <f>"GET [base]/"&amp;B128&amp;"?patient=1137192"</f>
+        <v>GET [base]/Specimen?patient=1137192</v>
+      </c>
+      <c r="AA128" s="8" t="str">
+        <f>"Fetches a bundle of all "&amp;B128&amp; " resources for the specified patient"</f>
+        <v>Fetches a bundle of all Specimen resources for the specified patient</v>
+      </c>
+      <c r="AB128" t="str">
+        <f>"SearchParameter-us-core-"&amp;LOWER((B128)&amp;"-"&amp;C128&amp;".html")</f>
+        <v>SearchParameter-us-core-specimen-patient.html</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:AB126" xr:uid="{1CF5B17E-E72E-48B2-A597-9C21C12723F0}"/>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="!">
+  <conditionalFormatting sqref="B1:B126 B129:B1048576">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",B1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B127:B128">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="!">
+      <formula>NOT(ISERROR(SEARCH("!",B127)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9834,8 +9968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E7AC33C-2643-EE4B-9487-6CC99572F031}">
   <dimension ref="A1:K96"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C94" sqref="C94"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12510,11 +12644,11 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>601</v>
+        <v>708</v>
       </c>
       <c r="C90" t="str">
         <f t="shared" si="4"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="D90" t="s">
         <v>607</v>
@@ -12536,7 +12670,7 @@
       </c>
       <c r="K90" t="str">
         <f>"Fetches a bundle of all "&amp;B90&amp;" resources for the specified "&amp;SUBSTITUTE(D90,","," and  ") &amp; "= 'sdoh'"</f>
-        <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient and  _tag= 'sdoh'</v>
+        <v>Fetches a bundle of all !QuestionnaireResponse resources for the specified patient and  _tag= 'sdoh'</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.2">
@@ -12575,11 +12709,11 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>601</v>
+        <v>708</v>
       </c>
       <c r="C92" t="str">
         <f t="shared" si="4"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="D92" s="16" t="s">
         <v>612</v>
@@ -12601,7 +12735,7 @@
       </c>
       <c r="K92" t="str">
         <f>"Fetches a bundle of all "&amp;B92&amp;" resources tagged as 'sdoh' for the specified patient and date"</f>
-        <v>Fetches a bundle of all QuestionnaireResponse resources tagged as 'sdoh' for the specified patient and date</v>
+        <v>Fetches a bundle of all !QuestionnaireResponse resources tagged as 'sdoh' for the specified patient and date</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.2">
@@ -12743,7 +12877,7 @@
   </sheetData>
   <autoFilter ref="A1:K96" xr:uid="{331E0B16-168F-459B-8951-3DF614BF0371}"/>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13839,17 +13973,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A9">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",A9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A55">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",A55)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14397,7 +14531,7 @@
     <sortCondition ref="A2:A21"/>
   </sortState>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14410,7 +14544,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Revert to simplegenderIdentify extension [FHIR-39615]
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947654B0-C7EC-B34F-B74D-491A90A4800A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8659270E-33BA-CA44-BA46-70B3897D80B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -3060,11 +3060,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B00118F-F6B9-6642-9BD4-D95AE82A4925}">
   <dimension ref="A1:AB128"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C96" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A128" sqref="A128"/>
+      <selection pane="bottomRight" activeCell="C135" sqref="C135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9393,7 +9393,7 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>601</v>
+        <v>708</v>
       </c>
       <c r="C119" t="s">
         <v>603</v>
@@ -9409,7 +9409,7 @@
       </c>
       <c r="G119" t="str">
         <f t="shared" si="7"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="H119" t="s">
         <v>51</v>
@@ -9434,7 +9434,7 @@
       </c>
       <c r="AB119" t="str">
         <f t="shared" si="9"/>
-        <v>SearchParameter-us-core-questionnaireresponse-tag.html</v>
+        <v>SearchParameter-us-core-!questionnaireresponse-tag.html</v>
       </c>
     </row>
     <row r="120" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -9968,8 +9968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E7AC33C-2643-EE4B-9487-6CC99572F031}">
   <dimension ref="A1:K96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B93" sqref="B93"/>
+    <sheetView topLeftCell="A64" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
**Applied:** Allow multiple NPIs for Organizations and Practitioners [FHIR-39382],Add support for Condition search that include patient + category + status [FHIR-39610]
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8659270E-33BA-CA44-BA46-70B3897D80B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A295B50E-38B6-1142-A3AE-BCB90E50E16C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -22,12 +22,12 @@
     <sheet name="ops" sheetId="5" r:id="rId7"/>
     <sheet name="interactions" sheetId="6" r:id="rId8"/>
     <sheet name="rest_interactions" sheetId="11" r:id="rId9"/>
-    <sheet name="sps" sheetId="20" r:id="rId10"/>
-    <sheet name="sp_combos" sheetId="22" r:id="rId11"/>
+    <sheet name="sps" sheetId="26" r:id="rId10"/>
+    <sheet name="sp_combos" sheetId="28" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">sp_combos!$A$1:$K$96</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">sps!$A$1:$AB$126</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">sp_combos!$A$1:$K$98</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">sps!$A$1:$AB$128</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,12 +49,12 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={F80C4D5F-754A-BE44-8144-8F9387CD5898}</author>
-    <author>tc={E78517F8-1EB7-C343-807E-3D9CF6C2C300}</author>
-    <author>tc={0694A05D-9B08-CE4F-A735-E8240B814808}</author>
+    <author>tc={224514F6-895E-1C49-9108-4433CDF530F9}</author>
+    <author>tc={F3437314-BB8A-B94D-9B51-75865A9CEDA0}</author>
+    <author>tc={8C6BA96D-1C82-F94D-8C98-FD6BB1BE52EF}</author>
   </authors>
   <commentList>
-    <comment ref="L40" authorId="0" shapeId="0" xr:uid="{F80C4D5F-754A-BE44-8144-8F9387CD5898}">
+    <comment ref="L40" authorId="0" shapeId="0" xr:uid="{224514F6-895E-1C49-9108-4433CDF530F9}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -62,7 +62,7 @@
     where does this show up?</t>
       </text>
     </comment>
-    <comment ref="Z44" authorId="1" shapeId="0" xr:uid="{E78517F8-1EB7-C343-807E-3D9CF6C2C300}">
+    <comment ref="Z44" authorId="1" shapeId="0" xr:uid="{F3437314-BB8A-B94D-9B51-75865A9CEDA0}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -70,7 +70,7 @@
     do i need this?</t>
       </text>
     </comment>
-    <comment ref="AA44" authorId="2" shapeId="0" xr:uid="{0694A05D-9B08-CE4F-A735-E8240B814808}">
+    <comment ref="AA44" authorId="2" shapeId="0" xr:uid="{8C6BA96D-1C82-F94D-8C98-FD6BB1BE52EF}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -85,12 +85,12 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={D123EF51-46F1-1341-AF16-81EA94978931}</author>
-    <author>tc={A157258E-CBF6-C345-9459-64FF9319F2BC}</author>
-    <author>tc={D311E409-D311-0C43-BC63-D68872BACEF4}</author>
+    <author>tc={2B2891A7-974D-E34F-88EF-DB827DB0B8CF}</author>
+    <author>tc={26C46AA4-A780-EA4D-9D86-8C9AF4A5553C}</author>
+    <author>tc={7ACCC7C3-24F8-B14F-A486-B9650B9C7D19}</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{D123EF51-46F1-1341-AF16-81EA94978931}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{2B2891A7-974D-E34F-88EF-DB827DB0B8CF}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -100,7 +100,7 @@
     make this a comma separate list of profiles</t>
       </text>
     </comment>
-    <comment ref="I1" authorId="1" shapeId="0" xr:uid="{A157258E-CBF6-C345-9459-64FF9319F2BC}">
+    <comment ref="I1" authorId="1" shapeId="0" xr:uid="{26C46AA4-A780-EA4D-9D86-8C9AF4A5553C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -108,7 +108,7 @@
     does this do anything if not delete row</t>
       </text>
     </comment>
-    <comment ref="I40" authorId="2" shapeId="0" xr:uid="{D311E409-D311-0C43-BC63-D68872BACEF4}">
+    <comment ref="I41" authorId="2" shapeId="0" xr:uid="{7ACCC7C3-24F8-B14F-A486-B9650B9C7D19}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -121,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2608" uniqueCount="709">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2608" uniqueCount="717">
   <si>
     <t>Element</t>
   </si>
@@ -2137,9 +2137,6 @@
   </si>
   <si>
     <t>GET [base]/Patient?family=Shaw&amp;death-date=2022-07-22</t>
-  </si>
-  <si>
-    <t>Implementation Notes: Fetches a bundle of all Condition resources for the specified patient and all "active" statuses (active,relapse,remission). This will *exclude* diagnoses and health concerns without a clinicalStatus specified.</t>
   </si>
   <si>
     <t>GET [base]/Condition?patient=1032702&amp;category=http://terminology.hl7.org/CodeSystem/condition-category\|encounter-diagnosis&amp;encounter=1036</t>
@@ -2348,12 +2345,59 @@
   <si>
     <t>!QuestionnaireResponse</t>
   </si>
+  <si>
+    <t>Fetches a bundle of all Condition resources for the specified patient and all "active" statuses (active,relapse,remission). This will *exclude* diagnoses and health concerns without a clinicalStatus specified.</t>
+  </si>
+  <si>
+    <t>patient,name</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>reference,string</t>
+  </si>
+  <si>
+    <t>GET [base]/RelatedPerson?patient=1137192&amp;name=van%20Putten</t>
+  </si>
+  <si>
+    <t>patient,category,clinical-status</t>
+  </si>
+  <si>
+    <t>support searching for all *active* problems or health concerns or  *active* encounter diagnosis for a patient</t>
+  </si>
+  <si>
+    <r>
+      <t>GET [</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>base</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>]/Condition?patient=1032702&amp;category=http://terminology.hl7.org/CodeSystem/condition-category\|problem-list-item&amp;clinical-status=http://terminology.hl7.org/CodeSystem/condition-clinical\|active,http://terminology.hl7.org/CodeSystem/condition-clinical\|recurrance,http://terminology.hl7.org/CodeSystem/condition-clinical\|remission</t>
+    </r>
+  </si>
+  <si>
+    <t>Fetches a bundle of all Condition resources for the specified patient and category for all "active" statuses (active,relapse,remission). This will *exclude* diagnoses and health concerns without a clinicalStatus specified.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2451,6 +2495,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFA31515"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -2504,7 +2566,7 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2542,6 +2604,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -2549,17 +2612,7 @@
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2936,13 +2989,13 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="L40" dT="2021-11-06T02:36:52.48" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{F80C4D5F-754A-BE44-8144-8F9387CD5898}">
+  <threadedComment ref="L40" dT="2021-11-06T02:36:52.48" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{224514F6-895E-1C49-9108-4433CDF530F9}">
     <text>where does this show up?</text>
   </threadedComment>
-  <threadedComment ref="Z44" dT="2021-11-06T02:39:25.62" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{E78517F8-1EB7-C343-807E-3D9CF6C2C300}">
+  <threadedComment ref="Z44" dT="2021-11-06T02:39:25.62" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{F3437314-BB8A-B94D-9B51-75865A9CEDA0}">
     <text>do i need this?</text>
   </threadedComment>
-  <threadedComment ref="AA44" dT="2021-11-06T02:40:08.93" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{0694A05D-9B08-CE4F-A735-E8240B814808}">
+  <threadedComment ref="AA44" dT="2021-11-06T02:40:08.93" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{8C6BA96D-1C82-F94D-8C98-FD6BB1BE52EF}">
     <text>do I need this?</text>
   </threadedComment>
 </ThreadedComments>
@@ -2950,16 +3003,16 @@
 
 <file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="C1" dT="2021-11-10T17:47:31.83" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{D123EF51-46F1-1341-AF16-81EA94978931}">
+  <threadedComment ref="C1" dT="2021-11-10T17:47:31.83" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{2B2891A7-974D-E34F-88EF-DB827DB0B8CF}">
     <text>add column for include file</text>
   </threadedComment>
-  <threadedComment ref="C1" dT="2021-11-10T17:48:52.85" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{CE8B7051-AD03-244E-85A2-5F2F1087AA1F}" parentId="{D123EF51-46F1-1341-AF16-81EA94978931}">
+  <threadedComment ref="C1" dT="2021-11-10T17:48:52.85" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{C50AFA52-937E-4941-BEDE-4A45C79B7720}" parentId="{2B2891A7-974D-E34F-88EF-DB827DB0B8CF}">
     <text>make this a comma separate list of profiles</text>
   </threadedComment>
-  <threadedComment ref="I1" dT="2021-11-08T19:54:50.37" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{A157258E-CBF6-C345-9459-64FF9319F2BC}">
+  <threadedComment ref="I1" dT="2021-11-08T19:54:50.37" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{26C46AA4-A780-EA4D-9D86-8C9AF4A5553C}">
     <text>does this do anything if not delete row</text>
   </threadedComment>
-  <threadedComment ref="I40" dT="2021-11-06T02:44:23.26" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{D311E409-D311-0C43-BC63-D68872BACEF4}">
+  <threadedComment ref="I41" dT="2021-11-06T02:44:23.26" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{7ACCC7C3-24F8-B14F-A486-B9650B9C7D19}">
     <text>is column being used???</text>
   </threadedComment>
 </ThreadedComments>
@@ -3057,14 +3110,11 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B00118F-F6B9-6642-9BD4-D95AE82A4925}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AA7F60C-00B2-A04B-8EF7-0C74D3232F71}">
   <dimension ref="A1:AB128"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C96" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C135" sqref="C135"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4289,9 +4339,6 @@
       <c r="H23" t="s">
         <v>51</v>
       </c>
-      <c r="I23" t="s">
-        <v>51</v>
-      </c>
       <c r="J23" t="s">
         <v>51</v>
       </c>
@@ -4390,9 +4437,6 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="H25" t="s">
-        <v>51</v>
-      </c>
-      <c r="I25" t="s">
         <v>51</v>
       </c>
       <c r="J25" t="s">
@@ -4688,9 +4732,6 @@
       <c r="H31" t="s">
         <v>53</v>
       </c>
-      <c r="I31" t="s">
-        <v>51</v>
-      </c>
       <c r="J31" t="s">
         <v>51</v>
       </c>
@@ -4726,7 +4767,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="C32" t="s">
         <v>50</v>
@@ -4751,7 +4792,7 @@
         <v>52</v>
       </c>
       <c r="L32" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="M32" t="s">
         <v>51</v>
@@ -4769,7 +4810,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="C33" t="s">
         <v>65</v>
@@ -4813,7 +4854,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="C34" t="s">
         <v>62</v>
@@ -4860,7 +4901,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="C35" t="s">
         <v>56</v>
@@ -4904,7 +4945,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="C36" t="s">
         <v>57</v>
@@ -4960,7 +5001,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="C37" t="s">
         <v>54</v>
@@ -5004,7 +5045,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="C38" t="s">
         <v>61</v>
@@ -7876,9 +7917,6 @@
       <c r="H91" t="s">
         <v>51</v>
       </c>
-      <c r="I91" t="s">
-        <v>51</v>
-      </c>
       <c r="J91" t="s">
         <v>51</v>
       </c>
@@ -9181,7 +9219,7 @@
         <v>64</v>
       </c>
       <c r="E115" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G115" t="str">
         <f t="shared" si="7"/>
@@ -9190,9 +9228,6 @@
       <c r="H115" t="s">
         <v>51</v>
       </c>
-      <c r="I115" t="s">
-        <v>51</v>
-      </c>
       <c r="J115" t="s">
         <v>51</v>
       </c>
@@ -9269,7 +9304,7 @@
         <v>support fetching a QuestionnaireResponse</v>
       </c>
       <c r="Z116" s="4" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="AB116" t="str">
         <f t="shared" si="9"/>
@@ -9381,7 +9416,7 @@
         <v>51</v>
       </c>
       <c r="Y118" s="19" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="AB118" t="str">
         <f t="shared" si="9"/>
@@ -9393,7 +9428,7 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="C119" t="s">
         <v>603</v>
@@ -9421,16 +9456,16 @@
         <v>52</v>
       </c>
       <c r="L119" t="s">
+        <v>671</v>
+      </c>
+      <c r="M119" t="s">
+        <v>51</v>
+      </c>
+      <c r="O119" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y119" s="19" t="s">
         <v>672</v>
-      </c>
-      <c r="M119" t="s">
-        <v>51</v>
-      </c>
-      <c r="O119" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y119" s="19" t="s">
-        <v>673</v>
       </c>
       <c r="AB119" t="str">
         <f t="shared" si="9"/>
@@ -9486,7 +9521,7 @@
         <v>87</v>
       </c>
       <c r="Y120" s="19" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="AB120" t="str">
         <f t="shared" si="9"/>
@@ -9536,7 +9571,7 @@
         <v>51</v>
       </c>
       <c r="Y121" s="19" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="AB121" t="str">
         <f t="shared" si="9"/>
@@ -9569,9 +9604,6 @@
       <c r="H122" t="s">
         <v>51</v>
       </c>
-      <c r="I122" t="s">
-        <v>51</v>
-      </c>
       <c r="J122" t="s">
         <v>51</v>
       </c>
@@ -9628,9 +9660,6 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</v>
       </c>
       <c r="H123" t="s">
-        <v>51</v>
-      </c>
-      <c r="I123" t="s">
         <v>51</v>
       </c>
       <c r="J123" t="s">
@@ -9656,7 +9685,7 @@
       <c r="Z123" s="4"/>
       <c r="AA123" s="8"/>
       <c r="AB123" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B123)&amp;"-"&amp;C123&amp;".html")</f>
+        <f t="shared" ref="AB123:AB128" si="11">"SearchParameter-us-core-"&amp;LOWER((B123)&amp;"-"&amp;C123&amp;".html")</f>
         <v>SearchParameter-us-core-medicationdispense-status.html</v>
       </c>
     </row>
@@ -9684,9 +9713,6 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</v>
       </c>
       <c r="H124" t="s">
-        <v>51</v>
-      </c>
-      <c r="I124" t="s">
         <v>51</v>
       </c>
       <c r="J124" t="s">
@@ -9712,7 +9738,7 @@
       <c r="Z124" s="4"/>
       <c r="AA124" s="8"/>
       <c r="AB124" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B124)&amp;"-"&amp;C124&amp;".html")</f>
+        <f t="shared" si="11"/>
         <v>SearchParameter-us-core-medicationdispense-type.html</v>
       </c>
     </row>
@@ -9742,9 +9768,6 @@
       <c r="H125" t="s">
         <v>51</v>
       </c>
-      <c r="I125" t="s">
-        <v>51</v>
-      </c>
       <c r="J125" t="s">
         <v>51</v>
       </c>
@@ -9772,7 +9795,7 @@
         <v>Fetches a bundle of all MedicationDispense resources for the specified patient.</v>
       </c>
       <c r="AB125" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B125)&amp;"-"&amp;C125&amp;".html")</f>
+        <f t="shared" si="11"/>
         <v>SearchParameter-us-core-medicationdispense-patient.html</v>
       </c>
     </row>
@@ -9802,9 +9825,6 @@
       <c r="H126" t="s">
         <v>51</v>
       </c>
-      <c r="I126" t="s">
-        <v>51</v>
-      </c>
       <c r="J126" t="s">
         <v>51</v>
       </c>
@@ -9829,7 +9849,7 @@
       </c>
       <c r="AA126" s="8"/>
       <c r="AB126" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B126)&amp;"-"&amp;C126&amp;".html")</f>
+        <f t="shared" si="11"/>
         <v>SearchParameter-us-core-!medicationdispense-whenhandedover.html</v>
       </c>
     </row>
@@ -9838,7 +9858,7 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C127" t="s">
         <v>50</v>
@@ -9876,14 +9896,14 @@
         <v>51</v>
       </c>
       <c r="Y127" s="4" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="Z127" s="4" t="str">
         <f>"GET [base]/"&amp;B127&amp;"?"&amp;C127&amp;"=123"</f>
         <v>GET [base]/Specimen?_id=123</v>
       </c>
       <c r="AB127" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B127)&amp;"-"&amp;C127&amp;".html")</f>
+        <f t="shared" si="11"/>
         <v>SearchParameter-us-core-specimen-_id.html</v>
       </c>
     </row>
@@ -9892,7 +9912,7 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C128" t="s">
         <v>84</v>
@@ -9942,20 +9962,15 @@
         <v>Fetches a bundle of all Specimen resources for the specified patient</v>
       </c>
       <c r="AB128" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B128)&amp;"-"&amp;C128&amp;".html")</f>
+        <f t="shared" si="11"/>
         <v>SearchParameter-us-core-specimen-patient.html</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AB126" xr:uid="{1CF5B17E-E72E-48B2-A597-9C21C12723F0}"/>
-  <conditionalFormatting sqref="B1:B126 B129:B1048576">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="!">
+  <autoFilter ref="A1:AB128" xr:uid="{1CF5B17E-E72E-48B2-A597-9C21C12723F0}"/>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",B1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B127:B128">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="!">
-      <formula>NOT(ISERROR(SEARCH("!",B127)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9965,11 +9980,12 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E7AC33C-2643-EE4B-9487-6CC99572F031}">
-  <dimension ref="A1:K96"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87C20678-B78A-D247-9ACE-3705AD98F5E0}">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:K98"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B90" sqref="B90"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="J131" sqref="J131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10021,7 +10037,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -10029,7 +10045,7 @@
         <v>151</v>
       </c>
       <c r="C2" t="str">
-        <f t="shared" ref="C2:C46" si="0">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B2)</f>
+        <f t="shared" ref="C2:C47" si="0">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B2)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D2" t="s">
@@ -10046,7 +10062,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -10071,7 +10087,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and patient</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -10096,7 +10112,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and patient and type</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -10121,7 +10137,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and type</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -10152,7 +10168,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified class and patient</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -10177,7 +10193,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and status</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -10202,7 +10218,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and status and type</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -10228,7 +10244,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and type</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -10255,7 +10271,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and status</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -10281,7 +10297,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and status and type</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -10306,7 +10322,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and type</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -10337,7 +10353,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified date and patient</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -10362,7 +10378,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified date and patient and type</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -10387,7 +10403,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified date and type</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -10418,7 +10434,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified patient and type</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -10449,7 +10465,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified patient and location</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -10475,7 +10491,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified patient and status and type</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -10506,7 +10522,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified patient and status</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -10537,7 +10553,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified patient and discharge-disposition</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -10564,7 +10580,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified status and type</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -10590,7 +10606,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and publisher</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -10615,7 +10631,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and publisher and status</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -10641,7 +10657,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and status</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -10668,7 +10684,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and status</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -10695,7 +10711,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and status and version</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -10722,7 +10738,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and version</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -10747,7 +10763,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified status and title and version</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -10772,7 +10788,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified status and version</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -10797,7 +10813,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified title and version</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -10828,7 +10844,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified birthdate and family</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -10859,7 +10875,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified death-date and family</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -10890,7 +10906,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified birthdate and name</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -10921,7 +10937,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified family and gender</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -10952,7 +10968,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified gender and name</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -10982,7 +10998,7 @@
         <v>312</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>649</v>
+        <v>708</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
@@ -10999,9 +11015,6 @@
       <c r="D37" t="s">
         <v>139</v>
       </c>
-      <c r="E37" t="s">
-        <v>51</v>
-      </c>
       <c r="F37" t="s">
         <v>11</v>
       </c>
@@ -11018,7 +11031,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -11030,7 +11043,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D38" t="s">
-        <v>555</v>
+        <v>713</v>
       </c>
       <c r="F38" t="s">
         <v>64</v>
@@ -11038,14 +11051,17 @@
       <c r="G38" t="s">
         <v>100</v>
       </c>
+      <c r="H38" t="s">
+        <v>396</v>
+      </c>
       <c r="I38" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="J38" s="4" t="s">
-        <v>650</v>
+        <v>714</v>
+      </c>
+      <c r="J38" s="25" t="s">
+        <v>715</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>556</v>
+        <v>716</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
@@ -11060,7 +11076,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D39" t="s">
-        <v>141</v>
+        <v>555</v>
       </c>
       <c r="F39" t="s">
         <v>64</v>
@@ -11069,13 +11085,13 @@
         <v>100</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>313</v>
+        <v>649</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>146</v>
+        <v>556</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
@@ -11090,22 +11106,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D40" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F40" t="s">
         <v>64</v>
       </c>
       <c r="G40" t="s">
-        <v>143</v>
+        <v>100</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>557</v>
+        <v>313</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
@@ -11120,7 +11136,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D41" t="s">
-        <v>558</v>
+        <v>142</v>
       </c>
       <c r="F41" t="s">
         <v>64</v>
@@ -11132,7 +11148,7 @@
         <v>147</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="K41" s="4" t="s">
         <v>150</v>
@@ -11150,7 +11166,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D42" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="F42" t="s">
         <v>64</v>
@@ -11162,7 +11178,7 @@
         <v>147</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="K42" s="4" t="s">
         <v>150</v>
@@ -11180,7 +11196,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D43" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="F43" t="s">
         <v>64</v>
@@ -11192,7 +11208,7 @@
         <v>147</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="K43" s="4" t="s">
         <v>150</v>
@@ -11203,63 +11219,62 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>18</v>
+        <v>132</v>
       </c>
       <c r="C44" t="str">
         <f t="shared" si="0"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-allergyintolerance</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D44" t="s">
-        <v>138</v>
+        <v>562</v>
       </c>
       <c r="F44" t="s">
         <v>64</v>
       </c>
       <c r="G44" t="s">
-        <v>100</v>
+        <v>143</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>308</v>
+        <v>563</v>
       </c>
       <c r="K44" s="4" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>155</v>
+        <v>18</v>
       </c>
       <c r="C45" t="str">
         <f t="shared" si="0"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-immunization</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-allergyintolerance</v>
       </c>
       <c r="D45" t="s">
-        <v>158</v>
+        <v>138</v>
       </c>
       <c r="F45" t="s">
         <v>64</v>
       </c>
       <c r="G45" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>490</v>
-      </c>
-      <c r="K45" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B45&amp;" resources for the specified "&amp;SUBSTITUTE(D45,","," and ")</f>
-        <v>Fetches a bundle of all Immunization resources for the specified patient and date</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+        <v>308</v>
+      </c>
+      <c r="K45" s="4" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -11271,34 +11286,35 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-immunization</v>
       </c>
       <c r="D46" t="s">
-        <v>110</v>
+        <v>158</v>
       </c>
       <c r="F46" t="s">
         <v>64</v>
       </c>
       <c r="G46" t="s">
-        <v>143</v>
+        <v>107</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>296</v>
+        <v>161</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>157</v>
+        <v>490</v>
       </c>
       <c r="K46" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B46&amp;" resources for the specified "&amp;SUBSTITUTE(D46,","," and ")</f>
-        <v>Fetches a bundle of all Immunization resources for the specified patient and status</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+        <v>Fetches a bundle of all Immunization resources for the specified patient and date</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>173</v>
-      </c>
-      <c r="C47" t="s">
-        <v>662</v>
+        <v>155</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-immunization</v>
       </c>
       <c r="D47" t="s">
         <v>110</v>
@@ -11307,20 +11323,20 @@
         <v>64</v>
       </c>
       <c r="G47" t="s">
-        <v>100</v>
+        <v>143</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>194</v>
+        <v>296</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
       <c r="K47" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B47&amp;" resources for the specified "&amp;SUBSTITUTE(D47,","," and ")</f>
-        <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and status</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+        <v>Fetches a bundle of all Immunization resources for the specified patient and status</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -11328,32 +11344,29 @@
         <v>173</v>
       </c>
       <c r="C48" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="D48" t="s">
-        <v>139</v>
+        <v>110</v>
       </c>
       <c r="F48" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="G48" t="s">
         <v>100</v>
       </c>
-      <c r="H48" t="s">
-        <v>309</v>
-      </c>
       <c r="I48" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="J48" s="7" t="s">
-        <v>190</v>
+        <v>194</v>
+      </c>
+      <c r="J48" s="4" t="s">
+        <v>178</v>
       </c>
       <c r="K48" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B48&amp;" resources for the specified patient and  a category code = `LAB`"</f>
-        <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  a category code = `LAB`</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+        <f>"Fetches a bundle of all "&amp;B48&amp;" resources for the specified "&amp;SUBSTITUTE(D48,","," and ")</f>
+        <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and status</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -11361,10 +11374,10 @@
         <v>173</v>
       </c>
       <c r="C49" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="D49" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F49" t="s">
         <v>11</v>
@@ -11372,18 +11385,21 @@
       <c r="G49" t="s">
         <v>100</v>
       </c>
+      <c r="H49" t="s">
+        <v>309</v>
+      </c>
       <c r="I49" s="4" t="s">
-        <v>214</v>
+        <v>187</v>
       </c>
       <c r="J49" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K49" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B49&amp;" resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes."</f>
-        <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+        <f>"Fetches a bundle of all "&amp;B49&amp;" resources for the specified patient and  a category code = `LAB`"</f>
+        <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  a category code = `LAB`</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -11391,32 +11407,29 @@
         <v>173</v>
       </c>
       <c r="C50" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="D50" t="s">
-        <v>188</v>
+        <v>141</v>
       </c>
       <c r="F50" t="s">
         <v>11</v>
       </c>
       <c r="G50" t="s">
-        <v>211</v>
-      </c>
-      <c r="H50" t="s">
-        <v>309</v>
+        <v>100</v>
       </c>
       <c r="I50" s="4" t="s">
-        <v>189</v>
+        <v>214</v>
       </c>
       <c r="J50" s="7" t="s">
-        <v>491</v>
+        <v>191</v>
       </c>
       <c r="K50" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B50&amp;" resources for the specified patient and date and a category code = `LAB`"</f>
-        <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and a category code = `LAB`</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+        <f>"Fetches a bundle of all "&amp;B50&amp;" resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes."</f>
+        <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -11424,60 +11437,62 @@
         <v>173</v>
       </c>
       <c r="C51" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="D51" t="s">
-        <v>212</v>
+        <v>188</v>
       </c>
       <c r="F51" t="s">
-        <v>64</v>
+        <v>11</v>
       </c>
       <c r="G51" t="s">
         <v>211</v>
       </c>
+      <c r="H51" t="s">
+        <v>309</v>
+      </c>
       <c r="I51" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="J51" s="7" t="s">
+        <v>491</v>
+      </c>
+      <c r="K51" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B51&amp;" resources for the specified patient and date and a category code = `LAB`"</f>
+        <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and a category code = `LAB`</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>173</v>
+      </c>
+      <c r="C52" t="s">
+        <v>661</v>
+      </c>
+      <c r="D52" t="s">
+        <v>212</v>
+      </c>
+      <c r="F52" t="s">
+        <v>64</v>
+      </c>
+      <c r="G52" t="s">
+        <v>211</v>
+      </c>
+      <c r="I52" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="J51" s="4" t="s">
+      <c r="J52" s="4" t="s">
         <v>492</v>
       </c>
-      <c r="K51" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B51&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
+      <c r="K52" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B52&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <v>51</v>
-      </c>
-      <c r="B52" t="s">
-        <v>174</v>
-      </c>
-      <c r="C52" t="str">
-        <f t="shared" ref="C52:C62" si="2">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B52)</f>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
-      </c>
-      <c r="D52" t="s">
-        <v>300</v>
-      </c>
-      <c r="F52" t="s">
-        <v>64</v>
-      </c>
-      <c r="G52" t="s">
-        <v>100</v>
-      </c>
-      <c r="I52" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="J52" s="4" t="s">
-        <v>301</v>
-      </c>
-      <c r="K52" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B52&amp;" resources for the specified "&amp;SUBSTITUTE(D52,","," and ")</f>
-        <v>Fetches a bundle of all Goal resources for the specified patient and lifecycle-status</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -11485,63 +11500,61 @@
         <v>174</v>
       </c>
       <c r="C53" t="str">
+        <f t="shared" ref="C53:C63" si="2">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B53)</f>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
+      </c>
+      <c r="D53" t="s">
+        <v>300</v>
+      </c>
+      <c r="F53" t="s">
+        <v>64</v>
+      </c>
+      <c r="G53" t="s">
+        <v>100</v>
+      </c>
+      <c r="I53" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="J53" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="K53" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B53&amp;" resources for the specified "&amp;SUBSTITUTE(D53,","," and ")</f>
+        <v>Fetches a bundle of all Goal resources for the specified patient and lifecycle-status</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>174</v>
+      </c>
+      <c r="C54" t="str">
         <f t="shared" si="2"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D54" t="s">
         <v>397</v>
       </c>
-      <c r="F53" t="s">
-        <v>64</v>
-      </c>
-      <c r="G53" t="s">
+      <c r="F54" t="s">
+        <v>64</v>
+      </c>
+      <c r="G54" t="s">
         <v>143</v>
       </c>
-      <c r="I53" s="4" t="s">
+      <c r="I54" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="J53" s="4" t="s">
+      <c r="J54" s="4" t="s">
         <v>398</v>
       </c>
-      <c r="K53" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B53&amp;" resources for the specified "&amp;SUBSTITUTE(D53,","," and ")</f>
+      <c r="K54" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B54&amp;" resources for the specified "&amp;SUBSTITUTE(D54,","," and ")</f>
         <v>Fetches a bundle of all Goal resources for the specified patient and target-date</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A54">
-        <v>53</v>
-      </c>
-      <c r="B54" t="s">
-        <v>175</v>
-      </c>
-      <c r="C54" t="str">
-        <f t="shared" si="2"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
-      </c>
-      <c r="D54" t="s">
-        <v>417</v>
-      </c>
-      <c r="F54" t="s">
-        <v>11</v>
-      </c>
-      <c r="G54" t="s">
-        <v>100</v>
-      </c>
-      <c r="H54" t="s">
-        <v>437</v>
-      </c>
-      <c r="I54" s="4" t="s">
-        <v>418</v>
-      </c>
-      <c r="J54" s="4" t="s">
-        <v>438</v>
-      </c>
-      <c r="K54" s="4" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -11553,7 +11566,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D55" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="F55" t="s">
         <v>11</v>
@@ -11565,16 +11578,16 @@
         <v>437</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>179</v>
+        <v>418</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="K55" s="4" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -11586,10 +11599,10 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D56" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F56" t="s">
-        <v>64</v>
+        <v>11</v>
       </c>
       <c r="G56" t="s">
         <v>100</v>
@@ -11601,13 +11614,13 @@
         <v>179</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="K56" s="4" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -11619,59 +11632,61 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D57" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F57" t="s">
         <v>64</v>
       </c>
       <c r="G57" t="s">
-        <v>211</v>
+        <v>100</v>
       </c>
       <c r="H57" t="s">
         <v>437</v>
       </c>
       <c r="I57" s="4" t="s">
-        <v>222</v>
+        <v>179</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>493</v>
+        <v>442</v>
       </c>
       <c r="K57" s="4" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>422</v>
+        <v>175</v>
       </c>
       <c r="C58" t="str">
         <f t="shared" si="2"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationstatement</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D58" t="s">
-        <v>110</v>
+        <v>421</v>
       </c>
       <c r="F58" t="s">
         <v>64</v>
       </c>
       <c r="G58" t="s">
-        <v>100</v>
+        <v>211</v>
+      </c>
+      <c r="H58" t="s">
+        <v>437</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>181</v>
+        <v>222</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>399</v>
-      </c>
-      <c r="K58" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B58&amp;" resources for the specified "&amp;SUBSTITUTE(D58,","," and ")</f>
-        <v>Fetches a bundle of all !MedicationStatement resources for the specified patient and status</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+        <v>493</v>
+      </c>
+      <c r="K58" s="4" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -11683,56 +11698,56 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationstatement</v>
       </c>
       <c r="D59" t="s">
-        <v>224</v>
+        <v>110</v>
       </c>
       <c r="F59" t="s">
         <v>64</v>
       </c>
       <c r="G59" t="s">
-        <v>143</v>
+        <v>100</v>
       </c>
       <c r="I59" s="4" t="s">
-        <v>223</v>
+        <v>181</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>400</v>
-      </c>
-      <c r="K59" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+        <v>399</v>
+      </c>
+      <c r="K59" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B59&amp;" resources for the specified "&amp;SUBSTITUTE(D59,","," and ")</f>
+        <v>Fetches a bundle of all !MedicationStatement resources for the specified patient and status</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>176</v>
+        <v>422</v>
       </c>
       <c r="C60" t="str">
         <f t="shared" si="2"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationstatement</v>
       </c>
       <c r="D60" t="s">
-        <v>110</v>
+        <v>224</v>
       </c>
       <c r="F60" t="s">
         <v>64</v>
       </c>
       <c r="G60" t="s">
-        <v>100</v>
+        <v>143</v>
       </c>
       <c r="I60" s="4" t="s">
-        <v>197</v>
+        <v>223</v>
       </c>
       <c r="J60" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="K60" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B60&amp;" resources for the specified "&amp;SUBSTITUTE(D60,","," and ")</f>
-        <v>Fetches a bundle of all Procedure resources for the specified patient and status</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+        <v>400</v>
+      </c>
+      <c r="K60" s="4" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -11744,26 +11759,26 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
       </c>
       <c r="D61" t="s">
-        <v>158</v>
+        <v>110</v>
       </c>
       <c r="F61" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="G61" t="s">
         <v>100</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="K61" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B61&amp;" resources for the specified "&amp;SUBSTITUTE(D61,","," and ")</f>
-        <v>Fetches a bundle of all Procedure resources for the specified patient and date</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+        <v>Fetches a bundle of all Procedure resources for the specified patient and status</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -11775,58 +11790,57 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
       </c>
       <c r="D62" t="s">
-        <v>212</v>
+        <v>158</v>
       </c>
       <c r="F62" t="s">
-        <v>64</v>
+        <v>11</v>
       </c>
       <c r="G62" t="s">
-        <v>211</v>
+        <v>100</v>
       </c>
       <c r="I62" s="4" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>494</v>
+        <v>210</v>
       </c>
       <c r="K62" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B62&amp;" resources for the specified patient and date and procedure code(s).  SHOULD support search by multiple codes."</f>
-        <v>Fetches a bundle of all Procedure resources for the specified patient and date and procedure code(s).  SHOULD support search by multiple codes.</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+        <f>"Fetches a bundle of all "&amp;B62&amp;" resources for the specified "&amp;SUBSTITUTE(D62,","," and ")</f>
+        <v>Fetches a bundle of all Procedure resources for the specified patient and date</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>177</v>
-      </c>
-      <c r="C63" t="s">
-        <v>663</v>
+        <v>176</v>
+      </c>
+      <c r="C63" t="str">
+        <f t="shared" si="2"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
       </c>
       <c r="D63" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
       <c r="F63" t="s">
         <v>64</v>
       </c>
       <c r="G63" t="s">
-        <v>100</v>
-      </c>
-      <c r="H63" t="s">
-        <v>423</v>
+        <v>211</v>
       </c>
       <c r="I63" s="4" t="s">
-        <v>268</v>
+        <v>219</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>424</v>
-      </c>
-      <c r="K63" s="4" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+        <v>494</v>
+      </c>
+      <c r="K63" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B63&amp;" resources for the specified patient and date and procedure code(s).  SHOULD support search by multiple codes."</f>
+        <v>Fetches a bundle of all Procedure resources for the specified patient and date and procedure code(s).  SHOULD support search by multiple codes.</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -11834,13 +11848,13 @@
         <v>177</v>
       </c>
       <c r="C64" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="D64" t="s">
-        <v>139</v>
+        <v>229</v>
       </c>
       <c r="F64" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="G64" t="s">
         <v>100</v>
@@ -11849,17 +11863,16 @@
         <v>423</v>
       </c>
       <c r="I64" s="4" t="s">
-        <v>213</v>
+        <v>268</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>425</v>
-      </c>
-      <c r="K64" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B64&amp;" resources for the specified patient and a category code = `laboratory`"</f>
-        <v>Fetches a bundle of all Observation resources for the specified patient and a category code = `laboratory`</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+        <v>424</v>
+      </c>
+      <c r="K64" s="4" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -11867,10 +11880,10 @@
         <v>177</v>
       </c>
       <c r="C65" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="D65" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F65" t="s">
         <v>11</v>
@@ -11878,18 +11891,21 @@
       <c r="G65" t="s">
         <v>100</v>
       </c>
+      <c r="H65" t="s">
+        <v>423</v>
+      </c>
       <c r="I65" s="4" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>314</v>
+        <v>425</v>
       </c>
       <c r="K65" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B65&amp;" resources for the specified patient and observation code(s).  SHOULD support search by multiple report codes. The Observation `code` parameter searches `Observation.code only."</f>
-        <v>Fetches a bundle of all Observation resources for the specified patient and observation code(s).  SHOULD support search by multiple report codes. The Observation `code` parameter searches `Observation.code only.</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+        <f>"Fetches a bundle of all "&amp;B65&amp;" resources for the specified patient and a category code = `laboratory`"</f>
+        <v>Fetches a bundle of all Observation resources for the specified patient and a category code = `laboratory`</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -11897,32 +11913,29 @@
         <v>177</v>
       </c>
       <c r="C66" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="D66" t="s">
-        <v>188</v>
+        <v>141</v>
       </c>
       <c r="F66" t="s">
         <v>11</v>
       </c>
       <c r="G66" t="s">
-        <v>211</v>
-      </c>
-      <c r="H66" t="s">
-        <v>423</v>
+        <v>100</v>
       </c>
       <c r="I66" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J66" s="4" t="s">
-        <v>495</v>
+        <v>314</v>
       </c>
       <c r="K66" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B66&amp;" resources for the specified patient and date and a category code = `laboratory`"</f>
-        <v>Fetches a bundle of all Observation resources for the specified patient and date and a category code = `laboratory`</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+        <f>"Fetches a bundle of all "&amp;B66&amp;" resources for the specified patient and observation code(s).  SHOULD support search by multiple report codes. The Observation `code` parameter searches `Observation.code only."</f>
+        <v>Fetches a bundle of all Observation resources for the specified patient and observation code(s).  SHOULD support search by multiple report codes. The Observation `code` parameter searches `Observation.code only.</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -11930,92 +11943,92 @@
         <v>177</v>
       </c>
       <c r="C67" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="D67" t="s">
-        <v>212</v>
+        <v>188</v>
       </c>
       <c r="F67" t="s">
-        <v>64</v>
+        <v>11</v>
       </c>
       <c r="G67" t="s">
         <v>211</v>
       </c>
+      <c r="H67" t="s">
+        <v>423</v>
+      </c>
       <c r="I67" s="4" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="K67" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B67&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
-        <v>Fetches a bundle of all Observation resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+        <f>"Fetches a bundle of all "&amp;B67&amp;" resources for the specified patient and date and a category code = `laboratory`"</f>
+        <v>Fetches a bundle of all Observation resources for the specified patient and date and a category code = `laboratory`</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>304</v>
+        <v>177</v>
       </c>
       <c r="C68" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="D68" t="s">
-        <v>110</v>
+        <v>212</v>
       </c>
       <c r="F68" t="s">
         <v>64</v>
       </c>
       <c r="G68" t="s">
-        <v>100</v>
+        <v>211</v>
       </c>
       <c r="I68" s="4" t="s">
-        <v>199</v>
+        <v>215</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>198</v>
+        <v>496</v>
       </c>
       <c r="K68" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B68&amp;" resources for the specified "&amp;SUBSTITUTE(D68,","," and ")</f>
-        <v>Fetches a bundle of all !Observation resources for the specified patient and status</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+        <f>"Fetches a bundle of all "&amp;B68&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
+        <v>Fetches a bundle of all Observation resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>226</v>
+        <v>304</v>
       </c>
       <c r="C69" t="s">
-        <v>228</v>
+        <v>662</v>
       </c>
       <c r="D69" t="s">
-        <v>139</v>
+        <v>110</v>
       </c>
       <c r="F69" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="G69" t="s">
         <v>100</v>
       </c>
-      <c r="H69" t="s">
-        <v>310</v>
-      </c>
       <c r="I69" s="4" t="s">
-        <v>234</v>
+        <v>199</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>235</v>
+        <v>198</v>
       </c>
       <c r="K69" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B69&amp;" resources for the specified "&amp;SUBSTITUTE(D69,","," and ")&amp;"=`assess-plan`"</f>
-        <v>Fetches a bundle of all CarePlan resources for the specified patient and category=`assess-plan`</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+        <f>"Fetches a bundle of all "&amp;B69&amp;" resources for the specified "&amp;SUBSTITUTE(D69,","," and ")</f>
+        <v>Fetches a bundle of all !Observation resources for the specified patient and status</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -12026,28 +12039,29 @@
         <v>228</v>
       </c>
       <c r="D70" t="s">
-        <v>188</v>
+        <v>139</v>
       </c>
       <c r="F70" t="s">
-        <v>64</v>
+        <v>11</v>
       </c>
       <c r="G70" t="s">
-        <v>211</v>
+        <v>100</v>
       </c>
       <c r="H70" t="s">
         <v>310</v>
       </c>
       <c r="I70" s="4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>497</v>
-      </c>
-      <c r="K70" s="4" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+        <v>235</v>
+      </c>
+      <c r="K70" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B70&amp;" resources for the specified "&amp;SUBSTITUTE(D70,","," and ")&amp;"=`assess-plan`"</f>
+        <v>Fetches a bundle of all CarePlan resources for the specified patient and category=`assess-plan`</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -12058,28 +12072,28 @@
         <v>228</v>
       </c>
       <c r="D71" t="s">
-        <v>229</v>
+        <v>188</v>
       </c>
       <c r="F71" t="s">
         <v>64</v>
       </c>
       <c r="G71" t="s">
-        <v>100</v>
+        <v>211</v>
       </c>
       <c r="H71" t="s">
         <v>310</v>
       </c>
       <c r="I71" s="4" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="J71" s="4" t="s">
-        <v>236</v>
+        <v>497</v>
       </c>
       <c r="K71" s="4" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -12090,154 +12104,153 @@
         <v>228</v>
       </c>
       <c r="D72" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F72" t="s">
         <v>64</v>
       </c>
       <c r="G72" t="s">
-        <v>211</v>
+        <v>100</v>
       </c>
       <c r="H72" t="s">
         <v>310</v>
       </c>
       <c r="I72" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J72" s="4" t="s">
-        <v>498</v>
+        <v>236</v>
       </c>
       <c r="K72" s="4" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" ht="136" x14ac:dyDescent="0.2">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>240</v>
-      </c>
-      <c r="C73" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B73)</f>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
+        <v>226</v>
+      </c>
+      <c r="C73" t="s">
+        <v>228</v>
       </c>
       <c r="D73" t="s">
-        <v>110</v>
+        <v>230</v>
       </c>
       <c r="F73" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="G73" t="s">
-        <v>100</v>
+        <v>211</v>
       </c>
       <c r="H73" t="s">
-        <v>295</v>
+        <v>310</v>
       </c>
       <c r="I73" s="4" t="s">
-        <v>564</v>
+        <v>232</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>565</v>
-      </c>
-      <c r="K73" s="8" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+        <v>498</v>
+      </c>
+      <c r="K73" s="4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" ht="136" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>172</v>
+        <v>240</v>
       </c>
       <c r="C74" t="str">
-        <f t="shared" ref="C74:C79" si="3">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B74)</f>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B74)</f>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
       </c>
       <c r="D74" t="s">
         <v>110</v>
       </c>
       <c r="F74" t="s">
-        <v>64</v>
+        <v>11</v>
       </c>
       <c r="G74" t="s">
         <v>100</v>
       </c>
+      <c r="H74" t="s">
+        <v>295</v>
+      </c>
       <c r="I74" s="4" t="s">
-        <v>275</v>
+        <v>564</v>
       </c>
       <c r="J74" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="K74" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B74&amp;" resources for the specified "&amp;SUBSTITUTE(D74,","," and ") &amp;". See the implementation notes above for how to access the actual document."</f>
-        <v>Fetches a bundle of all DocumentReference resources for the specified patient and status. See the implementation notes above for how to access the actual document.</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>565</v>
+      </c>
+      <c r="K74" s="8" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
       <c r="B75" t="s">
+        <v>172</v>
+      </c>
+      <c r="C75" t="str">
+        <f t="shared" ref="C75:C80" si="3">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B75)</f>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
+      </c>
+      <c r="D75" t="s">
+        <v>110</v>
+      </c>
+      <c r="F75" t="s">
+        <v>64</v>
+      </c>
+      <c r="G75" t="s">
+        <v>100</v>
+      </c>
+      <c r="I75" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="J75" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="K75" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B75&amp;" resources for the specified "&amp;SUBSTITUTE(D75,","," and ") &amp;". See the implementation notes above for how to access the actual document."</f>
+        <v>Fetches a bundle of all DocumentReference resources for the specified patient and status. See the implementation notes above for how to access the actual document.</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
         <v>274</v>
       </c>
-      <c r="C75" t="str">
+      <c r="C76" t="str">
         <f t="shared" si="3"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!documentreference</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D76" t="s">
         <v>273</v>
       </c>
-      <c r="F75" t="s">
-        <v>64</v>
-      </c>
-      <c r="G75" t="s">
+      <c r="F76" t="s">
+        <v>64</v>
+      </c>
+      <c r="G76" t="s">
         <v>143</v>
       </c>
-      <c r="I75" s="4" t="s">
+      <c r="I76" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="J75" s="4"/>
-      <c r="K75" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B75&amp;" resources for the specified "&amp;SUBSTITUTE(D75,","," and ") &amp;". See the implementation notes above for how to access the actual document."</f>
+      <c r="J76" s="4"/>
+      <c r="K76" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B76&amp;" resources for the specified "&amp;SUBSTITUTE(D76,","," and ") &amp;". See the implementation notes above for how to access the actual document."</f>
         <v>Fetches a bundle of all !DocumentReference resources for the specified patient and period. See the implementation notes above for how to access the actual document.</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A76">
-        <v>75</v>
-      </c>
-      <c r="B76" t="s">
-        <v>172</v>
-      </c>
-      <c r="C76" t="str">
-        <f t="shared" si="3"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
-      </c>
-      <c r="D76" t="s">
-        <v>139</v>
-      </c>
-      <c r="F76" t="s">
-        <v>11</v>
-      </c>
-      <c r="G76" t="s">
-        <v>100</v>
-      </c>
-      <c r="H76" t="s">
-        <v>311</v>
-      </c>
-      <c r="I76" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="J76" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="K76" s="4" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -12249,28 +12262,28 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D77" t="s">
-        <v>188</v>
+        <v>139</v>
       </c>
       <c r="F77" t="s">
         <v>11</v>
       </c>
       <c r="G77" t="s">
-        <v>211</v>
+        <v>100</v>
       </c>
       <c r="H77" t="s">
         <v>311</v>
       </c>
       <c r="I77" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="J77" s="7" t="s">
-        <v>499</v>
+        <v>279</v>
+      </c>
+      <c r="J77" s="4" t="s">
+        <v>276</v>
       </c>
       <c r="K77" s="4" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
@@ -12282,25 +12295,28 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D78" t="s">
-        <v>112</v>
+        <v>188</v>
       </c>
       <c r="F78" t="s">
         <v>11</v>
       </c>
       <c r="G78" t="s">
-        <v>100</v>
+        <v>211</v>
+      </c>
+      <c r="H78" t="s">
+        <v>311</v>
       </c>
       <c r="I78" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="J78" s="4" t="s">
-        <v>372</v>
+        <v>280</v>
+      </c>
+      <c r="J78" s="7" t="s">
+        <v>499</v>
       </c>
       <c r="K78" s="4" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>
@@ -12312,55 +12328,56 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D79" t="s">
-        <v>283</v>
+        <v>112</v>
       </c>
       <c r="F79" t="s">
-        <v>64</v>
+        <v>11</v>
       </c>
       <c r="G79" t="s">
-        <v>211</v>
+        <v>100</v>
       </c>
       <c r="I79" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J79" s="4" t="s">
-        <v>500</v>
-      </c>
-      <c r="K79" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B79&amp;" resources for the specified "&amp;SUBSTITUTE(D79,","," and ") &amp;". See the implementation notes above for how to access the actual document."</f>
-        <v>Fetches a bundle of all DocumentReference resources for the specified patient and type and period. See the implementation notes above for how to access the actual document.</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+        <v>372</v>
+      </c>
+      <c r="K79" s="4" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>241</v>
-      </c>
-      <c r="C80" t="s">
-        <v>664</v>
+        <v>172</v>
+      </c>
+      <c r="C80" t="str">
+        <f t="shared" si="3"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D80" t="s">
-        <v>112</v>
+        <v>283</v>
       </c>
       <c r="F80" t="s">
         <v>64</v>
       </c>
       <c r="G80" t="s">
-        <v>100</v>
+        <v>211</v>
       </c>
       <c r="I80" s="4" t="s">
-        <v>371</v>
+        <v>285</v>
       </c>
       <c r="J80" s="4" t="s">
-        <v>373</v>
-      </c>
-      <c r="K80" s="4" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+        <v>500</v>
+      </c>
+      <c r="K80" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B80&amp;" resources for the specified "&amp;SUBSTITUTE(D80,","," and ") &amp;". See the implementation notes above for how to access the actual document."</f>
+        <v>Fetches a bundle of all DocumentReference resources for the specified patient and type and period. See the implementation notes above for how to access the actual document.</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>80</v>
       </c>
@@ -12368,13 +12385,10 @@
         <v>241</v>
       </c>
       <c r="C81" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D81" t="s">
-        <v>110</v>
-      </c>
-      <c r="E81" t="s">
-        <v>51</v>
+        <v>112</v>
       </c>
       <c r="F81" t="s">
         <v>64</v>
@@ -12383,28 +12397,27 @@
         <v>100</v>
       </c>
       <c r="I81" s="4" t="s">
-        <v>651</v>
+        <v>371</v>
       </c>
       <c r="J81" s="4" t="s">
-        <v>652</v>
+        <v>373</v>
       </c>
       <c r="K81" s="4" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>240</v>
-      </c>
-      <c r="C82" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B82)</f>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
+        <v>241</v>
+      </c>
+      <c r="C82" t="s">
+        <v>663</v>
       </c>
       <c r="D82" t="s">
-        <v>567</v>
+        <v>110</v>
       </c>
       <c r="F82" t="s">
         <v>64</v>
@@ -12413,28 +12426,28 @@
         <v>100</v>
       </c>
       <c r="I82" s="4" t="s">
-        <v>568</v>
+        <v>650</v>
       </c>
       <c r="J82" s="4" t="s">
-        <v>569</v>
+        <v>651</v>
       </c>
       <c r="K82" s="4" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>531</v>
+        <v>240</v>
       </c>
       <c r="C83" t="str">
-        <f t="shared" ref="C83:C96" si="4">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B83)</f>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B83)</f>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
       </c>
       <c r="D83" t="s">
-        <v>110</v>
+        <v>567</v>
       </c>
       <c r="F83" t="s">
         <v>64</v>
@@ -12443,17 +12456,16 @@
         <v>100</v>
       </c>
       <c r="I83" s="4" t="s">
-        <v>287</v>
+        <v>568</v>
       </c>
       <c r="J83" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="K83" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B83&amp;" resources for the specified "&amp;SUBSTITUTE(D83,","," and ")</f>
-        <v>Fetches a bundle of all ServiceRequest resources for the specified patient and status</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+        <v>569</v>
+      </c>
+      <c r="K83" s="4" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>83</v>
       </c>
@@ -12461,30 +12473,30 @@
         <v>531</v>
       </c>
       <c r="C84" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="C84:C97" si="4">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B84)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D84" t="s">
-        <v>139</v>
+        <v>110</v>
       </c>
       <c r="F84" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="G84" t="s">
         <v>100</v>
       </c>
       <c r="I84" s="4" t="s">
-        <v>192</v>
+        <v>287</v>
       </c>
       <c r="J84" s="4" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="K84" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B84&amp;" resources for the specified patient and  a category code"</f>
-        <v>Fetches a bundle of all ServiceRequest resources for the specified patient and  a category code</v>
-      </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+        <f>"Fetches a bundle of all "&amp;B84&amp;" resources for the specified "&amp;SUBSTITUTE(D84,","," and ")</f>
+        <v>Fetches a bundle of all ServiceRequest resources for the specified patient and status</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>84</v>
       </c>
@@ -12496,7 +12508,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D85" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F85" t="s">
         <v>11</v>
@@ -12505,17 +12517,17 @@
         <v>100</v>
       </c>
       <c r="I85" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J85" s="4" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="K85" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B85&amp;" resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes."</f>
-        <v>Fetches a bundle of all ServiceRequest resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+        <f>"Fetches a bundle of all "&amp;B85&amp;" resources for the specified patient and  a category code"</f>
+        <v>Fetches a bundle of all ServiceRequest resources for the specified patient and  a category code</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>85</v>
       </c>
@@ -12527,26 +12539,26 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D86" t="s">
-        <v>574</v>
+        <v>141</v>
       </c>
       <c r="F86" t="s">
         <v>11</v>
       </c>
       <c r="G86" t="s">
-        <v>211</v>
+        <v>100</v>
       </c>
       <c r="I86" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J86" s="4" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="K86" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B86&amp;" resources for the specified patient and date and a category code"</f>
-        <v>Fetches a bundle of all ServiceRequest resources for the specified patient and date and a category code</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+        <f>"Fetches a bundle of all "&amp;B86&amp;" resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes."</f>
+        <v>Fetches a bundle of all ServiceRequest resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>86</v>
       </c>
@@ -12558,69 +12570,69 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D87" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="F87" t="s">
-        <v>64</v>
+        <v>11</v>
       </c>
       <c r="G87" t="s">
         <v>211</v>
       </c>
       <c r="I87" s="4" t="s">
-        <v>577</v>
+        <v>195</v>
       </c>
       <c r="J87" s="4" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="K87" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B87&amp;" resources for the specified patient and date and service code(s).  SHOULD support search by multiple report codes."</f>
-        <v>Fetches a bundle of all ServiceRequest resources for the specified patient and date and service code(s).  SHOULD support search by multiple report codes.</v>
-      </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+        <f>"Fetches a bundle of all "&amp;B87&amp;" resources for the specified patient and date and a category code"</f>
+        <v>Fetches a bundle of all ServiceRequest resources for the specified patient and date and a category code</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>174</v>
+        <v>531</v>
       </c>
       <c r="C88" t="str">
         <f t="shared" si="4"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D88" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="F88" t="s">
         <v>64</v>
       </c>
       <c r="G88" t="s">
-        <v>100</v>
+        <v>211</v>
       </c>
       <c r="I88" s="4" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="J88" s="4" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="K88" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B88&amp;" resources for the specified "&amp;SUBSTITUTE(D88,","," and ")</f>
-        <v>Fetches a bundle of all Goal resources for the specified patient and description</v>
-      </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+        <f>"Fetches a bundle of all "&amp;B88&amp;" resources for the specified patient and date and service code(s).  SHOULD support search by multiple report codes."</f>
+        <v>Fetches a bundle of all ServiceRequest resources for the specified patient and date and service code(s).  SHOULD support search by multiple report codes.</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>601</v>
+        <v>174</v>
       </c>
       <c r="C89" t="str">
         <f t="shared" si="4"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D89" t="s">
-        <v>110</v>
+        <v>579</v>
       </c>
       <c r="F89" t="s">
         <v>64</v>
@@ -12628,30 +12640,30 @@
       <c r="G89" t="s">
         <v>100</v>
       </c>
-      <c r="I89" t="s">
-        <v>605</v>
+      <c r="I89" s="4" t="s">
+        <v>580</v>
       </c>
       <c r="J89" s="4" t="s">
-        <v>606</v>
+        <v>581</v>
       </c>
       <c r="K89" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B89&amp;" resources for the specified "&amp;SUBSTITUTE(D89,","," and ")</f>
-        <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient and status</v>
-      </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+        <v>Fetches a bundle of all Goal resources for the specified patient and description</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>708</v>
+        <v>601</v>
       </c>
       <c r="C90" t="str">
         <f t="shared" si="4"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D90" t="s">
-        <v>607</v>
+        <v>110</v>
       </c>
       <c r="F90" t="s">
         <v>64</v>
@@ -12659,152 +12671,148 @@
       <c r="G90" t="s">
         <v>100</v>
       </c>
-      <c r="H90" t="s">
-        <v>608</v>
-      </c>
       <c r="I90" t="s">
         <v>605</v>
       </c>
       <c r="J90" s="4" t="s">
-        <v>609</v>
-      </c>
-      <c r="K90" t="str">
-        <f>"Fetches a bundle of all "&amp;B90&amp;" resources for the specified "&amp;SUBSTITUTE(D90,","," and  ") &amp; "= 'sdoh'"</f>
-        <v>Fetches a bundle of all !QuestionnaireResponse resources for the specified patient and  _tag= 'sdoh'</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+        <v>606</v>
+      </c>
+      <c r="K90" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B90&amp;" resources for the specified "&amp;SUBSTITUTE(D90,","," and ")</f>
+        <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient and status</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>601</v>
+        <v>707</v>
       </c>
       <c r="C91" t="str">
         <f t="shared" si="4"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="D91" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="F91" t="s">
         <v>64</v>
       </c>
       <c r="G91" t="s">
-        <v>143</v>
+        <v>100</v>
+      </c>
+      <c r="H91" t="s">
+        <v>608</v>
       </c>
       <c r="I91" t="s">
         <v>605</v>
       </c>
       <c r="J91" s="4" t="s">
-        <v>611</v>
-      </c>
-      <c r="K91" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B91&amp;" resources for the specified patient and date"</f>
-        <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient and date</v>
-      </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+        <v>609</v>
+      </c>
+      <c r="K91" t="str">
+        <f>"Fetches a bundle of all "&amp;B91&amp;" resources for the specified "&amp;SUBSTITUTE(D91,","," and  ") &amp; "= 'sdoh'"</f>
+        <v>Fetches a bundle of all !QuestionnaireResponse resources for the specified patient and  _tag= 'sdoh'</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>708</v>
+        <v>601</v>
       </c>
       <c r="C92" t="str">
         <f t="shared" si="4"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
-      </c>
-      <c r="D92" s="16" t="s">
-        <v>612</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
+      </c>
+      <c r="D92" t="s">
+        <v>610</v>
       </c>
       <c r="F92" t="s">
         <v>64</v>
       </c>
       <c r="G92" t="s">
-        <v>211</v>
-      </c>
-      <c r="H92" t="s">
-        <v>608</v>
+        <v>143</v>
       </c>
       <c r="I92" t="s">
         <v>605</v>
       </c>
       <c r="J92" s="4" t="s">
-        <v>613</v>
-      </c>
-      <c r="K92" t="str">
-        <f>"Fetches a bundle of all "&amp;B92&amp;" resources tagged as 'sdoh' for the specified patient and date"</f>
-        <v>Fetches a bundle of all !QuestionnaireResponse resources tagged as 'sdoh' for the specified patient and date</v>
-      </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+        <v>611</v>
+      </c>
+      <c r="K92" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B92&amp;" resources for the specified patient and date"</f>
+        <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient and date</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>601</v>
+        <v>707</v>
       </c>
       <c r="C93" t="str">
         <f t="shared" si="4"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="D93" s="16" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="F93" t="s">
         <v>64</v>
       </c>
       <c r="G93" t="s">
-        <v>85</v>
+        <v>211</v>
+      </c>
+      <c r="H93" t="s">
+        <v>608</v>
       </c>
       <c r="I93" t="s">
         <v>605</v>
       </c>
       <c r="J93" s="4" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="K93" t="str">
-        <f>"Fetches a bundle of all "&amp;B93&amp;" resources for the specified patient that have been completed against a specified form."</f>
-        <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient that have been completed against a specified form.</v>
-      </c>
-    </row>
-    <row r="94" spans="1:11" ht="151" customHeight="1" x14ac:dyDescent="0.2">
+        <f>"Fetches a bundle of all "&amp;B93&amp;" resources tagged as 'sdoh' for the specified patient and date"</f>
+        <v>Fetches a bundle of all !QuestionnaireResponse resources tagged as 'sdoh' for the specified patient and date</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>93</v>
       </c>
-      <c r="B94" s="16" t="s">
-        <v>641</v>
+      <c r="B94" t="s">
+        <v>601</v>
       </c>
       <c r="C94" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B94)</f>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</v>
+        <f t="shared" si="4"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D94" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="E94" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="F94" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="G94" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="H94" s="16"/>
-      <c r="I94" s="4" t="s">
-        <v>654</v>
+        <v>614</v>
+      </c>
+      <c r="F94" t="s">
+        <v>64</v>
+      </c>
+      <c r="G94" t="s">
+        <v>85</v>
+      </c>
+      <c r="I94" t="s">
+        <v>605</v>
       </c>
       <c r="J94" s="4" t="s">
-        <v>655</v>
+        <v>615</v>
       </c>
       <c r="K94" t="str">
-        <f>"Fetches a bundle of all "&amp;B94&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed))."</f>
-        <v>Fetches a bundle of all MedicationDispense resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed)).</v>
-      </c>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+        <f>"Fetches a bundle of all "&amp;B94&amp;" resources for the specified patient that have been completed against a specified form."</f>
+        <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient that have been completed against a specified form.</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" ht="151" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>94</v>
       </c>
@@ -12816,11 +12824,9 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</v>
       </c>
       <c r="D95" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="E95" s="16" t="s">
-        <v>51</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="E95" s="16"/>
       <c r="F95" s="16" t="s">
         <v>64</v>
       </c>
@@ -12829,61 +12835,133 @@
       </c>
       <c r="H95" s="16"/>
       <c r="I95" s="4" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="J95" s="4" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="K95" t="str">
-        <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed) and type of dispense (e.g., partially dispensed)."</f>
-        <v>Fetches a bundle of all MedicationDispense resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed) and type of dispense (e.g., partially dispensed).</v>
-      </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+        <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed))."</f>
+        <v>Fetches a bundle of all MedicationDispense resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed)).</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>95</v>
       </c>
       <c r="B96" s="16" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="C96" t="str">
         <f t="shared" si="4"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationdispense</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</v>
       </c>
       <c r="D96" s="16" t="s">
-        <v>658</v>
-      </c>
-      <c r="E96" s="16" t="s">
-        <v>51</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="E96" s="16"/>
       <c r="F96" s="16" t="s">
         <v>64</v>
       </c>
       <c r="G96" s="16" t="s">
-        <v>143</v>
+        <v>100</v>
       </c>
       <c r="H96" s="16"/>
       <c r="I96" s="4" t="s">
+        <v>655</v>
+      </c>
+      <c r="J96" s="4" t="s">
+        <v>656</v>
+      </c>
+      <c r="K96" t="str">
+        <f>"Fetches a bundle of all "&amp;B96&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed) and type of dispense (e.g., partially dispensed)."</f>
+        <v>Fetches a bundle of all MedicationDispense resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed) and type of dispense (e.g., partially dispensed).</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97" s="16" t="s">
+        <v>644</v>
+      </c>
+      <c r="C97" t="str">
+        <f t="shared" si="4"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationdispense</v>
+      </c>
+      <c r="D97" s="16" t="s">
+        <v>657</v>
+      </c>
+      <c r="E97" s="16"/>
+      <c r="F97" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="G97" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="H97" s="16"/>
+      <c r="I97" s="4" t="s">
+        <v>658</v>
+      </c>
+      <c r="J97" s="4" t="s">
         <v>659</v>
       </c>
-      <c r="J96" s="4" t="s">
-        <v>660</v>
-      </c>
-      <c r="K96" t="str">
-        <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient for a given dispense and date or range"</f>
+      <c r="K97" t="str">
+        <f>"Fetches a bundle of all "&amp;B96&amp;" resources for the specified patient for a given dispense and date or range"</f>
         <v>Fetches a bundle of all MedicationDispense resources for the specified patient for a given dispense and date or range</v>
       </c>
     </row>
+    <row r="98" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98" s="16" t="s">
+        <v>528</v>
+      </c>
+      <c r="C98" s="22" t="s">
+        <v>526</v>
+      </c>
+      <c r="D98" s="16" t="s">
+        <v>709</v>
+      </c>
+      <c r="E98" s="16" t="s">
+        <v>710</v>
+      </c>
+      <c r="F98" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="G98" s="16" t="s">
+        <v>711</v>
+      </c>
+      <c r="H98" s="16"/>
+      <c r="I98" s="4"/>
+      <c r="J98" s="4" t="s">
+        <v>712</v>
+      </c>
+      <c r="K98" t="str">
+        <f>"Fetches a bundle of all "&amp;B98&amp;" resources for the specified patient that may match any of the string fields in the name element (including family, give, prefix, suffix, suffix, and/or text)"</f>
+        <v>Fetches a bundle of all RelatedPerson resources for the specified patient that may match any of the string fields in the name element (including family, give, prefix, suffix, suffix, and/or text)</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:K96" xr:uid="{331E0B16-168F-459B-8951-3DF614BF0371}"/>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="!">
+  <autoFilter ref="A1:K98" xr:uid="{331E0B16-168F-459B-8951-3DF614BF0371}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Condition"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <conditionalFormatting sqref="B99:B1048576 B1:B97">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="C98" r:id="rId1" xr:uid="{0977E462-75F6-3C45-AA3B-490AE1C5558B}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -13038,7 +13116,7 @@
         <v>525</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="D2" t="s">
         <v>64</v>
@@ -13046,7 +13124,7 @@
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>520</v>
@@ -13231,10 +13309,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>675</v>
+      </c>
+      <c r="B7" t="s">
         <v>676</v>
-      </c>
-      <c r="B7" t="s">
-        <v>677</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
@@ -13385,7 +13463,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B18" t="s">
         <v>596</v>
@@ -13469,10 +13547,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>677</v>
+      </c>
+      <c r="B24" t="s">
         <v>678</v>
-      </c>
-      <c r="B24" t="s">
-        <v>679</v>
       </c>
       <c r="D24" t="s">
         <v>11</v>
@@ -13497,10 +13575,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>679</v>
+      </c>
+      <c r="B26" t="s">
         <v>680</v>
-      </c>
-      <c r="B26" t="s">
-        <v>681</v>
       </c>
       <c r="D26" t="s">
         <v>11</v>
@@ -13511,10 +13589,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>681</v>
+      </c>
+      <c r="B27" t="s">
         <v>682</v>
-      </c>
-      <c r="B27" t="s">
-        <v>683</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
@@ -13525,10 +13603,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>683</v>
+      </c>
+      <c r="B28" t="s">
         <v>684</v>
-      </c>
-      <c r="B28" t="s">
-        <v>685</v>
       </c>
       <c r="D28" t="s">
         <v>11</v>
@@ -13539,7 +13617,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="18" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B29" t="s">
         <v>597</v>
@@ -13567,10 +13645,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B31" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D31" t="s">
         <v>11</v>
@@ -13707,10 +13785,10 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="B41" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="D41" t="s">
         <v>11</v>
@@ -13735,7 +13813,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="18" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B43" t="s">
         <v>599</v>
@@ -13749,10 +13827,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B44" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="D44" t="s">
         <v>11</v>
@@ -13903,21 +13981,21 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="B55" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="D55" t="s">
         <v>11</v>
       </c>
       <c r="E55" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B56" t="s">
         <v>600</v>
@@ -13959,31 +14037,31 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="18" t="s">
+        <v>689</v>
+      </c>
+      <c r="B59" t="s">
         <v>690</v>
       </c>
-      <c r="B59" t="s">
+      <c r="D59" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59" t="s">
         <v>691</v>
-      </c>
-      <c r="D59" t="s">
-        <v>11</v>
-      </c>
-      <c r="E59" t="s">
-        <v>692</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A9">
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",A9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A55">
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",A55)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14213,7 +14291,7 @@
         <v>64</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="X8" s="13" t="s">
         <v>433</v>
@@ -14247,7 +14325,7 @@
         <v>64</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="X10" s="13" t="s">
         <v>433</v>
@@ -14400,7 +14478,7 @@
         <v>64</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="X19" s="13"/>
       <c r="Y19" s="13"/>
@@ -14449,18 +14527,18 @@
         <v>64</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="23" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B23" t="s">
         <v>64</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="X23" s="13"/>
       <c r="Y23" s="13"/>
@@ -14473,7 +14551,7 @@
         <v>64</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="X24" s="13" t="s">
         <v>433</v>
@@ -14531,7 +14609,7 @@
     <sortCondition ref="A2:A21"/>
   </sortState>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14604,7 +14682,7 @@
         <v>64</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -14708,7 +14786,7 @@
         <v>416</v>
       </c>
       <c r="Y1" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="Z1" t="s">
         <v>602</v>

</xml_diff>

<commit_message>
FHIR-41238 Typo change `Condition.onsetDate` to `Condition.onsetDateTime`
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93519112-5C7A-B24D-80E0-55CC8BD43649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F46AA277-B28D-354B-84CA-442464242326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2376,17 +2376,6 @@
     <t>resolves</t>
   </si>
   <si>
-    <t>* For Encounter Diagnosis use the *US Core Condition Encounter Diagnosis Profile*.
-    * When `Condition.category` is "encounter-diagnosis" the encounter, **SHOULD** be referenced in `Condition.encounter`.
-* For Problems and Health Concerns use the *US Core Condition Problems and Health Concerns Profile*.
-    * When `Condition.category` is a "problems-list-item", the `Condition.clinicalStatus **SHOULD NOT** be unknown.
-* There is no single element in Condition that represents the date of diagnosis. It may be the assertedDate Extension, `Condition.onsetDate`, or `Condition.recordedDate`.
-    * Although all three are marked as must support, the server is not required to support all.
-	* A server **SHALL** support `Condition.recordedDate`.
-    * A server **SHALL** support at least one of the assertedDate Extension and `Condition.onsetDate`. A server may support both, which means they support all 3 locations.
-    * The client application **SHALL** support all three elements.</t>
-  </si>
-  <si>
     <t>Media</t>
   </si>
   <si>
@@ -2438,6 +2427,17 @@
 - Observation: US Core Observation Screening Assessment Profile
 - Questionnaire/QuestionnaireResponse: SDC Base Questionnaire/US Core QuestionnaireResponse Profile
 US Core Servers **SHALL** suport US Core Observation Screening Assessment Profile and **SHOULD** support the  SDC Base Questionnaire Profile/US Core QuestionnaireResponse Profile</t>
+  </si>
+  <si>
+    <t>* For Encounter Diagnosis use the *US Core Condition Encounter Diagnosis Profile*.
+    * When `Condition.category` is "encounter-diagnosis" the encounter, **SHOULD** be referenced in `Condition.encounter`.
+* For Problems and Health Concerns use the *US Core Condition Problems and Health Concerns Profile*.
+    * When `Condition.category` is a "problems-list-item", the `Condition.clinicalStatus **SHOULD NOT** be unknown.
+* There is no single element in Condition that represents the date of diagnosis. It may be the assertedDate Extension, `Condition.onsetDateTime`, or `Condition.recordedDate`.
+    * Although all three are marked as must support, the server is not required to support all.
+	* A server **SHALL** support `Condition.recordedDate`.
+    * A server **SHALL** support at least one of the assertedDate Extension and `Condition.onsetDateTime`. A server may support both, which means they support all 3 locations.
+    * The client application **SHALL** support all three elements.</t>
   </si>
 </sst>
 </file>
@@ -14309,7 +14309,7 @@
         <v>64</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>715</v>
+        <v>730</v>
       </c>
       <c r="X5" s="13" t="s">
         <v>433</v>
@@ -14400,13 +14400,13 @@
     </row>
     <row r="11" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>725</v>
+      </c>
+      <c r="B11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="26" t="s">
         <v>726</v>
-      </c>
-      <c r="B11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C11" s="26" t="s">
-        <v>727</v>
       </c>
       <c r="T11" t="s">
         <v>714</v>
@@ -14436,13 +14436,13 @@
     </row>
     <row r="13" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>727</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="26" t="s">
         <v>728</v>
-      </c>
-      <c r="B13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="26" t="s">
-        <v>729</v>
       </c>
       <c r="T13" t="s">
         <v>714</v>
@@ -14485,13 +14485,13 @@
     </row>
     <row r="16" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>715</v>
+      </c>
+      <c r="B16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="26" t="s">
         <v>716</v>
-      </c>
-      <c r="B16" t="s">
-        <v>64</v>
-      </c>
-      <c r="C16" s="26" t="s">
-        <v>717</v>
       </c>
       <c r="X16" s="13"/>
       <c r="Y16" s="13"/>
@@ -14540,7 +14540,7 @@
         <v>64</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="V19" t="s">
         <v>64</v>
@@ -14633,7 +14633,7 @@
         <v>64</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="X24" s="13"/>
       <c r="Y24" s="13"/>
@@ -14693,7 +14693,7 @@
         <v>64</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="X28" s="13"/>
       <c r="Y28" s="13"/>
@@ -14706,7 +14706,7 @@
         <v>64</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="X29" s="13" t="s">
         <v>433</v>
@@ -14912,7 +14912,7 @@
         <v>353</v>
       </c>
       <c r="F1" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="G1" t="s">
         <v>354</v>
@@ -14930,13 +14930,13 @@
         <v>357</v>
       </c>
       <c r="L1" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="M1" t="s">
         <v>358</v>
       </c>
       <c r="N1" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="O1" t="s">
         <v>359</v>
@@ -14945,13 +14945,13 @@
         <v>360</v>
       </c>
       <c r="Q1" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="R1" t="s">
         <v>361</v>
       </c>
       <c r="S1" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="T1" t="s">
         <v>362</v>
@@ -14999,7 +14999,7 @@
         <v>432</v>
       </c>
       <c r="AI1" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add uscdi element Average Blood Pressure part 1
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B84FC9-4834-BB49-A517-FDBFC8BDD1AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C142AC2-1D48-B149-A52B-D5168B9669DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51760" yWindow="500" windowWidth="30240" windowHeight="18880" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="50700" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
     <sheet name="meta" sheetId="1" r:id="rId2"/>
     <sheet name="igs" sheetId="10" r:id="rId3"/>
     <sheet name="capstatements" sheetId="13" r:id="rId4"/>
-    <sheet name="profiles" sheetId="25" r:id="rId5"/>
-    <sheet name="resources" sheetId="31" r:id="rId6"/>
+    <sheet name="profiles" sheetId="33" r:id="rId5"/>
+    <sheet name="resources" sheetId="32" r:id="rId6"/>
     <sheet name="ops" sheetId="5" r:id="rId7"/>
     <sheet name="interactions" sheetId="6" r:id="rId8"/>
     <sheet name="rest_interactions" sheetId="11" r:id="rId9"/>
@@ -121,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2748" uniqueCount="731">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2753" uniqueCount="734">
   <si>
     <t>Element</t>
   </si>
@@ -2023,15 +2023,6 @@
   </si>
   <si>
     <t>* Based upon the ONC U.S. Core Data for Interoperability (USCDI) requirements, CVX vaccine codes are required and the NDC vaccine codes **SHOULD** be supported as translations to them.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Systems **SHOULD** support `Observation.effectivePeriod` to accurately represent tests that are collected over a period of time (for example, a 24-Hour Urine Collection test).
-* An Observation without a value, **SHALL** include a reason why the data is absent unless there are component observations, or references to other Observations that are grouped within it
-    * Systems that never provide an observation without a value are not required to support `Observation.dataAbsentReason`
-*  An `Observation.component` without a value, **SHALL** include a reason why the data is absent.
-    * Systems that never provide an component observation without a component value are not required to support `Observation.component.dataAbsentReason`.
-* Systems **SHOULD** support `Observation.effectivePeriod` to accurately represent procedure tests that are collected over a period of time.
-</t>
   </si>
   <si>
     <t>* Systems **SHALL** support National Provider Identifier (NPI) for organizations and **SHOULD** support Clinical Laboratory Improvement Amendments (CLIA) identifiers for `Organization.Identifier`.</t>
@@ -2263,9 +2254,6 @@
   </si>
   <si>
     <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-extension-questionnaire-uri</t>
   </si>
   <si>
     <t>Questionnaire</t>
@@ -2438,6 +2426,26 @@
 - Observation: US Core Observation Screening Assessment Profile
 - Questionnaire/QuestionnaireResponse: SDC Base Questionnaire/US Core QuestionnaireResponse Profile
 US Core Servers **SHALL** support US Core Observation Screening Assessment Profile and **SHOULD** support the  SDC Base Questionnaire Profile/US Core QuestionnaireResponse Profile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Systems **SHOULD** support `Observation.effectivePeriod` to accurately represent tests that are collected over a period of time (for example, a 24-Hour Urine Collection test).
+* An Observation without a value, **SHALL** include a reason why the data is absent unless there are component observations, or references to other Observations that are grouped within it
+    * Systems that never provide an observation without a value are not required to support `Observation.dataAbsentReason`
+*  An `Observation.component` without a value, **SHALL** include a reason why the data is absent.
+    * Systems that never provide an component observation without a component value are not required to support `Observation.component.dataAbsentReason`.
+</t>
+  </si>
+  <si>
+    <t>='[uscore-server.xlsx]profiles'!$A$64</t>
+  </si>
+  <si>
+    <t>!http://hl7.org/fhir/us/core/StructureDefinition/us-core-extension-questionnaire-uri</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-average-blood-pressure</t>
+  </si>
+  <si>
+    <t>US Core Average Blood Pressure Profile</t>
   </si>
 </sst>
 </file>
@@ -2607,7 +2615,7 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2641,7 +2649,6 @@
     <xf numFmtId="49" fontId="13" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -4445,7 +4452,7 @@
         <v>19</v>
       </c>
       <c r="C25" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="D25" t="s">
         <v>28</v>
@@ -4719,7 +4726,7 @@
         <v>51</v>
       </c>
       <c r="Y30" s="4" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="Z30" t="s">
         <v>167</v>
@@ -4741,7 +4748,7 @@
         <v>79</v>
       </c>
       <c r="C31" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="D31" t="s">
         <v>28</v>
@@ -4763,19 +4770,19 @@
         <v>52</v>
       </c>
       <c r="L31" t="s">
+        <v>632</v>
+      </c>
+      <c r="M31" t="s">
+        <v>51</v>
+      </c>
+      <c r="O31" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y31" s="4" t="s">
         <v>633</v>
       </c>
-      <c r="M31" t="s">
-        <v>51</v>
-      </c>
-      <c r="O31" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y31" s="4" t="s">
+      <c r="Z31" t="s">
         <v>634</v>
-      </c>
-      <c r="Z31" t="s">
-        <v>635</v>
       </c>
       <c r="AA31" s="8" t="str">
         <f>"Fetches a bundle of all "&amp;B31&amp;" resources matching the name"</f>
@@ -4791,7 +4798,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C32" t="s">
         <v>50</v>
@@ -4816,7 +4823,7 @@
         <v>52</v>
       </c>
       <c r="L32" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="M32" t="s">
         <v>51</v>
@@ -4834,7 +4841,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C33" t="s">
         <v>65</v>
@@ -4878,7 +4885,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C34" t="s">
         <v>62</v>
@@ -4925,7 +4932,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C35" t="s">
         <v>56</v>
@@ -4969,7 +4976,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C36" t="s">
         <v>57</v>
@@ -5025,7 +5032,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C37" t="s">
         <v>54</v>
@@ -5069,7 +5076,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C38" t="s">
         <v>61</v>
@@ -9269,7 +9276,7 @@
         <v>51</v>
       </c>
       <c r="Y115" s="4" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="Z115" s="4" t="str">
         <f>"GET [base]/"&amp;B115&amp;"?"&amp;C115&amp;"=Mary Shaw"</f>
@@ -9328,7 +9335,7 @@
         <v>support fetching a QuestionnaireResponse</v>
       </c>
       <c r="Z116" s="4" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="AB116" t="str">
         <f t="shared" si="9"/>
@@ -9440,7 +9447,7 @@
         <v>51</v>
       </c>
       <c r="Y118" s="19" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="AB118" t="str">
         <f t="shared" si="9"/>
@@ -9452,7 +9459,7 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="C119" t="s">
         <v>602</v>
@@ -9480,16 +9487,16 @@
         <v>52</v>
       </c>
       <c r="L119" t="s">
+        <v>666</v>
+      </c>
+      <c r="M119" t="s">
+        <v>51</v>
+      </c>
+      <c r="O119" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y119" s="19" t="s">
         <v>667</v>
-      </c>
-      <c r="M119" t="s">
-        <v>51</v>
-      </c>
-      <c r="O119" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y119" s="19" t="s">
-        <v>668</v>
       </c>
       <c r="AB119" t="str">
         <f t="shared" si="9"/>
@@ -9545,7 +9552,7 @@
         <v>87</v>
       </c>
       <c r="Y120" s="19" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="AB120" t="str">
         <f t="shared" si="9"/>
@@ -9595,7 +9602,7 @@
         <v>51</v>
       </c>
       <c r="Y121" s="19" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="AB121" t="str">
         <f t="shared" si="9"/>
@@ -9607,7 +9614,7 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C122" t="s">
         <v>84</v>
@@ -9645,7 +9652,7 @@
         <v>51</v>
       </c>
       <c r="Y122" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="Z122" s="4" t="str">
         <f>"GET [base]/"&amp;B122&amp;"?patient=1137192"</f>
@@ -9665,7 +9672,7 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C123" t="s">
         <v>56</v>
@@ -9718,7 +9725,7 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C124" t="s">
         <v>12</v>
@@ -9771,7 +9778,7 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C125" t="s">
         <v>84</v>
@@ -9809,10 +9816,10 @@
         <v>51</v>
       </c>
       <c r="X125" s="6" t="s">
+        <v>638</v>
+      </c>
+      <c r="Z125" s="8" t="s">
         <v>639</v>
-      </c>
-      <c r="Z125" s="8" t="s">
-        <v>640</v>
       </c>
       <c r="AA125" s="8" t="str">
         <f>"Fetches a bundle of all "&amp;B125&amp; " resources for the specified patient."</f>
@@ -9828,10 +9835,10 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
+        <v>640</v>
+      </c>
+      <c r="C126" t="s">
         <v>641</v>
-      </c>
-      <c r="C126" t="s">
-        <v>642</v>
       </c>
       <c r="D126" t="s">
         <v>28</v>
@@ -9882,7 +9889,7 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="C127" t="s">
         <v>50</v>
@@ -9920,7 +9927,7 @@
         <v>51</v>
       </c>
       <c r="Y127" s="4" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="Z127" s="4" t="str">
         <f>"GET [base]/"&amp;B127&amp;"?"&amp;C127&amp;"=123"</f>
@@ -9936,7 +9943,7 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="C128" t="s">
         <v>84</v>
@@ -9993,7 +10000,7 @@
   </sheetData>
   <autoFilter ref="A1:AB128" xr:uid="{1CF5B17E-E72E-48B2-A597-9C21C12723F0}"/>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10879,7 +10886,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D32" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="F32" t="s">
         <v>64</v>
@@ -10888,10 +10895,10 @@
         <v>128</v>
       </c>
       <c r="I32" s="4" t="s">
+        <v>643</v>
+      </c>
+      <c r="J32" s="4" t="s">
         <v>644</v>
-      </c>
-      <c r="J32" s="4" t="s">
-        <v>645</v>
       </c>
       <c r="K32" s="4" t="str">
         <f t="shared" si="1"/>
@@ -11021,7 +11028,7 @@
         <v>312</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
@@ -11066,7 +11073,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D38" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="E38" t="s">
         <v>51</v>
@@ -11081,13 +11088,13 @@
         <v>396</v>
       </c>
       <c r="I38" s="4" t="s">
+        <v>707</v>
+      </c>
+      <c r="J38" s="24" t="s">
+        <v>708</v>
+      </c>
+      <c r="K38" s="4" t="s">
         <v>709</v>
-      </c>
-      <c r="J38" s="25" t="s">
-        <v>710</v>
-      </c>
-      <c r="K38" s="4" t="s">
-        <v>711</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
@@ -11114,7 +11121,7 @@
         <v>144</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="K39" s="4" t="s">
         <v>555</v>
@@ -11370,7 +11377,7 @@
         <v>173</v>
       </c>
       <c r="C48" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D48" t="s">
         <v>110</v>
@@ -11400,7 +11407,7 @@
         <v>173</v>
       </c>
       <c r="C49" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D49" t="s">
         <v>139</v>
@@ -11433,7 +11440,7 @@
         <v>173</v>
       </c>
       <c r="C50" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D50" t="s">
         <v>141</v>
@@ -11463,7 +11470,7 @@
         <v>173</v>
       </c>
       <c r="C51" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D51" t="s">
         <v>188</v>
@@ -11496,7 +11503,7 @@
         <v>173</v>
       </c>
       <c r="C52" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D52" t="s">
         <v>212</v>
@@ -11874,7 +11881,7 @@
         <v>177</v>
       </c>
       <c r="C64" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="D64" t="s">
         <v>229</v>
@@ -11906,7 +11913,7 @@
         <v>177</v>
       </c>
       <c r="C65" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="D65" t="s">
         <v>139</v>
@@ -11939,7 +11946,7 @@
         <v>177</v>
       </c>
       <c r="C66" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="D66" t="s">
         <v>141</v>
@@ -11969,7 +11976,7 @@
         <v>177</v>
       </c>
       <c r="C67" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="D67" t="s">
         <v>188</v>
@@ -12002,7 +12009,7 @@
         <v>177</v>
       </c>
       <c r="C68" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="D68" t="s">
         <v>212</v>
@@ -12032,7 +12039,7 @@
         <v>304</v>
       </c>
       <c r="C69" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="D69" t="s">
         <v>110</v>
@@ -12411,7 +12418,7 @@
         <v>241</v>
       </c>
       <c r="C81" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="D81" t="s">
         <v>112</v>
@@ -12440,7 +12447,7 @@
         <v>241</v>
       </c>
       <c r="C82" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="D82" t="s">
         <v>110</v>
@@ -12452,13 +12459,13 @@
         <v>100</v>
       </c>
       <c r="I82" s="4" t="s">
+        <v>646</v>
+      </c>
+      <c r="J82" s="4" t="s">
         <v>647</v>
       </c>
-      <c r="J82" s="4" t="s">
+      <c r="K82" s="4" t="s">
         <v>648</v>
-      </c>
-      <c r="K82" s="4" t="s">
-        <v>649</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
@@ -12713,7 +12720,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="C91" t="str">
         <f t="shared" si="4"/>
@@ -12778,7 +12785,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="C93" t="str">
         <f t="shared" si="4"/>
@@ -12843,7 +12850,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="16" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C95" t="str">
         <f t="shared" si="4"/>
@@ -12861,10 +12868,10 @@
       </c>
       <c r="H95" s="16"/>
       <c r="I95" s="4" t="s">
+        <v>649</v>
+      </c>
+      <c r="J95" s="4" t="s">
         <v>650</v>
-      </c>
-      <c r="J95" s="4" t="s">
-        <v>651</v>
       </c>
       <c r="K95" t="str">
         <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed))."</f>
@@ -12876,7 +12883,7 @@
         <v>95</v>
       </c>
       <c r="B96" s="16" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C96" t="str">
         <f t="shared" si="4"/>
@@ -12894,10 +12901,10 @@
       </c>
       <c r="H96" s="16"/>
       <c r="I96" s="4" t="s">
+        <v>651</v>
+      </c>
+      <c r="J96" s="4" t="s">
         <v>652</v>
-      </c>
-      <c r="J96" s="4" t="s">
-        <v>653</v>
       </c>
       <c r="K96" t="str">
         <f>"Fetches a bundle of all "&amp;B96&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed) and type of dispense (e.g., partially dispensed)."</f>
@@ -12909,14 +12916,14 @@
         <v>96</v>
       </c>
       <c r="B97" s="16" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="C97" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationdispense</v>
       </c>
       <c r="D97" s="16" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="E97" s="16"/>
       <c r="F97" s="16" t="s">
@@ -12927,10 +12934,10 @@
       </c>
       <c r="H97" s="16"/>
       <c r="I97" s="4" t="s">
+        <v>654</v>
+      </c>
+      <c r="J97" s="4" t="s">
         <v>655</v>
-      </c>
-      <c r="J97" s="4" t="s">
-        <v>656</v>
       </c>
       <c r="K97" t="str">
         <f>"Fetches a bundle of all "&amp;B96&amp;" resources for the specified patient for a given dispense and date or range"</f>
@@ -12948,21 +12955,21 @@
         <v>525</v>
       </c>
       <c r="D98" s="16" t="s">
+        <v>702</v>
+      </c>
+      <c r="E98" s="16" t="s">
+        <v>703</v>
+      </c>
+      <c r="F98" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="G98" s="16" t="s">
         <v>704</v>
-      </c>
-      <c r="E98" s="16" t="s">
-        <v>705</v>
-      </c>
-      <c r="F98" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="G98" s="16" t="s">
-        <v>706</v>
       </c>
       <c r="H98" s="16"/>
       <c r="I98" s="4"/>
       <c r="J98" s="4" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="K98" t="str">
         <f>"Fetches a bundle of all "&amp;B98&amp;" resources for the specified patient that may match any of the string fields in the name element (including family, give, prefix, suffix, suffix, and/or text)"</f>
@@ -12972,7 +12979,7 @@
   </sheetData>
   <autoFilter ref="A1:K98" xr:uid="{331E0B16-168F-459B-8951-3DF614BF0371}"/>
   <conditionalFormatting sqref="B1:B97 B99:B1048576">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12990,7 +12997,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13136,7 +13143,7 @@
         <v>524</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="D2" t="s">
         <v>64</v>
@@ -13144,7 +13151,7 @@
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>519</v>
@@ -13224,11 +13231,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AF3E0BA-3FCD-D647-BD07-B7C9B2EC4519}">
-  <dimension ref="A1:E59"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBCBF51F-5B9F-2E4B-B3D8-96EF6A727C11}">
+  <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView topLeftCell="A41" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13301,7 +13308,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B5" t="s">
         <v>615</v>
@@ -13315,7 +13322,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B6" t="s">
         <v>616</v>
@@ -13329,16 +13336,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>670</v>
+      </c>
+      <c r="B7" t="s">
         <v>671</v>
       </c>
-      <c r="B7" t="s">
-        <v>672</v>
-      </c>
       <c r="D7" t="s">
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -13399,7 +13406,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B12" t="s">
         <v>347</v>
@@ -13481,9 +13488,9 @@
         <v>586</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="23" t="s">
-        <v>694</v>
+    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="20" t="s">
+        <v>731</v>
       </c>
       <c r="B18" t="s">
         <v>595</v>
@@ -13567,16 +13574,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>672</v>
+      </c>
+      <c r="B24" t="s">
         <v>673</v>
       </c>
-      <c r="B24" t="s">
-        <v>674</v>
-      </c>
       <c r="D24" t="s">
         <v>11</v>
       </c>
       <c r="E24" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -13595,10 +13602,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>674</v>
+      </c>
+      <c r="B26" t="s">
         <v>675</v>
-      </c>
-      <c r="B26" t="s">
-        <v>676</v>
       </c>
       <c r="D26" t="s">
         <v>11</v>
@@ -13609,10 +13616,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>676</v>
+      </c>
+      <c r="B27" t="s">
         <v>677</v>
-      </c>
-      <c r="B27" t="s">
-        <v>678</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
@@ -13623,10 +13630,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>678</v>
+      </c>
+      <c r="B28" t="s">
         <v>679</v>
-      </c>
-      <c r="B28" t="s">
-        <v>680</v>
       </c>
       <c r="D28" t="s">
         <v>11</v>
@@ -13637,7 +13644,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="18" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B29" t="s">
         <v>596</v>
@@ -13665,10 +13672,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B31" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="D31" t="s">
         <v>11</v>
@@ -13805,10 +13812,10 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B41" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="D41" t="s">
         <v>11</v>
@@ -13818,11 +13825,11 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="18" t="s">
-        <v>457</v>
+      <c r="A42" t="s">
+        <v>732</v>
       </c>
       <c r="B42" t="s">
-        <v>458</v>
+        <v>733</v>
       </c>
       <c r="D42" t="s">
         <v>11</v>
@@ -13833,10 +13840,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="18" t="s">
-        <v>683</v>
+        <v>457</v>
       </c>
       <c r="B43" t="s">
-        <v>598</v>
+        <v>458</v>
       </c>
       <c r="D43" t="s">
         <v>11</v>
@@ -13846,11 +13853,11 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>684</v>
+      <c r="A44" s="18" t="s">
+        <v>682</v>
       </c>
       <c r="B44" t="s">
-        <v>691</v>
+        <v>598</v>
       </c>
       <c r="D44" t="s">
         <v>11</v>
@@ -13860,11 +13867,11 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="18" t="s">
-        <v>480</v>
+      <c r="A45" t="s">
+        <v>683</v>
       </c>
       <c r="B45" t="s">
-        <v>481</v>
+        <v>690</v>
       </c>
       <c r="D45" t="s">
         <v>11</v>
@@ -13875,10 +13882,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="18" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B46" t="s">
-        <v>628</v>
+        <v>481</v>
       </c>
       <c r="D46" t="s">
         <v>11</v>
@@ -13889,10 +13896,10 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="18" t="s">
-        <v>465</v>
+        <v>478</v>
       </c>
       <c r="B47" t="s">
-        <v>466</v>
+        <v>627</v>
       </c>
       <c r="D47" t="s">
         <v>11</v>
@@ -13903,10 +13910,10 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="18" t="s">
-        <v>455</v>
+        <v>465</v>
       </c>
       <c r="B48" t="s">
-        <v>456</v>
+        <v>466</v>
       </c>
       <c r="D48" t="s">
         <v>11</v>
@@ -13917,178 +13924,189 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="18" t="s">
-        <v>330</v>
+        <v>455</v>
       </c>
       <c r="B49" t="s">
-        <v>331</v>
+        <v>456</v>
       </c>
       <c r="D49" t="s">
         <v>11</v>
       </c>
       <c r="E49" t="s">
-        <v>252</v>
+        <v>177</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="18" t="s">
-        <v>69</v>
+        <v>330</v>
       </c>
       <c r="B50" t="s">
-        <v>346</v>
+        <v>331</v>
       </c>
       <c r="D50" t="s">
         <v>11</v>
       </c>
       <c r="E50" t="s">
-        <v>19</v>
+        <v>252</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="18" t="s">
-        <v>321</v>
+        <v>69</v>
       </c>
       <c r="B51" t="s">
-        <v>322</v>
+        <v>346</v>
       </c>
       <c r="D51" t="s">
         <v>11</v>
       </c>
       <c r="E51" t="s">
-        <v>259</v>
+        <v>19</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="18" t="s">
-        <v>338</v>
+        <v>321</v>
       </c>
       <c r="B52" t="s">
-        <v>339</v>
+        <v>322</v>
       </c>
       <c r="D52" t="s">
         <v>11</v>
       </c>
       <c r="E52" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="18" t="s">
-        <v>332</v>
+        <v>338</v>
       </c>
       <c r="B53" t="s">
-        <v>333</v>
+        <v>339</v>
       </c>
       <c r="D53" t="s">
         <v>11</v>
       </c>
       <c r="E53" t="s">
-        <v>176</v>
+        <v>261</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="18" t="s">
+        <v>332</v>
+      </c>
+      <c r="B54" t="s">
+        <v>333</v>
+      </c>
+      <c r="D54" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" s="18" t="s">
         <v>413</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" t="s">
         <v>414</v>
       </c>
-      <c r="D54" t="s">
-        <v>11</v>
-      </c>
-      <c r="E54" t="s">
+      <c r="D55" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" t="s">
         <v>415</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>692</v>
-      </c>
-      <c r="B55" t="s">
-        <v>697</v>
-      </c>
-      <c r="D55" t="s">
-        <v>11</v>
-      </c>
-      <c r="E55" t="s">
-        <v>695</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>691</v>
+      </c>
+      <c r="B56" t="s">
+        <v>695</v>
+      </c>
+      <c r="D56" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" t="s">
         <v>693</v>
       </c>
-      <c r="B56" t="s">
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>692</v>
+      </c>
+      <c r="B57" t="s">
         <v>599</v>
       </c>
-      <c r="D56" t="s">
-        <v>11</v>
-      </c>
-      <c r="E56" t="s">
+      <c r="D57" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57" t="s">
         <v>600</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" s="18" t="s">
-        <v>525</v>
-      </c>
-      <c r="B57" t="s">
-        <v>526</v>
-      </c>
-      <c r="D57" t="s">
-        <v>11</v>
-      </c>
-      <c r="E57" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="18" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="B58" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="D58" t="s">
         <v>11</v>
       </c>
       <c r="E58" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="18" t="s">
+        <v>528</v>
+      </c>
+      <c r="B59" t="s">
+        <v>529</v>
+      </c>
+      <c r="D59" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>684</v>
+      </c>
+      <c r="B60" t="s">
         <v>685</v>
       </c>
-      <c r="B59" t="s">
+      <c r="D60" t="s">
+        <v>11</v>
+      </c>
+      <c r="E60" t="s">
         <v>686</v>
-      </c>
-      <c r="D59" t="s">
-        <v>11</v>
-      </c>
-      <c r="E59" t="s">
-        <v>687</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <hyperlinks>
-    <hyperlink ref="A18" r:id="rId1" xr:uid="{EB703517-1E0F-514C-9C3F-F3364468974B}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B8A3D0-39EC-EF46-8CF3-3AA444A18DC6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9ACEDC0-A695-4042-BE38-A780F3DE9AE3}">
   <dimension ref="A1:Y69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -14195,7 +14213,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="T2" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="U2" t="s">
         <v>64</v>
@@ -14218,7 +14236,7 @@
         <v>474</v>
       </c>
       <c r="T3" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="U3" t="s">
         <v>64</v>
@@ -14241,7 +14259,7 @@
         <v>619</v>
       </c>
       <c r="T4" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="U4" t="s">
         <v>64</v>
@@ -14267,10 +14285,10 @@
         <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="T5" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="U5" t="s">
         <v>64</v>
@@ -14284,13 +14302,13 @@
     </row>
     <row r="6" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="T6" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="U6" t="s">
         <v>64</v>
@@ -14313,7 +14331,7 @@
         <v>620</v>
       </c>
       <c r="T7" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="U7" t="s">
         <v>64</v>
@@ -14334,7 +14352,7 @@
       </c>
       <c r="C8" s="2"/>
       <c r="T8" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="U8" t="s">
         <v>64</v>
@@ -14354,10 +14372,10 @@
         <v>11</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="T9" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="U9" t="s">
         <v>64</v>
@@ -14377,10 +14395,10 @@
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="T10" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="U10" t="s">
         <v>64</v>
@@ -14394,16 +14412,16 @@
     </row>
     <row r="11" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="26" t="s">
-        <v>724</v>
+      <c r="C11" s="25" t="s">
+        <v>722</v>
       </c>
       <c r="T11" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="U11" t="s">
         <v>64</v>
@@ -14419,10 +14437,10 @@
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="T12" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="U12" t="s">
         <v>64</v>
@@ -14436,16 +14454,16 @@
     </row>
     <row r="13" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="B13" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="26" t="s">
-        <v>726</v>
+      <c r="C13" s="25" t="s">
+        <v>724</v>
       </c>
       <c r="T13" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="U13" t="s">
         <v>64</v>
@@ -14464,7 +14482,7 @@
         <v>621</v>
       </c>
       <c r="T14" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="U14" t="s">
         <v>64</v>
@@ -14484,7 +14502,7 @@
         <v>11</v>
       </c>
       <c r="T15" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="U15" t="s">
         <v>64</v>
@@ -14494,16 +14512,16 @@
     </row>
     <row r="16" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="B16" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="26" t="s">
-        <v>714</v>
+      <c r="C16" s="25" t="s">
+        <v>712</v>
       </c>
       <c r="T16" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="U16" t="s">
         <v>64</v>
@@ -14522,7 +14540,7 @@
         <v>475</v>
       </c>
       <c r="T17" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="U17" t="s">
         <v>64</v>
@@ -14541,7 +14559,7 @@
         <v>476</v>
       </c>
       <c r="T18" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="U18" t="s">
         <v>64</v>
@@ -14561,25 +14579,25 @@
     </row>
     <row r="19" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>637</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="T19" t="s">
+        <v>710</v>
+      </c>
+      <c r="U19" t="s">
+        <v>64</v>
+      </c>
+      <c r="V19" t="s">
+        <v>64</v>
+      </c>
+      <c r="W19" s="6" t="s">
         <v>638</v>
-      </c>
-      <c r="B19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>715</v>
-      </c>
-      <c r="T19" t="s">
-        <v>712</v>
-      </c>
-      <c r="U19" t="s">
-        <v>64</v>
-      </c>
-      <c r="V19" t="s">
-        <v>64</v>
-      </c>
-      <c r="W19" s="6" t="s">
-        <v>639</v>
       </c>
       <c r="X19" s="13" t="s">
         <v>433</v>
@@ -14599,7 +14617,7 @@
         <v>477</v>
       </c>
       <c r="T20" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="U20" t="s">
         <v>64</v>
@@ -14625,10 +14643,10 @@
         <v>11</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>622</v>
+        <v>729</v>
       </c>
       <c r="T21" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="U21" t="s">
         <v>64</v>
@@ -14648,10 +14666,10 @@
         <v>11</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="T22" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="U22" t="s">
         <v>64</v>
@@ -14667,10 +14685,10 @@
         <v>11</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="T23" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="U23" t="s">
         <v>64</v>
@@ -14690,10 +14708,10 @@
         <v>11</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="T24" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="U24" t="s">
         <v>64</v>
@@ -14709,10 +14727,10 @@
         <v>11</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="T25" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="U25" t="s">
         <v>64</v>
@@ -14734,10 +14752,10 @@
         <v>11</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="T26" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="U26" t="s">
         <v>64</v>
@@ -14757,10 +14775,10 @@
         <v>11</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="T27" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="U27" t="s">
         <v>64</v>
@@ -14768,13 +14786,13 @@
     </row>
     <row r="28" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="B28" t="s">
         <v>64</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="X28" s="13"/>
       <c r="Y28" s="13"/>
@@ -14787,7 +14805,7 @@
         <v>64</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="X29" s="13" t="s">
         <v>433</v>
@@ -14804,7 +14822,7 @@
         <v>11</v>
       </c>
       <c r="T30" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="U30" t="s">
         <v>64</v>
@@ -14824,7 +14842,7 @@
         <v>11</v>
       </c>
       <c r="T31" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="U31" t="s">
         <v>64</v>
@@ -14838,13 +14856,13 @@
     </row>
     <row r="32" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B32" t="s">
         <v>11</v>
       </c>
       <c r="T32" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="U32" t="s">
         <v>64</v>
@@ -14858,6 +14876,11 @@
       </c>
       <c r="B33" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>730</v>
       </c>
     </row>
     <row r="66" spans="22:25" ht="21" customHeight="1" x14ac:dyDescent="0.2">
@@ -14870,7 +14893,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14942,8 +14965,8 @@
       <c r="D3" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="24" t="s">
-        <v>700</v>
+      <c r="E3" s="23" t="s">
+        <v>698</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -14996,7 +15019,7 @@
         <v>353</v>
       </c>
       <c r="F1" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="G1" t="s">
         <v>354</v>
@@ -15014,13 +15037,13 @@
         <v>357</v>
       </c>
       <c r="L1" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="M1" t="s">
         <v>358</v>
       </c>
       <c r="N1" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="O1" t="s">
         <v>359</v>
@@ -15029,13 +15052,13 @@
         <v>360</v>
       </c>
       <c r="Q1" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="R1" t="s">
         <v>361</v>
       </c>
       <c r="S1" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="T1" t="s">
         <v>362</v>
@@ -15068,7 +15091,7 @@
         <v>416</v>
       </c>
       <c r="AD1" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="AE1" t="s">
         <v>601</v>
@@ -15083,7 +15106,7 @@
         <v>432</v>
       </c>
       <c r="AI1" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add USCDI Goals and Preferences part 1
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C142AC2-1D48-B149-A52B-D5168B9669DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6AAD4F7-0A4B-7D49-800A-6A9737C4E73E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50700" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="50700" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
     <sheet name="meta" sheetId="1" r:id="rId2"/>
     <sheet name="igs" sheetId="10" r:id="rId3"/>
     <sheet name="capstatements" sheetId="13" r:id="rId4"/>
-    <sheet name="profiles" sheetId="33" r:id="rId5"/>
+    <sheet name="profiles" sheetId="34" r:id="rId5"/>
     <sheet name="resources" sheetId="32" r:id="rId6"/>
     <sheet name="ops" sheetId="5" r:id="rId7"/>
     <sheet name="interactions" sheetId="6" r:id="rId8"/>
@@ -121,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2753" uniqueCount="734">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2761" uniqueCount="738">
   <si>
     <t>Element</t>
   </si>
@@ -2446,6 +2446,18 @@
   </si>
   <si>
     <t>US Core Average Blood Pressure Profile</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-treatment-intervention-preference</t>
+  </si>
+  <si>
+    <t>US Core Treatment Intervention Preference Profile</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-care-experience-preference</t>
+  </si>
+  <si>
+    <t>US Core Care Experience Preference Profile</t>
   </si>
 </sst>
 </file>
@@ -10000,7 +10012,7 @@
   </sheetData>
   <autoFilter ref="A1:AB128" xr:uid="{1CF5B17E-E72E-48B2-A597-9C21C12723F0}"/>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12979,7 +12991,7 @@
   </sheetData>
   <autoFilter ref="A1:K98" xr:uid="{331E0B16-168F-459B-8951-3DF614BF0371}"/>
   <conditionalFormatting sqref="B1:B97 B99:B1048576">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13231,11 +13243,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBCBF51F-5B9F-2E4B-B3D8-96EF6A727C11}">
-  <dimension ref="A1:E60"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CECBDE16-5B3B-D24D-8161-5797A7035D04}">
+  <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13685,11 +13697,11 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="18" t="s">
-        <v>469</v>
+      <c r="A32" t="s">
+        <v>734</v>
       </c>
       <c r="B32" t="s">
-        <v>470</v>
+        <v>735</v>
       </c>
       <c r="D32" t="s">
         <v>11</v>
@@ -13699,11 +13711,11 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="18" t="s">
-        <v>467</v>
+      <c r="A33" t="s">
+        <v>736</v>
       </c>
       <c r="B33" t="s">
-        <v>468</v>
+        <v>737</v>
       </c>
       <c r="D33" t="s">
         <v>11</v>
@@ -13714,10 +13726,10 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="18" t="s">
-        <v>482</v>
+        <v>469</v>
       </c>
       <c r="B34" t="s">
-        <v>483</v>
+        <v>470</v>
       </c>
       <c r="D34" t="s">
         <v>11</v>
@@ -13728,10 +13740,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="18" t="s">
-        <v>411</v>
+        <v>467</v>
       </c>
       <c r="B35" t="s">
-        <v>412</v>
+        <v>468</v>
       </c>
       <c r="D35" t="s">
         <v>11</v>
@@ -13742,10 +13754,10 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="18" t="s">
-        <v>267</v>
+        <v>482</v>
       </c>
       <c r="B36" t="s">
-        <v>325</v>
+        <v>483</v>
       </c>
       <c r="D36" t="s">
         <v>11</v>
@@ -13756,10 +13768,10 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="18" t="s">
-        <v>522</v>
+        <v>411</v>
       </c>
       <c r="B37" t="s">
-        <v>597</v>
+        <v>412</v>
       </c>
       <c r="D37" t="s">
         <v>11</v>
@@ -13770,10 +13782,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="18" t="s">
-        <v>461</v>
+        <v>267</v>
       </c>
       <c r="B38" t="s">
-        <v>462</v>
+        <v>325</v>
       </c>
       <c r="D38" t="s">
         <v>11</v>
@@ -13784,10 +13796,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="18" t="s">
-        <v>463</v>
+        <v>522</v>
       </c>
       <c r="B39" t="s">
-        <v>464</v>
+        <v>597</v>
       </c>
       <c r="D39" t="s">
         <v>11</v>
@@ -13798,10 +13810,10 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="18" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="B40" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="D40" t="s">
         <v>11</v>
@@ -13811,11 +13823,11 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>687</v>
+      <c r="A41" s="18" t="s">
+        <v>463</v>
       </c>
       <c r="B41" t="s">
-        <v>689</v>
+        <v>464</v>
       </c>
       <c r="D41" t="s">
         <v>11</v>
@@ -13825,11 +13837,11 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>732</v>
+      <c r="A42" s="18" t="s">
+        <v>459</v>
       </c>
       <c r="B42" t="s">
-        <v>733</v>
+        <v>460</v>
       </c>
       <c r="D42" t="s">
         <v>11</v>
@@ -13839,11 +13851,11 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="18" t="s">
-        <v>457</v>
+      <c r="A43" t="s">
+        <v>687</v>
       </c>
       <c r="B43" t="s">
-        <v>458</v>
+        <v>689</v>
       </c>
       <c r="D43" t="s">
         <v>11</v>
@@ -13853,11 +13865,11 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="18" t="s">
-        <v>682</v>
+      <c r="A44" t="s">
+        <v>732</v>
       </c>
       <c r="B44" t="s">
-        <v>598</v>
+        <v>733</v>
       </c>
       <c r="D44" t="s">
         <v>11</v>
@@ -13867,11 +13879,11 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>683</v>
+      <c r="A45" s="18" t="s">
+        <v>457</v>
       </c>
       <c r="B45" t="s">
-        <v>690</v>
+        <v>458</v>
       </c>
       <c r="D45" t="s">
         <v>11</v>
@@ -13882,10 +13894,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="18" t="s">
-        <v>480</v>
+        <v>682</v>
       </c>
       <c r="B46" t="s">
-        <v>481</v>
+        <v>598</v>
       </c>
       <c r="D46" t="s">
         <v>11</v>
@@ -13895,11 +13907,11 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="18" t="s">
-        <v>478</v>
+      <c r="A47" t="s">
+        <v>683</v>
       </c>
       <c r="B47" t="s">
-        <v>627</v>
+        <v>690</v>
       </c>
       <c r="D47" t="s">
         <v>11</v>
@@ -13910,10 +13922,10 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="18" t="s">
-        <v>465</v>
+        <v>480</v>
       </c>
       <c r="B48" t="s">
-        <v>466</v>
+        <v>481</v>
       </c>
       <c r="D48" t="s">
         <v>11</v>
@@ -13924,10 +13936,10 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="18" t="s">
-        <v>455</v>
+        <v>478</v>
       </c>
       <c r="B49" t="s">
-        <v>456</v>
+        <v>627</v>
       </c>
       <c r="D49" t="s">
         <v>11</v>
@@ -13938,155 +13950,183 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="18" t="s">
-        <v>330</v>
+        <v>465</v>
       </c>
       <c r="B50" t="s">
-        <v>331</v>
+        <v>466</v>
       </c>
       <c r="D50" t="s">
         <v>11</v>
       </c>
       <c r="E50" t="s">
-        <v>252</v>
+        <v>177</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="18" t="s">
-        <v>69</v>
+        <v>455</v>
       </c>
       <c r="B51" t="s">
-        <v>346</v>
+        <v>456</v>
       </c>
       <c r="D51" t="s">
         <v>11</v>
       </c>
       <c r="E51" t="s">
-        <v>19</v>
+        <v>177</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="18" t="s">
-        <v>321</v>
+        <v>330</v>
       </c>
       <c r="B52" t="s">
-        <v>322</v>
+        <v>331</v>
       </c>
       <c r="D52" t="s">
         <v>11</v>
       </c>
       <c r="E52" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="18" t="s">
-        <v>338</v>
+        <v>69</v>
       </c>
       <c r="B53" t="s">
-        <v>339</v>
+        <v>346</v>
       </c>
       <c r="D53" t="s">
         <v>11</v>
       </c>
       <c r="E53" t="s">
-        <v>261</v>
+        <v>19</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="18" t="s">
-        <v>332</v>
+        <v>321</v>
       </c>
       <c r="B54" t="s">
-        <v>333</v>
+        <v>322</v>
       </c>
       <c r="D54" t="s">
         <v>11</v>
       </c>
       <c r="E54" t="s">
-        <v>176</v>
+        <v>259</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="18" t="s">
+        <v>338</v>
+      </c>
+      <c r="B55" t="s">
+        <v>339</v>
+      </c>
+      <c r="D55" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" s="18" t="s">
+        <v>332</v>
+      </c>
+      <c r="B56" t="s">
+        <v>333</v>
+      </c>
+      <c r="D56" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" s="18" t="s">
         <v>413</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B57" t="s">
         <v>414</v>
       </c>
-      <c r="D55" t="s">
-        <v>11</v>
-      </c>
-      <c r="E55" t="s">
+      <c r="D57" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>691</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B58" t="s">
         <v>695</v>
       </c>
-      <c r="D56" t="s">
-        <v>11</v>
-      </c>
-      <c r="E56" t="s">
+      <c r="D58" t="s">
+        <v>11</v>
+      </c>
+      <c r="E58" t="s">
         <v>693</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>692</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B59" t="s">
         <v>599</v>
       </c>
-      <c r="D57" t="s">
-        <v>11</v>
-      </c>
-      <c r="E57" t="s">
+      <c r="D59" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59" t="s">
         <v>600</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" s="18" t="s">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" s="18" t="s">
         <v>525</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B60" t="s">
         <v>526</v>
       </c>
-      <c r="D58" t="s">
-        <v>11</v>
-      </c>
-      <c r="E58" t="s">
+      <c r="D60" t="s">
+        <v>11</v>
+      </c>
+      <c r="E60" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" s="18" t="s">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" s="18" t="s">
         <v>528</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B61" t="s">
         <v>529</v>
       </c>
-      <c r="D59" t="s">
-        <v>11</v>
-      </c>
-      <c r="E59" t="s">
+      <c r="D61" t="s">
+        <v>11</v>
+      </c>
+      <c r="E61" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>684</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B62" t="s">
         <v>685</v>
       </c>
-      <c r="D60" t="s">
-        <v>11</v>
-      </c>
-      <c r="E60" t="s">
+      <c r="D62" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" t="s">
         <v>686</v>
       </c>
     </row>
@@ -14105,7 +14145,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9ACEDC0-A695-4042-BE38-A780F3DE9AE3}">
   <dimension ref="A1:Y69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
@@ -14893,7 +14933,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",A1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update approach to flagging Additional USCDI Requirements FHIR-41572, Add Procedure.reasonCode and Procedure.reasonReference as Reason for Referral FHIR-42136
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6AAD4F7-0A4B-7D49-800A-6A9737C4E73E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE6467C-4517-C148-B430-6C2CE2BB268D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50700" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="50700" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="igs" sheetId="10" r:id="rId3"/>
     <sheet name="capstatements" sheetId="13" r:id="rId4"/>
     <sheet name="profiles" sheetId="34" r:id="rId5"/>
-    <sheet name="resources" sheetId="32" r:id="rId6"/>
+    <sheet name="resources" sheetId="35" r:id="rId6"/>
     <sheet name="ops" sheetId="5" r:id="rId7"/>
     <sheet name="interactions" sheetId="6" r:id="rId8"/>
     <sheet name="rest_interactions" sheetId="11" r:id="rId9"/>
@@ -2041,11 +2041,6 @@
 * The Patient's Social Security Numbers **SHOULD NOT** be used as a patient identifier in `Patient.identifier.value`.</t>
   </si>
   <si>
-    <t>* Procedure codes can be taken from SNOMED-CT, CPT, HCPCS II, ICD-10-PCS, CDT. LOINC.
-  * Only LOINC concepts that reflect actual procedures **SHOULD** be used
-* A procedure including an implantable device **SHOULD** use `Procedure.focalDevice` with a reference to the *US Core Implantable Device Profile*.</t>
-  </si>
-  <si>
     <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition-encounter-diagnosis</t>
   </si>
   <si>
@@ -2436,9 +2431,6 @@
 </t>
   </si>
   <si>
-    <t>='[uscore-server.xlsx]profiles'!$A$64</t>
-  </si>
-  <si>
     <t>!http://hl7.org/fhir/us/core/StructureDefinition/us-core-extension-questionnaire-uri</t>
   </si>
   <si>
@@ -2458,6 +2450,29 @@
   </si>
   <si>
     <t>US Core Care Experience Preference Profile</t>
+  </si>
+  <si>
+    <t>* Procedure codes can be taken from SNOMED-CT, CPT, HCPCS II, ICD-10-PCS, CDT. LOINC.
+  * Only LOINC concepts that reflect actual procedures **SHOULD** be used
+* A procedure including an implantable device **SHOULD** use `Procedure.focalDevice` with a reference to the *US Core Implantable Device Profile*.
+* The Reason or justification for a referral or consultation is communicated through:
+  1. `ServiceRequest.reason` or `ServiceRequest.reason`, and `Procedure.basedOn` that links the Procedure to the US Core ServiceRequest Profile.
+     - `ServiceRequest.reasonCode` and `ServiceRequest.reasonReference` are marked as Additional USCDI Requirements. The certifying server system is not required to support both but **SHALL** support at least one of these elements. The certifying client application **SHALL** support both elements.
+     - As documented [here](general-guidance.html#referencing-us-core-profiles), when using  `ServiceRequest.reasonReference`, the referenced resources **SHOULD** be a US Core Profile.
+  1. `Procedure.reasonCode` or `Procedure.reasonReference` when the Procedure does not have an associated ServiceRequest.
+     - Although both `Procedure.reasonCode` and `Procedure.reasonReference` are marked as Additional USCDI Requirements. The certifying server system is not required to support both but **SHALL** support at least one of these elements. The certifying client application **SHALL** support both elements.
+     - As documented [here](general-guidance.html#referencing-us-core-profiles), when using  `Procedure.reasonReference`, the referenced resources **SHOULD** be a US Core Profile.
+    Certifying Servers and Clients **SHALL** support options 1 and 2 as Additional USCDI Requirements.</t>
+  </si>
+  <si>
+    <t>* The Reason or justification for a referral or consultation is communicated through:
+  1. `ServiceRequest.reason` or `ServiceRequest.reason`, and `Procedure.basedOn` that links the Procedure to the US Core ServiceRequest Profile.
+     - `ServiceRequest.reasonCode` and `ServiceRequest.reasonReference` are marked as Additional USCDI Requirements. The certifying server system is not required to support both but **SHALL** support at least one of these elements. The certifying client application **SHALL** support both elements.
+     - As documented [here](general-guidance.html#referencing-us-core-profiles), when using  `ServiceRequest.reasonReference`, the referenced resources **SHOULD** be a US Core Profile.
+  1. `Procedure.reasonCode` or `Procedure.reasonReference` when the Procedure does not have an associated ServiceRequest.
+     - Although both `Procedure.reasonCode` and `Procedure.reasonReference` are marked as Additional USCDI Requirements. The certifying server system is not required to support both but **SHALL** support at least one of these elements. The certifying client application **SHALL** support both elements.
+     - As documented [here](general-guidance.html#referencing-us-core-profiles), when using  `Procedure.reasonReference`, the referenced resources **SHOULD** be a US Core Profile.
+    Certifying Servers and Clients **SHALL** support options 1 and 2 as Additional USCDI Requirements.</t>
   </si>
 </sst>
 </file>
@@ -4464,7 +4479,7 @@
         <v>19</v>
       </c>
       <c r="C25" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="D25" t="s">
         <v>28</v>
@@ -4738,7 +4753,7 @@
         <v>51</v>
       </c>
       <c r="Y30" s="4" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="Z30" t="s">
         <v>167</v>
@@ -4760,7 +4775,7 @@
         <v>79</v>
       </c>
       <c r="C31" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="D31" t="s">
         <v>28</v>
@@ -4782,19 +4797,19 @@
         <v>52</v>
       </c>
       <c r="L31" t="s">
+        <v>631</v>
+      </c>
+      <c r="M31" t="s">
+        <v>51</v>
+      </c>
+      <c r="O31" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y31" s="4" t="s">
         <v>632</v>
       </c>
-      <c r="M31" t="s">
-        <v>51</v>
-      </c>
-      <c r="O31" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y31" s="4" t="s">
+      <c r="Z31" t="s">
         <v>633</v>
-      </c>
-      <c r="Z31" t="s">
-        <v>634</v>
       </c>
       <c r="AA31" s="8" t="str">
         <f>"Fetches a bundle of all "&amp;B31&amp;" resources matching the name"</f>
@@ -4810,7 +4825,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C32" t="s">
         <v>50</v>
@@ -4835,7 +4850,7 @@
         <v>52</v>
       </c>
       <c r="L32" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="M32" t="s">
         <v>51</v>
@@ -4853,7 +4868,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C33" t="s">
         <v>65</v>
@@ -4897,7 +4912,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C34" t="s">
         <v>62</v>
@@ -4944,7 +4959,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C35" t="s">
         <v>56</v>
@@ -4988,7 +5003,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C36" t="s">
         <v>57</v>
@@ -5044,7 +5059,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C37" t="s">
         <v>54</v>
@@ -5088,7 +5103,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C38" t="s">
         <v>61</v>
@@ -9288,7 +9303,7 @@
         <v>51</v>
       </c>
       <c r="Y115" s="4" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="Z115" s="4" t="str">
         <f>"GET [base]/"&amp;B115&amp;"?"&amp;C115&amp;"=Mary Shaw"</f>
@@ -9347,7 +9362,7 @@
         <v>support fetching a QuestionnaireResponse</v>
       </c>
       <c r="Z116" s="4" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="AB116" t="str">
         <f t="shared" si="9"/>
@@ -9459,7 +9474,7 @@
         <v>51</v>
       </c>
       <c r="Y118" s="19" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="AB118" t="str">
         <f t="shared" si="9"/>
@@ -9471,7 +9486,7 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C119" t="s">
         <v>602</v>
@@ -9499,16 +9514,16 @@
         <v>52</v>
       </c>
       <c r="L119" t="s">
+        <v>665</v>
+      </c>
+      <c r="M119" t="s">
+        <v>51</v>
+      </c>
+      <c r="O119" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y119" s="19" t="s">
         <v>666</v>
-      </c>
-      <c r="M119" t="s">
-        <v>51</v>
-      </c>
-      <c r="O119" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y119" s="19" t="s">
-        <v>667</v>
       </c>
       <c r="AB119" t="str">
         <f t="shared" si="9"/>
@@ -9564,7 +9579,7 @@
         <v>87</v>
       </c>
       <c r="Y120" s="19" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="AB120" t="str">
         <f t="shared" si="9"/>
@@ -9614,7 +9629,7 @@
         <v>51</v>
       </c>
       <c r="Y121" s="19" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="AB121" t="str">
         <f t="shared" si="9"/>
@@ -9626,7 +9641,7 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C122" t="s">
         <v>84</v>
@@ -9664,7 +9679,7 @@
         <v>51</v>
       </c>
       <c r="Y122" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="Z122" s="4" t="str">
         <f>"GET [base]/"&amp;B122&amp;"?patient=1137192"</f>
@@ -9684,7 +9699,7 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C123" t="s">
         <v>56</v>
@@ -9737,7 +9752,7 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C124" t="s">
         <v>12</v>
@@ -9790,7 +9805,7 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C125" t="s">
         <v>84</v>
@@ -9828,10 +9843,10 @@
         <v>51</v>
       </c>
       <c r="X125" s="6" t="s">
+        <v>637</v>
+      </c>
+      <c r="Z125" s="8" t="s">
         <v>638</v>
-      </c>
-      <c r="Z125" s="8" t="s">
-        <v>639</v>
       </c>
       <c r="AA125" s="8" t="str">
         <f>"Fetches a bundle of all "&amp;B125&amp; " resources for the specified patient."</f>
@@ -9847,10 +9862,10 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
+        <v>639</v>
+      </c>
+      <c r="C126" t="s">
         <v>640</v>
-      </c>
-      <c r="C126" t="s">
-        <v>641</v>
       </c>
       <c r="D126" t="s">
         <v>28</v>
@@ -9901,7 +9916,7 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="C127" t="s">
         <v>50</v>
@@ -9939,7 +9954,7 @@
         <v>51</v>
       </c>
       <c r="Y127" s="4" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="Z127" s="4" t="str">
         <f>"GET [base]/"&amp;B127&amp;"?"&amp;C127&amp;"=123"</f>
@@ -9955,7 +9970,7 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="C128" t="s">
         <v>84</v>
@@ -10898,7 +10913,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D32" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="F32" t="s">
         <v>64</v>
@@ -10907,10 +10922,10 @@
         <v>128</v>
       </c>
       <c r="I32" s="4" t="s">
+        <v>642</v>
+      </c>
+      <c r="J32" s="4" t="s">
         <v>643</v>
-      </c>
-      <c r="J32" s="4" t="s">
-        <v>644</v>
       </c>
       <c r="K32" s="4" t="str">
         <f t="shared" si="1"/>
@@ -11040,7 +11055,7 @@
         <v>312</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
@@ -11085,7 +11100,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D38" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E38" t="s">
         <v>51</v>
@@ -11100,13 +11115,13 @@
         <v>396</v>
       </c>
       <c r="I38" s="4" t="s">
+        <v>706</v>
+      </c>
+      <c r="J38" s="24" t="s">
         <v>707</v>
       </c>
-      <c r="J38" s="24" t="s">
+      <c r="K38" s="4" t="s">
         <v>708</v>
-      </c>
-      <c r="K38" s="4" t="s">
-        <v>709</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
@@ -11133,7 +11148,7 @@
         <v>144</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="K39" s="4" t="s">
         <v>555</v>
@@ -11389,7 +11404,7 @@
         <v>173</v>
       </c>
       <c r="C48" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="D48" t="s">
         <v>110</v>
@@ -11419,7 +11434,7 @@
         <v>173</v>
       </c>
       <c r="C49" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="D49" t="s">
         <v>139</v>
@@ -11452,7 +11467,7 @@
         <v>173</v>
       </c>
       <c r="C50" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="D50" t="s">
         <v>141</v>
@@ -11482,7 +11497,7 @@
         <v>173</v>
       </c>
       <c r="C51" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="D51" t="s">
         <v>188</v>
@@ -11515,7 +11530,7 @@
         <v>173</v>
       </c>
       <c r="C52" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="D52" t="s">
         <v>212</v>
@@ -11893,7 +11908,7 @@
         <v>177</v>
       </c>
       <c r="C64" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D64" t="s">
         <v>229</v>
@@ -11925,7 +11940,7 @@
         <v>177</v>
       </c>
       <c r="C65" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D65" t="s">
         <v>139</v>
@@ -11958,7 +11973,7 @@
         <v>177</v>
       </c>
       <c r="C66" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D66" t="s">
         <v>141</v>
@@ -11988,7 +12003,7 @@
         <v>177</v>
       </c>
       <c r="C67" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D67" t="s">
         <v>188</v>
@@ -12021,7 +12036,7 @@
         <v>177</v>
       </c>
       <c r="C68" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D68" t="s">
         <v>212</v>
@@ -12051,7 +12066,7 @@
         <v>304</v>
       </c>
       <c r="C69" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D69" t="s">
         <v>110</v>
@@ -12430,7 +12445,7 @@
         <v>241</v>
       </c>
       <c r="C81" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="D81" t="s">
         <v>112</v>
@@ -12459,7 +12474,7 @@
         <v>241</v>
       </c>
       <c r="C82" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="D82" t="s">
         <v>110</v>
@@ -12471,13 +12486,13 @@
         <v>100</v>
       </c>
       <c r="I82" s="4" t="s">
+        <v>645</v>
+      </c>
+      <c r="J82" s="4" t="s">
         <v>646</v>
       </c>
-      <c r="J82" s="4" t="s">
+      <c r="K82" s="4" t="s">
         <v>647</v>
-      </c>
-      <c r="K82" s="4" t="s">
-        <v>648</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
@@ -12732,7 +12747,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C91" t="str">
         <f t="shared" si="4"/>
@@ -12797,7 +12812,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C93" t="str">
         <f t="shared" si="4"/>
@@ -12862,7 +12877,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="16" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C95" t="str">
         <f t="shared" si="4"/>
@@ -12880,10 +12895,10 @@
       </c>
       <c r="H95" s="16"/>
       <c r="I95" s="4" t="s">
+        <v>648</v>
+      </c>
+      <c r="J95" s="4" t="s">
         <v>649</v>
-      </c>
-      <c r="J95" s="4" t="s">
-        <v>650</v>
       </c>
       <c r="K95" t="str">
         <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed))."</f>
@@ -12895,7 +12910,7 @@
         <v>95</v>
       </c>
       <c r="B96" s="16" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C96" t="str">
         <f t="shared" si="4"/>
@@ -12913,10 +12928,10 @@
       </c>
       <c r="H96" s="16"/>
       <c r="I96" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="J96" s="4" t="s">
         <v>651</v>
-      </c>
-      <c r="J96" s="4" t="s">
-        <v>652</v>
       </c>
       <c r="K96" t="str">
         <f>"Fetches a bundle of all "&amp;B96&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed) and type of dispense (e.g., partially dispensed)."</f>
@@ -12928,14 +12943,14 @@
         <v>96</v>
       </c>
       <c r="B97" s="16" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C97" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationdispense</v>
       </c>
       <c r="D97" s="16" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E97" s="16"/>
       <c r="F97" s="16" t="s">
@@ -12946,10 +12961,10 @@
       </c>
       <c r="H97" s="16"/>
       <c r="I97" s="4" t="s">
+        <v>653</v>
+      </c>
+      <c r="J97" s="4" t="s">
         <v>654</v>
-      </c>
-      <c r="J97" s="4" t="s">
-        <v>655</v>
       </c>
       <c r="K97" t="str">
         <f>"Fetches a bundle of all "&amp;B96&amp;" resources for the specified patient for a given dispense and date or range"</f>
@@ -12967,21 +12982,21 @@
         <v>525</v>
       </c>
       <c r="D98" s="16" t="s">
+        <v>701</v>
+      </c>
+      <c r="E98" s="16" t="s">
         <v>702</v>
       </c>
-      <c r="E98" s="16" t="s">
+      <c r="F98" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="G98" s="16" t="s">
         <v>703</v>
-      </c>
-      <c r="F98" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="G98" s="16" t="s">
-        <v>704</v>
       </c>
       <c r="H98" s="16"/>
       <c r="I98" s="4"/>
       <c r="J98" s="4" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="K98" t="str">
         <f>"Fetches a bundle of all "&amp;B98&amp;" resources for the specified patient that may match any of the string fields in the name element (including family, give, prefix, suffix, suffix, and/or text)"</f>
@@ -13155,7 +13170,7 @@
         <v>524</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="D2" t="s">
         <v>64</v>
@@ -13163,7 +13178,7 @@
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>519</v>
@@ -13246,7 +13261,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CECBDE16-5B3B-D24D-8161-5797A7035D04}">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
@@ -13320,7 +13335,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B5" t="s">
         <v>615</v>
@@ -13334,7 +13349,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B6" t="s">
         <v>616</v>
@@ -13348,16 +13363,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>669</v>
+      </c>
+      <c r="B7" t="s">
         <v>670</v>
       </c>
-      <c r="B7" t="s">
-        <v>671</v>
-      </c>
       <c r="D7" t="s">
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -13418,7 +13433,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B12" t="s">
         <v>347</v>
@@ -13502,7 +13517,7 @@
     </row>
     <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="B18" t="s">
         <v>595</v>
@@ -13586,16 +13601,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>671</v>
+      </c>
+      <c r="B24" t="s">
         <v>672</v>
       </c>
-      <c r="B24" t="s">
-        <v>673</v>
-      </c>
       <c r="D24" t="s">
         <v>11</v>
       </c>
       <c r="E24" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -13614,10 +13629,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>673</v>
+      </c>
+      <c r="B26" t="s">
         <v>674</v>
-      </c>
-      <c r="B26" t="s">
-        <v>675</v>
       </c>
       <c r="D26" t="s">
         <v>11</v>
@@ -13628,10 +13643,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>675</v>
+      </c>
+      <c r="B27" t="s">
         <v>676</v>
-      </c>
-      <c r="B27" t="s">
-        <v>677</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
@@ -13642,10 +13657,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>677</v>
+      </c>
+      <c r="B28" t="s">
         <v>678</v>
-      </c>
-      <c r="B28" t="s">
-        <v>679</v>
       </c>
       <c r="D28" t="s">
         <v>11</v>
@@ -13656,7 +13671,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="18" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B29" t="s">
         <v>596</v>
@@ -13684,10 +13699,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B31" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="D31" t="s">
         <v>11</v>
@@ -13698,10 +13713,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="B32" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="D32" t="s">
         <v>11</v>
@@ -13712,10 +13727,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="B33" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="D33" t="s">
         <v>11</v>
@@ -13852,10 +13867,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B43" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="D43" t="s">
         <v>11</v>
@@ -13866,10 +13881,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="B44" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="D44" t="s">
         <v>11</v>
@@ -13894,7 +13909,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="18" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B46" t="s">
         <v>598</v>
@@ -13908,10 +13923,10 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B47" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="D47" t="s">
         <v>11</v>
@@ -13939,7 +13954,7 @@
         <v>478</v>
       </c>
       <c r="B49" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D49" t="s">
         <v>11</v>
@@ -14062,21 +14077,21 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B58" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="D58" t="s">
         <v>11</v>
       </c>
       <c r="E58" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B59" t="s">
         <v>599</v>
@@ -14118,21 +14133,21 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>683</v>
+      </c>
+      <c r="B62" t="s">
         <v>684</v>
       </c>
-      <c r="B62" t="s">
+      <c r="D62" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" t="s">
         <v>685</v>
-      </c>
-      <c r="D62" t="s">
-        <v>11</v>
-      </c>
-      <c r="E62" t="s">
-        <v>686</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14142,18 +14157,18 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9ACEDC0-A695-4042-BE38-A780F3DE9AE3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{352F3A6C-0DAD-1041-B50E-04478951E07A}">
   <dimension ref="A1:Y69"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="36.5" customWidth="1"/>
     <col min="2" max="2" width="25.33203125" customWidth="1"/>
-    <col min="3" max="3" width="49.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="99.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="11.33203125" customWidth="1"/>
@@ -14253,7 +14268,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="T2" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="U2" t="s">
         <v>64</v>
@@ -14276,7 +14291,7 @@
         <v>474</v>
       </c>
       <c r="T3" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="U3" t="s">
         <v>64</v>
@@ -14299,7 +14314,7 @@
         <v>619</v>
       </c>
       <c r="T4" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="U4" t="s">
         <v>64</v>
@@ -14325,10 +14340,10 @@
         <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="T5" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="U5" t="s">
         <v>64</v>
@@ -14342,13 +14357,13 @@
     </row>
     <row r="6" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="T6" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="U6" t="s">
         <v>64</v>
@@ -14371,7 +14386,7 @@
         <v>620</v>
       </c>
       <c r="T7" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="U7" t="s">
         <v>64</v>
@@ -14392,7 +14407,7 @@
       </c>
       <c r="C8" s="2"/>
       <c r="T8" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="U8" t="s">
         <v>64</v>
@@ -14412,10 +14427,10 @@
         <v>11</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="T9" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="U9" t="s">
         <v>64</v>
@@ -14435,10 +14450,10 @@
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="T10" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="U10" t="s">
         <v>64</v>
@@ -14452,16 +14467,16 @@
     </row>
     <row r="11" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>720</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="25" t="s">
         <v>721</v>
       </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>722</v>
-      </c>
       <c r="T11" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="U11" t="s">
         <v>64</v>
@@ -14477,10 +14492,10 @@
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="T12" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="U12" t="s">
         <v>64</v>
@@ -14494,16 +14509,16 @@
     </row>
     <row r="13" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>722</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="25" t="s">
         <v>723</v>
       </c>
-      <c r="B13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="25" t="s">
-        <v>724</v>
-      </c>
       <c r="T13" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="U13" t="s">
         <v>64</v>
@@ -14522,7 +14537,7 @@
         <v>621</v>
       </c>
       <c r="T14" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="U14" t="s">
         <v>64</v>
@@ -14542,7 +14557,7 @@
         <v>11</v>
       </c>
       <c r="T15" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="U15" t="s">
         <v>64</v>
@@ -14552,16 +14567,16 @@
     </row>
     <row r="16" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>710</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="25" t="s">
         <v>711</v>
       </c>
-      <c r="B16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="25" t="s">
-        <v>712</v>
-      </c>
       <c r="T16" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="U16" t="s">
         <v>64</v>
@@ -14580,7 +14595,7 @@
         <v>475</v>
       </c>
       <c r="T17" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="U17" t="s">
         <v>64</v>
@@ -14599,7 +14614,7 @@
         <v>476</v>
       </c>
       <c r="T18" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="U18" t="s">
         <v>64</v>
@@ -14619,25 +14634,25 @@
     </row>
     <row r="19" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>636</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="T19" t="s">
+        <v>709</v>
+      </c>
+      <c r="U19" t="s">
+        <v>64</v>
+      </c>
+      <c r="V19" t="s">
+        <v>64</v>
+      </c>
+      <c r="W19" s="6" t="s">
         <v>637</v>
-      </c>
-      <c r="B19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>713</v>
-      </c>
-      <c r="T19" t="s">
-        <v>710</v>
-      </c>
-      <c r="U19" t="s">
-        <v>64</v>
-      </c>
-      <c r="V19" t="s">
-        <v>64</v>
-      </c>
-      <c r="W19" s="6" t="s">
-        <v>638</v>
       </c>
       <c r="X19" s="13" t="s">
         <v>433</v>
@@ -14657,7 +14672,7 @@
         <v>477</v>
       </c>
       <c r="T20" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="U20" t="s">
         <v>64</v>
@@ -14683,10 +14698,10 @@
         <v>11</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="T21" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="U21" t="s">
         <v>64</v>
@@ -14709,7 +14724,7 @@
         <v>622</v>
       </c>
       <c r="T22" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="U22" t="s">
         <v>64</v>
@@ -14728,7 +14743,7 @@
         <v>623</v>
       </c>
       <c r="T23" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="U23" t="s">
         <v>64</v>
@@ -14748,10 +14763,10 @@
         <v>11</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="T24" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="U24" t="s">
         <v>64</v>
@@ -14767,10 +14782,10 @@
         <v>11</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="T25" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="U25" t="s">
         <v>64</v>
@@ -14784,7 +14799,7 @@
       <c r="X25" s="13"/>
       <c r="Y25" s="13"/>
     </row>
-    <row r="26" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" ht="321" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>176</v>
       </c>
@@ -14792,10 +14807,10 @@
         <v>11</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>624</v>
+        <v>736</v>
       </c>
       <c r="T26" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="U26" t="s">
         <v>64</v>
@@ -14815,10 +14830,10 @@
         <v>11</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="T27" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="U27" t="s">
         <v>64</v>
@@ -14826,13 +14841,13 @@
     </row>
     <row r="28" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="B28" t="s">
         <v>64</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="X28" s="13"/>
       <c r="Y28" s="13"/>
@@ -14845,7 +14860,7 @@
         <v>64</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="X29" s="13" t="s">
         <v>433</v>
@@ -14862,7 +14877,7 @@
         <v>11</v>
       </c>
       <c r="T30" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="U30" t="s">
         <v>64</v>
@@ -14881,8 +14896,11 @@
       <c r="B31" t="s">
         <v>11</v>
       </c>
+      <c r="C31" s="1" t="s">
+        <v>737</v>
+      </c>
       <c r="T31" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="U31" t="s">
         <v>64</v>
@@ -14896,13 +14914,13 @@
     </row>
     <row r="32" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B32" t="s">
         <v>11</v>
       </c>
       <c r="T32" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="U32" t="s">
         <v>64</v>
@@ -14916,11 +14934,6 @@
       </c>
       <c r="B33" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>730</v>
       </c>
     </row>
     <row r="66" spans="22:25" ht="21" customHeight="1" x14ac:dyDescent="0.2">
@@ -14933,7 +14946,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15006,7 +15019,7 @@
         <v>64</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -15059,7 +15072,7 @@
         <v>353</v>
       </c>
       <c r="F1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="G1" t="s">
         <v>354</v>
@@ -15077,13 +15090,13 @@
         <v>357</v>
       </c>
       <c r="L1" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="M1" t="s">
         <v>358</v>
       </c>
       <c r="N1" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="O1" t="s">
         <v>359</v>
@@ -15092,13 +15105,13 @@
         <v>360</v>
       </c>
       <c r="Q1" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="R1" t="s">
         <v>361</v>
       </c>
       <c r="S1" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="T1" t="s">
         <v>362</v>
@@ -15131,7 +15144,7 @@
         <v>416</v>
       </c>
       <c r="AD1" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="AE1" t="s">
         <v>601</v>
@@ -15146,7 +15159,7 @@
         <v>432</v>
       </c>
       <c r="AI1" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update guidance on referencing PractitionerRole [FHIR-42906]
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE6467C-4517-C148-B430-6C2CE2BB268D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A61CE5D8-9941-6A44-8790-9AA0E61C375B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50700" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="48500" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -2003,17 +2003,6 @@
     <t>1. See the [General Security Considerations](security.html) section for requirements and recommendations.</t>
   </si>
   <si>
-    <t>In order to access care team member's names, identifiers, locations, and contact information, the CareTeam profile supports several types of care team participants. They are represented as references to other profiles and include the following four profiles which are marked as must support:
-  1. US Core Practitioner Profile
-  1. US Core PractitionerRole Profile
-  1. US Core Patient Profile
-  1. US Core RelatedPerson Profile
-  * Although *both* US Core Practitioner Profile and US Core PractitionerRole are must support, the server system is not required to support both types of references (and `_include` search parameters), but **SHALL** support *at least* one of them.
-  * The client application **SHALL** support all four profile references.
-  * Bacause the *US Core PractitionerRole Profile* supplies the provider's location and contact information and a reference to the Practitioner, server systems **SHOULD** reference it instead of the *US Core Practitioner Profile*.
-  * Servers that supports only *US Core Practitioner Profile* **SHALL** provide implementation specific guidance how to access a provider's location and contact information using only the Practitioner resource.</t>
-  </si>
-  <si>
     <t>* Implantable medical devices that have UDI information **SHALL** represent the UDI code in `Device.udiCarrier.carrierHRF`.
    - All of the five UDI-PI elements that are present in the UDI code **SHALL** be represented in the corresponding US Core Implantable Device Profile element.
    UDI may not be present in all scenarios such as historical implantable devices, patient reported implant information, payer reported devices, or improperly documented implants. If UDI is not present and the manufacturer and/or model number information is available, they **SHOULD** be included to support historical reports of implantable medical devices as follows:
@@ -2414,9 +2403,6 @@
 </t>
   </si>
   <si>
-    <t>* The PractitionerRole Profiles is not explicitly referenced in any US Core Profile. However it **SHOULD** be used as the default profile if referenced by another US Core profile.</t>
-  </si>
-  <si>
     <t>US Core defines two ways to represent the questions and responses to screening and assessment instruments:
 - Observation: US Core Observation Screening Assessment Profile
 - Questionnaire/QuestionnaireResponse: SDC Base Questionnaire/US Core QuestionnaireResponse Profile
@@ -2473,6 +2459,20 @@
      - Although both `Procedure.reasonCode` and `Procedure.reasonReference` are marked as Additional USCDI Requirements. The certifying server system is not required to support both but **SHALL** support at least one of these elements. The certifying client application **SHALL** support both elements.
      - As documented [here](general-guidance.html#referencing-us-core-profiles), when using  `Procedure.reasonReference`, the referenced resources **SHOULD** be a US Core Profile.
     Certifying Servers and Clients **SHALL** support options 1 and 2 as Additional USCDI Requirements.</t>
+  </si>
+  <si>
+    <t>* Due to implementer feedback, some US Core Profiles reference the PractitionerRole resource instead of the US Core PractitionerRole Profile. However the US Core PractitionerRole Profile **SHOULD** be used as the default profile if referenced by another US Core profile.</t>
+  </si>
+  <si>
+    <t>In order to access care team member's names, identifiers, locations, and contact information, the CareTeam profile supports several types of care team participants. They are represented as references to other profiles and include the following four profiles which are marked as must support:
+  1. US Core Practitioner Profile
+  1. US Core PractitionerRole Profile
+  1. US Core Patient Profile
+  1. US Core RelatedPerson Profile
+  * Although *both* US Core Practitioner Profile and US Core PractitionerRole are must support, the server system is not required to support both types of references,, but **SHALL** support *at least* one of them.
+  * The client application **SHALL** support all four profile references.
+  * Bacause the *US Core PractitionerRole Profile* supplies the provider's location and contact information and a reference to the Practitioner, server systems **SHOULD** reference it instead of the *US Core Practitioner Profile*.
+  * Servers that supports only *US Core Practitioner Profile* **SHALL** provide implementation specific guidance how to access a provider's location and contact information using only the Practitioner resource.</t>
   </si>
 </sst>
 </file>
@@ -4479,7 +4479,7 @@
         <v>19</v>
       </c>
       <c r="C25" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="D25" t="s">
         <v>28</v>
@@ -4753,7 +4753,7 @@
         <v>51</v>
       </c>
       <c r="Y30" s="4" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="Z30" t="s">
         <v>167</v>
@@ -4775,7 +4775,7 @@
         <v>79</v>
       </c>
       <c r="C31" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="D31" t="s">
         <v>28</v>
@@ -4797,19 +4797,19 @@
         <v>52</v>
       </c>
       <c r="L31" t="s">
+        <v>630</v>
+      </c>
+      <c r="M31" t="s">
+        <v>51</v>
+      </c>
+      <c r="O31" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y31" s="4" t="s">
         <v>631</v>
       </c>
-      <c r="M31" t="s">
-        <v>51</v>
-      </c>
-      <c r="O31" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y31" s="4" t="s">
+      <c r="Z31" t="s">
         <v>632</v>
-      </c>
-      <c r="Z31" t="s">
-        <v>633</v>
       </c>
       <c r="AA31" s="8" t="str">
         <f>"Fetches a bundle of all "&amp;B31&amp;" resources matching the name"</f>
@@ -4825,7 +4825,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C32" t="s">
         <v>50</v>
@@ -4850,7 +4850,7 @@
         <v>52</v>
       </c>
       <c r="L32" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="M32" t="s">
         <v>51</v>
@@ -4868,7 +4868,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C33" t="s">
         <v>65</v>
@@ -4912,7 +4912,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C34" t="s">
         <v>62</v>
@@ -4959,7 +4959,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C35" t="s">
         <v>56</v>
@@ -5003,7 +5003,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C36" t="s">
         <v>57</v>
@@ -5059,7 +5059,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C37" t="s">
         <v>54</v>
@@ -5103,7 +5103,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C38" t="s">
         <v>61</v>
@@ -9303,7 +9303,7 @@
         <v>51</v>
       </c>
       <c r="Y115" s="4" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="Z115" s="4" t="str">
         <f>"GET [base]/"&amp;B115&amp;"?"&amp;C115&amp;"=Mary Shaw"</f>
@@ -9362,7 +9362,7 @@
         <v>support fetching a QuestionnaireResponse</v>
       </c>
       <c r="Z116" s="4" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="AB116" t="str">
         <f t="shared" si="9"/>
@@ -9474,7 +9474,7 @@
         <v>51</v>
       </c>
       <c r="Y118" s="19" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="AB118" t="str">
         <f t="shared" si="9"/>
@@ -9486,7 +9486,7 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="C119" t="s">
         <v>602</v>
@@ -9514,16 +9514,16 @@
         <v>52</v>
       </c>
       <c r="L119" t="s">
+        <v>664</v>
+      </c>
+      <c r="M119" t="s">
+        <v>51</v>
+      </c>
+      <c r="O119" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y119" s="19" t="s">
         <v>665</v>
-      </c>
-      <c r="M119" t="s">
-        <v>51</v>
-      </c>
-      <c r="O119" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y119" s="19" t="s">
-        <v>666</v>
       </c>
       <c r="AB119" t="str">
         <f t="shared" si="9"/>
@@ -9579,7 +9579,7 @@
         <v>87</v>
       </c>
       <c r="Y120" s="19" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="AB120" t="str">
         <f t="shared" si="9"/>
@@ -9629,7 +9629,7 @@
         <v>51</v>
       </c>
       <c r="Y121" s="19" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="AB121" t="str">
         <f t="shared" si="9"/>
@@ -9641,7 +9641,7 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="C122" t="s">
         <v>84</v>
@@ -9679,7 +9679,7 @@
         <v>51</v>
       </c>
       <c r="Y122" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="Z122" s="4" t="str">
         <f>"GET [base]/"&amp;B122&amp;"?patient=1137192"</f>
@@ -9699,7 +9699,7 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C123" t="s">
         <v>56</v>
@@ -9752,7 +9752,7 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C124" t="s">
         <v>12</v>
@@ -9805,7 +9805,7 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C125" t="s">
         <v>84</v>
@@ -9843,10 +9843,10 @@
         <v>51</v>
       </c>
       <c r="X125" s="6" t="s">
+        <v>636</v>
+      </c>
+      <c r="Z125" s="8" t="s">
         <v>637</v>
-      </c>
-      <c r="Z125" s="8" t="s">
-        <v>638</v>
       </c>
       <c r="AA125" s="8" t="str">
         <f>"Fetches a bundle of all "&amp;B125&amp; " resources for the specified patient."</f>
@@ -9862,10 +9862,10 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
+        <v>638</v>
+      </c>
+      <c r="C126" t="s">
         <v>639</v>
-      </c>
-      <c r="C126" t="s">
-        <v>640</v>
       </c>
       <c r="D126" t="s">
         <v>28</v>
@@ -9916,7 +9916,7 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="C127" t="s">
         <v>50</v>
@@ -9954,7 +9954,7 @@
         <v>51</v>
       </c>
       <c r="Y127" s="4" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="Z127" s="4" t="str">
         <f>"GET [base]/"&amp;B127&amp;"?"&amp;C127&amp;"=123"</f>
@@ -9970,7 +9970,7 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="C128" t="s">
         <v>84</v>
@@ -10027,7 +10027,7 @@
   </sheetData>
   <autoFilter ref="A1:AB128" xr:uid="{1CF5B17E-E72E-48B2-A597-9C21C12723F0}"/>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10913,7 +10913,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D32" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="F32" t="s">
         <v>64</v>
@@ -10922,10 +10922,10 @@
         <v>128</v>
       </c>
       <c r="I32" s="4" t="s">
+        <v>641</v>
+      </c>
+      <c r="J32" s="4" t="s">
         <v>642</v>
-      </c>
-      <c r="J32" s="4" t="s">
-        <v>643</v>
       </c>
       <c r="K32" s="4" t="str">
         <f t="shared" si="1"/>
@@ -11055,7 +11055,7 @@
         <v>312</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
@@ -11100,7 +11100,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D38" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E38" t="s">
         <v>51</v>
@@ -11115,13 +11115,13 @@
         <v>396</v>
       </c>
       <c r="I38" s="4" t="s">
+        <v>705</v>
+      </c>
+      <c r="J38" s="24" t="s">
         <v>706</v>
       </c>
-      <c r="J38" s="24" t="s">
+      <c r="K38" s="4" t="s">
         <v>707</v>
-      </c>
-      <c r="K38" s="4" t="s">
-        <v>708</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
@@ -11148,7 +11148,7 @@
         <v>144</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="K39" s="4" t="s">
         <v>555</v>
@@ -11404,7 +11404,7 @@
         <v>173</v>
       </c>
       <c r="C48" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="D48" t="s">
         <v>110</v>
@@ -11434,7 +11434,7 @@
         <v>173</v>
       </c>
       <c r="C49" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="D49" t="s">
         <v>139</v>
@@ -11467,7 +11467,7 @@
         <v>173</v>
       </c>
       <c r="C50" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="D50" t="s">
         <v>141</v>
@@ -11497,7 +11497,7 @@
         <v>173</v>
       </c>
       <c r="C51" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="D51" t="s">
         <v>188</v>
@@ -11530,7 +11530,7 @@
         <v>173</v>
       </c>
       <c r="C52" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="D52" t="s">
         <v>212</v>
@@ -11908,7 +11908,7 @@
         <v>177</v>
       </c>
       <c r="C64" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="D64" t="s">
         <v>229</v>
@@ -11940,7 +11940,7 @@
         <v>177</v>
       </c>
       <c r="C65" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="D65" t="s">
         <v>139</v>
@@ -11973,7 +11973,7 @@
         <v>177</v>
       </c>
       <c r="C66" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="D66" t="s">
         <v>141</v>
@@ -12003,7 +12003,7 @@
         <v>177</v>
       </c>
       <c r="C67" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="D67" t="s">
         <v>188</v>
@@ -12036,7 +12036,7 @@
         <v>177</v>
       </c>
       <c r="C68" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="D68" t="s">
         <v>212</v>
@@ -12066,7 +12066,7 @@
         <v>304</v>
       </c>
       <c r="C69" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="D69" t="s">
         <v>110</v>
@@ -12445,7 +12445,7 @@
         <v>241</v>
       </c>
       <c r="C81" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D81" t="s">
         <v>112</v>
@@ -12474,7 +12474,7 @@
         <v>241</v>
       </c>
       <c r="C82" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D82" t="s">
         <v>110</v>
@@ -12486,13 +12486,13 @@
         <v>100</v>
       </c>
       <c r="I82" s="4" t="s">
+        <v>644</v>
+      </c>
+      <c r="J82" s="4" t="s">
         <v>645</v>
       </c>
-      <c r="J82" s="4" t="s">
+      <c r="K82" s="4" t="s">
         <v>646</v>
-      </c>
-      <c r="K82" s="4" t="s">
-        <v>647</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
@@ -12747,7 +12747,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="C91" t="str">
         <f t="shared" si="4"/>
@@ -12812,7 +12812,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="C93" t="str">
         <f t="shared" si="4"/>
@@ -12877,7 +12877,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="16" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C95" t="str">
         <f t="shared" si="4"/>
@@ -12895,10 +12895,10 @@
       </c>
       <c r="H95" s="16"/>
       <c r="I95" s="4" t="s">
+        <v>647</v>
+      </c>
+      <c r="J95" s="4" t="s">
         <v>648</v>
-      </c>
-      <c r="J95" s="4" t="s">
-        <v>649</v>
       </c>
       <c r="K95" t="str">
         <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed))."</f>
@@ -12910,7 +12910,7 @@
         <v>95</v>
       </c>
       <c r="B96" s="16" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C96" t="str">
         <f t="shared" si="4"/>
@@ -12928,10 +12928,10 @@
       </c>
       <c r="H96" s="16"/>
       <c r="I96" s="4" t="s">
+        <v>649</v>
+      </c>
+      <c r="J96" s="4" t="s">
         <v>650</v>
-      </c>
-      <c r="J96" s="4" t="s">
-        <v>651</v>
       </c>
       <c r="K96" t="str">
         <f>"Fetches a bundle of all "&amp;B96&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed) and type of dispense (e.g., partially dispensed)."</f>
@@ -12943,14 +12943,14 @@
         <v>96</v>
       </c>
       <c r="B97" s="16" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="C97" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationdispense</v>
       </c>
       <c r="D97" s="16" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="E97" s="16"/>
       <c r="F97" s="16" t="s">
@@ -12961,10 +12961,10 @@
       </c>
       <c r="H97" s="16"/>
       <c r="I97" s="4" t="s">
+        <v>652</v>
+      </c>
+      <c r="J97" s="4" t="s">
         <v>653</v>
-      </c>
-      <c r="J97" s="4" t="s">
-        <v>654</v>
       </c>
       <c r="K97" t="str">
         <f>"Fetches a bundle of all "&amp;B96&amp;" resources for the specified patient for a given dispense and date or range"</f>
@@ -12982,21 +12982,21 @@
         <v>525</v>
       </c>
       <c r="D98" s="16" t="s">
+        <v>700</v>
+      </c>
+      <c r="E98" s="16" t="s">
         <v>701</v>
       </c>
-      <c r="E98" s="16" t="s">
+      <c r="F98" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="G98" s="16" t="s">
         <v>702</v>
-      </c>
-      <c r="F98" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="G98" s="16" t="s">
-        <v>703</v>
       </c>
       <c r="H98" s="16"/>
       <c r="I98" s="4"/>
       <c r="J98" s="4" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="K98" t="str">
         <f>"Fetches a bundle of all "&amp;B98&amp;" resources for the specified patient that may match any of the string fields in the name element (including family, give, prefix, suffix, suffix, and/or text)"</f>
@@ -13006,7 +13006,7 @@
   </sheetData>
   <autoFilter ref="A1:K98" xr:uid="{331E0B16-168F-459B-8951-3DF614BF0371}"/>
   <conditionalFormatting sqref="B1:B97 B99:B1048576">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13170,7 +13170,7 @@
         <v>524</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="D2" t="s">
         <v>64</v>
@@ -13178,7 +13178,7 @@
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>519</v>
@@ -13335,7 +13335,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B5" t="s">
         <v>615</v>
@@ -13349,7 +13349,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B6" t="s">
         <v>616</v>
@@ -13363,16 +13363,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>668</v>
+      </c>
+      <c r="B7" t="s">
         <v>669</v>
       </c>
-      <c r="B7" t="s">
-        <v>670</v>
-      </c>
       <c r="D7" t="s">
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -13433,7 +13433,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B12" t="s">
         <v>347</v>
@@ -13517,7 +13517,7 @@
     </row>
     <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="B18" t="s">
         <v>595</v>
@@ -13601,16 +13601,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>670</v>
+      </c>
+      <c r="B24" t="s">
         <v>671</v>
       </c>
-      <c r="B24" t="s">
-        <v>672</v>
-      </c>
       <c r="D24" t="s">
         <v>11</v>
       </c>
       <c r="E24" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -13629,10 +13629,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>672</v>
+      </c>
+      <c r="B26" t="s">
         <v>673</v>
-      </c>
-      <c r="B26" t="s">
-        <v>674</v>
       </c>
       <c r="D26" t="s">
         <v>11</v>
@@ -13643,10 +13643,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>674</v>
+      </c>
+      <c r="B27" t="s">
         <v>675</v>
-      </c>
-      <c r="B27" t="s">
-        <v>676</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
@@ -13657,10 +13657,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>676</v>
+      </c>
+      <c r="B28" t="s">
         <v>677</v>
-      </c>
-      <c r="B28" t="s">
-        <v>678</v>
       </c>
       <c r="D28" t="s">
         <v>11</v>
@@ -13671,7 +13671,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="18" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B29" t="s">
         <v>596</v>
@@ -13699,10 +13699,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B31" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="D31" t="s">
         <v>11</v>
@@ -13713,10 +13713,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="B32" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="D32" t="s">
         <v>11</v>
@@ -13727,10 +13727,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="B33" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="D33" t="s">
         <v>11</v>
@@ -13867,10 +13867,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B43" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="D43" t="s">
         <v>11</v>
@@ -13881,10 +13881,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="B44" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D44" t="s">
         <v>11</v>
@@ -13909,7 +13909,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="18" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B46" t="s">
         <v>598</v>
@@ -13923,10 +13923,10 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B47" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="D47" t="s">
         <v>11</v>
@@ -13954,7 +13954,7 @@
         <v>478</v>
       </c>
       <c r="B49" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="D49" t="s">
         <v>11</v>
@@ -14077,21 +14077,21 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B58" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D58" t="s">
         <v>11</v>
       </c>
       <c r="E58" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B59" t="s">
         <v>599</v>
@@ -14133,16 +14133,16 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>682</v>
+      </c>
+      <c r="B62" t="s">
         <v>683</v>
       </c>
-      <c r="B62" t="s">
+      <c r="D62" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" t="s">
         <v>684</v>
-      </c>
-      <c r="D62" t="s">
-        <v>11</v>
-      </c>
-      <c r="E62" t="s">
-        <v>685</v>
       </c>
     </row>
   </sheetData>
@@ -14160,8 +14160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{352F3A6C-0DAD-1041-B50E-04478951E07A}">
   <dimension ref="A1:Y69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -14268,7 +14268,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="T2" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="U2" t="s">
         <v>64</v>
@@ -14291,7 +14291,7 @@
         <v>474</v>
       </c>
       <c r="T3" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="U3" t="s">
         <v>64</v>
@@ -14311,10 +14311,10 @@
         <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>619</v>
+        <v>737</v>
       </c>
       <c r="T4" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="U4" t="s">
         <v>64</v>
@@ -14340,10 +14340,10 @@
         <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="T5" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="U5" t="s">
         <v>64</v>
@@ -14357,13 +14357,13 @@
     </row>
     <row r="6" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="T6" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="U6" t="s">
         <v>64</v>
@@ -14383,10 +14383,10 @@
         <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="T7" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="U7" t="s">
         <v>64</v>
@@ -14407,7 +14407,7 @@
       </c>
       <c r="C8" s="2"/>
       <c r="T8" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="U8" t="s">
         <v>64</v>
@@ -14427,10 +14427,10 @@
         <v>11</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="T9" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="U9" t="s">
         <v>64</v>
@@ -14450,10 +14450,10 @@
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="T10" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="U10" t="s">
         <v>64</v>
@@ -14467,16 +14467,16 @@
     </row>
     <row r="11" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>719</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="25" t="s">
         <v>720</v>
       </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>721</v>
-      </c>
       <c r="T11" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="U11" t="s">
         <v>64</v>
@@ -14492,10 +14492,10 @@
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="T12" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="U12" t="s">
         <v>64</v>
@@ -14509,16 +14509,16 @@
     </row>
     <row r="13" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>721</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="25" t="s">
         <v>722</v>
       </c>
-      <c r="B13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="25" t="s">
-        <v>723</v>
-      </c>
       <c r="T13" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="U13" t="s">
         <v>64</v>
@@ -14534,10 +14534,10 @@
         <v>11</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="T14" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="U14" t="s">
         <v>64</v>
@@ -14557,7 +14557,7 @@
         <v>11</v>
       </c>
       <c r="T15" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="U15" t="s">
         <v>64</v>
@@ -14567,16 +14567,16 @@
     </row>
     <row r="16" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>709</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="25" t="s">
         <v>710</v>
       </c>
-      <c r="B16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="25" t="s">
-        <v>711</v>
-      </c>
       <c r="T16" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="U16" t="s">
         <v>64</v>
@@ -14595,7 +14595,7 @@
         <v>475</v>
       </c>
       <c r="T17" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="U17" t="s">
         <v>64</v>
@@ -14614,7 +14614,7 @@
         <v>476</v>
       </c>
       <c r="T18" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="U18" t="s">
         <v>64</v>
@@ -14634,25 +14634,25 @@
     </row>
     <row r="19" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>635</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="T19" t="s">
+        <v>708</v>
+      </c>
+      <c r="U19" t="s">
+        <v>64</v>
+      </c>
+      <c r="V19" t="s">
+        <v>64</v>
+      </c>
+      <c r="W19" s="6" t="s">
         <v>636</v>
-      </c>
-      <c r="B19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>712</v>
-      </c>
-      <c r="T19" t="s">
-        <v>709</v>
-      </c>
-      <c r="U19" t="s">
-        <v>64</v>
-      </c>
-      <c r="V19" t="s">
-        <v>64</v>
-      </c>
-      <c r="W19" s="6" t="s">
-        <v>637</v>
       </c>
       <c r="X19" s="13" t="s">
         <v>433</v>
@@ -14672,7 +14672,7 @@
         <v>477</v>
       </c>
       <c r="T20" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="U20" t="s">
         <v>64</v>
@@ -14698,10 +14698,10 @@
         <v>11</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="T21" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="U21" t="s">
         <v>64</v>
@@ -14721,10 +14721,10 @@
         <v>11</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="T22" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="U22" t="s">
         <v>64</v>
@@ -14740,10 +14740,10 @@
         <v>11</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="T23" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="U23" t="s">
         <v>64</v>
@@ -14763,10 +14763,10 @@
         <v>11</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="T24" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="U24" t="s">
         <v>64</v>
@@ -14782,10 +14782,10 @@
         <v>11</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>726</v>
+        <v>736</v>
       </c>
       <c r="T25" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="U25" t="s">
         <v>64</v>
@@ -14807,10 +14807,10 @@
         <v>11</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="T26" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="U26" t="s">
         <v>64</v>
@@ -14830,10 +14830,10 @@
         <v>11</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="T27" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="U27" t="s">
         <v>64</v>
@@ -14841,13 +14841,13 @@
     </row>
     <row r="28" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B28" t="s">
         <v>64</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="X28" s="13"/>
       <c r="Y28" s="13"/>
@@ -14860,7 +14860,7 @@
         <v>64</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="X29" s="13" t="s">
         <v>433</v>
@@ -14877,7 +14877,7 @@
         <v>11</v>
       </c>
       <c r="T30" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="U30" t="s">
         <v>64</v>
@@ -14897,10 +14897,10 @@
         <v>11</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="T31" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="U31" t="s">
         <v>64</v>
@@ -14914,13 +14914,13 @@
     </row>
     <row r="32" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B32" t="s">
         <v>11</v>
       </c>
       <c r="T32" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="U32" t="s">
         <v>64</v>
@@ -14946,7 +14946,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15019,7 +15019,7 @@
         <v>64</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -15072,7 +15072,7 @@
         <v>353</v>
       </c>
       <c r="F1" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="G1" t="s">
         <v>354</v>
@@ -15090,13 +15090,13 @@
         <v>357</v>
       </c>
       <c r="L1" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="M1" t="s">
         <v>358</v>
       </c>
       <c r="N1" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="O1" t="s">
         <v>359</v>
@@ -15105,13 +15105,13 @@
         <v>360</v>
       </c>
       <c r="Q1" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="R1" t="s">
         <v>361</v>
       </c>
       <c r="S1" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="T1" t="s">
         <v>362</v>
@@ -15144,7 +15144,7 @@
         <v>416</v>
       </c>
       <c r="AD1" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="AE1" t="s">
         <v>601</v>
@@ -15159,7 +15159,7 @@
         <v>432</v>
       </c>
       <c r="AI1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Correct description of Occupation Profile [FHIR-42867]
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A61CE5D8-9941-6A44-8790-9AA0E61C375B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1FED13F-1B5E-874A-ACC8-35A3DC480351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48500" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="14640" windowWidth="51200" windowHeight="14160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -2469,7 +2469,7 @@
   1. US Core PractitionerRole Profile
   1. US Core Patient Profile
   1. US Core RelatedPerson Profile
-  * Although *both* US Core Practitioner Profile and US Core PractitionerRole are must support, the server system is not required to support both types of references,, but **SHALL** support *at least* one of them.
+  * Although *both* US Core Practitioner Profile and US Core PractitionerRole are must support, the server system is not required to support both types of references, but **SHALL** support *at least* one of them.
   * The client application **SHALL** support all four profile references.
   * Bacause the *US Core PractitionerRole Profile* supplies the provider's location and contact information and a reference to the Practitioner, server systems **SHOULD** reference it instead of the *US Core Practitioner Profile*.
   * Servers that supports only *US Core Practitioner Profile* **SHALL** provide implementation specific guidance how to access a provider's location and contact information using only the Practitioner resource.</t>
@@ -14160,7 +14160,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{352F3A6C-0DAD-1041-B50E-04478951E07A}">
   <dimension ref="A1:Y69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Clarify when to include multiple attachments as part of a clinical note FHIR-41902
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1FED13F-1B5E-874A-ACC8-35A3DC480351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB79BEB-1629-0843-8241-1526B1EA7178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="14640" windowWidth="51200" windowHeight="14160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51900" yWindow="6200" windowWidth="51200" windowHeight="20620" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -2135,15 +2135,6 @@
     <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-device</t>
   </si>
   <si>
-    <t>* The `DocumentReference.type` binding **SHALL** support at a minimum the [5 Common Clinical Notes](ValueSet-us-core-clinical-note-type.html) and may extend to the full US Core DocumentReference Type Value Set
-* The DocumentReference resources can represent the referenced content using either an address where the document can be retrieved using `DocumentReference.attachment.url` or the content as inline base64 encoded data using `DocumentReference.attachment.data`.
-    *  Although both are marked as must support, the server system is not required to support an address, and inline base64 encoded data, but **SHALL** support at least one of these elements.
-    *  The client application **SHALL** support both elements.
-    *  The `content.url` may refer to a FHIR Binary Resource (i.e. [base]/Binary/[id]), FHIR Document Bundle (i.e [base]/Bundle/[id] or another endpoint.
-        * If the endpoint is outside the FHIR base URL, it **SHOULD NOT** require additional authorization to access.
-* Every DocumentReference must have a responsible Organization. The organization responsible for the DocumentReference **SHALL** be present either in `DocumentReference.custodian` or accessible in the Provenance resource targeting the DocumentReference using `Provenance.agent.who` or `Provenance.agent.onBehalfOf`.</t>
-  </si>
-  <si>
     <t>http://hl7.org/fhir/smart-app-launch/history.html</t>
   </si>
   <si>
@@ -2473,6 +2464,16 @@
   * The client application **SHALL** support all four profile references.
   * Bacause the *US Core PractitionerRole Profile* supplies the provider's location and contact information and a reference to the Practitioner, server systems **SHOULD** reference it instead of the *US Core Practitioner Profile*.
   * Servers that supports only *US Core Practitioner Profile* **SHALL** provide implementation specific guidance how to access a provider's location and contact information using only the Practitioner resource.</t>
+  </si>
+  <si>
+    <t>* The `DocumentReference.type` binding **SHALL** support at a minimum the [5 Common Clinical Notes](ValueSet-us-core-clinical-note-type.html) and may extend to the full US Core DocumentReference Type Value Set
+* The DocumentReference resources can represent the referenced content using either an address where the document can be retrieved using `DocumentReference.attachment.url` or the content as inline base64 encoded data using `DocumentReference.attachment.data`.
+    *  Although both are marked as must support, the server system is not required to support an address, and inline base64 encoded data, but **SHALL** support at least one of these elements.
+    *  The client application **SHALL** support both elements.
+    *  The `content.url` may refer to a FHIR Binary Resource (i.e. [base]/Binary/[id]), FHIR Document Bundle (i.e [base]/Bundle/[id] or another endpoint.
+        * If the endpoint is outside the FHIR base URL, it **SHOULD NOT** require additional authorization to access.
+   * If there are multiple `DocumentReference.content` element repetitions, these **SHALL** all represent the same document in different format or attachment metadata. The content element **SHALL** not contain different versions of the same content. For version handling use multiple DocumentReferences with `DocumentReference.relatesTo`
+* Every DocumentReference must have a responsible Organization. The organization responsible for the DocumentReference **SHALL** be present either in `DocumentReference.custodian` or accessible in the Provenance resource targeting the DocumentReference using `Provenance.agent.who` or `Provenance.agent.onBehalfOf`.</t>
   </si>
 </sst>
 </file>
@@ -4825,7 +4826,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C32" t="s">
         <v>50</v>
@@ -4850,7 +4851,7 @@
         <v>52</v>
       </c>
       <c r="L32" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="M32" t="s">
         <v>51</v>
@@ -4868,7 +4869,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C33" t="s">
         <v>65</v>
@@ -4912,7 +4913,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C34" t="s">
         <v>62</v>
@@ -4959,7 +4960,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C35" t="s">
         <v>56</v>
@@ -5003,7 +5004,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C36" t="s">
         <v>57</v>
@@ -5059,7 +5060,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C37" t="s">
         <v>54</v>
@@ -5103,7 +5104,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C38" t="s">
         <v>61</v>
@@ -9362,7 +9363,7 @@
         <v>support fetching a QuestionnaireResponse</v>
       </c>
       <c r="Z116" s="4" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="AB116" t="str">
         <f t="shared" si="9"/>
@@ -9474,7 +9475,7 @@
         <v>51</v>
       </c>
       <c r="Y118" s="19" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="AB118" t="str">
         <f t="shared" si="9"/>
@@ -9486,7 +9487,7 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="C119" t="s">
         <v>602</v>
@@ -9514,16 +9515,16 @@
         <v>52</v>
       </c>
       <c r="L119" t="s">
+        <v>663</v>
+      </c>
+      <c r="M119" t="s">
+        <v>51</v>
+      </c>
+      <c r="O119" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y119" s="19" t="s">
         <v>664</v>
-      </c>
-      <c r="M119" t="s">
-        <v>51</v>
-      </c>
-      <c r="O119" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y119" s="19" t="s">
-        <v>665</v>
       </c>
       <c r="AB119" t="str">
         <f t="shared" si="9"/>
@@ -9579,7 +9580,7 @@
         <v>87</v>
       </c>
       <c r="Y120" s="19" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="AB120" t="str">
         <f t="shared" si="9"/>
@@ -9629,7 +9630,7 @@
         <v>51</v>
       </c>
       <c r="Y121" s="19" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="AB121" t="str">
         <f t="shared" si="9"/>
@@ -9916,7 +9917,7 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="C127" t="s">
         <v>50</v>
@@ -9954,7 +9955,7 @@
         <v>51</v>
       </c>
       <c r="Y127" s="4" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="Z127" s="4" t="str">
         <f>"GET [base]/"&amp;B127&amp;"?"&amp;C127&amp;"=123"</f>
@@ -9970,7 +9971,7 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="C128" t="s">
         <v>84</v>
@@ -11055,7 +11056,7 @@
         <v>312</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
@@ -11100,7 +11101,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D38" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="E38" t="s">
         <v>51</v>
@@ -11115,13 +11116,13 @@
         <v>396</v>
       </c>
       <c r="I38" s="4" t="s">
+        <v>704</v>
+      </c>
+      <c r="J38" s="24" t="s">
         <v>705</v>
       </c>
-      <c r="J38" s="24" t="s">
+      <c r="K38" s="4" t="s">
         <v>706</v>
-      </c>
-      <c r="K38" s="4" t="s">
-        <v>707</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
@@ -12747,7 +12748,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="C91" t="str">
         <f t="shared" si="4"/>
@@ -12812,7 +12813,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="C93" t="str">
         <f t="shared" si="4"/>
@@ -12982,21 +12983,21 @@
         <v>525</v>
       </c>
       <c r="D98" s="16" t="s">
+        <v>699</v>
+      </c>
+      <c r="E98" s="16" t="s">
         <v>700</v>
       </c>
-      <c r="E98" s="16" t="s">
+      <c r="F98" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="G98" s="16" t="s">
         <v>701</v>
-      </c>
-      <c r="F98" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="G98" s="16" t="s">
-        <v>702</v>
       </c>
       <c r="H98" s="16"/>
       <c r="I98" s="4"/>
       <c r="J98" s="4" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="K98" t="str">
         <f>"Fetches a bundle of all "&amp;B98&amp;" resources for the specified patient that may match any of the string fields in the name element (including family, give, prefix, suffix, suffix, and/or text)"</f>
@@ -13170,7 +13171,7 @@
         <v>524</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="D2" t="s">
         <v>64</v>
@@ -13363,10 +13364,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>667</v>
+      </c>
+      <c r="B7" t="s">
         <v>668</v>
-      </c>
-      <c r="B7" t="s">
-        <v>669</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
@@ -13517,7 +13518,7 @@
     </row>
     <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B18" t="s">
         <v>595</v>
@@ -13601,10 +13602,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>669</v>
+      </c>
+      <c r="B24" t="s">
         <v>670</v>
-      </c>
-      <c r="B24" t="s">
-        <v>671</v>
       </c>
       <c r="D24" t="s">
         <v>11</v>
@@ -13629,10 +13630,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>671</v>
+      </c>
+      <c r="B26" t="s">
         <v>672</v>
-      </c>
-      <c r="B26" t="s">
-        <v>673</v>
       </c>
       <c r="D26" t="s">
         <v>11</v>
@@ -13643,10 +13644,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>673</v>
+      </c>
+      <c r="B27" t="s">
         <v>674</v>
-      </c>
-      <c r="B27" t="s">
-        <v>675</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
@@ -13657,10 +13658,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>675</v>
+      </c>
+      <c r="B28" t="s">
         <v>676</v>
-      </c>
-      <c r="B28" t="s">
-        <v>677</v>
       </c>
       <c r="D28" t="s">
         <v>11</v>
@@ -13671,7 +13672,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="18" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B29" t="s">
         <v>596</v>
@@ -13699,10 +13700,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B31" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="D31" t="s">
         <v>11</v>
@@ -13713,10 +13714,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>729</v>
+      </c>
+      <c r="B32" t="s">
         <v>730</v>
-      </c>
-      <c r="B32" t="s">
-        <v>731</v>
       </c>
       <c r="D32" t="s">
         <v>11</v>
@@ -13727,10 +13728,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>731</v>
+      </c>
+      <c r="B33" t="s">
         <v>732</v>
-      </c>
-      <c r="B33" t="s">
-        <v>733</v>
       </c>
       <c r="D33" t="s">
         <v>11</v>
@@ -13867,10 +13868,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B43" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="D43" t="s">
         <v>11</v>
@@ -13881,10 +13882,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>727</v>
+      </c>
+      <c r="B44" t="s">
         <v>728</v>
-      </c>
-      <c r="B44" t="s">
-        <v>729</v>
       </c>
       <c r="D44" t="s">
         <v>11</v>
@@ -13909,7 +13910,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="18" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B46" t="s">
         <v>598</v>
@@ -13923,10 +13924,10 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B47" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="D47" t="s">
         <v>11</v>
@@ -14077,21 +14078,21 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B58" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="D58" t="s">
         <v>11</v>
       </c>
       <c r="E58" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B59" t="s">
         <v>599</v>
@@ -14133,16 +14134,16 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>681</v>
+      </c>
+      <c r="B62" t="s">
         <v>682</v>
       </c>
-      <c r="B62" t="s">
+      <c r="D62" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" t="s">
         <v>683</v>
-      </c>
-      <c r="D62" t="s">
-        <v>11</v>
-      </c>
-      <c r="E62" t="s">
-        <v>684</v>
       </c>
     </row>
   </sheetData>
@@ -14161,7 +14162,7 @@
   <dimension ref="A1:Y69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -14268,7 +14269,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="T2" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="U2" t="s">
         <v>64</v>
@@ -14291,7 +14292,7 @@
         <v>474</v>
       </c>
       <c r="T3" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="U3" t="s">
         <v>64</v>
@@ -14311,10 +14312,10 @@
         <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="T4" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="U4" t="s">
         <v>64</v>
@@ -14340,10 +14341,10 @@
         <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="T5" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="U5" t="s">
         <v>64</v>
@@ -14363,7 +14364,7 @@
         <v>11</v>
       </c>
       <c r="T6" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="U6" t="s">
         <v>64</v>
@@ -14386,7 +14387,7 @@
         <v>619</v>
       </c>
       <c r="T7" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="U7" t="s">
         <v>64</v>
@@ -14407,7 +14408,7 @@
       </c>
       <c r="C8" s="2"/>
       <c r="T8" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="U8" t="s">
         <v>64</v>
@@ -14427,10 +14428,10 @@
         <v>11</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>658</v>
+        <v>737</v>
       </c>
       <c r="T9" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="U9" t="s">
         <v>64</v>
@@ -14450,10 +14451,10 @@
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="T10" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="U10" t="s">
         <v>64</v>
@@ -14467,16 +14468,16 @@
     </row>
     <row r="11" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>718</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="25" t="s">
         <v>719</v>
       </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>720</v>
-      </c>
       <c r="T11" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="U11" t="s">
         <v>64</v>
@@ -14492,10 +14493,10 @@
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="T12" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="U12" t="s">
         <v>64</v>
@@ -14509,16 +14510,16 @@
     </row>
     <row r="13" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>720</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="25" t="s">
         <v>721</v>
       </c>
-      <c r="B13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="25" t="s">
-        <v>722</v>
-      </c>
       <c r="T13" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="U13" t="s">
         <v>64</v>
@@ -14537,7 +14538,7 @@
         <v>620</v>
       </c>
       <c r="T14" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="U14" t="s">
         <v>64</v>
@@ -14557,7 +14558,7 @@
         <v>11</v>
       </c>
       <c r="T15" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="U15" t="s">
         <v>64</v>
@@ -14567,16 +14568,16 @@
     </row>
     <row r="16" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>708</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="25" t="s">
         <v>709</v>
       </c>
-      <c r="B16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="25" t="s">
-        <v>710</v>
-      </c>
       <c r="T16" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="U16" t="s">
         <v>64</v>
@@ -14595,7 +14596,7 @@
         <v>475</v>
       </c>
       <c r="T17" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="U17" t="s">
         <v>64</v>
@@ -14614,7 +14615,7 @@
         <v>476</v>
       </c>
       <c r="T18" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="U18" t="s">
         <v>64</v>
@@ -14640,10 +14641,10 @@
         <v>11</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="T19" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="U19" t="s">
         <v>64</v>
@@ -14672,7 +14673,7 @@
         <v>477</v>
       </c>
       <c r="T20" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="U20" t="s">
         <v>64</v>
@@ -14698,10 +14699,10 @@
         <v>11</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="T21" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="U21" t="s">
         <v>64</v>
@@ -14724,7 +14725,7 @@
         <v>621</v>
       </c>
       <c r="T22" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="U22" t="s">
         <v>64</v>
@@ -14743,7 +14744,7 @@
         <v>622</v>
       </c>
       <c r="T23" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="U23" t="s">
         <v>64</v>
@@ -14763,10 +14764,10 @@
         <v>11</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="T24" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="U24" t="s">
         <v>64</v>
@@ -14782,10 +14783,10 @@
         <v>11</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="T25" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="U25" t="s">
         <v>64</v>
@@ -14807,10 +14808,10 @@
         <v>11</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="T26" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="U26" t="s">
         <v>64</v>
@@ -14830,10 +14831,10 @@
         <v>11</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="T27" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="U27" t="s">
         <v>64</v>
@@ -14841,13 +14842,13 @@
     </row>
     <row r="28" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B28" t="s">
         <v>64</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="X28" s="13"/>
       <c r="Y28" s="13"/>
@@ -14860,7 +14861,7 @@
         <v>64</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="X29" s="13" t="s">
         <v>433</v>
@@ -14877,7 +14878,7 @@
         <v>11</v>
       </c>
       <c r="T30" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="U30" t="s">
         <v>64</v>
@@ -14897,10 +14898,10 @@
         <v>11</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="T31" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="U31" t="s">
         <v>64</v>
@@ -14914,13 +14915,13 @@
     </row>
     <row r="32" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B32" t="s">
         <v>11</v>
       </c>
       <c r="T32" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="U32" t="s">
         <v>64</v>
@@ -15019,7 +15020,7 @@
         <v>64</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -15072,7 +15073,7 @@
         <v>353</v>
       </c>
       <c r="F1" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="G1" t="s">
         <v>354</v>
@@ -15090,13 +15091,13 @@
         <v>357</v>
       </c>
       <c r="L1" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="M1" t="s">
         <v>358</v>
       </c>
       <c r="N1" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="O1" t="s">
         <v>359</v>
@@ -15105,13 +15106,13 @@
         <v>360</v>
       </c>
       <c r="Q1" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="R1" t="s">
         <v>361</v>
       </c>
       <c r="S1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="T1" t="s">
         <v>362</v>
@@ -15144,7 +15145,7 @@
         <v>416</v>
       </c>
       <c r="AD1" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="AE1" t="s">
         <v>601</v>
@@ -15159,7 +15160,7 @@
         <v>432</v>
       </c>
       <c r="AI1" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update canonical urls in examples and capability statements to include the version [FHIR-41256]
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB79BEB-1629-0843-8241-1526B1EA7178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E35E1EB7-5AC3-8949-BE83-4B098A4C2FED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51900" yWindow="6200" windowWidth="51200" windowHeight="20620" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="6200" windowWidth="51200" windowHeight="20620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -1710,9 +1710,6 @@
     <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-sexual-orientation</t>
   </si>
   <si>
-    <t>5.0.0</t>
-  </si>
-  <si>
     <t>http://hl7.org/fhir/smart-app-launch/ImplementationGuide/hl7.fhir.uv.smart-app-launch</t>
   </si>
   <si>
@@ -2474,6 +2471,9 @@
         * If the endpoint is outside the FHIR base URL, it **SHOULD NOT** require additional authorization to access.
    * If there are multiple `DocumentReference.content` element repetitions, these **SHALL** all represent the same document in different format or attachment metadata. The content element **SHALL** not contain different versions of the same content. For version handling use multiple DocumentReferences with `DocumentReference.relatesTo`
 * Every DocumentReference must have a responsible Organization. The organization responsible for the DocumentReference **SHALL** be present either in `DocumentReference.custodian` or accessible in the Provenance resource targeting the DocumentReference using `Provenance.agent.who` or `Provenance.agent.onBehalfOf`.</t>
+  </si>
+  <si>
+    <t>7.0.0-ballot</t>
   </si>
 </sst>
 </file>
@@ -3104,7 +3104,7 @@
         <v>446</v>
       </c>
       <c r="B2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -3136,7 +3136,7 @@
         <v>62</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -3152,7 +3152,7 @@
         <v>453</v>
       </c>
       <c r="B8" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -3219,7 +3219,7 @@
         <v>39</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>30</v>
@@ -4175,7 +4175,7 @@
         <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D19" t="s">
         <v>28</v>
@@ -4333,7 +4333,7 @@
         <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D22" t="s">
         <v>28</v>
@@ -4480,7 +4480,7 @@
         <v>19</v>
       </c>
       <c r="C25" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D25" t="s">
         <v>28</v>
@@ -4536,7 +4536,7 @@
         <v>0</v>
       </c>
       <c r="F26" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="0"/>
@@ -4754,7 +4754,7 @@
         <v>51</v>
       </c>
       <c r="Y30" s="4" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="Z30" t="s">
         <v>167</v>
@@ -4776,7 +4776,7 @@
         <v>79</v>
       </c>
       <c r="C31" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="D31" t="s">
         <v>28</v>
@@ -4798,19 +4798,19 @@
         <v>52</v>
       </c>
       <c r="L31" t="s">
+        <v>629</v>
+      </c>
+      <c r="M31" t="s">
+        <v>51</v>
+      </c>
+      <c r="O31" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y31" s="4" t="s">
         <v>630</v>
       </c>
-      <c r="M31" t="s">
-        <v>51</v>
-      </c>
-      <c r="O31" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y31" s="4" t="s">
+      <c r="Z31" t="s">
         <v>631</v>
-      </c>
-      <c r="Z31" t="s">
-        <v>632</v>
       </c>
       <c r="AA31" s="8" t="str">
         <f>"Fetches a bundle of all "&amp;B31&amp;" resources matching the name"</f>
@@ -4826,7 +4826,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="C32" t="s">
         <v>50</v>
@@ -4851,7 +4851,7 @@
         <v>52</v>
       </c>
       <c r="L32" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="M32" t="s">
         <v>51</v>
@@ -4869,7 +4869,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="C33" t="s">
         <v>65</v>
@@ -4913,7 +4913,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="C34" t="s">
         <v>62</v>
@@ -4960,7 +4960,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="C35" t="s">
         <v>56</v>
@@ -5004,7 +5004,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="C36" t="s">
         <v>57</v>
@@ -5060,7 +5060,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="C37" t="s">
         <v>54</v>
@@ -5104,7 +5104,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="C38" t="s">
         <v>61</v>
@@ -5205,7 +5205,7 @@
         <v>132</v>
       </c>
       <c r="C40" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D40" t="s">
         <v>28</v>
@@ -5259,7 +5259,7 @@
         <v>132</v>
       </c>
       <c r="C41" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D41" t="s">
         <v>28</v>
@@ -5313,7 +5313,7 @@
         <v>132</v>
       </c>
       <c r="C42" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D42" t="s">
         <v>28</v>
@@ -5452,7 +5452,7 @@
         <v>51</v>
       </c>
       <c r="Y44" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="Z44" s="4" t="str">
         <f>"GET [base]/"&amp;B44&amp;"?patient=1137192"</f>
@@ -7659,7 +7659,7 @@
         <v>51</v>
       </c>
       <c r="X85" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="Y85" t="str">
         <f>"support searching for all "&amp;LOWER(B85)&amp;"s for a patient"</f>
@@ -7792,7 +7792,7 @@
         <v>240</v>
       </c>
       <c r="C88" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="D88" t="s">
         <v>64</v>
@@ -7830,7 +7830,7 @@
         <v>51</v>
       </c>
       <c r="Y88" s="4" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="Z88" s="4" t="str">
         <f>"GET [base]/"&amp;B88&amp;"?"&amp;C88&amp;"=http://snomed.info/sct\|17561000"</f>
@@ -8794,7 +8794,7 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C106" t="s">
         <v>56</v>
@@ -8847,7 +8847,7 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C107" t="s">
         <v>84</v>
@@ -8906,7 +8906,7 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C108" t="s">
         <v>134</v>
@@ -8956,7 +8956,7 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C109" t="s">
         <v>24</v>
@@ -9009,10 +9009,10 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C110" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D110" t="s">
         <v>28</v>
@@ -9063,7 +9063,7 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C111" t="s">
         <v>50</v>
@@ -9098,10 +9098,10 @@
         <v>51</v>
       </c>
       <c r="Y111" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="Z111" s="4" t="s">
         <v>546</v>
-      </c>
-      <c r="Z111" s="4" t="s">
-        <v>547</v>
       </c>
       <c r="AB111" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B111)&amp;"-"&amp;SUBSTITUTE(C111,"_","")&amp;".html")</f>
@@ -9159,7 +9159,7 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C113" t="s">
         <v>50</v>
@@ -9194,10 +9194,10 @@
         <v>51</v>
       </c>
       <c r="Y113" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="Z113" s="4" t="s">
         <v>548</v>
-      </c>
-      <c r="Z113" s="4" t="s">
-        <v>549</v>
       </c>
       <c r="AA113" s="8"/>
       <c r="AB113" t="str">
@@ -9210,7 +9210,7 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C114" t="s">
         <v>84</v>
@@ -9269,7 +9269,7 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C115" t="s">
         <v>21</v>
@@ -9304,7 +9304,7 @@
         <v>51</v>
       </c>
       <c r="Y115" s="4" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="Z115" s="4" t="str">
         <f>"GET [base]/"&amp;B115&amp;"?"&amp;C115&amp;"=Mary Shaw"</f>
@@ -9324,7 +9324,7 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C116" t="s">
         <v>50</v>
@@ -9363,7 +9363,7 @@
         <v>support fetching a QuestionnaireResponse</v>
       </c>
       <c r="Z116" s="4" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="AB116" t="str">
         <f t="shared" si="9"/>
@@ -9375,7 +9375,7 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C117" t="s">
         <v>84</v>
@@ -9434,7 +9434,7 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C118" t="s">
         <v>56</v>
@@ -9475,7 +9475,7 @@
         <v>51</v>
       </c>
       <c r="Y118" s="19" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="AB118" t="str">
         <f t="shared" si="9"/>
@@ -9487,10 +9487,10 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="C119" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="D119" t="s">
         <v>28</v>
@@ -9515,16 +9515,16 @@
         <v>52</v>
       </c>
       <c r="L119" t="s">
+        <v>662</v>
+      </c>
+      <c r="M119" t="s">
+        <v>51</v>
+      </c>
+      <c r="O119" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y119" s="19" t="s">
         <v>663</v>
-      </c>
-      <c r="M119" t="s">
-        <v>51</v>
-      </c>
-      <c r="O119" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y119" s="19" t="s">
-        <v>664</v>
       </c>
       <c r="AB119" t="str">
         <f t="shared" si="9"/>
@@ -9536,10 +9536,10 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C120" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D120" t="s">
         <v>28</v>
@@ -9580,7 +9580,7 @@
         <v>87</v>
       </c>
       <c r="Y120" s="19" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="AB120" t="str">
         <f t="shared" si="9"/>
@@ -9592,10 +9592,10 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C121" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D121" t="s">
         <v>28</v>
@@ -9630,7 +9630,7 @@
         <v>51</v>
       </c>
       <c r="Y121" s="19" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="AB121" t="str">
         <f t="shared" si="9"/>
@@ -9642,7 +9642,7 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C122" t="s">
         <v>84</v>
@@ -9680,7 +9680,7 @@
         <v>51</v>
       </c>
       <c r="Y122" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="Z122" s="4" t="str">
         <f>"GET [base]/"&amp;B122&amp;"?patient=1137192"</f>
@@ -9700,7 +9700,7 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C123" t="s">
         <v>56</v>
@@ -9753,7 +9753,7 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C124" t="s">
         <v>12</v>
@@ -9806,7 +9806,7 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C125" t="s">
         <v>84</v>
@@ -9844,10 +9844,10 @@
         <v>51</v>
       </c>
       <c r="X125" s="6" t="s">
+        <v>635</v>
+      </c>
+      <c r="Z125" s="8" t="s">
         <v>636</v>
-      </c>
-      <c r="Z125" s="8" t="s">
-        <v>637</v>
       </c>
       <c r="AA125" s="8" t="str">
         <f>"Fetches a bundle of all "&amp;B125&amp; " resources for the specified patient."</f>
@@ -9863,10 +9863,10 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
+        <v>637</v>
+      </c>
+      <c r="C126" t="s">
         <v>638</v>
-      </c>
-      <c r="C126" t="s">
-        <v>639</v>
       </c>
       <c r="D126" t="s">
         <v>28</v>
@@ -9917,7 +9917,7 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="C127" t="s">
         <v>50</v>
@@ -9955,7 +9955,7 @@
         <v>51</v>
       </c>
       <c r="Y127" s="4" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="Z127" s="4" t="str">
         <f>"GET [base]/"&amp;B127&amp;"?"&amp;C127&amp;"=123"</f>
@@ -9971,7 +9971,7 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="C128" t="s">
         <v>84</v>
@@ -10074,7 +10074,7 @@
         <v>90</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>91</v>
@@ -10504,7 +10504,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D17" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F17" t="s">
         <v>64</v>
@@ -10516,7 +10516,7 @@
         <v>289</v>
       </c>
       <c r="J17" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="K17" s="4" t="str">
         <f t="shared" si="1"/>
@@ -10592,7 +10592,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D20" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="F20" t="s">
         <v>64</v>
@@ -10604,7 +10604,7 @@
         <v>294</v>
       </c>
       <c r="J20" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="K20" s="4" t="str">
         <f t="shared" si="1"/>
@@ -10914,7 +10914,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D32" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="F32" t="s">
         <v>64</v>
@@ -10923,10 +10923,10 @@
         <v>128</v>
       </c>
       <c r="I32" s="4" t="s">
+        <v>640</v>
+      </c>
+      <c r="J32" s="4" t="s">
         <v>641</v>
-      </c>
-      <c r="J32" s="4" t="s">
-        <v>642</v>
       </c>
       <c r="K32" s="4" t="str">
         <f t="shared" si="1"/>
@@ -11056,7 +11056,7 @@
         <v>312</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
@@ -11101,7 +11101,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D38" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="E38" t="s">
         <v>51</v>
@@ -11116,13 +11116,13 @@
         <v>396</v>
       </c>
       <c r="I38" s="4" t="s">
+        <v>703</v>
+      </c>
+      <c r="J38" s="24" t="s">
         <v>704</v>
       </c>
-      <c r="J38" s="24" t="s">
+      <c r="K38" s="4" t="s">
         <v>705</v>
-      </c>
-      <c r="K38" s="4" t="s">
-        <v>706</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
@@ -11137,7 +11137,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D39" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="F39" t="s">
         <v>64</v>
@@ -11149,10 +11149,10 @@
         <v>144</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
@@ -11209,7 +11209,7 @@
         <v>147</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="K41" s="4" t="s">
         <v>150</v>
@@ -11227,7 +11227,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D42" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="F42" t="s">
         <v>64</v>
@@ -11239,7 +11239,7 @@
         <v>147</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="K42" s="4" t="s">
         <v>150</v>
@@ -11257,7 +11257,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D43" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="F43" t="s">
         <v>64</v>
@@ -11269,7 +11269,7 @@
         <v>147</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="K43" s="4" t="s">
         <v>150</v>
@@ -11287,7 +11287,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D44" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="F44" t="s">
         <v>64</v>
@@ -11299,7 +11299,7 @@
         <v>147</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="K44" s="4" t="s">
         <v>150</v>
@@ -11405,7 +11405,7 @@
         <v>173</v>
       </c>
       <c r="C48" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="D48" t="s">
         <v>110</v>
@@ -11435,7 +11435,7 @@
         <v>173</v>
       </c>
       <c r="C49" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="D49" t="s">
         <v>139</v>
@@ -11468,7 +11468,7 @@
         <v>173</v>
       </c>
       <c r="C50" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="D50" t="s">
         <v>141</v>
@@ -11498,7 +11498,7 @@
         <v>173</v>
       </c>
       <c r="C51" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="D51" t="s">
         <v>188</v>
@@ -11531,7 +11531,7 @@
         <v>173</v>
       </c>
       <c r="C52" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="D52" t="s">
         <v>212</v>
@@ -11909,7 +11909,7 @@
         <v>177</v>
       </c>
       <c r="C64" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="D64" t="s">
         <v>229</v>
@@ -11941,7 +11941,7 @@
         <v>177</v>
       </c>
       <c r="C65" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="D65" t="s">
         <v>139</v>
@@ -11974,7 +11974,7 @@
         <v>177</v>
       </c>
       <c r="C66" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="D66" t="s">
         <v>141</v>
@@ -12004,7 +12004,7 @@
         <v>177</v>
       </c>
       <c r="C67" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="D67" t="s">
         <v>188</v>
@@ -12037,7 +12037,7 @@
         <v>177</v>
       </c>
       <c r="C68" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="D68" t="s">
         <v>212</v>
@@ -12067,7 +12067,7 @@
         <v>304</v>
       </c>
       <c r="C69" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="D69" t="s">
         <v>110</v>
@@ -12242,13 +12242,13 @@
         <v>295</v>
       </c>
       <c r="I74" s="4" t="s">
+        <v>562</v>
+      </c>
+      <c r="J74" s="4" t="s">
         <v>563</v>
       </c>
-      <c r="J74" s="4" t="s">
+      <c r="K74" s="8" t="s">
         <v>564</v>
-      </c>
-      <c r="K74" s="8" t="s">
-        <v>565</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
@@ -12446,7 +12446,7 @@
         <v>241</v>
       </c>
       <c r="C81" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="D81" t="s">
         <v>112</v>
@@ -12475,7 +12475,7 @@
         <v>241</v>
       </c>
       <c r="C82" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="D82" t="s">
         <v>110</v>
@@ -12487,13 +12487,13 @@
         <v>100</v>
       </c>
       <c r="I82" s="4" t="s">
+        <v>643</v>
+      </c>
+      <c r="J82" s="4" t="s">
         <v>644</v>
       </c>
-      <c r="J82" s="4" t="s">
+      <c r="K82" s="4" t="s">
         <v>645</v>
-      </c>
-      <c r="K82" s="4" t="s">
-        <v>646</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
@@ -12508,7 +12508,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
       </c>
       <c r="D83" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F83" t="s">
         <v>64</v>
@@ -12517,13 +12517,13 @@
         <v>100</v>
       </c>
       <c r="I83" s="4" t="s">
+        <v>566</v>
+      </c>
+      <c r="J83" s="4" t="s">
         <v>567</v>
       </c>
-      <c r="J83" s="4" t="s">
+      <c r="K83" s="4" t="s">
         <v>568</v>
-      </c>
-      <c r="K83" s="4" t="s">
-        <v>569</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
@@ -12531,7 +12531,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C84" t="str">
         <f t="shared" ref="C84:C97" si="4">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B84)</f>
@@ -12550,7 +12550,7 @@
         <v>287</v>
       </c>
       <c r="J84" s="4" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="K84" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B84&amp;" resources for the specified "&amp;SUBSTITUTE(D84,","," and ")</f>
@@ -12562,7 +12562,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C85" t="str">
         <f t="shared" si="4"/>
@@ -12581,7 +12581,7 @@
         <v>192</v>
       </c>
       <c r="J85" s="4" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="K85" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B85&amp;" resources for the specified patient and  a category code"</f>
@@ -12593,7 +12593,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C86" t="str">
         <f t="shared" si="4"/>
@@ -12612,7 +12612,7 @@
         <v>193</v>
       </c>
       <c r="J86" s="4" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="K86" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B86&amp;" resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes."</f>
@@ -12624,14 +12624,14 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C87" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D87" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="F87" t="s">
         <v>11</v>
@@ -12643,7 +12643,7 @@
         <v>195</v>
       </c>
       <c r="J87" s="4" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="K87" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B87&amp;" resources for the specified patient and date and a category code"</f>
@@ -12655,14 +12655,14 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C88" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D88" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="F88" t="s">
         <v>64</v>
@@ -12671,10 +12671,10 @@
         <v>211</v>
       </c>
       <c r="I88" s="4" t="s">
+        <v>575</v>
+      </c>
+      <c r="J88" s="4" t="s">
         <v>576</v>
-      </c>
-      <c r="J88" s="4" t="s">
-        <v>577</v>
       </c>
       <c r="K88" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B88&amp;" resources for the specified patient and date and service code(s).  SHOULD support search by multiple report codes."</f>
@@ -12693,7 +12693,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D89" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="F89" t="s">
         <v>64</v>
@@ -12702,10 +12702,10 @@
         <v>100</v>
       </c>
       <c r="I89" s="4" t="s">
+        <v>578</v>
+      </c>
+      <c r="J89" s="4" t="s">
         <v>579</v>
-      </c>
-      <c r="J89" s="4" t="s">
-        <v>580</v>
       </c>
       <c r="K89" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B89&amp;" resources for the specified "&amp;SUBSTITUTE(D89,","," and ")</f>
@@ -12717,7 +12717,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C90" t="str">
         <f t="shared" si="4"/>
@@ -12733,10 +12733,10 @@
         <v>100</v>
       </c>
       <c r="I90" t="s">
+        <v>603</v>
+      </c>
+      <c r="J90" s="4" t="s">
         <v>604</v>
-      </c>
-      <c r="J90" s="4" t="s">
-        <v>605</v>
       </c>
       <c r="K90" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B90&amp;" resources for the specified "&amp;SUBSTITUTE(D90,","," and ")</f>
@@ -12748,14 +12748,14 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="C91" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="D91" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="F91" t="s">
         <v>64</v>
@@ -12764,13 +12764,13 @@
         <v>100</v>
       </c>
       <c r="H91" t="s">
+        <v>606</v>
+      </c>
+      <c r="I91" t="s">
+        <v>603</v>
+      </c>
+      <c r="J91" s="4" t="s">
         <v>607</v>
-      </c>
-      <c r="I91" t="s">
-        <v>604</v>
-      </c>
-      <c r="J91" s="4" t="s">
-        <v>608</v>
       </c>
       <c r="K91" t="str">
         <f>"Fetches a bundle of all "&amp;B91&amp;" resources for the specified "&amp;SUBSTITUTE(D91,","," and  ") &amp; "= 'sdoh'"</f>
@@ -12782,14 +12782,14 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C92" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D92" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F92" t="s">
         <v>64</v>
@@ -12798,10 +12798,10 @@
         <v>143</v>
       </c>
       <c r="I92" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="J92" s="4" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="K92" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B92&amp;" resources for the specified patient and date"</f>
@@ -12813,14 +12813,14 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="C93" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="D93" s="16" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="F93" t="s">
         <v>64</v>
@@ -12829,13 +12829,13 @@
         <v>211</v>
       </c>
       <c r="H93" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="I93" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="J93" s="4" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="K93" t="str">
         <f>"Fetches a bundle of all "&amp;B93&amp;" resources tagged as 'sdoh' for the specified patient and date"</f>
@@ -12847,14 +12847,14 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C94" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D94" s="16" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="F94" t="s">
         <v>64</v>
@@ -12863,10 +12863,10 @@
         <v>85</v>
       </c>
       <c r="I94" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="J94" s="4" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="K94" t="str">
         <f>"Fetches a bundle of all "&amp;B94&amp;" resources for the specified patient that have been completed against a specified form."</f>
@@ -12878,7 +12878,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="16" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C95" t="str">
         <f t="shared" si="4"/>
@@ -12896,10 +12896,10 @@
       </c>
       <c r="H95" s="16"/>
       <c r="I95" s="4" t="s">
+        <v>646</v>
+      </c>
+      <c r="J95" s="4" t="s">
         <v>647</v>
-      </c>
-      <c r="J95" s="4" t="s">
-        <v>648</v>
       </c>
       <c r="K95" t="str">
         <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed))."</f>
@@ -12911,7 +12911,7 @@
         <v>95</v>
       </c>
       <c r="B96" s="16" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C96" t="str">
         <f t="shared" si="4"/>
@@ -12929,10 +12929,10 @@
       </c>
       <c r="H96" s="16"/>
       <c r="I96" s="4" t="s">
+        <v>648</v>
+      </c>
+      <c r="J96" s="4" t="s">
         <v>649</v>
-      </c>
-      <c r="J96" s="4" t="s">
-        <v>650</v>
       </c>
       <c r="K96" t="str">
         <f>"Fetches a bundle of all "&amp;B96&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed) and type of dispense (e.g., partially dispensed)."</f>
@@ -12944,14 +12944,14 @@
         <v>96</v>
       </c>
       <c r="B97" s="16" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C97" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationdispense</v>
       </c>
       <c r="D97" s="16" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="E97" s="16"/>
       <c r="F97" s="16" t="s">
@@ -12962,10 +12962,10 @@
       </c>
       <c r="H97" s="16"/>
       <c r="I97" s="4" t="s">
+        <v>651</v>
+      </c>
+      <c r="J97" s="4" t="s">
         <v>652</v>
-      </c>
-      <c r="J97" s="4" t="s">
-        <v>653</v>
       </c>
       <c r="K97" t="str">
         <f>"Fetches a bundle of all "&amp;B96&amp;" resources for the specified patient for a given dispense and date or range"</f>
@@ -12977,27 +12977,27 @@
         <v>97</v>
       </c>
       <c r="B98" s="16" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C98" s="22" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D98" s="16" t="s">
+        <v>698</v>
+      </c>
+      <c r="E98" s="16" t="s">
         <v>699</v>
       </c>
-      <c r="E98" s="16" t="s">
+      <c r="F98" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="G98" s="16" t="s">
         <v>700</v>
-      </c>
-      <c r="F98" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="G98" s="16" t="s">
-        <v>701</v>
       </c>
       <c r="H98" s="16"/>
       <c r="I98" s="4"/>
       <c r="J98" s="4" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="K98" t="str">
         <f>"Fetches a bundle of all "&amp;B98&amp;" resources for the specified patient that may match any of the string fields in the name element (including family, give, prefix, suffix, suffix, and/or text)"</f>
@@ -13024,8 +13024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13047,7 +13047,7 @@
         <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>523</v>
+        <v>737</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -13087,7 +13087,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -13095,7 +13095,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -13168,10 +13168,10 @@
         <v>509</v>
       </c>
       <c r="B2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D2" t="s">
         <v>64</v>
@@ -13179,7 +13179,7 @@
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>519</v>
@@ -13336,10 +13336,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B5" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
@@ -13350,10 +13350,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B6" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -13364,16 +13364,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>666</v>
+      </c>
+      <c r="B7" t="s">
         <v>667</v>
       </c>
-      <c r="B7" t="s">
-        <v>668</v>
-      </c>
       <c r="D7" t="s">
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -13434,7 +13434,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B12" t="s">
         <v>347</v>
@@ -13448,86 +13448,86 @@
     </row>
     <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
+        <v>583</v>
+      </c>
+      <c r="B13" t="s">
         <v>584</v>
       </c>
-      <c r="B13" t="s">
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
         <v>585</v>
-      </c>
-      <c r="D13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" t="s">
-        <v>586</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
+        <v>586</v>
+      </c>
+      <c r="B14" t="s">
         <v>587</v>
       </c>
-      <c r="B14" t="s">
-        <v>588</v>
-      </c>
       <c r="D14" t="s">
         <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
+        <v>588</v>
+      </c>
+      <c r="B15" t="s">
         <v>589</v>
       </c>
-      <c r="B15" t="s">
-        <v>590</v>
-      </c>
       <c r="D15" t="s">
         <v>11</v>
       </c>
       <c r="E15" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
+        <v>590</v>
+      </c>
+      <c r="B16" t="s">
         <v>591</v>
       </c>
-      <c r="B16" t="s">
-        <v>592</v>
-      </c>
       <c r="D16" t="s">
         <v>11</v>
       </c>
       <c r="E16" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
+        <v>592</v>
+      </c>
+      <c r="B17" t="s">
         <v>593</v>
       </c>
-      <c r="B17" t="s">
-        <v>594</v>
-      </c>
       <c r="D17" t="s">
         <v>11</v>
       </c>
       <c r="E17" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B18" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="D18" t="s">
         <v>11</v>
       </c>
       <c r="E18" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -13602,16 +13602,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>668</v>
+      </c>
+      <c r="B24" t="s">
         <v>669</v>
       </c>
-      <c r="B24" t="s">
-        <v>670</v>
-      </c>
       <c r="D24" t="s">
         <v>11</v>
       </c>
       <c r="E24" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -13630,10 +13630,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>670</v>
+      </c>
+      <c r="B26" t="s">
         <v>671</v>
-      </c>
-      <c r="B26" t="s">
-        <v>672</v>
       </c>
       <c r="D26" t="s">
         <v>11</v>
@@ -13644,10 +13644,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>672</v>
+      </c>
+      <c r="B27" t="s">
         <v>673</v>
-      </c>
-      <c r="B27" t="s">
-        <v>674</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
@@ -13658,10 +13658,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>674</v>
+      </c>
+      <c r="B28" t="s">
         <v>675</v>
-      </c>
-      <c r="B28" t="s">
-        <v>676</v>
       </c>
       <c r="D28" t="s">
         <v>11</v>
@@ -13672,10 +13672,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="18" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B29" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D29" t="s">
         <v>11</v>
@@ -13700,10 +13700,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B31" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="D31" t="s">
         <v>11</v>
@@ -13714,10 +13714,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>728</v>
+      </c>
+      <c r="B32" t="s">
         <v>729</v>
-      </c>
-      <c r="B32" t="s">
-        <v>730</v>
       </c>
       <c r="D32" t="s">
         <v>11</v>
@@ -13728,10 +13728,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>730</v>
+      </c>
+      <c r="B33" t="s">
         <v>731</v>
-      </c>
-      <c r="B33" t="s">
-        <v>732</v>
       </c>
       <c r="D33" t="s">
         <v>11</v>
@@ -13815,7 +13815,7 @@
         <v>522</v>
       </c>
       <c r="B39" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D39" t="s">
         <v>11</v>
@@ -13868,10 +13868,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B43" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="D43" t="s">
         <v>11</v>
@@ -13882,10 +13882,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>726</v>
+      </c>
+      <c r="B44" t="s">
         <v>727</v>
-      </c>
-      <c r="B44" t="s">
-        <v>728</v>
       </c>
       <c r="D44" t="s">
         <v>11</v>
@@ -13910,10 +13910,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="18" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B46" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="D46" t="s">
         <v>11</v>
@@ -13924,10 +13924,10 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B47" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="D47" t="s">
         <v>11</v>
@@ -13955,7 +13955,7 @@
         <v>478</v>
       </c>
       <c r="B49" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="D49" t="s">
         <v>11</v>
@@ -14078,72 +14078,72 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B58" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="D58" t="s">
         <v>11</v>
       </c>
       <c r="E58" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B59" t="s">
+        <v>598</v>
+      </c>
+      <c r="D59" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59" t="s">
         <v>599</v>
-      </c>
-      <c r="D59" t="s">
-        <v>11</v>
-      </c>
-      <c r="E59" t="s">
-        <v>600</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="18" t="s">
+        <v>524</v>
+      </c>
+      <c r="B60" t="s">
         <v>525</v>
       </c>
-      <c r="B60" t="s">
+      <c r="D60" t="s">
+        <v>11</v>
+      </c>
+      <c r="E60" t="s">
         <v>526</v>
-      </c>
-      <c r="D60" t="s">
-        <v>11</v>
-      </c>
-      <c r="E60" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="18" t="s">
+        <v>527</v>
+      </c>
+      <c r="B61" t="s">
         <v>528</v>
       </c>
-      <c r="B61" t="s">
+      <c r="D61" t="s">
+        <v>11</v>
+      </c>
+      <c r="E61" t="s">
         <v>529</v>
-      </c>
-      <c r="D61" t="s">
-        <v>11</v>
-      </c>
-      <c r="E61" t="s">
-        <v>530</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>680</v>
+      </c>
+      <c r="B62" t="s">
         <v>681</v>
       </c>
-      <c r="B62" t="s">
+      <c r="D62" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" t="s">
         <v>682</v>
-      </c>
-      <c r="D62" t="s">
-        <v>11</v>
-      </c>
-      <c r="E62" t="s">
-        <v>683</v>
       </c>
     </row>
   </sheetData>
@@ -14161,7 +14161,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{352F3A6C-0DAD-1041-B50E-04478951E07A}">
   <dimension ref="A1:Y69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -14269,7 +14269,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="T2" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="U2" t="s">
         <v>64</v>
@@ -14292,7 +14292,7 @@
         <v>474</v>
       </c>
       <c r="T3" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="U3" t="s">
         <v>64</v>
@@ -14312,19 +14312,19 @@
         <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="T4" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="U4" t="s">
         <v>64</v>
       </c>
       <c r="V4" t="s">
+        <v>530</v>
+      </c>
+      <c r="W4" t="s">
         <v>531</v>
-      </c>
-      <c r="W4" t="s">
-        <v>532</v>
       </c>
       <c r="X4" s="13" t="s">
         <v>433</v>
@@ -14341,10 +14341,10 @@
         <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="T5" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="U5" t="s">
         <v>64</v>
@@ -14358,13 +14358,13 @@
     </row>
     <row r="6" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="T6" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="U6" t="s">
         <v>64</v>
@@ -14384,10 +14384,10 @@
         <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="T7" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="U7" t="s">
         <v>64</v>
@@ -14408,7 +14408,7 @@
       </c>
       <c r="C8" s="2"/>
       <c r="T8" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="U8" t="s">
         <v>64</v>
@@ -14428,10 +14428,10 @@
         <v>11</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="T9" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="U9" t="s">
         <v>64</v>
@@ -14451,10 +14451,10 @@
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="T10" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="U10" t="s">
         <v>64</v>
@@ -14468,16 +14468,16 @@
     </row>
     <row r="11" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>717</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="25" t="s">
         <v>718</v>
       </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>719</v>
-      </c>
       <c r="T11" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="U11" t="s">
         <v>64</v>
@@ -14493,10 +14493,10 @@
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="T12" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="U12" t="s">
         <v>64</v>
@@ -14510,16 +14510,16 @@
     </row>
     <row r="13" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>719</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="25" t="s">
         <v>720</v>
       </c>
-      <c r="B13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="25" t="s">
-        <v>721</v>
-      </c>
       <c r="T13" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="U13" t="s">
         <v>64</v>
@@ -14535,10 +14535,10 @@
         <v>11</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="T14" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="U14" t="s">
         <v>64</v>
@@ -14558,7 +14558,7 @@
         <v>11</v>
       </c>
       <c r="T15" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="U15" t="s">
         <v>64</v>
@@ -14568,16 +14568,16 @@
     </row>
     <row r="16" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>707</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="25" t="s">
         <v>708</v>
       </c>
-      <c r="B16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="25" t="s">
-        <v>709</v>
-      </c>
       <c r="T16" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="U16" t="s">
         <v>64</v>
@@ -14596,7 +14596,7 @@
         <v>475</v>
       </c>
       <c r="T17" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="U17" t="s">
         <v>64</v>
@@ -14615,7 +14615,7 @@
         <v>476</v>
       </c>
       <c r="T18" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="U18" t="s">
         <v>64</v>
@@ -14635,25 +14635,25 @@
     </row>
     <row r="19" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>634</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>709</v>
+      </c>
+      <c r="T19" t="s">
+        <v>706</v>
+      </c>
+      <c r="U19" t="s">
+        <v>64</v>
+      </c>
+      <c r="V19" t="s">
+        <v>64</v>
+      </c>
+      <c r="W19" s="6" t="s">
         <v>635</v>
-      </c>
-      <c r="B19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>710</v>
-      </c>
-      <c r="T19" t="s">
-        <v>707</v>
-      </c>
-      <c r="U19" t="s">
-        <v>64</v>
-      </c>
-      <c r="V19" t="s">
-        <v>64</v>
-      </c>
-      <c r="W19" s="6" t="s">
-        <v>636</v>
       </c>
       <c r="X19" s="13" t="s">
         <v>433</v>
@@ -14673,7 +14673,7 @@
         <v>477</v>
       </c>
       <c r="T20" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="U20" t="s">
         <v>64</v>
@@ -14699,10 +14699,10 @@
         <v>11</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="T21" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="U21" t="s">
         <v>64</v>
@@ -14722,10 +14722,10 @@
         <v>11</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="T22" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="U22" t="s">
         <v>64</v>
@@ -14741,10 +14741,10 @@
         <v>11</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="T23" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="U23" t="s">
         <v>64</v>
@@ -14764,10 +14764,10 @@
         <v>11</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="T24" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="U24" t="s">
         <v>64</v>
@@ -14783,10 +14783,10 @@
         <v>11</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="T25" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="U25" t="s">
         <v>64</v>
@@ -14808,10 +14808,10 @@
         <v>11</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="T26" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="U26" t="s">
         <v>64</v>
@@ -14831,10 +14831,10 @@
         <v>11</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="T27" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="U27" t="s">
         <v>64</v>
@@ -14842,26 +14842,26 @@
     </row>
     <row r="28" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B28" t="s">
         <v>64</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="X28" s="13"/>
       <c r="Y28" s="13"/>
     </row>
     <row r="29" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B29" t="s">
         <v>64</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="X29" s="13" t="s">
         <v>433</v>
@@ -14872,13 +14872,13 @@
     </row>
     <row r="30" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B30" t="s">
         <v>11</v>
       </c>
       <c r="T30" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="U30" t="s">
         <v>64</v>
@@ -14892,16 +14892,16 @@
     </row>
     <row r="31" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B31" t="s">
         <v>11</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="T31" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="U31" t="s">
         <v>64</v>
@@ -14915,13 +14915,13 @@
     </row>
     <row r="32" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B32" t="s">
         <v>11</v>
       </c>
       <c r="T32" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="U32" t="s">
         <v>64</v>
@@ -15020,7 +15020,7 @@
         <v>64</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -15073,7 +15073,7 @@
         <v>353</v>
       </c>
       <c r="F1" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="G1" t="s">
         <v>354</v>
@@ -15091,13 +15091,13 @@
         <v>357</v>
       </c>
       <c r="L1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="M1" t="s">
         <v>358</v>
       </c>
       <c r="N1" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="O1" t="s">
         <v>359</v>
@@ -15106,13 +15106,13 @@
         <v>360</v>
       </c>
       <c r="Q1" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="R1" t="s">
         <v>361</v>
       </c>
       <c r="S1" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="T1" t="s">
         <v>362</v>
@@ -15145,22 +15145,22 @@
         <v>416</v>
       </c>
       <c r="AD1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="AE1" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="AF1" t="s">
+        <v>532</v>
+      </c>
+      <c r="AG1" t="s">
         <v>533</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>534</v>
       </c>
       <c r="AH1" t="s">
         <v>432</v>
       </c>
       <c r="AI1" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fix table rendering to remove duplicates[FHIR-43432] ix Rendering in granular scope tables[FHIR-43770] Fix format error [FHIR-43773] Undo copy/paste error to US Simple Observation Profile description [FHIR-43954]
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E35E1EB7-5AC3-8949-BE83-4B098A4C2FED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB17C19-FD18-0040-8026-039079C51DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51200" yWindow="6200" windowWidth="51200" windowHeight="20620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2473,7 +2473,7 @@
 * Every DocumentReference must have a responsible Organization. The organization responsible for the DocumentReference **SHALL** be present either in `DocumentReference.custodian` or accessible in the Provenance resource targeting the DocumentReference using `Provenance.agent.who` or `Provenance.agent.onBehalfOf`.</t>
   </si>
   <si>
-    <t>7.0.0-ballot</t>
+    <t>7.0.0</t>
   </si>
 </sst>
 </file>
@@ -2752,9 +2752,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2792,7 +2792,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2898,7 +2898,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3040,7 +3040,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -13025,7 +13025,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Remove US Core from CapabilityStatement.instantiates [FHIR-44121](https://jira.hl7.org/browse/FHIR-44121) Include FHIR R6 Sex and Gender content in Patient Profile Introduction [FHIR-44123] Remove ASKU from value sets and use DAR concept instead [FHIR-44127] Add non-binary to gender identity value set [FHIR-44132]
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB17C19-FD18-0040-8026-039079C51DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BC218F-E44A-2049-80BC-F06E696E54F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="6200" windowWidth="51200" windowHeight="20620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="6200" windowWidth="51200" windowHeight="20620" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -13024,7 +13024,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
+    <sheetView zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -13203,8 +13203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B31AD37-8183-744F-9AC6-9E533D1B51F5}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13237,9 +13237,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="B2" s="16" t="b">
-        <v>1</v>
-      </c>
+      <c r="B2" s="16"/>
       <c r="C2" t="s">
         <v>512</v>
       </c>

</xml_diff>

<commit_message>
fix last updated guidance in guidance page and capabilitystatements
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF761E01-F60E-234C-8C31-3EAC11F47EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB9FE7B-0CA9-004C-9CAC-DDCC14FD6C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="65700" yWindow="500" windowWidth="36700" windowHeight="28300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="65700" yWindow="500" windowWidth="36700" windowHeight="28300" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="ops" sheetId="5" r:id="rId7"/>
     <sheet name="interactions" sheetId="6" r:id="rId8"/>
     <sheet name="rest_interactions" sheetId="11" r:id="rId9"/>
-    <sheet name="sps" sheetId="38" r:id="rId10"/>
+    <sheet name="sps" sheetId="41" r:id="rId10"/>
     <sheet name="sp_combos" sheetId="40" r:id="rId11"/>
   </sheets>
   <definedNames>
@@ -49,12 +49,12 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={7D29DF1C-FB2E-FC48-BE2F-66EF4287E6FA}</author>
-    <author>tc={5E644239-03A8-B241-B5D5-D5C1D8E34C85}</author>
-    <author>tc={EBD53F31-30F5-CE44-9305-CAA9594E3EDF}</author>
+    <author>tc={8CB123FC-5C46-8947-9C0D-DFCF10660619}</author>
+    <author>tc={B37DA331-C8FE-E947-AEA5-FE79EDB28DDF}</author>
+    <author>tc={3D476BDD-1A14-564F-955C-6F85F5A4037C}</author>
   </authors>
   <commentList>
-    <comment ref="L36" authorId="0" shapeId="0" xr:uid="{7D29DF1C-FB2E-FC48-BE2F-66EF4287E6FA}">
+    <comment ref="L36" authorId="0" shapeId="0" xr:uid="{8CB123FC-5C46-8947-9C0D-DFCF10660619}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -62,7 +62,7 @@
     where does this show up?</t>
       </text>
     </comment>
-    <comment ref="Z40" authorId="1" shapeId="0" xr:uid="{5E644239-03A8-B241-B5D5-D5C1D8E34C85}">
+    <comment ref="Z40" authorId="1" shapeId="0" xr:uid="{B37DA331-C8FE-E947-AEA5-FE79EDB28DDF}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -70,7 +70,7 @@
     do i need this?</t>
       </text>
     </comment>
-    <comment ref="AA40" authorId="2" shapeId="0" xr:uid="{EBD53F31-30F5-CE44-9305-CAA9594E3EDF}">
+    <comment ref="AA40" authorId="2" shapeId="0" xr:uid="{3D476BDD-1A14-564F-955C-6F85F5A4037C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -121,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2821" uniqueCount="739">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2821" uniqueCount="740">
   <si>
     <t>Element</t>
   </si>
@@ -2512,6 +2512,11 @@
 * When `DiagnosticReport.category` is "LAB" the encounter, Updates to Meta.lastUpdated **SHOULD** reflect:
     * New laboratory reports
      * Changes in the status of laboratory reports including events that trigger the same status (e.g., amended → amended).</t>
+  </si>
+  <si>
+    <t>A server **SHALL** document the types of changes that can be detected using this parameter.
+A client **SHALL** provide a value precise to the *second + time offset*.
+A server **SHALL** support a value precise to the *second + time offset*.</t>
   </si>
 </sst>
 </file>
@@ -3100,13 +3105,13 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="L36" dT="2021-11-06T02:36:52.48" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{7D29DF1C-FB2E-FC48-BE2F-66EF4287E6FA}">
+  <threadedComment ref="L36" dT="2021-11-06T02:36:52.48" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{8CB123FC-5C46-8947-9C0D-DFCF10660619}">
     <text>where does this show up?</text>
   </threadedComment>
-  <threadedComment ref="Z40" dT="2021-11-06T02:39:25.62" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{5E644239-03A8-B241-B5D5-D5C1D8E34C85}">
+  <threadedComment ref="Z40" dT="2021-11-06T02:39:25.62" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{B37DA331-C8FE-E947-AEA5-FE79EDB28DDF}">
     <text>do i need this?</text>
   </threadedComment>
-  <threadedComment ref="AA40" dT="2021-11-06T02:40:08.93" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{EBD53F31-30F5-CE44-9305-CAA9594E3EDF}">
+  <threadedComment ref="AA40" dT="2021-11-06T02:40:08.93" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{3D476BDD-1A14-564F-955C-6F85F5A4037C}">
     <text>do I need this?</text>
   </threadedComment>
 </ThreadedComments>
@@ -3221,21 +3226,21 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{592C5153-4F70-1D4C-823A-EC5145CB6EBE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6E4BFB6-BCF6-9B4E-99D0-56861089466F}">
   <dimension ref="A1:AB132"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="Z28" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Z48" sqref="Z48"/>
+      <selection pane="bottomRight" activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="21.5" customWidth="1"/>
     <col min="3" max="3" width="33.5" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.5" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
     <col min="6" max="6" width="37.83203125" customWidth="1"/>
     <col min="7" max="7" width="60" customWidth="1"/>
@@ -5525,7 +5530,7 @@
         <v>SearchParameter-us-core-condition-recorded-date.html</v>
       </c>
     </row>
-    <row r="44" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:28" ht="144" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -5542,7 +5547,7 @@
         <v>0</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>476</v>
+        <v>739</v>
       </c>
       <c r="G44" t="str">
         <f t="shared" si="0"/>
@@ -5957,7 +5962,7 @@
         <v>SearchParameter-us-core-diagnosticreport-date.html</v>
       </c>
     </row>
-    <row r="52" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:28" ht="144" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -5974,7 +5979,7 @@
         <v>0</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>476</v>
+        <v>739</v>
       </c>
       <c r="G52" t="str">
         <f t="shared" si="0"/>
@@ -6657,7 +6662,7 @@
         <v>SearchParameter-us-core-encounter-date.html</v>
       </c>
     </row>
-    <row r="65" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:28" ht="144" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -6674,7 +6679,7 @@
         <v>0</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>476</v>
+        <v>739</v>
       </c>
       <c r="G65" t="str">
         <f t="shared" si="0"/>
@@ -8267,7 +8272,7 @@
         <v>SearchParameter-us-core-observation-date.html</v>
       </c>
     </row>
-    <row r="95" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:28" ht="144" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>94</v>
       </c>
@@ -8284,7 +8289,7 @@
         <v>0</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>476</v>
+        <v>739</v>
       </c>
       <c r="G95" t="str">
         <f t="shared" si="6"/>
@@ -10320,7 +10325,7 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13393,8 +13398,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:K101" xr:uid="{331E0B16-168F-459B-8951-3DF614BF0371}"/>
-  <conditionalFormatting sqref="B102:B1048576 B1:B100">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="!">
+  <conditionalFormatting sqref="B1:B100 B102:B1048576">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14546,7 +14551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{352F3A6C-0DAD-1041-B50E-04478951E07A}">
   <dimension ref="A1:Y69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
QA updates and final lastupdated changes
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB9FE7B-0CA9-004C-9CAC-DDCC14FD6C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FEEA87F-6F83-3F4F-8D95-40E65E52E0EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="65700" yWindow="500" windowWidth="36700" windowHeight="28300" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="65700" yWindow="500" windowWidth="36700" windowHeight="28300" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="interactions" sheetId="6" r:id="rId8"/>
     <sheet name="rest_interactions" sheetId="11" r:id="rId9"/>
     <sheet name="sps" sheetId="41" r:id="rId10"/>
-    <sheet name="sp_combos" sheetId="40" r:id="rId11"/>
+    <sheet name="sp_combos" sheetId="42" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">sp_combos!$A$1:$K$101</definedName>
@@ -85,12 +85,12 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={C8BBFBFF-0747-CE42-91C6-ECA3F83A9C84}</author>
-    <author>tc={C15970E2-3257-3B43-A998-0E8DD4DF70EF}</author>
-    <author>tc={E17BCB79-CEE9-F54E-8457-5810F8FF6D2A}</author>
+    <author>tc={3DAACC62-5CC1-D449-86F5-43599C868B72}</author>
+    <author>tc={B39110A3-A06E-B24B-9981-6F91D625D438}</author>
+    <author>tc={EE5E6114-960A-FD4A-98D4-1B83CD8D3DF4}</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{C8BBFBFF-0747-CE42-91C6-ECA3F83A9C84}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{3DAACC62-5CC1-D449-86F5-43599C868B72}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -100,7 +100,7 @@
     make this a comma separate list of profiles</t>
       </text>
     </comment>
-    <comment ref="I1" authorId="1" shapeId="0" xr:uid="{C15970E2-3257-3B43-A998-0E8DD4DF70EF}">
+    <comment ref="I1" authorId="1" shapeId="0" xr:uid="{B39110A3-A06E-B24B-9981-6F91D625D438}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -108,7 +108,7 @@
     does this do anything if not delete row</t>
       </text>
     </comment>
-    <comment ref="I43" authorId="2" shapeId="0" xr:uid="{E17BCB79-CEE9-F54E-8457-5810F8FF6D2A}">
+    <comment ref="I42" authorId="2" shapeId="0" xr:uid="{EE5E6114-960A-FD4A-98D4-1B83CD8D3DF4}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -2328,6 +2328,174 @@
     <t>patient,category,_lastUpdated</t>
   </si>
   <si>
+    <t>GET [base]/DiagnosticReport?patient=f201&amp;category=http://terminology.hl7.org/CodeSystem/v2-0074\|LAB&amp;_lastUpdated=ge2010-01-14T00:00:00Z</t>
+  </si>
+  <si>
+    <t>GET [base]/Observation?patient=1134281&amp;category={% if include.system %}{{include.system }}\|{% endif %}{{include.category | default: '[category]'}}&amp;status=final</t>
+  </si>
+  <si>
+    <t>GET [base]/Observation?patient=1134281&amp;amp;category={% if include.system %}{{include.system }}\|{% endif %}{{include.category | default: &amp;#39;[category]&amp;#39;}}</t>
+  </si>
+  <si>
+    <t>GET [base]/Observation?patient=1134281&amp;amp;code=http://loinc.org\|{{include.code1 | default: '[code]'}}
+      {% if include.code2 %}2. GET [base]/Observation?patient=1134281&amp;amp;code=http://loinc.org\|{{include.code1 | default: '[code]'}},http://loinc.org\|{{include.code2 | default: '[code]'}},http://loinc.org\|{{include.code3 | default: '[code]'}}{% endif %}</t>
+  </si>
+  <si>
+    <t>GET [base]Observation?patient=555580&amp;category={% if include.system %}{{include.system }}\|{% endif %}{{include.category | default: '[category]'}}&amp;date=ge2018-03-14T00:00:00Z</t>
+  </si>
+  <si>
+    <t>GET [base]Observation?patient=555580&amp;{% if include.system %}{{include.system }}\|{% endif %}{{include.category | default: '[category]'}}&amp;_lastUpdated=ge2024-01-01T00:00:00Z</t>
+  </si>
+  <si>
+    <t>GET [base]Observation?patient=555580&amp;code=http://loinc.org\|{{include.code1 | default: '[code]'}}&amp;date=ge2019-01-01T00:00:00Z</t>
+  </si>
+  <si>
+    <t>* The `DocumentReference.type` binding **SHALL** support at a minimum the [5 Common Clinical Notes](ValueSet-us-core-clinical-note-type.html) and may extend to the full US Core DocumentReference Type Value Set
+* The DocumentReference resources can represent the referenced content using either an address where the document can be retrieved using `DocumentReference.attachment.url` or the content as inline base64 encoded data using `DocumentReference.attachment.data`.
+    *  Although both are marked as must support, the server system is not required to support an address, and inline base64 encoded data, but **SHALL** support at least one of these elements.
+    *  The client application **SHALL** support both elements.
+    *  The `content.url` may refer to a FHIR Binary Resource (i.e. [base]/Binary/[id]), FHIR Document Bundle (i.e [base]/Bundle/[id] or another endpoint.
+        * If the endpoint is outside the FHIR base URL, it **SHOULD NOT** require additional authorization to access.
+   * If there are multiple `DocumentReference.content` element repetitions, these **SHALL** all represent the same document in different format or attachment metadata. The content element **SHALL NOT** contain different versions of the same content. For version handling use multiple DocumentReferences with `DocumentReference.relatesTo`
+* Every DocumentReference must have a responsible Organization. The organization responsible for the DocumentReference **SHALL** be present either in `DocumentReference.custodian` or accessible in the Provenance resource targeting the DocumentReference using `Provenance.agent.who` or `Provenance.agent.onBehalfOf`.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* The Encounter resource can represent a reason using either a code with `Encounter.reasonCode`, or a reference with `Encounter.reasonReference` to  Condition or other resource.
+   * Although both are marked as must support, the server systems are not required to support both a code and a reference, but they **SHALL** support *at least one* of these elements.
+   * The client application **SHALL** support both elements.
+   * if `Encounter.reasonReference` references an Observation, it **SHOULD** conform to a US Core Observation if applicable. (for example, a laboratory result should conform to the US Core Laboratory Result Observation Profile)
+* The location address can be represented by either by the Location referenced by `Encounter.location.location` or indirectly through the Organization referenced by `Encounter.serviceProvider`.
+   * Although both are marked as must support, the server systems are not required to support both `Encounter.location.location` and `Encounter.serviceProvider`, but they **SHALL** support *at least one* of these elements.
+   * The client application **SHALL** support both elements.
+* If the event facility/location differs from the `Encounter.location`, systems **SHOULD** reference it directly:
+</t>
+  </si>
+  <si>
+    <t>* Systems **SHOULD** follow the Project US@ Technical Specification for Patient Addresses Final Version 1.0 as the standard style guide for `Location.address.line` and  `Location.address.city`.</t>
+  </si>
+  <si>
+    <t>* Systems **SHALL** support National Provider Identifier (NPI) for organizations and **SHOULD** support Clinical Laboratory Improvement Amendments (CLIA) identifiers for `Organization.Identifier`.
+* Systems **SHOULD** follow the Project US@ Technical Specification for Patient Addresses Final Version 1.0 as the standard style guide for `Organization.address.line` and  `Organization.address.city`.</t>
+  </si>
+  <si>
+    <t>* For ONC's USCDI requirements, each Patient must support the following additional elements. These elements are included in the formal definition of the profile. The patient examples include all of these elements.
+  1. contact detail (e.g. a telephone number or an email address)
+  1. a communication language
+  1. a race
+  1. an ethnicity
+  1. a birth sex*
+  1. previous name
+     - Previous name is represented by providing an end date in the `Patient.name.period` element for a previous name.
+  1. suffix
+     - Suffix is represented using the `Patient.name.suffix` element.
+* The Patient's Social Security Numbers **SHOULD NOT** be used as a patient identifier in `Patient.identifier.value`.
+* Although Patient.deceased[x] is marked as 𝗔𝗗𝗗𝗜𝗧𝗜𝗢𝗡𝗔𝗟 𝗨𝗦𝗖𝗗𝗜, certifying systems are not required to support both choices, but **SHALL** support at least `Patient.deceasedDateTime`.
+* Certifying systems **SHALL** and non-certifying systems **SHOULD** follow the Project US@ Technical Specification for Patient Addresses Final Version 1.0 as the standard style guide for `Patient.address.line` and  `Patient.address.city` for new and updated records.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Servers that support only US Core Practitioner Profile **SHALL** provide implementation specific guidance how to access a provider’s location and contact information using only the Practitioner resource.
+   * Although Practitioner.address is marked as Must Support, the server system is not required to support it if they support the US Core PractitionerRole Profile, but **SHALL** support it if they do not support the US Core PractitionerRole Profile. The client application **SHALL** support both.
+* Systems **SHOULD** follow the Project US@ Technical Specification for Patient Addresses Final Version 1.0 as the standard style guide for `Practitioner.address.line` and  `Practitioner.address.city`.
+</t>
+  </si>
+  <si>
+    <t>* Procedure codes can be taken from SNOMED-CT, CPT, HCPCS II, ICD-10-PCS, CDT. LOINC.
+  * Only LOINC concepts that reflect actual procedures **SHOULD** be used
+* A procedure including an implantable device **SHOULD** use `Procedure.focalDevice` with a reference to the *US Core Implantable Device Profile*.
+* Servers and Clients **SHALL** support both US Core ServiceRequest and US Core Procedure Profiles for communicating the reason or justification for a referral as Additional USCDI Requirements. Typically, the reason or justification for a referral or consultation is communicated through `Procedure.basedOn` linking the Procedure to the US Core ServiceRequest Profile that includes either `ServiceRequest.reasonCode` or `ServiceRequest.reasonReference`. When the Procedure does not have an associated ServiceRequest, it is communicated through the US Core Procedure Profile's `Procedure.reasonCode` or `Procedure.reasonReference`.  Depending on the procedure being documented, a server will select the appropriate Profile to use.
+   * Although both `Procedure.reasonCode` and `Procedure.reasonReference` are marked as Additional USCDI Requirements. The certifying server system is not required to support both but **SHALL** support at least one of these elements. The certifying client application **SHALL** support both elements.
+      * when using  `Procedure.reasonReference`:
+         * Servers **SHALL** support *at least one* target resource in `Procedure.reasonReference`. Clients **SHALL** support all target resources .
+         * The referenced resources **SHOULD** be a US Core Profile.</t>
+  </si>
+  <si>
+    <t>* Systems **SHOULD** follow the Project US@ Technical Specification for Patient Addresses Final Version 1.0 as the standard style guide for `RelatedPerson.address.line` and  `RelatedPerson.address.city`.</t>
+  </si>
+  <si>
+    <t>* Servers and Clients **SHALL** support both US Core ServiceRequest and US Core Procedure Profiles for communicating the reason or justification for a referral as Additional USCDI Requirements. Typically, the reason or justification for a referral or consultation is communicated through `Procedure.basedOn` linking the Procedure to the US Core ServiceRequest Profile that includes either `ServiceRequest.reasonCode` or `ServiceRequest.reasonReference`. When the Procedure does not have an associated ServiceRequest, it is communicated through the US Core Procedure Profile's `Procedure.reasonCode` or `Procedure.reasonReference`.  Depending on the procedure being documented, a server will select the appropriate Profile to use.
+   * `ServiceRequest.reasonCode` and `ServiceRequest.reasonReference` are marked as Additional USCDI Requirements. The certifying server system is not required to support both but **SHALL** support at least one of these elements. The certifying client application **SHALL** support both elements.
+      * when using  `ServiceRequest.reasonReference`:
+         * Servers **SHALL** support *at least one* target resource in `ServiceRequest.reasonReference`. Clients **SHALL** support all target resources.
+         * The referenced resources **SHOULD** be a US Core Profile.</t>
+  </si>
+  <si>
+    <t>* Although both `Specimen.identifier` and `Specimen.accessionIdentifier` are marked as Must Support, the server system is not required to support both, but **SHALL** support at least one of these elements. The client application **SHALL** support both.</t>
+  </si>
+  <si>
+    <t>* In order to access care team member's names, identifiers, locations, and contact information, the CareTeam profile supports several types of care team participants. They are represented as references to other profiles and include the following four profiles which are marked as must support:
+  1. US Core Practitioner Profile
+  1. US Core PractitionerRole Profile
+  1. US Core Patient Profile
+  1. US Core RelatedPerson Profile
+* Although *both* US Core Practitioner Profile and US Core PractitionerRole are must support, the server system is not required to support both types of references, but **SHALL** support *at least* one of them.
+* The client application **SHALL** support all four profile references.
+* Bacause the *US Core PractitionerRole Profile* supplies the provider's location and contact information and a reference to the Practitioner, server systems **SHOULD** reference it instead of the *US Core Practitioner Profile*.
+* Servers that support only US Core Practitioner Profile and do not support the US Core PractitionerRole Profile **SHALL** provide implementation specific guidance how to access a provider’s location and contact information using only the Practitioner resource.</t>
+  </si>
+  <si>
+    <t>* The MedicationRequest resources can represent a medication using either a code or refer to the Medication resource. When referencing Medication, the resource may be [contained](http://hl7.org/fhir/R4/references.html#contained) or an external resource. The server application **MAY** choose any one way or more than one method, but if an external reference to Medication is used, the server **SHALL** support the _include` parameter for searching this element. The client application must support all methods.
+   * For example, A server **SHALL** be capable of returning all medications for a patient using one of or both:
+      *  `GET /MedicationRequest?patient=[id]`
+      *  `GET /MedicationRequest?patient=[id]&amp;_include=MedicationRequest:medication`
+* The MedicationRequest resource can represent that information is from a secondary source using either a boolean flag or reference in `MedicationRequest.reportedBoolean`, or a reference using `MedicationRequest.reportedReference` to Practitioner or other resource.
+   *   Although both are marked as must support, the server systems are not required to support both a boolean and a reference, but **SHALL** choose to support at least one of these elements.
+   *  The client application **SHALL** support both elements.
+* When recording “self-prescribed” medication, requester **SHOULD** be used to indicate the Patient or RelatedPerson as the prescriber. (See the Medication List section for guidance on accessing a patient medications including over the counter (OTC) medication and other substances taken for medical and recreational use.)
+* The MedicationRequest resource can communicate the reason or indication for treatment using either a code in MedicationRequest.reasonCode or a reference using MedicationRequest.reasonReference.
+* Although both `MedicationRequest.reasonCode` and `MedicationRequest.reasonReference` are marked as Additional USCDI Requirements. The certifying server system is not required to support both but **SHALL** support at least one of these elements. The certifying client application **SHALL** support both elements.
+   * when using MedicationRequest.reasonReference:
+       * Servers **SHALL** support at least one target resource in `MedicationRequest.reasonReference`. Clients **SHALL** support all target resources.
+      *  The referenced resources **SHOULD** be a US Core Profile as documented in Referencing US Core Profiles.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* The MedicationDispense resources can represent a medication using either a code or refer to the Medication resource. When referencing Medication, the resource may be [contained](http://hl7.org/fhir/R4/references.html#contained) or an external resource. The server application **MAY** choose any one way or more than one method, but if an external reference to Medication is used, the server **SHALL** support the _include` parameter for searching this element. The client application must support all methods.
+  * For example, A server **SHALL** be capable of returning dispense records for all medications for a patient using one of or both:
+     *  `GET /MedicationDispense?patient=[id]`
+     *  `GET /MedicationDispense?patient=[id]&amp;_include=MedicationDispense:medication`
+</t>
+  </si>
+  <si>
+    <t>* US Core defines two ways to represent the questions and responses to screening and assessment instruments:
+  - Observation: US Core Observation Screening Assessment Profile
+  - Questionnaire/QuestionnaireResponse: SDC Base Questionnaire/US Core QuestionnaireResponse Profile
+* US Core Servers **SHALL** support US Core Observation Screening Assessment Profile and **SHOULD** support the  SDC Base Questionnaire Profile/US Core QuestionnaireResponse Profile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Clients **SHALL** support at least one Observation Profile
+* Systems **SHOULD** support `Observation.effectivePeriod` to accurately represent tests that are collected over a period of time (for example, a 24-Hour Urine Collection test).
+* An Observation without a value, **SHALL** include a reason why the data is absent unless there are component observations, or references to other Observations that are grouped within it
+    * Systems that never provide an observation without a value are not required to support `Observation.dataAbsentReason`
+*  An `Observation.component` without a value, **SHALL** include a reason why the data is absent.
+    * Systems that never provide an component observation without a component value are not required to support `Observation.component.dataAbsentReason`.
+* When `Observation.category` is "laboratory" the encounter, Updates to Meta.lastUpdated **SHOULD** reflect:
+    * New laboratory results
+     * Changes in the status of laboratory results including events that trigger the same status (e.g., amended → amended).
+</t>
+  </si>
+  <si>
+    <t>* Clients **SHALL** support at least one Condition Profile
+* For Encounter Diagnosis use the *US Core Condition Encounter Diagnosis Profile*.
+    * When `Condition.category` is "encounter-diagnosis" the encounter, **SHOULD** be referenced in `Condition.encounter`.
+* For Problems and Health Concerns use the *US Core Condition Problems and Health Concerns Profile*.
+    * When `Condition.category` is a "problems-list-item", the `Condition.clinicalStatus **SHOULD NOT** be unknown.
+* There is no single element in Condition that represents the date of diagnosis. It may be the assertedDate Extension, `Condition.onsetDateTime`, or `Condition.recordedDate`.
+    * Although all three are marked as must support, the server is not required to support all.
+	* A server **SHALL** support `Condition.recordedDate`.
+    * A server **SHALL** support at least one of the assertedDate Extension and `Condition.onsetDateTime`. A server may support both, which means they support all three elements.
+    * The client application **SHALL** support all three elements.</t>
+  </si>
+  <si>
+    <t>* Clients **SHALL** support at least one DiagnosticReport Profile
+* When `DiagnosticReport.category` is "LAB" the encounter, Updates to Meta.lastUpdated **SHOULD** reflect:
+    * New laboratory reports
+     * Changes in the status of laboratory reports including events that trigger the same status (e.g., amended → amended).</t>
+  </si>
+  <si>
+    <t>A server **SHALL** document the types of changes that can be detected using this parameter.
+A client **SHALL** provide a value precise to the *second + time offset*.
+A server **SHALL** support a value precise to the *second + time offset*.</t>
+  </si>
+  <si>
     <r>
       <t>GET [</t>
     </r>
@@ -2347,176 +2515,8 @@
         <rFont val="Menlo"/>
         <family val="2"/>
       </rPr>
-      <t>]/Condition?patient=1032702&amp;category=http://terminology.hl7.org/CodeSystem/condition-category\|problem-list-item&amp;_lastUpdated=ge2024-01-01T00:00:00Z</t>
+      <t>]/Condition?patient=1032702&amp;_lastUpdated=ge2024-01-01T00:00:00Z</t>
     </r>
-  </si>
-  <si>
-    <t>GET [base]/DiagnosticReport?patient=f201&amp;category=http://terminology.hl7.org/CodeSystem/v2-0074\|LAB&amp;_lastUpdated=ge2010-01-14T00:00:00Z</t>
-  </si>
-  <si>
-    <t>GET [base]/Observation?patient=1134281&amp;category={% if include.system %}{{include.system }}\|{% endif %}{{include.category | default: '[category]'}}&amp;status=final</t>
-  </si>
-  <si>
-    <t>GET [base]/Observation?patient=1134281&amp;amp;category={% if include.system %}{{include.system }}\|{% endif %}{{include.category | default: &amp;#39;[category]&amp;#39;}}</t>
-  </si>
-  <si>
-    <t>GET [base]/Observation?patient=1134281&amp;amp;code=http://loinc.org\|{{include.code1 | default: '[code]'}}
-      {% if include.code2 %}2. GET [base]/Observation?patient=1134281&amp;amp;code=http://loinc.org\|{{include.code1 | default: '[code]'}},http://loinc.org\|{{include.code2 | default: '[code]'}},http://loinc.org\|{{include.code3 | default: '[code]'}}{% endif %}</t>
-  </si>
-  <si>
-    <t>GET [base]Observation?patient=555580&amp;category={% if include.system %}{{include.system }}\|{% endif %}{{include.category | default: '[category]'}}&amp;date=ge2018-03-14T00:00:00Z</t>
-  </si>
-  <si>
-    <t>GET [base]Observation?patient=555580&amp;{% if include.system %}{{include.system }}\|{% endif %}{{include.category | default: '[category]'}}&amp;_lastUpdated=ge2024-01-01T00:00:00Z</t>
-  </si>
-  <si>
-    <t>GET [base]Observation?patient=555580&amp;code=http://loinc.org\|{{include.code1 | default: '[code]'}}&amp;date=ge2019-01-01T00:00:00Z</t>
-  </si>
-  <si>
-    <t>* The `DocumentReference.type` binding **SHALL** support at a minimum the [5 Common Clinical Notes](ValueSet-us-core-clinical-note-type.html) and may extend to the full US Core DocumentReference Type Value Set
-* The DocumentReference resources can represent the referenced content using either an address where the document can be retrieved using `DocumentReference.attachment.url` or the content as inline base64 encoded data using `DocumentReference.attachment.data`.
-    *  Although both are marked as must support, the server system is not required to support an address, and inline base64 encoded data, but **SHALL** support at least one of these elements.
-    *  The client application **SHALL** support both elements.
-    *  The `content.url` may refer to a FHIR Binary Resource (i.e. [base]/Binary/[id]), FHIR Document Bundle (i.e [base]/Bundle/[id] or another endpoint.
-        * If the endpoint is outside the FHIR base URL, it **SHOULD NOT** require additional authorization to access.
-   * If there are multiple `DocumentReference.content` element repetitions, these **SHALL** all represent the same document in different format or attachment metadata. The content element **SHALL NOT** contain different versions of the same content. For version handling use multiple DocumentReferences with `DocumentReference.relatesTo`
-* Every DocumentReference must have a responsible Organization. The organization responsible for the DocumentReference **SHALL** be present either in `DocumentReference.custodian` or accessible in the Provenance resource targeting the DocumentReference using `Provenance.agent.who` or `Provenance.agent.onBehalfOf`.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* The Encounter resource can represent a reason using either a code with `Encounter.reasonCode`, or a reference with `Encounter.reasonReference` to  Condition or other resource.
-   * Although both are marked as must support, the server systems are not required to support both a code and a reference, but they **SHALL** support *at least one* of these elements.
-   * The client application **SHALL** support both elements.
-   * if `Encounter.reasonReference` references an Observation, it **SHOULD** conform to a US Core Observation if applicable. (for example, a laboratory result should conform to the US Core Laboratory Result Observation Profile)
-* The location address can be represented by either by the Location referenced by `Encounter.location.location` or indirectly through the Organization referenced by `Encounter.serviceProvider`.
-   * Although both are marked as must support, the server systems are not required to support both `Encounter.location.location` and `Encounter.serviceProvider`, but they **SHALL** support *at least one* of these elements.
-   * The client application **SHALL** support both elements.
-* If the event facility/location differs from the `Encounter.location`, systems **SHOULD** reference it directly:
-</t>
-  </si>
-  <si>
-    <t>* Systems **SHOULD** follow the Project US@ Technical Specification for Patient Addresses Final Version 1.0 as the standard style guide for `Location.address.line` and  `Location.address.city`.</t>
-  </si>
-  <si>
-    <t>* Systems **SHALL** support National Provider Identifier (NPI) for organizations and **SHOULD** support Clinical Laboratory Improvement Amendments (CLIA) identifiers for `Organization.Identifier`.
-* Systems **SHOULD** follow the Project US@ Technical Specification for Patient Addresses Final Version 1.0 as the standard style guide for `Organization.address.line` and  `Organization.address.city`.</t>
-  </si>
-  <si>
-    <t>* For ONC's USCDI requirements, each Patient must support the following additional elements. These elements are included in the formal definition of the profile. The patient examples include all of these elements.
-  1. contact detail (e.g. a telephone number or an email address)
-  1. a communication language
-  1. a race
-  1. an ethnicity
-  1. a birth sex*
-  1. previous name
-     - Previous name is represented by providing an end date in the `Patient.name.period` element for a previous name.
-  1. suffix
-     - Suffix is represented using the `Patient.name.suffix` element.
-* The Patient's Social Security Numbers **SHOULD NOT** be used as a patient identifier in `Patient.identifier.value`.
-* Although Patient.deceased[x] is marked as 𝗔𝗗𝗗𝗜𝗧𝗜𝗢𝗡𝗔𝗟 𝗨𝗦𝗖𝗗𝗜, certifying systems are not required to support both choices, but **SHALL** support at least `Patient.deceasedDateTime`.
-* Certifying systems **SHALL** and non-certifying systems **SHOULD** follow the Project US@ Technical Specification for Patient Addresses Final Version 1.0 as the standard style guide for `Patient.address.line` and  `Patient.address.city` for new and updated records.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Servers that support only US Core Practitioner Profile **SHALL** provide implementation specific guidance how to access a provider’s location and contact information using only the Practitioner resource.
-   * Although Practitioner.address is marked as Must Support, the server system is not required to support it if they support the US Core PractitionerRole Profile, but **SHALL** support it if they do not support the US Core PractitionerRole Profile. The client application **SHALL** support both.
-* Systems **SHOULD** follow the Project US@ Technical Specification for Patient Addresses Final Version 1.0 as the standard style guide for `Practitioner.address.line` and  `Practitioner.address.city`.
-</t>
-  </si>
-  <si>
-    <t>* Procedure codes can be taken from SNOMED-CT, CPT, HCPCS II, ICD-10-PCS, CDT. LOINC.
-  * Only LOINC concepts that reflect actual procedures **SHOULD** be used
-* A procedure including an implantable device **SHOULD** use `Procedure.focalDevice` with a reference to the *US Core Implantable Device Profile*.
-* Servers and Clients **SHALL** support both US Core ServiceRequest and US Core Procedure Profiles for communicating the reason or justification for a referral as Additional USCDI Requirements. Typically, the reason or justification for a referral or consultation is communicated through `Procedure.basedOn` linking the Procedure to the US Core ServiceRequest Profile that includes either `ServiceRequest.reasonCode` or `ServiceRequest.reasonReference`. When the Procedure does not have an associated ServiceRequest, it is communicated through the US Core Procedure Profile's `Procedure.reasonCode` or `Procedure.reasonReference`.  Depending on the procedure being documented, a server will select the appropriate Profile to use.
-   * Although both `Procedure.reasonCode` and `Procedure.reasonReference` are marked as Additional USCDI Requirements. The certifying server system is not required to support both but **SHALL** support at least one of these elements. The certifying client application **SHALL** support both elements.
-      * when using  `Procedure.reasonReference`:
-         * Servers **SHALL** support *at least one* target resource in `Procedure.reasonReference`. Clients **SHALL** support all target resources .
-         * The referenced resources **SHOULD** be a US Core Profile.</t>
-  </si>
-  <si>
-    <t>* Systems **SHOULD** follow the Project US@ Technical Specification for Patient Addresses Final Version 1.0 as the standard style guide for `RelatedPerson.address.line` and  `RelatedPerson.address.city`.</t>
-  </si>
-  <si>
-    <t>* Servers and Clients **SHALL** support both US Core ServiceRequest and US Core Procedure Profiles for communicating the reason or justification for a referral as Additional USCDI Requirements. Typically, the reason or justification for a referral or consultation is communicated through `Procedure.basedOn` linking the Procedure to the US Core ServiceRequest Profile that includes either `ServiceRequest.reasonCode` or `ServiceRequest.reasonReference`. When the Procedure does not have an associated ServiceRequest, it is communicated through the US Core Procedure Profile's `Procedure.reasonCode` or `Procedure.reasonReference`.  Depending on the procedure being documented, a server will select the appropriate Profile to use.
-   * `ServiceRequest.reasonCode` and `ServiceRequest.reasonReference` are marked as Additional USCDI Requirements. The certifying server system is not required to support both but **SHALL** support at least one of these elements. The certifying client application **SHALL** support both elements.
-      * when using  `ServiceRequest.reasonReference`:
-         * Servers **SHALL** support *at least one* target resource in `ServiceRequest.reasonReference`. Clients **SHALL** support all target resources.
-         * The referenced resources **SHOULD** be a US Core Profile.</t>
-  </si>
-  <si>
-    <t>* Although both `Specimen.identifier` and `Specimen.accessionIdentifier` are marked as Must Support, the server system is not required to support both, but **SHALL** support at least one of these elements. The client application **SHALL** support both.</t>
-  </si>
-  <si>
-    <t>* In order to access care team member's names, identifiers, locations, and contact information, the CareTeam profile supports several types of care team participants. They are represented as references to other profiles and include the following four profiles which are marked as must support:
-  1. US Core Practitioner Profile
-  1. US Core PractitionerRole Profile
-  1. US Core Patient Profile
-  1. US Core RelatedPerson Profile
-* Although *both* US Core Practitioner Profile and US Core PractitionerRole are must support, the server system is not required to support both types of references, but **SHALL** support *at least* one of them.
-* The client application **SHALL** support all four profile references.
-* Bacause the *US Core PractitionerRole Profile* supplies the provider's location and contact information and a reference to the Practitioner, server systems **SHOULD** reference it instead of the *US Core Practitioner Profile*.
-* Servers that support only US Core Practitioner Profile and do not support the US Core PractitionerRole Profile **SHALL** provide implementation specific guidance how to access a provider’s location and contact information using only the Practitioner resource.</t>
-  </si>
-  <si>
-    <t>* The MedicationRequest resources can represent a medication using either a code or refer to the Medication resource. When referencing Medication, the resource may be [contained](http://hl7.org/fhir/R4/references.html#contained) or an external resource. The server application **MAY** choose any one way or more than one method, but if an external reference to Medication is used, the server **SHALL** support the _include` parameter for searching this element. The client application must support all methods.
-   * For example, A server **SHALL** be capable of returning all medications for a patient using one of or both:
-      *  `GET /MedicationRequest?patient=[id]`
-      *  `GET /MedicationRequest?patient=[id]&amp;_include=MedicationRequest:medication`
-* The MedicationRequest resource can represent that information is from a secondary source using either a boolean flag or reference in `MedicationRequest.reportedBoolean`, or a reference using `MedicationRequest.reportedReference` to Practitioner or other resource.
-   *   Although both are marked as must support, the server systems are not required to support both a boolean and a reference, but **SHALL** choose to support at least one of these elements.
-   *  The client application **SHALL** support both elements.
-* When recording “self-prescribed” medication, requester **SHOULD** be used to indicate the Patient or RelatedPerson as the prescriber. (See the Medication List section for guidance on accessing a patient medications including over the counter (OTC) medication and other substances taken for medical and recreational use.)
-* The MedicationRequest resource can communicate the reason or indication for treatment using either a code in MedicationRequest.reasonCode or a reference using MedicationRequest.reasonReference.
-* Although both `MedicationRequest.reasonCode` and `MedicationRequest.reasonReference` are marked as Additional USCDI Requirements. The certifying server system is not required to support both but **SHALL** support at least one of these elements. The certifying client application **SHALL** support both elements.
-   * when using MedicationRequest.reasonReference:
-       * Servers **SHALL** support at least one target resource in `MedicationRequest.reasonReference`. Clients **SHALL** support all target resources.
-      *  The referenced resources **SHOULD** be a US Core Profile as documented in Referencing US Core Profiles.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* The MedicationDispense resources can represent a medication using either a code or refer to the Medication resource. When referencing Medication, the resource may be [contained](http://hl7.org/fhir/R4/references.html#contained) or an external resource. The server application **MAY** choose any one way or more than one method, but if an external reference to Medication is used, the server **SHALL** support the _include` parameter for searching this element. The client application must support all methods.
-  * For example, A server **SHALL** be capable of returning dispense records for all medications for a patient using one of or both:
-     *  `GET /MedicationDispense?patient=[id]`
-     *  `GET /MedicationDispense?patient=[id]&amp;_include=MedicationDispense:medication`
-</t>
-  </si>
-  <si>
-    <t>* US Core defines two ways to represent the questions and responses to screening and assessment instruments:
-  - Observation: US Core Observation Screening Assessment Profile
-  - Questionnaire/QuestionnaireResponse: SDC Base Questionnaire/US Core QuestionnaireResponse Profile
-* US Core Servers **SHALL** support US Core Observation Screening Assessment Profile and **SHOULD** support the  SDC Base Questionnaire Profile/US Core QuestionnaireResponse Profile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Clients **SHALL** support at least one Observation Profile
-* Systems **SHOULD** support `Observation.effectivePeriod` to accurately represent tests that are collected over a period of time (for example, a 24-Hour Urine Collection test).
-* An Observation without a value, **SHALL** include a reason why the data is absent unless there are component observations, or references to other Observations that are grouped within it
-    * Systems that never provide an observation without a value are not required to support `Observation.dataAbsentReason`
-*  An `Observation.component` without a value, **SHALL** include a reason why the data is absent.
-    * Systems that never provide an component observation without a component value are not required to support `Observation.component.dataAbsentReason`.
-* When `Observation.category` is "laboratory" the encounter, Updates to Meta.lastUpdated **SHOULD** reflect:
-    * New laboratory results
-     * Changes in the status of laboratory results including events that trigger the same status (e.g., amended → amended).
-</t>
-  </si>
-  <si>
-    <t>* Clients **SHALL** support at least one Condition Profile
-* For Encounter Diagnosis use the *US Core Condition Encounter Diagnosis Profile*.
-    * When `Condition.category` is "encounter-diagnosis" the encounter, **SHOULD** be referenced in `Condition.encounter`.
-* For Problems and Health Concerns use the *US Core Condition Problems and Health Concerns Profile*.
-    * When `Condition.category` is a "problems-list-item", the `Condition.clinicalStatus **SHOULD NOT** be unknown.
-* There is no single element in Condition that represents the date of diagnosis. It may be the assertedDate Extension, `Condition.onsetDateTime`, or `Condition.recordedDate`.
-    * Although all three are marked as must support, the server is not required to support all.
-	* A server **SHALL** support `Condition.recordedDate`.
-    * A server **SHALL** support at least one of the assertedDate Extension and `Condition.onsetDateTime`. A server may support both, which means they support all three elements.
-    * The client application **SHALL** support all three elements.</t>
-  </si>
-  <si>
-    <t>* Clients **SHALL** support at least one DiagnosticReport Profile
-* When `DiagnosticReport.category` is "LAB" the encounter, Updates to Meta.lastUpdated **SHOULD** reflect:
-    * New laboratory reports
-     * Changes in the status of laboratory reports including events that trigger the same status (e.g., amended → amended).</t>
-  </si>
-  <si>
-    <t>A server **SHALL** document the types of changes that can be detected using this parameter.
-A client **SHALL** provide a value precise to the *second + time offset*.
-A server **SHALL** support a value precise to the *second + time offset*.</t>
   </si>
 </sst>
 </file>
@@ -3119,16 +3119,16 @@
 
 <file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="C1" dT="2021-11-10T17:47:31.83" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{C8BBFBFF-0747-CE42-91C6-ECA3F83A9C84}">
+  <threadedComment ref="C1" dT="2021-11-10T17:47:31.83" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{3DAACC62-5CC1-D449-86F5-43599C868B72}">
     <text>add column for include file</text>
   </threadedComment>
-  <threadedComment ref="C1" dT="2021-11-10T17:48:52.85" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{2DCEE40D-F75B-B843-936D-793E8B6393A9}" parentId="{C8BBFBFF-0747-CE42-91C6-ECA3F83A9C84}">
+  <threadedComment ref="C1" dT="2021-11-10T17:48:52.85" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{BE96FDCF-3E98-7B43-9F9F-E7BCAC6DA2A1}" parentId="{3DAACC62-5CC1-D449-86F5-43599C868B72}">
     <text>make this a comma separate list of profiles</text>
   </threadedComment>
-  <threadedComment ref="I1" dT="2021-11-08T19:54:50.37" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{C15970E2-3257-3B43-A998-0E8DD4DF70EF}">
+  <threadedComment ref="I1" dT="2021-11-08T19:54:50.37" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{B39110A3-A06E-B24B-9981-6F91D625D438}">
     <text>does this do anything if not delete row</text>
   </threadedComment>
-  <threadedComment ref="I43" dT="2021-11-06T02:44:23.26" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{E17BCB79-CEE9-F54E-8457-5810F8FF6D2A}">
+  <threadedComment ref="I42" dT="2021-11-06T02:44:23.26" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{EE5E6114-960A-FD4A-98D4-1B83CD8D3DF4}">
     <text>is column being used???</text>
   </threadedComment>
 </ThreadedComments>
@@ -3229,7 +3229,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6E4BFB6-BCF6-9B4E-99D0-56861089466F}">
   <dimension ref="A1:AB132"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -5547,7 +5547,7 @@
         <v>0</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="G44" t="str">
         <f t="shared" si="0"/>
@@ -5979,7 +5979,7 @@
         <v>0</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="G52" t="str">
         <f t="shared" si="0"/>
@@ -6679,7 +6679,7 @@
         <v>0</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="G65" t="str">
         <f t="shared" si="0"/>
@@ -8289,7 +8289,7 @@
         <v>0</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="G95" t="str">
         <f t="shared" si="6"/>
@@ -10176,7 +10176,7 @@
         <v>475</v>
       </c>
       <c r="G130" t="str">
-        <f t="shared" ref="G130:G160" si="9">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B130)</f>
+        <f t="shared" ref="G130:G132" si="9">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B130)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="H130" t="s">
@@ -10325,7 +10325,7 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10336,14 +10336,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A384A127-0B27-5647-AD97-BD21E1AA8E5D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAFF496C-66FE-FC40-BBAB-C828675ADA30}">
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="K8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A26" sqref="A26"/>
+      <selection pane="bottomRight" activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11484,9 +11484,9 @@
         <v>540</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B41" t="s">
         <v>131</v>
@@ -11496,29 +11496,27 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D41" t="s">
-        <v>713</v>
-      </c>
-      <c r="E41" t="s">
-        <v>51</v>
+        <v>140</v>
       </c>
       <c r="F41" t="s">
         <v>64</v>
       </c>
       <c r="G41" t="s">
-        <v>207</v>
-      </c>
-      <c r="I41" s="4"/>
-      <c r="J41" s="24" t="s">
-        <v>714</v>
-      </c>
-      <c r="K41" s="24" t="str">
-        <f>"Fetches a bundle of all "&amp;B41&amp;" resources for the specified "&amp;SUBSTITUTE(D41,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
-        <v>Fetches a bundle of all Condition resources for the specified patient and category and _lastUpdated. See the US Core General Guidance page for [Searching Using lastUpdated].</v>
+        <v>99</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="J41" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="K41" s="4" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B42" t="s">
         <v>131</v>
@@ -11528,27 +11526,27 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D42" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F42" t="s">
         <v>64</v>
       </c>
       <c r="G42" t="s">
-        <v>99</v>
+        <v>142</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>307</v>
+        <v>541</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B43" t="s">
         <v>131</v>
@@ -11558,7 +11556,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D43" t="s">
-        <v>141</v>
+        <v>542</v>
       </c>
       <c r="F43" t="s">
         <v>64</v>
@@ -11570,7 +11568,7 @@
         <v>146</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="K43" s="4" t="s">
         <v>149</v>
@@ -11578,7 +11576,7 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B44" t="s">
         <v>131</v>
@@ -11588,7 +11586,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D44" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="F44" t="s">
         <v>64</v>
@@ -11600,7 +11598,7 @@
         <v>146</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="K44" s="4" t="s">
         <v>149</v>
@@ -11608,7 +11606,7 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B45" t="s">
         <v>131</v>
@@ -11618,7 +11616,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D45" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="F45" t="s">
         <v>64</v>
@@ -11630,25 +11628,28 @@
         <v>146</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="K45" s="4" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B46" t="s">
         <v>131</v>
       </c>
       <c r="C46" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B46)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D46" t="s">
-        <v>546</v>
+        <v>711</v>
+      </c>
+      <c r="E46" t="s">
+        <v>51</v>
       </c>
       <c r="F46" t="s">
         <v>64</v>
@@ -11656,14 +11657,13 @@
       <c r="G46" t="s">
         <v>142</v>
       </c>
-      <c r="I46" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="J46" s="4" t="s">
-        <v>547</v>
-      </c>
-      <c r="K46" s="4" t="s">
-        <v>149</v>
+      <c r="I46" s="4"/>
+      <c r="J46" s="24" t="s">
+        <v>739</v>
+      </c>
+      <c r="K46" s="24" t="str">
+        <f>"Fetches a bundle of all "&amp;B46&amp;" resources for the specified "&amp;SUBSTITUTE(D46,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
+        <v>Fetches a bundle of all Condition resources for the specified patient and _lastUpdated. See the US Core General Guidance page for [Searching Using lastUpdated].</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
@@ -11909,7 +11909,7 @@
       </c>
       <c r="I54" s="4"/>
       <c r="J54" s="27" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="K54" s="24" t="str">
         <f>"Fetches a bundle of all "&amp;B54&amp;" resources for the specified "&amp;SUBSTITUTE(D54,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
@@ -12320,7 +12320,7 @@
         <v>264</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="K67" s="4" t="s">
         <v>299</v>
@@ -12352,7 +12352,7 @@
         <v>209</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="K68" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B68&amp;" resources for the specified patient and a category code = `laboratory`"</f>
@@ -12382,7 +12382,7 @@
         <v>212</v>
       </c>
       <c r="J69" s="8" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="K69" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B69&amp;" resources for the specified patient and observation code(s).  SHOULD support search by multiple report codes. The Observation `code` parameter searches `Observation.code only."</f>
@@ -12415,7 +12415,7 @@
         <v>213</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="K70" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B70&amp;" resources for the specified patient and date and a category code = `laboratory`"</f>
@@ -12446,7 +12446,7 @@
       </c>
       <c r="I71" s="4"/>
       <c r="J71" s="27" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="K71" s="24" t="str">
         <f>"Fetches a bundle of all "&amp;B71&amp;" resources for the specified "&amp;SUBSTITUTE(D71,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
@@ -12476,7 +12476,7 @@
         <v>211</v>
       </c>
       <c r="J72" s="4" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="K72" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B72&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
@@ -13398,13 +13398,13 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:K101" xr:uid="{331E0B16-168F-459B-8951-3DF614BF0371}"/>
-  <conditionalFormatting sqref="B1:B100 B102:B1048576">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="!">
+  <conditionalFormatting sqref="B102:B1048576 B1:B100">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C101" r:id="rId1" xr:uid="{8DFABA24-24DC-E548-86F0-F789DD265203}"/>
+    <hyperlink ref="C101" r:id="rId1" xr:uid="{1EAF46C7-3D36-1B4E-B601-050DE1E6B350}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
@@ -14702,7 +14702,7 @@
         <v>64</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="T4" t="s">
         <v>688</v>
@@ -14731,7 +14731,7 @@
         <v>64</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="T5" t="s">
         <v>688</v>
@@ -14797,7 +14797,7 @@
         <v>64</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="T8" t="s">
         <v>688</v>
@@ -14820,7 +14820,7 @@
         <v>64</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="T9" t="s">
         <v>688</v>
@@ -14843,7 +14843,7 @@
         <v>64</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="T10" t="s">
         <v>688</v>
@@ -14950,7 +14950,7 @@
         <v>64</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="T15" t="s">
         <v>688</v>
@@ -15007,7 +15007,7 @@
         <v>64</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="T18" t="s">
         <v>688</v>
@@ -15036,7 +15036,7 @@
         <v>64</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="T19" t="s">
         <v>688</v>
@@ -15094,7 +15094,7 @@
         <v>64</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="T21" t="s">
         <v>688</v>
@@ -15117,7 +15117,7 @@
         <v>64</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="T22" t="s">
         <v>688</v>
@@ -15136,7 +15136,7 @@
         <v>64</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="T23" t="s">
         <v>688</v>
@@ -15159,7 +15159,7 @@
         <v>64</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="T24" t="s">
         <v>688</v>
@@ -15203,7 +15203,7 @@
         <v>64</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="T26" t="s">
         <v>688</v>
@@ -15243,7 +15243,7 @@
         <v>64</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="X28" s="13"/>
       <c r="Y28" s="13"/>
@@ -15256,7 +15256,7 @@
         <v>64</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="X29" s="13" t="s">
         <v>424</v>
@@ -15273,7 +15273,7 @@
         <v>64</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="T30" t="s">
         <v>688</v>
@@ -15296,7 +15296,7 @@
         <v>64</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="T31" t="s">
         <v>688</v>
@@ -15319,7 +15319,7 @@
         <v>64</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="T32" t="s">
         <v>688</v>

</xml_diff>

<commit_message>
final QA, updated Jira, added pucblication request file, removed change highlighting.
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FEEA87F-6F83-3F4F-8D95-40E65E52E0EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC449E9-20FB-414E-99C1-2B8F13F0D297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="65700" yWindow="500" windowWidth="36700" windowHeight="28300" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="65700" yWindow="500" windowWidth="36700" windowHeight="28300" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -22,8 +22,8 @@
     <sheet name="ops" sheetId="5" r:id="rId7"/>
     <sheet name="interactions" sheetId="6" r:id="rId8"/>
     <sheet name="rest_interactions" sheetId="11" r:id="rId9"/>
-    <sheet name="sps" sheetId="41" r:id="rId10"/>
-    <sheet name="sp_combos" sheetId="42" r:id="rId11"/>
+    <sheet name="sps" sheetId="43" r:id="rId10"/>
+    <sheet name="sp_combos" sheetId="44" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">sp_combos!$A$1:$K$101</definedName>
@@ -49,12 +49,12 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={8CB123FC-5C46-8947-9C0D-DFCF10660619}</author>
-    <author>tc={B37DA331-C8FE-E947-AEA5-FE79EDB28DDF}</author>
-    <author>tc={3D476BDD-1A14-564F-955C-6F85F5A4037C}</author>
+    <author>tc={64E811D6-A1D6-EE44-9BB3-6CF3612B7A7B}</author>
+    <author>tc={3016521A-9845-D24A-92EE-982F72D03861}</author>
+    <author>tc={6405F4A6-C332-7D4A-95AF-8C84ED333C1D}</author>
   </authors>
   <commentList>
-    <comment ref="L36" authorId="0" shapeId="0" xr:uid="{8CB123FC-5C46-8947-9C0D-DFCF10660619}">
+    <comment ref="L36" authorId="0" shapeId="0" xr:uid="{64E811D6-A1D6-EE44-9BB3-6CF3612B7A7B}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -62,7 +62,7 @@
     where does this show up?</t>
       </text>
     </comment>
-    <comment ref="Z40" authorId="1" shapeId="0" xr:uid="{B37DA331-C8FE-E947-AEA5-FE79EDB28DDF}">
+    <comment ref="Z40" authorId="1" shapeId="0" xr:uid="{3016521A-9845-D24A-92EE-982F72D03861}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -70,7 +70,7 @@
     do i need this?</t>
       </text>
     </comment>
-    <comment ref="AA40" authorId="2" shapeId="0" xr:uid="{3D476BDD-1A14-564F-955C-6F85F5A4037C}">
+    <comment ref="AA40" authorId="2" shapeId="0" xr:uid="{6405F4A6-C332-7D4A-95AF-8C84ED333C1D}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -85,12 +85,12 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={3DAACC62-5CC1-D449-86F5-43599C868B72}</author>
-    <author>tc={B39110A3-A06E-B24B-9981-6F91D625D438}</author>
-    <author>tc={EE5E6114-960A-FD4A-98D4-1B83CD8D3DF4}</author>
+    <author>tc={26E7129E-8BEC-7D43-ABDD-C22EB5B5D76E}</author>
+    <author>tc={88C72358-53B7-EC40-9A60-63ACA4CC2425}</author>
+    <author>tc={CDB5B6C6-2EF9-974D-BA8C-671D42D9A4E2}</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{3DAACC62-5CC1-D449-86F5-43599C868B72}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{26E7129E-8BEC-7D43-ABDD-C22EB5B5D76E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -100,7 +100,7 @@
     make this a comma separate list of profiles</t>
       </text>
     </comment>
-    <comment ref="I1" authorId="1" shapeId="0" xr:uid="{B39110A3-A06E-B24B-9981-6F91D625D438}">
+    <comment ref="I1" authorId="1" shapeId="0" xr:uid="{88C72358-53B7-EC40-9A60-63ACA4CC2425}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -108,7 +108,7 @@
     does this do anything if not delete row</t>
       </text>
     </comment>
-    <comment ref="I42" authorId="2" shapeId="0" xr:uid="{EE5E6114-960A-FD4A-98D4-1B83CD8D3DF4}">
+    <comment ref="I42" authorId="2" shapeId="0" xr:uid="{CDB5B6C6-2EF9-974D-BA8C-671D42D9A4E2}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -121,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2821" uniqueCount="740">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2813" uniqueCount="740">
   <si>
     <t>Element</t>
   </si>
@@ -3105,13 +3105,13 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="L36" dT="2021-11-06T02:36:52.48" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{8CB123FC-5C46-8947-9C0D-DFCF10660619}">
+  <threadedComment ref="L36" dT="2021-11-06T02:36:52.48" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{64E811D6-A1D6-EE44-9BB3-6CF3612B7A7B}">
     <text>where does this show up?</text>
   </threadedComment>
-  <threadedComment ref="Z40" dT="2021-11-06T02:39:25.62" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{B37DA331-C8FE-E947-AEA5-FE79EDB28DDF}">
+  <threadedComment ref="Z40" dT="2021-11-06T02:39:25.62" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{3016521A-9845-D24A-92EE-982F72D03861}">
     <text>do i need this?</text>
   </threadedComment>
-  <threadedComment ref="AA40" dT="2021-11-06T02:40:08.93" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{3D476BDD-1A14-564F-955C-6F85F5A4037C}">
+  <threadedComment ref="AA40" dT="2021-11-06T02:40:08.93" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{6405F4A6-C332-7D4A-95AF-8C84ED333C1D}">
     <text>do I need this?</text>
   </threadedComment>
 </ThreadedComments>
@@ -3119,16 +3119,16 @@
 
 <file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="C1" dT="2021-11-10T17:47:31.83" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{3DAACC62-5CC1-D449-86F5-43599C868B72}">
+  <threadedComment ref="C1" dT="2021-11-10T17:47:31.83" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{26E7129E-8BEC-7D43-ABDD-C22EB5B5D76E}">
     <text>add column for include file</text>
   </threadedComment>
-  <threadedComment ref="C1" dT="2021-11-10T17:48:52.85" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{BE96FDCF-3E98-7B43-9F9F-E7BCAC6DA2A1}" parentId="{3DAACC62-5CC1-D449-86F5-43599C868B72}">
+  <threadedComment ref="C1" dT="2021-11-10T17:48:52.85" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{C7673D4F-A0FB-804C-A6C1-2F2C3DD753BA}" parentId="{26E7129E-8BEC-7D43-ABDD-C22EB5B5D76E}">
     <text>make this a comma separate list of profiles</text>
   </threadedComment>
-  <threadedComment ref="I1" dT="2021-11-08T19:54:50.37" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{B39110A3-A06E-B24B-9981-6F91D625D438}">
+  <threadedComment ref="I1" dT="2021-11-08T19:54:50.37" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{88C72358-53B7-EC40-9A60-63ACA4CC2425}">
     <text>does this do anything if not delete row</text>
   </threadedComment>
-  <threadedComment ref="I42" dT="2021-11-06T02:44:23.26" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{EE5E6114-960A-FD4A-98D4-1B83CD8D3DF4}">
+  <threadedComment ref="I42" dT="2021-11-06T02:44:23.26" personId="{14A52E69-4757-9B48-BCB0-430F0B406E9E}" id="{CDB5B6C6-2EF9-974D-BA8C-671D42D9A4E2}">
     <text>is column being used???</text>
   </threadedComment>
 </ThreadedComments>
@@ -3226,14 +3226,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6E4BFB6-BCF6-9B4E-99D0-56861089466F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{427A2FB7-DA88-6B49-A242-D69B65B8CD67}">
   <dimension ref="A1:AB132"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B33" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G44" sqref="G44"/>
+      <selection pane="bottomRight" activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5556,9 +5556,6 @@
       <c r="H44" t="s">
         <v>51</v>
       </c>
-      <c r="I44" t="s">
-        <v>51</v>
-      </c>
       <c r="J44" t="s">
         <v>51</v>
       </c>
@@ -5988,9 +5985,6 @@
       <c r="H52" t="s">
         <v>51</v>
       </c>
-      <c r="I52" t="s">
-        <v>51</v>
-      </c>
       <c r="J52" t="s">
         <v>51</v>
       </c>
@@ -6686,9 +6680,6 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="H65" t="s">
-        <v>51</v>
-      </c>
-      <c r="I65" t="s">
         <v>51</v>
       </c>
       <c r="J65" t="s">
@@ -8298,9 +8289,6 @@
       <c r="H95" t="s">
         <v>51</v>
       </c>
-      <c r="I95" t="s">
-        <v>51</v>
-      </c>
       <c r="J95" t="s">
         <v>51</v>
       </c>
@@ -10176,7 +10164,7 @@
         <v>475</v>
       </c>
       <c r="G130" t="str">
-        <f t="shared" ref="G130:G132" si="9">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B130)</f>
+        <f t="shared" ref="G130:G160" si="9">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B130)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="H130" t="s">
@@ -10336,14 +10324,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAFF496C-66FE-FC40-BBAB-C828675ADA30}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D897541-DBC5-C24B-A9D0-741176A79580}">
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="K8" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K39" sqref="K39"/>
+      <selection pane="bottomRight" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10403,7 +10391,7 @@
         <v>150</v>
       </c>
       <c r="C2" t="str">
-        <f t="shared" ref="C2:C49" si="0">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B2)</f>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B2)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D2" t="s">
@@ -10416,7 +10404,7 @@
         <v>93</v>
       </c>
       <c r="K2" s="4" t="str">
-        <f t="shared" ref="K2:K36" si="1">"Fetches a bundle of all "&amp;B2&amp;" resources matching the specified "&amp;SUBSTITUTE(D2,","," and ")</f>
+        <f>"Fetches a bundle of all "&amp;B2&amp;" resources matching the specified "&amp;SUBSTITUTE(D2,","," and ")</f>
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date</v>
       </c>
     </row>
@@ -10428,7 +10416,7 @@
         <v>150</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B3)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D3" t="s">
@@ -10441,7 +10429,7 @@
         <v>95</v>
       </c>
       <c r="K3" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>"Fetches a bundle of all "&amp;B3&amp;" resources matching the specified "&amp;SUBSTITUTE(D3,","," and ")</f>
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and patient</v>
       </c>
     </row>
@@ -10453,7 +10441,7 @@
         <v>150</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B4)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D4" t="s">
@@ -10466,7 +10454,7 @@
         <v>95</v>
       </c>
       <c r="K4" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>"Fetches a bundle of all "&amp;B4&amp;" resources matching the specified "&amp;SUBSTITUTE(D4,","," and ")</f>
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and patient and type</v>
       </c>
     </row>
@@ -10478,7 +10466,7 @@
         <v>150</v>
       </c>
       <c r="C5" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B5)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D5" t="s">
@@ -10491,7 +10479,7 @@
         <v>93</v>
       </c>
       <c r="K5" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>"Fetches a bundle of all "&amp;B5&amp;" resources matching the specified "&amp;SUBSTITUTE(D5,","," and ")</f>
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and type</v>
       </c>
     </row>
@@ -10503,7 +10491,7 @@
         <v>20</v>
       </c>
       <c r="C6" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B6)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D6" t="s">
@@ -10522,7 +10510,7 @@
         <v>286</v>
       </c>
       <c r="K6" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>"Fetches a bundle of all "&amp;B6&amp;" resources matching the specified "&amp;SUBSTITUTE(D6,","," and ")</f>
         <v>Fetches a bundle of all Encounter resources matching the specified class and patient</v>
       </c>
     </row>
@@ -10534,7 +10522,7 @@
         <v>150</v>
       </c>
       <c r="C7" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B7)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D7" t="s">
@@ -10547,7 +10535,7 @@
         <v>99</v>
       </c>
       <c r="K7" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>"Fetches a bundle of all "&amp;B7&amp;" resources matching the specified "&amp;SUBSTITUTE(D7,","," and ")</f>
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and status</v>
       </c>
     </row>
@@ -10559,7 +10547,7 @@
         <v>150</v>
       </c>
       <c r="C8" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B8)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D8" t="s">
@@ -10572,7 +10560,7 @@
         <v>99</v>
       </c>
       <c r="K8" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>"Fetches a bundle of all "&amp;B8&amp;" resources matching the specified "&amp;SUBSTITUTE(D8,","," and ")</f>
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and status and type</v>
       </c>
     </row>
@@ -10584,7 +10572,7 @@
         <v>150</v>
       </c>
       <c r="C9" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B9)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D9" t="s">
@@ -10598,7 +10586,7 @@
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>"Fetches a bundle of all "&amp;B9&amp;" resources matching the specified "&amp;SUBSTITUTE(D9,","," and ")</f>
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and type</v>
       </c>
     </row>
@@ -10610,7 +10598,7 @@
         <v>150</v>
       </c>
       <c r="C10" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B10)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D10" t="s">
@@ -10625,7 +10613,7 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>"Fetches a bundle of all "&amp;B10&amp;" resources matching the specified "&amp;SUBSTITUTE(D10,","," and ")</f>
         <v>Fetches a bundle of all !Encounter resources matching the specified class and status</v>
       </c>
     </row>
@@ -10637,7 +10625,7 @@
         <v>150</v>
       </c>
       <c r="C11" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B11)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D11" t="s">
@@ -10651,7 +10639,7 @@
       </c>
       <c r="I11" s="4"/>
       <c r="K11" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>"Fetches a bundle of all "&amp;B11&amp;" resources matching the specified "&amp;SUBSTITUTE(D11,","," and ")</f>
         <v>Fetches a bundle of all !Encounter resources matching the specified class and status and type</v>
       </c>
     </row>
@@ -10663,7 +10651,7 @@
         <v>150</v>
       </c>
       <c r="C12" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B12)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D12" t="s">
@@ -10676,7 +10664,7 @@
         <v>52</v>
       </c>
       <c r="K12" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>"Fetches a bundle of all "&amp;B12&amp;" resources matching the specified "&amp;SUBSTITUTE(D12,","," and ")</f>
         <v>Fetches a bundle of all !Encounter resources matching the specified class and type</v>
       </c>
     </row>
@@ -10688,7 +10676,7 @@
         <v>20</v>
       </c>
       <c r="C13" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B13)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D13" t="s">
@@ -10707,7 +10695,7 @@
         <v>478</v>
       </c>
       <c r="K13" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>"Fetches a bundle of all "&amp;B13&amp;" resources matching the specified "&amp;SUBSTITUTE(D13,","," and ")</f>
         <v>Fetches a bundle of all Encounter resources matching the specified date and patient</v>
       </c>
     </row>
@@ -10719,7 +10707,7 @@
         <v>150</v>
       </c>
       <c r="C14" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B14)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D14" t="s">
@@ -10732,7 +10720,7 @@
         <v>95</v>
       </c>
       <c r="K14" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>"Fetches a bundle of all "&amp;B14&amp;" resources matching the specified "&amp;SUBSTITUTE(D14,","," and ")</f>
         <v>Fetches a bundle of all !Encounter resources matching the specified date and patient and type</v>
       </c>
     </row>
@@ -10744,7 +10732,7 @@
         <v>150</v>
       </c>
       <c r="C15" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B15)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D15" t="s">
@@ -10757,7 +10745,7 @@
         <v>93</v>
       </c>
       <c r="K15" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>"Fetches a bundle of all "&amp;B15&amp;" resources matching the specified "&amp;SUBSTITUTE(D15,","," and ")</f>
         <v>Fetches a bundle of all !Encounter resources matching the specified date and type</v>
       </c>
     </row>
@@ -10769,7 +10757,7 @@
         <v>20</v>
       </c>
       <c r="C16" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B16)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D16" t="s">
@@ -10788,7 +10776,7 @@
         <v>287</v>
       </c>
       <c r="K16" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>"Fetches a bundle of all "&amp;B16&amp;" resources matching the specified "&amp;SUBSTITUTE(D16,","," and ")</f>
         <v>Fetches a bundle of all Encounter resources matching the specified patient and type</v>
       </c>
     </row>
@@ -10800,7 +10788,7 @@
         <v>20</v>
       </c>
       <c r="C17" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B17)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D17" t="s">
@@ -10819,7 +10807,7 @@
         <v>536</v>
       </c>
       <c r="K17" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>"Fetches a bundle of all "&amp;B17&amp;" resources matching the specified "&amp;SUBSTITUTE(D17,","," and ")</f>
         <v>Fetches a bundle of all Encounter resources matching the specified patient and location</v>
       </c>
     </row>
@@ -10831,14 +10819,11 @@
         <v>20</v>
       </c>
       <c r="C18" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B18)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D18" t="s">
         <v>711</v>
-      </c>
-      <c r="E18" t="s">
-        <v>51</v>
       </c>
       <c r="F18" t="s">
         <v>64</v>
@@ -10863,7 +10848,7 @@
         <v>150</v>
       </c>
       <c r="C19" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B19)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D19" t="s">
@@ -10877,7 +10862,7 @@
       </c>
       <c r="J19" s="4"/>
       <c r="K19" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>"Fetches a bundle of all "&amp;B19&amp;" resources matching the specified "&amp;SUBSTITUTE(D19,","," and ")</f>
         <v>Fetches a bundle of all !Encounter resources matching the specified patient and status and type</v>
       </c>
     </row>
@@ -10889,7 +10874,7 @@
         <v>20</v>
       </c>
       <c r="C20" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B20)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D20" t="s">
@@ -10908,7 +10893,7 @@
         <v>288</v>
       </c>
       <c r="K20" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>"Fetches a bundle of all "&amp;B20&amp;" resources matching the specified "&amp;SUBSTITUTE(D20,","," and ")</f>
         <v>Fetches a bundle of all Encounter resources matching the specified patient and status</v>
       </c>
     </row>
@@ -10920,7 +10905,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B21)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D21" t="s">
@@ -10939,7 +10924,7 @@
         <v>538</v>
       </c>
       <c r="K21" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>"Fetches a bundle of all "&amp;B21&amp;" resources matching the specified "&amp;SUBSTITUTE(D21,","," and ")</f>
         <v>Fetches a bundle of all Encounter resources matching the specified patient and discharge-disposition</v>
       </c>
     </row>
@@ -10951,7 +10936,7 @@
         <v>150</v>
       </c>
       <c r="C22" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B22)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D22" t="s">
@@ -10966,7 +10951,7 @@
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>"Fetches a bundle of all "&amp;B22&amp;" resources matching the specified "&amp;SUBSTITUTE(D22,","," and ")</f>
         <v>Fetches a bundle of all !Encounter resources matching the specified status and type</v>
       </c>
     </row>
@@ -10978,7 +10963,7 @@
         <v>151</v>
       </c>
       <c r="C23" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B23)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D23" t="s">
@@ -10992,7 +10977,7 @@
       </c>
       <c r="J23" s="4"/>
       <c r="K23" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>"Fetches a bundle of all "&amp;B23&amp;" resources matching the specified "&amp;SUBSTITUTE(D23,","," and ")</f>
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and publisher</v>
       </c>
     </row>
@@ -11004,7 +10989,7 @@
         <v>151</v>
       </c>
       <c r="C24" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B24)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D24" t="s">
@@ -11017,7 +11002,7 @@
         <v>116</v>
       </c>
       <c r="K24" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>"Fetches a bundle of all "&amp;B24&amp;" resources matching the specified "&amp;SUBSTITUTE(D24,","," and ")</f>
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and publisher and status</v>
       </c>
     </row>
@@ -11029,7 +11014,7 @@
         <v>151</v>
       </c>
       <c r="C25" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B25)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D25" t="s">
@@ -11043,7 +11028,7 @@
       </c>
       <c r="I25" s="4"/>
       <c r="K25" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>"Fetches a bundle of all "&amp;B25&amp;" resources matching the specified "&amp;SUBSTITUTE(D25,","," and ")</f>
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and status</v>
       </c>
     </row>
@@ -11055,7 +11040,7 @@
         <v>151</v>
       </c>
       <c r="C26" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B26)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D26" t="s">
@@ -11070,7 +11055,7 @@
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
       <c r="K26" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>"Fetches a bundle of all "&amp;B26&amp;" resources matching the specified "&amp;SUBSTITUTE(D26,","," and ")</f>
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and status</v>
       </c>
     </row>
@@ -11082,7 +11067,7 @@
         <v>151</v>
       </c>
       <c r="C27" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B27)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D27" t="s">
@@ -11097,7 +11082,7 @@
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>"Fetches a bundle of all "&amp;B27&amp;" resources matching the specified "&amp;SUBSTITUTE(D27,","," and ")</f>
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and status and version</v>
       </c>
     </row>
@@ -11109,7 +11094,7 @@
         <v>151</v>
       </c>
       <c r="C28" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B28)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D28" t="s">
@@ -11124,7 +11109,7 @@
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>"Fetches a bundle of all "&amp;B28&amp;" resources matching the specified "&amp;SUBSTITUTE(D28,","," and ")</f>
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and version</v>
       </c>
     </row>
@@ -11136,7 +11121,7 @@
         <v>151</v>
       </c>
       <c r="C29" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B29)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D29" t="s">
@@ -11149,7 +11134,7 @@
         <v>120</v>
       </c>
       <c r="K29" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>"Fetches a bundle of all "&amp;B29&amp;" resources matching the specified "&amp;SUBSTITUTE(D29,","," and ")</f>
         <v>Fetches a bundle of all !Questionnaire resources matching the specified status and title and version</v>
       </c>
     </row>
@@ -11161,7 +11146,7 @@
         <v>151</v>
       </c>
       <c r="C30" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B30)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D30" t="s">
@@ -11174,7 +11159,7 @@
         <v>52</v>
       </c>
       <c r="K30" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>"Fetches a bundle of all "&amp;B30&amp;" resources matching the specified "&amp;SUBSTITUTE(D30,","," and ")</f>
         <v>Fetches a bundle of all !Questionnaire resources matching the specified status and version</v>
       </c>
     </row>
@@ -11186,7 +11171,7 @@
         <v>151</v>
       </c>
       <c r="C31" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B31)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D31" t="s">
@@ -11199,7 +11184,7 @@
         <v>120</v>
       </c>
       <c r="K31" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>"Fetches a bundle of all "&amp;B31&amp;" resources matching the specified "&amp;SUBSTITUTE(D31,","," and ")</f>
         <v>Fetches a bundle of all !Questionnaire resources matching the specified title and version</v>
       </c>
     </row>
@@ -11211,7 +11196,7 @@
         <v>19</v>
       </c>
       <c r="C32" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B32)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D32" t="s">
@@ -11230,7 +11215,7 @@
         <v>170</v>
       </c>
       <c r="K32" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>"Fetches a bundle of all "&amp;B32&amp;" resources matching the specified "&amp;SUBSTITUTE(D32,","," and ")</f>
         <v>Fetches a bundle of all Patient resources matching the specified birthdate and family</v>
       </c>
     </row>
@@ -11242,7 +11227,7 @@
         <v>19</v>
       </c>
       <c r="C33" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B33)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D33" t="s">
@@ -11261,7 +11246,7 @@
         <v>625</v>
       </c>
       <c r="K33" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>"Fetches a bundle of all "&amp;B33&amp;" resources matching the specified "&amp;SUBSTITUTE(D33,","," and ")</f>
         <v>Fetches a bundle of all Patient resources matching the specified death-date and family</v>
       </c>
     </row>
@@ -11273,7 +11258,7 @@
         <v>19</v>
       </c>
       <c r="C34" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B34)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D34" t="s">
@@ -11292,7 +11277,7 @@
         <v>167</v>
       </c>
       <c r="K34" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>"Fetches a bundle of all "&amp;B34&amp;" resources matching the specified "&amp;SUBSTITUTE(D34,","," and ")</f>
         <v>Fetches a bundle of all Patient resources matching the specified birthdate and name</v>
       </c>
     </row>
@@ -11304,7 +11289,7 @@
         <v>19</v>
       </c>
       <c r="C35" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B35)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D35" t="s">
@@ -11323,7 +11308,7 @@
         <v>169</v>
       </c>
       <c r="K35" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>"Fetches a bundle of all "&amp;B35&amp;" resources matching the specified "&amp;SUBSTITUTE(D35,","," and ")</f>
         <v>Fetches a bundle of all Patient resources matching the specified family and gender</v>
       </c>
     </row>
@@ -11335,7 +11320,7 @@
         <v>19</v>
       </c>
       <c r="C36" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B36)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D36" t="s">
@@ -11354,7 +11339,7 @@
         <v>168</v>
       </c>
       <c r="K36" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>"Fetches a bundle of all "&amp;B36&amp;" resources matching the specified "&amp;SUBSTITUTE(D36,","," and ")</f>
         <v>Fetches a bundle of all Patient resources matching the specified gender and name</v>
       </c>
     </row>
@@ -11366,7 +11351,7 @@
         <v>131</v>
       </c>
       <c r="C37" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B37)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D37" t="s">
@@ -11399,7 +11384,7 @@
         <v>131</v>
       </c>
       <c r="C38" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B38)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D38" t="s">
@@ -11429,7 +11414,7 @@
         <v>131</v>
       </c>
       <c r="C39" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B39)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D39" t="s">
@@ -11462,7 +11447,7 @@
         <v>131</v>
       </c>
       <c r="C40" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B40)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D40" t="s">
@@ -11492,7 +11477,7 @@
         <v>131</v>
       </c>
       <c r="C41" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B41)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D41" t="s">
@@ -11522,7 +11507,7 @@
         <v>131</v>
       </c>
       <c r="C42" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B42)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D42" t="s">
@@ -11552,7 +11537,7 @@
         <v>131</v>
       </c>
       <c r="C43" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B43)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D43" t="s">
@@ -11582,7 +11567,7 @@
         <v>131</v>
       </c>
       <c r="C44" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B44)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D44" t="s">
@@ -11612,7 +11597,7 @@
         <v>131</v>
       </c>
       <c r="C45" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B45)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D45" t="s">
@@ -11648,9 +11633,6 @@
       <c r="D46" t="s">
         <v>711</v>
       </c>
-      <c r="E46" t="s">
-        <v>51</v>
-      </c>
       <c r="F46" t="s">
         <v>64</v>
       </c>
@@ -11674,7 +11656,7 @@
         <v>18</v>
       </c>
       <c r="C47" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B47)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-allergyintolerance</v>
       </c>
       <c r="D47" t="s">
@@ -11704,7 +11686,7 @@
         <v>154</v>
       </c>
       <c r="C48" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B48)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-immunization</v>
       </c>
       <c r="D48" t="s">
@@ -11735,7 +11717,7 @@
         <v>154</v>
       </c>
       <c r="C49" t="str">
-        <f t="shared" si="0"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B49)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-immunization</v>
       </c>
       <c r="D49" t="s">
@@ -11892,14 +11874,11 @@
         <v>172</v>
       </c>
       <c r="C54" t="str">
-        <f t="shared" ref="C54:C66" si="2">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B54)</f>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B54)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-diagnosticreport</v>
       </c>
       <c r="D54" t="s">
         <v>713</v>
-      </c>
-      <c r="E54" t="s">
-        <v>51</v>
       </c>
       <c r="F54" t="s">
         <v>64</v>
@@ -11954,7 +11933,7 @@
         <v>173</v>
       </c>
       <c r="C56" t="str">
-        <f t="shared" si="2"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B56)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D56" t="s">
@@ -11985,7 +11964,7 @@
         <v>173</v>
       </c>
       <c r="C57" t="str">
-        <f t="shared" si="2"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B57)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D57" t="s">
@@ -12016,7 +11995,7 @@
         <v>174</v>
       </c>
       <c r="C58" t="str">
-        <f t="shared" si="2"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B58)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D58" t="s">
@@ -12049,7 +12028,7 @@
         <v>174</v>
       </c>
       <c r="C59" t="str">
-        <f t="shared" si="2"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B59)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D59" t="s">
@@ -12082,7 +12061,7 @@
         <v>174</v>
       </c>
       <c r="C60" t="str">
-        <f t="shared" si="2"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B60)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D60" t="s">
@@ -12115,7 +12094,7 @@
         <v>174</v>
       </c>
       <c r="C61" t="str">
-        <f t="shared" si="2"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B61)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D61" t="s">
@@ -12148,7 +12127,7 @@
         <v>415</v>
       </c>
       <c r="C62" t="str">
-        <f t="shared" si="2"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B62)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationstatement</v>
       </c>
       <c r="D62" t="s">
@@ -12179,7 +12158,7 @@
         <v>415</v>
       </c>
       <c r="C63" t="str">
-        <f t="shared" si="2"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B63)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationstatement</v>
       </c>
       <c r="D63" t="s">
@@ -12209,7 +12188,7 @@
         <v>175</v>
       </c>
       <c r="C64" t="str">
-        <f t="shared" si="2"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B64)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
       </c>
       <c r="D64" t="s">
@@ -12240,7 +12219,7 @@
         <v>175</v>
       </c>
       <c r="C65" t="str">
-        <f t="shared" si="2"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B65)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
       </c>
       <c r="D65" t="s">
@@ -12271,7 +12250,7 @@
         <v>175</v>
       </c>
       <c r="C66" t="str">
-        <f t="shared" si="2"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B66)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
       </c>
       <c r="D66" t="s">
@@ -12435,9 +12414,6 @@
       <c r="D71" t="s">
         <v>713</v>
       </c>
-      <c r="E71" t="s">
-        <v>51</v>
-      </c>
       <c r="F71" t="s">
         <v>64</v>
       </c>
@@ -12653,7 +12629,7 @@
         <v>171</v>
       </c>
       <c r="C78" t="str">
-        <f t="shared" ref="C78:C83" si="3">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B78)</f>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B78)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D78" t="s">
@@ -12684,7 +12660,7 @@
         <v>269</v>
       </c>
       <c r="C79" t="str">
-        <f t="shared" si="3"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B79)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!documentreference</v>
       </c>
       <c r="D79" t="s">
@@ -12713,7 +12689,7 @@
         <v>171</v>
       </c>
       <c r="C80" t="str">
-        <f t="shared" si="3"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B80)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D80" t="s">
@@ -12746,7 +12722,7 @@
         <v>171</v>
       </c>
       <c r="C81" t="str">
-        <f t="shared" si="3"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B81)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D81" t="s">
@@ -12779,7 +12755,7 @@
         <v>171</v>
       </c>
       <c r="C82" t="str">
-        <f t="shared" si="3"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B82)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D82" t="s">
@@ -12809,7 +12785,7 @@
         <v>171</v>
       </c>
       <c r="C83" t="str">
-        <f t="shared" si="3"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B83)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D83" t="s">
@@ -12928,7 +12904,7 @@
         <v>517</v>
       </c>
       <c r="C87" t="str">
-        <f t="shared" ref="C87:C100" si="4">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B87)</f>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B87)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D87" t="s">
@@ -12959,7 +12935,7 @@
         <v>517</v>
       </c>
       <c r="C88" t="str">
-        <f t="shared" si="4"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B88)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D88" t="s">
@@ -12990,7 +12966,7 @@
         <v>517</v>
       </c>
       <c r="C89" t="str">
-        <f t="shared" si="4"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B89)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D89" t="s">
@@ -13021,7 +12997,7 @@
         <v>517</v>
       </c>
       <c r="C90" t="str">
-        <f t="shared" si="4"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B90)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D90" t="s">
@@ -13052,7 +13028,7 @@
         <v>517</v>
       </c>
       <c r="C91" t="str">
-        <f t="shared" si="4"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B91)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D91" t="s">
@@ -13083,7 +13059,7 @@
         <v>173</v>
       </c>
       <c r="C92" t="str">
-        <f t="shared" si="4"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B92)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D92" t="s">
@@ -13114,7 +13090,7 @@
         <v>585</v>
       </c>
       <c r="C93" t="str">
-        <f t="shared" si="4"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B93)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D93" t="s">
@@ -13145,7 +13121,7 @@
         <v>679</v>
       </c>
       <c r="C94" t="str">
-        <f t="shared" si="4"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B94)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="D94" t="s">
@@ -13179,7 +13155,7 @@
         <v>585</v>
       </c>
       <c r="C95" t="str">
-        <f t="shared" si="4"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B95)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D95" t="s">
@@ -13210,7 +13186,7 @@
         <v>679</v>
       </c>
       <c r="C96" t="str">
-        <f t="shared" si="4"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B96)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="D96" s="16" t="s">
@@ -13244,7 +13220,7 @@
         <v>585</v>
       </c>
       <c r="C97" t="str">
-        <f t="shared" si="4"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B97)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D97" s="16" t="s">
@@ -13275,7 +13251,7 @@
         <v>618</v>
       </c>
       <c r="C98" t="str">
-        <f t="shared" si="4"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B98)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</v>
       </c>
       <c r="D98" s="16" t="s">
@@ -13308,7 +13284,7 @@
         <v>618</v>
       </c>
       <c r="C99" t="str">
-        <f t="shared" si="4"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B99)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</v>
       </c>
       <c r="D99" s="16" t="s">
@@ -13341,7 +13317,7 @@
         <v>621</v>
       </c>
       <c r="C100" t="str">
-        <f t="shared" si="4"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B100)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationdispense</v>
       </c>
       <c r="D100" s="16" t="s">
@@ -13398,13 +13374,13 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:K101" xr:uid="{331E0B16-168F-459B-8951-3DF614BF0371}"/>
-  <conditionalFormatting sqref="B102:B1048576 B1:B100">
+  <conditionalFormatting sqref="B1:B100 B102:B1048576">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C101" r:id="rId1" xr:uid="{1EAF46C7-3D36-1B4E-B601-050DE1E6B350}"/>
+    <hyperlink ref="C101" r:id="rId1" xr:uid="{8FF299B3-788F-704F-8CF5-5179C2FB9CEC}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>

</xml_diff>

<commit_message>
Clarify Role and use of US Core SearchParameters vs FHIR standard SearchParameters [FHIR-46036]
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC449E9-20FB-414E-99C1-2B8F13F0D297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{806D6901-D360-034B-B321-E3B69D0ECA54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="65700" yWindow="500" windowWidth="36700" windowHeight="28300" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="65700" yWindow="500" windowWidth="36700" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -1944,11 +1944,6 @@
     <t>US Core Condition Problems and Health Concerns Profile</t>
   </si>
   <si>
-    <t>The US Core Client **SHALL**:
-1. Support fetching and querying of one or more US Core profile(s), using the supported RESTful interactions and search parameters declared in the US Core Server CapabilityStatement.
-1. Follow the requirements documented in the [General Requirements](general-requirements.html) and [Must Support](must-support.html) pages</t>
-  </si>
-  <si>
     <t>1. See the [General Security Considerations](security.html) section for requirements and recommendations.</t>
   </si>
   <si>
@@ -2518,12 +2513,24 @@
       <t>]/Condition?patient=1032702&amp;_lastUpdated=ge2024-01-01T00:00:00Z</t>
     </r>
   </si>
+  <si>
+    <t>The US Core Client **SHALL**:
+1. Support fetching and querying of one or more US Core profile(s), using the supported RESTful interactions and search parameters declared in the US Core Server CapabilityStatement.
+1. Follow the requirements documented in the [General Requirements](general-requirements.html) and [Must Support](must-support.html) pages
+**NOTE**: US Core SearchParameters referenced in this CapabilityStatement that are derived from standard FHIR SearchParameters are only defined to document Server and Client expectations. They specify additional expectations for the following SearchParameter elements:
+- `multipleAnd`
+- `multipleOr`
+- `comparator`
+- `modifier`
+- `chain`
+For search operations, Clients **SHOULD** use the standard FHIR SearchParameters.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2637,12 +2644,6 @@
       <sz val="14"/>
       <color rgb="FF172B4D"/>
       <name val="Helvetica Neue"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -3229,7 +3230,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{427A2FB7-DA88-6B49-A242-D69B65B8CD67}">
   <dimension ref="A1:AB132"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -3344,7 +3345,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C2" t="s">
         <v>50</v>
@@ -3369,7 +3370,7 @@
         <v>52</v>
       </c>
       <c r="L2" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="M2" t="s">
         <v>51</v>
@@ -3391,7 +3392,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C3" t="s">
         <v>65</v>
@@ -3435,7 +3436,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C4" t="s">
         <v>62</v>
@@ -3482,7 +3483,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C5" t="s">
         <v>56</v>
@@ -3526,7 +3527,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C6" t="s">
         <v>57</v>
@@ -3582,7 +3583,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C7" t="s">
         <v>54</v>
@@ -3626,7 +3627,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C8" t="s">
         <v>61</v>
@@ -3971,10 +3972,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>620</v>
+      </c>
+      <c r="C15" t="s">
         <v>621</v>
-      </c>
-      <c r="C15" t="s">
-        <v>622</v>
       </c>
       <c r="D15" t="s">
         <v>28</v>
@@ -4460,7 +4461,7 @@
         <v>78</v>
       </c>
       <c r="C24" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="D24" t="s">
         <v>28</v>
@@ -4482,19 +4483,19 @@
         <v>52</v>
       </c>
       <c r="L24" t="s">
+        <v>612</v>
+      </c>
+      <c r="M24" t="s">
+        <v>51</v>
+      </c>
+      <c r="O24" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y24" s="4" t="s">
         <v>613</v>
       </c>
-      <c r="M24" t="s">
-        <v>51</v>
-      </c>
-      <c r="O24" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y24" s="4" t="s">
+      <c r="Z24" t="s">
         <v>614</v>
-      </c>
-      <c r="Z24" t="s">
-        <v>615</v>
       </c>
       <c r="AA24" s="8" t="str">
         <f>"Fetches a bundle of all "&amp;B24&amp;" resources matching the name"</f>
@@ -4510,7 +4511,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="C25" t="s">
         <v>587</v>
@@ -4538,16 +4539,16 @@
         <v>52</v>
       </c>
       <c r="L25" t="s">
+        <v>645</v>
+      </c>
+      <c r="M25" t="s">
+        <v>51</v>
+      </c>
+      <c r="O25" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y25" s="19" t="s">
         <v>646</v>
-      </c>
-      <c r="M25" t="s">
-        <v>51</v>
-      </c>
-      <c r="O25" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y25" s="19" t="s">
-        <v>647</v>
       </c>
       <c r="AB25" t="str">
         <f t="shared" si="1"/>
@@ -5538,7 +5539,7 @@
         <v>131</v>
       </c>
       <c r="C44" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D44" t="s">
         <v>28</v>
@@ -5547,7 +5548,7 @@
         <v>0</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="G44" t="str">
         <f t="shared" si="0"/>
@@ -5589,7 +5590,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C45" t="s">
         <v>83</v>
@@ -5627,7 +5628,7 @@
         <v>51</v>
       </c>
       <c r="Y45" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Z45" s="4" t="str">
         <f>"GET [base]/"&amp;B45&amp;"?patient=1137192"</f>
@@ -5967,7 +5968,7 @@
         <v>172</v>
       </c>
       <c r="C52" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D52" t="s">
         <v>28</v>
@@ -5976,7 +5977,7 @@
         <v>0</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="G52" t="str">
         <f t="shared" si="0"/>
@@ -6664,7 +6665,7 @@
         <v>20</v>
       </c>
       <c r="C65" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D65" t="s">
         <v>28</v>
@@ -6673,7 +6674,7 @@
         <v>0</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="G65" t="str">
         <f t="shared" si="0"/>
@@ -7684,7 +7685,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C84" t="s">
         <v>83</v>
@@ -7722,10 +7723,10 @@
         <v>51</v>
       </c>
       <c r="X84" s="6" t="s">
+        <v>618</v>
+      </c>
+      <c r="Z84" s="8" t="s">
         <v>619</v>
-      </c>
-      <c r="Z84" s="8" t="s">
-        <v>620</v>
       </c>
       <c r="AA84" s="8" t="str">
         <f>"Fetches a bundle of all "&amp;B84&amp; " resources for the specified patient."</f>
@@ -7741,7 +7742,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C85" t="s">
         <v>56</v>
@@ -7794,7 +7795,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C86" t="s">
         <v>12</v>
@@ -8271,7 +8272,7 @@
         <v>176</v>
       </c>
       <c r="C95" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D95" t="s">
         <v>28</v>
@@ -8280,7 +8281,7 @@
         <v>0</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="G95" t="str">
         <f t="shared" si="6"/>
@@ -8645,7 +8646,7 @@
         <v>19</v>
       </c>
       <c r="C102" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D102" t="s">
         <v>28</v>
@@ -8919,7 +8920,7 @@
         <v>51</v>
       </c>
       <c r="Y107" s="4" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="Z107" t="s">
         <v>166</v>
@@ -9486,7 +9487,7 @@
         <v>support both read QuestionnaireResponse by `id` **AND** QuestionnaireResponse search</v>
       </c>
       <c r="Z117" s="4" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="AB117" t="str">
         <f t="shared" si="4"/>
@@ -9542,7 +9543,7 @@
         <v>86</v>
       </c>
       <c r="Y118" s="19" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="AB118" t="str">
         <f t="shared" si="4"/>
@@ -9651,7 +9652,7 @@
         <v>51</v>
       </c>
       <c r="Y120" s="19" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="AB120" t="str">
         <f t="shared" si="4"/>
@@ -9704,7 +9705,7 @@
         <v>51</v>
       </c>
       <c r="Y121" s="19" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="AB121" t="str">
         <f t="shared" si="4"/>
@@ -9803,7 +9804,7 @@
         <v>51</v>
       </c>
       <c r="Y123" s="4" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="Z123" s="4" t="str">
         <f>"GET [base]/"&amp;B123&amp;"?"&amp;C123&amp;"=Mary Shaw"</f>
@@ -10164,7 +10165,7 @@
         <v>475</v>
       </c>
       <c r="G130" t="str">
-        <f t="shared" ref="G130:G160" si="9">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B130)</f>
+        <f t="shared" ref="G130:G132" si="9">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B130)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="H130" t="s">
@@ -10202,7 +10203,7 @@
         <v>130</v>
       </c>
       <c r="B131" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="C131" t="s">
         <v>50</v>
@@ -10254,7 +10255,7 @@
         <v>131</v>
       </c>
       <c r="B132" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="C132" t="s">
         <v>83</v>
@@ -10391,7 +10392,7 @@
         <v>150</v>
       </c>
       <c r="C2" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B2)</f>
+        <f t="shared" ref="C2:C49" si="0">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B2)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D2" t="s">
@@ -10404,7 +10405,7 @@
         <v>93</v>
       </c>
       <c r="K2" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B2&amp;" resources matching the specified "&amp;SUBSTITUTE(D2,","," and ")</f>
+        <f t="shared" ref="K2:K17" si="1">"Fetches a bundle of all "&amp;B2&amp;" resources matching the specified "&amp;SUBSTITUTE(D2,","," and ")</f>
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date</v>
       </c>
     </row>
@@ -10416,7 +10417,7 @@
         <v>150</v>
       </c>
       <c r="C3" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B3)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D3" t="s">
@@ -10429,7 +10430,7 @@
         <v>95</v>
       </c>
       <c r="K3" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B3&amp;" resources matching the specified "&amp;SUBSTITUTE(D3,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and patient</v>
       </c>
     </row>
@@ -10441,7 +10442,7 @@
         <v>150</v>
       </c>
       <c r="C4" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B4)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D4" t="s">
@@ -10454,7 +10455,7 @@
         <v>95</v>
       </c>
       <c r="K4" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B4&amp;" resources matching the specified "&amp;SUBSTITUTE(D4,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and patient and type</v>
       </c>
     </row>
@@ -10466,7 +10467,7 @@
         <v>150</v>
       </c>
       <c r="C5" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B5)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D5" t="s">
@@ -10479,7 +10480,7 @@
         <v>93</v>
       </c>
       <c r="K5" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B5&amp;" resources matching the specified "&amp;SUBSTITUTE(D5,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and type</v>
       </c>
     </row>
@@ -10491,7 +10492,7 @@
         <v>20</v>
       </c>
       <c r="C6" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B6)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D6" t="s">
@@ -10510,7 +10511,7 @@
         <v>286</v>
       </c>
       <c r="K6" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B6&amp;" resources matching the specified "&amp;SUBSTITUTE(D6,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all Encounter resources matching the specified class and patient</v>
       </c>
     </row>
@@ -10522,7 +10523,7 @@
         <v>150</v>
       </c>
       <c r="C7" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B7)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D7" t="s">
@@ -10535,7 +10536,7 @@
         <v>99</v>
       </c>
       <c r="K7" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B7&amp;" resources matching the specified "&amp;SUBSTITUTE(D7,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and status</v>
       </c>
     </row>
@@ -10547,7 +10548,7 @@
         <v>150</v>
       </c>
       <c r="C8" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B8)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D8" t="s">
@@ -10560,7 +10561,7 @@
         <v>99</v>
       </c>
       <c r="K8" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B8&amp;" resources matching the specified "&amp;SUBSTITUTE(D8,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and status and type</v>
       </c>
     </row>
@@ -10572,7 +10573,7 @@
         <v>150</v>
       </c>
       <c r="C9" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B9)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D9" t="s">
@@ -10586,7 +10587,7 @@
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B9&amp;" resources matching the specified "&amp;SUBSTITUTE(D9,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and type</v>
       </c>
     </row>
@@ -10598,7 +10599,7 @@
         <v>150</v>
       </c>
       <c r="C10" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B10)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D10" t="s">
@@ -10613,7 +10614,7 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B10&amp;" resources matching the specified "&amp;SUBSTITUTE(D10,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all !Encounter resources matching the specified class and status</v>
       </c>
     </row>
@@ -10625,7 +10626,7 @@
         <v>150</v>
       </c>
       <c r="C11" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B11)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D11" t="s">
@@ -10639,7 +10640,7 @@
       </c>
       <c r="I11" s="4"/>
       <c r="K11" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B11&amp;" resources matching the specified "&amp;SUBSTITUTE(D11,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all !Encounter resources matching the specified class and status and type</v>
       </c>
     </row>
@@ -10651,7 +10652,7 @@
         <v>150</v>
       </c>
       <c r="C12" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B12)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D12" t="s">
@@ -10664,7 +10665,7 @@
         <v>52</v>
       </c>
       <c r="K12" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B12&amp;" resources matching the specified "&amp;SUBSTITUTE(D12,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all !Encounter resources matching the specified class and type</v>
       </c>
     </row>
@@ -10676,7 +10677,7 @@
         <v>20</v>
       </c>
       <c r="C13" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B13)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D13" t="s">
@@ -10695,7 +10696,7 @@
         <v>478</v>
       </c>
       <c r="K13" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B13&amp;" resources matching the specified "&amp;SUBSTITUTE(D13,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all Encounter resources matching the specified date and patient</v>
       </c>
     </row>
@@ -10707,7 +10708,7 @@
         <v>150</v>
       </c>
       <c r="C14" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B14)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D14" t="s">
@@ -10720,7 +10721,7 @@
         <v>95</v>
       </c>
       <c r="K14" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B14&amp;" resources matching the specified "&amp;SUBSTITUTE(D14,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all !Encounter resources matching the specified date and patient and type</v>
       </c>
     </row>
@@ -10732,7 +10733,7 @@
         <v>150</v>
       </c>
       <c r="C15" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B15)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D15" t="s">
@@ -10745,7 +10746,7 @@
         <v>93</v>
       </c>
       <c r="K15" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B15&amp;" resources matching the specified "&amp;SUBSTITUTE(D15,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all !Encounter resources matching the specified date and type</v>
       </c>
     </row>
@@ -10757,7 +10758,7 @@
         <v>20</v>
       </c>
       <c r="C16" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B16)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D16" t="s">
@@ -10776,7 +10777,7 @@
         <v>287</v>
       </c>
       <c r="K16" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B16&amp;" resources matching the specified "&amp;SUBSTITUTE(D16,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all Encounter resources matching the specified patient and type</v>
       </c>
     </row>
@@ -10788,7 +10789,7 @@
         <v>20</v>
       </c>
       <c r="C17" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B17)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D17" t="s">
@@ -10807,7 +10808,7 @@
         <v>536</v>
       </c>
       <c r="K17" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B17&amp;" resources matching the specified "&amp;SUBSTITUTE(D17,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all Encounter resources matching the specified patient and location</v>
       </c>
     </row>
@@ -10819,11 +10820,11 @@
         <v>20</v>
       </c>
       <c r="C18" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B18)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D18" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="F18" t="s">
         <v>64</v>
@@ -10833,7 +10834,7 @@
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="27" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="K18" s="24" t="str">
         <f>"Fetches a bundle of all "&amp;B18&amp;" resources for the specified "&amp;SUBSTITUTE(D18,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
@@ -10848,7 +10849,7 @@
         <v>150</v>
       </c>
       <c r="C19" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B19)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D19" t="s">
@@ -10862,7 +10863,7 @@
       </c>
       <c r="J19" s="4"/>
       <c r="K19" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B19&amp;" resources matching the specified "&amp;SUBSTITUTE(D19,","," and ")</f>
+        <f t="shared" ref="K19:K36" si="2">"Fetches a bundle of all "&amp;B19&amp;" resources matching the specified "&amp;SUBSTITUTE(D19,","," and ")</f>
         <v>Fetches a bundle of all !Encounter resources matching the specified patient and status and type</v>
       </c>
     </row>
@@ -10874,7 +10875,7 @@
         <v>20</v>
       </c>
       <c r="C20" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B20)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D20" t="s">
@@ -10893,7 +10894,7 @@
         <v>288</v>
       </c>
       <c r="K20" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B20&amp;" resources matching the specified "&amp;SUBSTITUTE(D20,","," and ")</f>
+        <f t="shared" si="2"/>
         <v>Fetches a bundle of all Encounter resources matching the specified patient and status</v>
       </c>
     </row>
@@ -10905,7 +10906,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B21)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D21" t="s">
@@ -10924,7 +10925,7 @@
         <v>538</v>
       </c>
       <c r="K21" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B21&amp;" resources matching the specified "&amp;SUBSTITUTE(D21,","," and ")</f>
+        <f t="shared" si="2"/>
         <v>Fetches a bundle of all Encounter resources matching the specified patient and discharge-disposition</v>
       </c>
     </row>
@@ -10936,7 +10937,7 @@
         <v>150</v>
       </c>
       <c r="C22" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B22)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D22" t="s">
@@ -10951,7 +10952,7 @@
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B22&amp;" resources matching the specified "&amp;SUBSTITUTE(D22,","," and ")</f>
+        <f t="shared" si="2"/>
         <v>Fetches a bundle of all !Encounter resources matching the specified status and type</v>
       </c>
     </row>
@@ -10963,7 +10964,7 @@
         <v>151</v>
       </c>
       <c r="C23" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B23)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D23" t="s">
@@ -10977,7 +10978,7 @@
       </c>
       <c r="J23" s="4"/>
       <c r="K23" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B23&amp;" resources matching the specified "&amp;SUBSTITUTE(D23,","," and ")</f>
+        <f t="shared" si="2"/>
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and publisher</v>
       </c>
     </row>
@@ -10989,7 +10990,7 @@
         <v>151</v>
       </c>
       <c r="C24" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B24)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D24" t="s">
@@ -11002,7 +11003,7 @@
         <v>116</v>
       </c>
       <c r="K24" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B24&amp;" resources matching the specified "&amp;SUBSTITUTE(D24,","," and ")</f>
+        <f t="shared" si="2"/>
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and publisher and status</v>
       </c>
     </row>
@@ -11014,7 +11015,7 @@
         <v>151</v>
       </c>
       <c r="C25" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B25)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D25" t="s">
@@ -11028,7 +11029,7 @@
       </c>
       <c r="I25" s="4"/>
       <c r="K25" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B25&amp;" resources matching the specified "&amp;SUBSTITUTE(D25,","," and ")</f>
+        <f t="shared" si="2"/>
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and status</v>
       </c>
     </row>
@@ -11040,7 +11041,7 @@
         <v>151</v>
       </c>
       <c r="C26" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B26)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D26" t="s">
@@ -11055,7 +11056,7 @@
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
       <c r="K26" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B26&amp;" resources matching the specified "&amp;SUBSTITUTE(D26,","," and ")</f>
+        <f t="shared" si="2"/>
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and status</v>
       </c>
     </row>
@@ -11067,7 +11068,7 @@
         <v>151</v>
       </c>
       <c r="C27" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B27)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D27" t="s">
@@ -11082,7 +11083,7 @@
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B27&amp;" resources matching the specified "&amp;SUBSTITUTE(D27,","," and ")</f>
+        <f t="shared" si="2"/>
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and status and version</v>
       </c>
     </row>
@@ -11094,7 +11095,7 @@
         <v>151</v>
       </c>
       <c r="C28" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B28)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D28" t="s">
@@ -11109,7 +11110,7 @@
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B28&amp;" resources matching the specified "&amp;SUBSTITUTE(D28,","," and ")</f>
+        <f t="shared" si="2"/>
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and version</v>
       </c>
     </row>
@@ -11121,7 +11122,7 @@
         <v>151</v>
       </c>
       <c r="C29" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B29)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D29" t="s">
@@ -11134,7 +11135,7 @@
         <v>120</v>
       </c>
       <c r="K29" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B29&amp;" resources matching the specified "&amp;SUBSTITUTE(D29,","," and ")</f>
+        <f t="shared" si="2"/>
         <v>Fetches a bundle of all !Questionnaire resources matching the specified status and title and version</v>
       </c>
     </row>
@@ -11146,7 +11147,7 @@
         <v>151</v>
       </c>
       <c r="C30" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B30)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D30" t="s">
@@ -11159,7 +11160,7 @@
         <v>52</v>
       </c>
       <c r="K30" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B30&amp;" resources matching the specified "&amp;SUBSTITUTE(D30,","," and ")</f>
+        <f t="shared" si="2"/>
         <v>Fetches a bundle of all !Questionnaire resources matching the specified status and version</v>
       </c>
     </row>
@@ -11171,7 +11172,7 @@
         <v>151</v>
       </c>
       <c r="C31" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B31)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D31" t="s">
@@ -11184,7 +11185,7 @@
         <v>120</v>
       </c>
       <c r="K31" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B31&amp;" resources matching the specified "&amp;SUBSTITUTE(D31,","," and ")</f>
+        <f t="shared" si="2"/>
         <v>Fetches a bundle of all !Questionnaire resources matching the specified title and version</v>
       </c>
     </row>
@@ -11196,7 +11197,7 @@
         <v>19</v>
       </c>
       <c r="C32" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B32)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D32" t="s">
@@ -11215,7 +11216,7 @@
         <v>170</v>
       </c>
       <c r="K32" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B32&amp;" resources matching the specified "&amp;SUBSTITUTE(D32,","," and ")</f>
+        <f t="shared" si="2"/>
         <v>Fetches a bundle of all Patient resources matching the specified birthdate and family</v>
       </c>
     </row>
@@ -11227,11 +11228,11 @@
         <v>19</v>
       </c>
       <c r="C33" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B33)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D33" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F33" t="s">
         <v>64</v>
@@ -11240,13 +11241,13 @@
         <v>127</v>
       </c>
       <c r="I33" s="4" t="s">
+        <v>623</v>
+      </c>
+      <c r="J33" s="4" t="s">
         <v>624</v>
       </c>
-      <c r="J33" s="4" t="s">
-        <v>625</v>
-      </c>
       <c r="K33" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B33&amp;" resources matching the specified "&amp;SUBSTITUTE(D33,","," and ")</f>
+        <f t="shared" si="2"/>
         <v>Fetches a bundle of all Patient resources matching the specified death-date and family</v>
       </c>
     </row>
@@ -11258,7 +11259,7 @@
         <v>19</v>
       </c>
       <c r="C34" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B34)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D34" t="s">
@@ -11277,7 +11278,7 @@
         <v>167</v>
       </c>
       <c r="K34" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B34&amp;" resources matching the specified "&amp;SUBSTITUTE(D34,","," and ")</f>
+        <f t="shared" si="2"/>
         <v>Fetches a bundle of all Patient resources matching the specified birthdate and name</v>
       </c>
     </row>
@@ -11289,7 +11290,7 @@
         <v>19</v>
       </c>
       <c r="C35" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B35)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D35" t="s">
@@ -11308,7 +11309,7 @@
         <v>169</v>
       </c>
       <c r="K35" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B35&amp;" resources matching the specified "&amp;SUBSTITUTE(D35,","," and ")</f>
+        <f t="shared" si="2"/>
         <v>Fetches a bundle of all Patient resources matching the specified family and gender</v>
       </c>
     </row>
@@ -11320,7 +11321,7 @@
         <v>19</v>
       </c>
       <c r="C36" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B36)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D36" t="s">
@@ -11339,7 +11340,7 @@
         <v>168</v>
       </c>
       <c r="K36" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B36&amp;" resources matching the specified "&amp;SUBSTITUTE(D36,","," and ")</f>
+        <f t="shared" si="2"/>
         <v>Fetches a bundle of all Patient resources matching the specified gender and name</v>
       </c>
     </row>
@@ -11351,7 +11352,7 @@
         <v>131</v>
       </c>
       <c r="C37" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B37)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D37" t="s">
@@ -11373,7 +11374,7 @@
         <v>306</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
@@ -11384,7 +11385,7 @@
         <v>131</v>
       </c>
       <c r="C38" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B38)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D38" t="s">
@@ -11414,11 +11415,11 @@
         <v>131</v>
       </c>
       <c r="C39" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B39)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D39" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="F39" t="s">
         <v>64</v>
@@ -11430,13 +11431,13 @@
         <v>389</v>
       </c>
       <c r="I39" s="4" t="s">
+        <v>684</v>
+      </c>
+      <c r="J39" s="24" t="s">
         <v>685</v>
       </c>
-      <c r="J39" s="24" t="s">
+      <c r="K39" s="4" t="s">
         <v>686</v>
-      </c>
-      <c r="K39" s="4" t="s">
-        <v>687</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
@@ -11447,7 +11448,7 @@
         <v>131</v>
       </c>
       <c r="C40" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B40)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D40" t="s">
@@ -11463,7 +11464,7 @@
         <v>143</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="K40" s="4" t="s">
         <v>540</v>
@@ -11477,7 +11478,7 @@
         <v>131</v>
       </c>
       <c r="C41" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B41)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D41" t="s">
@@ -11507,7 +11508,7 @@
         <v>131</v>
       </c>
       <c r="C42" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B42)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D42" t="s">
@@ -11537,7 +11538,7 @@
         <v>131</v>
       </c>
       <c r="C43" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B43)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D43" t="s">
@@ -11567,7 +11568,7 @@
         <v>131</v>
       </c>
       <c r="C44" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B44)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D44" t="s">
@@ -11597,7 +11598,7 @@
         <v>131</v>
       </c>
       <c r="C45" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B45)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D45" t="s">
@@ -11627,11 +11628,11 @@
         <v>131</v>
       </c>
       <c r="C46" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B46)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D46" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="F46" t="s">
         <v>64</v>
@@ -11641,7 +11642,7 @@
       </c>
       <c r="I46" s="4"/>
       <c r="J46" s="24" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="K46" s="24" t="str">
         <f>"Fetches a bundle of all "&amp;B46&amp;" resources for the specified "&amp;SUBSTITUTE(D46,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
@@ -11656,7 +11657,7 @@
         <v>18</v>
       </c>
       <c r="C47" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B47)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-allergyintolerance</v>
       </c>
       <c r="D47" t="s">
@@ -11686,7 +11687,7 @@
         <v>154</v>
       </c>
       <c r="C48" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B48)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-immunization</v>
       </c>
       <c r="D48" t="s">
@@ -11717,7 +11718,7 @@
         <v>154</v>
       </c>
       <c r="C49" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B49)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-immunization</v>
       </c>
       <c r="D49" t="s">
@@ -11748,7 +11749,7 @@
         <v>172</v>
       </c>
       <c r="C50" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="D50" t="s">
         <v>109</v>
@@ -11778,7 +11779,7 @@
         <v>172</v>
       </c>
       <c r="C51" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="D51" t="s">
         <v>138</v>
@@ -11811,7 +11812,7 @@
         <v>172</v>
       </c>
       <c r="C52" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="D52" t="s">
         <v>140</v>
@@ -11841,7 +11842,7 @@
         <v>172</v>
       </c>
       <c r="C53" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="D53" t="s">
         <v>187</v>
@@ -11878,7 +11879,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-diagnosticreport</v>
       </c>
       <c r="D54" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="F54" t="s">
         <v>64</v>
@@ -11888,7 +11889,7 @@
       </c>
       <c r="I54" s="4"/>
       <c r="J54" s="27" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="K54" s="24" t="str">
         <f>"Fetches a bundle of all "&amp;B54&amp;" resources for the specified "&amp;SUBSTITUTE(D54,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
@@ -11903,7 +11904,7 @@
         <v>172</v>
       </c>
       <c r="C55" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="D55" t="s">
         <v>208</v>
@@ -11933,7 +11934,7 @@
         <v>173</v>
       </c>
       <c r="C56" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B56)</f>
+        <f t="shared" ref="C56:C66" si="3">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B56)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D56" t="s">
@@ -11964,7 +11965,7 @@
         <v>173</v>
       </c>
       <c r="C57" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B57)</f>
+        <f t="shared" si="3"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D57" t="s">
@@ -11995,7 +11996,7 @@
         <v>174</v>
       </c>
       <c r="C58" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B58)</f>
+        <f t="shared" si="3"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D58" t="s">
@@ -12028,7 +12029,7 @@
         <v>174</v>
       </c>
       <c r="C59" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B59)</f>
+        <f t="shared" si="3"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D59" t="s">
@@ -12061,7 +12062,7 @@
         <v>174</v>
       </c>
       <c r="C60" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B60)</f>
+        <f t="shared" si="3"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D60" t="s">
@@ -12094,7 +12095,7 @@
         <v>174</v>
       </c>
       <c r="C61" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B61)</f>
+        <f t="shared" si="3"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D61" t="s">
@@ -12127,7 +12128,7 @@
         <v>415</v>
       </c>
       <c r="C62" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B62)</f>
+        <f t="shared" si="3"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationstatement</v>
       </c>
       <c r="D62" t="s">
@@ -12158,7 +12159,7 @@
         <v>415</v>
       </c>
       <c r="C63" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B63)</f>
+        <f t="shared" si="3"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationstatement</v>
       </c>
       <c r="D63" t="s">
@@ -12188,7 +12189,7 @@
         <v>175</v>
       </c>
       <c r="C64" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B64)</f>
+        <f t="shared" si="3"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
       </c>
       <c r="D64" t="s">
@@ -12219,7 +12220,7 @@
         <v>175</v>
       </c>
       <c r="C65" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B65)</f>
+        <f t="shared" si="3"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
       </c>
       <c r="D65" t="s">
@@ -12250,7 +12251,7 @@
         <v>175</v>
       </c>
       <c r="C66" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B66)</f>
+        <f t="shared" si="3"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
       </c>
       <c r="D66" t="s">
@@ -12281,7 +12282,7 @@
         <v>176</v>
       </c>
       <c r="C67" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="D67" t="s">
         <v>225</v>
@@ -12299,7 +12300,7 @@
         <v>264</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="K67" s="4" t="s">
         <v>299</v>
@@ -12313,7 +12314,7 @@
         <v>176</v>
       </c>
       <c r="C68" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="D68" t="s">
         <v>138</v>
@@ -12331,7 +12332,7 @@
         <v>209</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="K68" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B68&amp;" resources for the specified patient and a category code = `laboratory`"</f>
@@ -12346,7 +12347,7 @@
         <v>176</v>
       </c>
       <c r="C69" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="D69" t="s">
         <v>140</v>
@@ -12361,7 +12362,7 @@
         <v>212</v>
       </c>
       <c r="J69" s="8" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="K69" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B69&amp;" resources for the specified patient and observation code(s).  SHOULD support search by multiple report codes. The Observation `code` parameter searches `Observation.code only."</f>
@@ -12376,7 +12377,7 @@
         <v>176</v>
       </c>
       <c r="C70" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="D70" t="s">
         <v>187</v>
@@ -12394,7 +12395,7 @@
         <v>213</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="K70" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B70&amp;" resources for the specified patient and date and a category code = `laboratory`"</f>
@@ -12409,10 +12410,10 @@
         <v>176</v>
       </c>
       <c r="C71" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="D71" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="F71" t="s">
         <v>64</v>
@@ -12422,7 +12423,7 @@
       </c>
       <c r="I71" s="4"/>
       <c r="J71" s="27" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="K71" s="24" t="str">
         <f>"Fetches a bundle of all "&amp;B71&amp;" resources for the specified "&amp;SUBSTITUTE(D71,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
@@ -12437,7 +12438,7 @@
         <v>176</v>
       </c>
       <c r="C72" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="D72" t="s">
         <v>208</v>
@@ -12452,7 +12453,7 @@
         <v>211</v>
       </c>
       <c r="J72" s="4" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="K72" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B72&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
@@ -12596,7 +12597,7 @@
         <v>236</v>
       </c>
       <c r="C77" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B77)</f>
+        <f t="shared" ref="C77:C83" si="4">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B77)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
       </c>
       <c r="D77" t="s">
@@ -12629,7 +12630,7 @@
         <v>171</v>
       </c>
       <c r="C78" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B78)</f>
+        <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D78" t="s">
@@ -12660,7 +12661,7 @@
         <v>269</v>
       </c>
       <c r="C79" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B79)</f>
+        <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!documentreference</v>
       </c>
       <c r="D79" t="s">
@@ -12689,7 +12690,7 @@
         <v>171</v>
       </c>
       <c r="C80" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B80)</f>
+        <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D80" t="s">
@@ -12722,7 +12723,7 @@
         <v>171</v>
       </c>
       <c r="C81" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B81)</f>
+        <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D81" t="s">
@@ -12755,7 +12756,7 @@
         <v>171</v>
       </c>
       <c r="C82" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B82)</f>
+        <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D82" t="s">
@@ -12785,7 +12786,7 @@
         <v>171</v>
       </c>
       <c r="C83" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B83)</f>
+        <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D83" t="s">
@@ -12816,7 +12817,7 @@
         <v>237</v>
       </c>
       <c r="C84" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="D84" t="s">
         <v>111</v>
@@ -12845,7 +12846,7 @@
         <v>237</v>
       </c>
       <c r="C85" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="D85" t="s">
         <v>109</v>
@@ -12857,13 +12858,13 @@
         <v>99</v>
       </c>
       <c r="I85" s="4" t="s">
+        <v>626</v>
+      </c>
+      <c r="J85" s="4" t="s">
         <v>627</v>
       </c>
-      <c r="J85" s="4" t="s">
+      <c r="K85" s="4" t="s">
         <v>628</v>
-      </c>
-      <c r="K85" s="4" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
@@ -12874,7 +12875,7 @@
         <v>236</v>
       </c>
       <c r="C86" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B86)</f>
+        <f t="shared" ref="C86:C100" si="5">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B86)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
       </c>
       <c r="D86" t="s">
@@ -12904,7 +12905,7 @@
         <v>517</v>
       </c>
       <c r="C87" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B87)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D87" t="s">
@@ -12935,7 +12936,7 @@
         <v>517</v>
       </c>
       <c r="C88" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B88)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D88" t="s">
@@ -12966,7 +12967,7 @@
         <v>517</v>
       </c>
       <c r="C89" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B89)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D89" t="s">
@@ -12997,7 +12998,7 @@
         <v>517</v>
       </c>
       <c r="C90" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B90)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D90" t="s">
@@ -13028,7 +13029,7 @@
         <v>517</v>
       </c>
       <c r="C91" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B91)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D91" t="s">
@@ -13059,7 +13060,7 @@
         <v>173</v>
       </c>
       <c r="C92" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B92)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D92" t="s">
@@ -13090,7 +13091,7 @@
         <v>585</v>
       </c>
       <c r="C93" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B93)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D93" t="s">
@@ -13118,10 +13119,10 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="C94" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B94)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="D94" t="s">
@@ -13155,7 +13156,7 @@
         <v>585</v>
       </c>
       <c r="C95" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B95)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D95" t="s">
@@ -13183,10 +13184,10 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="C96" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B96)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="D96" s="16" t="s">
@@ -13220,7 +13221,7 @@
         <v>585</v>
       </c>
       <c r="C97" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B97)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D97" s="16" t="s">
@@ -13248,10 +13249,10 @@
         <v>97</v>
       </c>
       <c r="B98" s="16" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C98" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B98)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</v>
       </c>
       <c r="D98" s="16" t="s">
@@ -13266,10 +13267,10 @@
       </c>
       <c r="H98" s="16"/>
       <c r="I98" s="4" t="s">
+        <v>629</v>
+      </c>
+      <c r="J98" s="4" t="s">
         <v>630</v>
-      </c>
-      <c r="J98" s="4" t="s">
-        <v>631</v>
       </c>
       <c r="K98" t="str">
         <f>"Fetches a bundle of all "&amp;B98&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed))."</f>
@@ -13281,10 +13282,10 @@
         <v>98</v>
       </c>
       <c r="B99" s="16" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C99" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B99)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</v>
       </c>
       <c r="D99" s="16" t="s">
@@ -13299,10 +13300,10 @@
       </c>
       <c r="H99" s="16"/>
       <c r="I99" s="4" t="s">
+        <v>631</v>
+      </c>
+      <c r="J99" s="4" t="s">
         <v>632</v>
-      </c>
-      <c r="J99" s="4" t="s">
-        <v>633</v>
       </c>
       <c r="K99" t="str">
         <f>"Fetches a bundle of all "&amp;B99&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed) and type of dispense (e.g., partially dispensed)."</f>
@@ -13314,14 +13315,14 @@
         <v>99</v>
       </c>
       <c r="B100" s="16" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C100" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B100)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationdispense</v>
       </c>
       <c r="D100" s="16" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="E100" s="16"/>
       <c r="F100" s="16" t="s">
@@ -13332,10 +13333,10 @@
       </c>
       <c r="H100" s="16"/>
       <c r="I100" s="4" t="s">
+        <v>634</v>
+      </c>
+      <c r="J100" s="4" t="s">
         <v>635</v>
-      </c>
-      <c r="J100" s="4" t="s">
-        <v>636</v>
       </c>
       <c r="K100" t="str">
         <f>"Fetches a bundle of all "&amp;B99&amp;" resources for the specified patient for a given dispense and date or range"</f>
@@ -13353,19 +13354,19 @@
         <v>512</v>
       </c>
       <c r="D101" s="16" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="E101" s="16"/>
       <c r="F101" s="16" t="s">
         <v>64</v>
       </c>
       <c r="G101" s="16" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H101" s="16"/>
       <c r="I101" s="4"/>
       <c r="J101" s="4" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="K101" t="str">
         <f>"Fetches a bundle of all "&amp;B101&amp;" resources for the specified patient that may match any of the string fields in the name element (including family, give, prefix, suffix, suffix, and/or text)"</f>
@@ -13392,8 +13393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13415,7 +13416,7 @@
         <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -13455,7 +13456,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>602</v>
+        <v>739</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -13463,7 +13464,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -13539,7 +13540,7 @@
         <v>511</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="D2" t="s">
         <v>64</v>
@@ -13547,7 +13548,7 @@
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>507</v>
@@ -13702,7 +13703,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B5" t="s">
         <v>600</v>
@@ -13716,7 +13717,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B6" t="s">
         <v>601</v>
@@ -13730,16 +13731,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>649</v>
+      </c>
+      <c r="B7" t="s">
         <v>650</v>
       </c>
-      <c r="B7" t="s">
-        <v>651</v>
-      </c>
       <c r="D7" t="s">
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -13800,7 +13801,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B12" t="s">
         <v>340</v>
@@ -13884,7 +13885,7 @@
     </row>
     <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B18" t="s">
         <v>580</v>
@@ -13968,16 +13969,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>651</v>
+      </c>
+      <c r="B24" t="s">
         <v>652</v>
       </c>
-      <c r="B24" t="s">
-        <v>653</v>
-      </c>
       <c r="D24" t="s">
         <v>11</v>
       </c>
       <c r="E24" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -13996,10 +13997,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>653</v>
+      </c>
+      <c r="B26" t="s">
         <v>654</v>
-      </c>
-      <c r="B26" t="s">
-        <v>655</v>
       </c>
       <c r="D26" t="s">
         <v>11</v>
@@ -14010,10 +14011,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>655</v>
+      </c>
+      <c r="B27" t="s">
         <v>656</v>
-      </c>
-      <c r="B27" t="s">
-        <v>657</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
@@ -14024,10 +14025,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>657</v>
+      </c>
+      <c r="B28" t="s">
         <v>658</v>
-      </c>
-      <c r="B28" t="s">
-        <v>659</v>
       </c>
       <c r="D28" t="s">
         <v>11</v>
@@ -14038,7 +14039,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="18" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B29" t="s">
         <v>581</v>
@@ -14066,10 +14067,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B31" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="D31" t="s">
         <v>11</v>
@@ -14080,10 +14081,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>703</v>
+      </c>
+      <c r="B32" t="s">
         <v>704</v>
-      </c>
-      <c r="B32" t="s">
-        <v>705</v>
       </c>
       <c r="D32" t="s">
         <v>11</v>
@@ -14094,10 +14095,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>705</v>
+      </c>
+      <c r="B33" t="s">
         <v>706</v>
-      </c>
-      <c r="B33" t="s">
-        <v>707</v>
       </c>
       <c r="D33" t="s">
         <v>11</v>
@@ -14234,10 +14235,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B43" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="D43" t="s">
         <v>11</v>
@@ -14248,10 +14249,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>701</v>
+      </c>
+      <c r="B44" t="s">
         <v>702</v>
-      </c>
-      <c r="B44" t="s">
-        <v>703</v>
       </c>
       <c r="D44" t="s">
         <v>11</v>
@@ -14276,7 +14277,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="18" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B46" t="s">
         <v>583</v>
@@ -14290,10 +14291,10 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B47" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="D47" t="s">
         <v>11</v>
@@ -14321,7 +14322,7 @@
         <v>468</v>
       </c>
       <c r="B49" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D49" t="s">
         <v>11</v>
@@ -14444,21 +14445,21 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B58" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="D58" t="s">
         <v>11</v>
       </c>
       <c r="E58" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B59" t="s">
         <v>584</v>
@@ -14500,16 +14501,16 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>663</v>
+      </c>
+      <c r="B62" t="s">
         <v>664</v>
       </c>
-      <c r="B62" t="s">
+      <c r="D62" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" t="s">
         <v>665</v>
-      </c>
-      <c r="D62" t="s">
-        <v>11</v>
-      </c>
-      <c r="E62" t="s">
-        <v>666</v>
       </c>
     </row>
   </sheetData>
@@ -14635,7 +14636,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="T2" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="U2" t="s">
         <v>64</v>
@@ -14658,7 +14659,7 @@
         <v>465</v>
       </c>
       <c r="T3" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="U3" t="s">
         <v>64</v>
@@ -14678,10 +14679,10 @@
         <v>64</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="T4" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="U4" t="s">
         <v>64</v>
@@ -14707,10 +14708,10 @@
         <v>64</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="T5" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="U5" t="s">
         <v>64</v>
@@ -14724,13 +14725,13 @@
     </row>
     <row r="6" spans="1:25" ht="16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B6" t="s">
         <v>64</v>
       </c>
       <c r="T6" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="U6" t="s">
         <v>64</v>
@@ -14750,10 +14751,10 @@
         <v>64</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="T7" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="U7" t="s">
         <v>64</v>
@@ -14773,10 +14774,10 @@
         <v>64</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="T8" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="U8" t="s">
         <v>64</v>
@@ -14796,10 +14797,10 @@
         <v>64</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="T9" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="U9" t="s">
         <v>64</v>
@@ -14819,10 +14820,10 @@
         <v>64</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="T10" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="U10" t="s">
         <v>64</v>
@@ -14836,16 +14837,16 @@
     </row>
     <row r="11" spans="1:25" ht="35" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>696</v>
+      </c>
+      <c r="B11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="25" t="s">
         <v>697</v>
       </c>
-      <c r="B11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>698</v>
-      </c>
       <c r="T11" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="U11" t="s">
         <v>64</v>
@@ -14861,10 +14862,10 @@
         <v>64</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="T12" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="U12" t="s">
         <v>64</v>
@@ -14878,16 +14879,16 @@
     </row>
     <row r="13" spans="1:25" ht="52" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>698</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="25" t="s">
         <v>699</v>
       </c>
-      <c r="B13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="25" t="s">
-        <v>700</v>
-      </c>
       <c r="T13" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="U13" t="s">
         <v>64</v>
@@ -14903,10 +14904,10 @@
         <v>64</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="T14" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="U14" t="s">
         <v>64</v>
@@ -14926,10 +14927,10 @@
         <v>64</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="T15" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="U15" t="s">
         <v>64</v>
@@ -14939,16 +14940,16 @@
     </row>
     <row r="16" spans="1:25" ht="35" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>688</v>
+      </c>
+      <c r="B16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="25" t="s">
         <v>689</v>
       </c>
-      <c r="B16" t="s">
-        <v>64</v>
-      </c>
-      <c r="C16" s="25" t="s">
-        <v>690</v>
-      </c>
       <c r="T16" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="U16" t="s">
         <v>64</v>
@@ -14967,7 +14968,7 @@
         <v>466</v>
       </c>
       <c r="T17" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="U17" t="s">
         <v>64</v>
@@ -14983,10 +14984,10 @@
         <v>64</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="T18" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="U18" t="s">
         <v>64</v>
@@ -15006,25 +15007,25 @@
     </row>
     <row r="19" spans="1:25" ht="161" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>617</v>
+      </c>
+      <c r="B19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="T19" t="s">
+        <v>687</v>
+      </c>
+      <c r="U19" t="s">
+        <v>64</v>
+      </c>
+      <c r="V19" t="s">
+        <v>64</v>
+      </c>
+      <c r="W19" s="6" t="s">
         <v>618</v>
-      </c>
-      <c r="B19" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>733</v>
-      </c>
-      <c r="T19" t="s">
-        <v>688</v>
-      </c>
-      <c r="U19" t="s">
-        <v>64</v>
-      </c>
-      <c r="V19" t="s">
-        <v>64</v>
-      </c>
-      <c r="W19" s="6" t="s">
-        <v>619</v>
       </c>
       <c r="X19" s="13" t="s">
         <v>424</v>
@@ -15044,7 +15045,7 @@
         <v>467</v>
       </c>
       <c r="T20" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="U20" t="s">
         <v>64</v>
@@ -15070,10 +15071,10 @@
         <v>64</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="T21" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="U21" t="s">
         <v>64</v>
@@ -15093,10 +15094,10 @@
         <v>64</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="T22" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="U22" t="s">
         <v>64</v>
@@ -15112,10 +15113,10 @@
         <v>64</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="T23" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="U23" t="s">
         <v>64</v>
@@ -15135,10 +15136,10 @@
         <v>64</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="T24" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="U24" t="s">
         <v>64</v>
@@ -15154,10 +15155,10 @@
         <v>64</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="T25" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="U25" t="s">
         <v>64</v>
@@ -15179,10 +15180,10 @@
         <v>64</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="T26" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="U26" t="s">
         <v>64</v>
@@ -15202,10 +15203,10 @@
         <v>64</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="T27" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="U27" t="s">
         <v>64</v>
@@ -15213,13 +15214,13 @@
     </row>
     <row r="28" spans="1:25" ht="113" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B28" t="s">
         <v>64</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="X28" s="13"/>
       <c r="Y28" s="13"/>
@@ -15232,7 +15233,7 @@
         <v>64</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="X29" s="13" t="s">
         <v>424</v>
@@ -15249,10 +15250,10 @@
         <v>64</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="T30" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="U30" t="s">
         <v>64</v>
@@ -15272,10 +15273,10 @@
         <v>64</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="T31" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="U31" t="s">
         <v>64</v>
@@ -15289,16 +15290,16 @@
     </row>
     <row r="32" spans="1:25" ht="33" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B32" t="s">
         <v>64</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="T32" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="U32" t="s">
         <v>64</v>
@@ -15397,7 +15398,7 @@
         <v>64</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -15450,7 +15451,7 @@
         <v>346</v>
       </c>
       <c r="F1" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="G1" t="s">
         <v>347</v>
@@ -15468,13 +15469,13 @@
         <v>350</v>
       </c>
       <c r="L1" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="M1" t="s">
         <v>351</v>
       </c>
       <c r="N1" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="O1" t="s">
         <v>352</v>
@@ -15483,13 +15484,13 @@
         <v>353</v>
       </c>
       <c r="Q1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="R1" t="s">
         <v>354</v>
       </c>
       <c r="S1" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="T1" t="s">
         <v>355</v>
@@ -15522,7 +15523,7 @@
         <v>409</v>
       </c>
       <c r="AD1" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="AE1" t="s">
         <v>586</v>
@@ -15537,7 +15538,7 @@
         <v>423</v>
       </c>
       <c r="AI1" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Correct Examples FHIR-46099 Procedure.code should be Procedure.performed FHIR-46037 Spelling errors in US Core Server Capability Statement FHIR-45451 Clarify Role and use of US Core SearchParameters vs FHIR standard SearchParameters FHIR-46036
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{806D6901-D360-034B-B321-E3B69D0ECA54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{883FAFB7-EB4C-7E47-8DCA-C91A7258793A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="65700" yWindow="500" windowWidth="36700" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17800" yWindow="500" windowWidth="36700" windowHeight="28300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
     <sheet name="meta" sheetId="1" r:id="rId2"/>
     <sheet name="igs" sheetId="10" r:id="rId3"/>
     <sheet name="capstatements" sheetId="13" r:id="rId4"/>
-    <sheet name="profiles" sheetId="34" r:id="rId5"/>
+    <sheet name="profiles" sheetId="45" r:id="rId5"/>
     <sheet name="resources" sheetId="35" r:id="rId6"/>
     <sheet name="ops" sheetId="5" r:id="rId7"/>
     <sheet name="interactions" sheetId="6" r:id="rId8"/>
@@ -1519,12 +1519,6 @@
     <t>http://build.fhir.org/ig/HL7/US-Core/package.tgz</t>
   </si>
   <si>
-    <t>* Additional considerations for systems aligning with [HL7 Consolidated (C-CDA)](http://www.hl7.org/implement/standards/product_brief.cfm?product_id=492) Care Plan requirements:
-    - US Core Goal **SHOULD** be present in CarePlan.goal
-    - US Core Condition **SHOULD** be present in CarePlan.addresses
-    - Assement and Plan **MAY** be included as narrative text</t>
-  </si>
-  <si>
     <t>* The  MedicationRequest resource can represent a medication, using an external reference to a Medication resource. If an external Medication Resource is used in a MedicationRequest, then the READ  **SHALL**  be supported.</t>
   </si>
   <si>
@@ -2251,9 +2245,6 @@
     <t>Media</t>
   </si>
   <si>
-    <t>The Media Resource is a Must Suppot referenced resource when using the US Core DiagnosticReport Profile for Report and Note Exchange.</t>
-  </si>
-  <si>
     <t>conf_Media</t>
   </si>
   <si>
@@ -2275,9 +2266,6 @@
     <t>Endpoint</t>
   </si>
   <si>
-    <t>The Media Resource is a Must Suppot referenced resource when using the US Core PracitionerRole Profile.</t>
-  </si>
-  <si>
     <t>HealthcareService</t>
   </si>
   <si>
@@ -2306,9 +2294,6 @@
   </si>
   <si>
     <t>* Due to implementer feedback, some US Core Profiles reference the PractitionerRole resource instead of the US Core PractitionerRole Profile. However the US Core PractitionerRole Profile **SHOULD** be used as the default profile if referenced by another US Core profile.</t>
-  </si>
-  <si>
-    <t>7.0.0</t>
   </si>
   <si>
     <t>_lastUpdated</t>
@@ -2524,6 +2509,21 @@
 - `modifier`
 - `chain`
 For search operations, Clients **SHOULD** use the standard FHIR SearchParameters.</t>
+  </si>
+  <si>
+    <t>8.0.0-ballot</t>
+  </si>
+  <si>
+    <t>The Media Resource is a Must Support referenced resource when using the US Core DiagnosticReport Profile for Report and Note Exchange.</t>
+  </si>
+  <si>
+    <t>* Additional considerations for systems aligning with [HL7 Consolidated (C-CDA)](http://www.hl7.org/implement/standards/product_brief.cfm?product_id=492) Care Plan requirements:
+    - US Core Goal **SHOULD** be present in CarePlan.goal
+    - US Core Condition **SHOULD** be present in CarePlan.addresses
+    - Assessment and Plan **MAY** be included as narrative text</t>
+  </si>
+  <si>
+    <t>The Media Resource is a Must Support referenced resource when using the US Core PractitionerRole Profile.</t>
   </si>
 </sst>
 </file>
@@ -3162,7 +3162,7 @@
         <v>437</v>
       </c>
       <c r="B2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -3194,7 +3194,7 @@
         <v>62</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -3210,12 +3210,12 @@
         <v>444</v>
       </c>
       <c r="B8" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
@@ -3280,7 +3280,7 @@
         <v>39</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>30</v>
@@ -3345,7 +3345,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="C2" t="s">
         <v>50</v>
@@ -3370,7 +3370,7 @@
         <v>52</v>
       </c>
       <c r="L2" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="M2" t="s">
         <v>51</v>
@@ -3392,7 +3392,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="C3" t="s">
         <v>65</v>
@@ -3436,7 +3436,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="C4" t="s">
         <v>62</v>
@@ -3483,7 +3483,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="C5" t="s">
         <v>56</v>
@@ -3527,7 +3527,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="C6" t="s">
         <v>57</v>
@@ -3583,7 +3583,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="C7" t="s">
         <v>54</v>
@@ -3627,7 +3627,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="C8" t="s">
         <v>61</v>
@@ -3683,7 +3683,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
@@ -3878,7 +3878,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="0"/>
@@ -3972,10 +3972,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>619</v>
+      </c>
+      <c r="C15" t="s">
         <v>620</v>
-      </c>
-      <c r="C15" t="s">
-        <v>621</v>
       </c>
       <c r="D15" t="s">
         <v>28</v>
@@ -3984,7 +3984,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
@@ -4038,7 +4038,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="0"/>
@@ -4092,7 +4092,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
@@ -4150,7 +4150,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="0"/>
@@ -4461,7 +4461,7 @@
         <v>78</v>
       </c>
       <c r="C24" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="D24" t="s">
         <v>28</v>
@@ -4483,19 +4483,19 @@
         <v>52</v>
       </c>
       <c r="L24" t="s">
+        <v>611</v>
+      </c>
+      <c r="M24" t="s">
+        <v>51</v>
+      </c>
+      <c r="O24" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y24" s="4" t="s">
         <v>612</v>
       </c>
-      <c r="M24" t="s">
-        <v>51</v>
-      </c>
-      <c r="O24" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y24" s="4" t="s">
+      <c r="Z24" t="s">
         <v>613</v>
-      </c>
-      <c r="Z24" t="s">
-        <v>614</v>
       </c>
       <c r="AA24" s="8" t="str">
         <f>"Fetches a bundle of all "&amp;B24&amp;" resources matching the name"</f>
@@ -4511,10 +4511,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="C25" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="D25" t="s">
         <v>28</v>
@@ -4523,7 +4523,7 @@
         <v>0</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" si="0"/>
@@ -4539,16 +4539,16 @@
         <v>52</v>
       </c>
       <c r="L25" t="s">
+        <v>644</v>
+      </c>
+      <c r="M25" t="s">
+        <v>51</v>
+      </c>
+      <c r="O25" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y25" s="19" t="s">
         <v>645</v>
-      </c>
-      <c r="M25" t="s">
-        <v>51</v>
-      </c>
-      <c r="O25" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y25" s="19" t="s">
-        <v>646</v>
       </c>
       <c r="AB25" t="str">
         <f t="shared" si="1"/>
@@ -4572,7 +4572,7 @@
         <v>0</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="0"/>
@@ -4621,7 +4621,7 @@
         <v>1</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" si="0"/>
@@ -4679,7 +4679,7 @@
         <v>0</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" si="0"/>
@@ -4729,7 +4729,7 @@
         <v>0</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="0"/>
@@ -4783,7 +4783,7 @@
         <v>0</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G30" t="str">
         <f t="shared" si="0"/>
@@ -4842,7 +4842,7 @@
         <v>0</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G31" t="str">
         <f t="shared" si="0"/>
@@ -4895,7 +4895,7 @@
         <v>0</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G32" t="str">
         <f t="shared" si="0"/>
@@ -4921,7 +4921,7 @@
         <v>51</v>
       </c>
       <c r="X32" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="Y32" t="str">
         <f>"support searching for all "&amp;LOWER(B32)&amp;"s for a patient"</f>
@@ -4948,7 +4948,7 @@
         <v>236</v>
       </c>
       <c r="C33" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D33" t="s">
         <v>64</v>
@@ -4957,7 +4957,7 @@
         <v>0</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G33" t="str">
         <f t="shared" si="0"/>
@@ -4986,7 +4986,7 @@
         <v>51</v>
       </c>
       <c r="Y33" s="4" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Z33" s="4" t="str">
         <f>"GET [base]/"&amp;B33&amp;"?"&amp;C33&amp;"=http://snomed.info/sct\|17561000"</f>
@@ -5015,7 +5015,7 @@
         <v>0</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G34" t="str">
         <f t="shared" si="0"/>
@@ -5059,7 +5059,7 @@
         <v>131</v>
       </c>
       <c r="C35" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D35" t="s">
         <v>28</v>
@@ -5068,7 +5068,7 @@
         <v>0</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G35" t="str">
         <f t="shared" si="0"/>
@@ -5113,7 +5113,7 @@
         <v>131</v>
       </c>
       <c r="C36" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D36" t="s">
         <v>28</v>
@@ -5122,7 +5122,7 @@
         <v>0</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G36" t="str">
         <f t="shared" si="0"/>
@@ -5176,7 +5176,7 @@
         <v>0</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G37" t="str">
         <f t="shared" si="0"/>
@@ -5226,7 +5226,7 @@
         <v>0</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G38" t="str">
         <f t="shared" si="0"/>
@@ -5274,7 +5274,7 @@
         <v>0</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G39" t="str">
         <f t="shared" si="0"/>
@@ -5324,7 +5324,7 @@
         <v>0</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G40" t="str">
         <f t="shared" si="0"/>
@@ -5350,7 +5350,7 @@
         <v>51</v>
       </c>
       <c r="Y40" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z40" s="4" t="str">
         <f>"GET [base]/"&amp;B40&amp;"?patient=1137192"</f>
@@ -5382,7 +5382,7 @@
         <v>0</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G41" t="str">
         <f t="shared" si="0"/>
@@ -5436,7 +5436,7 @@
         <v>1</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G42" t="str">
         <f t="shared" si="0"/>
@@ -5485,7 +5485,7 @@
         <v>131</v>
       </c>
       <c r="C43" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D43" t="s">
         <v>28</v>
@@ -5494,7 +5494,7 @@
         <v>0</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G43" t="str">
         <f t="shared" si="0"/>
@@ -5539,7 +5539,7 @@
         <v>131</v>
       </c>
       <c r="C44" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="D44" t="s">
         <v>28</v>
@@ -5548,7 +5548,7 @@
         <v>0</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="G44" t="str">
         <f t="shared" si="0"/>
@@ -5590,7 +5590,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C45" t="s">
         <v>83</v>
@@ -5602,7 +5602,7 @@
         <v>1</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G45" t="str">
         <f t="shared" si="0"/>
@@ -5628,7 +5628,7 @@
         <v>51</v>
       </c>
       <c r="Y45" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="Z45" s="4" t="str">
         <f>"GET [base]/"&amp;B45&amp;"?patient=1137192"</f>
@@ -5660,7 +5660,7 @@
         <v>1</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G46" t="str">
         <f t="shared" si="0"/>
@@ -5719,7 +5719,7 @@
         <v>0</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G47" t="str">
         <f t="shared" si="0"/>
@@ -5771,7 +5771,7 @@
         <v>0</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G48" t="str">
         <f t="shared" si="0"/>
@@ -5820,7 +5820,7 @@
         <v>0</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G49" t="str">
         <f t="shared" si="0"/>
@@ -5870,7 +5870,7 @@
         <v>0</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G50" t="str">
         <f t="shared" si="0"/>
@@ -5923,7 +5923,7 @@
         <v>0</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G51" t="str">
         <f t="shared" si="0"/>
@@ -5968,7 +5968,7 @@
         <v>172</v>
       </c>
       <c r="C52" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="D52" t="s">
         <v>28</v>
@@ -5977,7 +5977,7 @@
         <v>0</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="G52" t="str">
         <f t="shared" si="0"/>
@@ -6031,7 +6031,7 @@
         <v>1</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G53" t="str">
         <f t="shared" si="0"/>
@@ -6090,7 +6090,7 @@
         <v>0</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G54" t="str">
         <f t="shared" si="0"/>
@@ -6197,7 +6197,7 @@
         <v>0</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G56" t="str">
         <f t="shared" si="0"/>
@@ -6247,7 +6247,7 @@
         <v>0</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G57" t="str">
         <f t="shared" si="0"/>
@@ -6301,7 +6301,7 @@
         <v>1</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G58" t="str">
         <f t="shared" si="0"/>
@@ -6360,7 +6360,7 @@
         <v>0</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G59" t="str">
         <f t="shared" si="0"/>
@@ -6413,7 +6413,7 @@
         <v>0</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G60" t="str">
         <f t="shared" si="0"/>
@@ -6466,7 +6466,7 @@
         <v>0</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G61" t="str">
         <f t="shared" si="0"/>
@@ -6570,7 +6570,7 @@
         <v>0</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G63" t="str">
         <f t="shared" si="0"/>
@@ -6620,7 +6620,7 @@
         <v>0</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G64" t="str">
         <f t="shared" si="0"/>
@@ -6665,7 +6665,7 @@
         <v>20</v>
       </c>
       <c r="C65" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="D65" t="s">
         <v>28</v>
@@ -6674,7 +6674,7 @@
         <v>0</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="G65" t="str">
         <f t="shared" si="0"/>
@@ -6719,7 +6719,7 @@
         <v>20</v>
       </c>
       <c r="C66" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D66" t="s">
         <v>28</v>
@@ -6728,7 +6728,7 @@
         <v>0</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G66" t="str">
         <f t="shared" ref="G66:G129" si="6">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B66)</f>
@@ -6778,7 +6778,7 @@
         <v>1</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G67" t="str">
         <f t="shared" si="6"/>
@@ -6826,7 +6826,7 @@
         <v>20</v>
       </c>
       <c r="C68" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D68" t="s">
         <v>28</v>
@@ -6835,7 +6835,7 @@
         <v>0</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G68" t="str">
         <f t="shared" si="6"/>
@@ -6893,7 +6893,7 @@
         <v>1</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G69" t="str">
         <f t="shared" si="6"/>
@@ -6951,7 +6951,7 @@
         <v>0</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G70" t="str">
         <f t="shared" si="6"/>
@@ -7001,7 +7001,7 @@
         <v>0</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G71" t="str">
         <f t="shared" si="6"/>
@@ -7097,7 +7097,7 @@
         <v>0</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G73" t="str">
         <f t="shared" si="6"/>
@@ -7147,7 +7147,7 @@
         <v>1</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G74" t="str">
         <f t="shared" si="6"/>
@@ -7206,7 +7206,7 @@
         <v>0</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="G75" t="str">
         <f t="shared" si="6"/>
@@ -7260,7 +7260,7 @@
         <v>0</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G76" t="str">
         <f t="shared" si="6"/>
@@ -7314,7 +7314,7 @@
         <v>1</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G77" t="str">
         <f t="shared" si="6"/>
@@ -7373,7 +7373,7 @@
         <v>0</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G78" t="str">
         <f t="shared" si="6"/>
@@ -7685,7 +7685,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C84" t="s">
         <v>83</v>
@@ -7697,7 +7697,7 @@
         <v>1</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G84" t="str">
         <f t="shared" si="6"/>
@@ -7723,10 +7723,10 @@
         <v>51</v>
       </c>
       <c r="X84" s="6" t="s">
+        <v>617</v>
+      </c>
+      <c r="Z84" s="8" t="s">
         <v>618</v>
-      </c>
-      <c r="Z84" s="8" t="s">
-        <v>619</v>
       </c>
       <c r="AA84" s="8" t="str">
         <f>"Fetches a bundle of all "&amp;B84&amp; " resources for the specified patient."</f>
@@ -7742,7 +7742,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C85" t="s">
         <v>56</v>
@@ -7754,7 +7754,7 @@
         <v>0</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G85" t="str">
         <f t="shared" si="6"/>
@@ -7795,7 +7795,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C86" t="s">
         <v>12</v>
@@ -7807,7 +7807,7 @@
         <v>0</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G86" t="str">
         <f t="shared" si="6"/>
@@ -7860,7 +7860,7 @@
         <v>0</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G87" t="str">
         <f t="shared" si="6"/>
@@ -7914,7 +7914,7 @@
         <v>0</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G88" t="str">
         <f t="shared" si="6"/>
@@ -7965,7 +7965,7 @@
         <v>0</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G89" t="str">
         <f t="shared" si="6"/>
@@ -8018,7 +8018,7 @@
         <v>0</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G90" t="str">
         <f t="shared" si="6"/>
@@ -8071,7 +8071,7 @@
         <v>0</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G91" t="str">
         <f t="shared" si="6"/>
@@ -8124,7 +8124,7 @@
         <v>0</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G92" t="str">
         <f t="shared" si="6"/>
@@ -8174,7 +8174,7 @@
         <v>0</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G93" t="str">
         <f t="shared" si="6"/>
@@ -8227,7 +8227,7 @@
         <v>0</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G94" t="str">
         <f t="shared" si="6"/>
@@ -8272,7 +8272,7 @@
         <v>176</v>
       </c>
       <c r="C95" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="D95" t="s">
         <v>28</v>
@@ -8281,7 +8281,7 @@
         <v>0</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="G95" t="str">
         <f t="shared" si="6"/>
@@ -8335,7 +8335,7 @@
         <v>0</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G96" t="str">
         <f t="shared" si="6"/>
@@ -8394,7 +8394,7 @@
         <v>0</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G97" t="str">
         <f t="shared" si="6"/>
@@ -8608,7 +8608,7 @@
         <v>0</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="G101" t="str">
         <f t="shared" si="6"/>
@@ -8646,7 +8646,7 @@
         <v>19</v>
       </c>
       <c r="C102" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="D102" t="s">
         <v>28</v>
@@ -8655,7 +8655,7 @@
         <v>0</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="G102" t="str">
         <f t="shared" si="6"/>
@@ -8702,7 +8702,7 @@
         <v>0</v>
       </c>
       <c r="F103" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="G103" t="str">
         <f t="shared" si="6"/>
@@ -8748,7 +8748,7 @@
         <v>0</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G104" t="str">
         <f t="shared" si="6"/>
@@ -8840,7 +8840,7 @@
         <v>1</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G106" t="str">
         <f t="shared" si="6"/>
@@ -8920,7 +8920,7 @@
         <v>51</v>
       </c>
       <c r="Y107" s="4" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="Z107" t="s">
         <v>166</v>
@@ -9004,7 +9004,7 @@
         <v>1</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G109" t="str">
         <f t="shared" si="6"/>
@@ -9117,7 +9117,7 @@
         <v>1</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G111" t="str">
         <f t="shared" si="6"/>
@@ -9181,7 +9181,7 @@
         <v>1</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G112" t="str">
         <f t="shared" si="6"/>
@@ -9242,7 +9242,7 @@
         <v>0</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G113" t="str">
         <f t="shared" si="6"/>
@@ -9295,7 +9295,7 @@
         <v>0</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G114" t="str">
         <f t="shared" si="6"/>
@@ -9349,7 +9349,7 @@
         <v>1</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G115" t="str">
         <f t="shared" si="6"/>
@@ -9407,7 +9407,7 @@
         <v>0</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G116" t="str">
         <f t="shared" si="6"/>
@@ -9448,7 +9448,7 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C117" t="s">
         <v>50</v>
@@ -9487,7 +9487,7 @@
         <v>support both read QuestionnaireResponse by `id` **AND** QuestionnaireResponse search</v>
       </c>
       <c r="Z117" s="4" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="AB117" t="str">
         <f t="shared" si="4"/>
@@ -9499,10 +9499,10 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C118" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D118" t="s">
         <v>28</v>
@@ -9511,7 +9511,7 @@
         <v>0</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G118" t="str">
         <f t="shared" si="6"/>
@@ -9543,7 +9543,7 @@
         <v>86</v>
       </c>
       <c r="Y118" s="19" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="AB118" t="str">
         <f t="shared" si="4"/>
@@ -9555,7 +9555,7 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C119" t="s">
         <v>83</v>
@@ -9567,7 +9567,7 @@
         <v>1</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G119" t="str">
         <f t="shared" si="6"/>
@@ -9614,10 +9614,10 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C120" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D120" t="s">
         <v>28</v>
@@ -9626,7 +9626,7 @@
         <v>0</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G120" t="str">
         <f t="shared" si="6"/>
@@ -9652,7 +9652,7 @@
         <v>51</v>
       </c>
       <c r="Y120" s="19" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="AB120" t="str">
         <f t="shared" si="4"/>
@@ -9664,7 +9664,7 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C121" t="s">
         <v>56</v>
@@ -9676,7 +9676,7 @@
         <v>0</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G121" t="str">
         <f t="shared" si="6"/>
@@ -9705,7 +9705,7 @@
         <v>51</v>
       </c>
       <c r="Y121" s="19" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="AB121" t="str">
         <f t="shared" si="4"/>
@@ -9717,7 +9717,7 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C122" t="s">
         <v>50</v>
@@ -9756,7 +9756,7 @@
         <v>support both read RelatedPerson by `id` **AND** RelatedPerson search</v>
       </c>
       <c r="Z122" s="4" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="AA122" s="8"/>
       <c r="AB122" t="str">
@@ -9769,7 +9769,7 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C123" t="s">
         <v>21</v>
@@ -9804,7 +9804,7 @@
         <v>51</v>
       </c>
       <c r="Y123" s="4" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="Z123" s="4" t="str">
         <f>"GET [base]/"&amp;B123&amp;"?"&amp;C123&amp;"=Mary Shaw"</f>
@@ -9824,7 +9824,7 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C124" t="s">
         <v>83</v>
@@ -9836,7 +9836,7 @@
         <v>1</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G124" t="str">
         <f t="shared" si="6"/>
@@ -9883,7 +9883,7 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C125" t="s">
         <v>50</v>
@@ -9922,7 +9922,7 @@
         <v>support both read ServiceRequest by `id` **AND** ServiceRequest search</v>
       </c>
       <c r="Z125" s="4" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="AB125" t="str">
         <f t="shared" si="8"/>
@@ -9934,10 +9934,10 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C126" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D126" t="s">
         <v>28</v>
@@ -9946,7 +9946,7 @@
         <v>0</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G126" t="str">
         <f t="shared" si="6"/>
@@ -9988,7 +9988,7 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C127" t="s">
         <v>133</v>
@@ -10000,7 +10000,7 @@
         <v>0</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G127" t="str">
         <f t="shared" si="6"/>
@@ -10038,7 +10038,7 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C128" t="s">
         <v>24</v>
@@ -10050,7 +10050,7 @@
         <v>0</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G128" t="str">
         <f t="shared" si="6"/>
@@ -10091,7 +10091,7 @@
         <v>128</v>
       </c>
       <c r="B129" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C129" t="s">
         <v>83</v>
@@ -10103,7 +10103,7 @@
         <v>1</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G129" t="str">
         <f t="shared" si="6"/>
@@ -10150,7 +10150,7 @@
         <v>129</v>
       </c>
       <c r="B130" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C130" t="s">
         <v>56</v>
@@ -10162,7 +10162,7 @@
         <v>0</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G130" t="str">
         <f t="shared" ref="G130:G132" si="9">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B130)</f>
@@ -10203,7 +10203,7 @@
         <v>130</v>
       </c>
       <c r="B131" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C131" t="s">
         <v>50</v>
@@ -10255,7 +10255,7 @@
         <v>131</v>
       </c>
       <c r="B132" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C132" t="s">
         <v>83</v>
@@ -10314,7 +10314,7 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10363,7 +10363,7 @@
         <v>89</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>90</v>
@@ -10693,7 +10693,7 @@
         <v>283</v>
       </c>
       <c r="J13" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="K13" s="4" t="str">
         <f t="shared" si="1"/>
@@ -10793,7 +10793,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D17" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="F17" t="s">
         <v>64</v>
@@ -10805,7 +10805,7 @@
         <v>284</v>
       </c>
       <c r="J17" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="K17" s="4" t="str">
         <f t="shared" si="1"/>
@@ -10824,7 +10824,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D18" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
       <c r="F18" t="s">
         <v>64</v>
@@ -10834,7 +10834,7 @@
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="27" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
       <c r="K18" s="24" t="str">
         <f>"Fetches a bundle of all "&amp;B18&amp;" resources for the specified "&amp;SUBSTITUTE(D18,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
@@ -10910,7 +10910,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D21" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F21" t="s">
         <v>64</v>
@@ -10922,7 +10922,7 @@
         <v>289</v>
       </c>
       <c r="J21" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="K21" s="4" t="str">
         <f t="shared" si="2"/>
@@ -11232,7 +11232,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D33" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="F33" t="s">
         <v>64</v>
@@ -11241,10 +11241,10 @@
         <v>127</v>
       </c>
       <c r="I33" s="4" t="s">
+        <v>622</v>
+      </c>
+      <c r="J33" s="4" t="s">
         <v>623</v>
-      </c>
-      <c r="J33" s="4" t="s">
-        <v>624</v>
       </c>
       <c r="K33" s="4" t="str">
         <f t="shared" si="2"/>
@@ -11374,7 +11374,7 @@
         <v>306</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
@@ -11419,7 +11419,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D39" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="F39" t="s">
         <v>64</v>
@@ -11431,13 +11431,13 @@
         <v>389</v>
       </c>
       <c r="I39" s="4" t="s">
+        <v>683</v>
+      </c>
+      <c r="J39" s="24" t="s">
         <v>684</v>
       </c>
-      <c r="J39" s="24" t="s">
+      <c r="K39" s="4" t="s">
         <v>685</v>
-      </c>
-      <c r="K39" s="4" t="s">
-        <v>686</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
@@ -11452,7 +11452,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D40" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="F40" t="s">
         <v>64</v>
@@ -11464,10 +11464,10 @@
         <v>143</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
@@ -11524,7 +11524,7 @@
         <v>146</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="K42" s="4" t="s">
         <v>149</v>
@@ -11542,7 +11542,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D43" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="F43" t="s">
         <v>64</v>
@@ -11554,7 +11554,7 @@
         <v>146</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="K43" s="4" t="s">
         <v>149</v>
@@ -11572,7 +11572,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D44" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="F44" t="s">
         <v>64</v>
@@ -11584,7 +11584,7 @@
         <v>146</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="K44" s="4" t="s">
         <v>149</v>
@@ -11602,7 +11602,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D45" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="F45" t="s">
         <v>64</v>
@@ -11614,7 +11614,7 @@
         <v>146</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="K45" s="4" t="s">
         <v>149</v>
@@ -11632,7 +11632,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D46" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
       <c r="F46" t="s">
         <v>64</v>
@@ -11642,7 +11642,7 @@
       </c>
       <c r="I46" s="4"/>
       <c r="J46" s="24" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
       <c r="K46" s="24" t="str">
         <f>"Fetches a bundle of all "&amp;B46&amp;" resources for the specified "&amp;SUBSTITUTE(D46,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
@@ -11703,7 +11703,7 @@
         <v>160</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="K48" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B48&amp;" resources for the specified "&amp;SUBSTITUTE(D48,","," and ")</f>
@@ -11749,7 +11749,7 @@
         <v>172</v>
       </c>
       <c r="C50" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="D50" t="s">
         <v>109</v>
@@ -11779,7 +11779,7 @@
         <v>172</v>
       </c>
       <c r="C51" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="D51" t="s">
         <v>138</v>
@@ -11812,7 +11812,7 @@
         <v>172</v>
       </c>
       <c r="C52" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="D52" t="s">
         <v>140</v>
@@ -11842,7 +11842,7 @@
         <v>172</v>
       </c>
       <c r="C53" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="D53" t="s">
         <v>187</v>
@@ -11860,7 +11860,7 @@
         <v>188</v>
       </c>
       <c r="J53" s="7" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="K53" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B53&amp;" resources for the specified patient and date and a category code = `LAB`"</f>
@@ -11879,7 +11879,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-diagnosticreport</v>
       </c>
       <c r="D54" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
       <c r="F54" t="s">
         <v>64</v>
@@ -11889,7 +11889,7 @@
       </c>
       <c r="I54" s="4"/>
       <c r="J54" s="27" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="K54" s="24" t="str">
         <f>"Fetches a bundle of all "&amp;B54&amp;" resources for the specified "&amp;SUBSTITUTE(D54,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
@@ -11904,7 +11904,7 @@
         <v>172</v>
       </c>
       <c r="C55" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="D55" t="s">
         <v>208</v>
@@ -11919,7 +11919,7 @@
         <v>214</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K55" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B55&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
@@ -12114,7 +12114,7 @@
         <v>218</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="K61" s="4" t="s">
         <v>435</v>
@@ -12267,7 +12267,7 @@
         <v>215</v>
       </c>
       <c r="J66" s="4" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="K66" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B66&amp;" resources for the specified patient and date and procedure code(s).  SHOULD support search by multiple codes."</f>
@@ -12282,7 +12282,7 @@
         <v>176</v>
       </c>
       <c r="C67" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="D67" t="s">
         <v>225</v>
@@ -12300,7 +12300,7 @@
         <v>264</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="K67" s="4" t="s">
         <v>299</v>
@@ -12314,7 +12314,7 @@
         <v>176</v>
       </c>
       <c r="C68" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="D68" t="s">
         <v>138</v>
@@ -12332,7 +12332,7 @@
         <v>209</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="K68" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B68&amp;" resources for the specified patient and a category code = `laboratory`"</f>
@@ -12347,7 +12347,7 @@
         <v>176</v>
       </c>
       <c r="C69" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="D69" t="s">
         <v>140</v>
@@ -12362,7 +12362,7 @@
         <v>212</v>
       </c>
       <c r="J69" s="8" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="K69" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B69&amp;" resources for the specified patient and observation code(s).  SHOULD support search by multiple report codes. The Observation `code` parameter searches `Observation.code only."</f>
@@ -12377,7 +12377,7 @@
         <v>176</v>
       </c>
       <c r="C70" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="D70" t="s">
         <v>187</v>
@@ -12395,7 +12395,7 @@
         <v>213</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="K70" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B70&amp;" resources for the specified patient and date and a category code = `laboratory`"</f>
@@ -12410,10 +12410,10 @@
         <v>176</v>
       </c>
       <c r="C71" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="D71" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
       <c r="F71" t="s">
         <v>64</v>
@@ -12423,7 +12423,7 @@
       </c>
       <c r="I71" s="4"/>
       <c r="J71" s="27" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="K71" s="24" t="str">
         <f>"Fetches a bundle of all "&amp;B71&amp;" resources for the specified "&amp;SUBSTITUTE(D71,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
@@ -12438,7 +12438,7 @@
         <v>176</v>
       </c>
       <c r="C72" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="D72" t="s">
         <v>208</v>
@@ -12453,7 +12453,7 @@
         <v>211</v>
       </c>
       <c r="J72" s="4" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
       <c r="K72" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B72&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
@@ -12519,7 +12519,7 @@
         <v>229</v>
       </c>
       <c r="J74" s="4" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="K74" s="4" t="s">
         <v>233</v>
@@ -12583,7 +12583,7 @@
         <v>228</v>
       </c>
       <c r="J76" s="4" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="K76" s="4" t="s">
         <v>235</v>
@@ -12613,13 +12613,13 @@
         <v>290</v>
       </c>
       <c r="I77" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="J77" s="4" t="s">
         <v>548</v>
       </c>
-      <c r="J77" s="4" t="s">
+      <c r="K77" s="8" t="s">
         <v>549</v>
-      </c>
-      <c r="K77" s="8" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
@@ -12742,7 +12742,7 @@
         <v>275</v>
       </c>
       <c r="J81" s="7" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="K81" s="4" t="s">
         <v>277</v>
@@ -12802,7 +12802,7 @@
         <v>280</v>
       </c>
       <c r="J83" s="4" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="K83" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B83&amp;" resources for the specified "&amp;SUBSTITUTE(D83,","," and ") &amp;". See the implementation notes above for how to access the actual document."</f>
@@ -12817,7 +12817,7 @@
         <v>237</v>
       </c>
       <c r="C84" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="D84" t="s">
         <v>111</v>
@@ -12846,7 +12846,7 @@
         <v>237</v>
       </c>
       <c r="C85" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="D85" t="s">
         <v>109</v>
@@ -12858,13 +12858,13 @@
         <v>99</v>
       </c>
       <c r="I85" s="4" t="s">
+        <v>625</v>
+      </c>
+      <c r="J85" s="4" t="s">
         <v>626</v>
       </c>
-      <c r="J85" s="4" t="s">
+      <c r="K85" s="4" t="s">
         <v>627</v>
-      </c>
-      <c r="K85" s="4" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
@@ -12879,7 +12879,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
       </c>
       <c r="D86" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F86" t="s">
         <v>64</v>
@@ -12888,13 +12888,13 @@
         <v>99</v>
       </c>
       <c r="I86" s="4" t="s">
+        <v>551</v>
+      </c>
+      <c r="J86" s="4" t="s">
         <v>552</v>
       </c>
-      <c r="J86" s="4" t="s">
+      <c r="K86" s="4" t="s">
         <v>553</v>
-      </c>
-      <c r="K86" s="4" t="s">
-        <v>554</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.2">
@@ -12902,7 +12902,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C87" t="str">
         <f t="shared" si="5"/>
@@ -12921,7 +12921,7 @@
         <v>282</v>
       </c>
       <c r="J87" s="4" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="K87" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B87&amp;" resources for the specified "&amp;SUBSTITUTE(D87,","," and ")</f>
@@ -12933,7 +12933,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C88" t="str">
         <f t="shared" si="5"/>
@@ -12952,7 +12952,7 @@
         <v>191</v>
       </c>
       <c r="J88" s="4" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="K88" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B88&amp;" resources for the specified patient and  a category code"</f>
@@ -12964,7 +12964,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C89" t="str">
         <f t="shared" si="5"/>
@@ -12983,7 +12983,7 @@
         <v>192</v>
       </c>
       <c r="J89" s="4" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="K89" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B89&amp;" resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes."</f>
@@ -12995,14 +12995,14 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C90" t="str">
         <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D90" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F90" t="s">
         <v>11</v>
@@ -13014,7 +13014,7 @@
         <v>194</v>
       </c>
       <c r="J90" s="4" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="K90" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B90&amp;" resources for the specified patient and date and a category code"</f>
@@ -13026,14 +13026,14 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C91" t="str">
         <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D91" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="F91" t="s">
         <v>64</v>
@@ -13042,10 +13042,10 @@
         <v>207</v>
       </c>
       <c r="I91" s="4" t="s">
+        <v>560</v>
+      </c>
+      <c r="J91" s="4" t="s">
         <v>561</v>
-      </c>
-      <c r="J91" s="4" t="s">
-        <v>562</v>
       </c>
       <c r="K91" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B91&amp;" resources for the specified patient and date and service code(s).  SHOULD support search by multiple report codes."</f>
@@ -13064,7 +13064,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D92" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="F92" t="s">
         <v>64</v>
@@ -13073,10 +13073,10 @@
         <v>99</v>
       </c>
       <c r="I92" s="4" t="s">
+        <v>563</v>
+      </c>
+      <c r="J92" s="4" t="s">
         <v>564</v>
-      </c>
-      <c r="J92" s="4" t="s">
-        <v>565</v>
       </c>
       <c r="K92" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B92&amp;" resources for the specified "&amp;SUBSTITUTE(D92,","," and ")</f>
@@ -13088,7 +13088,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C93" t="str">
         <f t="shared" si="5"/>
@@ -13104,10 +13104,10 @@
         <v>99</v>
       </c>
       <c r="I93" t="s">
+        <v>588</v>
+      </c>
+      <c r="J93" s="4" t="s">
         <v>589</v>
-      </c>
-      <c r="J93" s="4" t="s">
-        <v>590</v>
       </c>
       <c r="K93" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B93&amp;" resources for the specified "&amp;SUBSTITUTE(D93,","," and ")</f>
@@ -13119,14 +13119,14 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="C94" t="str">
         <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="D94" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="F94" t="s">
         <v>64</v>
@@ -13135,13 +13135,13 @@
         <v>99</v>
       </c>
       <c r="H94" t="s">
+        <v>591</v>
+      </c>
+      <c r="I94" t="s">
+        <v>588</v>
+      </c>
+      <c r="J94" s="4" t="s">
         <v>592</v>
-      </c>
-      <c r="I94" t="s">
-        <v>589</v>
-      </c>
-      <c r="J94" s="4" t="s">
-        <v>593</v>
       </c>
       <c r="K94" t="str">
         <f>"Fetches a bundle of all "&amp;B94&amp;" resources for the specified "&amp;SUBSTITUTE(D94,","," and  ") &amp; "= 'sdoh'"</f>
@@ -13153,14 +13153,14 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C95" t="str">
         <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D95" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="F95" t="s">
         <v>64</v>
@@ -13169,10 +13169,10 @@
         <v>142</v>
       </c>
       <c r="I95" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="J95" s="4" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="K95" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient and date"</f>
@@ -13184,14 +13184,14 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="C96" t="str">
         <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="D96" s="16" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="F96" t="s">
         <v>64</v>
@@ -13200,13 +13200,13 @@
         <v>207</v>
       </c>
       <c r="H96" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I96" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="J96" s="4" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="K96" t="str">
         <f>"Fetches a bundle of all "&amp;B96&amp;" resources tagged as 'sdoh' for the specified patient and date"</f>
@@ -13218,14 +13218,14 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C97" t="str">
         <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D97" s="16" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="F97" t="s">
         <v>64</v>
@@ -13234,10 +13234,10 @@
         <v>84</v>
       </c>
       <c r="I97" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="J97" s="4" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="K97" t="str">
         <f>"Fetches a bundle of all "&amp;B97&amp;" resources for the specified patient that have been completed against a specified form."</f>
@@ -13249,7 +13249,7 @@
         <v>97</v>
       </c>
       <c r="B98" s="16" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C98" t="str">
         <f t="shared" si="5"/>
@@ -13267,10 +13267,10 @@
       </c>
       <c r="H98" s="16"/>
       <c r="I98" s="4" t="s">
+        <v>628</v>
+      </c>
+      <c r="J98" s="4" t="s">
         <v>629</v>
-      </c>
-      <c r="J98" s="4" t="s">
-        <v>630</v>
       </c>
       <c r="K98" t="str">
         <f>"Fetches a bundle of all "&amp;B98&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed))."</f>
@@ -13282,7 +13282,7 @@
         <v>98</v>
       </c>
       <c r="B99" s="16" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C99" t="str">
         <f t="shared" si="5"/>
@@ -13300,10 +13300,10 @@
       </c>
       <c r="H99" s="16"/>
       <c r="I99" s="4" t="s">
+        <v>630</v>
+      </c>
+      <c r="J99" s="4" t="s">
         <v>631</v>
-      </c>
-      <c r="J99" s="4" t="s">
-        <v>632</v>
       </c>
       <c r="K99" t="str">
         <f>"Fetches a bundle of all "&amp;B99&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed) and type of dispense (e.g., partially dispensed)."</f>
@@ -13315,14 +13315,14 @@
         <v>99</v>
       </c>
       <c r="B100" s="16" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C100" t="str">
         <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationdispense</v>
       </c>
       <c r="D100" s="16" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="E100" s="16"/>
       <c r="F100" s="16" t="s">
@@ -13333,10 +13333,10 @@
       </c>
       <c r="H100" s="16"/>
       <c r="I100" s="4" t="s">
+        <v>633</v>
+      </c>
+      <c r="J100" s="4" t="s">
         <v>634</v>
-      </c>
-      <c r="J100" s="4" t="s">
-        <v>635</v>
       </c>
       <c r="K100" t="str">
         <f>"Fetches a bundle of all "&amp;B99&amp;" resources for the specified patient for a given dispense and date or range"</f>
@@ -13348,25 +13348,25 @@
         <v>100</v>
       </c>
       <c r="B101" s="16" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C101" s="22" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D101" s="16" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="E101" s="16"/>
       <c r="F101" s="16" t="s">
         <v>64</v>
       </c>
       <c r="G101" s="16" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="H101" s="16"/>
       <c r="I101" s="4"/>
       <c r="J101" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="K101" t="str">
         <f>"Fetches a bundle of all "&amp;B101&amp;" resources for the specified patient that may match any of the string fields in the name element (including family, give, prefix, suffix, suffix, and/or text)"</f>
@@ -13376,7 +13376,7 @@
   </sheetData>
   <autoFilter ref="A1:K101" xr:uid="{331E0B16-168F-459B-8951-3DF614BF0371}"/>
   <conditionalFormatting sqref="B1:B100 B102:B1048576">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13393,8 +13393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A7" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13413,26 +13413,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>708</v>
+        <v>382</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>427</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>436</v>
+        <v>736</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>427</v>
       </c>
       <c r="B4" t="s">
-        <v>382</v>
+        <v>436</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -13440,7 +13440,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -13451,12 +13451,12 @@
         <v>381</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="241" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="288" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -13464,36 +13464,36 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>488</v>
+      </c>
+      <c r="B9" t="s">
         <v>489</v>
-      </c>
-      <c r="B9" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>490</v>
+      </c>
+      <c r="B10" t="s">
         <v>491</v>
-      </c>
-      <c r="B10" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>492</v>
+      </c>
+      <c r="B11" s="14" t="s">
         <v>493</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B12" t="s">
         <v>64</v>
@@ -13514,6 +13514,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="48.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="71" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="51.1640625" customWidth="1"/>
   </cols>
@@ -13523,7 +13524,7 @@
         <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C1" t="s">
         <v>54</v>
@@ -13534,13 +13535,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="D2" t="s">
         <v>64</v>
@@ -13548,13 +13549,13 @@
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B3" s="21" t="s">
+        <v>506</v>
+      </c>
+      <c r="C3" s="21" t="s">
         <v>507</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>508</v>
       </c>
       <c r="D3" s="21" t="s">
         <v>64</v>
@@ -13587,16 +13588,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>497</v>
+      </c>
+      <c r="B1" t="s">
         <v>498</v>
-      </c>
-      <c r="B1" t="s">
-        <v>499</v>
       </c>
       <c r="C1" t="s">
         <v>21</v>
       </c>
       <c r="D1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E1" t="s">
         <v>54</v>
@@ -13608,13 +13609,13 @@
     <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B2" s="16"/>
       <c r="C2" t="s">
+        <v>499</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>500</v>
       </c>
-      <c r="D2" s="15" t="s">
-        <v>501</v>
-      </c>
       <c r="E2" s="15" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -13626,11 +13627,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CECBDE16-5B3B-D24D-8161-5797A7035D04}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AFD1E51-334E-C94B-9199-BB3C0A09D724}">
   <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D13" sqref="D1:D1048576"/>
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13703,10 +13704,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B5" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
@@ -13717,10 +13718,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B6" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -13731,16 +13732,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>648</v>
+      </c>
+      <c r="B7" t="s">
         <v>649</v>
       </c>
-      <c r="B7" t="s">
-        <v>650</v>
-      </c>
       <c r="D7" t="s">
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -13801,7 +13802,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B12" t="s">
         <v>340</v>
@@ -13815,86 +13816,86 @@
     </row>
     <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
+        <v>568</v>
+      </c>
+      <c r="B13" t="s">
         <v>569</v>
       </c>
-      <c r="B13" t="s">
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
         <v>570</v>
-      </c>
-      <c r="D13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" t="s">
-        <v>571</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
+        <v>571</v>
+      </c>
+      <c r="B14" t="s">
         <v>572</v>
       </c>
-      <c r="B14" t="s">
-        <v>573</v>
-      </c>
       <c r="D14" t="s">
         <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
+        <v>573</v>
+      </c>
+      <c r="B15" t="s">
         <v>574</v>
       </c>
-      <c r="B15" t="s">
-        <v>575</v>
-      </c>
       <c r="D15" t="s">
         <v>11</v>
       </c>
       <c r="E15" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
+        <v>575</v>
+      </c>
+      <c r="B16" t="s">
         <v>576</v>
       </c>
-      <c r="B16" t="s">
-        <v>577</v>
-      </c>
       <c r="D16" t="s">
         <v>11</v>
       </c>
       <c r="E16" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
+        <v>577</v>
+      </c>
+      <c r="B17" t="s">
         <v>578</v>
       </c>
-      <c r="B17" t="s">
-        <v>579</v>
-      </c>
       <c r="D17" t="s">
         <v>11</v>
       </c>
       <c r="E17" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="B18" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D18" t="s">
         <v>11</v>
       </c>
       <c r="E18" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -13969,16 +13970,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>650</v>
+      </c>
+      <c r="B24" t="s">
         <v>651</v>
       </c>
-      <c r="B24" t="s">
-        <v>652</v>
-      </c>
       <c r="D24" t="s">
         <v>11</v>
       </c>
       <c r="E24" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -13997,10 +13998,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>652</v>
+      </c>
+      <c r="B26" t="s">
         <v>653</v>
-      </c>
-      <c r="B26" t="s">
-        <v>654</v>
       </c>
       <c r="D26" t="s">
         <v>11</v>
@@ -14011,10 +14012,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>654</v>
+      </c>
+      <c r="B27" t="s">
         <v>655</v>
-      </c>
-      <c r="B27" t="s">
-        <v>656</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
@@ -14025,10 +14026,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>656</v>
+      </c>
+      <c r="B28" t="s">
         <v>657</v>
-      </c>
-      <c r="B28" t="s">
-        <v>658</v>
       </c>
       <c r="D28" t="s">
         <v>11</v>
@@ -14039,10 +14040,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="18" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B29" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D29" t="s">
         <v>11</v>
@@ -14067,10 +14068,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B31" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="D31" t="s">
         <v>11</v>
@@ -14081,10 +14082,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="B32" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="D32" t="s">
         <v>11</v>
@@ -14095,10 +14096,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="B33" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="D33" t="s">
         <v>11</v>
@@ -14137,10 +14138,10 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="18" t="s">
+        <v>471</v>
+      </c>
+      <c r="B36" t="s">
         <v>472</v>
-      </c>
-      <c r="B36" t="s">
-        <v>473</v>
       </c>
       <c r="D36" t="s">
         <v>11</v>
@@ -14179,10 +14180,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="18" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B39" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="D39" t="s">
         <v>11</v>
@@ -14220,7 +14221,7 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="18" t="s">
+      <c r="A42" t="s">
         <v>450</v>
       </c>
       <c r="B42" t="s">
@@ -14235,10 +14236,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B43" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="D43" t="s">
         <v>11</v>
@@ -14249,10 +14250,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
       <c r="B44" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="D44" t="s">
         <v>11</v>
@@ -14277,10 +14278,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="18" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B46" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D46" t="s">
         <v>11</v>
@@ -14291,10 +14292,10 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B47" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="D47" t="s">
         <v>11</v>
@@ -14305,10 +14306,10 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="18" t="s">
+        <v>469</v>
+      </c>
+      <c r="B48" t="s">
         <v>470</v>
-      </c>
-      <c r="B48" t="s">
-        <v>471</v>
       </c>
       <c r="D48" t="s">
         <v>11</v>
@@ -14319,10 +14320,10 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="18" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B49" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D49" t="s">
         <v>11</v>
@@ -14445,77 +14446,77 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B58" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="D58" t="s">
         <v>11</v>
       </c>
       <c r="E58" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B59" t="s">
+        <v>583</v>
+      </c>
+      <c r="D59" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59" t="s">
         <v>584</v>
-      </c>
-      <c r="D59" t="s">
-        <v>11</v>
-      </c>
-      <c r="E59" t="s">
-        <v>585</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="18" t="s">
+        <v>511</v>
+      </c>
+      <c r="B60" t="s">
         <v>512</v>
       </c>
-      <c r="B60" t="s">
+      <c r="D60" t="s">
+        <v>11</v>
+      </c>
+      <c r="E60" t="s">
         <v>513</v>
-      </c>
-      <c r="D60" t="s">
-        <v>11</v>
-      </c>
-      <c r="E60" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="18" t="s">
+        <v>514</v>
+      </c>
+      <c r="B61" t="s">
         <v>515</v>
       </c>
-      <c r="B61" t="s">
+      <c r="D61" t="s">
+        <v>11</v>
+      </c>
+      <c r="E61" t="s">
         <v>516</v>
-      </c>
-      <c r="D61" t="s">
-        <v>11</v>
-      </c>
-      <c r="E61" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>662</v>
+      </c>
+      <c r="B62" t="s">
         <v>663</v>
       </c>
-      <c r="B62" t="s">
+      <c r="D62" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" t="s">
         <v>664</v>
-      </c>
-      <c r="D62" t="s">
-        <v>11</v>
-      </c>
-      <c r="E62" t="s">
-        <v>665</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14528,8 +14529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{352F3A6C-0DAD-1041-B50E-04478951E07A}">
   <dimension ref="A1:Y69"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14613,16 +14614,16 @@
         <v>380</v>
       </c>
       <c r="V1" s="3" t="s">
+        <v>501</v>
+      </c>
+      <c r="W1" s="3" t="s">
         <v>502</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>503</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>504</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="17" thickTop="1" x14ac:dyDescent="0.25">
@@ -14636,7 +14637,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="T2" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="U2" t="s">
         <v>64</v>
@@ -14656,10 +14657,10 @@
         <v>64</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>465</v>
+        <v>738</v>
       </c>
       <c r="T3" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="U3" t="s">
         <v>64</v>
@@ -14679,19 +14680,19 @@
         <v>64</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
       <c r="T4" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="U4" t="s">
         <v>64</v>
       </c>
       <c r="V4" t="s">
+        <v>517</v>
+      </c>
+      <c r="W4" t="s">
         <v>518</v>
-      </c>
-      <c r="W4" t="s">
-        <v>519</v>
       </c>
       <c r="X4" s="13" t="s">
         <v>424</v>
@@ -14708,10 +14709,10 @@
         <v>64</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
       <c r="T5" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="U5" t="s">
         <v>64</v>
@@ -14725,13 +14726,13 @@
     </row>
     <row r="6" spans="1:25" ht="16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B6" t="s">
         <v>64</v>
       </c>
       <c r="T6" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="U6" t="s">
         <v>64</v>
@@ -14751,10 +14752,10 @@
         <v>64</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="T7" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="U7" t="s">
         <v>64</v>
@@ -14774,10 +14775,10 @@
         <v>64</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
       <c r="T8" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="U8" t="s">
         <v>64</v>
@@ -14797,10 +14798,10 @@
         <v>64</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="T9" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="U9" t="s">
         <v>64</v>
@@ -14820,10 +14821,10 @@
         <v>64</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="T10" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="U10" t="s">
         <v>64</v>
@@ -14837,16 +14838,16 @@
     </row>
     <row r="11" spans="1:25" ht="35" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="B11" t="s">
         <v>64</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>697</v>
+        <v>739</v>
       </c>
       <c r="T11" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="U11" t="s">
         <v>64</v>
@@ -14862,10 +14863,10 @@
         <v>64</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="T12" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="U12" t="s">
         <v>64</v>
@@ -14879,16 +14880,16 @@
     </row>
     <row r="13" spans="1:25" ht="52" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
       <c r="B13" t="s">
         <v>28</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="T13" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="U13" t="s">
         <v>64</v>
@@ -14904,10 +14905,10 @@
         <v>64</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="T14" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="U14" t="s">
         <v>64</v>
@@ -14927,10 +14928,10 @@
         <v>64</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="T15" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="U15" t="s">
         <v>64</v>
@@ -14940,16 +14941,16 @@
     </row>
     <row r="16" spans="1:25" ht="35" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B16" t="s">
         <v>64</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>689</v>
+        <v>737</v>
       </c>
       <c r="T16" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="U16" t="s">
         <v>64</v>
@@ -14965,10 +14966,10 @@
         <v>64</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="T17" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="U17" t="s">
         <v>64</v>
@@ -14984,10 +14985,10 @@
         <v>64</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
       <c r="T18" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="U18" t="s">
         <v>64</v>
@@ -15007,25 +15008,25 @@
     </row>
     <row r="19" spans="1:25" ht="161" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>616</v>
+      </c>
+      <c r="B19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="T19" t="s">
+        <v>686</v>
+      </c>
+      <c r="U19" t="s">
+        <v>64</v>
+      </c>
+      <c r="V19" t="s">
+        <v>64</v>
+      </c>
+      <c r="W19" s="6" t="s">
         <v>617</v>
-      </c>
-      <c r="B19" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>732</v>
-      </c>
-      <c r="T19" t="s">
-        <v>687</v>
-      </c>
-      <c r="U19" t="s">
-        <v>64</v>
-      </c>
-      <c r="V19" t="s">
-        <v>64</v>
-      </c>
-      <c r="W19" s="6" t="s">
-        <v>618</v>
       </c>
       <c r="X19" s="13" t="s">
         <v>424</v>
@@ -15042,10 +15043,10 @@
         <v>64</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="T20" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="U20" t="s">
         <v>64</v>
@@ -15071,10 +15072,10 @@
         <v>64</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="T21" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="U21" t="s">
         <v>64</v>
@@ -15094,10 +15095,10 @@
         <v>64</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="T22" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="U22" t="s">
         <v>64</v>
@@ -15113,10 +15114,10 @@
         <v>64</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="T23" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="U23" t="s">
         <v>64</v>
@@ -15136,10 +15137,10 @@
         <v>64</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
       <c r="T24" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="U24" t="s">
         <v>64</v>
@@ -15155,16 +15156,16 @@
         <v>64</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="T25" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="U25" t="s">
         <v>64</v>
       </c>
       <c r="V25" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="W25" t="s">
         <v>261</v>
@@ -15180,10 +15181,10 @@
         <v>64</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="T26" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="U26" t="s">
         <v>64</v>
@@ -15203,10 +15204,10 @@
         <v>64</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="T27" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="U27" t="s">
         <v>64</v>
@@ -15214,26 +15215,26 @@
     </row>
     <row r="28" spans="1:25" ht="113" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B28" t="s">
         <v>64</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="X28" s="13"/>
       <c r="Y28" s="13"/>
     </row>
     <row r="29" spans="1:25" ht="113" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B29" t="s">
         <v>64</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="X29" s="13" t="s">
         <v>424</v>
@@ -15244,16 +15245,16 @@
     </row>
     <row r="30" spans="1:25" ht="33" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B30" t="s">
         <v>64</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
       <c r="T30" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="U30" t="s">
         <v>64</v>
@@ -15265,18 +15266,18 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:25" ht="225" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" ht="387" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B31" t="s">
         <v>64</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
       <c r="T31" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="U31" t="s">
         <v>64</v>
@@ -15290,16 +15291,16 @@
     </row>
     <row r="32" spans="1:25" ht="33" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B32" t="s">
         <v>64</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="T32" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="U32" t="s">
         <v>64</v>
@@ -15325,7 +15326,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15398,7 +15399,7 @@
         <v>64</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -15451,7 +15452,7 @@
         <v>346</v>
       </c>
       <c r="F1" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="G1" t="s">
         <v>347</v>
@@ -15469,13 +15470,13 @@
         <v>350</v>
       </c>
       <c r="L1" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="M1" t="s">
         <v>351</v>
       </c>
       <c r="N1" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="O1" t="s">
         <v>352</v>
@@ -15484,13 +15485,13 @@
         <v>353</v>
       </c>
       <c r="Q1" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="R1" t="s">
         <v>354</v>
       </c>
       <c r="S1" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="T1" t="s">
         <v>355</v>
@@ -15523,22 +15524,22 @@
         <v>409</v>
       </c>
       <c r="AD1" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="AE1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="AF1" t="s">
+        <v>519</v>
+      </c>
+      <c r="AG1" t="s">
         <v>520</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>521</v>
       </c>
       <c r="AH1" t="s">
         <v>423</v>
       </c>
       <c r="AI1" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Remove resolves declaration from US Core CapabilityStatements [FHIR-48446] Change "status" to "active flag" in US Core RelatedPerson introduction[FHIR-48439] Tighten constraint on name.use to support better patient matching [FHIR-48416] Clarify conformance requirements for structured assessments [FHIR-47139] Replace US Core Discharge Disposition Value Set with equivalent [THO] Value Set [FHIR-47416]
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{883FAFB7-EB4C-7E47-8DCA-C91A7258793A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BEA14C2-A593-C94F-A573-AEF5FB73EED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17800" yWindow="500" windowWidth="36700" windowHeight="28300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -121,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2813" uniqueCount="740">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2755" uniqueCount="739">
   <si>
     <t>Element</t>
   </si>
@@ -2237,9 +2237,6 @@
   </si>
   <si>
     <t>Fetches a bundle of all Condition resources for the specified patient and category for all "active" statuses (active,relapse,remission). This will *exclude* diagnoses and health concerns without a clinicalStatus specified.</t>
-  </si>
-  <si>
-    <t>resolves</t>
   </si>
   <si>
     <t>Media</t>
@@ -5539,7 +5536,7 @@
         <v>131</v>
       </c>
       <c r="C44" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D44" t="s">
         <v>28</v>
@@ -5548,7 +5545,7 @@
         <v>0</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="G44" t="str">
         <f t="shared" si="0"/>
@@ -5968,7 +5965,7 @@
         <v>172</v>
       </c>
       <c r="C52" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D52" t="s">
         <v>28</v>
@@ -5977,7 +5974,7 @@
         <v>0</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="G52" t="str">
         <f t="shared" si="0"/>
@@ -6665,7 +6662,7 @@
         <v>20</v>
       </c>
       <c r="C65" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D65" t="s">
         <v>28</v>
@@ -6674,7 +6671,7 @@
         <v>0</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="G65" t="str">
         <f t="shared" si="0"/>
@@ -8272,7 +8269,7 @@
         <v>176</v>
       </c>
       <c r="C95" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D95" t="s">
         <v>28</v>
@@ -8281,7 +8278,7 @@
         <v>0</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="G95" t="str">
         <f t="shared" si="6"/>
@@ -10314,7 +10311,7 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10824,7 +10821,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D18" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="F18" t="s">
         <v>64</v>
@@ -10834,7 +10831,7 @@
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="27" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="K18" s="24" t="str">
         <f>"Fetches a bundle of all "&amp;B18&amp;" resources for the specified "&amp;SUBSTITUTE(D18,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
@@ -11632,7 +11629,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D46" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="F46" t="s">
         <v>64</v>
@@ -11642,7 +11639,7 @@
       </c>
       <c r="I46" s="4"/>
       <c r="J46" s="24" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="K46" s="24" t="str">
         <f>"Fetches a bundle of all "&amp;B46&amp;" resources for the specified "&amp;SUBSTITUTE(D46,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
@@ -11879,7 +11876,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-diagnosticreport</v>
       </c>
       <c r="D54" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="F54" t="s">
         <v>64</v>
@@ -11889,7 +11886,7 @@
       </c>
       <c r="I54" s="4"/>
       <c r="J54" s="27" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="K54" s="24" t="str">
         <f>"Fetches a bundle of all "&amp;B54&amp;" resources for the specified "&amp;SUBSTITUTE(D54,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
@@ -12300,7 +12297,7 @@
         <v>264</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="K67" s="4" t="s">
         <v>299</v>
@@ -12332,7 +12329,7 @@
         <v>209</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="K68" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B68&amp;" resources for the specified patient and a category code = `laboratory`"</f>
@@ -12362,7 +12359,7 @@
         <v>212</v>
       </c>
       <c r="J69" s="8" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="K69" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B69&amp;" resources for the specified patient and observation code(s).  SHOULD support search by multiple report codes. The Observation `code` parameter searches `Observation.code only."</f>
@@ -12395,7 +12392,7 @@
         <v>213</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="K70" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B70&amp;" resources for the specified patient and date and a category code = `laboratory`"</f>
@@ -12413,7 +12410,7 @@
         <v>637</v>
       </c>
       <c r="D71" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="F71" t="s">
         <v>64</v>
@@ -12423,7 +12420,7 @@
       </c>
       <c r="I71" s="4"/>
       <c r="J71" s="27" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="K71" s="24" t="str">
         <f>"Fetches a bundle of all "&amp;B71&amp;" resources for the specified "&amp;SUBSTITUTE(D71,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
@@ -12453,7 +12450,7 @@
         <v>211</v>
       </c>
       <c r="J72" s="4" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="K72" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B72&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
@@ -13376,7 +13373,7 @@
   </sheetData>
   <autoFilter ref="A1:K101" xr:uid="{331E0B16-168F-459B-8951-3DF614BF0371}"/>
   <conditionalFormatting sqref="B1:B100 B102:B1048576">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13424,7 +13421,7 @@
         <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -13456,7 +13453,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -13886,7 +13883,7 @@
     </row>
     <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="B18" t="s">
         <v>579</v>
@@ -14082,10 +14079,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>699</v>
+      </c>
+      <c r="B32" t="s">
         <v>700</v>
-      </c>
-      <c r="B32" t="s">
-        <v>701</v>
       </c>
       <c r="D32" t="s">
         <v>11</v>
@@ -14096,10 +14093,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>701</v>
+      </c>
+      <c r="B33" t="s">
         <v>702</v>
-      </c>
-      <c r="B33" t="s">
-        <v>703</v>
       </c>
       <c r="D33" t="s">
         <v>11</v>
@@ -14250,10 +14247,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>697</v>
+      </c>
+      <c r="B44" t="s">
         <v>698</v>
-      </c>
-      <c r="B44" t="s">
-        <v>699</v>
       </c>
       <c r="D44" t="s">
         <v>11</v>
@@ -14516,7 +14513,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14529,11 +14526,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{352F3A6C-0DAD-1041-B50E-04478951E07A}">
   <dimension ref="A1:Y69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="U32" sqref="U32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="23" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="36.5" customWidth="1"/>
     <col min="2" max="2" width="25.33203125" customWidth="1"/>
@@ -14549,7 +14546,7 @@
     <col min="22" max="25" width="38.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -14626,7 +14623,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="17" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="23" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -14636,12 +14633,6 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="T2" t="s">
-        <v>686</v>
-      </c>
-      <c r="U2" t="s">
-        <v>64</v>
-      </c>
       <c r="X2" s="13" t="s">
         <v>424</v>
       </c>
@@ -14649,7 +14640,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="81" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>222</v>
       </c>
@@ -14657,13 +14648,7 @@
         <v>64</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>738</v>
-      </c>
-      <c r="T3" t="s">
-        <v>686</v>
-      </c>
-      <c r="U3" t="s">
-        <v>64</v>
+        <v>737</v>
       </c>
       <c r="X3" s="13" t="s">
         <v>424</v>
@@ -14672,7 +14657,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="241" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>236</v>
       </c>
@@ -14680,13 +14665,7 @@
         <v>64</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>726</v>
-      </c>
-      <c r="T4" t="s">
-        <v>686</v>
-      </c>
-      <c r="U4" t="s">
-        <v>64</v>
+        <v>725</v>
       </c>
       <c r="V4" t="s">
         <v>517</v>
@@ -14701,7 +14680,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="193" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>131</v>
       </c>
@@ -14709,13 +14688,7 @@
         <v>64</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="T5" t="s">
-        <v>686</v>
-      </c>
-      <c r="U5" t="s">
-        <v>64</v>
+        <v>730</v>
       </c>
       <c r="X5" s="13" t="s">
         <v>424</v>
@@ -14724,19 +14697,13 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>614</v>
       </c>
       <c r="B6" t="s">
         <v>64</v>
       </c>
-      <c r="T6" t="s">
-        <v>686</v>
-      </c>
-      <c r="U6" t="s">
-        <v>64</v>
-      </c>
       <c r="X6" s="13" t="s">
         <v>424</v>
       </c>
@@ -14744,7 +14711,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="209" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>237</v>
       </c>
@@ -14754,12 +14721,6 @@
       <c r="C7" s="1" t="s">
         <v>602</v>
       </c>
-      <c r="T7" t="s">
-        <v>686</v>
-      </c>
-      <c r="U7" t="s">
-        <v>64</v>
-      </c>
       <c r="X7" s="13" t="s">
         <v>424</v>
       </c>
@@ -14767,7 +14728,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="65" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>172</v>
       </c>
@@ -14775,13 +14736,7 @@
         <v>64</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>732</v>
-      </c>
-      <c r="T8" t="s">
-        <v>686</v>
-      </c>
-      <c r="U8" t="s">
-        <v>64</v>
+        <v>731</v>
       </c>
       <c r="X8" s="13" t="s">
         <v>424</v>
@@ -14790,7 +14745,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="273" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>171</v>
       </c>
@@ -14798,13 +14753,7 @@
         <v>64</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>716</v>
-      </c>
-      <c r="T9" t="s">
-        <v>686</v>
-      </c>
-      <c r="U9" t="s">
-        <v>64</v>
+        <v>715</v>
       </c>
       <c r="X9" s="13" t="s">
         <v>424</v>
@@ -14813,7 +14762,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="241" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -14821,13 +14770,7 @@
         <v>64</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>717</v>
-      </c>
-      <c r="T10" t="s">
-        <v>686</v>
-      </c>
-      <c r="U10" t="s">
-        <v>64</v>
+        <v>716</v>
       </c>
       <c r="X10" s="13" t="s">
         <v>424</v>
@@ -14836,26 +14779,20 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="B11" t="s">
         <v>64</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>739</v>
-      </c>
-      <c r="T11" t="s">
-        <v>686</v>
-      </c>
-      <c r="U11" t="s">
-        <v>64</v>
+        <v>738</v>
       </c>
       <c r="X11" s="13"/>
       <c r="Y11" s="13"/>
     </row>
-    <row r="12" spans="1:25" ht="33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>173</v>
       </c>
@@ -14865,12 +14802,6 @@
       <c r="C12" s="1" t="s">
         <v>675</v>
       </c>
-      <c r="T12" t="s">
-        <v>686</v>
-      </c>
-      <c r="U12" t="s">
-        <v>64</v>
-      </c>
       <c r="X12" s="13" t="s">
         <v>424</v>
       </c>
@@ -14878,26 +14809,20 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="52" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>694</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="25" t="s">
         <v>695</v>
-      </c>
-      <c r="B13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="25" t="s">
-        <v>696</v>
-      </c>
-      <c r="T13" t="s">
-        <v>686</v>
-      </c>
-      <c r="U13" t="s">
-        <v>64</v>
       </c>
       <c r="X13" s="13"/>
       <c r="Y13" s="13"/>
     </row>
-    <row r="14" spans="1:25" ht="33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>154</v>
       </c>
@@ -14907,12 +14832,6 @@
       <c r="C14" s="1" t="s">
         <v>603</v>
       </c>
-      <c r="T14" t="s">
-        <v>686</v>
-      </c>
-      <c r="U14" t="s">
-        <v>64</v>
-      </c>
       <c r="X14" s="13" t="s">
         <v>424</v>
       </c>
@@ -14920,7 +14839,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>238</v>
       </c>
@@ -14928,37 +14847,25 @@
         <v>64</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>718</v>
-      </c>
-      <c r="T15" t="s">
-        <v>686</v>
-      </c>
-      <c r="U15" t="s">
-        <v>64</v>
+        <v>717</v>
       </c>
       <c r="X15" s="13"/>
       <c r="Y15" s="13"/>
     </row>
-    <row r="16" spans="1:25" ht="35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B16" t="s">
         <v>64</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>737</v>
-      </c>
-      <c r="T16" t="s">
-        <v>686</v>
-      </c>
-      <c r="U16" t="s">
-        <v>64</v>
+        <v>736</v>
       </c>
       <c r="X16" s="13"/>
       <c r="Y16" s="13"/>
     </row>
-    <row r="17" spans="1:25" ht="33" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>329</v>
       </c>
@@ -14968,16 +14875,10 @@
       <c r="C17" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="T17" t="s">
-        <v>686</v>
-      </c>
-      <c r="U17" t="s">
-        <v>64</v>
-      </c>
       <c r="X17" s="13"/>
       <c r="Y17" s="13"/>
     </row>
-    <row r="18" spans="1:25" ht="409.6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>174</v>
       </c>
@@ -14985,13 +14886,7 @@
         <v>64</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>727</v>
-      </c>
-      <c r="T18" t="s">
-        <v>686</v>
-      </c>
-      <c r="U18" t="s">
-        <v>64</v>
+        <v>726</v>
       </c>
       <c r="V18" t="s">
         <v>64</v>
@@ -15006,7 +14901,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="161" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>616</v>
       </c>
@@ -15014,13 +14909,7 @@
         <v>64</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>728</v>
-      </c>
-      <c r="T19" t="s">
-        <v>686</v>
-      </c>
-      <c r="U19" t="s">
-        <v>64</v>
+        <v>727</v>
       </c>
       <c r="V19" t="s">
         <v>64</v>
@@ -15035,7 +14924,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="193" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>415</v>
       </c>
@@ -15045,12 +14934,6 @@
       <c r="C20" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="T20" t="s">
-        <v>686</v>
-      </c>
-      <c r="U20" t="s">
-        <v>64</v>
-      </c>
       <c r="V20" t="s">
         <v>64</v>
       </c>
@@ -15064,7 +14947,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="241" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>176</v>
       </c>
@@ -15072,13 +14955,7 @@
         <v>64</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="T21" t="s">
-        <v>686</v>
-      </c>
-      <c r="U21" t="s">
-        <v>64</v>
+        <v>729</v>
       </c>
       <c r="X21" s="13" t="s">
         <v>424</v>
@@ -15087,7 +14964,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="65" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>248</v>
       </c>
@@ -15095,18 +14972,12 @@
         <v>64</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>719</v>
-      </c>
-      <c r="T22" t="s">
-        <v>686</v>
-      </c>
-      <c r="U22" t="s">
-        <v>64</v>
+        <v>718</v>
       </c>
       <c r="X22" s="13"/>
       <c r="Y22" s="13"/>
     </row>
-    <row r="23" spans="1:25" ht="289" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -15114,13 +14985,7 @@
         <v>64</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>720</v>
-      </c>
-      <c r="T23" t="s">
-        <v>686</v>
-      </c>
-      <c r="U23" t="s">
-        <v>64</v>
+        <v>719</v>
       </c>
       <c r="X23" s="13" t="s">
         <v>424</v>
@@ -15129,7 +14994,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:25" ht="129" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>255</v>
       </c>
@@ -15137,18 +15002,12 @@
         <v>64</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>721</v>
-      </c>
-      <c r="T24" t="s">
-        <v>686</v>
-      </c>
-      <c r="U24" t="s">
-        <v>64</v>
+        <v>720</v>
       </c>
       <c r="X24" s="13"/>
       <c r="Y24" s="13"/>
     </row>
-    <row r="25" spans="1:25" ht="49" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>257</v>
       </c>
@@ -15156,13 +15015,7 @@
         <v>64</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>704</v>
-      </c>
-      <c r="T25" t="s">
-        <v>686</v>
-      </c>
-      <c r="U25" t="s">
-        <v>64</v>
+        <v>703</v>
       </c>
       <c r="V25" t="s">
         <v>505</v>
@@ -15173,7 +15026,7 @@
       <c r="X25" s="13"/>
       <c r="Y25" s="13"/>
     </row>
-    <row r="26" spans="1:25" ht="289" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>175</v>
       </c>
@@ -15181,13 +15034,7 @@
         <v>64</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>722</v>
-      </c>
-      <c r="T26" t="s">
-        <v>686</v>
-      </c>
-      <c r="U26" t="s">
-        <v>64</v>
+        <v>721</v>
       </c>
       <c r="X26" s="13" t="s">
         <v>424</v>
@@ -15196,7 +15043,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:25" ht="365" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>408</v>
       </c>
@@ -15206,14 +15053,8 @@
       <c r="C27" s="1" t="s">
         <v>674</v>
       </c>
-      <c r="T27" t="s">
-        <v>686</v>
-      </c>
-      <c r="U27" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="28" spans="1:25" ht="113" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>671</v>
       </c>
@@ -15221,12 +15062,12 @@
         <v>64</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="X28" s="13"/>
       <c r="Y28" s="13"/>
     </row>
-    <row r="29" spans="1:25" ht="113" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>584</v>
       </c>
@@ -15234,7 +15075,7 @@
         <v>64</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="X29" s="13" t="s">
         <v>424</v>
@@ -15243,7 +15084,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:25" ht="33" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>513</v>
       </c>
@@ -15251,13 +15092,7 @@
         <v>64</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>723</v>
-      </c>
-      <c r="T30" t="s">
-        <v>686</v>
-      </c>
-      <c r="U30" t="s">
-        <v>64</v>
+        <v>722</v>
       </c>
       <c r="X30" s="13" t="s">
         <v>424</v>
@@ -15266,7 +15101,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:25" ht="387" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>516</v>
       </c>
@@ -15274,13 +15109,7 @@
         <v>64</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>724</v>
-      </c>
-      <c r="T31" t="s">
-        <v>686</v>
-      </c>
-      <c r="U31" t="s">
-        <v>64</v>
+        <v>723</v>
       </c>
       <c r="X31" s="13" t="s">
         <v>424</v>
@@ -15289,7 +15118,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:25" ht="33" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>664</v>
       </c>
@@ -15297,18 +15126,12 @@
         <v>64</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>725</v>
-      </c>
-      <c r="T32" t="s">
-        <v>686</v>
-      </c>
-      <c r="U32" t="s">
-        <v>64</v>
+        <v>724</v>
       </c>
       <c r="X32" s="13"/>
       <c r="Y32" s="13"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>420</v>
       </c>
@@ -15316,17 +15139,17 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="22:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="66" spans="22:25" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="V66" s="6"/>
       <c r="X66" s="6"/>
       <c r="Y66" s="6"/>
     </row>
-    <row r="69" spans="22:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="69" spans="22:25" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y69" s="6"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15452,7 +15275,7 @@
         <v>346</v>
       </c>
       <c r="F1" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="G1" t="s">
         <v>347</v>
@@ -15470,13 +15293,13 @@
         <v>350</v>
       </c>
       <c r="L1" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="M1" t="s">
         <v>351</v>
       </c>
       <c r="N1" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="O1" t="s">
         <v>352</v>
@@ -15485,13 +15308,13 @@
         <v>353</v>
       </c>
       <c r="Q1" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="R1" t="s">
         <v>354</v>
       </c>
       <c r="S1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="T1" t="s">
         <v>355</v>
@@ -15539,7 +15362,7 @@
         <v>423</v>
       </c>
       <c r="AI1" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Clarify when granular scopes overlap [FHIR-46748] Replace US Core Survey Codes Value Set with [Value Set Authority Center (VSAC)] Value Set and remove Laboratory LOINCs [FHIR-46347] Specify SMART App Launch Version [FHIR-46279]
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BEA14C2-A593-C94F-A573-AEF5FB73EED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0417C5-186F-2848-8558-E4940C979F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17800" yWindow="500" windowWidth="36700" windowHeight="28300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17800" yWindow="500" windowWidth="36700" windowHeight="28300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -1620,9 +1620,6 @@
     <t>canonical</t>
   </si>
   <si>
-    <t>SMART Application Launch Framework Implementation Guide</t>
-  </si>
-  <si>
     <t>imports</t>
   </si>
   <si>
@@ -1660,9 +1657,6 @@
   </si>
   <si>
     <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-sexual-orientation</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/smart-app-launch/ImplementationGuide/hl7.fhir.uv.smart-app-launch</t>
   </si>
   <si>
     <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-relatedperson</t>
@@ -2055,9 +2049,6 @@
   </si>
   <si>
     <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-device</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/smart-app-launch/history.html</t>
   </si>
   <si>
     <t>!!Questionnaire</t>
@@ -2521,6 +2512,15 @@
   </si>
   <si>
     <t>The Media Resource is a Must Support referenced resource when using the US Core PractitionerRole Profile.</t>
+  </si>
+  <si>
+    <t>SMART App Launch 2.0.0</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/smart-app-launch/ImplementationGuide/hl7.fhir.uv.smart-app-launch|2.0.0</t>
+  </si>
+  <si>
+    <t>https://hl7.org/fhir/smart-app-launch/STU2/</t>
   </si>
 </sst>
 </file>
@@ -2696,7 +2696,7 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2739,6 +2739,7 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="3" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -3159,7 +3160,7 @@
         <v>437</v>
       </c>
       <c r="B2" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -3191,7 +3192,7 @@
         <v>62</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -3207,7 +3208,7 @@
         <v>444</v>
       </c>
       <c r="B8" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -3277,7 +3278,7 @@
         <v>39</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>30</v>
@@ -3342,7 +3343,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="C2" t="s">
         <v>50</v>
@@ -3367,7 +3368,7 @@
         <v>52</v>
       </c>
       <c r="L2" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="M2" t="s">
         <v>51</v>
@@ -3389,7 +3390,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="C3" t="s">
         <v>65</v>
@@ -3433,7 +3434,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="C4" t="s">
         <v>62</v>
@@ -3480,7 +3481,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="C5" t="s">
         <v>56</v>
@@ -3524,7 +3525,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="C6" t="s">
         <v>57</v>
@@ -3580,7 +3581,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="C7" t="s">
         <v>54</v>
@@ -3624,7 +3625,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="C8" t="s">
         <v>61</v>
@@ -3969,10 +3970,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="C15" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="D15" t="s">
         <v>28</v>
@@ -4458,7 +4459,7 @@
         <v>78</v>
       </c>
       <c r="C24" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="D24" t="s">
         <v>28</v>
@@ -4480,19 +4481,19 @@
         <v>52</v>
       </c>
       <c r="L24" t="s">
+        <v>609</v>
+      </c>
+      <c r="M24" t="s">
+        <v>51</v>
+      </c>
+      <c r="O24" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y24" s="4" t="s">
+        <v>610</v>
+      </c>
+      <c r="Z24" t="s">
         <v>611</v>
-      </c>
-      <c r="M24" t="s">
-        <v>51</v>
-      </c>
-      <c r="O24" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y24" s="4" t="s">
-        <v>612</v>
-      </c>
-      <c r="Z24" t="s">
-        <v>613</v>
       </c>
       <c r="AA24" s="8" t="str">
         <f>"Fetches a bundle of all "&amp;B24&amp;" resources matching the name"</f>
@@ -4508,10 +4509,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="C25" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="D25" t="s">
         <v>28</v>
@@ -4536,7 +4537,7 @@
         <v>52</v>
       </c>
       <c r="L25" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="M25" t="s">
         <v>51</v>
@@ -4545,7 +4546,7 @@
         <v>51</v>
       </c>
       <c r="Y25" s="19" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="AB25" t="str">
         <f t="shared" si="1"/>
@@ -4918,7 +4919,7 @@
         <v>51</v>
       </c>
       <c r="X32" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="Y32" t="str">
         <f>"support searching for all "&amp;LOWER(B32)&amp;"s for a patient"</f>
@@ -4945,7 +4946,7 @@
         <v>236</v>
       </c>
       <c r="C33" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="D33" t="s">
         <v>64</v>
@@ -4983,7 +4984,7 @@
         <v>51</v>
       </c>
       <c r="Y33" s="4" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="Z33" s="4" t="str">
         <f>"GET [base]/"&amp;B33&amp;"?"&amp;C33&amp;"=http://snomed.info/sct\|17561000"</f>
@@ -5056,7 +5057,7 @@
         <v>131</v>
       </c>
       <c r="C35" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="D35" t="s">
         <v>28</v>
@@ -5110,7 +5111,7 @@
         <v>131</v>
       </c>
       <c r="C36" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="D36" t="s">
         <v>28</v>
@@ -5347,7 +5348,7 @@
         <v>51</v>
       </c>
       <c r="Y40" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="Z40" s="4" t="str">
         <f>"GET [base]/"&amp;B40&amp;"?patient=1137192"</f>
@@ -5482,7 +5483,7 @@
         <v>131</v>
       </c>
       <c r="C43" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="D43" t="s">
         <v>28</v>
@@ -5536,7 +5537,7 @@
         <v>131</v>
       </c>
       <c r="C44" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="D44" t="s">
         <v>28</v>
@@ -5545,7 +5546,7 @@
         <v>0</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="G44" t="str">
         <f t="shared" si="0"/>
@@ -5587,7 +5588,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="C45" t="s">
         <v>83</v>
@@ -5625,7 +5626,7 @@
         <v>51</v>
       </c>
       <c r="Y45" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="Z45" s="4" t="str">
         <f>"GET [base]/"&amp;B45&amp;"?patient=1137192"</f>
@@ -5965,7 +5966,7 @@
         <v>172</v>
       </c>
       <c r="C52" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="D52" t="s">
         <v>28</v>
@@ -5974,7 +5975,7 @@
         <v>0</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="G52" t="str">
         <f t="shared" si="0"/>
@@ -6662,7 +6663,7 @@
         <v>20</v>
       </c>
       <c r="C65" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="D65" t="s">
         <v>28</v>
@@ -6671,7 +6672,7 @@
         <v>0</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="G65" t="str">
         <f t="shared" si="0"/>
@@ -6716,7 +6717,7 @@
         <v>20</v>
       </c>
       <c r="C66" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="D66" t="s">
         <v>28</v>
@@ -6823,7 +6824,7 @@
         <v>20</v>
       </c>
       <c r="C68" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="D68" t="s">
         <v>28</v>
@@ -7682,7 +7683,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="C84" t="s">
         <v>83</v>
@@ -7720,10 +7721,10 @@
         <v>51</v>
       </c>
       <c r="X84" s="6" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="Z84" s="8" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="AA84" s="8" t="str">
         <f>"Fetches a bundle of all "&amp;B84&amp; " resources for the specified patient."</f>
@@ -7739,7 +7740,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="C85" t="s">
         <v>56</v>
@@ -7792,7 +7793,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="C86" t="s">
         <v>12</v>
@@ -8269,7 +8270,7 @@
         <v>176</v>
       </c>
       <c r="C95" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="D95" t="s">
         <v>28</v>
@@ -8278,7 +8279,7 @@
         <v>0</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="G95" t="str">
         <f t="shared" si="6"/>
@@ -8643,7 +8644,7 @@
         <v>19</v>
       </c>
       <c r="C102" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="D102" t="s">
         <v>28</v>
@@ -8699,7 +8700,7 @@
         <v>0</v>
       </c>
       <c r="F103" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="G103" t="str">
         <f t="shared" si="6"/>
@@ -8917,7 +8918,7 @@
         <v>51</v>
       </c>
       <c r="Y107" s="4" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="Z107" t="s">
         <v>166</v>
@@ -9445,7 +9446,7 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="C117" t="s">
         <v>50</v>
@@ -9484,7 +9485,7 @@
         <v>support both read QuestionnaireResponse by `id` **AND** QuestionnaireResponse search</v>
       </c>
       <c r="Z117" s="4" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="AB117" t="str">
         <f t="shared" si="4"/>
@@ -9496,10 +9497,10 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="C118" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="D118" t="s">
         <v>28</v>
@@ -9540,7 +9541,7 @@
         <v>86</v>
       </c>
       <c r="Y118" s="19" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="AB118" t="str">
         <f t="shared" si="4"/>
@@ -9552,7 +9553,7 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="C119" t="s">
         <v>83</v>
@@ -9611,10 +9612,10 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="C120" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="D120" t="s">
         <v>28</v>
@@ -9649,7 +9650,7 @@
         <v>51</v>
       </c>
       <c r="Y120" s="19" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="AB120" t="str">
         <f t="shared" si="4"/>
@@ -9661,7 +9662,7 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="C121" t="s">
         <v>56</v>
@@ -9702,7 +9703,7 @@
         <v>51</v>
       </c>
       <c r="Y121" s="19" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="AB121" t="str">
         <f t="shared" si="4"/>
@@ -9714,7 +9715,7 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C122" t="s">
         <v>50</v>
@@ -9753,7 +9754,7 @@
         <v>support both read RelatedPerson by `id` **AND** RelatedPerson search</v>
       </c>
       <c r="Z122" s="4" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="AA122" s="8"/>
       <c r="AB122" t="str">
@@ -9766,7 +9767,7 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C123" t="s">
         <v>21</v>
@@ -9801,7 +9802,7 @@
         <v>51</v>
       </c>
       <c r="Y123" s="4" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="Z123" s="4" t="str">
         <f>"GET [base]/"&amp;B123&amp;"?"&amp;C123&amp;"=Mary Shaw"</f>
@@ -9821,7 +9822,7 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C124" t="s">
         <v>83</v>
@@ -9880,7 +9881,7 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C125" t="s">
         <v>50</v>
@@ -9919,7 +9920,7 @@
         <v>support both read ServiceRequest by `id` **AND** ServiceRequest search</v>
       </c>
       <c r="Z125" s="4" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="AB125" t="str">
         <f t="shared" si="8"/>
@@ -9931,10 +9932,10 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C126" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="D126" t="s">
         <v>28</v>
@@ -9985,7 +9986,7 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C127" t="s">
         <v>133</v>
@@ -10035,7 +10036,7 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C128" t="s">
         <v>24</v>
@@ -10088,7 +10089,7 @@
         <v>128</v>
       </c>
       <c r="B129" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C129" t="s">
         <v>83</v>
@@ -10147,7 +10148,7 @@
         <v>129</v>
       </c>
       <c r="B130" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C130" t="s">
         <v>56</v>
@@ -10200,7 +10201,7 @@
         <v>130</v>
       </c>
       <c r="B131" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="C131" t="s">
         <v>50</v>
@@ -10252,7 +10253,7 @@
         <v>131</v>
       </c>
       <c r="B132" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="C132" t="s">
         <v>83</v>
@@ -10360,7 +10361,7 @@
         <v>89</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>90</v>
@@ -10790,7 +10791,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D17" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="F17" t="s">
         <v>64</v>
@@ -10802,7 +10803,7 @@
         <v>284</v>
       </c>
       <c r="J17" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K17" s="4" t="str">
         <f t="shared" si="1"/>
@@ -10821,7 +10822,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D18" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="F18" t="s">
         <v>64</v>
@@ -10831,7 +10832,7 @@
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="27" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="K18" s="24" t="str">
         <f>"Fetches a bundle of all "&amp;B18&amp;" resources for the specified "&amp;SUBSTITUTE(D18,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
@@ -10907,7 +10908,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D21" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="F21" t="s">
         <v>64</v>
@@ -10919,7 +10920,7 @@
         <v>289</v>
       </c>
       <c r="J21" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="K21" s="4" t="str">
         <f t="shared" si="2"/>
@@ -11229,7 +11230,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D33" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="F33" t="s">
         <v>64</v>
@@ -11238,10 +11239,10 @@
         <v>127</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="K33" s="4" t="str">
         <f t="shared" si="2"/>
@@ -11371,7 +11372,7 @@
         <v>306</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
@@ -11416,7 +11417,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D39" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="F39" t="s">
         <v>64</v>
@@ -11428,13 +11429,13 @@
         <v>389</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="J39" s="24" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
@@ -11449,7 +11450,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D40" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="F40" t="s">
         <v>64</v>
@@ -11461,10 +11462,10 @@
         <v>143</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
@@ -11521,7 +11522,7 @@
         <v>146</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="K42" s="4" t="s">
         <v>149</v>
@@ -11539,7 +11540,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D43" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="F43" t="s">
         <v>64</v>
@@ -11551,7 +11552,7 @@
         <v>146</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="K43" s="4" t="s">
         <v>149</v>
@@ -11569,7 +11570,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D44" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="F44" t="s">
         <v>64</v>
@@ -11581,7 +11582,7 @@
         <v>146</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="K44" s="4" t="s">
         <v>149</v>
@@ -11599,7 +11600,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D45" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="F45" t="s">
         <v>64</v>
@@ -11611,7 +11612,7 @@
         <v>146</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="K45" s="4" t="s">
         <v>149</v>
@@ -11629,7 +11630,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D46" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="F46" t="s">
         <v>64</v>
@@ -11639,7 +11640,7 @@
       </c>
       <c r="I46" s="4"/>
       <c r="J46" s="24" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="K46" s="24" t="str">
         <f>"Fetches a bundle of all "&amp;B46&amp;" resources for the specified "&amp;SUBSTITUTE(D46,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
@@ -11746,7 +11747,7 @@
         <v>172</v>
       </c>
       <c r="C50" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="D50" t="s">
         <v>109</v>
@@ -11776,7 +11777,7 @@
         <v>172</v>
       </c>
       <c r="C51" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="D51" t="s">
         <v>138</v>
@@ -11809,7 +11810,7 @@
         <v>172</v>
       </c>
       <c r="C52" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="D52" t="s">
         <v>140</v>
@@ -11839,7 +11840,7 @@
         <v>172</v>
       </c>
       <c r="C53" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="D53" t="s">
         <v>187</v>
@@ -11876,7 +11877,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-diagnosticreport</v>
       </c>
       <c r="D54" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="F54" t="s">
         <v>64</v>
@@ -11886,7 +11887,7 @@
       </c>
       <c r="I54" s="4"/>
       <c r="J54" s="27" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="K54" s="24" t="str">
         <f>"Fetches a bundle of all "&amp;B54&amp;" resources for the specified "&amp;SUBSTITUTE(D54,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
@@ -11901,7 +11902,7 @@
         <v>172</v>
       </c>
       <c r="C55" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="D55" t="s">
         <v>208</v>
@@ -12279,7 +12280,7 @@
         <v>176</v>
       </c>
       <c r="C67" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="D67" t="s">
         <v>225</v>
@@ -12297,7 +12298,7 @@
         <v>264</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="K67" s="4" t="s">
         <v>299</v>
@@ -12311,7 +12312,7 @@
         <v>176</v>
       </c>
       <c r="C68" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="D68" t="s">
         <v>138</v>
@@ -12329,7 +12330,7 @@
         <v>209</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="K68" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B68&amp;" resources for the specified patient and a category code = `laboratory`"</f>
@@ -12344,7 +12345,7 @@
         <v>176</v>
       </c>
       <c r="C69" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="D69" t="s">
         <v>140</v>
@@ -12359,7 +12360,7 @@
         <v>212</v>
       </c>
       <c r="J69" s="8" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="K69" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B69&amp;" resources for the specified patient and observation code(s).  SHOULD support search by multiple report codes. The Observation `code` parameter searches `Observation.code only."</f>
@@ -12374,7 +12375,7 @@
         <v>176</v>
       </c>
       <c r="C70" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="D70" t="s">
         <v>187</v>
@@ -12392,7 +12393,7 @@
         <v>213</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
       <c r="K70" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B70&amp;" resources for the specified patient and date and a category code = `laboratory`"</f>
@@ -12407,10 +12408,10 @@
         <v>176</v>
       </c>
       <c r="C71" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="D71" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="F71" t="s">
         <v>64</v>
@@ -12420,7 +12421,7 @@
       </c>
       <c r="I71" s="4"/>
       <c r="J71" s="27" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
       <c r="K71" s="24" t="str">
         <f>"Fetches a bundle of all "&amp;B71&amp;" resources for the specified "&amp;SUBSTITUTE(D71,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
@@ -12435,7 +12436,7 @@
         <v>176</v>
       </c>
       <c r="C72" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="D72" t="s">
         <v>208</v>
@@ -12450,7 +12451,7 @@
         <v>211</v>
       </c>
       <c r="J72" s="4" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="K72" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B72&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
@@ -12610,13 +12611,13 @@
         <v>290</v>
       </c>
       <c r="I77" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="J77" s="4" t="s">
+        <v>546</v>
+      </c>
+      <c r="K77" s="8" t="s">
         <v>547</v>
-      </c>
-      <c r="J77" s="4" t="s">
-        <v>548</v>
-      </c>
-      <c r="K77" s="8" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
@@ -12814,7 +12815,7 @@
         <v>237</v>
       </c>
       <c r="C84" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="D84" t="s">
         <v>111</v>
@@ -12843,7 +12844,7 @@
         <v>237</v>
       </c>
       <c r="C85" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="D85" t="s">
         <v>109</v>
@@ -12855,13 +12856,13 @@
         <v>99</v>
       </c>
       <c r="I85" s="4" t="s">
+        <v>623</v>
+      </c>
+      <c r="J85" s="4" t="s">
+        <v>624</v>
+      </c>
+      <c r="K85" s="4" t="s">
         <v>625</v>
-      </c>
-      <c r="J85" s="4" t="s">
-        <v>626</v>
-      </c>
-      <c r="K85" s="4" t="s">
-        <v>627</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
@@ -12876,7 +12877,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
       </c>
       <c r="D86" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="F86" t="s">
         <v>64</v>
@@ -12885,13 +12886,13 @@
         <v>99</v>
       </c>
       <c r="I86" s="4" t="s">
+        <v>549</v>
+      </c>
+      <c r="J86" s="4" t="s">
+        <v>550</v>
+      </c>
+      <c r="K86" s="4" t="s">
         <v>551</v>
-      </c>
-      <c r="J86" s="4" t="s">
-        <v>552</v>
-      </c>
-      <c r="K86" s="4" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.2">
@@ -12899,7 +12900,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C87" t="str">
         <f t="shared" si="5"/>
@@ -12918,7 +12919,7 @@
         <v>282</v>
       </c>
       <c r="J87" s="4" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="K87" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B87&amp;" resources for the specified "&amp;SUBSTITUTE(D87,","," and ")</f>
@@ -12930,7 +12931,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C88" t="str">
         <f t="shared" si="5"/>
@@ -12949,7 +12950,7 @@
         <v>191</v>
       </c>
       <c r="J88" s="4" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="K88" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B88&amp;" resources for the specified patient and  a category code"</f>
@@ -12961,7 +12962,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C89" t="str">
         <f t="shared" si="5"/>
@@ -12980,7 +12981,7 @@
         <v>192</v>
       </c>
       <c r="J89" s="4" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="K89" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B89&amp;" resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes."</f>
@@ -12992,14 +12993,14 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C90" t="str">
         <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D90" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="F90" t="s">
         <v>11</v>
@@ -13011,7 +13012,7 @@
         <v>194</v>
       </c>
       <c r="J90" s="4" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="K90" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B90&amp;" resources for the specified patient and date and a category code"</f>
@@ -13023,14 +13024,14 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C91" t="str">
         <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D91" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="F91" t="s">
         <v>64</v>
@@ -13039,10 +13040,10 @@
         <v>207</v>
       </c>
       <c r="I91" s="4" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="J91" s="4" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="K91" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B91&amp;" resources for the specified patient and date and service code(s).  SHOULD support search by multiple report codes."</f>
@@ -13061,7 +13062,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D92" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="F92" t="s">
         <v>64</v>
@@ -13070,10 +13071,10 @@
         <v>99</v>
       </c>
       <c r="I92" s="4" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="J92" s="4" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="K92" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B92&amp;" resources for the specified "&amp;SUBSTITUTE(D92,","," and ")</f>
@@ -13085,7 +13086,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="C93" t="str">
         <f t="shared" si="5"/>
@@ -13101,10 +13102,10 @@
         <v>99</v>
       </c>
       <c r="I93" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="J93" s="4" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="K93" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B93&amp;" resources for the specified "&amp;SUBSTITUTE(D93,","," and ")</f>
@@ -13116,14 +13117,14 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="C94" t="str">
         <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="D94" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="F94" t="s">
         <v>64</v>
@@ -13132,13 +13133,13 @@
         <v>99</v>
       </c>
       <c r="H94" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="I94" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="J94" s="4" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="K94" t="str">
         <f>"Fetches a bundle of all "&amp;B94&amp;" resources for the specified "&amp;SUBSTITUTE(D94,","," and  ") &amp; "= 'sdoh'"</f>
@@ -13150,14 +13151,14 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="C95" t="str">
         <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D95" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="F95" t="s">
         <v>64</v>
@@ -13166,10 +13167,10 @@
         <v>142</v>
       </c>
       <c r="I95" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="J95" s="4" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="K95" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient and date"</f>
@@ -13181,14 +13182,14 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="C96" t="str">
         <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="D96" s="16" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="F96" t="s">
         <v>64</v>
@@ -13197,13 +13198,13 @@
         <v>207</v>
       </c>
       <c r="H96" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="I96" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="J96" s="4" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="K96" t="str">
         <f>"Fetches a bundle of all "&amp;B96&amp;" resources tagged as 'sdoh' for the specified patient and date"</f>
@@ -13215,14 +13216,14 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="C97" t="str">
         <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D97" s="16" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="F97" t="s">
         <v>64</v>
@@ -13231,10 +13232,10 @@
         <v>84</v>
       </c>
       <c r="I97" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="J97" s="4" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="K97" t="str">
         <f>"Fetches a bundle of all "&amp;B97&amp;" resources for the specified patient that have been completed against a specified form."</f>
@@ -13246,7 +13247,7 @@
         <v>97</v>
       </c>
       <c r="B98" s="16" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="C98" t="str">
         <f t="shared" si="5"/>
@@ -13264,10 +13265,10 @@
       </c>
       <c r="H98" s="16"/>
       <c r="I98" s="4" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="J98" s="4" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="K98" t="str">
         <f>"Fetches a bundle of all "&amp;B98&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed))."</f>
@@ -13279,7 +13280,7 @@
         <v>98</v>
       </c>
       <c r="B99" s="16" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="C99" t="str">
         <f t="shared" si="5"/>
@@ -13297,10 +13298,10 @@
       </c>
       <c r="H99" s="16"/>
       <c r="I99" s="4" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="J99" s="4" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="K99" t="str">
         <f>"Fetches a bundle of all "&amp;B99&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed) and type of dispense (e.g., partially dispensed)."</f>
@@ -13312,14 +13313,14 @@
         <v>99</v>
       </c>
       <c r="B100" s="16" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="C100" t="str">
         <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationdispense</v>
       </c>
       <c r="D100" s="16" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="E100" s="16"/>
       <c r="F100" s="16" t="s">
@@ -13330,10 +13331,10 @@
       </c>
       <c r="H100" s="16"/>
       <c r="I100" s="4" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="J100" s="4" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="K100" t="str">
         <f>"Fetches a bundle of all "&amp;B99&amp;" resources for the specified patient for a given dispense and date or range"</f>
@@ -13345,25 +13346,25 @@
         <v>100</v>
       </c>
       <c r="B101" s="16" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C101" s="22" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D101" s="16" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="E101" s="16"/>
       <c r="F101" s="16" t="s">
         <v>64</v>
       </c>
       <c r="G101" s="16" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="H101" s="16"/>
       <c r="I101" s="4"/>
       <c r="J101" s="4" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="K101" t="str">
         <f>"Fetches a bundle of all "&amp;B101&amp;" resources for the specified patient that may match any of the string fields in the name element (including family, give, prefix, suffix, suffix, and/or text)"</f>
@@ -13421,7 +13422,7 @@
         <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -13453,7 +13454,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -13461,7 +13462,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -13505,8 +13506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A70CC787-78D8-4AA0-BE43-37746049F77C}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13532,27 +13533,27 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>496</v>
-      </c>
-      <c r="B2" t="s">
-        <v>510</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>639</v>
+        <v>736</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>737</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>738</v>
       </c>
       <c r="D2" t="s">
-        <v>64</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="B3" s="21" t="s">
+        <v>505</v>
+      </c>
+      <c r="C3" s="21" t="s">
         <v>506</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>507</v>
       </c>
       <c r="D3" s="21" t="s">
         <v>64</v>
@@ -13560,7 +13561,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{DEF66039-9B20-2C43-9CB5-B3AF8A8243E1}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{FE115460-0CCD-6748-BBEA-04F340C9195B}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{C55A810B-6D78-4449-9125-2BF6B32AEF5A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13585,10 +13587,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>496</v>
+      </c>
+      <c r="B1" t="s">
         <v>497</v>
-      </c>
-      <c r="B1" t="s">
-        <v>498</v>
       </c>
       <c r="C1" t="s">
         <v>21</v>
@@ -13606,13 +13608,13 @@
     <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B2" s="16"/>
       <c r="C2" t="s">
+        <v>498</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>499</v>
       </c>
-      <c r="D2" s="15" t="s">
-        <v>500</v>
-      </c>
       <c r="E2" s="15" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -13701,10 +13703,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B5" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
@@ -13715,10 +13717,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="B6" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -13729,16 +13731,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="B7" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -13799,7 +13801,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="B12" t="s">
         <v>340</v>
@@ -13813,86 +13815,86 @@
     </row>
     <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
+        <v>566</v>
+      </c>
+      <c r="B13" t="s">
+        <v>567</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
         <v>568</v>
-      </c>
-      <c r="B13" t="s">
-        <v>569</v>
-      </c>
-      <c r="D13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B14" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="D14" t="s">
         <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="B15" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="D15" t="s">
         <v>11</v>
       </c>
       <c r="E15" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="B16" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="D16" t="s">
         <v>11</v>
       </c>
       <c r="E16" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="B17" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="D17" t="s">
         <v>11</v>
       </c>
       <c r="E17" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="B18" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="D18" t="s">
         <v>11</v>
       </c>
       <c r="E18" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -13967,16 +13969,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="B24" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="D24" t="s">
         <v>11</v>
       </c>
       <c r="E24" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -13995,10 +13997,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="B26" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="D26" t="s">
         <v>11</v>
@@ -14009,10 +14011,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="B27" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
@@ -14023,10 +14025,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="B28" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="D28" t="s">
         <v>11</v>
@@ -14037,10 +14039,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="18" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="B29" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="D29" t="s">
         <v>11</v>
@@ -14065,10 +14067,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="B31" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="D31" t="s">
         <v>11</v>
@@ -14079,10 +14081,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="B32" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="D32" t="s">
         <v>11</v>
@@ -14093,10 +14095,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
       <c r="B33" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="D33" t="s">
         <v>11</v>
@@ -14177,10 +14179,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="18" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B39" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="D39" t="s">
         <v>11</v>
@@ -14233,10 +14235,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="B43" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="D43" t="s">
         <v>11</v>
@@ -14247,10 +14249,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="B44" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
       <c r="D44" t="s">
         <v>11</v>
@@ -14275,10 +14277,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="18" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="B46" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="D46" t="s">
         <v>11</v>
@@ -14289,10 +14291,10 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="B47" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="D47" t="s">
         <v>11</v>
@@ -14320,7 +14322,7 @@
         <v>467</v>
       </c>
       <c r="B49" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="D49" t="s">
         <v>11</v>
@@ -14443,72 +14445,72 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="B58" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="D58" t="s">
         <v>11</v>
       </c>
       <c r="E58" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="B59" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="D59" t="s">
         <v>11</v>
       </c>
       <c r="E59" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="18" t="s">
+        <v>509</v>
+      </c>
+      <c r="B60" t="s">
+        <v>510</v>
+      </c>
+      <c r="D60" t="s">
+        <v>11</v>
+      </c>
+      <c r="E60" t="s">
         <v>511</v>
-      </c>
-      <c r="B60" t="s">
-        <v>512</v>
-      </c>
-      <c r="D60" t="s">
-        <v>11</v>
-      </c>
-      <c r="E60" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="18" t="s">
+        <v>512</v>
+      </c>
+      <c r="B61" t="s">
+        <v>513</v>
+      </c>
+      <c r="D61" t="s">
+        <v>11</v>
+      </c>
+      <c r="E61" t="s">
         <v>514</v>
-      </c>
-      <c r="B61" t="s">
-        <v>515</v>
-      </c>
-      <c r="D61" t="s">
-        <v>11</v>
-      </c>
-      <c r="E61" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="B62" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="D62" t="s">
         <v>11</v>
       </c>
       <c r="E62" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
     </row>
   </sheetData>
@@ -14526,8 +14528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{352F3A6C-0DAD-1041-B50E-04478951E07A}">
   <dimension ref="A1:Y69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="U32" sqref="U32"/>
+    <sheetView topLeftCell="S17" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2:U20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="23" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -14611,16 +14613,16 @@
         <v>380</v>
       </c>
       <c r="V1" s="3" t="s">
+        <v>500</v>
+      </c>
+      <c r="W1" s="3" t="s">
         <v>501</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>502</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>503</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="23" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -14648,7 +14650,7 @@
         <v>64</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
       <c r="X3" s="13" t="s">
         <v>424</v>
@@ -14665,13 +14667,13 @@
         <v>64</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="V4" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="W4" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="X4" s="13" t="s">
         <v>424</v>
@@ -14688,7 +14690,7 @@
         <v>64</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
       <c r="X5" s="13" t="s">
         <v>424</v>
@@ -14699,7 +14701,7 @@
     </row>
     <row r="6" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="B6" t="s">
         <v>64</v>
@@ -14719,7 +14721,7 @@
         <v>64</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="X7" s="13" t="s">
         <v>424</v>
@@ -14736,7 +14738,7 @@
         <v>64</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="X8" s="13" t="s">
         <v>424</v>
@@ -14753,7 +14755,7 @@
         <v>64</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="X9" s="13" t="s">
         <v>424</v>
@@ -14770,7 +14772,7 @@
         <v>64</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
       <c r="X10" s="13" t="s">
         <v>424</v>
@@ -14781,13 +14783,13 @@
     </row>
     <row r="11" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="B11" t="s">
         <v>64</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="X11" s="13"/>
       <c r="Y11" s="13"/>
@@ -14800,7 +14802,7 @@
         <v>64</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="X12" s="13" t="s">
         <v>424</v>
@@ -14811,13 +14813,13 @@
     </row>
     <row r="13" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="B13" t="s">
         <v>28</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="X13" s="13"/>
       <c r="Y13" s="13"/>
@@ -14830,7 +14832,7 @@
         <v>64</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="X14" s="13" t="s">
         <v>424</v>
@@ -14847,20 +14849,20 @@
         <v>64</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="X15" s="13"/>
       <c r="Y15" s="13"/>
     </row>
     <row r="16" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="B16" t="s">
         <v>64</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="X16" s="13"/>
       <c r="Y16" s="13"/>
@@ -14886,7 +14888,7 @@
         <v>64</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="V18" t="s">
         <v>64</v>
@@ -14903,19 +14905,19 @@
     </row>
     <row r="19" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="B19" t="s">
         <v>64</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="V19" t="s">
         <v>64</v>
       </c>
       <c r="W19" s="6" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="X19" s="13" t="s">
         <v>424</v>
@@ -14955,7 +14957,7 @@
         <v>64</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
       <c r="X21" s="13" t="s">
         <v>424</v>
@@ -14972,7 +14974,7 @@
         <v>64</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
       <c r="X22" s="13"/>
       <c r="Y22" s="13"/>
@@ -14985,7 +14987,7 @@
         <v>64</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="X23" s="13" t="s">
         <v>424</v>
@@ -15002,7 +15004,7 @@
         <v>64</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
       <c r="X24" s="13"/>
       <c r="Y24" s="13"/>
@@ -15015,10 +15017,10 @@
         <v>64</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="V25" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="W25" t="s">
         <v>261</v>
@@ -15034,7 +15036,7 @@
         <v>64</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
       <c r="X26" s="13" t="s">
         <v>424</v>
@@ -15051,31 +15053,31 @@
         <v>64</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
     </row>
     <row r="28" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="B28" t="s">
         <v>64</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
       <c r="X28" s="13"/>
       <c r="Y28" s="13"/>
     </row>
     <row r="29" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="B29" t="s">
         <v>64</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
       <c r="X29" s="13" t="s">
         <v>424</v>
@@ -15086,13 +15088,13 @@
     </row>
     <row r="30" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="B30" t="s">
         <v>64</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="X30" s="13" t="s">
         <v>424</v>
@@ -15103,13 +15105,13 @@
     </row>
     <row r="31" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B31" t="s">
         <v>64</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="X31" s="13" t="s">
         <v>424</v>
@@ -15120,13 +15122,13 @@
     </row>
     <row r="32" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="B32" t="s">
         <v>64</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
       <c r="X32" s="13"/>
       <c r="Y32" s="13"/>
@@ -15222,7 +15224,7 @@
         <v>64</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -15275,7 +15277,7 @@
         <v>346</v>
       </c>
       <c r="F1" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
       <c r="G1" t="s">
         <v>347</v>
@@ -15293,13 +15295,13 @@
         <v>350</v>
       </c>
       <c r="L1" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="M1" t="s">
         <v>351</v>
       </c>
       <c r="N1" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="O1" t="s">
         <v>352</v>
@@ -15308,13 +15310,13 @@
         <v>353</v>
       </c>
       <c r="Q1" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="R1" t="s">
         <v>354</v>
       </c>
       <c r="S1" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="T1" t="s">
         <v>355</v>
@@ -15347,22 +15349,22 @@
         <v>409</v>
       </c>
       <c r="AD1" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="AE1" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="AF1" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="AG1" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="AH1" t="s">
         <v>423</v>
       </c>
       <c r="AI1" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
QA Clarify Role and use of US Core SearchParameters vs FHIR standard SearchParameters FHIR-46036
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0417C5-186F-2848-8558-E4940C979F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732F070D-AD7E-714D-B2F4-289D091BE330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17800" yWindow="500" windowWidth="36700" windowHeight="28300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34340" yWindow="500" windowWidth="36700" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -2487,6 +2487,30 @@
     </r>
   </si>
   <si>
+    <t>8.0.0-ballot</t>
+  </si>
+  <si>
+    <t>The Media Resource is a Must Support referenced resource when using the US Core DiagnosticReport Profile for Report and Note Exchange.</t>
+  </si>
+  <si>
+    <t>* Additional considerations for systems aligning with [HL7 Consolidated (C-CDA)](http://www.hl7.org/implement/standards/product_brief.cfm?product_id=492) Care Plan requirements:
+    - US Core Goal **SHOULD** be present in CarePlan.goal
+    - US Core Condition **SHOULD** be present in CarePlan.addresses
+    - Assessment and Plan **MAY** be included as narrative text</t>
+  </si>
+  <si>
+    <t>The Media Resource is a Must Support referenced resource when using the US Core PractitionerRole Profile.</t>
+  </si>
+  <si>
+    <t>SMART App Launch 2.0.0</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/smart-app-launch/ImplementationGuide/hl7.fhir.uv.smart-app-launch|2.0.0</t>
+  </si>
+  <si>
+    <t>https://hl7.org/fhir/smart-app-launch/STU2/</t>
+  </si>
+  <si>
     <t>The US Core Client **SHALL**:
 1. Support fetching and querying of one or more US Core profile(s), using the supported RESTful interactions and search parameters declared in the US Core Server CapabilityStatement.
 1. Follow the requirements documented in the [General Requirements](general-requirements.html) and [Must Support](must-support.html) pages
@@ -2496,31 +2520,7 @@
 - `comparator`
 - `modifier`
 - `chain`
-For search operations, Clients **SHOULD** use the standard FHIR SearchParameters.</t>
-  </si>
-  <si>
-    <t>8.0.0-ballot</t>
-  </si>
-  <si>
-    <t>The Media Resource is a Must Support referenced resource when using the US Core DiagnosticReport Profile for Report and Note Exchange.</t>
-  </si>
-  <si>
-    <t>* Additional considerations for systems aligning with [HL7 Consolidated (C-CDA)](http://www.hl7.org/implement/standards/product_brief.cfm?product_id=492) Care Plan requirements:
-    - US Core Goal **SHOULD** be present in CarePlan.goal
-    - US Core Condition **SHOULD** be present in CarePlan.addresses
-    - Assessment and Plan **MAY** be included as narrative text</t>
-  </si>
-  <si>
-    <t>The Media Resource is a Must Support referenced resource when using the US Core PractitionerRole Profile.</t>
-  </si>
-  <si>
-    <t>SMART App Launch 2.0.0</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/smart-app-launch/ImplementationGuide/hl7.fhir.uv.smart-app-launch|2.0.0</t>
-  </si>
-  <si>
-    <t>https://hl7.org/fhir/smart-app-launch/STU2/</t>
+They **SHALL NOT** be interpreted as search parameters for search. Servers and Clients **SHOULD** use the standard FHIR SearchParameters.</t>
   </si>
 </sst>
 </file>
@@ -13391,8 +13391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13422,7 +13422,7 @@
         <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -13449,12 +13449,12 @@
         <v>381</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="288" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="304" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>731</v>
+        <v>738</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -13506,7 +13506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A70CC787-78D8-4AA0-BE43-37746049F77C}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -13533,13 +13533,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>735</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>736</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="C2" s="28" t="s">
         <v>737</v>
-      </c>
-      <c r="C2" s="28" t="s">
-        <v>738</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
@@ -14650,7 +14650,7 @@
         <v>64</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="X3" s="13" t="s">
         <v>424</v>
@@ -14789,7 +14789,7 @@
         <v>64</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="X11" s="13"/>
       <c r="Y11" s="13"/>
@@ -14862,7 +14862,7 @@
         <v>64</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="X16" s="13"/>
       <c r="Y16" s="13"/>

</xml_diff>

<commit_message>
FHIR-49413 Update lnumber of common clinical notes FHIR-49414 Typo in intro language
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732F070D-AD7E-714D-B2F4-289D091BE330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66770500-3BC3-4347-9A71-38DBCEC86B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34340" yWindow="500" windowWidth="36700" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2318,16 +2318,6 @@
     <t>GET [base]Observation?patient=555580&amp;code=http://loinc.org\|{{include.code1 | default: '[code]'}}&amp;date=ge2019-01-01T00:00:00Z</t>
   </si>
   <si>
-    <t>* The `DocumentReference.type` binding **SHALL** support at a minimum the [5 Common Clinical Notes](ValueSet-us-core-clinical-note-type.html) and may extend to the full US Core DocumentReference Type Value Set
-* The DocumentReference resources can represent the referenced content using either an address where the document can be retrieved using `DocumentReference.attachment.url` or the content as inline base64 encoded data using `DocumentReference.attachment.data`.
-    *  Although both are marked as must support, the server system is not required to support an address, and inline base64 encoded data, but **SHALL** support at least one of these elements.
-    *  The client application **SHALL** support both elements.
-    *  The `content.url` may refer to a FHIR Binary Resource (i.e. [base]/Binary/[id]), FHIR Document Bundle (i.e [base]/Bundle/[id] or another endpoint.
-        * If the endpoint is outside the FHIR base URL, it **SHOULD NOT** require additional authorization to access.
-   * If there are multiple `DocumentReference.content` element repetitions, these **SHALL** all represent the same document in different format or attachment metadata. The content element **SHALL NOT** contain different versions of the same content. For version handling use multiple DocumentReferences with `DocumentReference.relatesTo`
-* Every DocumentReference must have a responsible Organization. The organization responsible for the DocumentReference **SHALL** be present either in `DocumentReference.custodian` or accessible in the Provenance resource targeting the DocumentReference using `Provenance.agent.who` or `Provenance.agent.onBehalfOf`.</t>
-  </si>
-  <si>
     <t xml:space="preserve">* The Encounter resource can represent a reason using either a code with `Encounter.reasonCode`, or a reference with `Encounter.reasonReference` to  Condition or other resource.
    * Although both are marked as must support, the server systems are not required to support both a code and a reference, but they **SHALL** support *at least one* of these elements.
    * The client application **SHALL** support both elements.
@@ -2521,6 +2511,16 @@
 - `modifier`
 - `chain`
 They **SHALL NOT** be interpreted as search parameters for search. Servers and Clients **SHOULD** use the standard FHIR SearchParameters.</t>
+  </si>
+  <si>
+    <t>* The `DocumentReference.type` binding **SHALL** support at a minimum the [10 Common Clinical Notes](ValueSet-us-core-clinical-note-type.html) and may extend to the full US Core DocumentReference Type Value Set
+* The DocumentReference resources can represent the referenced content using either an address where the document can be retrieved using `DocumentReference.attachment.url` or the content as inline base64 encoded data using `DocumentReference.attachment.data`.
+    *  Although both are marked as must support, the server system is not required to support an address, and inline base64 encoded data, but **SHALL** support at least one of these elements.
+    *  The client application **SHALL** support both elements.
+    *  The `content.url` may refer to a FHIR Binary Resource (i.e. [base]/Binary/[id]), FHIR Document Bundle (i.e [base]/Bundle/[id] or another endpoint.
+        * If the endpoint is outside the FHIR base URL, it **SHOULD NOT** require additional authorization to access.
+   * If there are multiple `DocumentReference.content` element repetitions, these **SHALL** all represent the same document in different format or attachment metadata. The content element **SHALL NOT** contain different versions of the same content. For version handling use multiple DocumentReferences with `DocumentReference.relatesTo`
+* Every DocumentReference must have a responsible Organization. The organization responsible for the DocumentReference **SHALL** be present either in `DocumentReference.custodian` or accessible in the Provenance resource targeting the DocumentReference using `Provenance.agent.who` or `Provenance.agent.onBehalfOf`.</t>
   </si>
 </sst>
 </file>
@@ -5546,7 +5546,7 @@
         <v>0</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="G44" t="str">
         <f t="shared" si="0"/>
@@ -5975,7 +5975,7 @@
         <v>0</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="G52" t="str">
         <f t="shared" si="0"/>
@@ -6672,7 +6672,7 @@
         <v>0</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="G65" t="str">
         <f t="shared" si="0"/>
@@ -8279,7 +8279,7 @@
         <v>0</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="G95" t="str">
         <f t="shared" si="6"/>
@@ -11640,7 +11640,7 @@
       </c>
       <c r="I46" s="4"/>
       <c r="J46" s="24" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="K46" s="24" t="str">
         <f>"Fetches a bundle of all "&amp;B46&amp;" resources for the specified "&amp;SUBSTITUTE(D46,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
@@ -13422,7 +13422,7 @@
         <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -13454,7 +13454,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -13533,13 +13533,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>734</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>735</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="C2" s="28" t="s">
         <v>736</v>
-      </c>
-      <c r="C2" s="28" t="s">
-        <v>737</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
@@ -14650,7 +14650,7 @@
         <v>64</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="X3" s="13" t="s">
         <v>424</v>
@@ -14667,7 +14667,7 @@
         <v>64</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="V4" t="s">
         <v>515</v>
@@ -14690,7 +14690,7 @@
         <v>64</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="X5" s="13" t="s">
         <v>424</v>
@@ -14738,7 +14738,7 @@
         <v>64</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="X8" s="13" t="s">
         <v>424</v>
@@ -14755,7 +14755,7 @@
         <v>64</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>712</v>
+        <v>738</v>
       </c>
       <c r="X9" s="13" t="s">
         <v>424</v>
@@ -14772,7 +14772,7 @@
         <v>64</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="X10" s="13" t="s">
         <v>424</v>
@@ -14789,7 +14789,7 @@
         <v>64</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="X11" s="13"/>
       <c r="Y11" s="13"/>
@@ -14849,7 +14849,7 @@
         <v>64</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="X15" s="13"/>
       <c r="Y15" s="13"/>
@@ -14862,7 +14862,7 @@
         <v>64</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="X16" s="13"/>
       <c r="Y16" s="13"/>
@@ -14888,7 +14888,7 @@
         <v>64</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="V18" t="s">
         <v>64</v>
@@ -14911,7 +14911,7 @@
         <v>64</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="V19" t="s">
         <v>64</v>
@@ -14957,7 +14957,7 @@
         <v>64</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="X21" s="13" t="s">
         <v>424</v>
@@ -14974,7 +14974,7 @@
         <v>64</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="X22" s="13"/>
       <c r="Y22" s="13"/>
@@ -14987,7 +14987,7 @@
         <v>64</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="X23" s="13" t="s">
         <v>424</v>
@@ -15004,7 +15004,7 @@
         <v>64</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="X24" s="13"/>
       <c r="Y24" s="13"/>
@@ -15036,7 +15036,7 @@
         <v>64</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="X26" s="13" t="s">
         <v>424</v>
@@ -15064,7 +15064,7 @@
         <v>64</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="X28" s="13"/>
       <c r="Y28" s="13"/>
@@ -15077,7 +15077,7 @@
         <v>64</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="X29" s="13" t="s">
         <v>424</v>
@@ -15094,7 +15094,7 @@
         <v>64</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="X30" s="13" t="s">
         <v>424</v>
@@ -15111,7 +15111,7 @@
         <v>64</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="X31" s="13" t="s">
         <v>424</v>
@@ -15128,7 +15128,7 @@
         <v>64</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="X32" s="13"/>
       <c r="Y32" s="13"/>

</xml_diff>

<commit_message>
FHIR-50177 Changes to comply with Executive Order 14168
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC721EE6-3365-0B44-A19B-B1073442A9B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA6B28D-EA6A-8D44-86E2-640B7711D3B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34340" yWindow="500" windowWidth="36700" windowHeight="28300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34340" yWindow="500" windowWidth="36700" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -1824,9 +1824,6 @@
     <t>GET [base]/Goal?patient=1137192&amp;description=http://snomed.info/sct\|1078229009</t>
   </si>
   <si>
-    <t>Documents/FHIR/US-Core/input/</t>
-  </si>
-  <si>
     <t>HL7 International - Cross-Group Projects</t>
   </si>
   <si>
@@ -2474,9 +2471,6 @@
     </r>
   </si>
   <si>
-    <t>8.0.0-ballot</t>
-  </si>
-  <si>
     <t>The Media Resource is a Must Support referenced resource when using the US Core DiagnosticReport Profile for Report and Note Exchange.</t>
   </si>
   <si>
@@ -2496,18 +2490,6 @@
   </si>
   <si>
     <t>https://hl7.org/fhir/smart-app-launch/STU2/</t>
-  </si>
-  <si>
-    <t>The US Core Client **SHALL**:
-1. Support fetching and querying of one or more US Core profile(s), using the supported RESTful interactions and search parameters declared in the US Core Server CapabilityStatement.
-1. Follow the requirements documented in the [General Requirements](general-requirements.html) and [Must Support](must-support.html) pages
-**NOTE**: US Core SearchParameters referenced in this CapabilityStatement that are derived from standard FHIR SearchParameters are only defined to document Server and Client expectations. They specify additional expectations for the following SearchParameter elements:
-- `multipleAnd`
-- `multipleOr`
-- `comparator`
-- `modifier`
-- `chain`
-They **SHALL NOT** be interpreted as search parameters for search. Servers and Clients **SHOULD** use the standard FHIR SearchParameters.</t>
   </si>
   <si>
     <t>* The `DocumentReference.type` binding **SHALL** support at a minimum the [10 Common Clinical Notes](ValueSet-us-core-clinical-note-type.html) and may extend to the full US Core DocumentReference Type Value Set
@@ -2521,6 +2503,24 @@
   </si>
   <si>
     <t>The HealthcareService Resource is a referenced resource when using the US Core PractitionerRole Profile and subject to constraint us-core-13: "SHALL have a practitioner, an organization, a healthcare service, or a location."</t>
+  </si>
+  <si>
+    <t>The US Core Client **SHALL**:
+1. Support fetching and querying of one or more US Core profile(s), using the supported RESTful interactions and search parameters declared in the US Core Server CapabilityStatement.
+1. Follow the requirements documented in the [General Requirements](general-requirements.html) and [Must Support](must-support.html) pages
+**NOTE**: US Core SearchParameters referenced in this CapabilityStatement that are derived from standard FHIR SearchParameters are only defined to document Server and Client expectations. They specify additional expectations for the following SearchParameter elements:B7
+- `multipleAnd`
+- `multipleOr`
+- `comparator`
+- `modifier`
+- `chain`
+They **SHALL NOT** be interpreted as search parameters for search. Servers and Clients **SHOULD** use the standard FHIR SearchParameters.</t>
+  </si>
+  <si>
+    <t>8.0.0</t>
+  </si>
+  <si>
+    <t>/Users/ehaas/Documents/FHIR/US-Core/input/</t>
   </si>
 </sst>
 </file>
@@ -3137,8 +3137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40F68824-E615-4729-AAE0-A6F75FBDE06B}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView zoomScale="400" zoomScaleNormal="400" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScale="400" zoomScaleNormal="400" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3160,7 +3160,7 @@
         <v>437</v>
       </c>
       <c r="B2" t="s">
-        <v>563</v>
+        <v>738</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -3192,7 +3192,7 @@
         <v>62</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -3208,7 +3208,7 @@
         <v>444</v>
       </c>
       <c r="B8" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -3343,7 +3343,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C2" t="s">
         <v>50</v>
@@ -3368,7 +3368,7 @@
         <v>52</v>
       </c>
       <c r="L2" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="M2" t="s">
         <v>51</v>
@@ -3390,7 +3390,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C3" t="s">
         <v>65</v>
@@ -3434,7 +3434,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C4" t="s">
         <v>62</v>
@@ -3481,7 +3481,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C5" t="s">
         <v>56</v>
@@ -3525,7 +3525,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C6" t="s">
         <v>57</v>
@@ -3581,7 +3581,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C7" t="s">
         <v>54</v>
@@ -3625,7 +3625,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C8" t="s">
         <v>61</v>
@@ -3970,10 +3970,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>616</v>
+      </c>
+      <c r="C15" t="s">
         <v>617</v>
-      </c>
-      <c r="C15" t="s">
-        <v>618</v>
       </c>
       <c r="D15" t="s">
         <v>28</v>
@@ -4459,7 +4459,7 @@
         <v>78</v>
       </c>
       <c r="C24" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D24" t="s">
         <v>28</v>
@@ -4481,19 +4481,19 @@
         <v>52</v>
       </c>
       <c r="L24" t="s">
+        <v>608</v>
+      </c>
+      <c r="M24" t="s">
+        <v>51</v>
+      </c>
+      <c r="O24" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y24" s="4" t="s">
         <v>609</v>
       </c>
-      <c r="M24" t="s">
-        <v>51</v>
-      </c>
-      <c r="O24" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y24" s="4" t="s">
+      <c r="Z24" t="s">
         <v>610</v>
-      </c>
-      <c r="Z24" t="s">
-        <v>611</v>
       </c>
       <c r="AA24" s="8" t="str">
         <f>"Fetches a bundle of all "&amp;B24&amp;" resources matching the name"</f>
@@ -4509,10 +4509,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C25" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D25" t="s">
         <v>28</v>
@@ -4537,16 +4537,16 @@
         <v>52</v>
       </c>
       <c r="L25" t="s">
+        <v>640</v>
+      </c>
+      <c r="M25" t="s">
+        <v>51</v>
+      </c>
+      <c r="O25" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y25" s="19" t="s">
         <v>641</v>
-      </c>
-      <c r="M25" t="s">
-        <v>51</v>
-      </c>
-      <c r="O25" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y25" s="19" t="s">
-        <v>642</v>
       </c>
       <c r="AB25" t="str">
         <f t="shared" si="1"/>
@@ -5537,7 +5537,7 @@
         <v>131</v>
       </c>
       <c r="C44" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="D44" t="s">
         <v>28</v>
@@ -5546,7 +5546,7 @@
         <v>0</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="G44" t="str">
         <f t="shared" si="0"/>
@@ -5588,7 +5588,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C45" t="s">
         <v>83</v>
@@ -5626,7 +5626,7 @@
         <v>51</v>
       </c>
       <c r="Y45" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="Z45" s="4" t="str">
         <f>"GET [base]/"&amp;B45&amp;"?patient=1137192"</f>
@@ -5966,7 +5966,7 @@
         <v>172</v>
       </c>
       <c r="C52" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="D52" t="s">
         <v>28</v>
@@ -5975,7 +5975,7 @@
         <v>0</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="G52" t="str">
         <f t="shared" si="0"/>
@@ -6663,7 +6663,7 @@
         <v>20</v>
       </c>
       <c r="C65" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="D65" t="s">
         <v>28</v>
@@ -6672,7 +6672,7 @@
         <v>0</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="G65" t="str">
         <f t="shared" si="0"/>
@@ -7683,7 +7683,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C84" t="s">
         <v>83</v>
@@ -7721,10 +7721,10 @@
         <v>51</v>
       </c>
       <c r="X84" s="6" t="s">
+        <v>614</v>
+      </c>
+      <c r="Z84" s="8" t="s">
         <v>615</v>
-      </c>
-      <c r="Z84" s="8" t="s">
-        <v>616</v>
       </c>
       <c r="AA84" s="8" t="str">
         <f>"Fetches a bundle of all "&amp;B84&amp; " resources for the specified patient."</f>
@@ -7740,7 +7740,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C85" t="s">
         <v>56</v>
@@ -7793,7 +7793,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C86" t="s">
         <v>12</v>
@@ -8270,7 +8270,7 @@
         <v>176</v>
       </c>
       <c r="C95" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="D95" t="s">
         <v>28</v>
@@ -8279,7 +8279,7 @@
         <v>0</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="G95" t="str">
         <f t="shared" si="6"/>
@@ -8644,7 +8644,7 @@
         <v>19</v>
       </c>
       <c r="C102" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D102" t="s">
         <v>28</v>
@@ -8918,7 +8918,7 @@
         <v>51</v>
       </c>
       <c r="Y107" s="4" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="Z107" t="s">
         <v>166</v>
@@ -9446,7 +9446,7 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C117" t="s">
         <v>50</v>
@@ -9485,7 +9485,7 @@
         <v>support both read QuestionnaireResponse by `id` **AND** QuestionnaireResponse search</v>
       </c>
       <c r="Z117" s="4" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="AB117" t="str">
         <f t="shared" si="4"/>
@@ -9497,7 +9497,7 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C118" t="s">
         <v>529</v>
@@ -9541,7 +9541,7 @@
         <v>86</v>
       </c>
       <c r="Y118" s="19" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="AB118" t="str">
         <f t="shared" si="4"/>
@@ -9553,7 +9553,7 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C119" t="s">
         <v>83</v>
@@ -9612,10 +9612,10 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C120" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D120" t="s">
         <v>28</v>
@@ -9650,7 +9650,7 @@
         <v>51</v>
       </c>
       <c r="Y120" s="19" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="AB120" t="str">
         <f t="shared" si="4"/>
@@ -9662,7 +9662,7 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C121" t="s">
         <v>56</v>
@@ -9703,7 +9703,7 @@
         <v>51</v>
       </c>
       <c r="Y121" s="19" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="AB121" t="str">
         <f t="shared" si="4"/>
@@ -9802,7 +9802,7 @@
         <v>51</v>
       </c>
       <c r="Y123" s="4" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="Z123" s="4" t="str">
         <f>"GET [base]/"&amp;B123&amp;"?"&amp;C123&amp;"=Mary Shaw"</f>
@@ -10201,7 +10201,7 @@
         <v>130</v>
       </c>
       <c r="B131" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C131" t="s">
         <v>50</v>
@@ -10253,7 +10253,7 @@
         <v>131</v>
       </c>
       <c r="B132" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C132" t="s">
         <v>83</v>
@@ -10822,7 +10822,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D18" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="F18" t="s">
         <v>64</v>
@@ -10832,7 +10832,7 @@
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="27" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="K18" s="24" t="str">
         <f>"Fetches a bundle of all "&amp;B18&amp;" resources for the specified "&amp;SUBSTITUTE(D18,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
@@ -11230,7 +11230,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D33" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F33" t="s">
         <v>64</v>
@@ -11239,10 +11239,10 @@
         <v>127</v>
       </c>
       <c r="I33" s="4" t="s">
+        <v>619</v>
+      </c>
+      <c r="J33" s="4" t="s">
         <v>620</v>
-      </c>
-      <c r="J33" s="4" t="s">
-        <v>621</v>
       </c>
       <c r="K33" s="4" t="str">
         <f t="shared" si="2"/>
@@ -11372,7 +11372,7 @@
         <v>306</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
@@ -11417,7 +11417,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D39" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="F39" t="s">
         <v>64</v>
@@ -11429,13 +11429,13 @@
         <v>389</v>
       </c>
       <c r="I39" s="4" t="s">
+        <v>679</v>
+      </c>
+      <c r="J39" s="24" t="s">
         <v>680</v>
       </c>
-      <c r="J39" s="24" t="s">
+      <c r="K39" s="4" t="s">
         <v>681</v>
-      </c>
-      <c r="K39" s="4" t="s">
-        <v>682</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
@@ -11462,7 +11462,7 @@
         <v>143</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="K40" s="4" t="s">
         <v>537</v>
@@ -11630,7 +11630,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D46" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="F46" t="s">
         <v>64</v>
@@ -11640,7 +11640,7 @@
       </c>
       <c r="I46" s="4"/>
       <c r="J46" s="24" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="K46" s="24" t="str">
         <f>"Fetches a bundle of all "&amp;B46&amp;" resources for the specified "&amp;SUBSTITUTE(D46,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
@@ -11747,7 +11747,7 @@
         <v>172</v>
       </c>
       <c r="C50" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="D50" t="s">
         <v>109</v>
@@ -11777,7 +11777,7 @@
         <v>172</v>
       </c>
       <c r="C51" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="D51" t="s">
         <v>138</v>
@@ -11810,7 +11810,7 @@
         <v>172</v>
       </c>
       <c r="C52" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="D52" t="s">
         <v>140</v>
@@ -11840,7 +11840,7 @@
         <v>172</v>
       </c>
       <c r="C53" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="D53" t="s">
         <v>187</v>
@@ -11877,7 +11877,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-diagnosticreport</v>
       </c>
       <c r="D54" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="F54" t="s">
         <v>64</v>
@@ -11887,7 +11887,7 @@
       </c>
       <c r="I54" s="4"/>
       <c r="J54" s="27" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="K54" s="24" t="str">
         <f>"Fetches a bundle of all "&amp;B54&amp;" resources for the specified "&amp;SUBSTITUTE(D54,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
@@ -11902,7 +11902,7 @@
         <v>172</v>
       </c>
       <c r="C55" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="D55" t="s">
         <v>208</v>
@@ -12280,7 +12280,7 @@
         <v>176</v>
       </c>
       <c r="C67" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="D67" t="s">
         <v>225</v>
@@ -12298,7 +12298,7 @@
         <v>264</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="K67" s="4" t="s">
         <v>299</v>
@@ -12312,7 +12312,7 @@
         <v>176</v>
       </c>
       <c r="C68" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="D68" t="s">
         <v>138</v>
@@ -12330,7 +12330,7 @@
         <v>209</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="K68" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B68&amp;" resources for the specified patient and a category code = `laboratory`"</f>
@@ -12345,7 +12345,7 @@
         <v>176</v>
       </c>
       <c r="C69" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="D69" t="s">
         <v>140</v>
@@ -12360,7 +12360,7 @@
         <v>212</v>
       </c>
       <c r="J69" s="8" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="K69" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B69&amp;" resources for the specified patient and observation code(s).  SHOULD support search by multiple report codes. The Observation `code` parameter searches `Observation.code only."</f>
@@ -12375,7 +12375,7 @@
         <v>176</v>
       </c>
       <c r="C70" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="D70" t="s">
         <v>187</v>
@@ -12393,7 +12393,7 @@
         <v>213</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="K70" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B70&amp;" resources for the specified patient and date and a category code = `laboratory`"</f>
@@ -12408,10 +12408,10 @@
         <v>176</v>
       </c>
       <c r="C71" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="D71" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="F71" t="s">
         <v>64</v>
@@ -12421,7 +12421,7 @@
       </c>
       <c r="I71" s="4"/>
       <c r="J71" s="27" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="K71" s="24" t="str">
         <f>"Fetches a bundle of all "&amp;B71&amp;" resources for the specified "&amp;SUBSTITUTE(D71,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
@@ -12436,7 +12436,7 @@
         <v>176</v>
       </c>
       <c r="C72" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="D72" t="s">
         <v>208</v>
@@ -12451,7 +12451,7 @@
         <v>211</v>
       </c>
       <c r="J72" s="4" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="K72" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B72&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
@@ -12815,7 +12815,7 @@
         <v>237</v>
       </c>
       <c r="C84" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="D84" t="s">
         <v>111</v>
@@ -12844,7 +12844,7 @@
         <v>237</v>
       </c>
       <c r="C85" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="D85" t="s">
         <v>109</v>
@@ -12856,13 +12856,13 @@
         <v>99</v>
       </c>
       <c r="I85" s="4" t="s">
+        <v>622</v>
+      </c>
+      <c r="J85" s="4" t="s">
         <v>623</v>
       </c>
-      <c r="J85" s="4" t="s">
+      <c r="K85" s="4" t="s">
         <v>624</v>
-      </c>
-      <c r="K85" s="4" t="s">
-        <v>625</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
@@ -13086,7 +13086,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C93" t="str">
         <f t="shared" si="5"/>
@@ -13102,10 +13102,10 @@
         <v>99</v>
       </c>
       <c r="I93" t="s">
+        <v>585</v>
+      </c>
+      <c r="J93" s="4" t="s">
         <v>586</v>
-      </c>
-      <c r="J93" s="4" t="s">
-        <v>587</v>
       </c>
       <c r="K93" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B93&amp;" resources for the specified "&amp;SUBSTITUTE(D93,","," and ")</f>
@@ -13117,14 +13117,14 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C94" t="str">
         <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="D94" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="F94" t="s">
         <v>64</v>
@@ -13133,13 +13133,13 @@
         <v>99</v>
       </c>
       <c r="H94" t="s">
+        <v>588</v>
+      </c>
+      <c r="I94" t="s">
+        <v>585</v>
+      </c>
+      <c r="J94" s="4" t="s">
         <v>589</v>
-      </c>
-      <c r="I94" t="s">
-        <v>586</v>
-      </c>
-      <c r="J94" s="4" t="s">
-        <v>590</v>
       </c>
       <c r="K94" t="str">
         <f>"Fetches a bundle of all "&amp;B94&amp;" resources for the specified "&amp;SUBSTITUTE(D94,","," and  ") &amp; "= 'sdoh'"</f>
@@ -13151,14 +13151,14 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C95" t="str">
         <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D95" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="F95" t="s">
         <v>64</v>
@@ -13167,10 +13167,10 @@
         <v>142</v>
       </c>
       <c r="I95" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="J95" s="4" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="K95" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient and date"</f>
@@ -13182,14 +13182,14 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C96" t="str">
         <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="D96" s="16" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F96" t="s">
         <v>64</v>
@@ -13198,13 +13198,13 @@
         <v>207</v>
       </c>
       <c r="H96" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="I96" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="J96" s="4" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="K96" t="str">
         <f>"Fetches a bundle of all "&amp;B96&amp;" resources tagged as 'sdoh' for the specified patient and date"</f>
@@ -13216,14 +13216,14 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C97" t="str">
         <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D97" s="16" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="F97" t="s">
         <v>64</v>
@@ -13232,10 +13232,10 @@
         <v>84</v>
       </c>
       <c r="I97" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="J97" s="4" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="K97" t="str">
         <f>"Fetches a bundle of all "&amp;B97&amp;" resources for the specified patient that have been completed against a specified form."</f>
@@ -13247,7 +13247,7 @@
         <v>97</v>
       </c>
       <c r="B98" s="16" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C98" t="str">
         <f t="shared" si="5"/>
@@ -13265,10 +13265,10 @@
       </c>
       <c r="H98" s="16"/>
       <c r="I98" s="4" t="s">
+        <v>625</v>
+      </c>
+      <c r="J98" s="4" t="s">
         <v>626</v>
-      </c>
-      <c r="J98" s="4" t="s">
-        <v>627</v>
       </c>
       <c r="K98" t="str">
         <f>"Fetches a bundle of all "&amp;B98&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed))."</f>
@@ -13280,7 +13280,7 @@
         <v>98</v>
       </c>
       <c r="B99" s="16" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C99" t="str">
         <f t="shared" si="5"/>
@@ -13298,10 +13298,10 @@
       </c>
       <c r="H99" s="16"/>
       <c r="I99" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="J99" s="4" t="s">
         <v>628</v>
-      </c>
-      <c r="J99" s="4" t="s">
-        <v>629</v>
       </c>
       <c r="K99" t="str">
         <f>"Fetches a bundle of all "&amp;B99&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed) and type of dispense (e.g., partially dispensed)."</f>
@@ -13313,14 +13313,14 @@
         <v>99</v>
       </c>
       <c r="B100" s="16" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C100" t="str">
         <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationdispense</v>
       </c>
       <c r="D100" s="16" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="E100" s="16"/>
       <c r="F100" s="16" t="s">
@@ -13331,10 +13331,10 @@
       </c>
       <c r="H100" s="16"/>
       <c r="I100" s="4" t="s">
+        <v>630</v>
+      </c>
+      <c r="J100" s="4" t="s">
         <v>631</v>
-      </c>
-      <c r="J100" s="4" t="s">
-        <v>632</v>
       </c>
       <c r="K100" t="str">
         <f>"Fetches a bundle of all "&amp;B99&amp;" resources for the specified patient for a given dispense and date or range"</f>
@@ -13352,19 +13352,19 @@
         <v>509</v>
       </c>
       <c r="D101" s="16" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="E101" s="16"/>
       <c r="F101" s="16" t="s">
         <v>64</v>
       </c>
       <c r="G101" s="16" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="H101" s="16"/>
       <c r="I101" s="4"/>
       <c r="J101" s="4" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="K101" t="str">
         <f>"Fetches a bundle of all "&amp;B101&amp;" resources for the specified patient that may match any of the string fields in the name element (including family, give, prefix, suffix, suffix, and/or text)"</f>
@@ -13391,8 +13391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13422,7 +13422,7 @@
         <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>729</v>
+        <v>737</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -13462,7 +13462,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -13533,13 +13533,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>731</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>732</v>
+      </c>
+      <c r="C2" s="28" t="s">
         <v>733</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>734</v>
-      </c>
-      <c r="C2" s="28" t="s">
-        <v>735</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
@@ -13547,7 +13547,7 @@
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>505</v>
@@ -13630,7 +13630,7 @@
   <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13703,10 +13703,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B5" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
@@ -13717,10 +13717,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B6" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -13731,16 +13731,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>644</v>
+      </c>
+      <c r="B7" t="s">
         <v>645</v>
       </c>
-      <c r="B7" t="s">
-        <v>646</v>
-      </c>
       <c r="D7" t="s">
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -13801,7 +13801,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B12" t="s">
         <v>340</v>
@@ -13815,86 +13815,86 @@
     </row>
     <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
+        <v>565</v>
+      </c>
+      <c r="B13" t="s">
         <v>566</v>
       </c>
-      <c r="B13" t="s">
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
         <v>567</v>
-      </c>
-      <c r="D13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" t="s">
-        <v>568</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
+        <v>568</v>
+      </c>
+      <c r="B14" t="s">
         <v>569</v>
       </c>
-      <c r="B14" t="s">
-        <v>570</v>
-      </c>
       <c r="D14" t="s">
         <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
+        <v>570</v>
+      </c>
+      <c r="B15" t="s">
         <v>571</v>
       </c>
-      <c r="B15" t="s">
-        <v>572</v>
-      </c>
       <c r="D15" t="s">
         <v>11</v>
       </c>
       <c r="E15" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
+        <v>572</v>
+      </c>
+      <c r="B16" t="s">
         <v>573</v>
       </c>
-      <c r="B16" t="s">
-        <v>574</v>
-      </c>
       <c r="D16" t="s">
         <v>11</v>
       </c>
       <c r="E16" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
+        <v>574</v>
+      </c>
+      <c r="B17" t="s">
         <v>575</v>
       </c>
-      <c r="B17" t="s">
-        <v>576</v>
-      </c>
       <c r="D17" t="s">
         <v>11</v>
       </c>
       <c r="E17" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B18" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D18" t="s">
         <v>11</v>
       </c>
       <c r="E18" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -13969,16 +13969,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>646</v>
+      </c>
+      <c r="B24" t="s">
         <v>647</v>
       </c>
-      <c r="B24" t="s">
-        <v>648</v>
-      </c>
       <c r="D24" t="s">
         <v>11</v>
       </c>
       <c r="E24" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -13997,10 +13997,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>648</v>
+      </c>
+      <c r="B26" t="s">
         <v>649</v>
-      </c>
-      <c r="B26" t="s">
-        <v>650</v>
       </c>
       <c r="D26" t="s">
         <v>11</v>
@@ -14011,10 +14011,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>650</v>
+      </c>
+      <c r="B27" t="s">
         <v>651</v>
-      </c>
-      <c r="B27" t="s">
-        <v>652</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
@@ -14025,10 +14025,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>652</v>
+      </c>
+      <c r="B28" t="s">
         <v>653</v>
-      </c>
-      <c r="B28" t="s">
-        <v>654</v>
       </c>
       <c r="D28" t="s">
         <v>11</v>
@@ -14039,10 +14039,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="18" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B29" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="D29" t="s">
         <v>11</v>
@@ -14067,10 +14067,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B31" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="D31" t="s">
         <v>11</v>
@@ -14081,10 +14081,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>694</v>
+      </c>
+      <c r="B32" t="s">
         <v>695</v>
-      </c>
-      <c r="B32" t="s">
-        <v>696</v>
       </c>
       <c r="D32" t="s">
         <v>11</v>
@@ -14095,10 +14095,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>696</v>
+      </c>
+      <c r="B33" t="s">
         <v>697</v>
-      </c>
-      <c r="B33" t="s">
-        <v>698</v>
       </c>
       <c r="D33" t="s">
         <v>11</v>
@@ -14182,10 +14182,10 @@
         <v>508</v>
       </c>
       <c r="B39" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D39" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E39" t="s">
         <v>176</v>
@@ -14235,10 +14235,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B43" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D43" t="s">
         <v>11</v>
@@ -14249,10 +14249,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>692</v>
+      </c>
+      <c r="B44" t="s">
         <v>693</v>
-      </c>
-      <c r="B44" t="s">
-        <v>694</v>
       </c>
       <c r="D44" t="s">
         <v>11</v>
@@ -14277,10 +14277,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="18" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B46" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D46" t="s">
         <v>11</v>
@@ -14291,10 +14291,10 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B47" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D47" t="s">
         <v>11</v>
@@ -14322,7 +14322,7 @@
         <v>467</v>
       </c>
       <c r="B49" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="D49" t="s">
         <v>11</v>
@@ -14445,30 +14445,30 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B58" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="D58" t="s">
         <v>11</v>
       </c>
       <c r="E58" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B59" t="s">
+        <v>580</v>
+      </c>
+      <c r="D59" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59" t="s">
         <v>581</v>
-      </c>
-      <c r="D59" t="s">
-        <v>11</v>
-      </c>
-      <c r="E59" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -14501,16 +14501,16 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>658</v>
+      </c>
+      <c r="B62" t="s">
         <v>659</v>
       </c>
-      <c r="B62" t="s">
+      <c r="D62" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" t="s">
         <v>660</v>
-      </c>
-      <c r="D62" t="s">
-        <v>11</v>
-      </c>
-      <c r="E62" t="s">
-        <v>661</v>
       </c>
     </row>
   </sheetData>
@@ -14528,7 +14528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{352F3A6C-0DAD-1041-B50E-04478951E07A}">
   <dimension ref="A1:Y69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C9" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView topLeftCell="C9" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -14650,7 +14650,7 @@
         <v>64</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="X3" s="13" t="s">
         <v>424</v>
@@ -14667,7 +14667,7 @@
         <v>64</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="V4" t="s">
         <v>515</v>
@@ -14690,7 +14690,7 @@
         <v>64</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="X5" s="13" t="s">
         <v>424</v>
@@ -14701,7 +14701,7 @@
     </row>
     <row r="6" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B6" t="s">
         <v>64</v>
@@ -14721,7 +14721,7 @@
         <v>64</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="X7" s="13" t="s">
         <v>424</v>
@@ -14738,7 +14738,7 @@
         <v>64</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="X8" s="13" t="s">
         <v>424</v>
@@ -14755,7 +14755,7 @@
         <v>64</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
       <c r="X9" s="13" t="s">
         <v>424</v>
@@ -14772,7 +14772,7 @@
         <v>64</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="X10" s="13" t="s">
         <v>424</v>
@@ -14783,13 +14783,13 @@
     </row>
     <row r="11" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B11" t="s">
         <v>64</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="X11" s="13"/>
       <c r="Y11" s="13"/>
@@ -14802,7 +14802,7 @@
         <v>64</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="X12" s="13" t="s">
         <v>424</v>
@@ -14813,13 +14813,13 @@
     </row>
     <row r="13" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B13" t="s">
         <v>28</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="X13" s="13"/>
       <c r="Y13" s="13"/>
@@ -14832,7 +14832,7 @@
         <v>64</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="X14" s="13" t="s">
         <v>424</v>
@@ -14849,20 +14849,20 @@
         <v>64</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="X15" s="13"/>
       <c r="Y15" s="13"/>
     </row>
     <row r="16" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B16" t="s">
         <v>64</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="X16" s="13"/>
       <c r="Y16" s="13"/>
@@ -14888,7 +14888,7 @@
         <v>64</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="V18" t="s">
         <v>64</v>
@@ -14905,19 +14905,19 @@
     </row>
     <row r="19" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>613</v>
+      </c>
+      <c r="B19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>721</v>
+      </c>
+      <c r="V19" t="s">
+        <v>64</v>
+      </c>
+      <c r="W19" s="6" t="s">
         <v>614</v>
-      </c>
-      <c r="B19" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>722</v>
-      </c>
-      <c r="V19" t="s">
-        <v>64</v>
-      </c>
-      <c r="W19" s="6" t="s">
-        <v>615</v>
       </c>
       <c r="X19" s="13" t="s">
         <v>424</v>
@@ -14957,7 +14957,7 @@
         <v>64</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="X21" s="13" t="s">
         <v>424</v>
@@ -14974,7 +14974,7 @@
         <v>64</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="X22" s="13"/>
       <c r="Y22" s="13"/>
@@ -14987,7 +14987,7 @@
         <v>64</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="X23" s="13" t="s">
         <v>424</v>
@@ -15004,7 +15004,7 @@
         <v>64</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="X24" s="13"/>
       <c r="Y24" s="13"/>
@@ -15017,7 +15017,7 @@
         <v>64</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="V25" t="s">
         <v>504</v>
@@ -15036,7 +15036,7 @@
         <v>64</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="X26" s="13" t="s">
         <v>424</v>
@@ -15053,31 +15053,31 @@
         <v>64</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="28" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B28" t="s">
         <v>64</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="X28" s="13"/>
       <c r="Y28" s="13"/>
     </row>
     <row r="29" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B29" t="s">
         <v>64</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="X29" s="13" t="s">
         <v>424</v>
@@ -15094,7 +15094,7 @@
         <v>64</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="X30" s="13" t="s">
         <v>424</v>
@@ -15111,7 +15111,7 @@
         <v>64</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="X31" s="13" t="s">
         <v>424</v>
@@ -15122,13 +15122,13 @@
     </row>
     <row r="32" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B32" t="s">
         <v>64</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="X32" s="13"/>
       <c r="Y32" s="13"/>
@@ -15224,7 +15224,7 @@
         <v>64</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -15277,7 +15277,7 @@
         <v>346</v>
       </c>
       <c r="F1" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="G1" t="s">
         <v>347</v>
@@ -15295,13 +15295,13 @@
         <v>350</v>
       </c>
       <c r="L1" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="M1" t="s">
         <v>351</v>
       </c>
       <c r="N1" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="O1" t="s">
         <v>352</v>
@@ -15310,13 +15310,13 @@
         <v>353</v>
       </c>
       <c r="Q1" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="R1" t="s">
         <v>354</v>
       </c>
       <c r="S1" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="T1" t="s">
         <v>355</v>
@@ -15349,10 +15349,10 @@
         <v>409</v>
       </c>
       <c r="AD1" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="AE1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="AF1" t="s">
         <v>517</v>
@@ -15364,7 +15364,7 @@
         <v>423</v>
       </c>
       <c r="AI1" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
**Pre-Applied:** (Correction) Remove gender based search requirements [FHIR-50380](https://jira.hl7.org/browse/FHIR-50288) update must support tables
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA6B28D-EA6A-8D44-86E2-640B7711D3B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A6A5500-6C47-444E-A346-C0A6E7451B74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34340" yWindow="500" windowWidth="36700" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34340" yWindow="500" windowWidth="36700" windowHeight="28300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -2330,21 +2330,6 @@
 * Systems **SHOULD** follow the Project US@ Technical Specification for Patient Addresses Final Version 1.0 as the standard style guide for `Organization.address.line` and  `Organization.address.city`.</t>
   </si>
   <si>
-    <t>* For ONC's USCDI requirements, each Patient must support the following additional elements. These elements are included in the formal definition of the profile. The patient examples include all of these elements.
-  1. contact detail (e.g. a telephone number or an email address)
-  1. a communication language
-  1. a race
-  1. an ethnicity
-  1. a birth sex*
-  1. previous name
-     - Previous name is represented by providing an end date in the `Patient.name.period` element for a previous name.
-  1. suffix
-     - Suffix is represented using the `Patient.name.suffix` element.
-* The Patient's Social Security Numbers **SHOULD NOT** be used as a patient identifier in `Patient.identifier.value`.
-* Although Patient.deceased[x] is marked as 𝗔𝗗𝗗𝗜𝗧𝗜𝗢𝗡𝗔𝗟 𝗨𝗦𝗖𝗗𝗜, certifying systems are not required to support both choices, but **SHALL** support at least `Patient.deceasedDateTime`.
-* Certifying systems **SHALL** and non-certifying systems **SHOULD** follow the Project US@ Technical Specification for Patient Addresses Final Version 1.0 as the standard style guide for `Patient.address.line` and  `Patient.address.city` for new and updated records.</t>
-  </si>
-  <si>
     <t xml:space="preserve">* Servers that support only US Core Practitioner Profile **SHALL** provide implementation specific guidance how to access a provider’s location and contact information using only the Practitioner resource.
    * Although Practitioner.address is marked as Must Support, the server system is not required to support it if they support the US Core PractitionerRole Profile, but **SHALL** support it if they do not support the US Core PractitionerRole Profile. The client application **SHALL** support both.
 * Systems **SHOULD** follow the Project US@ Technical Specification for Patient Addresses Final Version 1.0 as the standard style guide for `Practitioner.address.line` and  `Practitioner.address.city`.
@@ -2521,6 +2506,11 @@
   </si>
   <si>
     <t>/Users/ehaas/Documents/FHIR/US-Core/input/</t>
+  </si>
+  <si>
+    <t>* The Patient's Social Security Numbers **SHOULD NOT** be used as a patient identifier in `Patient.identifier.value`.
+* Although Patient.deceased[x] is marked as 𝗔𝗗𝗗𝗜𝗧𝗜𝗢𝗡𝗔𝗟 𝗨𝗦𝗖𝗗𝗜, certifying systems are not required to support both choices, but **SHALL** support at least `Patient.deceasedDateTime`.
+* Certifying systems **SHALL** and non-certifying systems **SHOULD** follow the Project US@ Technical Specification for Patient Addresses Final Version 1.0 as the standard style guide for `Patient.address.line` and  `Patient.address.city` for new and updated records.</t>
   </si>
 </sst>
 </file>
@@ -3137,7 +3127,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40F68824-E615-4729-AAE0-A6F75FBDE06B}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="400" zoomScaleNormal="400" workbookViewId="0">
+    <sheetView zoomScale="400" zoomScaleNormal="400" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -3160,7 +3150,7 @@
         <v>437</v>
       </c>
       <c r="B2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -3229,10 +3219,10 @@
   <dimension ref="A1:AB132"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B69" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F62" sqref="F62"/>
+      <selection pane="bottomRight" activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5546,7 +5536,7 @@
         <v>0</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="G44" t="str">
         <f t="shared" si="0"/>
@@ -5975,7 +5965,7 @@
         <v>0</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="G52" t="str">
         <f t="shared" si="0"/>
@@ -6672,7 +6662,7 @@
         <v>0</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="G65" t="str">
         <f t="shared" si="0"/>
@@ -8279,7 +8269,7 @@
         <v>0</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="G95" t="str">
         <f t="shared" si="6"/>
@@ -8734,7 +8724,7 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
       <c r="C104" t="s">
         <v>74</v>
@@ -8750,7 +8740,7 @@
       </c>
       <c r="G104" t="str">
         <f t="shared" si="6"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!patient</v>
       </c>
       <c r="H104" t="s">
         <v>51</v>
@@ -8763,7 +8753,7 @@
       </c>
       <c r="L104" t="str">
         <f>B104&amp;"."&amp;C104</f>
-        <v>Patient.gender</v>
+        <v>!Patient.gender</v>
       </c>
       <c r="M104" t="s">
         <v>51</v>
@@ -8774,7 +8764,7 @@
       <c r="AA104" s="8"/>
       <c r="AB104" t="str">
         <f t="shared" si="4"/>
-        <v>SearchParameter-us-core-patient-gender.html</v>
+        <v>SearchParameter-us-core-!patient-gender.html</v>
       </c>
     </row>
     <row r="105" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -10327,10 +10317,10 @@
   <dimension ref="A1:K101"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E18" sqref="E18"/>
+      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11285,11 +11275,11 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
       <c r="C35" t="str">
         <f t="shared" si="0"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!patient</v>
       </c>
       <c r="D35" t="s">
         <v>129</v>
@@ -11308,7 +11298,7 @@
       </c>
       <c r="K35" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>Fetches a bundle of all Patient resources matching the specified family and gender</v>
+        <v>Fetches a bundle of all !Patient resources matching the specified family and gender</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
@@ -11316,11 +11306,11 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
       <c r="C36" t="str">
         <f t="shared" si="0"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!patient</v>
       </c>
       <c r="D36" t="s">
         <v>130</v>
@@ -11339,7 +11329,7 @@
       </c>
       <c r="K36" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>Fetches a bundle of all Patient resources matching the specified gender and name</v>
+        <v>Fetches a bundle of all !Patient resources matching the specified gender and name</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
@@ -11640,7 +11630,7 @@
       </c>
       <c r="I46" s="4"/>
       <c r="J46" s="24" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="K46" s="24" t="str">
         <f>"Fetches a bundle of all "&amp;B46&amp;" resources for the specified "&amp;SUBSTITUTE(D46,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
@@ -13422,7 +13412,7 @@
         <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -13454,7 +13444,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -13533,13 +13523,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>730</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>731</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="C2" s="28" t="s">
         <v>732</v>
-      </c>
-      <c r="C2" s="28" t="s">
-        <v>733</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
@@ -13629,8 +13619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AFD1E51-334E-C94B-9199-BB3C0A09D724}">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14528,8 +14518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{352F3A6C-0DAD-1041-B50E-04478951E07A}">
   <dimension ref="A1:Y69"/>
   <sheetViews>
-    <sheetView topLeftCell="C9" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A13" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="23" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -14650,7 +14640,7 @@
         <v>64</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="X3" s="13" t="s">
         <v>424</v>
@@ -14667,7 +14657,7 @@
         <v>64</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="V4" t="s">
         <v>515</v>
@@ -14690,7 +14680,7 @@
         <v>64</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="X5" s="13" t="s">
         <v>424</v>
@@ -14738,7 +14728,7 @@
         <v>64</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="X8" s="13" t="s">
         <v>424</v>
@@ -14755,7 +14745,7 @@
         <v>64</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="X9" s="13" t="s">
         <v>424</v>
@@ -14789,7 +14779,7 @@
         <v>64</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="X11" s="13"/>
       <c r="Y11" s="13"/>
@@ -14819,7 +14809,7 @@
         <v>28</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="X13" s="13"/>
       <c r="Y13" s="13"/>
@@ -14862,7 +14852,7 @@
         <v>64</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="X16" s="13"/>
       <c r="Y16" s="13"/>
@@ -14888,7 +14878,7 @@
         <v>64</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="V18" t="s">
         <v>64</v>
@@ -14911,7 +14901,7 @@
         <v>64</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="V19" t="s">
         <v>64</v>
@@ -14957,7 +14947,7 @@
         <v>64</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="X21" s="13" t="s">
         <v>424</v>
@@ -14979,7 +14969,7 @@
       <c r="X22" s="13"/>
       <c r="Y22" s="13"/>
     </row>
-    <row r="23" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" ht="97" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -14987,7 +14977,7 @@
         <v>64</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>713</v>
+        <v>738</v>
       </c>
       <c r="X23" s="13" t="s">
         <v>424</v>
@@ -15004,7 +14994,7 @@
         <v>64</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="X24" s="13"/>
       <c r="Y24" s="13"/>
@@ -15036,7 +15026,7 @@
         <v>64</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="X26" s="13" t="s">
         <v>424</v>
@@ -15064,7 +15054,7 @@
         <v>64</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="X28" s="13"/>
       <c r="Y28" s="13"/>
@@ -15077,7 +15067,7 @@
         <v>64</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="X29" s="13" t="s">
         <v>424</v>
@@ -15094,7 +15084,7 @@
         <v>64</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="X30" s="13" t="s">
         <v>424</v>
@@ -15111,7 +15101,7 @@
         <v>64</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="X31" s="13" t="s">
         <v>424</v>
@@ -15128,7 +15118,7 @@
         <v>64</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="X32" s="13"/>
       <c r="Y32" s="13"/>

</xml_diff>

<commit_message>
Change binding for US Core ADI DocumentReference  and .type [FHIR-49615 Update guidance if endpoint is outside the FHIR base URL [FHIR-49424] Clarify guidance for the Observation ADI Documentation Profile Observation.value element [FHIR-494 Define the Acronym 'ADI' in all pages where it is used [FHIR-49299
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A6A5500-6C47-444E-A346-C0A6E7451B74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA93E15-81CC-7C42-BB9F-55D17ED468EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34340" yWindow="500" windowWidth="36700" windowHeight="28300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34340" yWindow="500" windowWidth="36700" windowHeight="28300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -2477,16 +2477,6 @@
     <t>https://hl7.org/fhir/smart-app-launch/STU2/</t>
   </si>
   <si>
-    <t>* The `DocumentReference.type` binding **SHALL** support at a minimum the [10 Common Clinical Notes](ValueSet-us-core-clinical-note-type.html) and may extend to the full US Core DocumentReference Type Value Set
-* The DocumentReference resources can represent the referenced content using either an address where the document can be retrieved using `DocumentReference.attachment.url` or the content as inline base64 encoded data using `DocumentReference.attachment.data`.
-    *  Although both are marked as must support, the server system is not required to support an address, and inline base64 encoded data, but **SHALL** support at least one of these elements.
-    *  The client application **SHALL** support both elements.
-    *  The `content.attachment.url` may refer to a FHIR Binary Resource (i.e. [base]/Binary/[id]), FHIR Document Bundle (i.e [base]/Bundle/[id] or another endpoint.
-        * If the endpoint is outside the FHIR base URL, it **SHOULD NOT** require additional authorization to access.
-   * If there are multiple `DocumentReference.content` element repetitions, these **SHALL** all represent the same document in different format or attachment metadata. The content element **SHALL NOT** contain different versions of the same content. For version handling use multiple DocumentReferences with `DocumentReference.relatesTo`
-* Every DocumentReference must have a responsible Organization. The organization responsible for the DocumentReference **SHALL** be present either in `DocumentReference.custodian` or accessible in the Provenance resource targeting the DocumentReference using `Provenance.agent.who` or `Provenance.agent.onBehalfOf`.</t>
-  </si>
-  <si>
     <t>The HealthcareService Resource is a referenced resource when using the US Core PractitionerRole Profile and subject to constraint us-core-13: "SHALL have a practitioner, an organization, a healthcare service, or a location."</t>
   </si>
   <si>
@@ -2511,6 +2501,15 @@
     <t>* The Patient's Social Security Numbers **SHOULD NOT** be used as a patient identifier in `Patient.identifier.value`.
 * Although Patient.deceased[x] is marked as 𝗔𝗗𝗗𝗜𝗧𝗜𝗢𝗡𝗔𝗟 𝗨𝗦𝗖𝗗𝗜, certifying systems are not required to support both choices, but **SHALL** support at least `Patient.deceasedDateTime`.
 * Certifying systems **SHALL** and non-certifying systems **SHOULD** follow the Project US@ Technical Specification for Patient Addresses Final Version 1.0 as the standard style guide for `Patient.address.line` and  `Patient.address.city` for new and updated records.</t>
+  </si>
+  <si>
+    <t>* The `DocumentReference.type` binding **SHALL** support at a minimum the [10 Common Clinical Notes](ValueSet-us-core-clinical-note-type.html) and may extend to the full US Core DocumentReference Type Value Set
+* The DocumentReference resources can represent the referenced content using either an address where the document can be retrieved using `DocumentReference.attachment.url` or the content as inline base64 encoded data using `DocumentReference.attachment.data`.
+    *  Although both are marked as must support, the server system is not required to support an address, and inline base64 encoded data, but **SHALL** support at least one of these elements.
+    *  The client application **SHALL** support both elements.
+    *  The `content.attachment.url` may refer to a FHIR Binary Resource (i.e. [base]/Binary/[id]), FHIR Document Bundle (i.e [base]/Bundle/[id] or another endpoint.
+   * If there are multiple `DocumentReference.content` element repetitions, these **SHALL** all represent the same document in different format or attachment metadata. The content element **SHALL NOT** contain different versions of the same content. For version handling use multiple DocumentReferences with `DocumentReference.relatesTo`
+* Every DocumentReference must have a responsible Organization. The organization responsible for the DocumentReference **SHALL** be present either in `DocumentReference.custodian` or accessible in the Provenance resource targeting the DocumentReference using `Provenance.agent.who` or `Provenance.agent.onBehalfOf`.</t>
   </si>
 </sst>
 </file>
@@ -3150,7 +3149,7 @@
         <v>437</v>
       </c>
       <c r="B2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -13412,7 +13411,7 @@
         <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -13444,7 +13443,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -13619,7 +13618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AFD1E51-334E-C94B-9199-BB3C0A09D724}">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -14518,8 +14517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{352F3A6C-0DAD-1041-B50E-04478951E07A}">
   <dimension ref="A1:Y69"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="23" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -14745,7 +14744,7 @@
         <v>64</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>733</v>
+        <v>738</v>
       </c>
       <c r="X9" s="13" t="s">
         <v>424</v>
@@ -14809,7 +14808,7 @@
         <v>28</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="X13" s="13"/>
       <c r="Y13" s="13"/>
@@ -14977,7 +14976,7 @@
         <v>64</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="X23" s="13" t="s">
         <v>424</v>

</xml_diff>

<commit_message>
FHIR-50399 add copyrights on Q's Change number of common clinical notes to 10 [FHIR-49413] Clarify how to categorize CDA documents[FHIR-49612
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A622B9C-00F7-C048-97FA-9D1225828595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{875244A9-7019-9643-9716-161EC571EDBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="44580" yWindow="500" windowWidth="36700" windowHeight="28300" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -121,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2768" uniqueCount="748">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2768" uniqueCount="749">
   <si>
     <t>Element</t>
   </si>
@@ -5229,12 +5229,224 @@
   <si>
     <t>Fetches a bundle of all DocumentReference resources for the specified patient and type and period. See the implementation notes above for how to access the actual document.</t>
   </si>
+  <si>
+    <r>
+      <t>GET [</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>base</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>]/Condition?patient=1032702&amp;category=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF800000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>{% if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> include</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">system </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF800000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>%}{{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>include</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">system </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF800000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>}}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>\|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF800000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>{% endif</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF800000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>%}{{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>include</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">category </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">| </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">default: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>'[category]'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF800000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>}}&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>encounter=Encounter/1036</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5361,12 +5573,6 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Menlo"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -13037,7 +13243,7 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13052,10 +13258,10 @@
   <dimension ref="A1:K101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I47" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="J33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I77" sqref="I77"/>
+      <selection pane="bottomRight" activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14187,7 +14393,7 @@
         <v>142</v>
       </c>
       <c r="J40" s="23" t="s">
-        <v>717</v>
+        <v>748</v>
       </c>
       <c r="K40" s="23" t="s">
         <v>721</v>
@@ -17246,7 +17452,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17882,7 +18088,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",A1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update US Core Location Type Value Set to meet industry use cases FHIR-49401 and FHIR-50937
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243373A1-7A6E-674A-A637-02542A2C40D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B69F2C-6DBD-E547-BCD2-B3DAE734E42A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44580" yWindow="500" windowWidth="36700" windowHeight="28300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44580" yWindow="500" windowWidth="36700" windowHeight="28300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -2306,24 +2306,6 @@
 </t>
   </si>
   <si>
-    <t>* Clients **SHALL** support at least one Condition Profile
-* For Encounter Diagnosis use the *US Core Condition Encounter Diagnosis Profile*.
-    * When `Condition.category` is "encounter-diagnosis" the encounter, **SHOULD** be referenced in `Condition.encounter`.
-* For Problems and Health Concerns use the *US Core Condition Problems and Health Concerns Profile*.
-    * When `Condition.category` is a "problems-list-item", the `Condition.clinicalStatus **SHOULD NOT** be unknown.
-* There is no single element in Condition that represents the date of diagnosis. It may be the assertedDate Extension, `Condition.onsetDateTime`, or `Condition.recordedDate`.
-    * Although all three are marked as must support, the server is not required to support all.
-	* A server **SHALL** support `Condition.recordedDate`.
-    * A server **SHALL** support at least one of the assertedDate Extension and `Condition.onsetDateTime`. A server may support both, which means they support all three elements.
-    * The client application **SHALL** support all three elements.</t>
-  </si>
-  <si>
-    <t>* Clients **SHALL** support at least one DiagnosticReport Profile
-* When `DiagnosticReport.category` is "LAB" the encounter, Updates to Meta.lastUpdated **SHOULD** reflect:
-    * New laboratory reports
-     * Changes in the status of laboratory reports including events that trigger the same status (e.g., amended → amended).</t>
-  </si>
-  <si>
     <t>A server **SHALL** document the types of changes that can be detected using this parameter.
 A client **SHALL** provide a value precise to the *second + time offset*.
 A server **SHALL** support a value precise to the *second + time offset*.</t>
@@ -5440,6 +5422,32 @@
   </si>
   <si>
     <t>https://hl7.org/fhir/smart-app-launch/index.html</t>
+  </si>
+  <si>
+    <t>* For Encounter Diagnosis use the *US Core Condition Encounter Diagnosis Profile*.
+  * When `Condition.category` is "encounter-diagnosis" the encounter, **SHOULD** be referenced in `Condition.encounter`.
+* For Problems and Health Concerns use the *US Core Condition Problems and Health Concerns Profile*.
+  * When `Condition.category` is a "problems-list-item", the `Condition.clinicalStatus **SHOULD** be present.
+  * There is no single element in Condition that represents the date of diagnosis. It may be the assertedDate Extension, `Condition.onsetDateTime`, or `Condition.recordedDate`.
+      * Although all three are marked as must support, the server is not required to support all.
+  	* A server **SHALL** support `Condition.recordedDate`.
+      * A server **SHALL** support at least one of the assertedDate Extension and `Condition.onsetDateTime`. A server may support both, which means they support all three elements.
+      * The client application **SHALL** support all three elements.
+  * See the US Core General Guidance page for [Searching Using lastUpdated](general-guidance.html#searching-using-lastupdated). Updates to `.meta.lastUpdated` **SHOULD** reflect:
+    * New problems and health concerns
+    * Changes in the clinical status or verifications status of problems or health concerns</t>
+  </si>
+  <si>
+    <t>* For laboratory result reports use the *US Core DiagnosticReport Profile for Laboratory Results Reporting Profile*.
+  * Updates to `.meta.lastUpdated` **SHOULD** reflect:
+    * New laboratory reports
+    * Changes in the status of laboratory reports including events that trigger the same status (e.g., amended → amended).
+* For imaging and non-laboratory clinical test result reports use the *US Core DiagnosticReport Profile for Report and Note Exchange Profile*.
+  * Diagnostic imaging results in visual images requiring interpretation and clinical test results/reports may also reference images as part of the report. There is no single approach for accessing imaging studies alongside clinical data using a single authorization flow to give patients and providers access to the images.
+     * The `DiagnosticReport.media.link` element **SHOULD** be used to support links to various patient-friendly content, such as jpg images of x-rays (see the DiagnosticReport Chest X-ray Report Example).
+     * The `DiagnosticReport.imagingStudy` element **SHOULD** be used to support exchange with systems that can view DICOM (Digital Imaging and Communications in Medicine) studies, series, and SOP (Service-Object Pair) instances referenced in the [ImagingStudy] resource.
+     * Alternatively, systems can use business identifiers such as accession numbers in the `identifier` element to access the source images from external sources.
+* The `DiagnosticRequest.basedOn` element connects the DiagnosticReport to the originating order in the EHR. Systems that initiate the order **SHOULD** use this element when reporting the results.</t>
   </si>
 </sst>
 </file>
@@ -6091,7 +6099,7 @@
         <v>424</v>
       </c>
       <c r="B2" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -8477,7 +8485,7 @@
         <v>0</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="G44" t="str">
         <f t="shared" si="0"/>
@@ -8906,7 +8914,7 @@
         <v>0</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="G52" t="str">
         <f t="shared" si="0"/>
@@ -9603,7 +9611,7 @@
         <v>0</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="G65" t="str">
         <f t="shared" si="0"/>
@@ -11210,7 +11218,7 @@
         <v>0</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="G95" t="str">
         <f t="shared" si="6"/>
@@ -14303,7 +14311,7 @@
         <v>296</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14330,10 +14338,10 @@
         <v>142</v>
       </c>
       <c r="J38" s="23" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="K38" s="23" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14363,10 +14371,10 @@
         <v>654</v>
       </c>
       <c r="J39" s="23" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="K39" s="23" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14393,10 +14401,10 @@
         <v>142</v>
       </c>
       <c r="J40" s="23" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="K40" s="23" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14423,7 +14431,7 @@
         <v>143</v>
       </c>
       <c r="J41" s="23" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="K41" s="4" t="s">
         <v>144</v>
@@ -14453,7 +14461,7 @@
         <v>145</v>
       </c>
       <c r="J42" s="23" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="K42" s="4" t="s">
         <v>148</v>
@@ -14483,7 +14491,7 @@
         <v>145</v>
       </c>
       <c r="J43" s="23" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="K43" s="4" t="s">
         <v>148</v>
@@ -14513,7 +14521,7 @@
         <v>145</v>
       </c>
       <c r="J44" s="23" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="K44" s="4" t="s">
         <v>148</v>
@@ -14543,7 +14551,7 @@
         <v>145</v>
       </c>
       <c r="J45" s="23" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="K45" s="4" t="s">
         <v>148</v>
@@ -14571,7 +14579,7 @@
       </c>
       <c r="I46" s="4"/>
       <c r="J46" s="23" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="K46" s="23" t="str">
         <f>"Fetches a bundle of all "&amp;B46&amp;" resources for the specified "&amp;SUBSTITUTE(D46,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
@@ -14693,10 +14701,10 @@
         <v>189</v>
       </c>
       <c r="J50" s="23" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="K50" s="23" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14722,10 +14730,10 @@
         <v>184</v>
       </c>
       <c r="J51" s="23" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="K51" s="23" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14751,10 +14759,10 @@
         <v>206</v>
       </c>
       <c r="J52" s="23" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="K52" s="23" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14780,10 +14788,10 @@
         <v>186</v>
       </c>
       <c r="J53" s="23" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="K53" s="23" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14808,10 +14816,10 @@
       </c>
       <c r="I54" s="4"/>
       <c r="J54" s="23" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="K54" s="23" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14837,10 +14845,10 @@
         <v>210</v>
       </c>
       <c r="J55" s="23" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="K55" s="23" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
@@ -15563,10 +15571,10 @@
         <v>266</v>
       </c>
       <c r="J78" s="23" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="K78" s="23" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
     <row r="79" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -15593,7 +15601,7 @@
         <v>266</v>
       </c>
       <c r="K79" s="23" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
     </row>
     <row r="80" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -15620,10 +15628,10 @@
         <v>267</v>
       </c>
       <c r="J80" s="23" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="K80" s="23" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
     </row>
     <row r="81" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -15650,10 +15658,10 @@
         <v>268</v>
       </c>
       <c r="J81" s="23" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="K81" s="23" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
     </row>
     <row r="82" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -15680,7 +15688,7 @@
         <v>271</v>
       </c>
       <c r="J82" s="23" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="K82" s="23" t="s">
         <v>269</v>
@@ -15710,10 +15718,10 @@
         <v>272</v>
       </c>
       <c r="J83" s="23" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="K83" s="23" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
@@ -16331,7 +16339,7 @@
         <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -16363,7 +16371,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -16415,7 +16423,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A70CC787-78D8-4AA0-BE43-37746049F77C}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
@@ -16442,13 +16450,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>744</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>745</v>
+      </c>
+      <c r="C2" s="27" t="s">
         <v>746</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>747</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>748</v>
       </c>
       <c r="D2" t="s">
         <v>64</v>
@@ -16710,10 +16718,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="B12" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
@@ -16906,10 +16914,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="B26" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="D26" t="s">
         <v>11</v>
@@ -17465,8 +17473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{352F3A6C-0DAD-1041-B50E-04478951E07A}">
   <dimension ref="A1:Y69"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="23" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -17587,7 +17595,7 @@
         <v>64</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="X3" s="12" t="s">
         <v>412</v>
@@ -17627,7 +17635,7 @@
         <v>64</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>695</v>
+        <v>747</v>
       </c>
       <c r="X5" s="12" t="s">
         <v>412</v>
@@ -17675,7 +17683,7 @@
         <v>64</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>696</v>
+        <v>748</v>
       </c>
       <c r="X8" s="12" t="s">
         <v>412</v>
@@ -17692,7 +17700,7 @@
         <v>64</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="X9" s="12" t="s">
         <v>412</v>
@@ -17726,7 +17734,7 @@
         <v>64</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="X11" s="12"/>
       <c r="Y11" s="12"/>
@@ -17756,7 +17764,7 @@
         <v>28</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="X13" s="12"/>
       <c r="Y13" s="12"/>
@@ -17769,7 +17777,7 @@
         <v>64</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="X14" s="12" t="s">
         <v>412</v>
@@ -17799,7 +17807,7 @@
         <v>64</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="X16" s="12"/>
       <c r="Y16" s="12"/>
@@ -17924,7 +17932,7 @@
         <v>64</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="X23" s="12" t="s">
         <v>412</v>

</xml_diff>

<commit_message>
copyedit capabilitystatements, update Sequence from STU8 to STU 8
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B69F2C-6DBD-E547-BCD2-B3DAE734E42A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D35D1409-FEBB-8C49-8EAF-2E95DD486939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44580" yWindow="500" windowWidth="36700" windowHeight="28300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22600" yWindow="500" windowWidth="36700" windowHeight="28300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -2208,28 +2208,7 @@
     <t>GET [base]Observation?patient=555580&amp;code=http://loinc.org\|{{include.code1 | default: '[code]'}}&amp;date=ge2019-01-01T00:00:00Z</t>
   </si>
   <si>
-    <t xml:space="preserve">* The Encounter resource can represent a reason using either a code with `Encounter.reasonCode`, or a reference with `Encounter.reasonReference` to  Condition or other resource.
-   * Although both are marked as must support, the server systems are not required to support both a code and a reference, but they **SHALL** support *at least one* of these elements.
-   * The client application **SHALL** support both elements.
-   * if `Encounter.reasonReference` references an Observation, it **SHOULD** conform to a US Core Observation if applicable. (for example, a laboratory result should conform to the US Core Laboratory Result Observation Profile)
-* The location address can be represented by either by the Location referenced by `Encounter.location.location` or indirectly through the Organization referenced by `Encounter.serviceProvider`.
-   * Although both are marked as must support, the server systems are not required to support both `Encounter.location.location` and `Encounter.serviceProvider`, but they **SHALL** support *at least one* of these elements.
-   * The client application **SHALL** support both elements.
-* If the event facility/location differs from the `Encounter.location`, systems **SHOULD** reference it directly:
-</t>
-  </si>
-  <si>
     <t>* Systems **SHOULD** follow the Project US@ Technical Specification for Patient Addresses Final Version 1.0 as the standard style guide for `Location.address.line` and  `Location.address.city`.</t>
-  </si>
-  <si>
-    <t>* Systems **SHALL** support National Provider Identifier (NPI) for organizations and **SHOULD** support Clinical Laboratory Improvement Amendments (CLIA) identifiers for `Organization.Identifier`.
-* Systems **SHOULD** follow the Project US@ Technical Specification for Patient Addresses Final Version 1.0 as the standard style guide for `Organization.address.line` and  `Organization.address.city`.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Servers that support only US Core Practitioner Profile **SHALL** provide implementation specific guidance how to access a provider’s location and contact information using only the Practitioner resource.
-   * Although Practitioner.address is marked as Must Support, the server system is not required to support it if they support the US Core PractitionerRole Profile, but **SHALL** support it if they do not support the US Core PractitionerRole Profile. The client application **SHALL** support both.
-* Systems **SHOULD** follow the Project US@ Technical Specification for Patient Addresses Final Version 1.0 as the standard style guide for `Practitioner.address.line` and  `Practitioner.address.city`.
-</t>
   </si>
   <si>
     <t>* Procedure codes can be taken from SNOMED-CT, CPT, HCPCS II, ICD-10-PCS, CDT. LOINC.
@@ -2243,13 +2222,6 @@
   </si>
   <si>
     <t>* Systems **SHOULD** follow the Project US@ Technical Specification for Patient Addresses Final Version 1.0 as the standard style guide for `RelatedPerson.address.line` and  `RelatedPerson.address.city`.</t>
-  </si>
-  <si>
-    <t>* Servers and Clients **SHALL** support both US Core ServiceRequest and US Core Procedure Profiles for communicating the reason or justification for a referral as Additional USCDI Requirements. Typically, the reason or justification for a referral or consultation is communicated through `Procedure.basedOn` linking the Procedure to the US Core ServiceRequest Profile that includes either `ServiceRequest.reasonCode` or `ServiceRequest.reasonReference`. When the Procedure does not have an associated ServiceRequest, it is communicated through the US Core Procedure Profile's `Procedure.reasonCode` or `Procedure.reasonReference`.  Depending on the procedure being documented, a server will select the appropriate Profile to use.
-   * `ServiceRequest.reasonCode` and `ServiceRequest.reasonReference` are marked as Additional USCDI Requirements. The certifying server system is not required to support both but **SHALL** support at least one of these elements. The certifying client application **SHALL** support both elements.
-      * when using  `ServiceRequest.reasonReference`:
-         * Servers **SHALL** support *at least one* target resource in `ServiceRequest.reasonReference`. Clients **SHALL** support all target resources.
-         * The referenced resources **SHOULD** be a US Core Profile.</t>
   </si>
   <si>
     <t>* Although both `Specimen.identifier` and `Specimen.accessionIdentifier` are marked as Must Support, the server system is not required to support both, but **SHALL** support at least one of these elements. The client application **SHALL** support both.</t>
@@ -2266,44 +2238,10 @@
 * Servers that support only US Core Practitioner Profile and do not support the US Core PractitionerRole Profile **SHALL** provide implementation specific guidance how to access a provider’s location and contact information using only the Practitioner resource.</t>
   </si>
   <si>
-    <t>* The MedicationRequest resources can represent a medication using either a code or refer to the Medication resource. When referencing Medication, the resource may be [contained](http://hl7.org/fhir/R4/references.html#contained) or an external resource. The server application **MAY** choose any one way or more than one method, but if an external reference to Medication is used, the server **SHALL** support the _include` parameter for searching this element. The client application must support all methods.
-   * For example, A server **SHALL** be capable of returning all medications for a patient using one of or both:
-      *  `GET /MedicationRequest?patient=[id]`
-      *  `GET /MedicationRequest?patient=[id]&amp;_include=MedicationRequest:medication`
-* The MedicationRequest resource can represent that information is from a secondary source using either a boolean flag or reference in `MedicationRequest.reportedBoolean`, or a reference using `MedicationRequest.reportedReference` to Practitioner or other resource.
-   *   Although both are marked as must support, the server systems are not required to support both a boolean and a reference, but **SHALL** choose to support at least one of these elements.
-   *  The client application **SHALL** support both elements.
-* When recording “self-prescribed” medication, requester **SHOULD** be used to indicate the Patient or RelatedPerson as the prescriber. (See the Medication List section for guidance on accessing a patient medications including over the counter (OTC) medication and other substances taken for medical and recreational use.)
-* The MedicationRequest resource can communicate the reason or indication for treatment using either a code in MedicationRequest.reasonCode or a reference using MedicationRequest.reasonReference.
-* Although both `MedicationRequest.reasonCode` and `MedicationRequest.reasonReference` are marked as Additional USCDI Requirements. The certifying server system is not required to support both but **SHALL** support at least one of these elements. The certifying client application **SHALL** support both elements.
-   * when using MedicationRequest.reasonReference:
-       * Servers **SHALL** support at least one target resource in `MedicationRequest.reasonReference`. Clients **SHALL** support all target resources.
-      *  The referenced resources **SHOULD** be a US Core Profile as documented in Referencing US Core Profiles.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* The MedicationDispense resources can represent a medication using either a code or refer to the Medication resource. When referencing Medication, the resource may be [contained](http://hl7.org/fhir/R4/references.html#contained) or an external resource. The server application **MAY** choose any one way or more than one method, but if an external reference to Medication is used, the server **SHALL** support the _include` parameter for searching this element. The client application must support all methods.
-  * For example, A server **SHALL** be capable of returning dispense records for all medications for a patient using one of or both:
-     *  `GET /MedicationDispense?patient=[id]`
-     *  `GET /MedicationDispense?patient=[id]&amp;_include=MedicationDispense:medication`
-</t>
-  </si>
-  <si>
     <t>* US Core defines two ways to represent the questions and responses to screening and assessment instruments:
   - Observation: US Core Observation Screening Assessment Profile
   - Questionnaire/QuestionnaireResponse: SDC Base Questionnaire/US Core QuestionnaireResponse Profile
 * US Core Servers **SHALL** support US Core Observation Screening Assessment Profile and **SHOULD** support the  SDC Base Questionnaire Profile/US Core QuestionnaireResponse Profile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Clients **SHALL** support at least one Observation Profile
-* Systems **SHOULD** support `Observation.effectivePeriod` to accurately represent tests that are collected over a period of time (for example, a 24-Hour Urine Collection test).
-* An Observation without a value, **SHALL** include a reason why the data is absent unless there are component observations, or references to other Observations that are grouped within it
-    * Systems that never provide an observation without a value are not required to support `Observation.dataAbsentReason`
-*  An `Observation.component` without a value, **SHALL** include a reason why the data is absent.
-    * Systems that never provide an component observation without a component value are not required to support `Observation.component.dataAbsentReason`.
-* When `Observation.category` is "laboratory" the encounter, Updates to Meta.lastUpdated **SHOULD** reflect:
-    * New laboratory results
-     * Changes in the status of laboratory results including events that trigger the same status (e.g., amended → amended).
-</t>
   </si>
   <si>
     <t>A server **SHALL** document the types of changes that can be detected using this parameter.
@@ -2367,20 +2305,6 @@
     <t>/Users/ehaas/Documents/FHIR/US-Core/input/</t>
   </si>
   <si>
-    <t>* The Patient's Social Security Numbers **SHOULD NOT** be used as a patient identifier in `Patient.identifier.value`.
-* Although Patient.deceased[x] is marked as 𝗔𝗗𝗗𝗜𝗧𝗜𝗢𝗡𝗔𝗟 𝗨𝗦𝗖𝗗𝗜, certifying systems are not required to support both choices, but **SHALL** support at least `Patient.deceasedDateTime`.
-* Certifying systems **SHALL** and non-certifying systems **SHOULD** follow the Project US@ Technical Specification for Patient Addresses Final Version 1.0 as the standard style guide for `Patient.address.line` and  `Patient.address.city` for new and updated records.</t>
-  </si>
-  <si>
-    <t>* The `DocumentReference.type` binding **SHALL** support at a minimum the [10 Common Clinical Notes](ValueSet-us-core-clinical-note-type.html) and may extend to the full US Core DocumentReference Type Value Set
-* The DocumentReference resources can represent the referenced content using either an address where the document can be retrieved using `DocumentReference.attachment.url` or the content as inline base64 encoded data using `DocumentReference.attachment.data`.
-    *  Although both are marked as must support, the server system is not required to support an address, and inline base64 encoded data, but **SHALL** support at least one of these elements.
-    *  The client application **SHALL** support both elements.
-    *  The `content.attachment.url` may refer to a FHIR Binary Resource (i.e. [base]/Binary/[id]), FHIR Document Bundle (i.e [base]/Bundle/[id] or another endpoint.
-   * If there are multiple `DocumentReference.content` element repetitions, these **SHALL** all represent the same document in different format or attachment metadata. The content element **SHALL NOT** contain different versions of the same content. For version handling use multiple DocumentReferences with `DocumentReference.relatesTo`
-* Every DocumentReference must have a responsible Organization. The organization responsible for the DocumentReference **SHALL** be present either in `DocumentReference.custodian` or accessible in the Provenance resource targeting the DocumentReference using `Provenance.agent.who` or `Provenance.agent.onBehalfOf`.</t>
-  </si>
-  <si>
     <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-adi-documentreference</t>
   </si>
   <si>
@@ -5410,9 +5334,6 @@
       </rPr>
       <t>encounter=Encounter/1036</t>
     </r>
-  </si>
-  <si>
-    <t>* Based upon the ASTP U.S. Core Data for Interoperability (USCDI) requirements, CVX vaccine codes are required and the NDC vaccine codes **SHOULD** be supported as translations to them.</t>
   </si>
   <si>
     <t>SMART App Launch version  2.0.0 and later</t>
@@ -5433,9 +5354,9 @@
   	* A server **SHALL** support `Condition.recordedDate`.
       * A server **SHALL** support at least one of the assertedDate Extension and `Condition.onsetDateTime`. A server may support both, which means they support all three elements.
       * The client application **SHALL** support all three elements.
-  * See the US Core General Guidance page for [Searching Using lastUpdated](general-guidance.html#searching-using-lastupdated). Updates to `.meta.lastUpdated` **SHOULD** reflect:
+  * See the US Core General Guidance page for [Searching Using lastUpdated](general-guidance.html#searching-using-lastupdated). Updates to `Condition.meta.lastUpdated` **SHOULD** reflect:
     * New problems and health concerns
-    * Changes in the clinical status or verifications status of problems or health concerns</t>
+    * Changes in the clinical status or verifications status of problems or health concern</t>
   </si>
   <si>
     <t>* For laboratory result reports use the *US Core DiagnosticReport Profile for Laboratory Results Reporting Profile*.
@@ -5447,7 +5368,97 @@
      * The `DiagnosticReport.media.link` element **SHOULD** be used to support links to various patient-friendly content, such as jpg images of x-rays (see the DiagnosticReport Chest X-ray Report Example).
      * The `DiagnosticReport.imagingStudy` element **SHOULD** be used to support exchange with systems that can view DICOM (Digital Imaging and Communications in Medicine) studies, series, and SOP (Service-Object Pair) instances referenced in the [ImagingStudy] resource.
      * Alternatively, systems can use business identifiers such as accession numbers in the `identifier` element to access the source images from external sources.
-* The `DiagnosticRequest.basedOn` element connects the DiagnosticReport to the originating order in the EHR. Systems that initiate the order **SHOULD** use this element when reporting the results.</t>
+* The `DiagnosticRequest.basedOn` element connects the DiagnosticReport to the originating order in the EHR. Systems that initiate the lab order **SHOULD** use this element when reporting the results.</t>
+  </si>
+  <si>
+    <t>* For Advance Directive Information (ADI) documents use the *US Core ADI DocumentReference Profile*.
+* For other clinical documents use the *US Core DiagnosticReport Profile for Report and Note Exchange*.
+  * See the [Clinical Notes](clinical-notes.html) page for important definitions, requirements, and guidance on creating, using, and sharing Clinical Notes.
+  * The `DocumentReference.type` binding Must Support at a minimum the [10 Common Clinical Notes](ValueSet-us-core-clinical-note-type.html) and may extend to the full US Core DocumentReference Type Value Set
+* The DocumentReference resources can represent the referenced content using either an address where the document can be retrieved using `DocumentReference.attachment.url` or the content as inline base64 encoded data using `DocumentReference.attachment.data`.
+    *  Although both are marked as must support, the server system is not required to support an address, and inline base64 encoded data, but **SHALL** support at least one of these elements.
+    *  The client application **SHALL** support both elements.
+    *  The `content.attachment.url` may refer to a FHIR Binary Resource (i.e. [base]/Binary/[id]), FHIR Document Bundle (i.e [base]/Bundle/[id] or another endpoint.
+   * If there are multiple `DocumentReference.content` element repetitions, these **SHALL** all represent the same document in different format or attachment metadata. The content element **SHALL NOT** contain different versions of the same content. For version handling use multiple DocumentReferences with `DocumentReference.relatesTo`
+* Every DocumentReference must have a responsible Organization. The organization responsible for the DocumentReference **SHALL** be present either in `DocumentReference.custodian` or accessible in the Provenance resource targeting the DocumentReference using `Provenance.agent.who` or `Provenance.agent.onBehalfOf`.</t>
+  </si>
+  <si>
+    <t>* The Encounter resource can represent a reason using either a code with `Encounter.reasonCode`, or a reference with `Encounter.reasonReference` to  Condition or other resource.
+   * Although both are marked as must support, the server systems are not required to support both a code and a reference, but they **SHALL** support *at least one* of these elements.
+   * The client application **SHALL** support both elements.
+   * if `Encounter.reasonReference` references an Observation, it **SHOULD** conform to a US Core Observation if applicable. (for example, a laboratory result should conform to the US Core Laboratory Result Observation Profile)
+* The location address can be represented by either by the Location referenced by `Encounter.location.location` or indirectly through the Organization referenced by `Encounter.serviceProvider`.
+   * Although both are marked as must support, the server systems are not required to support both `Encounter.location.location` and `Encounter.serviceProvider`, but they **SHALL** support *at least one* of these elements.
+   * The client application **SHALL** support both elements.
+* If the event facility/location differs from the `Encounter.location`, systems **SHOULD** reference it directly:
+* Servers can use the US Core Interpreter Needed Extension on this profile or the [US Core Patient Profile] to communicate whether a patient needs an interpreter. Although the extension is marked as an *Additional USCDI Requirements* on both US Core Patient and US Core Encounter Profiles, the certifying Server system is not required to support the extension on both profiles, but **SHALL** support the extension on at least one. The certifying Client application **SHALL** support the extension on both profiles.
+  - Systems **SHOULD** designate the patient's preferred language in the `Patient.communication.preferred` element.
+* Updates to `.meta.lastUpdated` **SHOULD** reflect:
+  - New encounters/visits
+  - Changes in the status of encounters, including events that trigger the same status (e.g., in-progress → in-progress). These status changes correspond to events that can initiate [HL7 V2] ADT messages.</t>
+  </si>
+  <si>
+    <t>* Based upon the ASTP U.S. Core Data for Interoperability (USCDI) requirements, CVX vaccine codes are required and the NDC vaccine codes **SHOULD** be supported as an additional code.</t>
+  </si>
+  <si>
+    <t>* This Profile can represent a medication using a code or reference a Medication resource.
+  * The Server systems are not required to support both a code and a reference, but **SHALL** support at least one of these methods.
+  * The Client application **SHALL** support all methods.
+  * Systems that primarily rely on NDC codes instead of RxNorm to represent medications can use the National Library of Medicine's (NLM) NDC to RxNorm mappings to aid in additional codings.
+  * When referencing a Medication resource in `.medicationReference`, the resource may be contained or an external resource. If an external reference to a Medication resource is used, the Server **SHALL** support the `_include` parameter for searching this element. 
+* The MedicationRequest resource can represent that information is from a secondary source using either a boolean flag or reference in `MedicationRequest.reportedBoolean`, or a reference using `MedicationRequest.reportedReference` to Practitioner or other resource.
+   *  Although both are marked as must support, the server systems are not required to support both a boolean and a reference, but **SHALL** choose to support at least one of these elements.
+   *  The client application **SHALL** support both elements.
+* When recording “self-prescribed” medication, requester **SHOULD** be used to indicate the Patient or RelatedPerson as the prescriber. (See the Medication List section for guidance on accessing a patient medications including over the counter (OTC) medication and other substances taken for medical and recreational use.)
+* The MedicationRequest resource can communicate the reason or indication for treatment using either a code in MedicationRequest.reasonCode or a reference using MedicationRequest.reasonReference.
+  * Although both `MedicationRequest.reasonCode` and `MedicationRequest.reasonReference` are marked as Additional USCDI Requirements. The certifying server system is not required to support both but **SHALL** support at least one of these elements. The certifying client application **SHALL** support both elements.
+  * when using MedicationRequest.reasonReference:
+      * Servers **SHALL** support at least one target resource in `MedicationRequest.reasonReference`. Clients **SHALL** support all target resources.
+      * The referenced resources **SHOULD** be a US Core Profile as documented in Referencing US Core Profiles.</t>
+  </si>
+  <si>
+    <t>* This Profile can represent a medication using a code or reference a Medication resource.
+  * The Server systems are not required to support both a code and a reference, but **SHALL** support at least one of these methods.
+  * The Client application **SHALL** support all methods.
+  * Systems that primarily rely on NDC codes instead of RxNorm to represent medications can use the National Library of Medicine's (NLM) NDC to RxNorm mappings to aid in additional codings.
+  * When referencing a Medication resource in `.medicationReference`, the resource may be contained or an external resource. If an external reference to a Medication resource is used, the Server **SHALL** support the `_include` parameter for searching this element.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Systems **SHOULD** support `Observation.effectivePeriod` to accurately represent tests that are collected over a period of time (for example, a 24-Hour Urine Collection test).
+* An Observation without a value, **SHALL** include a reason why the data is absent unless there are component observations, or references to other Observations that are grouped within it
+    * Systems that never provide an observation without a value are not required to support `Observation.dataAbsentReason`
+*  An `Observation.component` without a value, **SHALL** include a reason why the data is absent.
+    * Systems that never provide an component observation without a component value are not required to support `Observation.component.dataAbsentReason`.
+ * There are multiple Observation profiles.  Refer to the specific profile page for profile specific conformance rules and guidance </t>
+  </si>
+  <si>
+    <t>* Systems **SHALL** support National Provider Identifier (NPI) for organizations and **SHOULD** support Clinical Laboratory Improvement Amendments (CLIA) and the National Association of Insurance Commissioners NAIC Company code (sometimes called "NAIC Number" or "cocode")  for `Organization.Identifier`.
+* Systems **SHOULD** follow the Project US@ Technical Specification for Patient Addresses Final Version 1.0 as the standard style guide for `Organization.address.line` and  `Organization.address.city`.</t>
+  </si>
+  <si>
+    <t>* The Patient's Social Security Numbers **SHOULD NOT** be used as a patient identifier in `Patient.identifier.value`.
+*  The Complex Extensions for Race and Ethnicity allow for one or more codes of which: Must Support at least one category code from the OMB Race and Ethnicity Category Value Sets that draw from the Race &amp; Ethnicity - CDC (CDCREC] code system.
+    - **MAY** include additional codes from the detailed ethnicity and detailed race value sets drawn from the Race &amp; Ethnicity - CDC (CDCREC) code system
+    - **SHALL** include a text description
+* Although Patient.deceased[x] is marked as 𝗔𝗗𝗗𝗜𝗧𝗜𝗢𝗡𝗔𝗟 𝗨𝗦𝗖𝗗𝗜, certifying systems are not required to support both choices, but **SHALL** support at least `Patient.deceasedDateTime`.
+*  Servers can use the US Core Interpreter Needed Extension on this profile or the US Core Encounter Profile to communicate whether a patient needs an interpreter. Although the extension is marked as an *Additional USCDI Requirement* on both US Core Patient and US Core Encounter Profiles, the certifying Server system is not required to support the extension on both profiles but **SHALL** support the extension on at least one. The certifying Client application **SHALL** support the extension on both profiles.
+     - Systems **SHOULD** designate the patient's preferred language in the `Patient.communication.preferred` element.
+* Certifying systems **SHALL** and non-certifying systems **SHOULD** follow the Project US@ Technical Specification for Patient Addresses Final Version 1.0 as the standard style guide for `Patient.address.line` and  `Patient.address.city` for new and updated records.</t>
+  </si>
+  <si>
+    <t>* Servers that support only US Core Practitioner Profile and do not support the US Core PractitionerRole Profile **SHALL** provide implementation specific guidance how to access a provider’s location and contact information using only the Practitioner resource.
+   * Although Practitioner.address is marked as Must Support, the server system is not required to support it if they support the US Core PractitionerRole Profile, but **SHALL** support it if they do not support the US Core PractitionerRole Profile. The client application **SHALL** support both.
+* To balance the privacy of healthcare workers with the patient's right to access information. Only professional/work contact information about the practitioner **SHOULD** be available to the patient (such as a work address or office telephone number).
+* Systems **SHOULD** follow the Project US@ Technical Specification for Patient Addresses Final Version 1.0 as the standard style guide for `Practitioner.address.line` and  `Practitioner.address.city`.</t>
+  </si>
+  <si>
+    <t>* The Must Support `ServiceRequest.category` is bound, *at a minimum*, to the [US Core ServiceRequest Category Codes](ValueSet-us-core-servicerequest-category.html), and other category codes can be used. API consumers can query by category when accessing patient information. For the USCDI *Laboratory Order*, *Imaging Order*, *Clinical Test Order*, and *Procedure Order* Data Elements, implementers **SHOULD** use the corresponding category codes listed in the table on the US Core ServiceRequest Profile page. For example, laboratory orders would have the category code "108252007" (Laboratory procedure).
+* The `ServiceRequest.code` value set is broad to accommodate a wide variety of use cases and **SHOULD** be constrained to a subset for a particular use case or domain.  These value sets contain concepts that span many use cases and are not bound to any USCDI Data Element. However, the table on the US Core ServiceRequest Profile page identifies *additional* value set bindings for the USCDI *Laboratory Order, Imaging Order and Clinical Test Order* Data Elements. Implementers **SHOULD** conform to the binding strengths for each USCDI Order context listed in the table. For example, laboratory orders are extensibly bound to the LOINC Common Laboratory Orders Value Set. Note that the USCDI Class *Procedure Order* Data Element has no additional binding.
+* Servers and Clients **SHALL** support both US Core ServiceRequest and US Core Procedure Profiles for communicating the reason or justification for a referral as Additional USCDI Requirements. Typically, the reason or justification for a referral or consultation is communicated through `Procedure.basedOn` linking the Procedure to the US Core ServiceRequest Profile that includes either `ServiceRequest.reasonCode` or `ServiceRequest.reasonReference`. When the Procedure does not have an associated ServiceRequest, it is communicated through the US Core Procedure Profile's `Procedure.reasonCode` or `Procedure.reasonReference`. Depending on the procedure being documented, a server will select the appropriate Profile to use.
+   * Although both `ServiceRequest.reasonCode` and `ServiceRequest.reasonReference` are marked as Additional USCDI Requirements, the certifying server system is not required to support both, but **SHALL** support at least one of these elements. The certifying client application **SHALL** support both elements.
+     * when using  `ServiceRequest.reasonReference`:
+       * Servers **SHALL** support *at least one* target resource in `ServiceRequest.reasonReference`. Clients **SHALL** support all target resources.
+       * The referenced resources **SHOULD** be a US Core Profile as documented in Referencing US Core Profiles.</t>
   </si>
 </sst>
 </file>
@@ -6099,7 +6110,7 @@
         <v>424</v>
       </c>
       <c r="B2" t="s">
-        <v>703</v>
+        <v>696</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -8485,7 +8496,7 @@
         <v>0</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>695</v>
+        <v>688</v>
       </c>
       <c r="G44" t="str">
         <f t="shared" si="0"/>
@@ -8914,7 +8925,7 @@
         <v>0</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>695</v>
+        <v>688</v>
       </c>
       <c r="G52" t="str">
         <f t="shared" si="0"/>
@@ -9611,7 +9622,7 @@
         <v>0</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>695</v>
+        <v>688</v>
       </c>
       <c r="G65" t="str">
         <f t="shared" si="0"/>
@@ -11218,7 +11229,7 @@
         <v>0</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>695</v>
+        <v>688</v>
       </c>
       <c r="G95" t="str">
         <f t="shared" si="6"/>
@@ -14311,7 +14322,7 @@
         <v>296</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>710</v>
+        <v>701</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14338,10 +14349,10 @@
         <v>142</v>
       </c>
       <c r="J38" s="23" t="s">
-        <v>711</v>
+        <v>702</v>
       </c>
       <c r="K38" s="23" t="s">
-        <v>712</v>
+        <v>703</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14371,10 +14382,10 @@
         <v>654</v>
       </c>
       <c r="J39" s="23" t="s">
-        <v>713</v>
+        <v>704</v>
       </c>
       <c r="K39" s="23" t="s">
-        <v>714</v>
+        <v>705</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14401,10 +14412,10 @@
         <v>142</v>
       </c>
       <c r="J40" s="23" t="s">
-        <v>742</v>
+        <v>733</v>
       </c>
       <c r="K40" s="23" t="s">
-        <v>715</v>
+        <v>706</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14431,7 +14442,7 @@
         <v>143</v>
       </c>
       <c r="J41" s="23" t="s">
-        <v>716</v>
+        <v>707</v>
       </c>
       <c r="K41" s="4" t="s">
         <v>144</v>
@@ -14461,7 +14472,7 @@
         <v>145</v>
       </c>
       <c r="J42" s="23" t="s">
-        <v>717</v>
+        <v>708</v>
       </c>
       <c r="K42" s="4" t="s">
         <v>148</v>
@@ -14491,7 +14502,7 @@
         <v>145</v>
       </c>
       <c r="J43" s="23" t="s">
-        <v>718</v>
+        <v>709</v>
       </c>
       <c r="K43" s="4" t="s">
         <v>148</v>
@@ -14521,7 +14532,7 @@
         <v>145</v>
       </c>
       <c r="J44" s="23" t="s">
-        <v>719</v>
+        <v>710</v>
       </c>
       <c r="K44" s="4" t="s">
         <v>148</v>
@@ -14551,7 +14562,7 @@
         <v>145</v>
       </c>
       <c r="J45" s="23" t="s">
-        <v>720</v>
+        <v>711</v>
       </c>
       <c r="K45" s="4" t="s">
         <v>148</v>
@@ -14579,7 +14590,7 @@
       </c>
       <c r="I46" s="4"/>
       <c r="J46" s="23" t="s">
-        <v>696</v>
+        <v>689</v>
       </c>
       <c r="K46" s="23" t="str">
         <f>"Fetches a bundle of all "&amp;B46&amp;" resources for the specified "&amp;SUBSTITUTE(D46,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
@@ -14701,10 +14712,10 @@
         <v>189</v>
       </c>
       <c r="J50" s="23" t="s">
-        <v>721</v>
+        <v>712</v>
       </c>
       <c r="K50" s="23" t="s">
-        <v>722</v>
+        <v>713</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14730,10 +14741,10 @@
         <v>184</v>
       </c>
       <c r="J51" s="23" t="s">
-        <v>723</v>
+        <v>714</v>
       </c>
       <c r="K51" s="23" t="s">
-        <v>724</v>
+        <v>715</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14759,10 +14770,10 @@
         <v>206</v>
       </c>
       <c r="J52" s="23" t="s">
-        <v>725</v>
+        <v>716</v>
       </c>
       <c r="K52" s="23" t="s">
-        <v>726</v>
+        <v>717</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14788,10 +14799,10 @@
         <v>186</v>
       </c>
       <c r="J53" s="23" t="s">
-        <v>727</v>
+        <v>718</v>
       </c>
       <c r="K53" s="23" t="s">
-        <v>728</v>
+        <v>719</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14816,10 +14827,10 @@
       </c>
       <c r="I54" s="4"/>
       <c r="J54" s="23" t="s">
-        <v>729</v>
+        <v>720</v>
       </c>
       <c r="K54" s="23" t="s">
-        <v>730</v>
+        <v>721</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14845,10 +14856,10 @@
         <v>210</v>
       </c>
       <c r="J55" s="23" t="s">
-        <v>731</v>
+        <v>722</v>
       </c>
       <c r="K55" s="23" t="s">
-        <v>732</v>
+        <v>723</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
@@ -15571,10 +15582,10 @@
         <v>266</v>
       </c>
       <c r="J78" s="23" t="s">
-        <v>721</v>
+        <v>712</v>
       </c>
       <c r="K78" s="23" t="s">
-        <v>733</v>
+        <v>724</v>
       </c>
     </row>
     <row r="79" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -15601,7 +15612,7 @@
         <v>266</v>
       </c>
       <c r="K79" s="23" t="s">
-        <v>734</v>
+        <v>725</v>
       </c>
     </row>
     <row r="80" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -15628,10 +15639,10 @@
         <v>267</v>
       </c>
       <c r="J80" s="23" t="s">
-        <v>735</v>
+        <v>726</v>
       </c>
       <c r="K80" s="23" t="s">
-        <v>736</v>
+        <v>727</v>
       </c>
     </row>
     <row r="81" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -15658,10 +15669,10 @@
         <v>268</v>
       </c>
       <c r="J81" s="23" t="s">
-        <v>737</v>
+        <v>728</v>
       </c>
       <c r="K81" s="23" t="s">
-        <v>738</v>
+        <v>729</v>
       </c>
     </row>
     <row r="82" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -15688,7 +15699,7 @@
         <v>271</v>
       </c>
       <c r="J82" s="23" t="s">
-        <v>739</v>
+        <v>730</v>
       </c>
       <c r="K82" s="23" t="s">
         <v>269</v>
@@ -15718,10 +15729,10 @@
         <v>272</v>
       </c>
       <c r="J83" s="23" t="s">
-        <v>740</v>
+        <v>731</v>
       </c>
       <c r="K83" s="23" t="s">
-        <v>741</v>
+        <v>732</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
@@ -16339,7 +16350,7 @@
         <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>702</v>
+        <v>695</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -16371,7 +16382,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>701</v>
+        <v>694</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -16450,13 +16461,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>744</v>
+        <v>734</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>745</v>
+        <v>735</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>746</v>
+        <v>736</v>
       </c>
       <c r="D2" t="s">
         <v>64</v>
@@ -16718,10 +16729,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
-        <v>706</v>
+        <v>697</v>
       </c>
       <c r="B12" t="s">
-        <v>707</v>
+        <v>698</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
@@ -16914,10 +16925,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>708</v>
+        <v>699</v>
       </c>
       <c r="B26" t="s">
-        <v>709</v>
+        <v>700</v>
       </c>
       <c r="D26" t="s">
         <v>11</v>
@@ -17473,8 +17484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{352F3A6C-0DAD-1041-B50E-04478951E07A}">
   <dimension ref="A1:Y69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="23" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -17595,7 +17606,7 @@
         <v>64</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>698</v>
+        <v>691</v>
       </c>
       <c r="X3" s="12" t="s">
         <v>412</v>
@@ -17612,7 +17623,7 @@
         <v>64</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="V4" t="s">
         <v>498</v>
@@ -17635,7 +17646,7 @@
         <v>64</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>747</v>
+        <v>737</v>
       </c>
       <c r="X5" s="12" t="s">
         <v>412</v>
@@ -17683,7 +17694,7 @@
         <v>64</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>748</v>
+        <v>738</v>
       </c>
       <c r="X8" s="12" t="s">
         <v>412</v>
@@ -17700,7 +17711,7 @@
         <v>64</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>705</v>
+        <v>739</v>
       </c>
       <c r="X9" s="12" t="s">
         <v>412</v>
@@ -17716,8 +17727,8 @@
       <c r="B10" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>682</v>
+      <c r="C10" s="2" t="s">
+        <v>740</v>
       </c>
       <c r="X10" s="12" t="s">
         <v>412</v>
@@ -17734,7 +17745,7 @@
         <v>64</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>699</v>
+        <v>692</v>
       </c>
       <c r="X11" s="12"/>
       <c r="Y11" s="12"/>
@@ -17764,7 +17775,7 @@
         <v>28</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>700</v>
+        <v>693</v>
       </c>
       <c r="X13" s="12"/>
       <c r="Y13" s="12"/>
@@ -17777,7 +17788,7 @@
         <v>64</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="X14" s="12" t="s">
         <v>412</v>
@@ -17794,7 +17805,7 @@
         <v>64</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="X15" s="12"/>
       <c r="Y15" s="12"/>
@@ -17807,7 +17818,7 @@
         <v>64</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>697</v>
+        <v>690</v>
       </c>
       <c r="X16" s="12"/>
       <c r="Y16" s="12"/>
@@ -17833,7 +17844,7 @@
         <v>64</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>691</v>
+        <v>742</v>
       </c>
       <c r="V18" t="s">
         <v>64</v>
@@ -17856,7 +17867,7 @@
         <v>64</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>692</v>
+        <v>743</v>
       </c>
       <c r="V19" t="s">
         <v>64</v>
@@ -17902,7 +17913,7 @@
         <v>64</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>694</v>
+        <v>744</v>
       </c>
       <c r="X21" s="12" t="s">
         <v>412</v>
@@ -17919,12 +17930,12 @@
         <v>64</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>684</v>
+        <v>745</v>
       </c>
       <c r="X22" s="12"/>
       <c r="Y22" s="12"/>
     </row>
-    <row r="23" spans="1:25" ht="97" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" ht="273" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -17932,7 +17943,7 @@
         <v>64</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>704</v>
+        <v>746</v>
       </c>
       <c r="X23" s="12" t="s">
         <v>412</v>
@@ -17949,7 +17960,7 @@
         <v>64</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>685</v>
+        <v>747</v>
       </c>
       <c r="X24" s="12"/>
       <c r="Y24" s="12"/>
@@ -17981,7 +17992,7 @@
         <v>64</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="X26" s="12" t="s">
         <v>412</v>
@@ -18009,7 +18020,7 @@
         <v>64</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>693</v>
+        <v>687</v>
       </c>
       <c r="X28" s="12"/>
       <c r="Y28" s="12"/>
@@ -18022,7 +18033,7 @@
         <v>64</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>693</v>
+        <v>687</v>
       </c>
       <c r="X29" s="12" t="s">
         <v>412</v>
@@ -18039,7 +18050,7 @@
         <v>64</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="X30" s="12" t="s">
         <v>412</v>
@@ -18055,8 +18066,8 @@
       <c r="B31" t="s">
         <v>64</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>688</v>
+      <c r="C31" s="2" t="s">
+        <v>748</v>
       </c>
       <c r="X31" s="12" t="s">
         <v>412</v>
@@ -18073,7 +18084,7 @@
         <v>64</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="X32" s="12"/>
       <c r="Y32" s="12"/>

</xml_diff>

<commit_message>
create USCore V6.1.0 - R6 release changes
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F46AA277-B28D-354B-84CA-442464242326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{018ECEF2-DCCB-024E-95EC-B5ECB854163B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -1890,9 +1890,6 @@
     <t>GET [base]/Goal?patient=1137192&amp;description=http://snomed.info/sct\|1078229009</t>
   </si>
   <si>
-    <t>Documents/FHIR/US-Core/input/</t>
-  </si>
-  <si>
     <t>HL7 International - Cross-Group Projects</t>
   </si>
   <si>
@@ -2438,6 +2435,9 @@
 	* A server **SHALL** support `Condition.recordedDate`.
     * A server **SHALL** support at least one of the assertedDate Extension and `Condition.onsetDateTime`. A server may support both, which means they support all 3 locations.
     * The client application **SHALL** support all three elements.</t>
+  </si>
+  <si>
+    <t>/Users/ehaas/Documents/FHIR/US-Core/input/</t>
   </si>
 </sst>
 </file>
@@ -2656,57 +2656,7 @@
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2767,9 +2717,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2807,7 +2757,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2913,7 +2863,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3055,7 +3005,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3096,8 +3046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40F68824-E615-4729-AAE0-A6F75FBDE06B}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView zoomScale="400" zoomScaleNormal="400" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="400" zoomScaleNormal="400" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3119,7 +3069,7 @@
         <v>446</v>
       </c>
       <c r="B2" t="s">
-        <v>582</v>
+        <v>730</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -3151,7 +3101,7 @@
         <v>62</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -3167,7 +3117,7 @@
         <v>453</v>
       </c>
       <c r="B8" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -4495,7 +4445,7 @@
         <v>19</v>
       </c>
       <c r="C25" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="D25" t="s">
         <v>28</v>
@@ -4769,7 +4719,7 @@
         <v>51</v>
       </c>
       <c r="Y30" s="4" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="Z30" t="s">
         <v>167</v>
@@ -4791,7 +4741,7 @@
         <v>79</v>
       </c>
       <c r="C31" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="D31" t="s">
         <v>28</v>
@@ -4813,19 +4763,19 @@
         <v>52</v>
       </c>
       <c r="L31" t="s">
+        <v>634</v>
+      </c>
+      <c r="M31" t="s">
+        <v>51</v>
+      </c>
+      <c r="O31" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y31" s="4" t="s">
         <v>635</v>
       </c>
-      <c r="M31" t="s">
-        <v>51</v>
-      </c>
-      <c r="O31" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y31" s="4" t="s">
+      <c r="Z31" t="s">
         <v>636</v>
-      </c>
-      <c r="Z31" t="s">
-        <v>637</v>
       </c>
       <c r="AA31" s="8" t="str">
         <f>"Fetches a bundle of all "&amp;B31&amp;" resources matching the name"</f>
@@ -4841,7 +4791,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C32" t="s">
         <v>50</v>
@@ -4866,7 +4816,7 @@
         <v>52</v>
       </c>
       <c r="L32" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="M32" t="s">
         <v>51</v>
@@ -4884,7 +4834,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C33" t="s">
         <v>65</v>
@@ -4928,7 +4878,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C34" t="s">
         <v>62</v>
@@ -4975,7 +4925,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C35" t="s">
         <v>56</v>
@@ -5019,7 +4969,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C36" t="s">
         <v>57</v>
@@ -5075,7 +5025,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C37" t="s">
         <v>54</v>
@@ -5119,7 +5069,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C38" t="s">
         <v>61</v>
@@ -9319,7 +9269,7 @@
         <v>51</v>
       </c>
       <c r="Y115" s="4" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="Z115" s="4" t="str">
         <f>"GET [base]/"&amp;B115&amp;"?"&amp;C115&amp;"=Mary Shaw"</f>
@@ -9339,7 +9289,7 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C116" t="s">
         <v>50</v>
@@ -9378,7 +9328,7 @@
         <v>support fetching a QuestionnaireResponse</v>
       </c>
       <c r="Z116" s="4" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="AB116" t="str">
         <f t="shared" si="9"/>
@@ -9390,7 +9340,7 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C117" t="s">
         <v>84</v>
@@ -9449,7 +9399,7 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C118" t="s">
         <v>56</v>
@@ -9490,7 +9440,7 @@
         <v>51</v>
       </c>
       <c r="Y118" s="19" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="AB118" t="str">
         <f t="shared" si="9"/>
@@ -9502,10 +9452,10 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="C119" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D119" t="s">
         <v>28</v>
@@ -9530,16 +9480,16 @@
         <v>52</v>
       </c>
       <c r="L119" t="s">
+        <v>668</v>
+      </c>
+      <c r="M119" t="s">
+        <v>51</v>
+      </c>
+      <c r="O119" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y119" s="19" t="s">
         <v>669</v>
-      </c>
-      <c r="M119" t="s">
-        <v>51</v>
-      </c>
-      <c r="O119" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y119" s="19" t="s">
-        <v>670</v>
       </c>
       <c r="AB119" t="str">
         <f t="shared" si="9"/>
@@ -9551,7 +9501,7 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C120" t="s">
         <v>546</v>
@@ -9595,7 +9545,7 @@
         <v>87</v>
       </c>
       <c r="Y120" s="19" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="AB120" t="str">
         <f t="shared" si="9"/>
@@ -9607,10 +9557,10 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C121" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="D121" t="s">
         <v>28</v>
@@ -9645,7 +9595,7 @@
         <v>51</v>
       </c>
       <c r="Y121" s="19" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="AB121" t="str">
         <f t="shared" si="9"/>
@@ -9657,7 +9607,7 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C122" t="s">
         <v>84</v>
@@ -9695,7 +9645,7 @@
         <v>51</v>
       </c>
       <c r="Y122" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="Z122" s="4" t="str">
         <f>"GET [base]/"&amp;B122&amp;"?patient=1137192"</f>
@@ -9715,7 +9665,7 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C123" t="s">
         <v>56</v>
@@ -9768,7 +9718,7 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C124" t="s">
         <v>12</v>
@@ -9821,7 +9771,7 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C125" t="s">
         <v>84</v>
@@ -9859,10 +9809,10 @@
         <v>51</v>
       </c>
       <c r="X125" s="6" t="s">
+        <v>640</v>
+      </c>
+      <c r="Z125" s="8" t="s">
         <v>641</v>
-      </c>
-      <c r="Z125" s="8" t="s">
-        <v>642</v>
       </c>
       <c r="AA125" s="8" t="str">
         <f>"Fetches a bundle of all "&amp;B125&amp; " resources for the specified patient."</f>
@@ -9878,10 +9828,10 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
+        <v>642</v>
+      </c>
+      <c r="C126" t="s">
         <v>643</v>
-      </c>
-      <c r="C126" t="s">
-        <v>644</v>
       </c>
       <c r="D126" t="s">
         <v>28</v>
@@ -9932,7 +9882,7 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="C127" t="s">
         <v>50</v>
@@ -9970,7 +9920,7 @@
         <v>51</v>
       </c>
       <c r="Y127" s="4" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="Z127" s="4" t="str">
         <f>"GET [base]/"&amp;B127&amp;"?"&amp;C127&amp;"=123"</f>
@@ -9986,7 +9936,7 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="C128" t="s">
         <v>84</v>
@@ -10929,7 +10879,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D32" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="F32" t="s">
         <v>64</v>
@@ -10938,10 +10888,10 @@
         <v>128</v>
       </c>
       <c r="I32" s="4" t="s">
+        <v>645</v>
+      </c>
+      <c r="J32" s="4" t="s">
         <v>646</v>
-      </c>
-      <c r="J32" s="4" t="s">
-        <v>647</v>
       </c>
       <c r="K32" s="4" t="str">
         <f t="shared" si="1"/>
@@ -11071,7 +11021,7 @@
         <v>312</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
@@ -11116,7 +11066,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D38" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E38" t="s">
         <v>51</v>
@@ -11131,13 +11081,13 @@
         <v>396</v>
       </c>
       <c r="I38" s="4" t="s">
+        <v>710</v>
+      </c>
+      <c r="J38" s="25" t="s">
         <v>711</v>
       </c>
-      <c r="J38" s="25" t="s">
+      <c r="K38" s="4" t="s">
         <v>712</v>
-      </c>
-      <c r="K38" s="4" t="s">
-        <v>713</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
@@ -11164,7 +11114,7 @@
         <v>144</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="K39" s="4" t="s">
         <v>556</v>
@@ -11420,7 +11370,7 @@
         <v>173</v>
       </c>
       <c r="C48" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="D48" t="s">
         <v>110</v>
@@ -11450,7 +11400,7 @@
         <v>173</v>
       </c>
       <c r="C49" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="D49" t="s">
         <v>139</v>
@@ -11483,7 +11433,7 @@
         <v>173</v>
       </c>
       <c r="C50" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="D50" t="s">
         <v>141</v>
@@ -11513,7 +11463,7 @@
         <v>173</v>
       </c>
       <c r="C51" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="D51" t="s">
         <v>188</v>
@@ -11546,7 +11496,7 @@
         <v>173</v>
       </c>
       <c r="C52" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="D52" t="s">
         <v>212</v>
@@ -11924,7 +11874,7 @@
         <v>177</v>
       </c>
       <c r="C64" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="D64" t="s">
         <v>229</v>
@@ -11956,7 +11906,7 @@
         <v>177</v>
       </c>
       <c r="C65" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="D65" t="s">
         <v>139</v>
@@ -11989,7 +11939,7 @@
         <v>177</v>
       </c>
       <c r="C66" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="D66" t="s">
         <v>141</v>
@@ -12019,7 +11969,7 @@
         <v>177</v>
       </c>
       <c r="C67" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="D67" t="s">
         <v>188</v>
@@ -12052,7 +12002,7 @@
         <v>177</v>
       </c>
       <c r="C68" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="D68" t="s">
         <v>212</v>
@@ -12082,7 +12032,7 @@
         <v>304</v>
       </c>
       <c r="C69" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="D69" t="s">
         <v>110</v>
@@ -12461,7 +12411,7 @@
         <v>241</v>
       </c>
       <c r="C81" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="D81" t="s">
         <v>112</v>
@@ -12490,7 +12440,7 @@
         <v>241</v>
       </c>
       <c r="C82" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="D82" t="s">
         <v>110</v>
@@ -12502,13 +12452,13 @@
         <v>100</v>
       </c>
       <c r="I82" s="4" t="s">
+        <v>648</v>
+      </c>
+      <c r="J82" s="4" t="s">
         <v>649</v>
       </c>
-      <c r="J82" s="4" t="s">
+      <c r="K82" s="4" t="s">
         <v>650</v>
-      </c>
-      <c r="K82" s="4" t="s">
-        <v>651</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
@@ -12732,7 +12682,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C90" t="str">
         <f t="shared" si="4"/>
@@ -12748,10 +12698,10 @@
         <v>100</v>
       </c>
       <c r="I90" t="s">
+        <v>604</v>
+      </c>
+      <c r="J90" s="4" t="s">
         <v>605</v>
-      </c>
-      <c r="J90" s="4" t="s">
-        <v>606</v>
       </c>
       <c r="K90" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B90&amp;" resources for the specified "&amp;SUBSTITUTE(D90,","," and ")</f>
@@ -12763,14 +12713,14 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="C91" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="D91" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="F91" t="s">
         <v>64</v>
@@ -12779,13 +12729,13 @@
         <v>100</v>
       </c>
       <c r="H91" t="s">
+        <v>607</v>
+      </c>
+      <c r="I91" t="s">
+        <v>604</v>
+      </c>
+      <c r="J91" s="4" t="s">
         <v>608</v>
-      </c>
-      <c r="I91" t="s">
-        <v>605</v>
-      </c>
-      <c r="J91" s="4" t="s">
-        <v>609</v>
       </c>
       <c r="K91" t="str">
         <f>"Fetches a bundle of all "&amp;B91&amp;" resources for the specified "&amp;SUBSTITUTE(D91,","," and  ") &amp; "= 'sdoh'"</f>
@@ -12797,14 +12747,14 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C92" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D92" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="F92" t="s">
         <v>64</v>
@@ -12813,10 +12763,10 @@
         <v>143</v>
       </c>
       <c r="I92" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="J92" s="4" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="K92" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B92&amp;" resources for the specified patient and date"</f>
@@ -12828,14 +12778,14 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="C93" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="D93" s="16" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="F93" t="s">
         <v>64</v>
@@ -12844,13 +12794,13 @@
         <v>211</v>
       </c>
       <c r="H93" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="I93" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="J93" s="4" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="K93" t="str">
         <f>"Fetches a bundle of all "&amp;B93&amp;" resources tagged as 'sdoh' for the specified patient and date"</f>
@@ -12862,14 +12812,14 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C94" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D94" s="16" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="F94" t="s">
         <v>64</v>
@@ -12878,10 +12828,10 @@
         <v>85</v>
       </c>
       <c r="I94" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="J94" s="4" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K94" t="str">
         <f>"Fetches a bundle of all "&amp;B94&amp;" resources for the specified patient that have been completed against a specified form."</f>
@@ -12893,7 +12843,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="16" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C95" t="str">
         <f t="shared" si="4"/>
@@ -12911,10 +12861,10 @@
       </c>
       <c r="H95" s="16"/>
       <c r="I95" s="4" t="s">
+        <v>651</v>
+      </c>
+      <c r="J95" s="4" t="s">
         <v>652</v>
-      </c>
-      <c r="J95" s="4" t="s">
-        <v>653</v>
       </c>
       <c r="K95" t="str">
         <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed))."</f>
@@ -12926,7 +12876,7 @@
         <v>95</v>
       </c>
       <c r="B96" s="16" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C96" t="str">
         <f t="shared" si="4"/>
@@ -12944,10 +12894,10 @@
       </c>
       <c r="H96" s="16"/>
       <c r="I96" s="4" t="s">
+        <v>653</v>
+      </c>
+      <c r="J96" s="4" t="s">
         <v>654</v>
-      </c>
-      <c r="J96" s="4" t="s">
-        <v>655</v>
       </c>
       <c r="K96" t="str">
         <f>"Fetches a bundle of all "&amp;B96&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed) and type of dispense (e.g., partially dispensed)."</f>
@@ -12959,14 +12909,14 @@
         <v>96</v>
       </c>
       <c r="B97" s="16" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C97" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationdispense</v>
       </c>
       <c r="D97" s="16" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="E97" s="16"/>
       <c r="F97" s="16" t="s">
@@ -12977,10 +12927,10 @@
       </c>
       <c r="H97" s="16"/>
       <c r="I97" s="4" t="s">
+        <v>656</v>
+      </c>
+      <c r="J97" s="4" t="s">
         <v>657</v>
-      </c>
-      <c r="J97" s="4" t="s">
-        <v>658</v>
       </c>
       <c r="K97" t="str">
         <f>"Fetches a bundle of all "&amp;B96&amp;" resources for the specified patient for a given dispense and date or range"</f>
@@ -12998,21 +12948,21 @@
         <v>526</v>
       </c>
       <c r="D98" s="16" t="s">
+        <v>705</v>
+      </c>
+      <c r="E98" s="16" t="s">
         <v>706</v>
       </c>
-      <c r="E98" s="16" t="s">
+      <c r="F98" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="G98" s="16" t="s">
         <v>707</v>
-      </c>
-      <c r="F98" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="G98" s="16" t="s">
-        <v>708</v>
       </c>
       <c r="H98" s="16"/>
       <c r="I98" s="4"/>
       <c r="J98" s="4" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="K98" t="str">
         <f>"Fetches a bundle of all "&amp;B98&amp;" resources for the specified patient that may match any of the string fields in the name element (including family, give, prefix, suffix, suffix, and/or text)"</f>
@@ -13021,7 +12971,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:K98" xr:uid="{331E0B16-168F-459B-8951-3DF614BF0371}"/>
-  <conditionalFormatting sqref="B99:B1048576 B1:B97">
+  <conditionalFormatting sqref="B1:B97 B99:B1048576">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",B1)))</formula>
     </cfRule>
@@ -13102,7 +13052,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -13110,7 +13060,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -13186,7 +13136,7 @@
         <v>525</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D2" t="s">
         <v>64</v>
@@ -13194,7 +13144,7 @@
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>520</v>
@@ -13351,10 +13301,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B5" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
@@ -13365,10 +13315,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B6" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -13379,16 +13329,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>672</v>
+      </c>
+      <c r="B7" t="s">
         <v>673</v>
       </c>
-      <c r="B7" t="s">
-        <v>674</v>
-      </c>
       <c r="D7" t="s">
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -13449,7 +13399,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B12" t="s">
         <v>347</v>
@@ -13463,86 +13413,86 @@
     </row>
     <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
+        <v>584</v>
+      </c>
+      <c r="B13" t="s">
         <v>585</v>
       </c>
-      <c r="B13" t="s">
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
         <v>586</v>
-      </c>
-      <c r="D13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" t="s">
-        <v>587</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
+        <v>587</v>
+      </c>
+      <c r="B14" t="s">
         <v>588</v>
       </c>
-      <c r="B14" t="s">
-        <v>589</v>
-      </c>
       <c r="D14" t="s">
         <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
+        <v>589</v>
+      </c>
+      <c r="B15" t="s">
         <v>590</v>
       </c>
-      <c r="B15" t="s">
-        <v>591</v>
-      </c>
       <c r="D15" t="s">
         <v>11</v>
       </c>
       <c r="E15" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
+        <v>591</v>
+      </c>
+      <c r="B16" t="s">
         <v>592</v>
       </c>
-      <c r="B16" t="s">
-        <v>593</v>
-      </c>
       <c r="D16" t="s">
         <v>11</v>
       </c>
       <c r="E16" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
+        <v>593</v>
+      </c>
+      <c r="B17" t="s">
         <v>594</v>
       </c>
-      <c r="B17" t="s">
-        <v>595</v>
-      </c>
       <c r="D17" t="s">
         <v>11</v>
       </c>
       <c r="E17" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B18" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D18" t="s">
         <v>11</v>
       </c>
       <c r="E18" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -13617,16 +13567,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>674</v>
+      </c>
+      <c r="B24" t="s">
         <v>675</v>
       </c>
-      <c r="B24" t="s">
-        <v>676</v>
-      </c>
       <c r="D24" t="s">
         <v>11</v>
       </c>
       <c r="E24" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -13645,10 +13595,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>676</v>
+      </c>
+      <c r="B26" t="s">
         <v>677</v>
-      </c>
-      <c r="B26" t="s">
-        <v>678</v>
       </c>
       <c r="D26" t="s">
         <v>11</v>
@@ -13659,10 +13609,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>678</v>
+      </c>
+      <c r="B27" t="s">
         <v>679</v>
-      </c>
-      <c r="B27" t="s">
-        <v>680</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
@@ -13673,10 +13623,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>680</v>
+      </c>
+      <c r="B28" t="s">
         <v>681</v>
-      </c>
-      <c r="B28" t="s">
-        <v>682</v>
       </c>
       <c r="D28" t="s">
         <v>11</v>
@@ -13687,10 +13637,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="18" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B29" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D29" t="s">
         <v>11</v>
@@ -13715,10 +13665,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B31" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D31" t="s">
         <v>11</v>
@@ -13802,7 +13752,7 @@
         <v>523</v>
       </c>
       <c r="B37" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="D37" t="s">
         <v>11</v>
@@ -13855,10 +13805,10 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B41" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="D41" t="s">
         <v>11</v>
@@ -13883,10 +13833,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="18" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B43" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="D43" t="s">
         <v>11</v>
@@ -13897,10 +13847,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B44" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="D44" t="s">
         <v>11</v>
@@ -13928,7 +13878,7 @@
         <v>479</v>
       </c>
       <c r="B46" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="D46" t="s">
         <v>11</v>
@@ -14051,30 +14001,30 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="B55" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="D55" t="s">
         <v>11</v>
       </c>
       <c r="E55" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B56" t="s">
+        <v>599</v>
+      </c>
+      <c r="D56" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" t="s">
         <v>600</v>
-      </c>
-      <c r="D56" t="s">
-        <v>11</v>
-      </c>
-      <c r="E56" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -14107,32 +14057,22 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="18" t="s">
+        <v>686</v>
+      </c>
+      <c r="B59" t="s">
         <v>687</v>
       </c>
-      <c r="B59" t="s">
+      <c r="D59" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59" t="s">
         <v>688</v>
       </c>
-      <c r="D59" t="s">
-        <v>11</v>
-      </c>
-      <c r="E59" t="s">
-        <v>689</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A9">
-    <cfRule type="containsText" dxfId="8" priority="3" operator="containsText" text="!">
-      <formula>NOT(ISERROR(SEARCH("!",A9)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",A1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A55">
-    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="!">
-      <formula>NOT(ISERROR(SEARCH("!",A55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -14147,7 +14087,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97A43D86-2C5C-EA46-9712-6B42B0091383}">
   <dimension ref="A1:Y69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
@@ -14286,7 +14226,7 @@
         <v>64</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="V4" t="s">
         <v>532</v>
@@ -14309,7 +14249,7 @@
         <v>64</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="X5" s="13" t="s">
         <v>433</v>
@@ -14320,7 +14260,7 @@
     </row>
     <row r="6" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B6" t="s">
         <v>64</v>
@@ -14340,7 +14280,7 @@
         <v>64</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="X7" s="13" t="s">
         <v>433</v>
@@ -14372,7 +14312,7 @@
         <v>64</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="X9" s="13" t="s">
         <v>433</v>
@@ -14389,7 +14329,7 @@
         <v>64</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="X10" s="13" t="s">
         <v>433</v>
@@ -14400,16 +14340,16 @@
     </row>
     <row r="11" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>724</v>
+      </c>
+      <c r="B11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="26" t="s">
         <v>725</v>
       </c>
-      <c r="B11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C11" s="26" t="s">
-        <v>726</v>
-      </c>
       <c r="T11" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="U11" t="s">
         <v>64</v>
@@ -14425,7 +14365,7 @@
         <v>64</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="X12" s="13" t="s">
         <v>433</v>
@@ -14436,16 +14376,16 @@
     </row>
     <row r="13" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>726</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="26" t="s">
         <v>727</v>
       </c>
-      <c r="B13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="26" t="s">
-        <v>728</v>
-      </c>
       <c r="T13" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="U13" t="s">
         <v>64</v>
@@ -14461,7 +14401,7 @@
         <v>64</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="X14" s="13" t="s">
         <v>433</v>
@@ -14485,13 +14425,13 @@
     </row>
     <row r="16" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>714</v>
+      </c>
+      <c r="B16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="26" t="s">
         <v>715</v>
-      </c>
-      <c r="B16" t="s">
-        <v>64</v>
-      </c>
-      <c r="C16" s="26" t="s">
-        <v>716</v>
       </c>
       <c r="X16" s="13"/>
       <c r="Y16" s="13"/>
@@ -14534,19 +14474,19 @@
     </row>
     <row r="19" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>639</v>
+      </c>
+      <c r="B19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>716</v>
+      </c>
+      <c r="V19" t="s">
+        <v>64</v>
+      </c>
+      <c r="W19" s="6" t="s">
         <v>640</v>
-      </c>
-      <c r="B19" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>717</v>
-      </c>
-      <c r="V19" t="s">
-        <v>64</v>
-      </c>
-      <c r="W19" s="6" t="s">
-        <v>641</v>
       </c>
       <c r="X19" s="13" t="s">
         <v>433</v>
@@ -14586,7 +14526,7 @@
         <v>64</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="X21" s="13" t="s">
         <v>433</v>
@@ -14603,7 +14543,7 @@
         <v>64</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="X22" s="13"/>
       <c r="Y22" s="13"/>
@@ -14616,7 +14556,7 @@
         <v>64</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="X23" s="13" t="s">
         <v>433</v>
@@ -14633,7 +14573,7 @@
         <v>64</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="X24" s="13"/>
       <c r="Y24" s="13"/>
@@ -14665,7 +14605,7 @@
         <v>64</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="X26" s="13" t="s">
         <v>433</v>
@@ -14682,31 +14622,31 @@
         <v>64</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="28" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="B28" t="s">
         <v>64</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="X28" s="13"/>
       <c r="Y28" s="13"/>
     </row>
     <row r="29" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B29" t="s">
         <v>64</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="X29" s="13" t="s">
         <v>433</v>
@@ -14745,7 +14685,7 @@
     </row>
     <row r="32" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B32" t="s">
         <v>64</v>
@@ -14770,24 +14710,9 @@
       <c r="Y69" s="6"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A30:A1048576 A1:A10 A12 A14:A27">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="!">
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",A1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A28:A29">
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="!">
-      <formula>NOT(ISERROR(SEARCH("!",A28)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A11">
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="!">
-      <formula>NOT(ISERROR(SEARCH("!",A11)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A13">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="!">
-      <formula>NOT(ISERROR(SEARCH("!",A13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14859,7 +14784,7 @@
         <v>64</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -14912,7 +14837,7 @@
         <v>353</v>
       </c>
       <c r="F1" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="G1" t="s">
         <v>354</v>
@@ -14930,13 +14855,13 @@
         <v>357</v>
       </c>
       <c r="L1" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="M1" t="s">
         <v>358</v>
       </c>
       <c r="N1" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="O1" t="s">
         <v>359</v>
@@ -14945,13 +14870,13 @@
         <v>360</v>
       </c>
       <c r="Q1" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="R1" t="s">
         <v>361</v>
       </c>
       <c r="S1" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="T1" t="s">
         <v>362</v>
@@ -14984,10 +14909,10 @@
         <v>416</v>
       </c>
       <c r="AD1" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="AE1" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="AF1" t="s">
         <v>534</v>
@@ -14999,7 +14924,7 @@
         <v>432</v>
       </c>
       <c r="AI1" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Clean up and document updated scripts
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-client.xlsx
+++ b/input/resources_spreadsheets/uscore-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC78579-BCF1-B24C-B9CE-4EDE8023D95C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A65F7D-83D3-7A4C-8B31-67AAC5D35EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -2295,18 +2295,6 @@
     <t>The HealthcareService Resource is a referenced resource when using the US Core PractitionerRole Profile and subject to constraint us-core-13: "SHALL have a practitioner, an organization, a healthcare service, or a location."</t>
   </si>
   <si>
-    <t>The US Core Client **SHALL**:
-1. Support fetching and querying of one or more US Core profile(s), using the supported RESTful interactions and search parameters declared in the US Core Server CapabilityStatement.
-1. Follow the requirements documented in the [General Requirements](general-requirements.html) and [Must Support](must-support.html) pages
-**NOTE**: US Core SearchParameters referenced in this CapabilityStatement that are derived from standard FHIR SearchParameters are only defined to document Server and Client expectations. They specify additional expectations for the following SearchParameter elements:B7
-- `multipleAnd`
-- `multipleOr`
-- `comparator`
-- `modifier`
-- `chain`
-They **SHALL NOT** be interpreted as search parameters for search. Servers and Clients **SHOULD** use the standard FHIR SearchParameters.</t>
-  </si>
-  <si>
     <t>/Users/ehaas/Documents/FHIR/US-Core/input/</t>
   </si>
   <si>
@@ -5515,6 +5503,18 @@
   </si>
   <si>
     <t>Fetches a bundle of all FamilyMemberHistory resources for the specified patient and condition</t>
+  </si>
+  <si>
+    <t>The US Core Client **SHALL**:
+1. Support fetching and querying of one or more US Core profile(s), using the supported RESTful interactions and search parameters declared in the US Core Server CapabilityStatement.
+1. Follow the requirements documented in the [General Requirements](general-requirements.html) and [Must Support](must-support.html) pages
+**NOTE**: US Core SearchParameters referenced in this CapabilityStatement that are derived from standard FHIR SearchParameters are only defined to document Server and Client expectations. They specify additional expectations for the following SearchParameter elements:
+- `multipleAnd`
+- `multipleOr`
+- `comparator`
+- `modifier`
+- `chain`
+They **SHALL NOT** be interpreted as search parameters for search. Servers and Clients **SHOULD** use the standard FHIR SearchParameters.</t>
   </si>
 </sst>
 </file>
@@ -6182,7 +6182,7 @@
         <v>422</v>
       </c>
       <c r="B2" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -10059,7 +10059,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="C72" t="s">
         <v>83</v>
@@ -10100,7 +10100,7 @@
         <v>51</v>
       </c>
       <c r="Y72" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="Z72" s="4" t="str">
         <f>"GET [base]/"&amp;B72&amp;"?patient=1137192"</f>
@@ -10120,7 +10120,7 @@
         <v>73</v>
       </c>
       <c r="B73" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="C73" t="s">
         <v>24</v>
@@ -10151,7 +10151,7 @@
         <v>52</v>
       </c>
       <c r="L73" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="M73" t="s">
         <v>51</v>
@@ -10172,7 +10172,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="C74" t="s">
         <v>56</v>
@@ -14553,7 +14553,7 @@
         <v>296</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14580,10 +14580,10 @@
         <v>142</v>
       </c>
       <c r="J38" s="23" t="s">
+        <v>696</v>
+      </c>
+      <c r="K38" s="23" t="s">
         <v>697</v>
-      </c>
-      <c r="K38" s="23" t="s">
-        <v>698</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14613,10 +14613,10 @@
         <v>650</v>
       </c>
       <c r="J39" s="23" t="s">
+        <v>698</v>
+      </c>
+      <c r="K39" s="23" t="s">
         <v>699</v>
-      </c>
-      <c r="K39" s="23" t="s">
-        <v>700</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14643,10 +14643,10 @@
         <v>142</v>
       </c>
       <c r="J40" s="23" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="K40" s="23" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14673,7 +14673,7 @@
         <v>143</v>
       </c>
       <c r="J41" s="23" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="K41" s="4" t="s">
         <v>144</v>
@@ -14703,7 +14703,7 @@
         <v>145</v>
       </c>
       <c r="J42" s="23" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="K42" s="4" t="s">
         <v>148</v>
@@ -14733,7 +14733,7 @@
         <v>145</v>
       </c>
       <c r="J43" s="23" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="K43" s="4" t="s">
         <v>148</v>
@@ -14763,7 +14763,7 @@
         <v>145</v>
       </c>
       <c r="J44" s="23" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="K44" s="4" t="s">
         <v>148</v>
@@ -14793,7 +14793,7 @@
         <v>145</v>
       </c>
       <c r="J45" s="23" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="K45" s="4" t="s">
         <v>148</v>
@@ -14943,10 +14943,10 @@
         <v>189</v>
       </c>
       <c r="J50" s="23" t="s">
+        <v>706</v>
+      </c>
+      <c r="K50" s="23" t="s">
         <v>707</v>
-      </c>
-      <c r="K50" s="23" t="s">
-        <v>708</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14972,10 +14972,10 @@
         <v>184</v>
       </c>
       <c r="J51" s="23" t="s">
+        <v>708</v>
+      </c>
+      <c r="K51" s="23" t="s">
         <v>709</v>
-      </c>
-      <c r="K51" s="23" t="s">
-        <v>710</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -15001,10 +15001,10 @@
         <v>206</v>
       </c>
       <c r="J52" s="23" t="s">
+        <v>710</v>
+      </c>
+      <c r="K52" s="23" t="s">
         <v>711</v>
-      </c>
-      <c r="K52" s="23" t="s">
-        <v>712</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -15030,10 +15030,10 @@
         <v>186</v>
       </c>
       <c r="J53" s="23" t="s">
+        <v>712</v>
+      </c>
+      <c r="K53" s="23" t="s">
         <v>713</v>
-      </c>
-      <c r="K53" s="23" t="s">
-        <v>714</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -15058,10 +15058,10 @@
       </c>
       <c r="I54" s="4"/>
       <c r="J54" s="23" t="s">
+        <v>714</v>
+      </c>
+      <c r="K54" s="23" t="s">
         <v>715</v>
-      </c>
-      <c r="K54" s="23" t="s">
-        <v>716</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -15087,10 +15087,10 @@
         <v>210</v>
       </c>
       <c r="J55" s="23" t="s">
+        <v>716</v>
+      </c>
+      <c r="K55" s="23" t="s">
         <v>717</v>
-      </c>
-      <c r="K55" s="23" t="s">
-        <v>718</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
@@ -15813,10 +15813,10 @@
         <v>266</v>
       </c>
       <c r="J78" s="23" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="K78" s="23" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="79" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -15843,7 +15843,7 @@
         <v>266</v>
       </c>
       <c r="K79" s="23" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="80" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -15870,10 +15870,10 @@
         <v>267</v>
       </c>
       <c r="J80" s="23" t="s">
+        <v>720</v>
+      </c>
+      <c r="K80" s="23" t="s">
         <v>721</v>
-      </c>
-      <c r="K80" s="23" t="s">
-        <v>722</v>
       </c>
     </row>
     <row r="81" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -15900,10 +15900,10 @@
         <v>268</v>
       </c>
       <c r="J81" s="23" t="s">
+        <v>722</v>
+      </c>
+      <c r="K81" s="23" t="s">
         <v>723</v>
-      </c>
-      <c r="K81" s="23" t="s">
-        <v>724</v>
       </c>
     </row>
     <row r="82" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -15930,7 +15930,7 @@
         <v>271</v>
       </c>
       <c r="J82" s="23" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="K82" s="23" t="s">
         <v>269</v>
@@ -15960,10 +15960,10 @@
         <v>272</v>
       </c>
       <c r="J83" s="23" t="s">
+        <v>725</v>
+      </c>
+      <c r="K83" s="23" t="s">
         <v>726</v>
-      </c>
-      <c r="K83" s="23" t="s">
-        <v>727</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
@@ -16535,7 +16535,7 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="C102" t="str">
         <f t="shared" ref="C102" si="6">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B102)</f>
@@ -16554,13 +16554,13 @@
         <v>99</v>
       </c>
       <c r="I102" s="4" t="s">
+        <v>755</v>
+      </c>
+      <c r="J102" s="23" t="s">
         <v>756</v>
       </c>
-      <c r="J102" s="23" t="s">
+      <c r="K102" s="4" t="s">
         <v>757</v>
-      </c>
-      <c r="K102" s="4" t="s">
-        <v>758</v>
       </c>
     </row>
   </sheetData>
@@ -16580,8 +16580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16611,7 +16611,7 @@
         <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -16643,7 +16643,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>690</v>
+        <v>758</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -16722,13 +16722,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>728</v>
+      </c>
+      <c r="B2" s="21" t="s">
         <v>729</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="C2" s="27" t="s">
         <v>730</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>731</v>
       </c>
       <c r="D2" t="s">
         <v>64</v>
@@ -16818,7 +16818,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E587077-1E4A-9B49-9E3A-06514799DDEB}">
   <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="A18" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
@@ -16937,7 +16937,7 @@
         <v>607</v>
       </c>
       <c r="B8" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
@@ -16990,10 +16990,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
+        <v>691</v>
+      </c>
+      <c r="B12" t="s">
         <v>692</v>
-      </c>
-      <c r="B12" t="s">
-        <v>693</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
@@ -17102,16 +17102,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>745</v>
+      </c>
+      <c r="B20" t="s">
         <v>746</v>
-      </c>
-      <c r="B20" t="s">
-        <v>747</v>
       </c>
       <c r="D20" t="s">
         <v>11</v>
       </c>
       <c r="E20" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -17200,10 +17200,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>693</v>
+      </c>
+      <c r="B27" t="s">
         <v>694</v>
-      </c>
-      <c r="B27" t="s">
-        <v>695</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
@@ -17718,10 +17718,10 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
+        <v>749</v>
+      </c>
+      <c r="B64" t="s">
         <v>750</v>
-      </c>
-      <c r="B64" t="s">
-        <v>751</v>
       </c>
       <c r="D64" t="s">
         <v>11</v>
@@ -17935,7 +17935,7 @@
         <v>64</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="X5" s="12" t="s">
         <v>410</v>
@@ -17966,7 +17966,7 @@
         <v>64</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="X7" s="12" t="s">
         <v>410</v>
@@ -17983,7 +17983,7 @@
         <v>64</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="X8" s="12" t="s">
         <v>410</v>
@@ -18000,7 +18000,7 @@
         <v>64</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="X9" s="12" t="s">
         <v>410</v>
@@ -18017,7 +18017,7 @@
         <v>64</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="X10" s="12" t="s">
         <v>410</v>
@@ -18041,7 +18041,7 @@
     </row>
     <row r="12" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B12" t="s">
         <v>64</v>
@@ -18092,7 +18092,7 @@
         <v>64</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="X15" s="12" t="s">
         <v>410</v>
@@ -18148,7 +18148,7 @@
         <v>64</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="V19" t="s">
         <v>64</v>
@@ -18171,7 +18171,7 @@
         <v>64</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="V20" t="s">
         <v>64</v>
@@ -18217,7 +18217,7 @@
         <v>64</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="X22" s="12" t="s">
         <v>410</v>
@@ -18234,7 +18234,7 @@
         <v>64</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="X23" s="12"/>
       <c r="Y23" s="12"/>
@@ -18247,7 +18247,7 @@
         <v>64</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="X24" s="12" t="s">
         <v>410</v>
@@ -18264,7 +18264,7 @@
         <v>64</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="X25" s="12"/>
       <c r="Y25" s="12"/>
@@ -18371,7 +18371,7 @@
         <v>64</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="X32" s="12" t="s">
         <v>410</v>
@@ -18558,7 +18558,7 @@
         <v>656</v>
       </c>
       <c r="M1" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="N1" t="s">
         <v>340</v>

</xml_diff>